<commit_message>
2019 October data update
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE_1" sheetId="5" r:id="rId1"/>
@@ -25,37 +25,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="CB5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC6" authorId="0" shapeId="0">
+    <comment ref="CD14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CC7" authorId="0" shapeId="0">
+    <comment ref="CE14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CC8" authorId="0" shapeId="0">
+    <comment ref="CD17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,232 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CC9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC11" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC12" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC13" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC14" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC15" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC17" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC18" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC21" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC23" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC24" authorId="0" shapeId="0">
+    <comment ref="CE17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -880,7 +625,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CC25" authorId="0" shapeId="0">
+    <comment ref="CD31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -895,472 +640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CC26" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC27" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC28" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC29" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC31" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC32" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC34" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC35" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC36" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC37" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC38" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CA39" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Correction
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC39" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC40" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC41" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC42" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC43" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC44" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC45" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC46" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC47" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC48" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC49" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC50" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC51" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC52" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC53" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC54" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC55" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">*  Preliminary
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CC56" authorId="0" shapeId="0">
+    <comment ref="CE31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1645,7 +925,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1667,6 +947,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2372,11 +1653,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:MG56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="CE5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5:CP56"/>
+      <selection pane="bottomRight" activeCell="CS19" sqref="CS19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2961,12 +2242,14 @@
         <v>8916.4000000000015</v>
       </c>
       <c r="CO5" s="6">
-        <v>9328.7999999999993</v>
+        <v>9329.5</v>
       </c>
       <c r="CP5" s="6">
-        <v>10517.2</v>
-      </c>
-      <c r="CQ5" s="6"/>
+        <v>10509.1</v>
+      </c>
+      <c r="CQ5" s="6">
+        <v>10955.199999999999</v>
+      </c>
       <c r="CR5" s="6"/>
       <c r="CS5" s="6"/>
       <c r="CT5" s="6"/>
@@ -3499,9 +2782,11 @@
         <v>153.69999999999999</v>
       </c>
       <c r="CP6" s="6">
-        <v>162.80000000000001</v>
-      </c>
-      <c r="CQ6" s="6"/>
+        <v>164.1</v>
+      </c>
+      <c r="CQ6" s="6">
+        <v>166.7</v>
+      </c>
       <c r="CR6" s="6"/>
       <c r="CS6" s="6"/>
       <c r="CT6" s="6"/>
@@ -4036,7 +3321,9 @@
       <c r="CP7" s="6">
         <v>28.9</v>
       </c>
-      <c r="CQ7" s="6"/>
+      <c r="CQ7" s="6">
+        <v>30.3</v>
+      </c>
       <c r="CR7" s="6"/>
       <c r="CS7" s="6"/>
       <c r="CT7" s="6"/>
@@ -4569,9 +3856,11 @@
         <v>190.79999999999998</v>
       </c>
       <c r="CP8" s="6">
-        <v>203.4</v>
-      </c>
-      <c r="CQ8" s="6"/>
+        <v>203.6</v>
+      </c>
+      <c r="CQ8" s="6">
+        <v>204.6</v>
+      </c>
       <c r="CR8" s="6"/>
       <c r="CS8" s="6"/>
       <c r="CT8" s="6"/>
@@ -5106,7 +4395,9 @@
       <c r="CP9" s="6">
         <v>103</v>
       </c>
-      <c r="CQ9" s="6"/>
+      <c r="CQ9" s="6">
+        <v>104.4</v>
+      </c>
       <c r="CR9" s="6"/>
       <c r="CS9" s="6"/>
       <c r="CT9" s="6"/>
@@ -5641,7 +4932,9 @@
       <c r="CP10" s="6">
         <v>1227.3</v>
       </c>
-      <c r="CQ10" s="6"/>
+      <c r="CQ10" s="6">
+        <v>1298.5</v>
+      </c>
       <c r="CR10" s="6"/>
       <c r="CS10" s="6"/>
       <c r="CT10" s="6"/>
@@ -6174,9 +5467,11 @@
         <v>196.4</v>
       </c>
       <c r="CP11" s="6">
-        <v>218.7</v>
-      </c>
-      <c r="CQ11" s="6"/>
+        <v>217.8</v>
+      </c>
+      <c r="CQ11" s="6">
+        <v>223.5</v>
+      </c>
       <c r="CR11" s="6"/>
       <c r="CS11" s="6"/>
       <c r="CT11" s="6"/>
@@ -6711,7 +6006,9 @@
       <c r="CP12" s="6">
         <v>121.5</v>
       </c>
-      <c r="CQ12" s="6"/>
+      <c r="CQ12" s="6">
+        <v>125.3</v>
+      </c>
       <c r="CR12" s="6"/>
       <c r="CS12" s="6"/>
       <c r="CT12" s="6"/>
@@ -7244,9 +6541,11 @@
         <v>31.1</v>
       </c>
       <c r="CP13" s="6">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="CQ13" s="6"/>
+        <v>35.6</v>
+      </c>
+      <c r="CQ13" s="6">
+        <v>37</v>
+      </c>
       <c r="CR13" s="6"/>
       <c r="CS13" s="6"/>
       <c r="CT13" s="6"/>
@@ -7594,8 +6893,8 @@
       <c r="CM14" s="8"/>
       <c r="CN14" s="8"/>
       <c r="CO14" s="8"/>
-      <c r="CP14" s="6"/>
-      <c r="CQ14" s="6"/>
+      <c r="CP14" s="8"/>
+      <c r="CQ14" s="8"/>
       <c r="CR14" s="6"/>
       <c r="CS14" s="6"/>
       <c r="CT14" s="6"/>
@@ -8128,9 +7427,11 @@
         <v>484</v>
       </c>
       <c r="CP15" s="6">
-        <v>504.90000000000003</v>
-      </c>
-      <c r="CQ15" s="6"/>
+        <v>505.3</v>
+      </c>
+      <c r="CQ15" s="6">
+        <v>513.5</v>
+      </c>
       <c r="CR15" s="6"/>
       <c r="CS15" s="6"/>
       <c r="CT15" s="6"/>
@@ -8663,9 +7964,11 @@
         <v>349.1</v>
       </c>
       <c r="CP16" s="6">
-        <v>356.1</v>
-      </c>
-      <c r="CQ16" s="6"/>
+        <v>355.7</v>
+      </c>
+      <c r="CQ16" s="6">
+        <v>358.1</v>
+      </c>
       <c r="CR16" s="6"/>
       <c r="CS16" s="6"/>
       <c r="CT16" s="6"/>
@@ -9013,8 +8316,8 @@
       <c r="CM17" s="8"/>
       <c r="CN17" s="8"/>
       <c r="CO17" s="8"/>
-      <c r="CP17" s="6"/>
-      <c r="CQ17" s="6"/>
+      <c r="CP17" s="8"/>
+      <c r="CQ17" s="8"/>
       <c r="CR17" s="6"/>
       <c r="CS17" s="6"/>
       <c r="CT17" s="6"/>
@@ -9547,9 +8850,11 @@
         <v>50.900000000000006</v>
       </c>
       <c r="CP18" s="6">
-        <v>59.1</v>
-      </c>
-      <c r="CQ18" s="6"/>
+        <v>59</v>
+      </c>
+      <c r="CQ18" s="6">
+        <v>63.4</v>
+      </c>
       <c r="CR18" s="6"/>
       <c r="CS18" s="6"/>
       <c r="CT18" s="6"/>
@@ -10084,7 +9389,9 @@
       <c r="CP19" s="6">
         <v>438.7</v>
       </c>
-      <c r="CQ19" s="6"/>
+      <c r="CQ19" s="6">
+        <v>453.1</v>
+      </c>
       <c r="CR19" s="6"/>
       <c r="CS19" s="6"/>
       <c r="CT19" s="6"/>
@@ -10617,9 +9924,11 @@
         <v>212.3</v>
       </c>
       <c r="CP20" s="6">
-        <v>238.3</v>
-      </c>
-      <c r="CQ20" s="6"/>
+        <v>235.6</v>
+      </c>
+      <c r="CQ20" s="6">
+        <v>237.6</v>
+      </c>
       <c r="CR20" s="6"/>
       <c r="CS20" s="6"/>
       <c r="CT20" s="6"/>
@@ -11154,7 +10463,9 @@
       <c r="CP21" s="6">
         <v>146.1</v>
       </c>
-      <c r="CQ21" s="6"/>
+      <c r="CQ21" s="6">
+        <v>153.19999999999999</v>
+      </c>
       <c r="CR21" s="6"/>
       <c r="CS21" s="6"/>
       <c r="CT21" s="6"/>
@@ -11687,9 +10998,11 @@
         <v>115.9</v>
       </c>
       <c r="CP22" s="6">
-        <v>139.1</v>
-      </c>
-      <c r="CQ22" s="6"/>
+        <v>138.5</v>
+      </c>
+      <c r="CQ22" s="6">
+        <v>144.80000000000001</v>
+      </c>
       <c r="CR22" s="6"/>
       <c r="CS22" s="6"/>
       <c r="CT22" s="6"/>
@@ -12224,7 +11537,9 @@
       <c r="CP23" s="6">
         <v>161.80000000000001</v>
       </c>
-      <c r="CQ23" s="6"/>
+      <c r="CQ23" s="6">
+        <v>163.30000000000001</v>
+      </c>
       <c r="CR23" s="6"/>
       <c r="CS23" s="6"/>
       <c r="CT23" s="6"/>
@@ -12759,7 +12074,9 @@
       <c r="CP24" s="6">
         <v>152.1</v>
       </c>
-      <c r="CQ24" s="6"/>
+      <c r="CQ24" s="6">
+        <v>157.1</v>
+      </c>
       <c r="CR24" s="6"/>
       <c r="CS24" s="6"/>
       <c r="CT24" s="6"/>
@@ -13294,7 +12611,9 @@
       <c r="CP25" s="6">
         <v>49.900000000000006</v>
       </c>
-      <c r="CQ25" s="6"/>
+      <c r="CQ25" s="6">
+        <v>51.6</v>
+      </c>
       <c r="CR25" s="6"/>
       <c r="CS25" s="6"/>
       <c r="CT25" s="6"/>
@@ -13829,7 +13148,9 @@
       <c r="CP26" s="6">
         <v>212.29999999999998</v>
       </c>
-      <c r="CQ26" s="6"/>
+      <c r="CQ26" s="6">
+        <v>225.4</v>
+      </c>
       <c r="CR26" s="6"/>
       <c r="CS26" s="6"/>
       <c r="CT26" s="6"/>
@@ -14364,7 +13685,9 @@
       <c r="CP27" s="6">
         <v>236.70000000000002</v>
       </c>
-      <c r="CQ27" s="6"/>
+      <c r="CQ27" s="6">
+        <v>246.7</v>
+      </c>
       <c r="CR27" s="6"/>
       <c r="CS27" s="6"/>
       <c r="CT27" s="6"/>
@@ -14897,9 +14220,11 @@
         <v>266.70000000000005</v>
       </c>
       <c r="CP28" s="6">
-        <v>322.5</v>
-      </c>
-      <c r="CQ28" s="6"/>
+        <v>322.20000000000005</v>
+      </c>
+      <c r="CQ28" s="6">
+        <v>336.1</v>
+      </c>
       <c r="CR28" s="6"/>
       <c r="CS28" s="6"/>
       <c r="CT28" s="6"/>
@@ -15434,7 +14759,9 @@
       <c r="CP29" s="6">
         <v>196.9</v>
       </c>
-      <c r="CQ29" s="6"/>
+      <c r="CQ29" s="6">
+        <v>212.5</v>
+      </c>
       <c r="CR29" s="6"/>
       <c r="CS29" s="6"/>
       <c r="CT29" s="6"/>
@@ -15969,7 +15296,9 @@
       <c r="CP30" s="6">
         <v>108.5</v>
       </c>
-      <c r="CQ30" s="6"/>
+      <c r="CQ30" s="6">
+        <v>109.2</v>
+      </c>
       <c r="CR30" s="6"/>
       <c r="CS30" s="6"/>
       <c r="CT30" s="6"/>
@@ -16317,8 +15646,8 @@
       <c r="CM31" s="8"/>
       <c r="CN31" s="8"/>
       <c r="CO31" s="8"/>
-      <c r="CP31" s="6"/>
-      <c r="CQ31" s="6"/>
+      <c r="CP31" s="8"/>
+      <c r="CQ31" s="8"/>
       <c r="CR31" s="6"/>
       <c r="CS31" s="6"/>
       <c r="CT31" s="6"/>
@@ -16853,7 +16182,9 @@
       <c r="CP32" s="6">
         <v>42</v>
       </c>
-      <c r="CQ32" s="6"/>
+      <c r="CQ32" s="6">
+        <v>45.1</v>
+      </c>
       <c r="CR32" s="6"/>
       <c r="CS32" s="6"/>
       <c r="CT32" s="6"/>
@@ -17386,9 +16717,11 @@
         <v>83.1</v>
       </c>
       <c r="CP33" s="6">
-        <v>93.2</v>
-      </c>
-      <c r="CQ33" s="6"/>
+        <v>93.4</v>
+      </c>
+      <c r="CQ33" s="6">
+        <v>97</v>
+      </c>
       <c r="CR33" s="6"/>
       <c r="CS33" s="6"/>
       <c r="CT33" s="6"/>
@@ -17921,9 +17254,11 @@
         <v>69.099999999999994</v>
       </c>
       <c r="CP34" s="6">
-        <v>79.900000000000006</v>
-      </c>
-      <c r="CQ34" s="6"/>
+        <v>77.8</v>
+      </c>
+      <c r="CQ34" s="6">
+        <v>76.099999999999994</v>
+      </c>
       <c r="CR34" s="6"/>
       <c r="CS34" s="6"/>
       <c r="CT34" s="6"/>
@@ -18456,9 +17791,11 @@
         <v>35.6</v>
       </c>
       <c r="CP35" s="6">
-        <v>45</v>
-      </c>
-      <c r="CQ35" s="6"/>
+        <v>45.099999999999994</v>
+      </c>
+      <c r="CQ35" s="6">
+        <v>47.6</v>
+      </c>
       <c r="CR35" s="6"/>
       <c r="CS35" s="6"/>
       <c r="CT35" s="6"/>
@@ -18993,7 +18330,9 @@
       <c r="CP36" s="6">
         <v>293.89999999999998</v>
       </c>
-      <c r="CQ36" s="6"/>
+      <c r="CQ36" s="6">
+        <v>318.5</v>
+      </c>
       <c r="CR36" s="6"/>
       <c r="CS36" s="6"/>
       <c r="CT36" s="6"/>
@@ -19526,9 +18865,11 @@
         <v>70.099999999999994</v>
       </c>
       <c r="CP37" s="6">
-        <v>75.900000000000006</v>
-      </c>
-      <c r="CQ37" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="CQ37" s="6">
+        <v>78.2</v>
+      </c>
       <c r="CR37" s="6"/>
       <c r="CS37" s="6"/>
       <c r="CT37" s="6"/>
@@ -20063,7 +19404,9 @@
       <c r="CP38" s="6">
         <v>637.9</v>
       </c>
-      <c r="CQ38" s="6"/>
+      <c r="CQ38" s="6">
+        <v>675.1</v>
+      </c>
       <c r="CR38" s="6"/>
       <c r="CS38" s="6"/>
       <c r="CT38" s="6"/>
@@ -20598,7 +19941,9 @@
       <c r="CP39" s="6">
         <v>330.4</v>
       </c>
-      <c r="CQ39" s="6"/>
+      <c r="CQ39" s="6">
+        <v>338.1</v>
+      </c>
       <c r="CR39" s="6"/>
       <c r="CS39" s="6"/>
       <c r="CT39" s="6"/>
@@ -21133,7 +20478,9 @@
       <c r="CP40" s="6">
         <v>36.6</v>
       </c>
-      <c r="CQ40" s="6"/>
+      <c r="CQ40" s="6">
+        <v>38.9</v>
+      </c>
       <c r="CR40" s="6"/>
       <c r="CS40" s="6"/>
       <c r="CT40" s="6"/>
@@ -21666,9 +21013,11 @@
         <v>355</v>
       </c>
       <c r="CP41" s="6">
-        <v>392.7</v>
-      </c>
-      <c r="CQ41" s="6"/>
+        <v>392.2</v>
+      </c>
+      <c r="CQ41" s="6">
+        <v>408.8</v>
+      </c>
       <c r="CR41" s="6"/>
       <c r="CS41" s="6"/>
       <c r="CT41" s="6"/>
@@ -22203,7 +21552,9 @@
       <c r="CP42" s="6">
         <v>143.80000000000001</v>
       </c>
-      <c r="CQ42" s="6"/>
+      <c r="CQ42" s="6">
+        <v>148.19999999999999</v>
+      </c>
       <c r="CR42" s="6"/>
       <c r="CS42" s="6"/>
       <c r="CT42" s="6"/>
@@ -22736,9 +22087,11 @@
         <v>107.30000000000001</v>
       </c>
       <c r="CP43" s="6">
-        <v>120.39999999999999</v>
-      </c>
-      <c r="CQ43" s="6"/>
+        <v>122.39999999999999</v>
+      </c>
+      <c r="CQ43" s="6">
+        <v>140.60000000000002</v>
+      </c>
       <c r="CR43" s="6"/>
       <c r="CS43" s="6"/>
       <c r="CT43" s="6"/>
@@ -23271,9 +22624,11 @@
         <v>283</v>
       </c>
       <c r="CP44" s="6">
-        <v>336.5</v>
-      </c>
-      <c r="CQ44" s="6"/>
+        <v>336.7</v>
+      </c>
+      <c r="CQ44" s="6">
+        <v>345.5</v>
+      </c>
       <c r="CR44" s="6"/>
       <c r="CS44" s="6"/>
       <c r="CT44" s="6"/>
@@ -23808,7 +23163,9 @@
       <c r="CP45" s="6">
         <v>26.2</v>
       </c>
-      <c r="CQ45" s="6"/>
+      <c r="CQ45" s="6">
+        <v>27.900000000000002</v>
+      </c>
       <c r="CR45" s="6"/>
       <c r="CS45" s="6"/>
       <c r="CT45" s="6"/>
@@ -24341,9 +23698,11 @@
         <v>152.1</v>
       </c>
       <c r="CP46" s="6">
-        <v>164.5</v>
-      </c>
-      <c r="CQ46" s="6"/>
+        <v>164.4</v>
+      </c>
+      <c r="CQ46" s="6">
+        <v>168.2</v>
+      </c>
       <c r="CR46" s="6"/>
       <c r="CS46" s="6"/>
       <c r="CT46" s="6"/>
@@ -24876,9 +24235,11 @@
         <v>28.799999999999997</v>
       </c>
       <c r="CP47" s="6">
-        <v>36</v>
-      </c>
-      <c r="CQ47" s="6"/>
+        <v>36.200000000000003</v>
+      </c>
+      <c r="CQ47" s="6">
+        <v>37.9</v>
+      </c>
       <c r="CR47" s="6"/>
       <c r="CS47" s="6"/>
       <c r="CT47" s="6"/>
@@ -25411,9 +24772,11 @@
         <v>183.5</v>
       </c>
       <c r="CP48" s="6">
-        <v>208.5</v>
-      </c>
-      <c r="CQ48" s="6"/>
+        <v>208.29999999999998</v>
+      </c>
+      <c r="CQ48" s="6">
+        <v>212.8</v>
+      </c>
       <c r="CR48" s="6"/>
       <c r="CS48" s="6"/>
       <c r="CT48" s="6"/>
@@ -25948,7 +25311,9 @@
       <c r="CP49" s="6">
         <v>1095.1000000000001</v>
       </c>
-      <c r="CQ49" s="6"/>
+      <c r="CQ49" s="6">
+        <v>1140.2</v>
+      </c>
       <c r="CR49" s="6"/>
       <c r="CS49" s="6"/>
       <c r="CT49" s="6"/>
@@ -26481,9 +25846,11 @@
         <v>103.3</v>
       </c>
       <c r="CP50" s="6">
-        <v>123.1</v>
-      </c>
-      <c r="CQ50" s="6"/>
+        <v>122.69999999999999</v>
+      </c>
+      <c r="CQ50" s="6">
+        <v>127.30000000000001</v>
+      </c>
       <c r="CR50" s="6"/>
       <c r="CS50" s="6"/>
       <c r="CT50" s="6"/>
@@ -27018,7 +26385,9 @@
       <c r="CP51" s="6">
         <v>31.400000000000002</v>
       </c>
-      <c r="CQ51" s="6"/>
+      <c r="CQ51" s="6">
+        <v>33.4</v>
+      </c>
       <c r="CR51" s="6"/>
       <c r="CS51" s="6"/>
       <c r="CT51" s="6"/>
@@ -27551,9 +26920,11 @@
         <v>275.3</v>
       </c>
       <c r="CP52" s="6">
-        <v>309.2</v>
-      </c>
-      <c r="CQ52" s="6"/>
+        <v>302.89999999999998</v>
+      </c>
+      <c r="CQ52" s="6">
+        <v>310.7</v>
+      </c>
       <c r="CR52" s="6"/>
       <c r="CS52" s="6"/>
       <c r="CT52" s="6"/>
@@ -28086,9 +27457,11 @@
         <v>226.3</v>
       </c>
       <c r="CP53" s="6">
-        <v>241.3</v>
-      </c>
-      <c r="CQ53" s="6"/>
+        <v>241.8</v>
+      </c>
+      <c r="CQ53" s="6">
+        <v>264.5</v>
+      </c>
       <c r="CR53" s="6"/>
       <c r="CS53" s="6"/>
       <c r="CT53" s="6"/>
@@ -28623,7 +27996,9 @@
       <c r="CP54" s="6">
         <v>61.4</v>
       </c>
-      <c r="CQ54" s="6"/>
+      <c r="CQ54" s="6">
+        <v>64.599999999999994</v>
+      </c>
       <c r="CR54" s="6"/>
       <c r="CS54" s="6"/>
       <c r="CT54" s="6"/>
@@ -29156,9 +28531,11 @@
         <v>165.2</v>
       </c>
       <c r="CP55" s="6">
-        <v>199</v>
-      </c>
-      <c r="CQ55" s="6"/>
+        <v>198.60000000000002</v>
+      </c>
+      <c r="CQ55" s="6">
+        <v>216.8</v>
+      </c>
       <c r="CR55" s="6"/>
       <c r="CS55" s="6"/>
       <c r="CT55" s="6"/>
@@ -29693,7 +29070,9 @@
       <c r="CP56" s="6">
         <v>29.6</v>
       </c>
-      <c r="CQ56" s="6"/>
+      <c r="CQ56" s="6">
+        <v>31</v>
+      </c>
       <c r="CR56" s="6"/>
       <c r="CS56" s="6"/>
       <c r="CT56" s="6"/>
@@ -29955,17 +29334,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CQ56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="BZ30" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="BV5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="CE35" sqref="CE35"/>
+      <selection pane="bottomRight" activeCell="CC8" sqref="CC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="81" max="95" width="9.140625" style="9"/>
+    <col min="81" max="82" width="9.140625" style="9"/>
+    <col min="83" max="83" width="9.140625" style="9" customWidth="1"/>
+    <col min="84" max="95" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -30531,14 +29912,16 @@
         <v>0.25298238118262878</v>
       </c>
       <c r="CC5" s="6">
-        <v>0.44468371467024786</v>
+        <v>0.45222072678331088</v>
       </c>
       <c r="CD5" s="10">
-        <v>0.61417774801493086</v>
-      </c>
-      <c r="CE5" s="9"/>
-      <c r="CF5" s="9"/>
-      <c r="CG5" s="9"/>
+        <v>0.53668803214388561</v>
+      </c>
+      <c r="CE5" s="11">
+        <v>0.63382998658852496</v>
+      </c>
+      <c r="CF5" s="11"/>
+      <c r="CG5" s="11"/>
       <c r="CH5" s="9"/>
       <c r="CI5" s="9"/>
       <c r="CJ5" s="9"/>
@@ -30795,11 +30178,13 @@
         <v>-1.2210796915167133</v>
       </c>
       <c r="CD6" s="10">
-        <v>-0.36719706242347977</v>
-      </c>
-      <c r="CE6" s="9"/>
-      <c r="CF6" s="9"/>
-      <c r="CG6" s="9"/>
+        <v>0.42839657282742788</v>
+      </c>
+      <c r="CE6" s="11">
+        <v>0.24052916416114084</v>
+      </c>
+      <c r="CF6" s="11"/>
+      <c r="CG6" s="11"/>
       <c r="CH6" s="9"/>
       <c r="CI6" s="9"/>
       <c r="CJ6" s="9"/>
@@ -31058,9 +30443,11 @@
       <c r="CD7" s="10">
         <v>-2.0338983050847506</v>
       </c>
-      <c r="CE7" s="9"/>
-      <c r="CF7" s="9"/>
-      <c r="CG7" s="9"/>
+      <c r="CE7" s="11">
+        <v>-1.9417475728155384</v>
+      </c>
+      <c r="CF7" s="11"/>
+      <c r="CG7" s="11"/>
       <c r="CH7" s="9"/>
       <c r="CI7" s="9"/>
       <c r="CJ7" s="9"/>
@@ -31317,11 +30704,13 @@
         <v>4.2053522665210048</v>
       </c>
       <c r="CD8" s="10">
-        <v>-0.82886396879571766</v>
-      </c>
-      <c r="CE8" s="9"/>
-      <c r="CF8" s="9"/>
-      <c r="CG8" s="9"/>
+        <v>-0.73135056070211035</v>
+      </c>
+      <c r="CE8" s="11">
+        <v>-1.0159651669085605</v>
+      </c>
+      <c r="CF8" s="11"/>
+      <c r="CG8" s="11"/>
       <c r="CH8" s="9"/>
       <c r="CI8" s="9"/>
       <c r="CJ8" s="9"/>
@@ -31580,9 +30969,11 @@
       <c r="CD9" s="10">
         <v>1.079489695780171</v>
       </c>
-      <c r="CE9" s="9"/>
-      <c r="CF9" s="9"/>
-      <c r="CG9" s="9"/>
+      <c r="CE9" s="11">
+        <v>0.19193857965451327</v>
+      </c>
+      <c r="CF9" s="11"/>
+      <c r="CG9" s="11"/>
       <c r="CH9" s="9"/>
       <c r="CI9" s="9"/>
       <c r="CJ9" s="9"/>
@@ -31841,9 +31232,11 @@
       <c r="CD10" s="10">
         <v>1.977565434150391</v>
       </c>
-      <c r="CE10" s="9"/>
-      <c r="CF10" s="9"/>
-      <c r="CG10" s="9"/>
+      <c r="CE10" s="11">
+        <v>1.4770240700218891</v>
+      </c>
+      <c r="CF10" s="11"/>
+      <c r="CG10" s="11"/>
       <c r="CH10" s="9"/>
       <c r="CI10" s="9"/>
       <c r="CJ10" s="9"/>
@@ -32100,11 +31493,13 @@
         <v>-0.55696202531645278</v>
       </c>
       <c r="CD11" s="10">
-        <v>2.1485287248948928</v>
-      </c>
-      <c r="CE11" s="9"/>
-      <c r="CF11" s="9"/>
-      <c r="CG11" s="9"/>
+        <v>1.7281644091545951</v>
+      </c>
+      <c r="CE11" s="11">
+        <v>2.2415370539798745</v>
+      </c>
+      <c r="CF11" s="11"/>
+      <c r="CG11" s="11"/>
       <c r="CH11" s="9"/>
       <c r="CI11" s="9"/>
       <c r="CJ11" s="9"/>
@@ -32363,9 +31758,11 @@
       <c r="CD12" s="10">
         <v>-1.5397082658022623</v>
       </c>
-      <c r="CE12" s="9"/>
-      <c r="CF12" s="9"/>
-      <c r="CG12" s="9"/>
+      <c r="CE12" s="11">
+        <v>-0.94861660079051613</v>
+      </c>
+      <c r="CF12" s="11"/>
+      <c r="CG12" s="11"/>
       <c r="CH12" s="9"/>
       <c r="CI12" s="9"/>
       <c r="CJ12" s="9"/>
@@ -32622,11 +32019,13 @@
         <v>3.6666666666666714</v>
       </c>
       <c r="CD13" s="10">
-        <v>3.779069767441873</v>
-      </c>
-      <c r="CE13" s="9"/>
-      <c r="CF13" s="9"/>
-      <c r="CG13" s="9"/>
+        <v>3.4883720930232642</v>
+      </c>
+      <c r="CE13" s="11">
+        <v>1.0928961748633841</v>
+      </c>
+      <c r="CF13" s="11"/>
+      <c r="CG13" s="11"/>
       <c r="CH13" s="9"/>
       <c r="CI13" s="9"/>
       <c r="CJ13" s="9"/>
@@ -32722,10 +32121,10 @@
       <c r="CA14" s="8"/>
       <c r="CB14" s="8"/>
       <c r="CC14" s="8"/>
-      <c r="CD14" s="10"/>
-      <c r="CE14" s="9"/>
-      <c r="CF14" s="9"/>
-      <c r="CG14" s="9"/>
+      <c r="CD14" s="8"/>
+      <c r="CE14" s="8"/>
+      <c r="CF14" s="11"/>
+      <c r="CG14" s="11"/>
       <c r="CH14" s="9"/>
       <c r="CI14" s="9"/>
       <c r="CJ14" s="9"/>
@@ -32982,11 +32381,13 @@
         <v>-0.12381345439538231</v>
       </c>
       <c r="CD15" s="10">
-        <v>0.69804547267651718</v>
-      </c>
-      <c r="CE15" s="9"/>
-      <c r="CF15" s="9"/>
-      <c r="CG15" s="9"/>
+        <v>0.77782209812525616</v>
+      </c>
+      <c r="CE15" s="11">
+        <v>1.1424069332282867</v>
+      </c>
+      <c r="CF15" s="11"/>
+      <c r="CG15" s="11"/>
       <c r="CH15" s="9"/>
       <c r="CI15" s="9"/>
       <c r="CJ15" s="9"/>
@@ -33243,11 +32644,13 @@
         <v>1.0127314814814814</v>
       </c>
       <c r="CD16" s="10">
-        <v>1.1647727272727337</v>
-      </c>
-      <c r="CE16" s="9"/>
-      <c r="CF16" s="9"/>
-      <c r="CG16" s="9"/>
+        <v>1.0511363636363604</v>
+      </c>
+      <c r="CE16" s="11">
+        <v>0.61815116605789422</v>
+      </c>
+      <c r="CF16" s="11"/>
+      <c r="CG16" s="11"/>
       <c r="CH16" s="9"/>
       <c r="CI16" s="9"/>
       <c r="CJ16" s="9"/>
@@ -33343,10 +32746,10 @@
       <c r="CA17" s="8"/>
       <c r="CB17" s="8"/>
       <c r="CC17" s="8"/>
-      <c r="CD17" s="10"/>
-      <c r="CE17" s="9"/>
-      <c r="CF17" s="9"/>
-      <c r="CG17" s="9"/>
+      <c r="CD17" s="8"/>
+      <c r="CE17" s="8"/>
+      <c r="CF17" s="11"/>
+      <c r="CG17" s="11"/>
       <c r="CH17" s="9"/>
       <c r="CI17" s="9"/>
       <c r="CJ17" s="9"/>
@@ -33603,11 +33006,13 @@
         <v>4.3032786885246077</v>
       </c>
       <c r="CD18" s="10">
-        <v>1.546391752577317</v>
-      </c>
-      <c r="CE18" s="9"/>
-      <c r="CF18" s="9"/>
-      <c r="CG18" s="9"/>
+        <v>1.3745704467353903</v>
+      </c>
+      <c r="CE18" s="11">
+        <v>1.4399999999999977</v>
+      </c>
+      <c r="CF18" s="11"/>
+      <c r="CG18" s="11"/>
       <c r="CH18" s="9"/>
       <c r="CI18" s="9"/>
       <c r="CJ18" s="9"/>
@@ -33866,9 +33271,11 @@
       <c r="CD19" s="10">
         <v>1.3163972286374108</v>
       </c>
-      <c r="CE19" s="9"/>
-      <c r="CF19" s="9"/>
-      <c r="CG19" s="9"/>
+      <c r="CE19" s="11">
+        <v>2.9071087894617333</v>
+      </c>
+      <c r="CF19" s="11"/>
+      <c r="CG19" s="11"/>
       <c r="CH19" s="9"/>
       <c r="CI19" s="9"/>
       <c r="CJ19" s="9"/>
@@ -34125,11 +33532,13 @@
         <v>-0.23496240601503759</v>
       </c>
       <c r="CD20" s="10">
-        <v>-0.33458803847761731</v>
-      </c>
-      <c r="CE20" s="9"/>
-      <c r="CF20" s="9"/>
-      <c r="CG20" s="9"/>
+        <v>-1.4638226683396069</v>
+      </c>
+      <c r="CE20" s="11">
+        <v>-1.2058212058212081</v>
+      </c>
+      <c r="CF20" s="11"/>
+      <c r="CG20" s="11"/>
       <c r="CH20" s="9"/>
       <c r="CI20" s="9"/>
       <c r="CJ20" s="9"/>
@@ -34388,9 +33797,11 @@
       <c r="CD21" s="10">
         <v>1.882845188284531</v>
       </c>
-      <c r="CE21" s="9"/>
-      <c r="CF21" s="9"/>
-      <c r="CG21" s="9"/>
+      <c r="CE21" s="11">
+        <v>1.6589250165892504</v>
+      </c>
+      <c r="CF21" s="11"/>
+      <c r="CG21" s="11"/>
       <c r="CH21" s="9"/>
       <c r="CI21" s="9"/>
       <c r="CJ21" s="9"/>
@@ -34647,11 +34058,13 @@
         <v>0.95818815331009943</v>
       </c>
       <c r="CD22" s="10">
-        <v>1.7556693489392874</v>
-      </c>
-      <c r="CE22" s="9"/>
-      <c r="CF22" s="9"/>
-      <c r="CG22" s="9"/>
+        <v>1.3167520117044706</v>
+      </c>
+      <c r="CE22" s="11">
+        <v>2.9871977240398415</v>
+      </c>
+      <c r="CF22" s="11"/>
+      <c r="CG22" s="11"/>
       <c r="CH22" s="9"/>
       <c r="CI22" s="9"/>
       <c r="CJ22" s="9"/>
@@ -34910,9 +34323,11 @@
       <c r="CD23" s="10">
         <v>-1.1002444987775128</v>
       </c>
-      <c r="CE23" s="9"/>
-      <c r="CF23" s="9"/>
-      <c r="CG23" s="9"/>
+      <c r="CE23" s="11">
+        <v>-1.0902483343428122</v>
+      </c>
+      <c r="CF23" s="11"/>
+      <c r="CG23" s="11"/>
       <c r="CH23" s="9"/>
       <c r="CI23" s="9"/>
       <c r="CJ23" s="9"/>
@@ -35171,9 +34586,11 @@
       <c r="CD24" s="10">
         <v>0.19762845849801247</v>
       </c>
-      <c r="CE24" s="9"/>
-      <c r="CF24" s="9"/>
-      <c r="CG24" s="9"/>
+      <c r="CE24" s="11">
+        <v>0.31928480204340454</v>
+      </c>
+      <c r="CF24" s="11"/>
+      <c r="CG24" s="11"/>
       <c r="CH24" s="9"/>
       <c r="CI24" s="9"/>
       <c r="CJ24" s="9"/>
@@ -35432,9 +34849,11 @@
       <c r="CD25" s="10">
         <v>1.4239333381965937E-14</v>
       </c>
-      <c r="CE25" s="9"/>
-      <c r="CF25" s="9"/>
-      <c r="CG25" s="9"/>
+      <c r="CE25" s="11">
+        <v>-0.38610038610037789</v>
+      </c>
+      <c r="CF25" s="11"/>
+      <c r="CG25" s="11"/>
       <c r="CH25" s="9"/>
       <c r="CI25" s="9"/>
       <c r="CJ25" s="9"/>
@@ -35693,9 +35112,11 @@
       <c r="CD26" s="10">
         <v>3.2085561497326176</v>
       </c>
-      <c r="CE26" s="9"/>
-      <c r="CF26" s="9"/>
-      <c r="CG26" s="9"/>
+      <c r="CE26" s="11">
+        <v>2.5944469731452058</v>
+      </c>
+      <c r="CF26" s="11"/>
+      <c r="CG26" s="11"/>
       <c r="CH26" s="9"/>
       <c r="CI26" s="9"/>
       <c r="CJ26" s="9"/>
@@ -35954,9 +35375,11 @@
       <c r="CD27" s="10">
         <v>0.63775510204081631</v>
       </c>
-      <c r="CE27" s="9"/>
-      <c r="CF27" s="9"/>
-      <c r="CG27" s="9"/>
+      <c r="CE27" s="11">
+        <v>0.52974735126323669</v>
+      </c>
+      <c r="CF27" s="11"/>
+      <c r="CG27" s="11"/>
       <c r="CH27" s="9"/>
       <c r="CI27" s="9"/>
       <c r="CJ27" s="9"/>
@@ -36213,11 +35636,13 @@
         <v>4.5062695924765119</v>
       </c>
       <c r="CD28" s="10">
-        <v>1.9601644008852319</v>
-      </c>
-      <c r="CE28" s="9"/>
-      <c r="CF28" s="9"/>
-      <c r="CG28" s="9"/>
+        <v>1.8653177363262832</v>
+      </c>
+      <c r="CE28" s="11">
+        <v>2.2824102251978089</v>
+      </c>
+      <c r="CF28" s="11"/>
+      <c r="CG28" s="11"/>
       <c r="CH28" s="9"/>
       <c r="CI28" s="9"/>
       <c r="CJ28" s="9"/>
@@ -36476,9 +35901,11 @@
       <c r="CD29" s="10">
         <v>-0.55555555555555269</v>
       </c>
-      <c r="CE29" s="9"/>
-      <c r="CF29" s="9"/>
-      <c r="CG29" s="9"/>
+      <c r="CE29" s="11">
+        <v>-0.14097744360902789</v>
+      </c>
+      <c r="CF29" s="11"/>
+      <c r="CG29" s="11"/>
       <c r="CH29" s="9"/>
       <c r="CI29" s="9"/>
       <c r="CJ29" s="9"/>
@@ -36737,9 +36164,11 @@
       <c r="CD30" s="10">
         <v>1.4018691588785046</v>
       </c>
-      <c r="CE30" s="9"/>
-      <c r="CF30" s="9"/>
-      <c r="CG30" s="9"/>
+      <c r="CE30" s="11">
+        <v>0.64516129032258329</v>
+      </c>
+      <c r="CF30" s="11"/>
+      <c r="CG30" s="11"/>
       <c r="CH30" s="9"/>
       <c r="CI30" s="9"/>
       <c r="CJ30" s="9"/>
@@ -36835,10 +36264,10 @@
       <c r="CA31" s="8"/>
       <c r="CB31" s="8"/>
       <c r="CC31" s="8"/>
-      <c r="CD31" s="10"/>
-      <c r="CE31" s="9"/>
-      <c r="CF31" s="9"/>
-      <c r="CG31" s="9"/>
+      <c r="CD31" s="8"/>
+      <c r="CE31" s="8"/>
+      <c r="CF31" s="11"/>
+      <c r="CG31" s="11"/>
       <c r="CH31" s="9"/>
       <c r="CI31" s="9"/>
       <c r="CJ31" s="9"/>
@@ -37097,9 +36526,11 @@
       <c r="CD32" s="10">
         <v>1.2048192771084338</v>
       </c>
-      <c r="CE32" s="9"/>
-      <c r="CF32" s="9"/>
-      <c r="CG32" s="9"/>
+      <c r="CE32" s="11">
+        <v>1.1210762331838564</v>
+      </c>
+      <c r="CF32" s="11"/>
+      <c r="CG32" s="11"/>
       <c r="CH32" s="9"/>
       <c r="CI32" s="9"/>
       <c r="CJ32" s="9"/>
@@ -37356,11 +36787,13 @@
         <v>2.0884520884520743</v>
       </c>
       <c r="CD33" s="10">
-        <v>1.0845986984815774</v>
-      </c>
-      <c r="CE33" s="9"/>
-      <c r="CF33" s="9"/>
-      <c r="CG33" s="9"/>
+        <v>1.3015184381778928</v>
+      </c>
+      <c r="CE33" s="11">
+        <v>1.7838405036726006</v>
+      </c>
+      <c r="CF33" s="11"/>
+      <c r="CG33" s="11"/>
       <c r="CH33" s="9"/>
       <c r="CI33" s="9"/>
       <c r="CJ33" s="9"/>
@@ -37617,11 +37050,13 @@
         <v>4.5385779122541612</v>
       </c>
       <c r="CD34" s="10">
-        <v>4.5811518324607325</v>
-      </c>
-      <c r="CE34" s="9"/>
-      <c r="CF34" s="9"/>
-      <c r="CG34" s="9"/>
+        <v>1.8324607329842819</v>
+      </c>
+      <c r="CE34" s="11">
+        <v>-1.4248704663212546</v>
+      </c>
+      <c r="CF34" s="11"/>
+      <c r="CG34" s="11"/>
       <c r="CH34" s="9"/>
       <c r="CI34" s="9"/>
       <c r="CJ34" s="9"/>
@@ -37878,11 +37313,13 @@
         <v>4.0935672514619839</v>
       </c>
       <c r="CD35" s="10">
-        <v>-3.8461538461538547</v>
-      </c>
-      <c r="CE35" s="9"/>
-      <c r="CF35" s="9"/>
-      <c r="CG35" s="9"/>
+        <v>-3.6324786324786533</v>
+      </c>
+      <c r="CE35" s="11">
+        <v>-3.4482758620689711</v>
+      </c>
+      <c r="CF35" s="11"/>
+      <c r="CG35" s="11"/>
       <c r="CH35" s="9"/>
       <c r="CI35" s="9"/>
       <c r="CJ35" s="9"/>
@@ -38141,9 +37578,11 @@
       <c r="CD36" s="10">
         <v>-0.1019714479945654</v>
       </c>
-      <c r="CE36" s="9"/>
-      <c r="CF36" s="9"/>
-      <c r="CG36" s="9"/>
+      <c r="CE36" s="11">
+        <v>-1.1176653213287868</v>
+      </c>
+      <c r="CF36" s="11"/>
+      <c r="CG36" s="11"/>
       <c r="CH36" s="9"/>
       <c r="CI36" s="9"/>
       <c r="CJ36" s="9"/>
@@ -38400,11 +37839,13 @@
         <v>-1.1283497884344307</v>
       </c>
       <c r="CD37" s="10">
-        <v>-2.3166023166023129</v>
-      </c>
-      <c r="CE37" s="9"/>
-      <c r="CF37" s="9"/>
-      <c r="CG37" s="9"/>
+        <v>-2.1879021879021914</v>
+      </c>
+      <c r="CE37" s="11">
+        <v>-1.3871374527112337</v>
+      </c>
+      <c r="CF37" s="11"/>
+      <c r="CG37" s="11"/>
       <c r="CH37" s="9"/>
       <c r="CI37" s="9"/>
       <c r="CJ37" s="9"/>
@@ -38663,9 +38104,11 @@
       <c r="CD38" s="10">
         <v>0.71045153141774553</v>
       </c>
-      <c r="CE38" s="9"/>
-      <c r="CF38" s="9"/>
-      <c r="CG38" s="9"/>
+      <c r="CE38" s="11">
+        <v>0.58104886769963904</v>
+      </c>
+      <c r="CF38" s="11"/>
+      <c r="CG38" s="11"/>
       <c r="CH38" s="9"/>
       <c r="CI38" s="9"/>
       <c r="CJ38" s="9"/>
@@ -38924,9 +38367,11 @@
       <c r="CD39" s="10">
         <v>-0.36188178528348774</v>
       </c>
-      <c r="CE39" s="9"/>
-      <c r="CF39" s="9"/>
-      <c r="CG39" s="9"/>
+      <c r="CE39" s="11">
+        <v>-0.11816838995568013</v>
+      </c>
+      <c r="CF39" s="11"/>
+      <c r="CG39" s="11"/>
       <c r="CH39" s="9"/>
       <c r="CI39" s="9"/>
       <c r="CJ39" s="9"/>
@@ -39185,9 +38630,11 @@
       <c r="CD40" s="10">
         <v>0.54945054945055727</v>
       </c>
-      <c r="CE40" s="9"/>
-      <c r="CF40" s="9"/>
-      <c r="CG40" s="9"/>
+      <c r="CE40" s="11">
+        <v>1.0389610389610353</v>
+      </c>
+      <c r="CF40" s="11"/>
+      <c r="CG40" s="11"/>
       <c r="CH40" s="9"/>
       <c r="CI40" s="9"/>
       <c r="CJ40" s="9"/>
@@ -39444,11 +38891,13 @@
         <v>1.9236290554120146</v>
       </c>
       <c r="CD41" s="10">
-        <v>0.95115681233932869</v>
-      </c>
-      <c r="CE41" s="9"/>
-      <c r="CF41" s="9"/>
-      <c r="CG41" s="9"/>
+        <v>0.8226221079691487</v>
+      </c>
+      <c r="CE41" s="11">
+        <v>2.5589563472152506</v>
+      </c>
+      <c r="CF41" s="11"/>
+      <c r="CG41" s="11"/>
       <c r="CH41" s="9"/>
       <c r="CI41" s="9"/>
       <c r="CJ41" s="9"/>
@@ -39707,9 +39156,11 @@
       <c r="CD42" s="10">
         <v>-0.69060773480662974</v>
       </c>
-      <c r="CE42" s="9"/>
-      <c r="CF42" s="9"/>
-      <c r="CG42" s="9"/>
+      <c r="CE42" s="11">
+        <v>-0.60362173038229761</v>
+      </c>
+      <c r="CF42" s="11"/>
+      <c r="CG42" s="11"/>
       <c r="CH42" s="9"/>
       <c r="CI42" s="9"/>
       <c r="CJ42" s="9"/>
@@ -39966,11 +39417,13 @@
         <v>1.0357815442561285</v>
       </c>
       <c r="CD43" s="10">
-        <v>-2.9814665592264329</v>
-      </c>
-      <c r="CE43" s="9"/>
-      <c r="CF43" s="9"/>
-      <c r="CG43" s="9"/>
+        <v>-1.3698630136986325</v>
+      </c>
+      <c r="CE43" s="11">
+        <v>0.93323761665471017</v>
+      </c>
+      <c r="CF43" s="11"/>
+      <c r="CG43" s="11"/>
       <c r="CH43" s="9"/>
       <c r="CI43" s="9"/>
       <c r="CJ43" s="9"/>
@@ -40227,11 +39680,13 @@
         <v>2.3508137432188065</v>
       </c>
       <c r="CD44" s="10">
-        <v>0.65809153454980218</v>
-      </c>
-      <c r="CE44" s="9"/>
-      <c r="CF44" s="9"/>
-      <c r="CG44" s="9"/>
+        <v>0.71791803769069018</v>
+      </c>
+      <c r="CE44" s="11">
+        <v>0.81704114385758797</v>
+      </c>
+      <c r="CF44" s="11"/>
+      <c r="CG44" s="11"/>
       <c r="CH44" s="9"/>
       <c r="CI44" s="9"/>
       <c r="CJ44" s="9"/>
@@ -40490,9 +39945,11 @@
       <c r="CD45" s="10">
         <v>-0.7575757575757549</v>
       </c>
-      <c r="CE45" s="9"/>
-      <c r="CF45" s="9"/>
-      <c r="CG45" s="9"/>
+      <c r="CE45" s="11">
+        <v>-0.71174377224199037</v>
+      </c>
+      <c r="CF45" s="11"/>
+      <c r="CG45" s="11"/>
       <c r="CH45" s="9"/>
       <c r="CI45" s="9"/>
       <c r="CJ45" s="9"/>
@@ -40749,11 +40206,13 @@
         <v>0.86206896551723</v>
       </c>
       <c r="CD46" s="10">
-        <v>0.67319461444308093</v>
-      </c>
-      <c r="CE46" s="9"/>
-      <c r="CF46" s="9"/>
-      <c r="CG46" s="9"/>
+        <v>0.61199510403916768</v>
+      </c>
+      <c r="CE46" s="11">
+        <v>1.386377335744414</v>
+      </c>
+      <c r="CF46" s="11"/>
+      <c r="CG46" s="11"/>
       <c r="CH46" s="9"/>
       <c r="CI46" s="9"/>
       <c r="CJ46" s="9"/>
@@ -41010,11 +40469,13 @@
         <v>-0.34602076124567965</v>
       </c>
       <c r="CD47" s="10">
-        <v>-0.82644628099172779</v>
-      </c>
-      <c r="CE47" s="9"/>
-      <c r="CF47" s="9"/>
-      <c r="CG47" s="9"/>
+        <v>-0.2754820936638962</v>
+      </c>
+      <c r="CE47" s="11">
+        <v>0.26455026455026831</v>
+      </c>
+      <c r="CF47" s="11"/>
+      <c r="CG47" s="11"/>
       <c r="CH47" s="9"/>
       <c r="CI47" s="9"/>
       <c r="CJ47" s="9"/>
@@ -41271,11 +40732,13 @@
         <v>1.2134583563154928</v>
       </c>
       <c r="CD48" s="10">
-        <v>0.919651500484016</v>
-      </c>
-      <c r="CE48" s="9"/>
-      <c r="CF48" s="9"/>
-      <c r="CG48" s="9"/>
+        <v>0.82284607938042598</v>
+      </c>
+      <c r="CE48" s="11">
+        <v>1.092636579572452</v>
+      </c>
+      <c r="CF48" s="11"/>
+      <c r="CG48" s="11"/>
       <c r="CH48" s="9"/>
       <c r="CI48" s="9"/>
       <c r="CJ48" s="9"/>
@@ -41534,9 +40997,11 @@
       <c r="CD49" s="10">
         <v>0.32982134677051184</v>
       </c>
-      <c r="CE49" s="9"/>
-      <c r="CF49" s="9"/>
-      <c r="CG49" s="9"/>
+      <c r="CE49" s="11">
+        <v>0.4847096148761787</v>
+      </c>
+      <c r="CF49" s="11"/>
+      <c r="CG49" s="11"/>
       <c r="CH49" s="9"/>
       <c r="CI49" s="9"/>
       <c r="CJ49" s="9"/>
@@ -41793,11 +41258,13 @@
         <v>-2.0853080568720408</v>
       </c>
       <c r="CD50" s="10">
-        <v>0.24429967426709867</v>
-      </c>
-      <c r="CE50" s="9"/>
-      <c r="CF50" s="9"/>
-      <c r="CG50" s="9"/>
+        <v>-8.1433224755707273E-2</v>
+      </c>
+      <c r="CE50" s="11">
+        <v>0.31520882584712817</v>
+      </c>
+      <c r="CF50" s="11"/>
+      <c r="CG50" s="11"/>
       <c r="CH50" s="9"/>
       <c r="CI50" s="9"/>
       <c r="CJ50" s="9"/>
@@ -42056,9 +41523,11 @@
       <c r="CD51" s="10">
         <v>-3.3846153846153779</v>
       </c>
-      <c r="CE51" s="9"/>
-      <c r="CF51" s="9"/>
-      <c r="CG51" s="9"/>
+      <c r="CE51" s="11">
+        <v>-5.3824362606232254</v>
+      </c>
+      <c r="CF51" s="11"/>
+      <c r="CG51" s="11"/>
       <c r="CH51" s="9"/>
       <c r="CI51" s="9"/>
       <c r="CJ51" s="9"/>
@@ -42315,11 +41784,13 @@
         <v>-1.1490125673249509</v>
       </c>
       <c r="CD52" s="10">
-        <v>-1.4344915524386357</v>
-      </c>
-      <c r="CE52" s="9"/>
-      <c r="CF52" s="9"/>
-      <c r="CG52" s="9"/>
+        <v>-3.4427797258527293</v>
+      </c>
+      <c r="CE52" s="11">
+        <v>-1.9873817034700352</v>
+      </c>
+      <c r="CF52" s="11"/>
+      <c r="CG52" s="11"/>
       <c r="CH52" s="9"/>
       <c r="CI52" s="9"/>
       <c r="CJ52" s="9"/>
@@ -42576,11 +42047,13 @@
         <v>0.75690115761354282</v>
       </c>
       <c r="CD53" s="10">
-        <v>-1.4297385620914917</v>
-      </c>
-      <c r="CE53" s="9"/>
-      <c r="CF53" s="9"/>
-      <c r="CG53" s="9"/>
+        <v>-1.2254901960784199</v>
+      </c>
+      <c r="CE53" s="11">
+        <v>-0.52651372696501597</v>
+      </c>
+      <c r="CF53" s="11"/>
+      <c r="CG53" s="11"/>
       <c r="CH53" s="9"/>
       <c r="CI53" s="9"/>
       <c r="CJ53" s="9"/>
@@ -42839,9 +42312,11 @@
       <c r="CD54" s="10">
         <v>-1.2861736334405212</v>
       </c>
-      <c r="CE54" s="9"/>
-      <c r="CF54" s="9"/>
-      <c r="CG54" s="9"/>
+      <c r="CE54" s="11">
+        <v>-0.9202453987729976</v>
+      </c>
+      <c r="CF54" s="11"/>
+      <c r="CG54" s="11"/>
       <c r="CH54" s="9"/>
       <c r="CI54" s="9"/>
       <c r="CJ54" s="9"/>
@@ -43098,11 +42573,13 @@
         <v>-1.3142174432497113</v>
       </c>
       <c r="CD55" s="10">
-        <v>-2.3073146784487073</v>
-      </c>
-      <c r="CE55" s="9"/>
-      <c r="CF55" s="9"/>
-      <c r="CG55" s="9"/>
+        <v>-2.503681885125181</v>
+      </c>
+      <c r="CE55" s="11">
+        <v>-0.13818516812528003</v>
+      </c>
+      <c r="CF55" s="11"/>
+      <c r="CG55" s="11"/>
       <c r="CH55" s="9"/>
       <c r="CI55" s="9"/>
       <c r="CJ55" s="9"/>
@@ -43361,9 +42838,11 @@
       <c r="CD56" s="10">
         <v>-0.33670033670034144</v>
       </c>
-      <c r="CE56" s="9"/>
-      <c r="CF56" s="9"/>
-      <c r="CG56" s="9"/>
+      <c r="CE56" s="11">
+        <v>-0.64102564102563875</v>
+      </c>
+      <c r="CF56" s="11"/>
+      <c r="CG56" s="11"/>
       <c r="CH56" s="9"/>
       <c r="CI56" s="9"/>
       <c r="CJ56" s="9"/>

</xml_diff>

<commit_message>
March 2020 Employment and earnings data update
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\aboddupalli\Box Sync\TPC\CENTER\SLFI\Interactive Data Tools\SEM\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EHuffer\Box Sync\TPC\CENTER\SLFI\Interactive Data Tools\SEM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE_1" sheetId="5" r:id="rId1"/>
@@ -856,7 +856,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1562,11 +1562,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:MG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="CW11" sqref="CW11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,6 +1875,9 @@
       <c r="CT4" s="4">
         <v>43831</v>
       </c>
+      <c r="CU4" s="4">
+        <v>43862</v>
+      </c>
     </row>
     <row r="5" spans="1:345" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -2171,7 +2174,9 @@
       <c r="CT5" s="6">
         <v>10568.6</v>
       </c>
-      <c r="CU5" s="6"/>
+      <c r="CU5" s="6">
+        <v>10978.3</v>
+      </c>
       <c r="CV5" s="6"/>
       <c r="CW5" s="6"/>
       <c r="CX5" s="6"/>
@@ -2712,9 +2717,11 @@
         <v>169.3</v>
       </c>
       <c r="CT6" s="6">
-        <v>166.60000000000002</v>
-      </c>
-      <c r="CU6" s="6"/>
+        <v>166.5</v>
+      </c>
+      <c r="CU6" s="6">
+        <v>169.6</v>
+      </c>
       <c r="CV6" s="6"/>
       <c r="CW6" s="6"/>
       <c r="CX6" s="6"/>
@@ -3255,9 +3262,11 @@
         <v>29.900000000000002</v>
       </c>
       <c r="CT7" s="6">
-        <v>29.700000000000003</v>
-      </c>
-      <c r="CU7" s="6"/>
+        <v>29.3</v>
+      </c>
+      <c r="CU7" s="6">
+        <v>30.599999999999998</v>
+      </c>
       <c r="CV7" s="6"/>
       <c r="CW7" s="6"/>
       <c r="CX7" s="6"/>
@@ -3798,9 +3807,11 @@
         <v>209.7</v>
       </c>
       <c r="CT8" s="6">
-        <v>206.10000000000002</v>
-      </c>
-      <c r="CU8" s="6"/>
+        <v>206.2</v>
+      </c>
+      <c r="CU8" s="6">
+        <v>212.7</v>
+      </c>
       <c r="CV8" s="6"/>
       <c r="CW8" s="6"/>
       <c r="CX8" s="6"/>
@@ -4343,7 +4354,9 @@
       <c r="CT9" s="6">
         <v>98.899999999999991</v>
       </c>
-      <c r="CU9" s="6"/>
+      <c r="CU9" s="6">
+        <v>101.1</v>
+      </c>
       <c r="CV9" s="6"/>
       <c r="CW9" s="6"/>
       <c r="CX9" s="6"/>
@@ -4884,9 +4897,11 @@
         <v>1298.6999999999998</v>
       </c>
       <c r="CT10" s="6">
-        <v>1275.5999999999999</v>
-      </c>
-      <c r="CU10" s="6"/>
+        <v>1277.9000000000001</v>
+      </c>
+      <c r="CU10" s="6">
+        <v>1293.9000000000001</v>
+      </c>
       <c r="CV10" s="6"/>
       <c r="CW10" s="6"/>
       <c r="CX10" s="6"/>
@@ -5427,9 +5442,11 @@
         <v>231.6</v>
       </c>
       <c r="CT11" s="6">
-        <v>219.8</v>
-      </c>
-      <c r="CU11" s="6"/>
+        <v>219.3</v>
+      </c>
+      <c r="CU11" s="6">
+        <v>232.3</v>
+      </c>
       <c r="CV11" s="6"/>
       <c r="CW11" s="6"/>
       <c r="CX11" s="6"/>
@@ -5972,7 +5989,9 @@
       <c r="CT12" s="6">
         <v>122.6</v>
       </c>
-      <c r="CU12" s="6"/>
+      <c r="CU12" s="6">
+        <v>128.80000000000001</v>
+      </c>
       <c r="CV12" s="6"/>
       <c r="CW12" s="6"/>
       <c r="CX12" s="6"/>
@@ -6513,9 +6532,11 @@
         <v>37.099999999999994</v>
       </c>
       <c r="CT13" s="6">
-        <v>35.1</v>
-      </c>
-      <c r="CU13" s="6"/>
+        <v>34.700000000000003</v>
+      </c>
+      <c r="CU13" s="6">
+        <v>35.799999999999997</v>
+      </c>
       <c r="CV13" s="6"/>
       <c r="CW13" s="6"/>
       <c r="CX13" s="6"/>
@@ -6864,7 +6885,7 @@
       <c r="CR14" s="8"/>
       <c r="CS14" s="8"/>
       <c r="CT14" s="8"/>
-      <c r="CU14" s="6"/>
+      <c r="CU14" s="8"/>
       <c r="CV14" s="6"/>
       <c r="CW14" s="6"/>
       <c r="CX14" s="6"/>
@@ -7405,9 +7426,11 @@
         <v>510.5</v>
       </c>
       <c r="CT15" s="6">
-        <v>510.29999999999995</v>
-      </c>
-      <c r="CU15" s="6"/>
+        <v>510.2</v>
+      </c>
+      <c r="CU15" s="6">
+        <v>519.1</v>
+      </c>
       <c r="CV15" s="6"/>
       <c r="CW15" s="6"/>
       <c r="CX15" s="6"/>
@@ -7948,9 +7971,11 @@
         <v>349.6</v>
       </c>
       <c r="CT16" s="6">
-        <v>344.9</v>
-      </c>
-      <c r="CU16" s="6"/>
+        <v>345</v>
+      </c>
+      <c r="CU16" s="6">
+        <v>350.9</v>
+      </c>
       <c r="CV16" s="6"/>
       <c r="CW16" s="6"/>
       <c r="CX16" s="6"/>
@@ -8299,7 +8324,7 @@
       <c r="CR17" s="8"/>
       <c r="CS17" s="8"/>
       <c r="CT17" s="8"/>
-      <c r="CU17" s="6"/>
+      <c r="CU17" s="8"/>
       <c r="CV17" s="6"/>
       <c r="CW17" s="6"/>
       <c r="CX17" s="6"/>
@@ -8840,9 +8865,11 @@
         <v>63.9</v>
       </c>
       <c r="CT18" s="6">
-        <v>60.900000000000006</v>
-      </c>
-      <c r="CU18" s="6"/>
+        <v>60.699999999999996</v>
+      </c>
+      <c r="CU18" s="6">
+        <v>63.7</v>
+      </c>
       <c r="CV18" s="6"/>
       <c r="CW18" s="6"/>
       <c r="CX18" s="6"/>
@@ -9385,7 +9412,9 @@
       <c r="CT19" s="6">
         <v>437.3</v>
       </c>
-      <c r="CU19" s="6"/>
+      <c r="CU19" s="6">
+        <v>457.6</v>
+      </c>
       <c r="CV19" s="6"/>
       <c r="CW19" s="6"/>
       <c r="CX19" s="6"/>
@@ -9926,9 +9955,11 @@
         <v>243.3</v>
       </c>
       <c r="CT20" s="6">
-        <v>233.7</v>
-      </c>
-      <c r="CU20" s="6"/>
+        <v>236</v>
+      </c>
+      <c r="CU20" s="6">
+        <v>243.7</v>
+      </c>
       <c r="CV20" s="6"/>
       <c r="CW20" s="6"/>
       <c r="CX20" s="6"/>
@@ -10469,9 +10500,11 @@
         <v>149.10000000000002</v>
       </c>
       <c r="CT21" s="6">
-        <v>144.10000000000002</v>
-      </c>
-      <c r="CU21" s="6"/>
+        <v>145</v>
+      </c>
+      <c r="CU21" s="6">
+        <v>150</v>
+      </c>
       <c r="CV21" s="6"/>
       <c r="CW21" s="6"/>
       <c r="CX21" s="6"/>
@@ -11012,9 +11045,11 @@
         <v>141.1</v>
       </c>
       <c r="CT22" s="6">
-        <v>134.1</v>
-      </c>
-      <c r="CU22" s="6"/>
+        <v>134.4</v>
+      </c>
+      <c r="CU22" s="6">
+        <v>140.5</v>
+      </c>
       <c r="CV22" s="6"/>
       <c r="CW22" s="6"/>
       <c r="CX22" s="6"/>
@@ -11557,7 +11592,9 @@
       <c r="CT23" s="6">
         <v>159.9</v>
       </c>
-      <c r="CU23" s="6"/>
+      <c r="CU23" s="6">
+        <v>164.3</v>
+      </c>
       <c r="CV23" s="6"/>
       <c r="CW23" s="6"/>
       <c r="CX23" s="6"/>
@@ -12100,7 +12137,9 @@
       <c r="CT24" s="6">
         <v>150.19999999999999</v>
       </c>
-      <c r="CU24" s="6"/>
+      <c r="CU24" s="6">
+        <v>155.6</v>
+      </c>
       <c r="CV24" s="6"/>
       <c r="CW24" s="6"/>
       <c r="CX24" s="6"/>
@@ -12643,7 +12682,9 @@
       <c r="CT25" s="6">
         <v>49.599999999999994</v>
       </c>
-      <c r="CU25" s="6"/>
+      <c r="CU25" s="6">
+        <v>51.1</v>
+      </c>
       <c r="CV25" s="6"/>
       <c r="CW25" s="6"/>
       <c r="CX25" s="6"/>
@@ -13186,7 +13227,9 @@
       <c r="CT26" s="6">
         <v>198.4</v>
       </c>
-      <c r="CU26" s="6"/>
+      <c r="CU26" s="6">
+        <v>212.9</v>
+      </c>
       <c r="CV26" s="6"/>
       <c r="CW26" s="6"/>
       <c r="CX26" s="6"/>
@@ -13729,7 +13772,9 @@
       <c r="CT27" s="6">
         <v>235.3</v>
       </c>
-      <c r="CU27" s="6"/>
+      <c r="CU27" s="6">
+        <v>249.5</v>
+      </c>
       <c r="CV27" s="6"/>
       <c r="CW27" s="6"/>
       <c r="CX27" s="6"/>
@@ -14270,9 +14315,11 @@
         <v>335.4</v>
       </c>
       <c r="CT28" s="6">
-        <v>314</v>
-      </c>
-      <c r="CU28" s="6"/>
+        <v>315.39999999999998</v>
+      </c>
+      <c r="CU28" s="6">
+        <v>332.20000000000005</v>
+      </c>
       <c r="CV28" s="6"/>
       <c r="CW28" s="6"/>
       <c r="CX28" s="6"/>
@@ -14813,9 +14860,11 @@
         <v>209</v>
       </c>
       <c r="CT29" s="6">
-        <v>209</v>
-      </c>
-      <c r="CU29" s="6"/>
+        <v>209.10000000000002</v>
+      </c>
+      <c r="CU29" s="6">
+        <v>214.5</v>
+      </c>
       <c r="CV29" s="6"/>
       <c r="CW29" s="6"/>
       <c r="CX29" s="6"/>
@@ -15358,7 +15407,9 @@
       <c r="CT30" s="6">
         <v>104.4</v>
       </c>
-      <c r="CU30" s="6"/>
+      <c r="CU30" s="6">
+        <v>108</v>
+      </c>
       <c r="CV30" s="6"/>
       <c r="CW30" s="6"/>
       <c r="CX30" s="6"/>
@@ -15707,7 +15758,7 @@
       <c r="CR31" s="8"/>
       <c r="CS31" s="8"/>
       <c r="CT31" s="8"/>
-      <c r="CU31" s="6"/>
+      <c r="CU31" s="8"/>
       <c r="CV31" s="6"/>
       <c r="CW31" s="6"/>
       <c r="CX31" s="6"/>
@@ -16250,7 +16301,9 @@
       <c r="CT32" s="6">
         <v>43.599999999999994</v>
       </c>
-      <c r="CU32" s="6"/>
+      <c r="CU32" s="6">
+        <v>45.1</v>
+      </c>
       <c r="CV32" s="6"/>
       <c r="CW32" s="6"/>
       <c r="CX32" s="6"/>
@@ -16793,7 +16846,9 @@
       <c r="CT33" s="6">
         <v>93.8</v>
       </c>
-      <c r="CU33" s="6"/>
+      <c r="CU33" s="6">
+        <v>95</v>
+      </c>
       <c r="CV33" s="6"/>
       <c r="CW33" s="6"/>
       <c r="CX33" s="6"/>
@@ -17336,7 +17391,9 @@
       <c r="CT34" s="6">
         <v>74.8</v>
       </c>
-      <c r="CU34" s="6"/>
+      <c r="CU34" s="6">
+        <v>80.900000000000006</v>
+      </c>
       <c r="CV34" s="6"/>
       <c r="CW34" s="6"/>
       <c r="CX34" s="6"/>
@@ -17877,9 +17934,11 @@
         <v>49.9</v>
       </c>
       <c r="CT35" s="6">
-        <v>45.1</v>
-      </c>
-      <c r="CU35" s="6"/>
+        <v>44.9</v>
+      </c>
+      <c r="CU35" s="6">
+        <v>49.9</v>
+      </c>
       <c r="CV35" s="6"/>
       <c r="CW35" s="6"/>
       <c r="CX35" s="6"/>
@@ -18422,7 +18481,9 @@
       <c r="CT36" s="6">
         <v>314.89999999999998</v>
       </c>
-      <c r="CU36" s="6"/>
+      <c r="CU36" s="6">
+        <v>323.3</v>
+      </c>
       <c r="CV36" s="6"/>
       <c r="CW36" s="6"/>
       <c r="CX36" s="6"/>
@@ -18963,9 +19024,11 @@
         <v>79.400000000000006</v>
       </c>
       <c r="CT37" s="6">
-        <v>75.3</v>
-      </c>
-      <c r="CU37" s="6"/>
+        <v>75.400000000000006</v>
+      </c>
+      <c r="CU37" s="6">
+        <v>80.5</v>
+      </c>
       <c r="CV37" s="6"/>
       <c r="CW37" s="6"/>
       <c r="CX37" s="6"/>
@@ -19508,7 +19571,9 @@
       <c r="CT38" s="6">
         <v>641.1</v>
       </c>
-      <c r="CU38" s="6"/>
+      <c r="CU38" s="6">
+        <v>668.4</v>
+      </c>
       <c r="CV38" s="6"/>
       <c r="CW38" s="6"/>
       <c r="CX38" s="6"/>
@@ -20051,7 +20116,9 @@
       <c r="CT39" s="6">
         <v>329.9</v>
       </c>
-      <c r="CU39" s="6"/>
+      <c r="CU39" s="6">
+        <v>337.9</v>
+      </c>
       <c r="CV39" s="6"/>
       <c r="CW39" s="6"/>
       <c r="CX39" s="6"/>
@@ -20594,7 +20661,9 @@
       <c r="CT40" s="6">
         <v>38.200000000000003</v>
       </c>
-      <c r="CU40" s="6"/>
+      <c r="CU40" s="6">
+        <v>39</v>
+      </c>
       <c r="CV40" s="6"/>
       <c r="CW40" s="6"/>
       <c r="CX40" s="6"/>
@@ -21135,9 +21204,11 @@
         <v>401.5</v>
       </c>
       <c r="CT41" s="6">
-        <v>374.2</v>
-      </c>
-      <c r="CU41" s="6"/>
+        <v>382.5</v>
+      </c>
+      <c r="CU41" s="6">
+        <v>402.79999999999995</v>
+      </c>
       <c r="CV41" s="6"/>
       <c r="CW41" s="6"/>
       <c r="CX41" s="6"/>
@@ -21680,7 +21751,9 @@
       <c r="CT42" s="6">
         <v>145.5</v>
       </c>
-      <c r="CU42" s="6"/>
+      <c r="CU42" s="6">
+        <v>153.30000000000001</v>
+      </c>
       <c r="CV42" s="6"/>
       <c r="CW42" s="6"/>
       <c r="CX42" s="6"/>
@@ -22221,9 +22294,11 @@
         <v>143.80000000000001</v>
       </c>
       <c r="CT43" s="6">
-        <v>141.20000000000002</v>
-      </c>
-      <c r="CU43" s="6"/>
+        <v>141.30000000000001</v>
+      </c>
+      <c r="CU43" s="6">
+        <v>144.9</v>
+      </c>
       <c r="CV43" s="6"/>
       <c r="CW43" s="6"/>
       <c r="CX43" s="6"/>
@@ -22764,9 +22839,11 @@
         <v>342</v>
       </c>
       <c r="CT44" s="6">
-        <v>325.5</v>
-      </c>
-      <c r="CU44" s="6"/>
+        <v>325.7</v>
+      </c>
+      <c r="CU44" s="6">
+        <v>346.09999999999997</v>
+      </c>
       <c r="CV44" s="6"/>
       <c r="CW44" s="6"/>
       <c r="CX44" s="6"/>
@@ -23309,7 +23386,9 @@
       <c r="CT45" s="6">
         <v>30.7</v>
       </c>
-      <c r="CU45" s="6"/>
+      <c r="CU45" s="6">
+        <v>30.8</v>
+      </c>
       <c r="CV45" s="6"/>
       <c r="CW45" s="6"/>
       <c r="CX45" s="6"/>
@@ -23850,9 +23929,11 @@
         <v>168.3</v>
       </c>
       <c r="CT46" s="6">
-        <v>165.10000000000002</v>
-      </c>
-      <c r="CU46" s="6"/>
+        <v>165.2</v>
+      </c>
+      <c r="CU46" s="6">
+        <v>167.8</v>
+      </c>
       <c r="CV46" s="6"/>
       <c r="CW46" s="6"/>
       <c r="CX46" s="6"/>
@@ -24393,9 +24474,11 @@
         <v>38</v>
       </c>
       <c r="CT47" s="6">
-        <v>36.700000000000003</v>
-      </c>
-      <c r="CU47" s="6"/>
+        <v>36.299999999999997</v>
+      </c>
+      <c r="CU47" s="6">
+        <v>37.5</v>
+      </c>
       <c r="CV47" s="6"/>
       <c r="CW47" s="6"/>
       <c r="CX47" s="6"/>
@@ -24936,9 +25019,11 @@
         <v>206</v>
       </c>
       <c r="CT48" s="6">
-        <v>198.8</v>
-      </c>
-      <c r="CU48" s="6"/>
+        <v>198</v>
+      </c>
+      <c r="CU48" s="6">
+        <v>206.8</v>
+      </c>
       <c r="CV48" s="6"/>
       <c r="CW48" s="6"/>
       <c r="CX48" s="6"/>
@@ -25479,9 +25564,11 @@
         <v>1152</v>
       </c>
       <c r="CT49" s="6">
-        <v>1125</v>
-      </c>
-      <c r="CU49" s="6"/>
+        <v>1121.3</v>
+      </c>
+      <c r="CU49" s="6">
+        <v>1150.2</v>
+      </c>
       <c r="CV49" s="6"/>
       <c r="CW49" s="6"/>
       <c r="CX49" s="6"/>
@@ -26022,9 +26109,11 @@
         <v>132.1</v>
       </c>
       <c r="CT50" s="6">
-        <v>128.30000000000001</v>
-      </c>
-      <c r="CU50" s="6"/>
+        <v>129.30000000000001</v>
+      </c>
+      <c r="CU50" s="6">
+        <v>132.6</v>
+      </c>
       <c r="CV50" s="6"/>
       <c r="CW50" s="6"/>
       <c r="CX50" s="6"/>
@@ -26567,7 +26656,9 @@
       <c r="CT51" s="6">
         <v>32</v>
       </c>
-      <c r="CU51" s="6"/>
+      <c r="CU51" s="6">
+        <v>34.900000000000006</v>
+      </c>
       <c r="CV51" s="6"/>
       <c r="CW51" s="6"/>
       <c r="CX51" s="6"/>
@@ -27108,9 +27199,11 @@
         <v>321.5</v>
       </c>
       <c r="CT52" s="6">
-        <v>311.39999999999998</v>
-      </c>
-      <c r="CU52" s="6"/>
+        <v>311.5</v>
+      </c>
+      <c r="CU52" s="6">
+        <v>323.60000000000002</v>
+      </c>
       <c r="CV52" s="6"/>
       <c r="CW52" s="6"/>
       <c r="CX52" s="6"/>
@@ -27651,9 +27744,11 @@
         <v>263</v>
       </c>
       <c r="CT53" s="6">
-        <v>266.2</v>
-      </c>
-      <c r="CU53" s="6"/>
+        <v>268.39999999999998</v>
+      </c>
+      <c r="CU53" s="6">
+        <v>269.89999999999998</v>
+      </c>
       <c r="CV53" s="6"/>
       <c r="CW53" s="6"/>
       <c r="CX53" s="6"/>
@@ -28196,7 +28291,9 @@
       <c r="CT54" s="6">
         <v>61.099999999999994</v>
       </c>
-      <c r="CU54" s="6"/>
+      <c r="CU54" s="6">
+        <v>63.1</v>
+      </c>
       <c r="CV54" s="6"/>
       <c r="CW54" s="6"/>
       <c r="CX54" s="6"/>
@@ -28737,9 +28834,11 @@
         <v>219.5</v>
       </c>
       <c r="CT55" s="6">
-        <v>202.10000000000002</v>
-      </c>
-      <c r="CU55" s="6"/>
+        <v>202.39999999999998</v>
+      </c>
+      <c r="CU55" s="6">
+        <v>219.70000000000002</v>
+      </c>
       <c r="CV55" s="6"/>
       <c r="CW55" s="6"/>
       <c r="CX55" s="6"/>
@@ -29280,9 +29379,11 @@
         <v>31</v>
       </c>
       <c r="CT56" s="6">
-        <v>29.4</v>
-      </c>
-      <c r="CU56" s="6"/>
+        <v>29.200000000000003</v>
+      </c>
+      <c r="CU56" s="6">
+        <v>30.4</v>
+      </c>
       <c r="CV56" s="6"/>
       <c r="CW56" s="6"/>
       <c r="CX56" s="6"/>
@@ -29540,11 +29641,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CQ56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="CC5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="CK53" sqref="CK53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29868,7 +29969,9 @@
       <c r="CH4" s="4">
         <v>43831</v>
       </c>
-      <c r="CI4" s="9"/>
+      <c r="CI4" s="4">
+        <v>43862</v>
+      </c>
       <c r="CJ4" s="9"/>
       <c r="CK4" s="9"/>
       <c r="CL4" s="9"/>
@@ -30137,7 +30240,9 @@
       <c r="CH5" s="10">
         <v>0.68401798643397127</v>
       </c>
-      <c r="CI5" s="9"/>
+      <c r="CI5" s="10">
+        <v>0.74885056943845729</v>
+      </c>
       <c r="CJ5" s="9"/>
       <c r="CK5" s="9"/>
       <c r="CL5" s="9"/>
@@ -30404,9 +30509,11 @@
         <v>0.95408467501492122</v>
       </c>
       <c r="CH6" s="10">
-        <v>1.153612629022486</v>
-      </c>
-      <c r="CI6" s="9"/>
+        <v>1.092896174863395</v>
+      </c>
+      <c r="CI6" s="10">
+        <v>1.3747758517632891</v>
+      </c>
       <c r="CJ6" s="9"/>
       <c r="CK6" s="9"/>
       <c r="CL6" s="9"/>
@@ -30673,9 +30780,11 @@
         <v>-1.6447368421052515</v>
       </c>
       <c r="CH7" s="10">
-        <v>-1.9801980198019731</v>
-      </c>
-      <c r="CI7" s="9"/>
+        <v>-3.3003300330033003</v>
+      </c>
+      <c r="CI7" s="10">
+        <v>-2.8571428571428639</v>
+      </c>
       <c r="CJ7" s="9"/>
       <c r="CK7" s="9"/>
       <c r="CL7" s="9"/>
@@ -30942,9 +31051,11 @@
         <v>3.1480570585341745</v>
       </c>
       <c r="CH8" s="10">
-        <v>2.7930174563591135</v>
-      </c>
-      <c r="CI8" s="9"/>
+        <v>2.8428927680797949</v>
+      </c>
+      <c r="CI8" s="10">
+        <v>2.6049204052098296</v>
+      </c>
       <c r="CJ8" s="9"/>
       <c r="CK8" s="9"/>
       <c r="CL8" s="9"/>
@@ -31213,7 +31324,9 @@
       <c r="CH9" s="10">
         <v>-1.9821605550049695</v>
       </c>
-      <c r="CI9" s="9"/>
+      <c r="CI9" s="10">
+        <v>-1.9398642095053347</v>
+      </c>
       <c r="CJ9" s="9"/>
       <c r="CK9" s="9"/>
       <c r="CL9" s="9"/>
@@ -31480,9 +31593,11 @@
         <v>0.67441860465114867</v>
       </c>
       <c r="CH10" s="10">
-        <v>0.71056371387967798</v>
-      </c>
-      <c r="CI10" s="9"/>
+        <v>0.89215221853783222</v>
+      </c>
+      <c r="CI10" s="10">
+        <v>0.93611046103440199</v>
+      </c>
       <c r="CJ10" s="9"/>
       <c r="CK10" s="9"/>
       <c r="CL10" s="9"/>
@@ -31749,9 +31864,11 @@
         <v>4.0898876404494358</v>
       </c>
       <c r="CH11" s="10">
-        <v>2.950819672131153</v>
-      </c>
-      <c r="CI11" s="9"/>
+        <v>2.7166276346604268</v>
+      </c>
+      <c r="CI11" s="10">
+        <v>2.9242357111209674</v>
+      </c>
       <c r="CJ11" s="9"/>
       <c r="CK11" s="9"/>
       <c r="CL11" s="9"/>
@@ -32020,7 +32137,9 @@
       <c r="CH12" s="10">
         <v>-0.32520325203252493</v>
       </c>
-      <c r="CI12" s="9"/>
+      <c r="CI12" s="10">
+        <v>0.62500000000000888</v>
+      </c>
       <c r="CJ12" s="9"/>
       <c r="CK12" s="9"/>
       <c r="CL12" s="9"/>
@@ -32287,9 +32406,11 @@
         <v>1.6438356164383405</v>
       </c>
       <c r="CH13" s="10">
-        <v>2.332361516034998</v>
-      </c>
-      <c r="CI13" s="9"/>
+        <v>1.1661807580175094</v>
+      </c>
+      <c r="CI13" s="10">
+        <v>0.84507042253520326</v>
+      </c>
       <c r="CJ13" s="9"/>
       <c r="CK13" s="9"/>
       <c r="CL13" s="9"/>
@@ -32388,7 +32509,7 @@
       <c r="CF14" s="8"/>
       <c r="CG14" s="8"/>
       <c r="CH14" s="8"/>
-      <c r="CI14" s="9"/>
+      <c r="CI14" s="8"/>
       <c r="CJ14" s="9"/>
       <c r="CK14" s="9"/>
       <c r="CL14" s="9"/>
@@ -32655,9 +32776,11 @@
         <v>-0.46792747124195311</v>
       </c>
       <c r="CH15" s="10">
-        <v>0.33425088478174042</v>
-      </c>
-      <c r="CI15" s="9"/>
+        <v>0.31458906802987924</v>
+      </c>
+      <c r="CI15" s="10">
+        <v>-7.6997112608272814E-2</v>
+      </c>
       <c r="CJ15" s="9"/>
       <c r="CK15" s="9"/>
       <c r="CL15" s="9"/>
@@ -32924,9 +33047,11 @@
         <v>-0.37047591906524785</v>
       </c>
       <c r="CH16" s="10">
-        <v>-0.14475969889982629</v>
-      </c>
-      <c r="CI16" s="9"/>
+        <v>-0.11580775911985446</v>
+      </c>
+      <c r="CI16" s="10">
+        <v>0.25714285714285062</v>
+      </c>
       <c r="CJ16" s="9"/>
       <c r="CK16" s="9"/>
       <c r="CL16" s="9"/>
@@ -33025,7 +33150,7 @@
       <c r="CF17" s="8"/>
       <c r="CG17" s="8"/>
       <c r="CH17" s="8"/>
-      <c r="CI17" s="9"/>
+      <c r="CI17" s="8"/>
       <c r="CJ17" s="9"/>
       <c r="CK17" s="9"/>
       <c r="CL17" s="9"/>
@@ -33292,9 +33417,11 @@
         <v>3.2310177705977265</v>
       </c>
       <c r="CH18" s="10">
-        <v>4.6391752577319636</v>
-      </c>
-      <c r="CI18" s="9"/>
+        <v>4.2955326460480974</v>
+      </c>
+      <c r="CI18" s="10">
+        <v>1.594896331738437</v>
+      </c>
       <c r="CJ18" s="9"/>
       <c r="CK18" s="9"/>
       <c r="CL18" s="9"/>
@@ -33563,7 +33690,9 @@
       <c r="CH19" s="10">
         <v>2.7249236551562186</v>
       </c>
-      <c r="CI19" s="9"/>
+      <c r="CI19" s="10">
+        <v>2.8083576724331611</v>
+      </c>
       <c r="CJ19" s="9"/>
       <c r="CK19" s="9"/>
       <c r="CL19" s="9"/>
@@ -33830,9 +33959,11 @@
         <v>1.1681754800823678E-14</v>
       </c>
       <c r="CH20" s="10">
-        <v>-1.6827934371055953</v>
-      </c>
-      <c r="CI20" s="9"/>
+        <v>-0.71518721076987324</v>
+      </c>
+      <c r="CI20" s="10">
+        <v>1.0364842454394694</v>
+      </c>
       <c r="CJ20" s="9"/>
       <c r="CK20" s="9"/>
       <c r="CL20" s="9"/>
@@ -34099,9 +34230,11 @@
         <v>-0.40080160320639008</v>
       </c>
       <c r="CH21" s="10">
-        <v>-0.41465100207323147</v>
-      </c>
-      <c r="CI21" s="9"/>
+        <v>0.20732550103663538</v>
+      </c>
+      <c r="CI21" s="10">
+        <v>0.8742434431741839</v>
+      </c>
       <c r="CJ21" s="9"/>
       <c r="CK21" s="9"/>
       <c r="CL21" s="9"/>
@@ -34368,9 +34501,11 @@
         <v>-0.49365303244006842</v>
       </c>
       <c r="CH22" s="10">
-        <v>1.0550113036925439</v>
-      </c>
-      <c r="CI22" s="9"/>
+        <v>1.2810851544838111</v>
+      </c>
+      <c r="CI22" s="10">
+        <v>-1.056338028169014</v>
+      </c>
       <c r="CJ22" s="9"/>
       <c r="CK22" s="9"/>
       <c r="CL22" s="9"/>
@@ -34639,7 +34774,9 @@
       <c r="CH23" s="10">
         <v>6.2578222778469528E-2</v>
       </c>
-      <c r="CI23" s="9"/>
+      <c r="CI23" s="10">
+        <v>-0.18226002430134344</v>
+      </c>
       <c r="CJ23" s="9"/>
       <c r="CK23" s="9"/>
       <c r="CL23" s="9"/>
@@ -34908,7 +35045,9 @@
       <c r="CH24" s="10">
         <v>0.67024128686327078</v>
       </c>
-      <c r="CI24" s="9"/>
+      <c r="CI24" s="10">
+        <v>0.45190445448677674</v>
+      </c>
       <c r="CJ24" s="9"/>
       <c r="CK24" s="9"/>
       <c r="CL24" s="9"/>
@@ -35177,7 +35316,9 @@
       <c r="CH25" s="10">
         <v>-0.80000000000001137</v>
       </c>
-      <c r="CI25" s="9"/>
+      <c r="CI25" s="10">
+        <v>-0.96899224806201545</v>
+      </c>
       <c r="CJ25" s="9"/>
       <c r="CK25" s="9"/>
       <c r="CL25" s="9"/>
@@ -35446,7 +35587,9 @@
       <c r="CH26" s="10">
         <v>-2.9828850855745692</v>
       </c>
-      <c r="CI26" s="9"/>
+      <c r="CI26" s="10">
+        <v>-2.3842274186153087</v>
+      </c>
       <c r="CJ26" s="9"/>
       <c r="CK26" s="9"/>
       <c r="CL26" s="9"/>
@@ -35715,7 +35858,9 @@
       <c r="CH27" s="10">
         <v>2.1267361111111134</v>
       </c>
-      <c r="CI27" s="9"/>
+      <c r="CI27" s="10">
+        <v>1.0121457489878543</v>
+      </c>
       <c r="CJ27" s="9"/>
       <c r="CK27" s="9"/>
       <c r="CL27" s="9"/>
@@ -35982,9 +36127,11 @@
         <v>1.7288444040036188</v>
       </c>
       <c r="CH28" s="10">
-        <v>0.28744809964866724</v>
-      </c>
-      <c r="CI28" s="9"/>
+        <v>0.73458958799104257</v>
+      </c>
+      <c r="CI28" s="10">
+        <v>1.2496190185918996</v>
+      </c>
       <c r="CJ28" s="9"/>
       <c r="CK28" s="9"/>
       <c r="CL28" s="9"/>
@@ -36251,9 +36398,11 @@
         <v>0.28790786948177677</v>
       </c>
       <c r="CH29" s="10">
-        <v>-4.7824007651838508E-2</v>
-      </c>
-      <c r="CI29" s="9"/>
+        <v>1.3592400492780492E-14</v>
+      </c>
+      <c r="CI29" s="10">
+        <v>1.0838831291234738</v>
+      </c>
       <c r="CJ29" s="9"/>
       <c r="CK29" s="9"/>
       <c r="CL29" s="9"/>
@@ -36522,7 +36671,9 @@
       <c r="CH30" s="10">
         <v>0.67502410800386003</v>
       </c>
-      <c r="CI30" s="9"/>
+      <c r="CI30" s="10">
+        <v>0.65237651444548261</v>
+      </c>
       <c r="CJ30" s="9"/>
       <c r="CK30" s="9"/>
       <c r="CL30" s="9"/>
@@ -36621,7 +36772,7 @@
       <c r="CF31" s="8"/>
       <c r="CG31" s="8"/>
       <c r="CH31" s="8"/>
-      <c r="CI31" s="9"/>
+      <c r="CI31" s="8"/>
       <c r="CJ31" s="9"/>
       <c r="CK31" s="9"/>
       <c r="CL31" s="9"/>
@@ -36890,7 +37041,9 @@
       <c r="CH32" s="10">
         <v>0.22988505747125129</v>
       </c>
-      <c r="CI32" s="9"/>
+      <c r="CI32" s="10">
+        <v>0.22222222222222537</v>
+      </c>
       <c r="CJ32" s="9"/>
       <c r="CK32" s="9"/>
       <c r="CL32" s="9"/>
@@ -37159,7 +37312,9 @@
       <c r="CH33" s="10">
         <v>0.10672358591248059</v>
       </c>
-      <c r="CI33" s="9"/>
+      <c r="CI33" s="10">
+        <v>0.42283298097250682</v>
+      </c>
       <c r="CJ33" s="9"/>
       <c r="CK33" s="9"/>
       <c r="CL33" s="9"/>
@@ -37428,7 +37583,9 @@
       <c r="CH34" s="10">
         <v>2.0463847203274215</v>
       </c>
-      <c r="CI34" s="9"/>
+      <c r="CI34" s="10">
+        <v>1.5056461731493134</v>
+      </c>
       <c r="CJ34" s="9"/>
       <c r="CK34" s="9"/>
       <c r="CL34" s="9"/>
@@ -37695,9 +37852,11 @@
         <v>1.4227642276422823</v>
       </c>
       <c r="CH35" s="10">
-        <v>-0.22123893805310046</v>
-      </c>
-      <c r="CI35" s="9"/>
+        <v>-0.66371681415930139</v>
+      </c>
+      <c r="CI35" s="10">
+        <v>0.80808080808080518</v>
+      </c>
       <c r="CJ35" s="9"/>
       <c r="CK35" s="9"/>
       <c r="CL35" s="9"/>
@@ -37966,7 +38125,9 @@
       <c r="CH36" s="10">
         <v>2.2734654108476779</v>
       </c>
-      <c r="CI36" s="9"/>
+      <c r="CI36" s="10">
+        <v>0.46612802983219387</v>
+      </c>
       <c r="CJ36" s="9"/>
       <c r="CK36" s="9"/>
       <c r="CL36" s="9"/>
@@ -38233,9 +38394,11 @@
         <v>0.3792667509481813</v>
       </c>
       <c r="CH37" s="10">
-        <v>-0.13262599469497152</v>
-      </c>
-      <c r="CI37" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="CI37" s="10">
+        <v>0.37406483790525114</v>
+      </c>
       <c r="CJ37" s="9"/>
       <c r="CK37" s="9"/>
       <c r="CL37" s="9"/>
@@ -38504,7 +38667,9 @@
       <c r="CH38" s="10">
         <v>0.10930668332293028</v>
       </c>
-      <c r="CI38" s="9"/>
+      <c r="CI38" s="10">
+        <v>0.11983223487117353</v>
+      </c>
       <c r="CJ38" s="9"/>
       <c r="CK38" s="9"/>
       <c r="CL38" s="9"/>
@@ -38773,7 +38938,9 @@
       <c r="CH39" s="10">
         <v>-0.54265902924329557</v>
       </c>
-      <c r="CI39" s="9"/>
+      <c r="CI39" s="10">
+        <v>-0.14775413711583926</v>
+      </c>
       <c r="CJ39" s="9"/>
       <c r="CK39" s="9"/>
       <c r="CL39" s="9"/>
@@ -39042,7 +39209,9 @@
       <c r="CH40" s="10">
         <v>0.79155672823220125</v>
       </c>
-      <c r="CI40" s="9"/>
+      <c r="CI40" s="10">
+        <v>0</v>
+      </c>
       <c r="CJ40" s="9"/>
       <c r="CK40" s="9"/>
       <c r="CL40" s="9"/>
@@ -39309,9 +39478,11 @@
         <v>-1.8577364947445667</v>
       </c>
       <c r="CH41" s="10">
-        <v>-3.6560247167868289</v>
-      </c>
-      <c r="CI41" s="9"/>
+        <v>-1.5190525231719962</v>
+      </c>
+      <c r="CI41" s="10">
+        <v>-1.3470487386725585</v>
+      </c>
       <c r="CJ41" s="9"/>
       <c r="CK41" s="9"/>
       <c r="CL41" s="9"/>
@@ -39580,7 +39751,9 @@
       <c r="CH42" s="10">
         <v>1.7482517482517483</v>
       </c>
-      <c r="CI42" s="9"/>
+      <c r="CI42" s="10">
+        <v>1.5904572564612363</v>
+      </c>
       <c r="CJ42" s="9"/>
       <c r="CK42" s="9"/>
       <c r="CL42" s="9"/>
@@ -39847,9 +40020,11 @@
         <v>2.2032693674484678</v>
       </c>
       <c r="CH43" s="10">
-        <v>2.3188405797101574</v>
-      </c>
-      <c r="CI43" s="9"/>
+        <v>2.3913043478260954</v>
+      </c>
+      <c r="CI43" s="10">
+        <v>2.7659574468085149</v>
+      </c>
       <c r="CJ43" s="9"/>
       <c r="CK43" s="9"/>
       <c r="CL43" s="9"/>
@@ -40116,9 +40291,11 @@
         <v>0.52910052910053251</v>
       </c>
       <c r="CH44" s="10">
-        <v>0.27726432532346801</v>
-      </c>
-      <c r="CI44" s="9"/>
+        <v>0.33887861983979228</v>
+      </c>
+      <c r="CI44" s="10">
+        <v>1.3469985358711467</v>
+      </c>
       <c r="CJ44" s="9"/>
       <c r="CK44" s="9"/>
       <c r="CL44" s="9"/>
@@ -40387,7 +40564,9 @@
       <c r="CH45" s="10">
         <v>-0.64724919093850908</v>
       </c>
-      <c r="CI45" s="9"/>
+      <c r="CI45" s="10">
+        <v>-0.32362459546924877</v>
+      </c>
       <c r="CJ45" s="9"/>
       <c r="CK45" s="9"/>
       <c r="CL45" s="9"/>
@@ -40654,9 +40833,11 @@
         <v>1.5078407720144751</v>
       </c>
       <c r="CH46" s="10">
-        <v>1.0403916768665955</v>
-      </c>
-      <c r="CI46" s="9"/>
+        <v>1.1015911872704913</v>
+      </c>
+      <c r="CI46" s="10">
+        <v>1.1452682338758322</v>
+      </c>
       <c r="CJ46" s="9"/>
       <c r="CK46" s="9"/>
       <c r="CL46" s="9"/>
@@ -40923,9 +41104,11 @@
         <v>0.52910052910053662</v>
       </c>
       <c r="CH47" s="10">
-        <v>0.82417582417581625</v>
-      </c>
-      <c r="CI47" s="9"/>
+        <v>-0.27472527472529812</v>
+      </c>
+      <c r="CI47" s="10">
+        <v>0</v>
+      </c>
       <c r="CJ47" s="9"/>
       <c r="CK47" s="9"/>
       <c r="CL47" s="9"/>
@@ -41192,9 +41375,11 @@
         <v>-2.0446980504041896</v>
       </c>
       <c r="CH48" s="10">
-        <v>0</v>
-      </c>
-      <c r="CI48" s="9"/>
+        <v>-0.40241448692153486</v>
+      </c>
+      <c r="CI48" s="10">
+        <v>-0.72011521843494952</v>
+      </c>
       <c r="CJ48" s="9"/>
       <c r="CK48" s="9"/>
       <c r="CL48" s="9"/>
@@ -41461,9 +41646,11 @@
         <v>1.0171869519466774</v>
       </c>
       <c r="CH49" s="10">
-        <v>1.4153069503290405</v>
-      </c>
-      <c r="CI49" s="9"/>
+        <v>1.081763274136843</v>
+      </c>
+      <c r="CI49" s="10">
+        <v>0.78864353312302837</v>
+      </c>
       <c r="CJ49" s="9"/>
       <c r="CK49" s="9"/>
       <c r="CL49" s="9"/>
@@ -41730,9 +41917,11 @@
         <v>3.7706205813039926</v>
       </c>
       <c r="CH50" s="10">
-        <v>2.8869286287089198</v>
-      </c>
-      <c r="CI50" s="9"/>
+        <v>3.688853247794726</v>
+      </c>
+      <c r="CI50" s="10">
+        <v>3.9999999999999956</v>
+      </c>
       <c r="CJ50" s="9"/>
       <c r="CK50" s="9"/>
       <c r="CL50" s="9"/>
@@ -42001,7 +42190,9 @@
       <c r="CH51" s="10">
         <v>1.9108280254777117</v>
       </c>
-      <c r="CI51" s="9"/>
+      <c r="CI51" s="10">
+        <v>2.0467836257310021</v>
+      </c>
       <c r="CJ51" s="9"/>
       <c r="CK51" s="9"/>
       <c r="CL51" s="9"/>
@@ -42268,9 +42459,11 @@
         <v>-0.15527950310559005</v>
       </c>
       <c r="CH52" s="10">
-        <v>0.1608234158893535</v>
-      </c>
-      <c r="CI52" s="9"/>
+        <v>0.19298809906723152</v>
+      </c>
+      <c r="CI52" s="10">
+        <v>-0.2466091245375939</v>
+      </c>
       <c r="CJ52" s="9"/>
       <c r="CK52" s="9"/>
       <c r="CL52" s="9"/>
@@ -42537,9 +42730,11 @@
         <v>0.38167938931297712</v>
       </c>
       <c r="CH53" s="10">
-        <v>0.33923859781378712</v>
-      </c>
-      <c r="CI53" s="9"/>
+        <v>1.168488503580839</v>
+      </c>
+      <c r="CI53" s="10">
+        <v>1.389932381667893</v>
+      </c>
       <c r="CJ53" s="9"/>
       <c r="CK53" s="9"/>
       <c r="CL53" s="9"/>
@@ -42808,7 +43003,9 @@
       <c r="CH54" s="10">
         <v>-0.81168831168831179</v>
       </c>
-      <c r="CI54" s="9"/>
+      <c r="CI54" s="10">
+        <v>-0.78616352201257855</v>
+      </c>
       <c r="CJ54" s="9"/>
       <c r="CK54" s="9"/>
       <c r="CL54" s="9"/>
@@ -43075,9 +43272,11 @@
         <v>0.7342817806333285</v>
       </c>
       <c r="CH55" s="10">
-        <v>1.4049172102358454</v>
-      </c>
-      <c r="CI55" s="9"/>
+        <v>1.555444054189661</v>
+      </c>
+      <c r="CI55" s="10">
+        <v>2.0436600092893662</v>
+      </c>
       <c r="CJ55" s="9"/>
       <c r="CK55" s="9"/>
       <c r="CL55" s="9"/>
@@ -43344,9 +43543,11 @@
         <v>0</v>
       </c>
       <c r="CH56" s="10">
-        <v>0</v>
-      </c>
-      <c r="CI56" s="9"/>
+        <v>-0.68027210884352296</v>
+      </c>
+      <c r="CI56" s="10">
+        <v>-1.2987012987012942</v>
+      </c>
       <c r="CJ56" s="9"/>
       <c r="CK56" s="9"/>
       <c r="CL56" s="9"/>

</xml_diff>

<commit_message>
December 17, 2021 update
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t xml:space="preserve">10/01/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/01/2021</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1215,10 +1218,13 @@
       <c r="DO4" t="s">
         <v>118</v>
       </c>
+      <c r="DP4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1569,15 +1575,18 @@
         <v>9058</v>
       </c>
       <c r="DN5" t="n">
-        <v>10084.2</v>
+        <v>10097.1</v>
       </c>
       <c r="DO5" t="n">
-        <v>10414.6</v>
+        <v>10405.6</v>
+      </c>
+      <c r="DP5" t="n">
+        <v>10516.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -1931,12 +1940,15 @@
         <v>164.4</v>
       </c>
       <c r="DO6" t="n">
-        <v>167.6</v>
+        <v>167.4</v>
+      </c>
+      <c r="DP6" t="n">
+        <v>168.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2290,12 +2302,15 @@
         <v>24.5</v>
       </c>
       <c r="DO7" t="n">
-        <v>25.6</v>
+        <v>25.5</v>
+      </c>
+      <c r="DP7" t="n">
+        <v>25.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2649,12 +2664,15 @@
         <v>193</v>
       </c>
       <c r="DO8" t="n">
-        <v>194.7</v>
+        <v>194.9</v>
+      </c>
+      <c r="DP8" t="n">
+        <v>198.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3009,11 +3027,14 @@
       </c>
       <c r="DO9" t="n">
         <v>96.3</v>
+      </c>
+      <c r="DP9" t="n">
+        <v>97</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3367,12 +3388,15 @@
         <v>1093.9</v>
       </c>
       <c r="DO10" t="n">
-        <v>1149.2</v>
+        <v>1145.2</v>
+      </c>
+      <c r="DP10" t="n">
+        <v>1169.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -3726,12 +3750,15 @@
         <v>209.3</v>
       </c>
       <c r="DO11" t="n">
-        <v>216.7</v>
+        <v>214.8</v>
+      </c>
+      <c r="DP11" t="n">
+        <v>218</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4086,11 +4113,14 @@
       </c>
       <c r="DO12" t="n">
         <v>123</v>
+      </c>
+      <c r="DP12" t="n">
+        <v>124.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4444,12 +4474,15 @@
         <v>34.6</v>
       </c>
       <c r="DO13" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="DP13" t="n">
         <v>36.4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4569,10 +4602,11 @@
       <c r="DM14"/>
       <c r="DN14"/>
       <c r="DO14"/>
+      <c r="DP14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -4926,12 +4960,15 @@
         <v>487.3</v>
       </c>
       <c r="DO15" t="n">
-        <v>492.9</v>
+        <v>492.8</v>
+      </c>
+      <c r="DP15" t="n">
+        <v>497.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5285,12 +5322,15 @@
         <v>338.3</v>
       </c>
       <c r="DO16" t="n">
-        <v>341.2</v>
+        <v>341.4</v>
+      </c>
+      <c r="DP16" t="n">
+        <v>341.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -5410,10 +5450,11 @@
       <c r="DM17"/>
       <c r="DN17"/>
       <c r="DO17"/>
+      <c r="DP17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -5768,11 +5809,14 @@
       </c>
       <c r="DO18" t="n">
         <v>63.8</v>
+      </c>
+      <c r="DP18" t="n">
+        <v>64.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6127,11 +6171,14 @@
       </c>
       <c r="DO19" t="n">
         <v>427.4</v>
+      </c>
+      <c r="DP19" t="n">
+        <v>430.4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -6485,12 +6532,15 @@
         <v>221.4</v>
       </c>
       <c r="DO20" t="n">
-        <v>222.7</v>
+        <v>224.1</v>
+      </c>
+      <c r="DP20" t="n">
+        <v>226.7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -6844,12 +6894,15 @@
         <v>139.7</v>
       </c>
       <c r="DO21" t="n">
-        <v>145.1</v>
+        <v>145.2</v>
+      </c>
+      <c r="DP21" t="n">
+        <v>146.4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -7204,11 +7257,14 @@
       </c>
       <c r="DO22" t="n">
         <v>133.6</v>
+      </c>
+      <c r="DP22" t="n">
+        <v>135.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -7562,12 +7618,15 @@
         <v>154.8</v>
       </c>
       <c r="DO23" t="n">
-        <v>157.1</v>
+        <v>157.4</v>
+      </c>
+      <c r="DP23" t="n">
+        <v>158.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -7922,11 +7981,14 @@
       </c>
       <c r="DO24" t="n">
         <v>142.8</v>
+      </c>
+      <c r="DP24" t="n">
+        <v>143.9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -8280,12 +8342,15 @@
         <v>46.6</v>
       </c>
       <c r="DO25" t="n">
-        <v>48.1</v>
+        <v>47.9</v>
+      </c>
+      <c r="DP25" t="n">
+        <v>48.4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -8639,12 +8704,15 @@
         <v>208.9</v>
       </c>
       <c r="DO26" t="n">
-        <v>219.8</v>
+        <v>219.7</v>
+      </c>
+      <c r="DP26" t="n">
+        <v>221.6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -8998,12 +9066,15 @@
         <v>227.8</v>
       </c>
       <c r="DO27" t="n">
-        <v>234.8</v>
+        <v>234</v>
+      </c>
+      <c r="DP27" t="n">
+        <v>236.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -9357,12 +9428,15 @@
         <v>301.5</v>
       </c>
       <c r="DO28" t="n">
-        <v>312.1</v>
+        <v>311.6</v>
+      </c>
+      <c r="DP28" t="n">
+        <v>314</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -9716,12 +9790,15 @@
         <v>186.6</v>
       </c>
       <c r="DO29" t="n">
-        <v>199.6</v>
+        <v>198.3</v>
+      </c>
+      <c r="DP29" t="n">
+        <v>200.5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -10076,11 +10153,14 @@
       </c>
       <c r="DO30" t="n">
         <v>103.2</v>
+      </c>
+      <c r="DP30" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -10200,10 +10280,11 @@
       <c r="DM31"/>
       <c r="DN31"/>
       <c r="DO31"/>
+      <c r="DP31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -10557,12 +10638,15 @@
         <v>41.1</v>
       </c>
       <c r="DO32" t="n">
-        <v>43.2</v>
+        <v>43</v>
+      </c>
+      <c r="DP32" t="n">
+        <v>43.6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -10916,12 +11000,15 @@
         <v>89.2</v>
       </c>
       <c r="DO33" t="n">
-        <v>92.7</v>
+        <v>92.5</v>
+      </c>
+      <c r="DP33" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -11276,11 +11363,14 @@
       </c>
       <c r="DO34" t="n">
         <v>78.5</v>
+      </c>
+      <c r="DP34" t="n">
+        <v>79.6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -11635,11 +11725,14 @@
       </c>
       <c r="DO35" t="n">
         <v>47.5</v>
+      </c>
+      <c r="DP35" t="n">
+        <v>47.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -11994,11 +12087,14 @@
       </c>
       <c r="DO36" t="n">
         <v>308.4</v>
+      </c>
+      <c r="DP36" t="n">
+        <v>310.7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -12352,12 +12448,15 @@
         <v>70.4</v>
       </c>
       <c r="DO37" t="n">
-        <v>71.2</v>
+        <v>72.5</v>
+      </c>
+      <c r="DP37" t="n">
+        <v>72.8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -12711,12 +12810,15 @@
         <v>624.1</v>
       </c>
       <c r="DO38" t="n">
-        <v>669.7</v>
+        <v>658.6</v>
+      </c>
+      <c r="DP38" t="n">
+        <v>667.2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -13071,11 +13173,14 @@
       </c>
       <c r="DO39" t="n">
         <v>309.1</v>
+      </c>
+      <c r="DP39" t="n">
+        <v>312.5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -13430,11 +13535,14 @@
       </c>
       <c r="DO40" t="n">
         <v>38.2</v>
+      </c>
+      <c r="DP40" t="n">
+        <v>38.6</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -13788,12 +13896,15 @@
         <v>377.8</v>
       </c>
       <c r="DO41" t="n">
-        <v>390.3</v>
+        <v>385.4</v>
+      </c>
+      <c r="DP41" t="n">
+        <v>390.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -14147,12 +14258,15 @@
         <v>142.6</v>
       </c>
       <c r="DO42" t="n">
-        <v>145.6</v>
+        <v>146.9</v>
+      </c>
+      <c r="DP42" t="n">
+        <v>147.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -14506,12 +14620,15 @@
         <v>121</v>
       </c>
       <c r="DO43" t="n">
-        <v>129.8</v>
+        <v>129.7</v>
+      </c>
+      <c r="DP43" t="n">
+        <v>131.4</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -14865,12 +14982,15 @@
         <v>317.5</v>
       </c>
       <c r="DO44" t="n">
-        <v>324.5</v>
+        <v>324.1</v>
+      </c>
+      <c r="DP44" t="n">
+        <v>327.4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -15225,11 +15345,14 @@
       </c>
       <c r="DO45" t="n">
         <v>29.6</v>
+      </c>
+      <c r="DP45" t="n">
+        <v>29.9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -15583,12 +15706,15 @@
         <v>158.6</v>
       </c>
       <c r="DO46" t="n">
-        <v>161.9</v>
+        <v>161.8</v>
+      </c>
+      <c r="DP46" t="n">
+        <v>163</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -15942,12 +16068,15 @@
         <v>35.2</v>
       </c>
       <c r="DO47" t="n">
-        <v>37</v>
+        <v>36.9</v>
+      </c>
+      <c r="DP47" t="n">
+        <v>37.4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -16301,12 +16430,15 @@
         <v>204.9</v>
       </c>
       <c r="DO48" t="n">
-        <v>207.6</v>
+        <v>207.9</v>
+      </c>
+      <c r="DP48" t="n">
+        <v>207.7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -16660,12 +16792,15 @@
         <v>1103.1</v>
       </c>
       <c r="DO49" t="n">
-        <v>1132.8</v>
+        <v>1132.3</v>
+      </c>
+      <c r="DP49" t="n">
+        <v>1142.6</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -17020,11 +17155,14 @@
       </c>
       <c r="DO50" t="n">
         <v>122.3</v>
+      </c>
+      <c r="DP50" t="n">
+        <v>123.4</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -17379,11 +17517,14 @@
       </c>
       <c r="DO51" t="n">
         <v>29.8</v>
+      </c>
+      <c r="DP51" t="n">
+        <v>30.2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -17737,12 +17878,15 @@
         <v>306.1</v>
       </c>
       <c r="DO52" t="n">
-        <v>315.4</v>
+        <v>314.6</v>
+      </c>
+      <c r="DP52" t="n">
+        <v>317.5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -18096,12 +18240,15 @@
         <v>230</v>
       </c>
       <c r="DO53" t="n">
-        <v>244.7</v>
+        <v>242.1</v>
+      </c>
+      <c r="DP53" t="n">
+        <v>247.6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -18456,11 +18603,14 @@
       </c>
       <c r="DO54" t="n">
         <v>59.5</v>
+      </c>
+      <c r="DP54" t="n">
+        <v>60.6</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -18814,12 +18964,15 @@
         <v>192.3</v>
       </c>
       <c r="DO55" t="n">
-        <v>201.1</v>
+        <v>201</v>
+      </c>
+      <c r="DP55" t="n">
+        <v>202.4</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -19173,7 +19326,10 @@
         <v>26.4</v>
       </c>
       <c r="DO56" t="n">
-        <v>27.4</v>
+        <v>27.3</v>
+      </c>
+      <c r="DP56" t="n">
+        <v>27.5</v>
       </c>
     </row>
   </sheetData>
@@ -19512,10 +19668,13 @@
       <c r="DC4" t="s">
         <v>118</v>
       </c>
+      <c r="DD4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -19830,15 +19989,18 @@
         <v>2.95404689648901</v>
       </c>
       <c r="DB5" t="n">
-        <v>3.38103830066433</v>
+        <v>3.51328631181826</v>
       </c>
       <c r="DC5" t="n">
-        <v>3.75277697526374</v>
+        <v>3.66311678737583</v>
+      </c>
+      <c r="DD5" t="n">
+        <v>4.020890827621</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -20156,12 +20318,15 @@
         <v>3.98481973434536</v>
       </c>
       <c r="DC6" t="n">
-        <v>2.94840294840294</v>
+        <v>2.82555282555282</v>
+      </c>
+      <c r="DD6" t="n">
+        <v>2.61716372489348</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -20479,12 +20644,15 @@
         <v>-4.29687500000001</v>
       </c>
       <c r="DC7" t="n">
-        <v>-4.11985018726591</v>
+        <v>-4.49438202247191</v>
+      </c>
+      <c r="DD7" t="n">
+        <v>-3.74531835205993</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -20802,12 +20970,15 @@
         <v>1.90073917634635</v>
       </c>
       <c r="DC8" t="n">
-        <v>2.36593059936909</v>
+        <v>2.47108307045216</v>
+      </c>
+      <c r="DD8" t="n">
+        <v>3.28295987493485</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -21126,11 +21297,14 @@
       </c>
       <c r="DC9" t="n">
         <v>-1.93482688391038</v>
+      </c>
+      <c r="DD9" t="n">
+        <v>-1.92113245702731</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -21448,12 +21622,15 @@
         <v>2.08100037327363</v>
       </c>
       <c r="DC10" t="n">
-        <v>3.2617485847785</v>
+        <v>2.90232725312247</v>
+      </c>
+      <c r="DD10" t="n">
+        <v>4.1789182927916</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -21771,12 +21948,15 @@
         <v>4.3369890329013</v>
       </c>
       <c r="DC11" t="n">
-        <v>4.53449107573564</v>
+        <v>3.61794500723588</v>
+      </c>
+      <c r="DD11" t="n">
+        <v>4.50623202301054</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -22095,11 +22275,14 @@
       </c>
       <c r="DC12" t="n">
         <v>0.737100737100742</v>
+      </c>
+      <c r="DD12" t="n">
+        <v>0.647249190938498</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -22417,12 +22600,15 @@
         <v>3.59281437125747</v>
       </c>
       <c r="DC13" t="n">
-        <v>5.20231213872832</v>
+        <v>3.46820809248554</v>
+      </c>
+      <c r="DD13" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -22530,10 +22716,11 @@
       <c r="DA14"/>
       <c r="DB14"/>
       <c r="DC14"/>
+      <c r="DD14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -22851,12 +23038,15 @@
         <v>3.52666241767579</v>
       </c>
       <c r="DC15" t="n">
-        <v>3.57217902920782</v>
+        <v>3.55116621138895</v>
+      </c>
+      <c r="DD15" t="n">
+        <v>4.12220129734255</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -23174,12 +23364,15 @@
         <v>2.98325722983258</v>
       </c>
       <c r="DC16" t="n">
-        <v>2.61654135338347</v>
+        <v>2.6766917293233</v>
+      </c>
+      <c r="DD16" t="n">
+        <v>2.73848931688232</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -23287,10 +23480,11 @@
       <c r="DA17"/>
       <c r="DB17"/>
       <c r="DC17"/>
+      <c r="DD17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -23609,11 +23803,14 @@
       </c>
       <c r="DC18" t="n">
         <v>6.86767169179229</v>
+      </c>
+      <c r="DD18" t="n">
+        <v>6.61157024793388</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -23932,11 +24129,14 @@
       </c>
       <c r="DC19" t="n">
         <v>2.22434824204735</v>
+      </c>
+      <c r="DD19" t="n">
+        <v>2.59833134684149</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -24254,12 +24454,15 @@
         <v>1.23456790123455</v>
       </c>
       <c r="DC20" t="n">
-        <v>1.13533151680291</v>
+        <v>1.77111716621254</v>
+      </c>
+      <c r="DD20" t="n">
+        <v>2.39385727190606</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -24577,12 +24780,15 @@
         <v>2.72058823529411</v>
       </c>
       <c r="DC21" t="n">
-        <v>2.47175141242938</v>
+        <v>2.54237288135593</v>
+      </c>
+      <c r="DD21" t="n">
+        <v>2.5928521373511</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -24901,11 +25107,14 @@
       </c>
       <c r="DC22" t="n">
         <v>1.51975683890578</v>
+      </c>
+      <c r="DD22" t="n">
+        <v>1.80859080633007</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -25223,12 +25432,15 @@
         <v>3.54515050167225</v>
       </c>
       <c r="DC23" t="n">
-        <v>2.7468933943754</v>
+        <v>2.94310006540222</v>
+      </c>
+      <c r="DD23" t="n">
+        <v>2.98120544394035</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -25547,11 +25759,14 @@
       </c>
       <c r="DC24" t="n">
         <v>0.210526315789482</v>
+      </c>
+      <c r="DD24" t="n">
+        <v>0.0695410292072085</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -25869,12 +26084,15 @@
         <v>0.431034482758611</v>
       </c>
       <c r="DC25" t="n">
-        <v>1.05042016806723</v>
+        <v>0.630252100840345</v>
+      </c>
+      <c r="DD25" t="n">
+        <v>0.414937759336105</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -26192,12 +26410,15 @@
         <v>7.90289256198345</v>
       </c>
       <c r="DC26" t="n">
-        <v>6.13230323515211</v>
+        <v>6.08401738290682</v>
+      </c>
+      <c r="DD26" t="n">
+        <v>7.26040658276862</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -26515,12 +26736,15 @@
         <v>9.25659472422063</v>
       </c>
       <c r="DC27" t="n">
-        <v>9.66837926202708</v>
+        <v>9.29472209248014</v>
+      </c>
+      <c r="DD27" t="n">
+        <v>8.97376898297285</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -26838,12 +27062,15 @@
         <v>5.9009483667018</v>
       </c>
       <c r="DC28" t="n">
-        <v>4.90756302521009</v>
+        <v>4.73949579831934</v>
+      </c>
+      <c r="DD28" t="n">
+        <v>5.54621848739496</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -27161,12 +27388,15 @@
         <v>0.0536193029490586</v>
       </c>
       <c r="DC29" t="n">
-        <v>0.757193336698637</v>
+        <v>0.100959111559827</v>
+      </c>
+      <c r="DD29" t="n">
+        <v>0.149850149850156</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -27485,11 +27715,14 @@
       </c>
       <c r="DC30" t="n">
         <v>-0.386100386100392</v>
+      </c>
+      <c r="DD30" t="n">
+        <v>1.35135135135136</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -27597,10 +27830,11 @@
       <c r="DA31"/>
       <c r="DB31"/>
       <c r="DC31"/>
+      <c r="DD31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -27918,12 +28152,15 @@
         <v>0.982800982800962</v>
       </c>
       <c r="DC32" t="n">
-        <v>2.1276595744681</v>
+        <v>1.65484633569741</v>
+      </c>
+      <c r="DD32" t="n">
+        <v>2.58823529411763</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -28241,12 +28478,15 @@
         <v>1.47895335608646</v>
       </c>
       <c r="DC33" t="n">
-        <v>3.34448160535117</v>
+        <v>3.12151616499442</v>
+      </c>
+      <c r="DD33" t="n">
+        <v>2.76243093922652</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -28565,11 +28805,14 @@
       </c>
       <c r="DC34" t="n">
         <v>3.28947368421053</v>
+      </c>
+      <c r="DD34" t="n">
+        <v>4.32503276539973</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -28888,11 +29131,14 @@
       </c>
       <c r="DC35" t="n">
         <v>5.08849557522123</v>
+      </c>
+      <c r="DD35" t="n">
+        <v>5.06607929515418</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -29211,11 +29457,14 @@
       </c>
       <c r="DC36" t="n">
         <v>5.65262076053441</v>
+      </c>
+      <c r="DD36" t="n">
+        <v>5.50084889643463</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -29533,12 +29782,15 @@
         <v>-1.94986072423399</v>
       </c>
       <c r="DC37" t="n">
-        <v>-2.59917920656636</v>
+        <v>-0.820793433652523</v>
+      </c>
+      <c r="DD37" t="n">
+        <v>0.552486187845312</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -29856,12 +30108,15 @@
         <v>0.938055959890032</v>
       </c>
       <c r="DC38" t="n">
-        <v>3.20542456464786</v>
+        <v>1.4948374171675</v>
+      </c>
+      <c r="DD38" t="n">
+        <v>2.15893431327515</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -30180,11 +30435,14 @@
       </c>
       <c r="DC39" t="n">
         <v>1.71108917407043</v>
+      </c>
+      <c r="DD39" t="n">
+        <v>1.72526041666667</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -30503,11 +30761,14 @@
       </c>
       <c r="DC40" t="n">
         <v>4.94505494505494</v>
+      </c>
+      <c r="DD40" t="n">
+        <v>4.8913043478261</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -30825,12 +31086,15 @@
         <v>4.39347886156396</v>
       </c>
       <c r="DC41" t="n">
-        <v>4.38619951858787</v>
+        <v>3.07568868681466</v>
+      </c>
+      <c r="DD41" t="n">
+        <v>3.06472919418759</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -31148,12 +31412,15 @@
         <v>1.56695156695158</v>
       </c>
       <c r="DC42" t="n">
-        <v>1.46341463414634</v>
+        <v>2.36933797909406</v>
+      </c>
+      <c r="DD42" t="n">
+        <v>2.64439805149618</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -31471,12 +31738,15 @@
         <v>8.61759425493716</v>
       </c>
       <c r="DC43" t="n">
-        <v>8.80134115674769</v>
+        <v>8.71751886001677</v>
+      </c>
+      <c r="DD43" t="n">
+        <v>9.04564315352697</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -31794,12 +32064,15 @@
         <v>1.95889531149646</v>
       </c>
       <c r="DC44" t="n">
-        <v>1.7560363750392</v>
+        <v>1.63060520539355</v>
+      </c>
+      <c r="DD44" t="n">
+        <v>1.86683260734289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -32118,11 +32391,14 @@
       </c>
       <c r="DC45" t="n">
         <v>8.82352941176469</v>
+      </c>
+      <c r="DD45" t="n">
+        <v>8.72727272727274</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -32440,12 +32716,15 @@
         <v>4.06824146981628</v>
       </c>
       <c r="DC46" t="n">
-        <v>2.98982188295167</v>
+        <v>2.92620865139951</v>
+      </c>
+      <c r="DD46" t="n">
+        <v>3.03413400758534</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -32763,12 +33042,15 @@
         <v>0.859598853868207</v>
       </c>
       <c r="DC47" t="n">
-        <v>2.20994475138121</v>
+        <v>1.93370165745855</v>
+      </c>
+      <c r="DD47" t="n">
+        <v>3.31491712707181</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -33086,12 +33368,15 @@
         <v>4.64759959141981</v>
       </c>
       <c r="DC48" t="n">
-        <v>3.07845084409137</v>
+        <v>3.22740814299902</v>
+      </c>
+      <c r="DD48" t="n">
+        <v>3.17933432687531</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -33409,12 +33694,15 @@
         <v>2.31889435117336</v>
       </c>
       <c r="DC49" t="n">
-        <v>1.55087404751232</v>
+        <v>1.50605109816226</v>
+      </c>
+      <c r="DD49" t="n">
+        <v>1.42020237883898</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -33733,11 +34021,14 @@
       </c>
       <c r="DC50" t="n">
         <v>5.24956970740104</v>
+      </c>
+      <c r="DD50" t="n">
+        <v>5.74121679520139</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -34056,11 +34347,14 @@
       </c>
       <c r="DC51" t="n">
         <v>1.36054421768707</v>
+      </c>
+      <c r="DD51" t="n">
+        <v>2.02702702702702</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -34378,12 +34672,15 @@
         <v>3.83310719131615</v>
       </c>
       <c r="DC52" t="n">
-        <v>5.37921817574339</v>
+        <v>5.11192783160709</v>
+      </c>
+      <c r="DD52" t="n">
+        <v>5.27188328912466</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -34701,12 +34998,15 @@
         <v>3.1852848811126</v>
       </c>
       <c r="DC53" t="n">
-        <v>10.0269784172662</v>
+        <v>8.85791366906474</v>
+      </c>
+      <c r="DD53" t="n">
+        <v>10.7334525939177</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -35025,11 +35325,14 @@
       </c>
       <c r="DC54" t="n">
         <v>0.676818950930636</v>
+      </c>
+      <c r="DD54" t="n">
+        <v>0.999999999999991</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -35347,12 +35650,15 @@
         <v>3.10991957104558</v>
       </c>
       <c r="DC55" t="n">
-        <v>3.07534597642235</v>
+        <v>3.02409021014863</v>
+      </c>
+      <c r="DD55" t="n">
+        <v>3.47648261758692</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -35670,7 +35976,10 @@
         <v>-3.64963503649635</v>
       </c>
       <c r="DC56" t="n">
-        <v>-3.52112676056337</v>
+        <v>-3.87323943661971</v>
+      </c>
+      <c r="DD56" t="n">
+        <v>-2.82685512367491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update April 15, 2022
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t xml:space="preserve">02/01/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/01/2022</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1239,10 +1242,13 @@
       <c r="DS4" t="s">
         <v>122</v>
       </c>
+      <c r="DT4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1605,15 +1611,18 @@
         <v>10626.9</v>
       </c>
       <c r="DR5" t="n">
-        <v>10326.2</v>
+        <v>10315.6</v>
       </c>
       <c r="DS5" t="n">
-        <v>10671</v>
+        <v>10637.7</v>
+      </c>
+      <c r="DT5" t="n">
+        <v>10693.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -1979,12 +1988,15 @@
         <v>164</v>
       </c>
       <c r="DS6" t="n">
-        <v>166.3</v>
+        <v>166.8</v>
+      </c>
+      <c r="DT6" t="n">
+        <v>169.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2350,12 +2362,15 @@
         <v>26.6</v>
       </c>
       <c r="DS7" t="n">
+        <v>27.6</v>
+      </c>
+      <c r="DT7" t="n">
         <v>27.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2721,12 +2736,15 @@
         <v>190.5</v>
       </c>
       <c r="DS8" t="n">
-        <v>195.1</v>
+        <v>195.6</v>
+      </c>
+      <c r="DT8" t="n">
+        <v>194.4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3093,11 +3111,14 @@
       </c>
       <c r="DS9" t="n">
         <v>102.5</v>
+      </c>
+      <c r="DT9" t="n">
+        <v>102.7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3463,12 +3484,15 @@
         <v>1188</v>
       </c>
       <c r="DS10" t="n">
-        <v>1209.2</v>
+        <v>1203.6</v>
+      </c>
+      <c r="DT10" t="n">
+        <v>1215.4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -3834,12 +3858,15 @@
         <v>203.6</v>
       </c>
       <c r="DS11" t="n">
-        <v>214.4</v>
+        <v>213</v>
+      </c>
+      <c r="DT11" t="n">
+        <v>216.4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4205,12 +4232,15 @@
         <v>120.7</v>
       </c>
       <c r="DS12" t="n">
-        <v>122.8</v>
+        <v>123.1</v>
+      </c>
+      <c r="DT12" t="n">
+        <v>123.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4576,12 +4606,15 @@
         <v>34.2</v>
       </c>
       <c r="DS13" t="n">
-        <v>35.6</v>
+        <v>36.1</v>
+      </c>
+      <c r="DT13" t="n">
+        <v>36.9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4705,10 +4738,11 @@
       <c r="DQ14"/>
       <c r="DR14"/>
       <c r="DS14"/>
+      <c r="DT14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5075,11 +5109,14 @@
       </c>
       <c r="DS15" t="n">
         <v>486.7</v>
+      </c>
+      <c r="DT15" t="n">
+        <v>485.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5445,12 +5482,15 @@
         <v>336.6</v>
       </c>
       <c r="DS16" t="n">
-        <v>340.2</v>
+        <v>340.3</v>
+      </c>
+      <c r="DT16" t="n">
+        <v>340.6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -5574,10 +5614,11 @@
       <c r="DQ17"/>
       <c r="DR17"/>
       <c r="DS17"/>
+      <c r="DT17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -5943,12 +5984,15 @@
         <v>61.5</v>
       </c>
       <c r="DS18" t="n">
-        <v>63.4</v>
+        <v>63.5</v>
+      </c>
+      <c r="DT18" t="n">
+        <v>63.3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6315,11 +6359,14 @@
       </c>
       <c r="DS19" t="n">
         <v>434.8</v>
+      </c>
+      <c r="DT19" t="n">
+        <v>439.6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -6685,12 +6732,15 @@
         <v>226.4</v>
       </c>
       <c r="DS20" t="n">
-        <v>234.8</v>
+        <v>233.3</v>
+      </c>
+      <c r="DT20" t="n">
+        <v>235</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7056,12 +7106,15 @@
         <v>138.6</v>
       </c>
       <c r="DS21" t="n">
-        <v>144.7</v>
+        <v>143.4</v>
+      </c>
+      <c r="DT21" t="n">
+        <v>143.4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -7427,12 +7480,15 @@
         <v>129.4</v>
       </c>
       <c r="DS22" t="n">
-        <v>133.7</v>
+        <v>133.5</v>
+      </c>
+      <c r="DT22" t="n">
+        <v>134.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -7798,12 +7854,15 @@
         <v>153.7</v>
       </c>
       <c r="DS23" t="n">
-        <v>160.4</v>
+        <v>157.1</v>
+      </c>
+      <c r="DT23" t="n">
+        <v>158.7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -8169,12 +8228,15 @@
         <v>142.8</v>
       </c>
       <c r="DS24" t="n">
-        <v>146.6</v>
+        <v>143.9</v>
+      </c>
+      <c r="DT24" t="n">
+        <v>143.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -8541,11 +8603,14 @@
       </c>
       <c r="DS25" t="n">
         <v>49.2</v>
+      </c>
+      <c r="DT25" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -8912,11 +8977,14 @@
       </c>
       <c r="DS26" t="n">
         <v>213.6</v>
+      </c>
+      <c r="DT26" t="n">
+        <v>216.9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -9282,12 +9350,15 @@
         <v>219</v>
       </c>
       <c r="DS27" t="n">
-        <v>228.8</v>
+        <v>229.9</v>
+      </c>
+      <c r="DT27" t="n">
+        <v>231.4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -9653,12 +9724,15 @@
         <v>290.1</v>
       </c>
       <c r="DS28" t="n">
-        <v>302.3</v>
+        <v>304.4</v>
+      </c>
+      <c r="DT28" t="n">
+        <v>306</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -10024,12 +10098,15 @@
         <v>198.1</v>
       </c>
       <c r="DS29" t="n">
-        <v>202.6</v>
+        <v>202.5</v>
+      </c>
+      <c r="DT29" t="n">
+        <v>202</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -10396,11 +10473,14 @@
       </c>
       <c r="DS30" t="n">
         <v>104</v>
+      </c>
+      <c r="DT30" t="n">
+        <v>103.8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -10524,10 +10604,11 @@
       <c r="DQ31"/>
       <c r="DR31"/>
       <c r="DS31"/>
+      <c r="DT31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -10893,12 +10974,15 @@
         <v>43.1</v>
       </c>
       <c r="DS32" t="n">
-        <v>44.4</v>
+        <v>44.1</v>
+      </c>
+      <c r="DT32" t="n">
+        <v>44.6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -11265,11 +11349,14 @@
       </c>
       <c r="DS33" t="n">
         <v>93.2</v>
+      </c>
+      <c r="DT33" t="n">
+        <v>93.7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -11636,11 +11723,14 @@
       </c>
       <c r="DS34" t="n">
         <v>76.3</v>
+      </c>
+      <c r="DT34" t="n">
+        <v>76.4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -12006,12 +12096,15 @@
         <v>42.2</v>
       </c>
       <c r="DS35" t="n">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="DT35" t="n">
+        <v>45.2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -12377,12 +12470,15 @@
         <v>299.1</v>
       </c>
       <c r="DS36" t="n">
-        <v>305.4</v>
+        <v>305.9</v>
+      </c>
+      <c r="DT36" t="n">
+        <v>307.9</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -12748,12 +12844,15 @@
         <v>71.9</v>
       </c>
       <c r="DS37" t="n">
-        <v>76.4</v>
+        <v>76.3</v>
+      </c>
+      <c r="DT37" t="n">
+        <v>77.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -13119,12 +13218,15 @@
         <v>658.1</v>
       </c>
       <c r="DS38" t="n">
-        <v>674.6</v>
+        <v>674.8</v>
+      </c>
+      <c r="DT38" t="n">
+        <v>677.8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -13491,11 +13593,14 @@
       </c>
       <c r="DS39" t="n">
         <v>321.7</v>
+      </c>
+      <c r="DT39" t="n">
+        <v>329.7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -13861,12 +13966,15 @@
         <v>37.9</v>
       </c>
       <c r="DS40" t="n">
+        <v>38.7</v>
+      </c>
+      <c r="DT40" t="n">
         <v>38.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -14232,12 +14340,15 @@
         <v>359.3</v>
       </c>
       <c r="DS41" t="n">
-        <v>375.4</v>
+        <v>378</v>
+      </c>
+      <c r="DT41" t="n">
+        <v>384.2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -14603,12 +14714,15 @@
         <v>139.2</v>
       </c>
       <c r="DS42" t="n">
-        <v>146.4</v>
+        <v>146.3</v>
+      </c>
+      <c r="DT42" t="n">
+        <v>147.1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -14974,12 +15088,15 @@
         <v>127.8</v>
       </c>
       <c r="DS43" t="n">
-        <v>130.6</v>
+        <v>130.8</v>
+      </c>
+      <c r="DT43" t="n">
+        <v>131.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -15345,12 +15462,15 @@
         <v>309.4</v>
       </c>
       <c r="DS44" t="n">
-        <v>322.1</v>
+        <v>319.8</v>
+      </c>
+      <c r="DT44" t="n">
+        <v>321.8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -15716,12 +15836,15 @@
         <v>28.5</v>
       </c>
       <c r="DS45" t="n">
-        <v>28.9</v>
+        <v>29.3</v>
+      </c>
+      <c r="DT45" t="n">
+        <v>29.4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -16088,11 +16211,14 @@
       </c>
       <c r="DS46" t="n">
         <v>165.3</v>
+      </c>
+      <c r="DT46" t="n">
+        <v>166.5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -16458,12 +16584,15 @@
         <v>36</v>
       </c>
       <c r="DS47" t="n">
-        <v>37.2</v>
+        <v>37.4</v>
+      </c>
+      <c r="DT47" t="n">
+        <v>37.6</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -16829,12 +16958,15 @@
         <v>194.1</v>
       </c>
       <c r="DS48" t="n">
-        <v>204.2</v>
+        <v>203.4</v>
+      </c>
+      <c r="DT48" t="n">
+        <v>203.9</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -17200,12 +17332,15 @@
         <v>1121.5</v>
       </c>
       <c r="DS49" t="n">
-        <v>1141.4</v>
+        <v>1144.2</v>
+      </c>
+      <c r="DT49" t="n">
+        <v>1146.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -17572,11 +17707,14 @@
       </c>
       <c r="DS50" t="n">
         <v>125.7</v>
+      </c>
+      <c r="DT50" t="n">
+        <v>126.6</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -17942,12 +18080,15 @@
         <v>29.8</v>
       </c>
       <c r="DS51" t="n">
-        <v>30.8</v>
+        <v>30.9</v>
+      </c>
+      <c r="DT51" t="n">
+        <v>30.3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -18313,12 +18454,15 @@
         <v>296.5</v>
       </c>
       <c r="DS52" t="n">
-        <v>315.7</v>
+        <v>316</v>
+      </c>
+      <c r="DT52" t="n">
+        <v>318</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -18684,12 +18828,15 @@
         <v>244.4</v>
       </c>
       <c r="DS53" t="n">
-        <v>251.5</v>
+        <v>248.9</v>
+      </c>
+      <c r="DT53" t="n">
+        <v>249.8</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -19055,12 +19202,15 @@
         <v>56.3</v>
       </c>
       <c r="DS54" t="n">
-        <v>60.2</v>
+        <v>60.3</v>
+      </c>
+      <c r="DT54" t="n">
+        <v>59.9</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -19427,11 +19577,14 @@
       </c>
       <c r="DS55" t="n">
         <v>206.4</v>
+      </c>
+      <c r="DT55" t="n">
+        <v>207.5</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -19797,7 +19950,10 @@
         <v>28.6</v>
       </c>
       <c r="DS56" t="n">
-        <v>29.6</v>
+        <v>29.7</v>
+      </c>
+      <c r="DT56" t="n">
+        <v>30.2</v>
       </c>
     </row>
   </sheetData>
@@ -20148,10 +20304,13 @@
       <c r="DG4" t="s">
         <v>122</v>
       </c>
+      <c r="DH4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -20478,15 +20637,18 @@
         <v>4.73670204902282</v>
       </c>
       <c r="DF5" t="n">
-        <v>3.97422343049892</v>
+        <v>3.8674923224085</v>
       </c>
       <c r="DG5" t="n">
-        <v>4.08497688301047</v>
+        <v>3.76016854918944</v>
+      </c>
+      <c r="DH5" t="n">
+        <v>3.1453456407882</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -20816,12 +20978,15 @@
         <v>2.11706102117061</v>
       </c>
       <c r="DG6" t="n">
-        <v>2.02453987730062</v>
+        <v>2.33128834355829</v>
+      </c>
+      <c r="DH6" t="n">
+        <v>3.04506699147381</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -21152,11 +21317,14 @@
       </c>
       <c r="DG7" t="n">
         <v>1.0989010989011</v>
+      </c>
+      <c r="DH7" t="n">
+        <v>1.09890109890109</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -21486,12 +21654,15 @@
         <v>2.52960172228202</v>
       </c>
       <c r="DG8" t="n">
-        <v>2.79241306638567</v>
+        <v>3.05584826132772</v>
+      </c>
+      <c r="DH8" t="n">
+        <v>2.26196738558652</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -21822,11 +21993,14 @@
       </c>
       <c r="DG9" t="n">
         <v>2.6026026026026</v>
+      </c>
+      <c r="DH9" t="n">
+        <v>2.39282153539382</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -22156,12 +22330,15 @@
         <v>6.72895517024527</v>
       </c>
       <c r="DG10" t="n">
-        <v>8.05111250111694</v>
+        <v>7.55071039227949</v>
+      </c>
+      <c r="DH10" t="n">
+        <v>6.99885553305751</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -22491,12 +22668,15 @@
         <v>4.84037075180225</v>
       </c>
       <c r="DG11" t="n">
-        <v>4.38169425511196</v>
+        <v>3.70009737098344</v>
+      </c>
+      <c r="DH11" t="n">
+        <v>3.49115255858441</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -22826,12 +23006,15 @@
         <v>1.51387720773758</v>
       </c>
       <c r="DG12" t="n">
-        <v>1.48760330578512</v>
+        <v>1.73553719008264</v>
+      </c>
+      <c r="DH12" t="n">
+        <v>0.899427636958306</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -23161,12 +23344,15 @@
         <v>4.26829268292685</v>
       </c>
       <c r="DG13" t="n">
-        <v>3.79008746355686</v>
+        <v>5.24781341107873</v>
+      </c>
+      <c r="DH13" t="n">
+        <v>3.94366197183098</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -23278,10 +23464,11 @@
       <c r="DE14"/>
       <c r="DF14"/>
       <c r="DG14"/>
+      <c r="DH14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -23611,12 +23798,15 @@
         <v>0.839278220730172</v>
       </c>
       <c r="DG15" t="n">
-        <v>0.537079115885152</v>
+        <v>0.537079115885141</v>
+      </c>
+      <c r="DH15" t="n">
+        <v>0.206355757325629</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -23946,12 +24136,15 @@
         <v>2.84142988084327</v>
       </c>
       <c r="DG16" t="n">
-        <v>3.46715328467153</v>
+        <v>3.49756690997565</v>
+      </c>
+      <c r="DH16" t="n">
+        <v>3.11837723281865</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -24063,10 +24256,11 @@
       <c r="DE17"/>
       <c r="DF17"/>
       <c r="DG17"/>
+      <c r="DH17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -24396,12 +24590,15 @@
         <v>10.4129263913824</v>
       </c>
       <c r="DG18" t="n">
-        <v>7.45762711864407</v>
+        <v>7.6271186440678</v>
+      </c>
+      <c r="DH18" t="n">
+        <v>6.03015075376885</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -24732,11 +24929,14 @@
       </c>
       <c r="DG19" t="n">
         <v>5.73929961089492</v>
+      </c>
+      <c r="DH19" t="n">
+        <v>5.72390572390573</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -25066,12 +25266,15 @@
         <v>6.94378837978272</v>
       </c>
       <c r="DG20" t="n">
-        <v>10.0796999531177</v>
+        <v>9.3764650726676</v>
+      </c>
+      <c r="DH20" t="n">
+        <v>7.11030082041932</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -25401,12 +25604,15 @@
         <v>3.51008215085884</v>
       </c>
       <c r="DG21" t="n">
-        <v>4.02588066139465</v>
+        <v>3.09130122214233</v>
+      </c>
+      <c r="DH21" t="n">
+        <v>2.50178699070765</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -25736,12 +25942,15 @@
         <v>1.88976377952756</v>
       </c>
       <c r="DG22" t="n">
-        <v>0.829562594268472</v>
+        <v>0.678733031674213</v>
+      </c>
+      <c r="DH22" t="n">
+        <v>0.299177262528052</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -26071,12 +26280,15 @@
         <v>5.41838134430725</v>
       </c>
       <c r="DG23" t="n">
-        <v>6.57807308970098</v>
+        <v>4.38538205980066</v>
+      </c>
+      <c r="DH23" t="n">
+        <v>4.54545454545453</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -26406,12 +26618,15 @@
         <v>-0.209643605870009</v>
       </c>
       <c r="DG24" t="n">
-        <v>0.410958904109585</v>
+        <v>-1.43835616438358</v>
+      </c>
+      <c r="DH24" t="n">
+        <v>-1.50995195607412</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -26742,11 +26957,14 @@
       </c>
       <c r="DG25" t="n">
         <v>2.50000000000001</v>
+      </c>
+      <c r="DH25" t="n">
+        <v>0.409836065573776</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -27077,11 +27295,14 @@
       </c>
       <c r="DG26" t="n">
         <v>7.01402805611222</v>
+      </c>
+      <c r="DH26" t="n">
+        <v>6.74212598425196</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -27411,12 +27632,15 @@
         <v>3.98860398860399</v>
       </c>
       <c r="DG27" t="n">
-        <v>4.18943533697633</v>
+        <v>4.69034608378871</v>
+      </c>
+      <c r="DH27" t="n">
+        <v>4.23423423423422</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -27746,12 +27970,15 @@
         <v>3.23843416370108</v>
       </c>
       <c r="DG28" t="n">
-        <v>2.96321525885556</v>
+        <v>3.6784741144414</v>
+      </c>
+      <c r="DH28" t="n">
+        <v>3.48326006087251</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -28081,12 +28308,15 @@
         <v>3.17708333333333</v>
       </c>
       <c r="DG29" t="n">
-        <v>2.01409869083587</v>
+        <v>1.96374622356496</v>
+      </c>
+      <c r="DH29" t="n">
+        <v>1.2531328320802</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -28417,11 +28647,14 @@
       </c>
       <c r="DG30" t="n">
         <v>2.56410256410256</v>
+      </c>
+      <c r="DH30" t="n">
+        <v>1.96463654223967</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -28533,10 +28766,11 @@
       <c r="DE31"/>
       <c r="DF31"/>
       <c r="DG31"/>
+      <c r="DH31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -28866,12 +29100,15 @@
         <v>2.86396181384247</v>
       </c>
       <c r="DG32" t="n">
-        <v>3.25581395348837</v>
+        <v>2.55813953488372</v>
+      </c>
+      <c r="DH32" t="n">
+        <v>2.29357798165138</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -29202,11 +29439,14 @@
       </c>
       <c r="DG33" t="n">
         <v>2.75633958103638</v>
+      </c>
+      <c r="DH33" t="n">
+        <v>2.96703296703297</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -29537,11 +29777,14 @@
       </c>
       <c r="DG34" t="n">
         <v>2.14190093708165</v>
+      </c>
+      <c r="DH34" t="n">
+        <v>1.73102529960055</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -29871,12 +30114,15 @@
         <v>1.4423076923077</v>
       </c>
       <c r="DG35" t="n">
-        <v>3.60360360360361</v>
+        <v>1.35135135135135</v>
+      </c>
+      <c r="DH35" t="n">
+        <v>-0.44052863436124</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -30206,12 +30452,15 @@
         <v>7.01252236135958</v>
       </c>
       <c r="DG36" t="n">
-        <v>4.51745379876798</v>
+        <v>4.68856947296374</v>
+      </c>
+      <c r="DH36" t="n">
+        <v>4.76352500850629</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -30541,12 +30790,15 @@
         <v>6.20384047267359</v>
       </c>
       <c r="DG37" t="n">
-        <v>6.40668523676881</v>
+        <v>6.26740947075209</v>
+      </c>
+      <c r="DH37" t="n">
+        <v>6.17283950617284</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -30876,12 +31128,15 @@
         <v>6.90383365821962</v>
       </c>
       <c r="DG38" t="n">
-        <v>6.87579214195185</v>
+        <v>6.90747782002535</v>
+      </c>
+      <c r="DH38" t="n">
+        <v>6.90851735015774</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -31212,11 +31467,14 @@
       </c>
       <c r="DG39" t="n">
         <v>4.72005208333333</v>
+      </c>
+      <c r="DH39" t="n">
+        <v>4.07196969696969</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -31546,12 +31804,15 @@
         <v>6.16246498599439</v>
       </c>
       <c r="DG40" t="n">
-        <v>3.74331550802139</v>
+        <v>3.47593582887702</v>
+      </c>
+      <c r="DH40" t="n">
+        <v>4.58221024258759</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -31881,12 +32142,15 @@
         <v>-1.48066904304909</v>
       </c>
       <c r="DG41" t="n">
-        <v>-0.608948901244377</v>
+        <v>0.079428117553617</v>
+      </c>
+      <c r="DH41" t="n">
+        <v>1.29185341418402</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -32216,12 +32480,15 @@
         <v>2.27773695811903</v>
       </c>
       <c r="DG42" t="n">
-        <v>1.66666666666667</v>
+        <v>1.59722222222223</v>
+      </c>
+      <c r="DH42" t="n">
+        <v>1.86980609418282</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -32551,12 +32818,15 @@
         <v>7.03517587939698</v>
       </c>
       <c r="DG43" t="n">
-        <v>6.96150696150695</v>
+        <v>7.12530712530713</v>
+      </c>
+      <c r="DH43" t="n">
+        <v>6.21970920840064</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -32886,12 +33156,15 @@
         <v>2.5522041763341</v>
       </c>
       <c r="DG44" t="n">
-        <v>2.09191759112519</v>
+        <v>1.36291600633915</v>
+      </c>
+      <c r="DH44" t="n">
+        <v>0.311720698254364</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -33221,12 +33494,15 @@
         <v>2.15053763440861</v>
       </c>
       <c r="DG45" t="n">
-        <v>1.76056338028168</v>
+        <v>3.16901408450704</v>
+      </c>
+      <c r="DH45" t="n">
+        <v>3.52112676056339</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -33557,11 +33833,14 @@
       </c>
       <c r="DG46" t="n">
         <v>3.9622641509434</v>
+      </c>
+      <c r="DH46" t="n">
+        <v>4.12757973733583</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -33891,12 +34170,15 @@
         <v>2.56410256410258</v>
       </c>
       <c r="DG47" t="n">
-        <v>2.76243093922652</v>
+        <v>3.31491712707181</v>
+      </c>
+      <c r="DH47" t="n">
+        <v>3.01369863013699</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -34226,12 +34508,15 @@
         <v>1.99684708355228</v>
       </c>
       <c r="DG48" t="n">
-        <v>1.79461615154535</v>
+        <v>1.39581256231304</v>
+      </c>
+      <c r="DH48" t="n">
+        <v>1.54382470119523</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -34561,12 +34846,15 @@
         <v>2.41073874532005</v>
       </c>
       <c r="DG49" t="n">
-        <v>2.58853136796694</v>
+        <v>2.84019413985261</v>
+      </c>
+      <c r="DH49" t="n">
+        <v>2.96256396444925</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -34897,11 +35185,14 @@
       </c>
       <c r="DG50" t="n">
         <v>3.54200988467876</v>
+      </c>
+      <c r="DH50" t="n">
+        <v>3.34693877551021</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -35231,12 +35522,15 @@
         <v>6.42857142857142</v>
       </c>
       <c r="DG51" t="n">
-        <v>0</v>
+        <v>0.324675324675329</v>
+      </c>
+      <c r="DH51" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -35566,12 +35860,15 @@
         <v>2.34725578184329</v>
       </c>
       <c r="DG52" t="n">
-        <v>4.8140770252324</v>
+        <v>4.91367861885791</v>
+      </c>
+      <c r="DH52" t="n">
+        <v>4.36494913029209</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -35901,12 +36198,15 @@
         <v>6.95842450765863</v>
       </c>
       <c r="DG53" t="n">
-        <v>8.73324686554258</v>
+        <v>7.60916558581927</v>
+      </c>
+      <c r="DH53" t="n">
+        <v>6.11724723874257</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -36236,12 +36536,15 @@
         <v>4.06654343807764</v>
       </c>
       <c r="DG54" t="n">
-        <v>2.90598290598291</v>
+        <v>3.07692307692307</v>
+      </c>
+      <c r="DH54" t="n">
+        <v>1.01180438448567</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -36571,12 +36874,15 @@
         <v>3.69181380417336</v>
       </c>
       <c r="DG55" t="n">
-        <v>3.87518872672371</v>
+        <v>3.8751887267237</v>
+      </c>
+      <c r="DH55" t="n">
+        <v>3.59460808786819</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -36906,7 +37212,10 @@
         <v>1.41843971631205</v>
       </c>
       <c r="DG56" t="n">
-        <v>0.0000000000000120024110770287</v>
+        <v>0.337837837837843</v>
+      </c>
+      <c r="DH56" t="n">
+        <v>0.332225913621255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
May 20, 2022, update
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t xml:space="preserve">03/01/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/01/2022</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1245,10 +1248,13 @@
       <c r="DT4" t="s">
         <v>123</v>
       </c>
+      <c r="DU4" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1614,15 +1620,18 @@
         <v>10315.6</v>
       </c>
       <c r="DS5" t="n">
-        <v>10637.7</v>
+        <v>10643.2</v>
       </c>
       <c r="DT5" t="n">
-        <v>10693.8</v>
+        <v>10691.6</v>
+      </c>
+      <c r="DU5" t="n">
+        <v>10712.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -1991,12 +2000,15 @@
         <v>166.8</v>
       </c>
       <c r="DT6" t="n">
-        <v>169.2</v>
+        <v>168.1</v>
+      </c>
+      <c r="DU6" t="n">
+        <v>168.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2365,12 +2377,15 @@
         <v>27.6</v>
       </c>
       <c r="DT7" t="n">
-        <v>27.6</v>
+        <v>27.7</v>
+      </c>
+      <c r="DU7" t="n">
+        <v>27.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2740,11 +2755,14 @@
       </c>
       <c r="DT8" t="n">
         <v>194.4</v>
+      </c>
+      <c r="DU8" t="n">
+        <v>196.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3114,11 +3132,14 @@
       </c>
       <c r="DT9" t="n">
         <v>102.7</v>
+      </c>
+      <c r="DU9" t="n">
+        <v>103.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3487,12 +3508,15 @@
         <v>1203.6</v>
       </c>
       <c r="DT10" t="n">
-        <v>1215.4</v>
+        <v>1220.3</v>
+      </c>
+      <c r="DU10" t="n">
+        <v>1226.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -3861,12 +3885,15 @@
         <v>213</v>
       </c>
       <c r="DT11" t="n">
-        <v>216.4</v>
+        <v>215.1</v>
+      </c>
+      <c r="DU11" t="n">
+        <v>214.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4236,11 +4263,14 @@
       </c>
       <c r="DT12" t="n">
         <v>123.4</v>
+      </c>
+      <c r="DU12" t="n">
+        <v>122.8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4609,12 +4639,15 @@
         <v>36.1</v>
       </c>
       <c r="DT13" t="n">
-        <v>36.9</v>
+        <v>36.7</v>
+      </c>
+      <c r="DU13" t="n">
+        <v>36.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4739,10 +4772,11 @@
       <c r="DR14"/>
       <c r="DS14"/>
       <c r="DT14"/>
+      <c r="DU14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5111,12 +5145,15 @@
         <v>486.7</v>
       </c>
       <c r="DT15" t="n">
-        <v>485.6</v>
+        <v>485.7</v>
+      </c>
+      <c r="DU15" t="n">
+        <v>487.3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5485,12 +5522,15 @@
         <v>340.3</v>
       </c>
       <c r="DT16" t="n">
-        <v>340.6</v>
+        <v>340.9</v>
+      </c>
+      <c r="DU16" t="n">
+        <v>340.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -5615,10 +5655,11 @@
       <c r="DR17"/>
       <c r="DS17"/>
       <c r="DT17"/>
+      <c r="DU17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -5987,12 +6028,15 @@
         <v>63.5</v>
       </c>
       <c r="DT18" t="n">
-        <v>63.3</v>
+        <v>63.4</v>
+      </c>
+      <c r="DU18" t="n">
+        <v>63.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6361,12 +6405,15 @@
         <v>434.8</v>
       </c>
       <c r="DT19" t="n">
-        <v>439.6</v>
+        <v>436.4</v>
+      </c>
+      <c r="DU19" t="n">
+        <v>441.2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -6735,12 +6782,15 @@
         <v>233.3</v>
       </c>
       <c r="DT20" t="n">
-        <v>235</v>
+        <v>234</v>
+      </c>
+      <c r="DU20" t="n">
+        <v>233.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7109,12 +7159,15 @@
         <v>143.4</v>
       </c>
       <c r="DT21" t="n">
-        <v>143.4</v>
+        <v>143.6</v>
+      </c>
+      <c r="DU21" t="n">
+        <v>143.7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -7483,12 +7536,15 @@
         <v>133.5</v>
       </c>
       <c r="DT22" t="n">
-        <v>134.1</v>
+        <v>133.9</v>
+      </c>
+      <c r="DU22" t="n">
+        <v>133.9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -7857,12 +7913,15 @@
         <v>157.1</v>
       </c>
       <c r="DT23" t="n">
-        <v>158.7</v>
+        <v>158.4</v>
+      </c>
+      <c r="DU23" t="n">
+        <v>158.2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -8232,11 +8291,14 @@
       </c>
       <c r="DT24" t="n">
         <v>143.5</v>
+      </c>
+      <c r="DU24" t="n">
+        <v>143.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -8605,12 +8667,15 @@
         <v>49.2</v>
       </c>
       <c r="DT25" t="n">
-        <v>49</v>
+        <v>49.2</v>
+      </c>
+      <c r="DU25" t="n">
+        <v>48.9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -8980,11 +9045,14 @@
       </c>
       <c r="DT26" t="n">
         <v>216.9</v>
+      </c>
+      <c r="DU26" t="n">
+        <v>217.9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -9353,12 +9421,15 @@
         <v>229.9</v>
       </c>
       <c r="DT27" t="n">
-        <v>231.4</v>
+        <v>231.1</v>
+      </c>
+      <c r="DU27" t="n">
+        <v>231.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -9727,12 +9798,15 @@
         <v>304.4</v>
       </c>
       <c r="DT28" t="n">
-        <v>306</v>
+        <v>305.6</v>
+      </c>
+      <c r="DU28" t="n">
+        <v>306.4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -10102,11 +10176,14 @@
       </c>
       <c r="DT29" t="n">
         <v>202</v>
+      </c>
+      <c r="DU29" t="n">
+        <v>202.4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -10475,12 +10552,15 @@
         <v>104</v>
       </c>
       <c r="DT30" t="n">
-        <v>103.8</v>
+        <v>103.9</v>
+      </c>
+      <c r="DU30" t="n">
+        <v>103.9</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -10605,10 +10685,11 @@
       <c r="DR31"/>
       <c r="DS31"/>
       <c r="DT31"/>
+      <c r="DU31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -10977,12 +11058,15 @@
         <v>44.1</v>
       </c>
       <c r="DT32" t="n">
-        <v>44.6</v>
+        <v>44.2</v>
+      </c>
+      <c r="DU32" t="n">
+        <v>43.9</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -11351,12 +11435,15 @@
         <v>93.2</v>
       </c>
       <c r="DT33" t="n">
-        <v>93.7</v>
+        <v>93.8</v>
+      </c>
+      <c r="DU33" t="n">
+        <v>93.8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -11725,12 +11812,15 @@
         <v>76.3</v>
       </c>
       <c r="DT34" t="n">
-        <v>76.4</v>
+        <v>76.6</v>
+      </c>
+      <c r="DU34" t="n">
+        <v>76.2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -12099,12 +12189,15 @@
         <v>45</v>
       </c>
       <c r="DT35" t="n">
-        <v>45.2</v>
+        <v>44.8</v>
+      </c>
+      <c r="DU35" t="n">
+        <v>44.8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -12473,12 +12566,15 @@
         <v>305.9</v>
       </c>
       <c r="DT36" t="n">
-        <v>307.9</v>
+        <v>307.8</v>
+      </c>
+      <c r="DU36" t="n">
+        <v>309.6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -12847,12 +12943,15 @@
         <v>76.3</v>
       </c>
       <c r="DT37" t="n">
-        <v>77.4</v>
+        <v>77</v>
+      </c>
+      <c r="DU37" t="n">
+        <v>77.1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -13221,12 +13320,15 @@
         <v>674.8</v>
       </c>
       <c r="DT38" t="n">
-        <v>677.8</v>
+        <v>678.3</v>
+      </c>
+      <c r="DU38" t="n">
+        <v>683.9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -13596,11 +13698,14 @@
       </c>
       <c r="DT39" t="n">
         <v>329.7</v>
+      </c>
+      <c r="DU39" t="n">
+        <v>330.9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -13970,11 +14075,14 @@
       </c>
       <c r="DT40" t="n">
         <v>38.8</v>
+      </c>
+      <c r="DU40" t="n">
+        <v>39.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -14343,12 +14451,15 @@
         <v>378</v>
       </c>
       <c r="DT41" t="n">
-        <v>384.2</v>
+        <v>382.2</v>
+      </c>
+      <c r="DU41" t="n">
+        <v>380.5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -14717,12 +14828,15 @@
         <v>146.3</v>
       </c>
       <c r="DT42" t="n">
-        <v>147.1</v>
+        <v>147.2</v>
+      </c>
+      <c r="DU42" t="n">
+        <v>148.1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -15091,12 +15205,15 @@
         <v>130.8</v>
       </c>
       <c r="DT43" t="n">
-        <v>131.5</v>
+        <v>131.8</v>
+      </c>
+      <c r="DU43" t="n">
+        <v>131.8</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -15465,12 +15582,15 @@
         <v>319.8</v>
       </c>
       <c r="DT44" t="n">
-        <v>321.8</v>
+        <v>321.1</v>
+      </c>
+      <c r="DU44" t="n">
+        <v>321</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -15840,11 +15960,14 @@
       </c>
       <c r="DT45" t="n">
         <v>29.4</v>
+      </c>
+      <c r="DU45" t="n">
+        <v>29.6</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -16213,12 +16336,15 @@
         <v>165.3</v>
       </c>
       <c r="DT46" t="n">
-        <v>166.5</v>
+        <v>166.6</v>
+      </c>
+      <c r="DU46" t="n">
+        <v>166.7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -16587,12 +16713,15 @@
         <v>37.4</v>
       </c>
       <c r="DT47" t="n">
-        <v>37.6</v>
+        <v>37.5</v>
+      </c>
+      <c r="DU47" t="n">
+        <v>37.1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -16961,12 +17090,15 @@
         <v>203.4</v>
       </c>
       <c r="DT48" t="n">
-        <v>203.9</v>
+        <v>204.4</v>
+      </c>
+      <c r="DU48" t="n">
+        <v>203.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -17335,12 +17467,15 @@
         <v>1144.2</v>
       </c>
       <c r="DT49" t="n">
-        <v>1146.9</v>
+        <v>1146.7</v>
+      </c>
+      <c r="DU49" t="n">
+        <v>1147.1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -17710,11 +17845,14 @@
       </c>
       <c r="DT50" t="n">
         <v>126.6</v>
+      </c>
+      <c r="DU50" t="n">
+        <v>125.9</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -18083,12 +18221,15 @@
         <v>30.9</v>
       </c>
       <c r="DT51" t="n">
-        <v>30.3</v>
+        <v>30.7</v>
+      </c>
+      <c r="DU51" t="n">
+        <v>30.9</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -18457,12 +18598,15 @@
         <v>316</v>
       </c>
       <c r="DT52" t="n">
-        <v>318</v>
+        <v>316.6</v>
+      </c>
+      <c r="DU52" t="n">
+        <v>318.5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -18831,12 +18975,15 @@
         <v>248.9</v>
       </c>
       <c r="DT53" t="n">
-        <v>249.8</v>
+        <v>250.4</v>
+      </c>
+      <c r="DU53" t="n">
+        <v>253.9</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -19205,12 +19352,15 @@
         <v>60.3</v>
       </c>
       <c r="DT54" t="n">
-        <v>59.9</v>
+        <v>60.7</v>
+      </c>
+      <c r="DU54" t="n">
+        <v>60.8</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -19579,12 +19729,15 @@
         <v>206.4</v>
       </c>
       <c r="DT55" t="n">
-        <v>207.5</v>
+        <v>207.4</v>
+      </c>
+      <c r="DU55" t="n">
+        <v>208.9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -19954,6 +20107,9 @@
       </c>
       <c r="DT56" t="n">
         <v>30.2</v>
+      </c>
+      <c r="DU56" t="n">
+        <v>30.1</v>
       </c>
     </row>
   </sheetData>
@@ -20307,10 +20463,13 @@
       <c r="DH4" t="s">
         <v>123</v>
       </c>
+      <c r="DI4" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -20640,15 +20799,18 @@
         <v>3.8674923224085</v>
       </c>
       <c r="DG5" t="n">
-        <v>3.76016854918944</v>
+        <v>3.81381557129201</v>
       </c>
       <c r="DH5" t="n">
-        <v>3.1453456407882</v>
+        <v>3.12412589098834</v>
+      </c>
+      <c r="DI5" t="n">
+        <v>2.93148342092872</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -20981,12 +21143,15 @@
         <v>2.33128834355829</v>
       </c>
       <c r="DH6" t="n">
-        <v>3.04506699147381</v>
+        <v>2.37515225334958</v>
+      </c>
+      <c r="DI6" t="n">
+        <v>2.61557177615571</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -21319,12 +21484,15 @@
         <v>1.0989010989011</v>
       </c>
       <c r="DH7" t="n">
-        <v>1.09890109890109</v>
+        <v>1.46520146520146</v>
+      </c>
+      <c r="DI7" t="n">
+        <v>0.724637681159418</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -21658,11 +21826,14 @@
       </c>
       <c r="DH8" t="n">
         <v>2.26196738558652</v>
+      </c>
+      <c r="DI8" t="n">
+        <v>2.93193717277487</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -21996,11 +22167,14 @@
       </c>
       <c r="DH9" t="n">
         <v>2.39282153539382</v>
+      </c>
+      <c r="DI9" t="n">
+        <v>2.37859266600594</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -22333,12 +22507,15 @@
         <v>7.55071039227949</v>
       </c>
       <c r="DH10" t="n">
-        <v>6.99885553305751</v>
+        <v>7.43023153446607</v>
+      </c>
+      <c r="DI10" t="n">
+        <v>6.54270570857591</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -22671,12 +22848,15 @@
         <v>3.70009737098344</v>
       </c>
       <c r="DH11" t="n">
-        <v>3.49115255858441</v>
+        <v>2.86944045911047</v>
+      </c>
+      <c r="DI11" t="n">
+        <v>2.19570405727923</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -23010,11 +23190,14 @@
       </c>
       <c r="DH12" t="n">
         <v>0.899427636958306</v>
+      </c>
+      <c r="DI12" t="n">
+        <v>1.15321252059307</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -23347,12 +23530,15 @@
         <v>5.24781341107873</v>
       </c>
       <c r="DH13" t="n">
-        <v>3.94366197183098</v>
+        <v>3.38028169014085</v>
+      </c>
+      <c r="DI13" t="n">
+        <v>1.66204986149585</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -23465,10 +23651,11 @@
       <c r="DF14"/>
       <c r="DG14"/>
       <c r="DH14"/>
+      <c r="DI14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -23801,12 +23988,15 @@
         <v>0.537079115885141</v>
       </c>
       <c r="DH15" t="n">
-        <v>0.206355757325629</v>
+        <v>0.226991333058185</v>
+      </c>
+      <c r="DI15" t="n">
+        <v>1.26766417290109</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -24139,12 +24329,15 @@
         <v>3.49756690997565</v>
       </c>
       <c r="DH16" t="n">
-        <v>3.11837723281865</v>
+        <v>3.20920375416287</v>
+      </c>
+      <c r="DI16" t="n">
+        <v>2.93317205926822</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -24257,10 +24450,11 @@
       <c r="DF17"/>
       <c r="DG17"/>
       <c r="DH17"/>
+      <c r="DI17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -24593,12 +24787,15 @@
         <v>7.6271186440678</v>
       </c>
       <c r="DH18" t="n">
-        <v>6.03015075376885</v>
+        <v>6.19765494137355</v>
+      </c>
+      <c r="DI18" t="n">
+        <v>7.41989881956155</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -24931,12 +25128,15 @@
         <v>5.73929961089492</v>
       </c>
       <c r="DH19" t="n">
-        <v>5.72390572390573</v>
+        <v>4.95430495430495</v>
+      </c>
+      <c r="DI19" t="n">
+        <v>5.02261366341349</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -25269,12 +25469,15 @@
         <v>9.3764650726676</v>
       </c>
       <c r="DH20" t="n">
-        <v>7.11030082041932</v>
+        <v>6.65451230628988</v>
+      </c>
+      <c r="DI20" t="n">
+        <v>6.3868613138686</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -25607,12 +25810,15 @@
         <v>3.09130122214233</v>
       </c>
       <c r="DH21" t="n">
-        <v>2.50178699070765</v>
+        <v>2.64474624731953</v>
+      </c>
+      <c r="DI21" t="n">
+        <v>2.49643366619116</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -25945,12 +26151,15 @@
         <v>0.678733031674213</v>
       </c>
       <c r="DH22" t="n">
-        <v>0.299177262528052</v>
+        <v>0.149588631264037</v>
+      </c>
+      <c r="DI22" t="n">
+        <v>0.149588631264037</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -26283,12 +26492,15 @@
         <v>4.38538205980066</v>
       </c>
       <c r="DH23" t="n">
-        <v>4.54545454545453</v>
+        <v>4.34782608695652</v>
+      </c>
+      <c r="DI23" t="n">
+        <v>3.26370757180157</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -26622,11 +26834,14 @@
       </c>
       <c r="DH24" t="n">
         <v>-1.50995195607412</v>
+      </c>
+      <c r="DI24" t="n">
+        <v>-2.05058099794942</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -26959,12 +27174,15 @@
         <v>2.50000000000001</v>
       </c>
       <c r="DH25" t="n">
-        <v>0.409836065573776</v>
+        <v>0.819672131147553</v>
+      </c>
+      <c r="DI25" t="n">
+        <v>0.204918032786888</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -27298,11 +27516,14 @@
       </c>
       <c r="DH26" t="n">
         <v>6.74212598425196</v>
+      </c>
+      <c r="DI26" t="n">
+        <v>5.46950629235238</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -27635,12 +27856,15 @@
         <v>4.69034608378871</v>
       </c>
       <c r="DH27" t="n">
-        <v>4.23423423423422</v>
+        <v>4.0990990990991</v>
+      </c>
+      <c r="DI27" t="n">
+        <v>2.52100840336134</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -27973,12 +28197,15 @@
         <v>3.6784741144414</v>
       </c>
       <c r="DH28" t="n">
-        <v>3.48326006087251</v>
+        <v>3.34798782549883</v>
+      </c>
+      <c r="DI28" t="n">
+        <v>4.18225093505609</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -28312,11 +28539,14 @@
       </c>
       <c r="DH29" t="n">
         <v>1.2531328320802</v>
+      </c>
+      <c r="DI29" t="n">
+        <v>0.847035376183353</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -28649,12 +28879,15 @@
         <v>2.56410256410256</v>
       </c>
       <c r="DH30" t="n">
-        <v>1.96463654223967</v>
+        <v>2.06286836935165</v>
+      </c>
+      <c r="DI30" t="n">
+        <v>1.96270853778214</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -28767,10 +29000,11 @@
       <c r="DF31"/>
       <c r="DG31"/>
       <c r="DH31"/>
+      <c r="DI31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -29103,12 +29337,15 @@
         <v>2.55813953488372</v>
       </c>
       <c r="DH32" t="n">
-        <v>2.29357798165138</v>
+        <v>1.37614678899083</v>
+      </c>
+      <c r="DI32" t="n">
+        <v>0.919540229885071</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -29441,12 +29678,15 @@
         <v>2.75633958103638</v>
       </c>
       <c r="DH33" t="n">
-        <v>2.96703296703297</v>
+        <v>3.07692307692307</v>
+      </c>
+      <c r="DI33" t="n">
+        <v>2.06746463547333</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -29779,12 +30019,15 @@
         <v>2.14190093708165</v>
       </c>
       <c r="DH34" t="n">
-        <v>1.73102529960055</v>
+        <v>1.99733688415446</v>
+      </c>
+      <c r="DI34" t="n">
+        <v>1.8716577540107</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -30117,12 +30360,15 @@
         <v>1.35135135135135</v>
       </c>
       <c r="DH35" t="n">
-        <v>-0.44052863436124</v>
+        <v>-1.3215859030837</v>
+      </c>
+      <c r="DI35" t="n">
+        <v>-2.18340611353713</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -30455,12 +30701,15 @@
         <v>4.68856947296374</v>
       </c>
       <c r="DH36" t="n">
-        <v>4.76352500850629</v>
+        <v>4.72949982987412</v>
+      </c>
+      <c r="DI36" t="n">
+        <v>4.52397029034437</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -30793,12 +31042,15 @@
         <v>6.26740947075209</v>
       </c>
       <c r="DH37" t="n">
-        <v>6.17283950617284</v>
+        <v>5.62414266117969</v>
+      </c>
+      <c r="DI37" t="n">
+        <v>5.47195622435021</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -31131,12 +31383,15 @@
         <v>6.90747782002535</v>
       </c>
       <c r="DH38" t="n">
-        <v>6.90851735015774</v>
+        <v>6.98738170347004</v>
+      </c>
+      <c r="DI38" t="n">
+        <v>7.75169371356549</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -31470,11 +31725,14 @@
       </c>
       <c r="DH39" t="n">
         <v>4.07196969696969</v>
+      </c>
+      <c r="DI39" t="n">
+        <v>3.63294707171938</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -31808,11 +32066,14 @@
       </c>
       <c r="DH40" t="n">
         <v>4.58221024258759</v>
+      </c>
+      <c r="DI40" t="n">
+        <v>5.39083557951482</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -32145,12 +32406,15 @@
         <v>0.079428117553617</v>
       </c>
       <c r="DH41" t="n">
-        <v>1.29185341418402</v>
+        <v>0.764566306353819</v>
+      </c>
+      <c r="DI41" t="n">
+        <v>-0.62679550796552</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -32483,12 +32747,15 @@
         <v>1.59722222222223</v>
       </c>
       <c r="DH42" t="n">
-        <v>1.86980609418282</v>
+        <v>1.93905817174514</v>
+      </c>
+      <c r="DI42" t="n">
+        <v>1.64722031571723</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -32821,12 +33088,15 @@
         <v>7.12530712530713</v>
       </c>
       <c r="DH43" t="n">
-        <v>6.21970920840064</v>
+        <v>6.46203554119545</v>
+      </c>
+      <c r="DI43" t="n">
+        <v>4.27215189873416</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -33159,12 +33429,15 @@
         <v>1.36291600633915</v>
       </c>
       <c r="DH44" t="n">
-        <v>0.311720698254364</v>
+        <v>0.0935162094763128</v>
+      </c>
+      <c r="DI44" t="n">
+        <v>0.249843847595239</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -33498,11 +33771,14 @@
       </c>
       <c r="DH45" t="n">
         <v>3.52112676056339</v>
+      </c>
+      <c r="DI45" t="n">
+        <v>3.85964912280702</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -33835,12 +34111,15 @@
         <v>3.9622641509434</v>
       </c>
       <c r="DH46" t="n">
-        <v>4.12757973733583</v>
+        <v>4.19011882426516</v>
+      </c>
+      <c r="DI46" t="n">
+        <v>4.25265791119449</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -34173,12 +34452,15 @@
         <v>3.31491712707181</v>
       </c>
       <c r="DH47" t="n">
-        <v>3.01369863013699</v>
+        <v>2.73972602739726</v>
+      </c>
+      <c r="DI47" t="n">
+        <v>1.92307692307693</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -34511,12 +34793,15 @@
         <v>1.39581256231304</v>
       </c>
       <c r="DH48" t="n">
-        <v>1.54382470119523</v>
+        <v>1.79282868525896</v>
+      </c>
+      <c r="DI48" t="n">
+        <v>1.04270109235352</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -34849,12 +35134,15 @@
         <v>2.84019413985261</v>
       </c>
       <c r="DH49" t="n">
-        <v>2.96256396444925</v>
+        <v>2.94460903133138</v>
+      </c>
+      <c r="DI49" t="n">
+        <v>2.95279124035181</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -35188,11 +35476,14 @@
       </c>
       <c r="DH50" t="n">
         <v>3.34693877551021</v>
+      </c>
+      <c r="DI50" t="n">
+        <v>3.53618421052633</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -35525,12 +35816,15 @@
         <v>0.324675324675329</v>
       </c>
       <c r="DH51" t="n">
-        <v>1</v>
+        <v>2.33333333333333</v>
+      </c>
+      <c r="DI51" t="n">
+        <v>2.31788079470197</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -35863,12 +36157,15 @@
         <v>4.91367861885791</v>
       </c>
       <c r="DH52" t="n">
-        <v>4.36494913029209</v>
+        <v>3.90548080078767</v>
+      </c>
+      <c r="DI52" t="n">
+        <v>3.67838541666667</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -36201,12 +36498,15 @@
         <v>7.60916558581927</v>
       </c>
       <c r="DH53" t="n">
-        <v>6.11724723874257</v>
+        <v>6.37213254035683</v>
+      </c>
+      <c r="DI53" t="n">
+        <v>4.96072757337743</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -36539,12 +36839,15 @@
         <v>3.07692307692307</v>
       </c>
       <c r="DH54" t="n">
-        <v>1.01180438448567</v>
+        <v>2.36087689713321</v>
+      </c>
+      <c r="DI54" t="n">
+        <v>1.16472545757072</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -36877,12 +37180,15 @@
         <v>3.8751887267237</v>
       </c>
       <c r="DH55" t="n">
-        <v>3.59460808786819</v>
+        <v>3.54468297553668</v>
+      </c>
+      <c r="DI55" t="n">
+        <v>3.1604938271605</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -37216,6 +37522,9 @@
       </c>
       <c r="DH56" t="n">
         <v>0.332225913621255</v>
+      </c>
+      <c r="DI56" t="n">
+        <v>1.00671140939598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
June 17, 2022, update
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t xml:space="preserve">04/01/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/01/2022</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1251,10 +1254,13 @@
       <c r="DU4" t="s">
         <v>124</v>
       </c>
+      <c r="DV4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1623,15 +1629,18 @@
         <v>10643.2</v>
       </c>
       <c r="DT5" t="n">
-        <v>10691.6</v>
+        <v>10692.1</v>
       </c>
       <c r="DU5" t="n">
-        <v>10712.8</v>
+        <v>10717.6</v>
+      </c>
+      <c r="DV5" t="n">
+        <v>10609.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2003,12 +2012,15 @@
         <v>168.1</v>
       </c>
       <c r="DU6" t="n">
-        <v>168.7</v>
+        <v>169.3</v>
+      </c>
+      <c r="DV6" t="n">
+        <v>169.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2381,11 +2393,14 @@
       </c>
       <c r="DU7" t="n">
         <v>27.8</v>
+      </c>
+      <c r="DV7" t="n">
+        <v>26.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2757,12 +2772,15 @@
         <v>194.4</v>
       </c>
       <c r="DU8" t="n">
-        <v>196.6</v>
+        <v>196.5</v>
+      </c>
+      <c r="DV8" t="n">
+        <v>188.4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3135,11 +3153,14 @@
       </c>
       <c r="DU9" t="n">
         <v>103.3</v>
+      </c>
+      <c r="DV9" t="n">
+        <v>102.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3511,12 +3532,15 @@
         <v>1220.3</v>
       </c>
       <c r="DU10" t="n">
-        <v>1226.2</v>
+        <v>1224.1</v>
+      </c>
+      <c r="DV10" t="n">
+        <v>1236.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -3889,11 +3913,14 @@
       </c>
       <c r="DU11" t="n">
         <v>214.1</v>
+      </c>
+      <c r="DV11" t="n">
+        <v>215.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4265,12 +4292,15 @@
         <v>123.4</v>
       </c>
       <c r="DU12" t="n">
-        <v>122.8</v>
+        <v>122.5</v>
+      </c>
+      <c r="DV12" t="n">
+        <v>119.3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4642,12 +4672,15 @@
         <v>36.7</v>
       </c>
       <c r="DU13" t="n">
-        <v>36.7</v>
+        <v>36.5</v>
+      </c>
+      <c r="DV13" t="n">
+        <v>35.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4773,10 +4806,11 @@
       <c r="DS14"/>
       <c r="DT14"/>
       <c r="DU14"/>
+      <c r="DV14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5148,12 +5182,15 @@
         <v>485.7</v>
       </c>
       <c r="DU15" t="n">
-        <v>487.3</v>
+        <v>487.2</v>
+      </c>
+      <c r="DV15" t="n">
+        <v>485.9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5525,12 +5562,15 @@
         <v>340.9</v>
       </c>
       <c r="DU16" t="n">
-        <v>340.4</v>
+        <v>340.5</v>
+      </c>
+      <c r="DV16" t="n">
+        <v>337</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -5656,10 +5696,11 @@
       <c r="DS17"/>
       <c r="DT17"/>
       <c r="DU17"/>
+      <c r="DV17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6031,12 +6072,15 @@
         <v>63.4</v>
       </c>
       <c r="DU18" t="n">
-        <v>63.7</v>
+        <v>64.1</v>
+      </c>
+      <c r="DV18" t="n">
+        <v>62.1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6409,11 +6453,14 @@
       </c>
       <c r="DU19" t="n">
         <v>441.2</v>
+      </c>
+      <c r="DV19" t="n">
+        <v>440.4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -6785,12 +6832,15 @@
         <v>234</v>
       </c>
       <c r="DU20" t="n">
-        <v>233.2</v>
+        <v>233.4</v>
+      </c>
+      <c r="DV20" t="n">
+        <v>227.3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7163,11 +7213,14 @@
       </c>
       <c r="DU21" t="n">
         <v>143.7</v>
+      </c>
+      <c r="DV21" t="n">
+        <v>143.5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -7539,12 +7592,15 @@
         <v>133.9</v>
       </c>
       <c r="DU22" t="n">
-        <v>133.9</v>
+        <v>134</v>
+      </c>
+      <c r="DV22" t="n">
+        <v>134.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -7916,12 +7972,15 @@
         <v>158.4</v>
       </c>
       <c r="DU23" t="n">
-        <v>158.2</v>
+        <v>158.5</v>
+      </c>
+      <c r="DV23" t="n">
+        <v>154.6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -8294,11 +8353,14 @@
       </c>
       <c r="DU24" t="n">
         <v>143.3</v>
+      </c>
+      <c r="DV24" t="n">
+        <v>143.8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -8671,11 +8733,14 @@
       </c>
       <c r="DU25" t="n">
         <v>48.9</v>
+      </c>
+      <c r="DV25" t="n">
+        <v>48.1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9048,11 +9113,14 @@
       </c>
       <c r="DU26" t="n">
         <v>217.9</v>
+      </c>
+      <c r="DV26" t="n">
+        <v>218.6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -9424,12 +9492,15 @@
         <v>231.1</v>
       </c>
       <c r="DU27" t="n">
-        <v>231.8</v>
+        <v>231.5</v>
+      </c>
+      <c r="DV27" t="n">
+        <v>232</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -9801,12 +9872,15 @@
         <v>305.6</v>
       </c>
       <c r="DU28" t="n">
-        <v>306.4</v>
+        <v>306.9</v>
+      </c>
+      <c r="DV28" t="n">
+        <v>283.4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -10178,12 +10252,15 @@
         <v>202</v>
       </c>
       <c r="DU29" t="n">
-        <v>202.4</v>
+        <v>201.6</v>
+      </c>
+      <c r="DV29" t="n">
+        <v>199.5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -10555,12 +10632,15 @@
         <v>103.9</v>
       </c>
       <c r="DU30" t="n">
-        <v>103.9</v>
+        <v>103.8</v>
+      </c>
+      <c r="DV30" t="n">
+        <v>102.6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -10686,10 +10766,11 @@
       <c r="DS31"/>
       <c r="DT31"/>
       <c r="DU31"/>
+      <c r="DV31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -11062,11 +11143,14 @@
       </c>
       <c r="DU32" t="n">
         <v>43.9</v>
+      </c>
+      <c r="DV32" t="n">
+        <v>43.8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -11438,12 +11522,15 @@
         <v>93.8</v>
       </c>
       <c r="DU33" t="n">
-        <v>93.8</v>
+        <v>93.9</v>
+      </c>
+      <c r="DV33" t="n">
+        <v>93.9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -11815,12 +11902,15 @@
         <v>76.6</v>
       </c>
       <c r="DU34" t="n">
-        <v>76.2</v>
+        <v>76.3</v>
+      </c>
+      <c r="DV34" t="n">
+        <v>76.3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -12192,12 +12282,15 @@
         <v>44.8</v>
       </c>
       <c r="DU35" t="n">
-        <v>44.8</v>
+        <v>45</v>
+      </c>
+      <c r="DV35" t="n">
+        <v>44.2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -12570,11 +12663,14 @@
       </c>
       <c r="DU36" t="n">
         <v>309.6</v>
+      </c>
+      <c r="DV36" t="n">
+        <v>305.5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -12947,11 +13043,14 @@
       </c>
       <c r="DU37" t="n">
         <v>77.1</v>
+      </c>
+      <c r="DV37" t="n">
+        <v>76.5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -13323,12 +13422,15 @@
         <v>678.3</v>
       </c>
       <c r="DU38" t="n">
-        <v>683.9</v>
+        <v>683.7</v>
+      </c>
+      <c r="DV38" t="n">
+        <v>680.7</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -13701,11 +13803,14 @@
       </c>
       <c r="DU39" t="n">
         <v>330.9</v>
+      </c>
+      <c r="DV39" t="n">
+        <v>328.4</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -14078,11 +14183,14 @@
       </c>
       <c r="DU40" t="n">
         <v>39.1</v>
+      </c>
+      <c r="DV40" t="n">
+        <v>38.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -14454,12 +14562,15 @@
         <v>382.2</v>
       </c>
       <c r="DU41" t="n">
-        <v>380.5</v>
+        <v>381</v>
+      </c>
+      <c r="DV41" t="n">
+        <v>372.8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -14831,12 +14942,15 @@
         <v>147.2</v>
       </c>
       <c r="DU42" t="n">
-        <v>148.1</v>
+        <v>148.2</v>
+      </c>
+      <c r="DV42" t="n">
+        <v>147.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -15209,11 +15323,14 @@
       </c>
       <c r="DU43" t="n">
         <v>131.8</v>
+      </c>
+      <c r="DV43" t="n">
+        <v>132.2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -15586,11 +15703,14 @@
       </c>
       <c r="DU44" t="n">
         <v>321</v>
+      </c>
+      <c r="DV44" t="n">
+        <v>318.1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -15963,11 +16083,14 @@
       </c>
       <c r="DU45" t="n">
         <v>29.6</v>
+      </c>
+      <c r="DV45" t="n">
+        <v>29.3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -16340,11 +16463,14 @@
       </c>
       <c r="DU46" t="n">
         <v>166.7</v>
+      </c>
+      <c r="DV46" t="n">
+        <v>165.2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -16716,12 +16842,15 @@
         <v>37.5</v>
       </c>
       <c r="DU47" t="n">
-        <v>37.1</v>
+        <v>37.3</v>
+      </c>
+      <c r="DV47" t="n">
+        <v>36.8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -17094,11 +17223,14 @@
       </c>
       <c r="DU48" t="n">
         <v>203.5</v>
+      </c>
+      <c r="DV48" t="n">
+        <v>200.8</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -17470,12 +17602,15 @@
         <v>1146.7</v>
       </c>
       <c r="DU49" t="n">
-        <v>1147.1</v>
+        <v>1146.8</v>
+      </c>
+      <c r="DV49" t="n">
+        <v>1142.6</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -17848,11 +17983,14 @@
       </c>
       <c r="DU50" t="n">
         <v>125.9</v>
+      </c>
+      <c r="DV50" t="n">
+        <v>125.4</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -18225,11 +18363,14 @@
       </c>
       <c r="DU51" t="n">
         <v>30.9</v>
+      </c>
+      <c r="DV51" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -18602,11 +18743,14 @@
       </c>
       <c r="DU52" t="n">
         <v>318.5</v>
+      </c>
+      <c r="DV52" t="n">
+        <v>310.4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -18979,11 +19123,14 @@
       </c>
       <c r="DU53" t="n">
         <v>253.9</v>
+      </c>
+      <c r="DV53" t="n">
+        <v>254.7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -19356,11 +19503,14 @@
       </c>
       <c r="DU54" t="n">
         <v>60.8</v>
+      </c>
+      <c r="DV54" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -19732,12 +19882,15 @@
         <v>207.4</v>
       </c>
       <c r="DU55" t="n">
-        <v>208.9</v>
+        <v>208.7</v>
+      </c>
+      <c r="DV55" t="n">
+        <v>205.2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -20109,6 +20262,9 @@
         <v>30.2</v>
       </c>
       <c r="DU56" t="n">
+        <v>30.1</v>
+      </c>
+      <c r="DV56" t="n">
         <v>30.1</v>
       </c>
     </row>
@@ -20466,10 +20622,13 @@
       <c r="DI4" t="s">
         <v>124</v>
       </c>
+      <c r="DJ4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -20802,15 +20961,18 @@
         <v>3.81381557129201</v>
       </c>
       <c r="DH5" t="n">
-        <v>3.12412589098834</v>
+        <v>3.12894856139741</v>
       </c>
       <c r="DI5" t="n">
-        <v>2.93148342092872</v>
+        <v>2.97760312076633</v>
+      </c>
+      <c r="DJ5" t="n">
+        <v>2.93601125503324</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -21146,12 +21308,15 @@
         <v>2.37515225334958</v>
       </c>
       <c r="DI6" t="n">
-        <v>2.61557177615571</v>
+        <v>2.98053527980536</v>
+      </c>
+      <c r="DJ6" t="n">
+        <v>2.91262135922329</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -21488,11 +21653,14 @@
       </c>
       <c r="DI7" t="n">
         <v>0.724637681159418</v>
+      </c>
+      <c r="DJ7" t="n">
+        <v>0.0000000000000135084170296597</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -21828,12 +21996,15 @@
         <v>2.26196738558652</v>
       </c>
       <c r="DI8" t="n">
-        <v>2.93193717277487</v>
+        <v>2.87958115183246</v>
+      </c>
+      <c r="DJ8" t="n">
+        <v>2.39130434782607</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -22170,11 +22341,14 @@
       </c>
       <c r="DI9" t="n">
         <v>2.37859266600594</v>
+      </c>
+      <c r="DJ9" t="n">
+        <v>2.40240240240239</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -22510,12 +22684,15 @@
         <v>7.43023153446607</v>
       </c>
       <c r="DI10" t="n">
-        <v>6.54270570857591</v>
+        <v>6.3602398123208</v>
+      </c>
+      <c r="DJ10" t="n">
+        <v>5.74899478141841</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -22852,11 +23029,14 @@
       </c>
       <c r="DI11" t="n">
         <v>2.19570405727923</v>
+      </c>
+      <c r="DJ11" t="n">
+        <v>2.28245363766049</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -23192,12 +23372,15 @@
         <v>0.899427636958306</v>
       </c>
       <c r="DI12" t="n">
-        <v>1.15321252059307</v>
+        <v>0.906095551894559</v>
+      </c>
+      <c r="DJ12" t="n">
+        <v>0.336417157275026</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -23533,12 +23716,15 @@
         <v>3.38028169014085</v>
       </c>
       <c r="DI13" t="n">
-        <v>1.66204986149585</v>
+        <v>1.10803324099723</v>
+      </c>
+      <c r="DJ13" t="n">
+        <v>0.852272727272719</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -23652,10 +23838,11 @@
       <c r="DG14"/>
       <c r="DH14"/>
       <c r="DI14"/>
+      <c r="DJ14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -23991,12 +24178,15 @@
         <v>0.226991333058185</v>
       </c>
       <c r="DI15" t="n">
-        <v>1.26766417290109</v>
+        <v>1.24688279301746</v>
+      </c>
+      <c r="DJ15" t="n">
+        <v>2.77072758037226</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -24332,12 +24522,15 @@
         <v>3.20920375416287</v>
       </c>
       <c r="DI16" t="n">
-        <v>2.93317205926822</v>
+        <v>2.96341094647717</v>
+      </c>
+      <c r="DJ16" t="n">
+        <v>2.27617602427921</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -24451,10 +24644,11 @@
       <c r="DG17"/>
       <c r="DH17"/>
       <c r="DI17"/>
+      <c r="DJ17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -24790,12 +24984,15 @@
         <v>6.19765494137355</v>
       </c>
       <c r="DI18" t="n">
-        <v>7.41989881956155</v>
+        <v>8.09443507588531</v>
+      </c>
+      <c r="DJ18" t="n">
+        <v>6.33561643835617</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -25132,11 +25329,14 @@
       </c>
       <c r="DI19" t="n">
         <v>5.02261366341349</v>
+      </c>
+      <c r="DJ19" t="n">
+        <v>5.5861903620235</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -25472,12 +25672,15 @@
         <v>6.65451230628988</v>
       </c>
       <c r="DI20" t="n">
-        <v>6.3868613138686</v>
+        <v>6.478102189781</v>
+      </c>
+      <c r="DJ20" t="n">
+        <v>2.89723856948846</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -25814,11 +26017,14 @@
       </c>
       <c r="DI21" t="n">
         <v>2.49643366619116</v>
+      </c>
+      <c r="DJ21" t="n">
+        <v>1.91761363636363</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -26154,12 +26360,15 @@
         <v>0.149588631264037</v>
       </c>
       <c r="DI22" t="n">
-        <v>0.149588631264037</v>
+        <v>0.224382946896044</v>
+      </c>
+      <c r="DJ22" t="n">
+        <v>0.224215246636759</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -26495,12 +26704,15 @@
         <v>4.34782608695652</v>
       </c>
       <c r="DI23" t="n">
-        <v>3.26370757180157</v>
+        <v>3.45953002610967</v>
+      </c>
+      <c r="DJ23" t="n">
+        <v>1.24426981008514</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -26837,11 +27049,14 @@
       </c>
       <c r="DI24" t="n">
         <v>-2.05058099794942</v>
+      </c>
+      <c r="DJ24" t="n">
+        <v>0.139275766016705</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -27178,11 +27393,14 @@
       </c>
       <c r="DI25" t="n">
         <v>0.204918032786888</v>
+      </c>
+      <c r="DJ25" t="n">
+        <v>0.208333333333336</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -27519,11 +27737,14 @@
       </c>
       <c r="DI26" t="n">
         <v>5.46950629235238</v>
+      </c>
+      <c r="DJ26" t="n">
+        <v>5.5019305019305</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -27859,12 +28080,15 @@
         <v>4.0990990990991</v>
       </c>
       <c r="DI27" t="n">
-        <v>2.52100840336134</v>
+        <v>2.38832375055286</v>
+      </c>
+      <c r="DJ27" t="n">
+        <v>3.43290236290682</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -28200,12 +28424,15 @@
         <v>3.34798782549883</v>
       </c>
       <c r="DI28" t="n">
-        <v>4.18225093505609</v>
+        <v>4.35226113566812</v>
+      </c>
+      <c r="DJ28" t="n">
+        <v>1.50429799426934</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -28541,12 +28768,15 @@
         <v>1.2531328320802</v>
       </c>
       <c r="DI29" t="n">
-        <v>0.847035376183353</v>
+        <v>0.44843049327356</v>
+      </c>
+      <c r="DJ29" t="n">
+        <v>0.554435483870965</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -28882,12 +29112,15 @@
         <v>2.06286836935165</v>
       </c>
       <c r="DI30" t="n">
-        <v>1.96270853778214</v>
+        <v>1.86457311089302</v>
+      </c>
+      <c r="DJ30" t="n">
+        <v>1.88679245283018</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -29001,10 +29234,11 @@
       <c r="DG31"/>
       <c r="DH31"/>
       <c r="DI31"/>
+      <c r="DJ31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -29341,11 +29575,14 @@
       </c>
       <c r="DI32" t="n">
         <v>0.919540229885071</v>
+      </c>
+      <c r="DJ32" t="n">
+        <v>0.921658986175112</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -29681,12 +29918,15 @@
         <v>3.07692307692307</v>
       </c>
       <c r="DI33" t="n">
-        <v>2.06746463547333</v>
+        <v>2.17627856365615</v>
+      </c>
+      <c r="DJ33" t="n">
+        <v>1.62337662337662</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -30022,12 +30262,15 @@
         <v>1.99733688415446</v>
       </c>
       <c r="DI34" t="n">
-        <v>1.8716577540107</v>
+        <v>2.00534759358289</v>
+      </c>
+      <c r="DJ34" t="n">
+        <v>2.5537634408602</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -30363,12 +30606,15 @@
         <v>-1.3215859030837</v>
       </c>
       <c r="DI35" t="n">
-        <v>-2.18340611353713</v>
+        <v>-1.7467248908297</v>
+      </c>
+      <c r="DJ35" t="n">
+        <v>-2.42825607064016</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -30705,11 +30951,14 @@
       </c>
       <c r="DI36" t="n">
         <v>4.52397029034437</v>
+      </c>
+      <c r="DJ36" t="n">
+        <v>4.6949965729952</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -31046,11 +31295,14 @@
       </c>
       <c r="DI37" t="n">
         <v>5.47195622435021</v>
+      </c>
+      <c r="DJ37" t="n">
+        <v>6.10263522884883</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -31386,12 +31638,15 @@
         <v>6.98738170347004</v>
       </c>
       <c r="DI38" t="n">
-        <v>7.75169371356549</v>
+        <v>7.72018276351034</v>
+      </c>
+      <c r="DJ38" t="n">
+        <v>7.2137344463695</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -31728,11 +31983,14 @@
       </c>
       <c r="DI39" t="n">
         <v>3.63294707171938</v>
+      </c>
+      <c r="DJ39" t="n">
+        <v>3.07595731324543</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -32069,11 +32327,14 @@
       </c>
       <c r="DI40" t="n">
         <v>5.39083557951482</v>
+      </c>
+      <c r="DJ40" t="n">
+        <v>5.72207084468663</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -32409,12 +32670,15 @@
         <v>0.764566306353819</v>
       </c>
       <c r="DI41" t="n">
-        <v>-0.62679550796552</v>
+        <v>-0.496213110472702</v>
+      </c>
+      <c r="DJ41" t="n">
+        <v>-0.903774587985138</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -32750,12 +33014,15 @@
         <v>1.93905817174514</v>
       </c>
       <c r="DI42" t="n">
-        <v>1.64722031571723</v>
+        <v>1.71585449553878</v>
+      </c>
+      <c r="DJ42" t="n">
+        <v>1.51410874053681</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -33092,11 +33359,14 @@
       </c>
       <c r="DI43" t="n">
         <v>4.27215189873416</v>
+      </c>
+      <c r="DJ43" t="n">
+        <v>4.17651694247438</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -33433,11 +33703,14 @@
       </c>
       <c r="DI44" t="n">
         <v>0.249843847595239</v>
+      </c>
+      <c r="DJ44" t="n">
+        <v>0.505529225908362</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -33774,11 +34047,14 @@
       </c>
       <c r="DI45" t="n">
         <v>3.85964912280702</v>
+      </c>
+      <c r="DJ45" t="n">
+        <v>1.38408304498271</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -34115,11 +34391,14 @@
       </c>
       <c r="DI46" t="n">
         <v>4.25265791119449</v>
+      </c>
+      <c r="DJ46" t="n">
+        <v>3.96475770925109</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -34455,12 +34734,15 @@
         <v>2.73972602739726</v>
       </c>
       <c r="DI47" t="n">
-        <v>1.92307692307693</v>
+        <v>2.47252747252747</v>
+      </c>
+      <c r="DJ47" t="n">
+        <v>1.93905817174514</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -34797,11 +35079,14 @@
       </c>
       <c r="DI48" t="n">
         <v>1.04270109235352</v>
+      </c>
+      <c r="DJ48" t="n">
+        <v>2.97435897435898</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -35137,12 +35422,15 @@
         <v>2.94460903133138</v>
       </c>
       <c r="DI49" t="n">
-        <v>2.95279124035181</v>
+        <v>2.9258660922635</v>
+      </c>
+      <c r="DJ49" t="n">
+        <v>2.66870338754603</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -35479,11 +35767,14 @@
       </c>
       <c r="DI50" t="n">
         <v>3.53618421052633</v>
+      </c>
+      <c r="DJ50" t="n">
+        <v>3.46534653465346</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -35820,11 +36111,14 @@
       </c>
       <c r="DI51" t="n">
         <v>2.31788079470197</v>
+      </c>
+      <c r="DJ51" t="n">
+        <v>-2.35690235690235</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -36161,11 +36455,14 @@
       </c>
       <c r="DI52" t="n">
         <v>3.67838541666667</v>
+      </c>
+      <c r="DJ52" t="n">
+        <v>3.26014637391881</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -36502,11 +36799,14 @@
       </c>
       <c r="DI53" t="n">
         <v>4.96072757337743</v>
+      </c>
+      <c r="DJ53" t="n">
+        <v>5.37856847331403</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -36843,11 +37143,14 @@
       </c>
       <c r="DI54" t="n">
         <v>1.16472545757072</v>
+      </c>
+      <c r="DJ54" t="n">
+        <v>0.671140939597313</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -37183,12 +37486,15 @@
         <v>3.54468297553668</v>
       </c>
       <c r="DI55" t="n">
-        <v>3.1604938271605</v>
+        <v>3.06172839506174</v>
+      </c>
+      <c r="DJ55" t="n">
+        <v>3.53178607467206</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -37524,6 +37830,9 @@
         <v>0.332225913621255</v>
       </c>
       <c r="DI56" t="n">
+        <v>1.00671140939598</v>
+      </c>
+      <c r="DJ56" t="n">
         <v>1.00671140939598</v>
       </c>
     </row>

</xml_diff>

<commit_message>
July 22, 2022, update
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t xml:space="preserve">05/01/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/01/2022</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1257,10 +1260,13 @@
       <c r="DV4" t="s">
         <v>125</v>
       </c>
+      <c r="DW4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1632,15 +1638,18 @@
         <v>10692.1</v>
       </c>
       <c r="DU5" t="n">
-        <v>10717.6</v>
+        <v>10712.1</v>
       </c>
       <c r="DV5" t="n">
-        <v>10609.1</v>
+        <v>10588.7</v>
+      </c>
+      <c r="DW5" t="n">
+        <v>10014.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2015,12 +2024,15 @@
         <v>169.3</v>
       </c>
       <c r="DV6" t="n">
-        <v>169.6</v>
+        <v>168.2</v>
+      </c>
+      <c r="DW6" t="n">
+        <v>165.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2395,12 +2407,15 @@
         <v>27.8</v>
       </c>
       <c r="DV7" t="n">
-        <v>26.3</v>
+        <v>26.2</v>
+      </c>
+      <c r="DW7" t="n">
+        <v>21.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2775,12 +2790,15 @@
         <v>196.5</v>
       </c>
       <c r="DV8" t="n">
-        <v>188.4</v>
+        <v>188.3</v>
+      </c>
+      <c r="DW8" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3156,11 +3174,14 @@
       </c>
       <c r="DV9" t="n">
         <v>102.3</v>
+      </c>
+      <c r="DW9" t="n">
+        <v>93.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3535,12 +3556,15 @@
         <v>1224.1</v>
       </c>
       <c r="DV10" t="n">
-        <v>1236.1</v>
+        <v>1238.2</v>
+      </c>
+      <c r="DW10" t="n">
+        <v>1222.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -3916,11 +3940,14 @@
       </c>
       <c r="DV11" t="n">
         <v>215.1</v>
+      </c>
+      <c r="DW11" t="n">
+        <v>195.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4295,12 +4322,15 @@
         <v>122.5</v>
       </c>
       <c r="DV12" t="n">
-        <v>119.3</v>
+        <v>119.4</v>
+      </c>
+      <c r="DW12" t="n">
+        <v>110.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4675,12 +4705,15 @@
         <v>36.5</v>
       </c>
       <c r="DV13" t="n">
-        <v>35.5</v>
+        <v>36.4</v>
+      </c>
+      <c r="DW13" t="n">
+        <v>34.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4807,10 +4840,11 @@
       <c r="DT14"/>
       <c r="DU14"/>
       <c r="DV14"/>
+      <c r="DW14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5186,11 +5220,14 @@
       </c>
       <c r="DV15" t="n">
         <v>485.9</v>
+      </c>
+      <c r="DW15" t="n">
+        <v>399.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5566,11 +5603,14 @@
       </c>
       <c r="DV16" t="n">
         <v>337</v>
+      </c>
+      <c r="DW16" t="n">
+        <v>330.5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -5697,10 +5737,11 @@
       <c r="DT17"/>
       <c r="DU17"/>
       <c r="DV17"/>
+      <c r="DW17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6076,11 +6117,14 @@
       </c>
       <c r="DV18" t="n">
         <v>62.1</v>
+      </c>
+      <c r="DW18" t="n">
+        <v>60.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6455,12 +6499,15 @@
         <v>441.2</v>
       </c>
       <c r="DV19" t="n">
-        <v>440.4</v>
+        <v>439.3</v>
+      </c>
+      <c r="DW19" t="n">
+        <v>403.9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -6835,12 +6882,15 @@
         <v>233.4</v>
       </c>
       <c r="DV20" t="n">
-        <v>227.3</v>
+        <v>232.3</v>
+      </c>
+      <c r="DW20" t="n">
+        <v>191.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7215,12 +7265,15 @@
         <v>143.7</v>
       </c>
       <c r="DV21" t="n">
-        <v>143.5</v>
+        <v>143.1</v>
+      </c>
+      <c r="DW21" t="n">
+        <v>132.6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -7595,12 +7648,15 @@
         <v>134</v>
       </c>
       <c r="DV22" t="n">
-        <v>134.1</v>
+        <v>133.8</v>
+      </c>
+      <c r="DW22" t="n">
+        <v>120.6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -7975,12 +8031,15 @@
         <v>158.5</v>
       </c>
       <c r="DV23" t="n">
-        <v>154.6</v>
+        <v>156.3</v>
+      </c>
+      <c r="DW23" t="n">
+        <v>148.3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -8355,12 +8414,15 @@
         <v>143.3</v>
       </c>
       <c r="DV24" t="n">
-        <v>143.8</v>
+        <v>143.4</v>
+      </c>
+      <c r="DW24" t="n">
+        <v>132.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -8736,11 +8798,14 @@
       </c>
       <c r="DV25" t="n">
         <v>48.1</v>
+      </c>
+      <c r="DW25" t="n">
+        <v>45.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9115,12 +9180,15 @@
         <v>217.9</v>
       </c>
       <c r="DV26" t="n">
-        <v>218.6</v>
+        <v>217.7</v>
+      </c>
+      <c r="DW26" t="n">
+        <v>202.1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -9495,12 +9563,15 @@
         <v>231.5</v>
       </c>
       <c r="DV27" t="n">
-        <v>232</v>
+        <v>231.3</v>
+      </c>
+      <c r="DW27" t="n">
+        <v>224.6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -9875,12 +9946,15 @@
         <v>306.9</v>
       </c>
       <c r="DV28" t="n">
-        <v>283.4</v>
+        <v>289.6</v>
+      </c>
+      <c r="DW28" t="n">
+        <v>271.3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -10255,12 +10329,15 @@
         <v>201.6</v>
       </c>
       <c r="DV29" t="n">
-        <v>199.5</v>
+        <v>199.7</v>
+      </c>
+      <c r="DW29" t="n">
+        <v>193.7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -10635,12 +10712,15 @@
         <v>103.8</v>
       </c>
       <c r="DV30" t="n">
-        <v>102.6</v>
+        <v>102.4</v>
+      </c>
+      <c r="DW30" t="n">
+        <v>99.2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -10767,10 +10847,11 @@
       <c r="DT31"/>
       <c r="DU31"/>
       <c r="DV31"/>
+      <c r="DW31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -11145,12 +11226,15 @@
         <v>43.9</v>
       </c>
       <c r="DV32" t="n">
-        <v>43.8</v>
+        <v>42.5</v>
+      </c>
+      <c r="DW32" t="n">
+        <v>40.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -11525,12 +11609,15 @@
         <v>93.9</v>
       </c>
       <c r="DV33" t="n">
-        <v>93.9</v>
+        <v>93.7</v>
+      </c>
+      <c r="DW33" t="n">
+        <v>88.7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -11905,12 +11992,15 @@
         <v>76.3</v>
       </c>
       <c r="DV34" t="n">
-        <v>76.3</v>
+        <v>75.9</v>
+      </c>
+      <c r="DW34" t="n">
+        <v>69.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -12285,12 +12375,15 @@
         <v>45</v>
       </c>
       <c r="DV35" t="n">
-        <v>44.2</v>
+        <v>44</v>
+      </c>
+      <c r="DW35" t="n">
+        <v>37.4</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -12665,12 +12758,15 @@
         <v>309.6</v>
       </c>
       <c r="DV36" t="n">
-        <v>305.5</v>
+        <v>304.7</v>
+      </c>
+      <c r="DW36" t="n">
+        <v>302.3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -13045,12 +13141,15 @@
         <v>77.1</v>
       </c>
       <c r="DV37" t="n">
-        <v>76.5</v>
+        <v>76.4</v>
+      </c>
+      <c r="DW37" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -13425,12 +13524,15 @@
         <v>683.7</v>
       </c>
       <c r="DV38" t="n">
-        <v>680.7</v>
+        <v>681.1</v>
+      </c>
+      <c r="DW38" t="n">
+        <v>667.9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -13805,12 +13907,15 @@
         <v>330.9</v>
       </c>
       <c r="DV39" t="n">
-        <v>328.4</v>
+        <v>328.3</v>
+      </c>
+      <c r="DW39" t="n">
+        <v>288.9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -14185,12 +14290,15 @@
         <v>39.1</v>
       </c>
       <c r="DV40" t="n">
-        <v>38.8</v>
+        <v>38.7</v>
+      </c>
+      <c r="DW40" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -14565,12 +14673,15 @@
         <v>381</v>
       </c>
       <c r="DV41" t="n">
-        <v>372.8</v>
+        <v>373.6</v>
+      </c>
+      <c r="DW41" t="n">
+        <v>340.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -14945,12 +15056,15 @@
         <v>148.2</v>
       </c>
       <c r="DV42" t="n">
-        <v>147.5</v>
+        <v>147.2</v>
+      </c>
+      <c r="DW42" t="n">
+        <v>133.7</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -15325,12 +15439,15 @@
         <v>131.8</v>
       </c>
       <c r="DV43" t="n">
-        <v>132.2</v>
+        <v>132.4</v>
+      </c>
+      <c r="DW43" t="n">
+        <v>130.2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -15705,12 +15822,15 @@
         <v>321</v>
       </c>
       <c r="DV44" t="n">
-        <v>318.1</v>
+        <v>318.3</v>
+      </c>
+      <c r="DW44" t="n">
+        <v>300.7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -16086,11 +16206,14 @@
       </c>
       <c r="DV45" t="n">
         <v>29.3</v>
+      </c>
+      <c r="DW45" t="n">
+        <v>27.2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -16466,11 +16589,14 @@
       </c>
       <c r="DV46" t="n">
         <v>165.2</v>
+      </c>
+      <c r="DW46" t="n">
+        <v>155.4</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -16846,11 +16972,14 @@
       </c>
       <c r="DV47" t="n">
         <v>36.8</v>
+      </c>
+      <c r="DW47" t="n">
+        <v>33.2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -17225,12 +17354,15 @@
         <v>203.5</v>
       </c>
       <c r="DV48" t="n">
-        <v>200.8</v>
+        <v>200.6</v>
+      </c>
+      <c r="DW48" t="n">
+        <v>191.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -17606,11 +17738,14 @@
       </c>
       <c r="DV49" t="n">
         <v>1142.6</v>
+      </c>
+      <c r="DW49" t="n">
+        <v>1103.1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -17986,11 +18121,14 @@
       </c>
       <c r="DV50" t="n">
         <v>125.4</v>
+      </c>
+      <c r="DW50" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -18365,12 +18503,15 @@
         <v>30.9</v>
       </c>
       <c r="DV51" t="n">
-        <v>29</v>
+        <v>29.1</v>
+      </c>
+      <c r="DW51" t="n">
+        <v>27.5</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -18745,12 +18886,15 @@
         <v>318.5</v>
       </c>
       <c r="DV52" t="n">
-        <v>310.4</v>
+        <v>309.8</v>
+      </c>
+      <c r="DW52" t="n">
+        <v>294.6</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -19125,12 +19269,15 @@
         <v>253.9</v>
       </c>
       <c r="DV53" t="n">
-        <v>254.7</v>
+        <v>254.9</v>
+      </c>
+      <c r="DW53" t="n">
+        <v>247.5</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -19506,11 +19653,14 @@
       </c>
       <c r="DV54" t="n">
         <v>60</v>
+      </c>
+      <c r="DW54" t="n">
+        <v>55.3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -19886,11 +20036,14 @@
       </c>
       <c r="DV55" t="n">
         <v>205.2</v>
+      </c>
+      <c r="DW55" t="n">
+        <v>187.1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -20266,6 +20419,9 @@
       </c>
       <c r="DV56" t="n">
         <v>30.1</v>
+      </c>
+      <c r="DW56" t="n">
+        <v>27.4</v>
       </c>
     </row>
   </sheetData>
@@ -20625,10 +20781,13 @@
       <c r="DJ4" t="s">
         <v>125</v>
       </c>
+      <c r="DK4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -20964,15 +21123,18 @@
         <v>3.12894856139741</v>
       </c>
       <c r="DI5" t="n">
-        <v>2.97760312076633</v>
+        <v>2.92475763136908</v>
       </c>
       <c r="DJ5" t="n">
-        <v>2.93601125503324</v>
+        <v>2.73807791199729</v>
+      </c>
+      <c r="DK5" t="n">
+        <v>1.79816625668342</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -21311,12 +21473,15 @@
         <v>2.98053527980536</v>
       </c>
       <c r="DJ6" t="n">
-        <v>2.91262135922329</v>
+        <v>2.06310679611649</v>
+      </c>
+      <c r="DK6" t="n">
+        <v>2.0923076923077</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -21655,12 +21820,15 @@
         <v>0.724637681159418</v>
       </c>
       <c r="DJ7" t="n">
-        <v>0.0000000000000135084170296597</v>
+        <v>-0.380228136882121</v>
+      </c>
+      <c r="DK7" t="n">
+        <v>-7.26495726495726</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -21999,12 +22167,15 @@
         <v>2.87958115183246</v>
       </c>
       <c r="DJ8" t="n">
-        <v>2.39130434782607</v>
+        <v>2.33695652173914</v>
+      </c>
+      <c r="DK8" t="n">
+        <v>-0.332225913621262</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -22344,11 +22515,14 @@
       </c>
       <c r="DJ9" t="n">
         <v>2.40240240240239</v>
+      </c>
+      <c r="DK9" t="n">
+        <v>2.39912758996729</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -22687,12 +22861,15 @@
         <v>6.3602398123208</v>
       </c>
       <c r="DJ10" t="n">
-        <v>5.74899478141841</v>
+        <v>5.92865086833773</v>
+      </c>
+      <c r="DK10" t="n">
+        <v>5.95578673602081</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -23032,11 +23209,14 @@
       </c>
       <c r="DJ11" t="n">
         <v>2.28245363766049</v>
+      </c>
+      <c r="DK11" t="n">
+        <v>-0.407539480387168</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -23375,12 +23555,15 @@
         <v>0.906095551894559</v>
       </c>
       <c r="DJ12" t="n">
-        <v>0.336417157275026</v>
+        <v>0.420521446593776</v>
+      </c>
+      <c r="DK12" t="n">
+        <v>-1.16591928251122</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -23719,12 +23902,15 @@
         <v>1.10803324099723</v>
       </c>
       <c r="DJ13" t="n">
-        <v>0.852272727272719</v>
+        <v>3.4090909090909</v>
+      </c>
+      <c r="DK13" t="n">
+        <v>2.39520958083834</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -23839,10 +24025,11 @@
       <c r="DH14"/>
       <c r="DI14"/>
       <c r="DJ14"/>
+      <c r="DK14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -24182,11 +24369,14 @@
       </c>
       <c r="DJ15" t="n">
         <v>2.77072758037226</v>
+      </c>
+      <c r="DK15" t="n">
+        <v>1.5497967479675</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -24526,11 +24716,14 @@
       </c>
       <c r="DJ16" t="n">
         <v>2.27617602427921</v>
+      </c>
+      <c r="DK16" t="n">
+        <v>3.60501567398119</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -24645,10 +24838,11 @@
       <c r="DH17"/>
       <c r="DI17"/>
       <c r="DJ17"/>
+      <c r="DK17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -24988,11 +25182,14 @@
       </c>
       <c r="DJ18" t="n">
         <v>6.33561643835617</v>
+      </c>
+      <c r="DK18" t="n">
+        <v>8.07899461400359</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -25331,12 +25528,15 @@
         <v>5.02261366341349</v>
       </c>
       <c r="DJ19" t="n">
-        <v>5.5861903620235</v>
+        <v>5.32246463677775</v>
+      </c>
+      <c r="DK19" t="n">
+        <v>5.15490757615203</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -25675,12 +25875,15 @@
         <v>6.478102189781</v>
       </c>
       <c r="DJ20" t="n">
-        <v>2.89723856948846</v>
+        <v>5.16070620190131</v>
+      </c>
+      <c r="DK20" t="n">
+        <v>-1.84899845916795</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -26019,12 +26222,15 @@
         <v>2.49643366619116</v>
       </c>
       <c r="DJ21" t="n">
-        <v>1.91761363636363</v>
+        <v>1.63352272727272</v>
+      </c>
+      <c r="DK21" t="n">
+        <v>1.84331797235023</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -26363,12 +26569,15 @@
         <v>0.224382946896044</v>
       </c>
       <c r="DJ22" t="n">
-        <v>0.224215246636759</v>
+        <v>0</v>
+      </c>
+      <c r="DK22" t="n">
+        <v>0.416319733555371</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -26707,12 +26916,15 @@
         <v>3.45953002610967</v>
       </c>
       <c r="DJ23" t="n">
-        <v>1.24426981008514</v>
+        <v>2.35756385068764</v>
+      </c>
+      <c r="DK23" t="n">
+        <v>1.02179836512262</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -27051,12 +27263,15 @@
         <v>-2.05058099794942</v>
       </c>
       <c r="DJ24" t="n">
-        <v>0.139275766016705</v>
+        <v>-0.139275766016725</v>
+      </c>
+      <c r="DK24" t="n">
+        <v>-0.897531787584135</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -27396,11 +27611,14 @@
       </c>
       <c r="DJ25" t="n">
         <v>0.208333333333336</v>
+      </c>
+      <c r="DK25" t="n">
+        <v>-1.08695652173913</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -27739,12 +27957,15 @@
         <v>5.46950629235238</v>
       </c>
       <c r="DJ26" t="n">
-        <v>5.5019305019305</v>
+        <v>5.06756756756757</v>
+      </c>
+      <c r="DK26" t="n">
+        <v>3.85405960945529</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -28083,12 +28304,15 @@
         <v>2.38832375055286</v>
       </c>
       <c r="DJ27" t="n">
-        <v>3.43290236290682</v>
+        <v>3.12082032991529</v>
+      </c>
+      <c r="DK27" t="n">
+        <v>-0.088967971530244</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -28427,12 +28651,15 @@
         <v>4.35226113566812</v>
       </c>
       <c r="DJ28" t="n">
-        <v>1.50429799426934</v>
+        <v>3.72492836676219</v>
+      </c>
+      <c r="DK28" t="n">
+        <v>1.87758167480285</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -28771,12 +28998,15 @@
         <v>0.44843049327356</v>
       </c>
       <c r="DJ29" t="n">
-        <v>0.554435483870965</v>
+        <v>0.655241935483862</v>
+      </c>
+      <c r="DK29" t="n">
+        <v>-0.360082304526743</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -29115,12 +29345,15 @@
         <v>1.86457311089302</v>
       </c>
       <c r="DJ30" t="n">
-        <v>1.88679245283018</v>
+        <v>1.68818272095333</v>
+      </c>
+      <c r="DK30" t="n">
+        <v>2.16271884654996</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -29235,10 +29468,11 @@
       <c r="DH31"/>
       <c r="DI31"/>
       <c r="DJ31"/>
+      <c r="DK31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -29577,12 +29811,15 @@
         <v>0.919540229885071</v>
       </c>
       <c r="DJ32" t="n">
-        <v>0.921658986175112</v>
+        <v>-2.07373271889401</v>
+      </c>
+      <c r="DK32" t="n">
+        <v>-1.95599022004889</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -29921,12 +30158,15 @@
         <v>2.17627856365615</v>
       </c>
       <c r="DJ33" t="n">
-        <v>1.62337662337662</v>
+        <v>1.40692640692639</v>
+      </c>
+      <c r="DK33" t="n">
+        <v>2.66203703703703</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -30265,12 +30505,15 @@
         <v>2.00534759358289</v>
       </c>
       <c r="DJ34" t="n">
-        <v>2.5537634408602</v>
+        <v>2.01612903225806</v>
+      </c>
+      <c r="DK34" t="n">
+        <v>1.91740412979351</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -30609,12 +30852,15 @@
         <v>-1.7467248908297</v>
       </c>
       <c r="DJ35" t="n">
-        <v>-2.42825607064016</v>
+        <v>-2.86975717439293</v>
+      </c>
+      <c r="DK35" t="n">
+        <v>0.537634408602139</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -30953,12 +31199,15 @@
         <v>4.52397029034437</v>
       </c>
       <c r="DJ36" t="n">
-        <v>4.6949965729952</v>
+        <v>4.42083618917066</v>
+      </c>
+      <c r="DK36" t="n">
+        <v>4.96527777777778</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -31297,12 +31546,15 @@
         <v>5.47195622435021</v>
       </c>
       <c r="DJ37" t="n">
-        <v>6.10263522884883</v>
+        <v>5.96393897364773</v>
+      </c>
+      <c r="DK37" t="n">
+        <v>2.04081632653061</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -31641,12 +31893,15 @@
         <v>7.72018276351034</v>
       </c>
       <c r="DJ38" t="n">
-        <v>7.2137344463695</v>
+        <v>7.27673649393604</v>
+      </c>
+      <c r="DK38" t="n">
+        <v>7.41395947249918</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -31985,12 +32240,15 @@
         <v>3.63294707171938</v>
       </c>
       <c r="DJ39" t="n">
-        <v>3.07595731324543</v>
+        <v>3.04456999372253</v>
+      </c>
+      <c r="DK39" t="n">
+        <v>-2.76001346348032</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -32329,12 +32587,15 @@
         <v>5.39083557951482</v>
       </c>
       <c r="DJ40" t="n">
-        <v>5.72207084468663</v>
+        <v>5.44959128065395</v>
+      </c>
+      <c r="DK40" t="n">
+        <v>4.93827160493825</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -32673,12 +32934,15 @@
         <v>-0.496213110472702</v>
       </c>
       <c r="DJ41" t="n">
-        <v>-0.903774587985138</v>
+        <v>-0.691121743753329</v>
+      </c>
+      <c r="DK41" t="n">
+        <v>-3.92655367231638</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -33017,12 +33281,15 @@
         <v>1.71585449553878</v>
       </c>
       <c r="DJ42" t="n">
-        <v>1.51410874053681</v>
+        <v>1.30763936682724</v>
+      </c>
+      <c r="DK42" t="n">
+        <v>0.677710843373477</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -33361,12 +33628,15 @@
         <v>4.27215189873416</v>
       </c>
       <c r="DJ43" t="n">
-        <v>4.17651694247438</v>
+        <v>4.33412135539795</v>
+      </c>
+      <c r="DK43" t="n">
+        <v>6.28571428571428</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -33705,12 +33975,15 @@
         <v>0.249843847595239</v>
       </c>
       <c r="DJ44" t="n">
-        <v>0.505529225908362</v>
+        <v>0.568720379146923</v>
+      </c>
+      <c r="DK44" t="n">
+        <v>0.838363514419852</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -34050,11 +34323,14 @@
       </c>
       <c r="DJ45" t="n">
         <v>1.38408304498271</v>
+      </c>
+      <c r="DK45" t="n">
+        <v>0.740740740740751</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -34394,11 +34670,14 @@
       </c>
       <c r="DJ46" t="n">
         <v>3.96475770925109</v>
+      </c>
+      <c r="DK46" t="n">
+        <v>0.843608046722915</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -34738,11 +35017,14 @@
       </c>
       <c r="DJ47" t="n">
         <v>1.93905817174514</v>
+      </c>
+      <c r="DK47" t="n">
+        <v>2.7863777089783</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -35081,12 +35363,15 @@
         <v>1.04270109235352</v>
       </c>
       <c r="DJ48" t="n">
-        <v>2.97435897435898</v>
+        <v>2.87179487179487</v>
+      </c>
+      <c r="DK48" t="n">
+        <v>1.59066808059385</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -35426,11 +35711,14 @@
       </c>
       <c r="DJ49" t="n">
         <v>2.66870338754603</v>
+      </c>
+      <c r="DK49" t="n">
+        <v>1.84655156495247</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -35770,11 +36058,14 @@
       </c>
       <c r="DJ50" t="n">
         <v>3.46534653465346</v>
+      </c>
+      <c r="DK50" t="n">
+        <v>1.69491525423729</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -36113,12 +36404,15 @@
         <v>2.31788079470197</v>
       </c>
       <c r="DJ51" t="n">
-        <v>-2.35690235690235</v>
+        <v>-2.02020202020201</v>
+      </c>
+      <c r="DK51" t="n">
+        <v>3.77358490566038</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -36457,12 +36751,15 @@
         <v>3.67838541666667</v>
       </c>
       <c r="DJ52" t="n">
-        <v>3.26014637391881</v>
+        <v>3.06054557551563</v>
+      </c>
+      <c r="DK52" t="n">
+        <v>0.204081632653069</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -36801,12 +37098,15 @@
         <v>4.96072757337743</v>
       </c>
       <c r="DJ53" t="n">
-        <v>5.37856847331403</v>
+        <v>5.46131568059579</v>
+      </c>
+      <c r="DK53" t="n">
+        <v>3.46989966555184</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -37146,11 +37446,14 @@
       </c>
       <c r="DJ54" t="n">
         <v>0.671140939597313</v>
+      </c>
+      <c r="DK54" t="n">
+        <v>0.362976406533568</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -37490,11 +37793,14 @@
       </c>
       <c r="DJ55" t="n">
         <v>3.53178607467206</v>
+      </c>
+      <c r="DK55" t="n">
+        <v>2.18459858001092</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -37834,6 +38140,9 @@
       </c>
       <c r="DJ56" t="n">
         <v>1.00671140939598</v>
+      </c>
+      <c r="DK56" t="n">
+        <v>-1.7921146953405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update August 19, 2022
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -396,6 +396,9 @@
     <t xml:space="preserve">06/01/2022</t>
   </si>
   <si>
+    <t xml:space="preserve">07/01/2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">United States</t>
   </si>
   <si>
@@ -555,7 +558,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -874,10 +877,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -1263,10 +1266,13 @@
       <c r="DW4" t="s">
         <v>126</v>
       </c>
+      <c r="DX4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1641,15 +1647,18 @@
         <v>10712.1</v>
       </c>
       <c r="DV5" t="n">
-        <v>10588.7</v>
+        <v>10590.2</v>
       </c>
       <c r="DW5" t="n">
-        <v>10014.7</v>
+        <v>9994.4</v>
+      </c>
+      <c r="DX5" t="n">
+        <v>8985.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2027,12 +2036,15 @@
         <v>168.2</v>
       </c>
       <c r="DW6" t="n">
-        <v>165.9</v>
+        <v>165.8</v>
+      </c>
+      <c r="DX6" t="n">
+        <v>157.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2410,12 +2422,15 @@
         <v>26.2</v>
       </c>
       <c r="DW7" t="n">
-        <v>21.7</v>
+        <v>21.5</v>
+      </c>
+      <c r="DX7" t="n">
+        <v>16.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2793,12 +2808,15 @@
         <v>188.3</v>
       </c>
       <c r="DW8" t="n">
-        <v>150</v>
+        <v>150.2</v>
+      </c>
+      <c r="DX8" t="n">
+        <v>146.8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3177,11 +3195,14 @@
       </c>
       <c r="DW9" t="n">
         <v>93.9</v>
+      </c>
+      <c r="DX9" t="n">
+        <v>82.8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3559,12 +3580,15 @@
         <v>1238.2</v>
       </c>
       <c r="DW10" t="n">
-        <v>1222.2</v>
+        <v>1223.2</v>
+      </c>
+      <c r="DX10" t="n">
+        <v>1053</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -3942,12 +3966,15 @@
         <v>215.1</v>
       </c>
       <c r="DW11" t="n">
-        <v>195.5</v>
+        <v>195.4</v>
+      </c>
+      <c r="DX11" t="n">
+        <v>181.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4325,12 +4352,15 @@
         <v>119.4</v>
       </c>
       <c r="DW12" t="n">
-        <v>110.2</v>
+        <v>110.4</v>
+      </c>
+      <c r="DX12" t="n">
+        <v>97.1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4708,12 +4738,15 @@
         <v>36.4</v>
       </c>
       <c r="DW13" t="n">
-        <v>34.2</v>
+        <v>33.5</v>
+      </c>
+      <c r="DX13" t="n">
+        <v>32.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4841,10 +4874,11 @@
       <c r="DU14"/>
       <c r="DV14"/>
       <c r="DW14"/>
+      <c r="DX14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5223,11 +5257,14 @@
       </c>
       <c r="DW15" t="n">
         <v>399.7</v>
+      </c>
+      <c r="DX15" t="n">
+        <v>391</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5605,12 +5642,15 @@
         <v>337</v>
       </c>
       <c r="DW16" t="n">
-        <v>330.5</v>
+        <v>330.9</v>
+      </c>
+      <c r="DX16" t="n">
+        <v>318.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -5738,10 +5778,11 @@
       <c r="DU17"/>
       <c r="DV17"/>
       <c r="DW17"/>
+      <c r="DX17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6120,11 +6161,14 @@
       </c>
       <c r="DW18" t="n">
         <v>60.2</v>
+      </c>
+      <c r="DX18" t="n">
+        <v>54.1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6502,12 +6546,15 @@
         <v>439.3</v>
       </c>
       <c r="DW19" t="n">
-        <v>403.9</v>
+        <v>405.1</v>
+      </c>
+      <c r="DX19" t="n">
+        <v>377.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -6885,12 +6932,15 @@
         <v>232.3</v>
       </c>
       <c r="DW20" t="n">
-        <v>191.1</v>
+        <v>191.4</v>
+      </c>
+      <c r="DX20" t="n">
+        <v>173.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7268,12 +7318,15 @@
         <v>143.1</v>
       </c>
       <c r="DW21" t="n">
-        <v>132.6</v>
+        <v>131.5</v>
+      </c>
+      <c r="DX21" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -7651,12 +7704,15 @@
         <v>133.8</v>
       </c>
       <c r="DW22" t="n">
-        <v>120.6</v>
+        <v>119.6</v>
+      </c>
+      <c r="DX22" t="n">
+        <v>100.9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8034,12 +8090,15 @@
         <v>156.3</v>
       </c>
       <c r="DW23" t="n">
-        <v>148.3</v>
+        <v>147.4</v>
+      </c>
+      <c r="DX23" t="n">
+        <v>121.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -8417,12 +8476,15 @@
         <v>143.4</v>
       </c>
       <c r="DW24" t="n">
-        <v>132.5</v>
+        <v>132.8</v>
+      </c>
+      <c r="DX24" t="n">
+        <v>127.7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -8800,12 +8862,15 @@
         <v>48.1</v>
       </c>
       <c r="DW25" t="n">
-        <v>45.5</v>
+        <v>46.7</v>
+      </c>
+      <c r="DX25" t="n">
+        <v>39.7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9184,11 +9249,14 @@
       </c>
       <c r="DW26" t="n">
         <v>202.1</v>
+      </c>
+      <c r="DX26" t="n">
+        <v>188.9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -9566,12 +9634,15 @@
         <v>231.3</v>
       </c>
       <c r="DW27" t="n">
-        <v>224.6</v>
+        <v>221.5</v>
+      </c>
+      <c r="DX27" t="n">
+        <v>194.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -9949,12 +10020,15 @@
         <v>289.6</v>
       </c>
       <c r="DW28" t="n">
-        <v>271.3</v>
+        <v>270.8</v>
+      </c>
+      <c r="DX28" t="n">
+        <v>243.4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -10332,12 +10406,15 @@
         <v>199.7</v>
       </c>
       <c r="DW29" t="n">
-        <v>193.7</v>
+        <v>192.9</v>
+      </c>
+      <c r="DX29" t="n">
+        <v>165.6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -10716,11 +10793,14 @@
       </c>
       <c r="DW30" t="n">
         <v>99.2</v>
+      </c>
+      <c r="DX30" t="n">
+        <v>93.6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -10848,10 +10928,11 @@
       <c r="DU31"/>
       <c r="DV31"/>
       <c r="DW31"/>
+      <c r="DX31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -11229,12 +11310,15 @@
         <v>42.5</v>
       </c>
       <c r="DW32" t="n">
-        <v>40.1</v>
+        <v>39.6</v>
+      </c>
+      <c r="DX32" t="n">
+        <v>33.3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -11612,12 +11696,15 @@
         <v>93.7</v>
       </c>
       <c r="DW33" t="n">
-        <v>88.7</v>
+        <v>88.2</v>
+      </c>
+      <c r="DX33" t="n">
+        <v>77.5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -11995,12 +12082,15 @@
         <v>75.9</v>
       </c>
       <c r="DW34" t="n">
-        <v>69.1</v>
+        <v>67.7</v>
+      </c>
+      <c r="DX34" t="n">
+        <v>64.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -12378,12 +12468,15 @@
         <v>44</v>
       </c>
       <c r="DW35" t="n">
-        <v>37.4</v>
+        <v>38.3</v>
+      </c>
+      <c r="DX35" t="n">
+        <v>31.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -12761,12 +12854,15 @@
         <v>304.7</v>
       </c>
       <c r="DW36" t="n">
-        <v>302.3</v>
+        <v>302.2</v>
+      </c>
+      <c r="DX36" t="n">
+        <v>247.1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -13144,12 +13240,15 @@
         <v>76.4</v>
       </c>
       <c r="DW37" t="n">
-        <v>65</v>
+        <v>63.8</v>
+      </c>
+      <c r="DX37" t="n">
+        <v>61.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -13527,12 +13626,15 @@
         <v>681.1</v>
       </c>
       <c r="DW38" t="n">
-        <v>667.9</v>
+        <v>666.6</v>
+      </c>
+      <c r="DX38" t="n">
+        <v>546.9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -13911,11 +14013,14 @@
       </c>
       <c r="DW39" t="n">
         <v>288.9</v>
+      </c>
+      <c r="DX39" t="n">
+        <v>240</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -14293,12 +14398,15 @@
         <v>38.7</v>
       </c>
       <c r="DW40" t="n">
-        <v>34</v>
+        <v>34.1</v>
+      </c>
+      <c r="DX40" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -14676,12 +14784,15 @@
         <v>373.6</v>
       </c>
       <c r="DW41" t="n">
-        <v>340.1</v>
+        <v>344.9</v>
+      </c>
+      <c r="DX41" t="n">
+        <v>330.4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -15059,12 +15170,15 @@
         <v>147.2</v>
       </c>
       <c r="DW42" t="n">
-        <v>133.7</v>
+        <v>131.1</v>
+      </c>
+      <c r="DX42" t="n">
+        <v>119.9</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -15442,12 +15556,15 @@
         <v>132.4</v>
       </c>
       <c r="DW43" t="n">
-        <v>130.2</v>
+        <v>129.7</v>
+      </c>
+      <c r="DX43" t="n">
+        <v>99.7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -15825,12 +15942,15 @@
         <v>318.3</v>
       </c>
       <c r="DW44" t="n">
-        <v>300.7</v>
+        <v>293.7</v>
+      </c>
+      <c r="DX44" t="n">
+        <v>264.3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -16209,11 +16329,14 @@
       </c>
       <c r="DW45" t="n">
         <v>27.2</v>
+      </c>
+      <c r="DX45" t="n">
+        <v>23.6</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -16591,12 +16714,15 @@
         <v>165.2</v>
       </c>
       <c r="DW46" t="n">
-        <v>155.4</v>
+        <v>159.5</v>
+      </c>
+      <c r="DX46" t="n">
+        <v>152.7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -16975,11 +17101,14 @@
       </c>
       <c r="DW47" t="n">
         <v>33.2</v>
+      </c>
+      <c r="DX47" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -17357,12 +17486,15 @@
         <v>200.6</v>
       </c>
       <c r="DW48" t="n">
-        <v>191.6</v>
+        <v>191.3</v>
+      </c>
+      <c r="DX48" t="n">
+        <v>167.8</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -17740,12 +17872,15 @@
         <v>1142.6</v>
       </c>
       <c r="DW49" t="n">
-        <v>1103.1</v>
+        <v>1104.1</v>
+      </c>
+      <c r="DX49" t="n">
+        <v>1032.4</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -18124,11 +18259,14 @@
       </c>
       <c r="DW50" t="n">
         <v>114</v>
+      </c>
+      <c r="DX50" t="n">
+        <v>102.2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -18506,12 +18644,15 @@
         <v>29.1</v>
       </c>
       <c r="DW51" t="n">
-        <v>27.5</v>
+        <v>28.8</v>
+      </c>
+      <c r="DX51" t="n">
+        <v>25.6</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -18889,12 +19030,15 @@
         <v>309.8</v>
       </c>
       <c r="DW52" t="n">
-        <v>294.6</v>
+        <v>295.2</v>
+      </c>
+      <c r="DX52" t="n">
+        <v>261.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -19272,12 +19416,15 @@
         <v>254.9</v>
       </c>
       <c r="DW53" t="n">
-        <v>247.5</v>
+        <v>247.9</v>
+      </c>
+      <c r="DX53" t="n">
+        <v>236</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -19655,12 +19802,15 @@
         <v>60</v>
       </c>
       <c r="DW54" t="n">
-        <v>55.3</v>
+        <v>54.3</v>
+      </c>
+      <c r="DX54" t="n">
+        <v>49.6</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -20038,12 +20188,15 @@
         <v>205.2</v>
       </c>
       <c r="DW55" t="n">
-        <v>187.1</v>
+        <v>186.3</v>
+      </c>
+      <c r="DX55" t="n">
+        <v>167</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -20421,7 +20574,10 @@
         <v>30.1</v>
       </c>
       <c r="DW56" t="n">
-        <v>27.4</v>
+        <v>27.3</v>
+      </c>
+      <c r="DX56" t="n">
+        <v>24.3</v>
       </c>
     </row>
   </sheetData>
@@ -20431,10 +20587,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -20784,10 +20940,13 @@
       <c r="DK4" t="s">
         <v>126</v>
       </c>
+      <c r="DL4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -21126,15 +21285,18 @@
         <v>2.92475763136908</v>
       </c>
       <c r="DJ5" t="n">
-        <v>2.73807791199729</v>
+        <v>2.75263183427935</v>
       </c>
       <c r="DK5" t="n">
-        <v>1.79816625668342</v>
+        <v>1.59181930919515</v>
+      </c>
+      <c r="DL5" t="n">
+        <v>1.38902993579545</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -21476,12 +21638,15 @@
         <v>2.06310679611649</v>
       </c>
       <c r="DK6" t="n">
-        <v>2.0923076923077</v>
+        <v>2.03076923076924</v>
+      </c>
+      <c r="DL6" t="n">
+        <v>1.15606936416186</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -21823,12 +21988,15 @@
         <v>-0.380228136882121</v>
       </c>
       <c r="DK7" t="n">
-        <v>-7.26495726495726</v>
+        <v>-8.11965811965811</v>
+      </c>
+      <c r="DL7" t="n">
+        <v>-17.4129353233831</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -22170,12 +22338,15 @@
         <v>2.33695652173914</v>
       </c>
       <c r="DK8" t="n">
-        <v>-0.332225913621262</v>
+        <v>-0.199335548172765</v>
+      </c>
+      <c r="DL8" t="n">
+        <v>0.479123887748129</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -22518,11 +22689,14 @@
       </c>
       <c r="DK9" t="n">
         <v>2.39912758996729</v>
+      </c>
+      <c r="DL9" t="n">
+        <v>1.97044334975369</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -22864,12 +23038,15 @@
         <v>5.92865086833773</v>
       </c>
       <c r="DK10" t="n">
-        <v>5.95578673602081</v>
+        <v>6.04247941048982</v>
+      </c>
+      <c r="DL10" t="n">
+        <v>4.526503871352</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -23211,12 +23388,15 @@
         <v>2.28245363766049</v>
       </c>
       <c r="DK11" t="n">
-        <v>-0.407539480387168</v>
+        <v>-0.458481915435575</v>
+      </c>
+      <c r="DL11" t="n">
+        <v>-2.89544235924932</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -23558,12 +23738,15 @@
         <v>0.420521446593776</v>
       </c>
       <c r="DK12" t="n">
-        <v>-1.16591928251122</v>
+        <v>-0.986547085201789</v>
+      </c>
+      <c r="DL12" t="n">
+        <v>0.413650465356794</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -23905,12 +24088,15 @@
         <v>3.4090909090909</v>
       </c>
       <c r="DK13" t="n">
-        <v>2.39520958083834</v>
+        <v>0.299401197604795</v>
+      </c>
+      <c r="DL13" t="n">
+        <v>-0.30487804878047</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -24026,10 +24212,11 @@
       <c r="DI14"/>
       <c r="DJ14"/>
       <c r="DK14"/>
+      <c r="DL14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -24372,11 +24559,14 @@
       </c>
       <c r="DK15" t="n">
         <v>1.5497967479675</v>
+      </c>
+      <c r="DL15" t="n">
+        <v>0.851173587825641</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -24718,12 +24908,15 @@
         <v>2.27617602427921</v>
       </c>
       <c r="DK16" t="n">
-        <v>3.60501567398119</v>
+        <v>3.73040752351096</v>
+      </c>
+      <c r="DL16" t="n">
+        <v>4.07963446475196</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -24839,10 +25032,11 @@
       <c r="DI17"/>
       <c r="DJ17"/>
       <c r="DK17"/>
+      <c r="DL17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -25185,11 +25379,14 @@
       </c>
       <c r="DK18" t="n">
         <v>8.07899461400359</v>
+      </c>
+      <c r="DL18" t="n">
+        <v>9.51417004048581</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -25531,12 +25728,15 @@
         <v>5.32246463677775</v>
       </c>
       <c r="DK19" t="n">
-        <v>5.15490757615203</v>
+        <v>5.46732621713095</v>
+      </c>
+      <c r="DL19" t="n">
+        <v>5.38805136795087</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -25878,12 +26078,15 @@
         <v>5.16070620190131</v>
       </c>
       <c r="DK20" t="n">
-        <v>-1.84899845916795</v>
+        <v>-1.69491525423729</v>
+      </c>
+      <c r="DL20" t="n">
+        <v>3.03571428571428</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -26225,12 +26428,15 @@
         <v>1.63352272727272</v>
       </c>
       <c r="DK21" t="n">
-        <v>1.84331797235023</v>
+        <v>0.998463901689717</v>
+      </c>
+      <c r="DL21" t="n">
+        <v>1.06382978723405</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -26572,12 +26778,15 @@
         <v>0</v>
       </c>
       <c r="DK22" t="n">
-        <v>0.416319733555371</v>
+        <v>-0.416319733555371</v>
+      </c>
+      <c r="DL22" t="n">
+        <v>-0.493096646942787</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -26919,12 +27128,15 @@
         <v>2.35756385068764</v>
       </c>
       <c r="DK23" t="n">
-        <v>1.02179836512262</v>
+        <v>0.408719346049042</v>
+      </c>
+      <c r="DL23" t="n">
+        <v>-1.45513338722717</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -27266,12 +27478,15 @@
         <v>-0.139275766016725</v>
       </c>
       <c r="DK24" t="n">
-        <v>-0.897531787584135</v>
+        <v>-0.673148840688091</v>
+      </c>
+      <c r="DL24" t="n">
+        <v>-0.545171339563854</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -27613,12 +27828,15 @@
         <v>0.208333333333336</v>
       </c>
       <c r="DK25" t="n">
-        <v>-1.08695652173913</v>
+        <v>1.52173913043479</v>
+      </c>
+      <c r="DL25" t="n">
+        <v>3.11688311688312</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -27961,11 +28179,14 @@
       </c>
       <c r="DK26" t="n">
         <v>3.85405960945529</v>
+      </c>
+      <c r="DL26" t="n">
+        <v>3.56359649122807</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -28307,12 +28528,15 @@
         <v>3.12082032991529</v>
       </c>
       <c r="DK27" t="n">
-        <v>-0.088967971530244</v>
+        <v>-1.46797153024912</v>
+      </c>
+      <c r="DL27" t="n">
+        <v>-2.25790265930759</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -28654,12 +28878,15 @@
         <v>3.72492836676219</v>
       </c>
       <c r="DK28" t="n">
-        <v>1.87758167480285</v>
+        <v>1.68982350732257</v>
+      </c>
+      <c r="DL28" t="n">
+        <v>2.0973154362416</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -29001,12 +29228,15 @@
         <v>0.655241935483862</v>
       </c>
       <c r="DK29" t="n">
-        <v>-0.360082304526743</v>
+        <v>-0.77160493827159</v>
+      </c>
+      <c r="DL29" t="n">
+        <v>-2.35849056603774</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -29349,11 +29579,14 @@
       </c>
       <c r="DK30" t="n">
         <v>2.16271884654996</v>
+      </c>
+      <c r="DL30" t="n">
+        <v>1.51843817787418</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -29469,10 +29702,11 @@
       <c r="DI31"/>
       <c r="DJ31"/>
       <c r="DK31"/>
+      <c r="DL31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -29814,12 +30048,15 @@
         <v>-2.07373271889401</v>
       </c>
       <c r="DK32" t="n">
-        <v>-1.95599022004889</v>
+        <v>-3.17848410757946</v>
+      </c>
+      <c r="DL32" t="n">
+        <v>0.301204819277091</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -30161,12 +30398,15 @@
         <v>1.40692640692639</v>
       </c>
       <c r="DK33" t="n">
-        <v>2.66203703703703</v>
+        <v>2.08333333333333</v>
+      </c>
+      <c r="DL33" t="n">
+        <v>-1.39949109414758</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -30508,12 +30748,15 @@
         <v>2.01612903225806</v>
       </c>
       <c r="DK34" t="n">
-        <v>1.91740412979351</v>
+        <v>-0.147492625368723</v>
+      </c>
+      <c r="DL34" t="n">
+        <v>1.42405063291138</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -30855,12 +31098,15 @@
         <v>-2.86975717439293</v>
       </c>
       <c r="DK35" t="n">
-        <v>0.537634408602139</v>
+        <v>2.95698924731181</v>
+      </c>
+      <c r="DL35" t="n">
+        <v>-0.314465408805025</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -31202,12 +31448,15 @@
         <v>4.42083618917066</v>
       </c>
       <c r="DK36" t="n">
-        <v>4.96527777777778</v>
+        <v>4.93055555555555</v>
+      </c>
+      <c r="DL36" t="n">
+        <v>2.10743801652892</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -31549,12 +31798,15 @@
         <v>5.96393897364773</v>
       </c>
       <c r="DK37" t="n">
-        <v>2.04081632653061</v>
+        <v>0.156985871271588</v>
+      </c>
+      <c r="DL37" t="n">
+        <v>0.490998363338796</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -31896,12 +32148,15 @@
         <v>7.27673649393604</v>
       </c>
       <c r="DK38" t="n">
-        <v>7.41395947249918</v>
+        <v>7.20488903184303</v>
+      </c>
+      <c r="DL38" t="n">
+        <v>7.06734534064212</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -32244,11 +32499,14 @@
       </c>
       <c r="DK39" t="n">
         <v>-2.76001346348032</v>
+      </c>
+      <c r="DL39" t="n">
+        <v>0.292519849561215</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -32590,12 +32848,15 @@
         <v>5.44959128065395</v>
       </c>
       <c r="DK40" t="n">
-        <v>4.93827160493825</v>
+        <v>5.2469135802469</v>
+      </c>
+      <c r="DL40" t="n">
+        <v>10.6870229007634</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -32937,12 +33198,15 @@
         <v>-0.691121743753329</v>
       </c>
       <c r="DK41" t="n">
-        <v>-3.92655367231638</v>
+        <v>-2.57062146892656</v>
+      </c>
+      <c r="DL41" t="n">
+        <v>-0.45194335643266</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -33284,12 +33548,15 @@
         <v>1.30763936682724</v>
       </c>
       <c r="DK42" t="n">
-        <v>0.677710843373477</v>
+        <v>-1.28012048192772</v>
+      </c>
+      <c r="DL42" t="n">
+        <v>-0.909090909090916</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -33631,12 +33898,15 @@
         <v>4.33412135539795</v>
       </c>
       <c r="DK43" t="n">
-        <v>6.28571428571428</v>
+        <v>5.87755102040815</v>
+      </c>
+      <c r="DL43" t="n">
+        <v>-9.85533453887884</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -33978,12 +34248,15 @@
         <v>0.568720379146923</v>
       </c>
       <c r="DK44" t="n">
-        <v>0.838363514419852</v>
+        <v>-1.50905432595573</v>
+      </c>
+      <c r="DL44" t="n">
+        <v>-2.75938189845475</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -34326,11 +34599,14 @@
       </c>
       <c r="DK45" t="n">
         <v>0.740740740740751</v>
+      </c>
+      <c r="DL45" t="n">
+        <v>3.05676855895196</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -34672,12 +34948,15 @@
         <v>3.96475770925109</v>
       </c>
       <c r="DK46" t="n">
-        <v>0.843608046722915</v>
+        <v>3.50421804023362</v>
+      </c>
+      <c r="DL46" t="n">
+        <v>5.89459084604716</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -35020,11 +35299,14 @@
       </c>
       <c r="DK47" t="n">
         <v>2.7863777089783</v>
+      </c>
+      <c r="DL47" t="n">
+        <v>1.08303249097472</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -35366,12 +35648,15 @@
         <v>2.87179487179487</v>
       </c>
       <c r="DK48" t="n">
-        <v>1.59066808059385</v>
+        <v>1.43160127253447</v>
+      </c>
+      <c r="DL48" t="n">
+        <v>4.09429280397024</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -35713,12 +35998,15 @@
         <v>2.66870338754603</v>
       </c>
       <c r="DK49" t="n">
-        <v>1.84655156495247</v>
+        <v>1.93887914320009</v>
+      </c>
+      <c r="DL49" t="n">
+        <v>0.301175556203236</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -36061,11 +36349,14 @@
       </c>
       <c r="DK50" t="n">
         <v>1.69491525423729</v>
+      </c>
+      <c r="DL50" t="n">
+        <v>1.89431704885345</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -36407,12 +36698,15 @@
         <v>-2.02020202020201</v>
       </c>
       <c r="DK51" t="n">
-        <v>3.77358490566038</v>
+        <v>8.67924528301886</v>
+      </c>
+      <c r="DL51" t="n">
+        <v>10.3448275862069</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -36754,12 +37048,15 @@
         <v>3.06054557551563</v>
       </c>
       <c r="DK52" t="n">
-        <v>0.204081632653069</v>
+        <v>0.408163265306138</v>
+      </c>
+      <c r="DL52" t="n">
+        <v>-0.229182582123746</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -37101,12 +37398,15 @@
         <v>5.46131568059579</v>
       </c>
       <c r="DK53" t="n">
-        <v>3.46989966555184</v>
+        <v>3.63712374581941</v>
+      </c>
+      <c r="DL53" t="n">
+        <v>4.74922325787838</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -37448,12 +37748,15 @@
         <v>0.671140939597313</v>
       </c>
       <c r="DK54" t="n">
-        <v>0.362976406533568</v>
+        <v>-1.4519056261343</v>
+      </c>
+      <c r="DL54" t="n">
+        <v>-0.799999999999997</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -37795,12 +38098,15 @@
         <v>3.53178607467206</v>
       </c>
       <c r="DK55" t="n">
-        <v>2.18459858001092</v>
+        <v>1.74767886400875</v>
+      </c>
+      <c r="DL55" t="n">
+        <v>-0.772430184194897</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -38142,7 +38448,10 @@
         <v>1.00671140939598</v>
       </c>
       <c r="DK56" t="n">
-        <v>-1.7921146953405</v>
+        <v>-2.15053763440859</v>
+      </c>
+      <c r="DL56" t="n">
+        <v>0.413223140495874</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM update on 10-21-2022
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t xml:space="preserve">08/01/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/01/2022</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1275,10 +1278,13 @@
       <c r="DY4" t="s">
         <v>128</v>
       </c>
+      <c r="DZ4" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1659,15 +1665,18 @@
         <v>9977.4</v>
       </c>
       <c r="DX5" t="n">
-        <v>8986.4</v>
+        <v>8988.5</v>
       </c>
       <c r="DY5" t="n">
-        <v>9266.1</v>
+        <v>9363</v>
+      </c>
+      <c r="DZ5" t="n">
+        <v>10427</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2051,12 +2060,15 @@
         <v>157.7</v>
       </c>
       <c r="DY6" t="n">
-        <v>161.4</v>
+        <v>161.2</v>
+      </c>
+      <c r="DZ6" t="n">
+        <v>167.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2440,12 +2452,15 @@
         <v>16.6</v>
       </c>
       <c r="DY7" t="n">
-        <v>20.5</v>
+        <v>19.9</v>
+      </c>
+      <c r="DZ7" t="n">
+        <v>24.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2829,12 +2844,15 @@
         <v>148.1</v>
       </c>
       <c r="DY8" t="n">
-        <v>186.3</v>
+        <v>181.1</v>
+      </c>
+      <c r="DZ8" t="n">
+        <v>195.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3219,11 +3237,14 @@
       </c>
       <c r="DY9" t="n">
         <v>87.6</v>
+      </c>
+      <c r="DZ9" t="n">
+        <v>101.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3607,12 +3628,15 @@
         <v>1051.5</v>
       </c>
       <c r="DY10" t="n">
-        <v>1087.4</v>
+        <v>1107.4</v>
+      </c>
+      <c r="DZ10" t="n">
+        <v>1174</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -3996,12 +4020,15 @@
         <v>181.7</v>
       </c>
       <c r="DY11" t="n">
-        <v>188.1</v>
+        <v>194.2</v>
+      </c>
+      <c r="DZ11" t="n">
+        <v>210.2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4385,12 +4412,15 @@
         <v>96.6</v>
       </c>
       <c r="DY12" t="n">
-        <v>93.7</v>
+        <v>96.7</v>
+      </c>
+      <c r="DZ12" t="n">
+        <v>121.3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4775,11 +4805,14 @@
       </c>
       <c r="DY13" t="n">
         <v>31.8</v>
+      </c>
+      <c r="DZ13" t="n">
+        <v>34.9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4909,10 +4942,11 @@
       <c r="DW14"/>
       <c r="DX14"/>
       <c r="DY14"/>
+      <c r="DZ14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5296,12 +5330,15 @@
         <v>391</v>
       </c>
       <c r="DY15" t="n">
-        <v>459.7</v>
+        <v>460.3</v>
+      </c>
+      <c r="DZ15" t="n">
+        <v>483.8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5685,12 +5722,15 @@
         <v>320</v>
       </c>
       <c r="DY16" t="n">
-        <v>343</v>
+        <v>341.8</v>
+      </c>
+      <c r="DZ16" t="n">
+        <v>348.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -5820,10 +5860,11 @@
       <c r="DW17"/>
       <c r="DX17"/>
       <c r="DY17"/>
+      <c r="DZ17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6207,12 +6248,15 @@
         <v>54.4</v>
       </c>
       <c r="DY18" t="n">
-        <v>53.6</v>
+        <v>55.1</v>
+      </c>
+      <c r="DZ18" t="n">
+        <v>62.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6596,12 +6640,15 @@
         <v>378.9</v>
       </c>
       <c r="DY19" t="n">
-        <v>385.4</v>
+        <v>383.5</v>
+      </c>
+      <c r="DZ19" t="n">
+        <v>444.4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -6985,12 +7032,15 @@
         <v>173.8</v>
       </c>
       <c r="DY20" t="n">
-        <v>207.1</v>
+        <v>208.6</v>
+      </c>
+      <c r="DZ20" t="n">
+        <v>231.9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7374,12 +7424,15 @@
         <v>114.4</v>
       </c>
       <c r="DY21" t="n">
-        <v>117.4</v>
+        <v>119.4</v>
+      </c>
+      <c r="DZ21" t="n">
+        <v>142.2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -7763,12 +7816,15 @@
         <v>101.7</v>
       </c>
       <c r="DY22" t="n">
-        <v>110.2</v>
+        <v>111.1</v>
+      </c>
+      <c r="DZ22" t="n">
+        <v>131.5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8152,12 +8208,15 @@
         <v>122.8</v>
       </c>
       <c r="DY23" t="n">
-        <v>147.7</v>
+        <v>149.3</v>
+      </c>
+      <c r="DZ23" t="n">
+        <v>165.3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -8542,11 +8601,14 @@
       </c>
       <c r="DY24" t="n">
         <v>135.9</v>
+      </c>
+      <c r="DZ24" t="n">
+        <v>144</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -8930,12 +8992,15 @@
         <v>39.8</v>
       </c>
       <c r="DY25" t="n">
-        <v>38.6</v>
+        <v>38.7</v>
+      </c>
+      <c r="DZ25" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9320,11 +9385,14 @@
       </c>
       <c r="DY26" t="n">
         <v>188.6</v>
+      </c>
+      <c r="DZ26" t="n">
+        <v>213.4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -9708,12 +9776,15 @@
         <v>195.4</v>
       </c>
       <c r="DY27" t="n">
-        <v>193</v>
+        <v>191.7</v>
+      </c>
+      <c r="DZ27" t="n">
+        <v>219.7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10097,12 +10168,15 @@
         <v>243.5</v>
       </c>
       <c r="DY28" t="n">
-        <v>250.1</v>
+        <v>250.3</v>
+      </c>
+      <c r="DZ28" t="n">
+        <v>296.6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -10487,11 +10561,14 @@
       </c>
       <c r="DY29" t="n">
         <v>162.3</v>
+      </c>
+      <c r="DZ29" t="n">
+        <v>189</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -10875,12 +10952,15 @@
         <v>93.6</v>
       </c>
       <c r="DY30" t="n">
-        <v>97.3</v>
+        <v>99.2</v>
+      </c>
+      <c r="DZ30" t="n">
+        <v>103.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11010,10 +11090,11 @@
       <c r="DW31"/>
       <c r="DX31"/>
       <c r="DY31"/>
+      <c r="DZ31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -11397,12 +11478,15 @@
         <v>32.4</v>
       </c>
       <c r="DY32" t="n">
-        <v>32.7</v>
+        <v>31.8</v>
+      </c>
+      <c r="DZ32" t="n">
+        <v>39.9</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -11786,12 +11870,15 @@
         <v>77.5</v>
       </c>
       <c r="DY33" t="n">
-        <v>80</v>
+        <v>80.3</v>
+      </c>
+      <c r="DZ33" t="n">
+        <v>91.7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -12175,12 +12262,15 @@
         <v>64.1</v>
       </c>
       <c r="DY34" t="n">
-        <v>67.4</v>
+        <v>67.2</v>
+      </c>
+      <c r="DZ34" t="n">
+        <v>75.9</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -12564,12 +12654,15 @@
         <v>31.6</v>
       </c>
       <c r="DY35" t="n">
-        <v>31.7</v>
+        <v>32.2</v>
+      </c>
+      <c r="DZ35" t="n">
+        <v>44.9</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -12953,12 +13046,15 @@
         <v>248.3</v>
       </c>
       <c r="DY36" t="n">
-        <v>251</v>
+        <v>251.1</v>
+      </c>
+      <c r="DZ36" t="n">
+        <v>297.1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -13342,12 +13438,15 @@
         <v>60.5</v>
       </c>
       <c r="DY37" t="n">
-        <v>68.9</v>
+        <v>69.3</v>
+      </c>
+      <c r="DZ37" t="n">
+        <v>75.6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -13731,12 +13830,15 @@
         <v>547.3</v>
       </c>
       <c r="DY38" t="n">
-        <v>542.1</v>
+        <v>544.1</v>
+      </c>
+      <c r="DZ38" t="n">
+        <v>646.5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -14121,11 +14223,14 @@
       </c>
       <c r="DY39" t="n">
         <v>286.8</v>
+      </c>
+      <c r="DZ39" t="n">
+        <v>317.5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -14509,12 +14614,15 @@
         <v>29.1</v>
       </c>
       <c r="DY40" t="n">
-        <v>29.7</v>
+        <v>29.8</v>
+      </c>
+      <c r="DZ40" t="n">
+        <v>37.3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -14898,12 +15006,15 @@
         <v>330</v>
       </c>
       <c r="DY41" t="n">
-        <v>332.5</v>
+        <v>333.9</v>
+      </c>
+      <c r="DZ41" t="n">
+        <v>369.9</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -15287,12 +15398,15 @@
         <v>121.2</v>
       </c>
       <c r="DY42" t="n">
-        <v>126</v>
+        <v>124.7</v>
+      </c>
+      <c r="DZ42" t="n">
+        <v>140.6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -15677,11 +15791,14 @@
       </c>
       <c r="DY43" t="n">
         <v>109.8</v>
+      </c>
+      <c r="DZ43" t="n">
+        <v>122.1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -16065,12 +16182,15 @@
         <v>267</v>
       </c>
       <c r="DY44" t="n">
-        <v>269.1</v>
+        <v>270.9</v>
+      </c>
+      <c r="DZ44" t="n">
+        <v>319.4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -16455,11 +16575,14 @@
       </c>
       <c r="DY45" t="n">
         <v>23.9</v>
+      </c>
+      <c r="DZ45" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -16843,12 +16966,15 @@
         <v>151</v>
       </c>
       <c r="DY46" t="n">
-        <v>158.2</v>
+        <v>153.1</v>
+      </c>
+      <c r="DZ46" t="n">
+        <v>165.5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -17232,12 +17358,15 @@
         <v>28.2</v>
       </c>
       <c r="DY47" t="n">
-        <v>29.2</v>
+        <v>29.3</v>
+      </c>
+      <c r="DZ47" t="n">
+        <v>36.8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -17622,11 +17751,14 @@
       </c>
       <c r="DY48" t="n">
         <v>183</v>
+      </c>
+      <c r="DZ48" t="n">
+        <v>206.1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -18010,12 +18142,15 @@
         <v>1036.4</v>
       </c>
       <c r="DY49" t="n">
-        <v>1048.3</v>
+        <v>1051.7</v>
+      </c>
+      <c r="DZ49" t="n">
+        <v>1116.3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -18400,11 +18535,14 @@
       </c>
       <c r="DY50" t="n">
         <v>108.2</v>
+      </c>
+      <c r="DZ50" t="n">
+        <v>121.6</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -18788,12 +18926,15 @@
         <v>25.6</v>
       </c>
       <c r="DY51" t="n">
-        <v>24.8</v>
+        <v>24.4</v>
+      </c>
+      <c r="DZ51" t="n">
+        <v>30.9</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -19177,12 +19318,15 @@
         <v>261.6</v>
       </c>
       <c r="DY52" t="n">
-        <v>283.1</v>
+        <v>283.4</v>
+      </c>
+      <c r="DZ52" t="n">
+        <v>315.3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -19566,12 +19710,15 @@
         <v>237</v>
       </c>
       <c r="DY53" t="n">
-        <v>226.9</v>
+        <v>231.7</v>
+      </c>
+      <c r="DZ53" t="n">
+        <v>239</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -19955,12 +20102,15 @@
         <v>49.6</v>
       </c>
       <c r="DY54" t="n">
-        <v>53</v>
+        <v>52.9</v>
+      </c>
+      <c r="DZ54" t="n">
+        <v>57.3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -20344,12 +20494,15 @@
         <v>169.4</v>
       </c>
       <c r="DY55" t="n">
-        <v>166.6</v>
+        <v>166.5</v>
+      </c>
+      <c r="DZ55" t="n">
+        <v>202.4</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -20733,7 +20886,10 @@
         <v>24.3</v>
       </c>
       <c r="DY56" t="n">
-        <v>24.6</v>
+        <v>24.7</v>
+      </c>
+      <c r="DZ56" t="n">
+        <v>28.9</v>
       </c>
     </row>
   </sheetData>
@@ -21102,10 +21258,13 @@
       <c r="DM4" t="s">
         <v>128</v>
       </c>
+      <c r="DN4" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -21450,15 +21609,18 @@
         <v>1.41901644676658</v>
       </c>
       <c r="DL5" t="n">
-        <v>1.40031368832019</v>
+        <v>1.42400956862215</v>
       </c>
       <c r="DM5" t="n">
-        <v>0.359583662771165</v>
+        <v>1.40909140140149</v>
+      </c>
+      <c r="DN5" t="n">
+        <v>1.27037159340338</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -21806,12 +21968,15 @@
         <v>1.28452151573539</v>
       </c>
       <c r="DM6" t="n">
-        <v>1.57331655129012</v>
+        <v>1.4474512271869</v>
+      </c>
+      <c r="DN6" t="n">
+        <v>1.64133738601823</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -22159,12 +22324,15 @@
         <v>-17.4129353233831</v>
       </c>
       <c r="DM7" t="n">
-        <v>-8.07174887892375</v>
+        <v>-10.762331838565</v>
+      </c>
+      <c r="DN7" t="n">
+        <v>-6.76691729323309</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -22512,12 +22680,15 @@
         <v>1.36892539356605</v>
       </c>
       <c r="DM8" t="n">
-        <v>4.66292134831461</v>
+        <v>1.74157303370788</v>
+      </c>
+      <c r="DN8" t="n">
+        <v>1.29466597617816</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -22866,11 +23037,14 @@
       </c>
       <c r="DM9" t="n">
         <v>2.21703617269544</v>
+      </c>
+      <c r="DN9" t="n">
+        <v>2.2199798183653</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -23218,12 +23392,15 @@
         <v>4.3776057176891</v>
       </c>
       <c r="DM10" t="n">
-        <v>2.4110001883594</v>
+        <v>4.29459408551518</v>
+      </c>
+      <c r="DN10" t="n">
+        <v>2.59547321506598</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -23571,12 +23748,15 @@
         <v>-2.57372654155497</v>
       </c>
       <c r="DM11" t="n">
-        <v>-1.82672233820459</v>
+        <v>1.35699373695198</v>
+      </c>
+      <c r="DN11" t="n">
+        <v>0.76701821668263</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -23924,12 +24104,15 @@
         <v>-0.103412616339173</v>
       </c>
       <c r="DM12" t="n">
-        <v>-0.846560846560844</v>
+        <v>2.32804232804233</v>
+      </c>
+      <c r="DN12" t="n">
+        <v>1.93277310924371</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -24278,11 +24461,14 @@
       </c>
       <c r="DM13" t="n">
         <v>-0.0000000000000111720555937123</v>
+      </c>
+      <c r="DN13" t="n">
+        <v>0.86705202312142</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -24400,10 +24586,11 @@
       <c r="DK14"/>
       <c r="DL14"/>
       <c r="DM14"/>
+      <c r="DN14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -24751,12 +24938,15 @@
         <v>0.851173587825641</v>
       </c>
       <c r="DM15" t="n">
-        <v>1.47902869757175</v>
+        <v>1.61147902869757</v>
+      </c>
+      <c r="DN15" t="n">
+        <v>1.06538541884269</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -25104,12 +25294,15 @@
         <v>4.43864229765014</v>
       </c>
       <c r="DM16" t="n">
-        <v>3.75075620084694</v>
+        <v>3.38777979431337</v>
+      </c>
+      <c r="DN16" t="n">
+        <v>3.72467222884386</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -25227,10 +25420,11 @@
       <c r="DK17"/>
       <c r="DL17"/>
       <c r="DM17"/>
+      <c r="DN17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -25578,12 +25772,15 @@
         <v>10.1214574898785</v>
       </c>
       <c r="DM18" t="n">
-        <v>8.50202429149797</v>
+        <v>11.5384615384615</v>
+      </c>
+      <c r="DN18" t="n">
+        <v>6.27118644067797</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -25931,12 +26128,15 @@
         <v>5.77889447236181</v>
       </c>
       <c r="DM19" t="n">
-        <v>5.7628979143798</v>
+        <v>5.24149286498352</v>
+      </c>
+      <c r="DN19" t="n">
+        <v>5.15854235683861</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -26284,12 +26484,15 @@
         <v>3.45238095238096</v>
       </c>
       <c r="DM20" t="n">
-        <v>0.925925925925929</v>
+        <v>1.65692007797273</v>
+      </c>
+      <c r="DN20" t="n">
+        <v>0.957771005659563</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -26637,12 +26840,15 @@
         <v>1.41843971631206</v>
       </c>
       <c r="DM21" t="n">
-        <v>0.686106346483715</v>
+        <v>2.40137221269298</v>
+      </c>
+      <c r="DN21" t="n">
+        <v>2.52343186733958</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -26990,12 +27196,15 @@
         <v>0.295857988165692</v>
       </c>
       <c r="DM22" t="n">
-        <v>-0.361663652802886</v>
+        <v>0.45207956600363</v>
+      </c>
+      <c r="DN22" t="n">
+        <v>0.843558282208585</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -27343,12 +27552,15 @@
         <v>-0.727566693613586</v>
       </c>
       <c r="DM23" t="n">
-        <v>1.65175498967652</v>
+        <v>2.75292498279422</v>
+      </c>
+      <c r="DN23" t="n">
+        <v>7.12896953985742</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -27697,11 +27909,14 @@
       </c>
       <c r="DM24" t="n">
         <v>0.741289844329112</v>
+      </c>
+      <c r="DN24" t="n">
+        <v>0.769769069279212</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -28049,12 +28264,15 @@
         <v>3.37662337662337</v>
       </c>
       <c r="DM25" t="n">
-        <v>2.38726790450928</v>
+        <v>2.6525198938992</v>
+      </c>
+      <c r="DN25" t="n">
+        <v>2.08333333333333</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -28403,11 +28621,14 @@
       </c>
       <c r="DM26" t="n">
         <v>1.61637931034481</v>
+      </c>
+      <c r="DN26" t="n">
+        <v>4.86486486486487</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -28755,12 +28976,15 @@
         <v>-1.9568489713999</v>
       </c>
       <c r="DM27" t="n">
-        <v>-2.03045685279188</v>
+        <v>-2.69035532994923</v>
+      </c>
+      <c r="DN27" t="n">
+        <v>-1.34710372698699</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -29108,12 +29332,15 @@
         <v>2.13926174496644</v>
       </c>
       <c r="DM28" t="n">
-        <v>0.846774193548385</v>
+        <v>0.927419354838714</v>
+      </c>
+      <c r="DN28" t="n">
+        <v>1.09066121336062</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -29462,11 +29689,14 @@
       </c>
       <c r="DM29" t="n">
         <v>-2.11097708082027</v>
+      </c>
+      <c r="DN29" t="n">
+        <v>-0.158478605388279</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -29814,12 +30044,15 @@
         <v>1.51843817787418</v>
       </c>
       <c r="DM30" t="n">
-        <v>-0.815494393476027</v>
+        <v>1.12130479102956</v>
+      </c>
+      <c r="DN30" t="n">
+        <v>-0.289017341040473</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -29937,10 +30170,11 @@
       <c r="DK31"/>
       <c r="DL31"/>
       <c r="DM31"/>
+      <c r="DN31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -30288,12 +30522,15 @@
         <v>-2.40963855421688</v>
       </c>
       <c r="DM32" t="n">
-        <v>-5.21739130434782</v>
+        <v>-7.82608695652174</v>
+      </c>
+      <c r="DN32" t="n">
+        <v>-4.54545454545453</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -30641,12 +30878,15 @@
         <v>-1.39949109414758</v>
       </c>
       <c r="DM33" t="n">
-        <v>0.755667506297222</v>
+        <v>1.13350125944583</v>
+      </c>
+      <c r="DN33" t="n">
+        <v>1.77580466148725</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -30994,12 +31234,15 @@
         <v>1.42405063291138</v>
       </c>
       <c r="DM34" t="n">
-        <v>3.37423312883436</v>
+        <v>3.06748466257666</v>
+      </c>
+      <c r="DN34" t="n">
+        <v>-1.55642023346302</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -31347,12 +31590,15 @@
         <v>-0.628930817610061</v>
       </c>
       <c r="DM35" t="n">
-        <v>-3.05810397553517</v>
+        <v>-1.52905198776758</v>
+      </c>
+      <c r="DN35" t="n">
+        <v>2.27790432801821</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -31700,12 +31946,15 @@
         <v>2.60330578512397</v>
       </c>
       <c r="DM36" t="n">
-        <v>1.90824198132358</v>
+        <v>1.94884287454324</v>
+      </c>
+      <c r="DN36" t="n">
+        <v>3.01664355062415</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -32053,12 +32302,15 @@
         <v>-0.981996726677569</v>
       </c>
       <c r="DM37" t="n">
-        <v>2.68256333830106</v>
+        <v>3.27868852459017</v>
+      </c>
+      <c r="DN37" t="n">
+        <v>4.13223140495868</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -32406,12 +32658,15 @@
         <v>7.1456538762725</v>
       </c>
       <c r="DM38" t="n">
-        <v>7.34653465346535</v>
+        <v>7.74257425742575</v>
+      </c>
+      <c r="DN38" t="n">
+        <v>3.47311139564661</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -32760,11 +33015,14 @@
       </c>
       <c r="DM39" t="n">
         <v>-0.554785020804426</v>
+      </c>
+      <c r="DN39" t="n">
+        <v>0.189334174818562</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -33112,12 +33370,15 @@
         <v>11.0687022900763</v>
       </c>
       <c r="DM40" t="n">
-        <v>6.83453237410073</v>
+        <v>7.19424460431653</v>
+      </c>
+      <c r="DN40" t="n">
+        <v>3.32409972299168</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -33465,12 +33726,15 @@
         <v>-0.572461584814696</v>
       </c>
       <c r="DM41" t="n">
-        <v>0.544299969761116</v>
+        <v>0.967644390686419</v>
+      </c>
+      <c r="DN41" t="n">
+        <v>1.84471365638766</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -33818,12 +34082,15 @@
         <v>0.165289256198338</v>
       </c>
       <c r="DM42" t="n">
-        <v>0.0794281175536208</v>
+        <v>-0.95313741064337</v>
+      </c>
+      <c r="DN42" t="n">
+        <v>-1.81564245810055</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -34172,11 +34439,14 @@
       </c>
       <c r="DM43" t="n">
         <v>0.826446280991728</v>
+      </c>
+      <c r="DN43" t="n">
+        <v>2.09030100334448</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -34524,12 +34794,15 @@
         <v>-1.76600441501104</v>
       </c>
       <c r="DM44" t="n">
-        <v>-2.67631103074142</v>
+        <v>-2.02531645569621</v>
+      </c>
+      <c r="DN44" t="n">
+        <v>0.440251572327037</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -34878,11 +35151,14 @@
       </c>
       <c r="DM45" t="n">
         <v>9.1324200913242</v>
+      </c>
+      <c r="DN45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -35230,12 +35506,15 @@
         <v>4.71567267683773</v>
       </c>
       <c r="DM46" t="n">
-        <v>4.42244224422442</v>
+        <v>1.05610561056105</v>
+      </c>
+      <c r="DN46" t="n">
+        <v>2.79503105590062</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -35583,12 +35862,15 @@
         <v>1.80505415162454</v>
       </c>
       <c r="DM47" t="n">
-        <v>1.38888888888891</v>
+        <v>1.73611111111111</v>
+      </c>
+      <c r="DN47" t="n">
+        <v>3.08123249299718</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -35937,11 +36219,14 @@
       </c>
       <c r="DM48" t="n">
         <v>2.92463442069741</v>
+      </c>
+      <c r="DN48" t="n">
+        <v>1.92878338278933</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -36289,12 +36574,15 @@
         <v>0.689789177110649</v>
       </c>
       <c r="DM49" t="n">
-        <v>1.13844669561022</v>
+        <v>1.46647370959962</v>
+      </c>
+      <c r="DN49" t="n">
+        <v>0.549450549450541</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -36643,11 +36931,14 @@
       </c>
       <c r="DM50" t="n">
         <v>1.7873941674506</v>
+      </c>
+      <c r="DN50" t="n">
+        <v>1.67224080267559</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -36995,12 +37286,15 @@
         <v>10.3448275862069</v>
       </c>
       <c r="DM51" t="n">
-        <v>2.4793388429752</v>
+        <v>0.826446280991733</v>
+      </c>
+      <c r="DN51" t="n">
+        <v>5.46075085324234</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -37348,12 +37642,15 @@
         <v>-0.0763941940412485</v>
       </c>
       <c r="DM52" t="n">
-        <v>1.61521895190237</v>
+        <v>1.72290021536251</v>
+      </c>
+      <c r="DN52" t="n">
+        <v>3.75123395853899</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -37701,12 +37998,15 @@
         <v>5.19307589880159</v>
       </c>
       <c r="DM53" t="n">
-        <v>3.98716773602199</v>
+        <v>6.18698441796518</v>
+      </c>
+      <c r="DN53" t="n">
+        <v>2.3993144815767</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -38054,12 +38354,15 @@
         <v>-0.799999999999997</v>
       </c>
       <c r="DM54" t="n">
-        <v>0.189035916824199</v>
+        <v>0.0000000000000134318097497183</v>
+      </c>
+      <c r="DN54" t="n">
+        <v>-1.71526586620926</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -38407,12 +38710,15 @@
         <v>0.65359477124181</v>
       </c>
       <c r="DM55" t="n">
-        <v>2.71270036991371</v>
+        <v>2.65104808877929</v>
+      </c>
+      <c r="DN55" t="n">
+        <v>2.27387569479537</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -38760,7 +39066,10 @@
         <v>0.413223140495874</v>
       </c>
       <c r="DM56" t="n">
-        <v>-0.404858299595162</v>
+        <v>-0.0000000000000143834561894757</v>
+      </c>
+      <c r="DN56" t="n">
+        <v>0.696864111498255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on December, 16th
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t xml:space="preserve">10/01/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/01/2022</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1287,10 +1290,13 @@
       <c r="EA4" t="s">
         <v>130</v>
       </c>
+      <c r="EB4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1677,15 +1683,18 @@
         <v>9367.3</v>
       </c>
       <c r="DZ5" t="n">
-        <v>10451.6</v>
+        <v>10465.6</v>
       </c>
       <c r="EA5" t="n">
-        <v>10779.6</v>
+        <v>10783.6</v>
+      </c>
+      <c r="EB5" t="n">
+        <v>10896.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2075,12 +2084,15 @@
         <v>167.4</v>
       </c>
       <c r="EA6" t="n">
-        <v>170.3</v>
+        <v>170.2</v>
+      </c>
+      <c r="EB6" t="n">
+        <v>171.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2471,11 +2483,14 @@
       </c>
       <c r="EA7" t="n">
         <v>29.2</v>
+      </c>
+      <c r="EB7" t="n">
+        <v>29.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2865,12 +2880,15 @@
         <v>195.3</v>
       </c>
       <c r="EA8" t="n">
-        <v>198</v>
+        <v>198.2</v>
+      </c>
+      <c r="EB8" t="n">
+        <v>201.7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3261,11 +3279,14 @@
       </c>
       <c r="EA9" t="n">
         <v>103.2</v>
+      </c>
+      <c r="EB9" t="n">
+        <v>103.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3655,12 +3676,15 @@
         <v>1172.9</v>
       </c>
       <c r="EA10" t="n">
-        <v>1210.1</v>
+        <v>1216.4</v>
+      </c>
+      <c r="EB10" t="n">
+        <v>1239.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4050,12 +4074,15 @@
         <v>210.6</v>
       </c>
       <c r="EA11" t="n">
-        <v>216.7</v>
+        <v>216.6</v>
+      </c>
+      <c r="EB11" t="n">
+        <v>219</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4445,12 +4472,15 @@
         <v>121.3</v>
       </c>
       <c r="EA12" t="n">
-        <v>124.8</v>
+        <v>124.2</v>
+      </c>
+      <c r="EB12" t="n">
+        <v>126.1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4840,12 +4870,15 @@
         <v>36.3</v>
       </c>
       <c r="EA13" t="n">
-        <v>37.3</v>
+        <v>37.2</v>
+      </c>
+      <c r="EB13" t="n">
+        <v>37.8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -4977,10 +5010,11 @@
       <c r="DY14"/>
       <c r="DZ14"/>
       <c r="EA14"/>
+      <c r="EB14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5371,11 +5405,14 @@
       </c>
       <c r="EA15" t="n">
         <v>489.8</v>
+      </c>
+      <c r="EB15" t="n">
+        <v>493.9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5765,12 +5802,15 @@
         <v>348</v>
       </c>
       <c r="EA16" t="n">
-        <v>351</v>
+        <v>350.9</v>
+      </c>
+      <c r="EB16" t="n">
+        <v>352.7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -5902,10 +5942,11 @@
       <c r="DY17"/>
       <c r="DZ17"/>
       <c r="EA17"/>
+      <c r="EB17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6295,12 +6336,15 @@
         <v>62.8</v>
       </c>
       <c r="EA18" t="n">
-        <v>65.7</v>
+        <v>65.6</v>
+      </c>
+      <c r="EB18" t="n">
+        <v>66.4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6690,12 +6734,15 @@
         <v>443</v>
       </c>
       <c r="EA19" t="n">
-        <v>446.7</v>
+        <v>446.8</v>
+      </c>
+      <c r="EB19" t="n">
+        <v>447.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7085,12 +7132,15 @@
         <v>232.4</v>
       </c>
       <c r="EA20" t="n">
-        <v>234.5</v>
+        <v>234.3</v>
+      </c>
+      <c r="EB20" t="n">
+        <v>235.8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7480,12 +7530,15 @@
         <v>141.5</v>
       </c>
       <c r="EA21" t="n">
-        <v>146.6</v>
+        <v>146.7</v>
+      </c>
+      <c r="EB21" t="n">
+        <v>148</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -7875,12 +7928,15 @@
         <v>131.3</v>
       </c>
       <c r="EA22" t="n">
-        <v>135.9</v>
+        <v>135.8</v>
+      </c>
+      <c r="EB22" t="n">
+        <v>136.8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8270,12 +8326,15 @@
         <v>161.9</v>
       </c>
       <c r="EA23" t="n">
-        <v>163.7</v>
+        <v>163.5</v>
+      </c>
+      <c r="EB23" t="n">
+        <v>165.7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -8665,12 +8724,15 @@
         <v>144.2</v>
       </c>
       <c r="EA24" t="n">
-        <v>145.6</v>
+        <v>145.3</v>
+      </c>
+      <c r="EB24" t="n">
+        <v>147.2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9061,11 +9123,14 @@
       </c>
       <c r="EA25" t="n">
         <v>50.1</v>
+      </c>
+      <c r="EB25" t="n">
+        <v>49.8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9456,11 +9521,14 @@
       </c>
       <c r="EA26" t="n">
         <v>217.8</v>
+      </c>
+      <c r="EB26" t="n">
+        <v>220.1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -9850,12 +9918,15 @@
         <v>231</v>
       </c>
       <c r="EA27" t="n">
-        <v>241.8</v>
+        <v>241.5</v>
+      </c>
+      <c r="EB27" t="n">
+        <v>245.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10246,11 +10317,14 @@
       </c>
       <c r="EA28" t="n">
         <v>311.6</v>
+      </c>
+      <c r="EB28" t="n">
+        <v>315.2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -10640,12 +10714,15 @@
         <v>189.1</v>
       </c>
       <c r="EA29" t="n">
-        <v>200.9</v>
+        <v>200.8</v>
+      </c>
+      <c r="EB29" t="n">
+        <v>203.3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11035,12 +11112,15 @@
         <v>103.9</v>
       </c>
       <c r="EA30" t="n">
-        <v>104.5</v>
+        <v>104.4</v>
+      </c>
+      <c r="EB30" t="n">
+        <v>104.3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11172,10 +11252,11 @@
       <c r="DY31"/>
       <c r="DZ31"/>
       <c r="EA31"/>
+      <c r="EB31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -11565,12 +11646,15 @@
         <v>40.8</v>
       </c>
       <c r="EA32" t="n">
-        <v>42.3</v>
+        <v>41.8</v>
+      </c>
+      <c r="EB32" t="n">
+        <v>42.4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -11960,12 +12044,15 @@
         <v>91.6</v>
       </c>
       <c r="EA33" t="n">
-        <v>95.5</v>
+        <v>95.3</v>
+      </c>
+      <c r="EB33" t="n">
+        <v>96</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -12355,12 +12442,15 @@
         <v>75.8</v>
       </c>
       <c r="EA34" t="n">
-        <v>76.8</v>
+        <v>77.2</v>
+      </c>
+      <c r="EB34" t="n">
+        <v>78.8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -12750,12 +12840,15 @@
         <v>44.1</v>
       </c>
       <c r="EA35" t="n">
-        <v>46.1</v>
+        <v>45.3</v>
+      </c>
+      <c r="EB35" t="n">
+        <v>45.5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -13145,12 +13238,15 @@
         <v>297.6</v>
       </c>
       <c r="EA36" t="n">
-        <v>313.3</v>
+        <v>312.8</v>
+      </c>
+      <c r="EB36" t="n">
+        <v>315.4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -13541,11 +13637,14 @@
       </c>
       <c r="EA37" t="n">
         <v>76.7</v>
+      </c>
+      <c r="EB37" t="n">
+        <v>77.9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -13935,12 +14034,15 @@
         <v>646.1</v>
       </c>
       <c r="EA38" t="n">
-        <v>687.6</v>
+        <v>687.4</v>
+      </c>
+      <c r="EB38" t="n">
+        <v>693.8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -14331,11 +14433,14 @@
       </c>
       <c r="EA39" t="n">
         <v>327.8</v>
+      </c>
+      <c r="EB39" t="n">
+        <v>334.9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -14726,11 +14831,14 @@
       </c>
       <c r="EA40" t="n">
         <v>39.1</v>
+      </c>
+      <c r="EB40" t="n">
+        <v>39.7</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -15120,12 +15228,15 @@
         <v>368</v>
       </c>
       <c r="EA41" t="n">
-        <v>387.7</v>
+        <v>377.6</v>
+      </c>
+      <c r="EB41" t="n">
+        <v>383.6</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -15515,12 +15626,15 @@
         <v>141.2</v>
       </c>
       <c r="EA42" t="n">
-        <v>144.2</v>
+        <v>144.3</v>
+      </c>
+      <c r="EB42" t="n">
+        <v>145</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -15910,12 +16024,15 @@
         <v>123.7</v>
       </c>
       <c r="EA43" t="n">
-        <v>135.3</v>
+        <v>134.5</v>
+      </c>
+      <c r="EB43" t="n">
+        <v>137.7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -16305,12 +16422,15 @@
         <v>318.3</v>
       </c>
       <c r="EA44" t="n">
-        <v>326.3</v>
+        <v>325.7</v>
+      </c>
+      <c r="EB44" t="n">
+        <v>330.1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -16701,11 +16821,14 @@
       </c>
       <c r="EA45" t="n">
         <v>28.9</v>
+      </c>
+      <c r="EB45" t="n">
+        <v>29.2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -17095,12 +17218,15 @@
         <v>165.4</v>
       </c>
       <c r="EA46" t="n">
-        <v>169.7</v>
+        <v>169.6</v>
+      </c>
+      <c r="EB46" t="n">
+        <v>171.4</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -17491,11 +17617,14 @@
       </c>
       <c r="EA47" t="n">
         <v>38.2</v>
+      </c>
+      <c r="EB47" t="n">
+        <v>38.5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -17886,11 +18015,14 @@
       </c>
       <c r="EA48" t="n">
         <v>209</v>
+      </c>
+      <c r="EB48" t="n">
+        <v>209.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -18280,12 +18412,15 @@
         <v>1116.9</v>
       </c>
       <c r="EA49" t="n">
-        <v>1153.4</v>
+        <v>1152.2</v>
+      </c>
+      <c r="EB49" t="n">
+        <v>1161.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -18676,11 +18811,14 @@
       </c>
       <c r="EA50" t="n">
         <v>125</v>
+      </c>
+      <c r="EB50" t="n">
+        <v>126.2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -19070,12 +19208,15 @@
         <v>30.8</v>
       </c>
       <c r="EA51" t="n">
-        <v>32.3</v>
+        <v>32.2</v>
+      </c>
+      <c r="EB51" t="n">
+        <v>32.2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -19465,12 +19606,15 @@
         <v>315.5</v>
       </c>
       <c r="EA52" t="n">
-        <v>319.6</v>
+        <v>322</v>
+      </c>
+      <c r="EB52" t="n">
+        <v>325.7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -19860,12 +20004,15 @@
         <v>242.8</v>
       </c>
       <c r="EA53" t="n">
-        <v>260.9</v>
+        <v>257</v>
+      </c>
+      <c r="EB53" t="n">
+        <v>260</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -20256,11 +20403,14 @@
       </c>
       <c r="EA54" t="n">
         <v>58.6</v>
+      </c>
+      <c r="EB54" t="n">
+        <v>59.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -20650,12 +20800,15 @@
         <v>202.9</v>
       </c>
       <c r="EA55" t="n">
-        <v>212.2</v>
+        <v>212.3</v>
+      </c>
+      <c r="EB55" t="n">
+        <v>213.9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -21046,6 +21199,9 @@
       </c>
       <c r="EA56" t="n">
         <v>30.2</v>
+      </c>
+      <c r="EB56" t="n">
+        <v>30.4</v>
       </c>
     </row>
   </sheetData>
@@ -21420,10 +21576,13 @@
       <c r="DO4" t="s">
         <v>130</v>
       </c>
+      <c r="DP4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -21774,15 +21933,18 @@
         <v>1.45566398423028</v>
       </c>
       <c r="DN5" t="n">
-        <v>1.50929469124531</v>
+        <v>1.6452671859521</v>
       </c>
       <c r="DO5" t="n">
-        <v>1.56211724358855</v>
+        <v>1.59980402871734</v>
+      </c>
+      <c r="DP5" t="n">
+        <v>1.80031204163045</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -22136,12 +22298,15 @@
         <v>1.7629179331307</v>
       </c>
       <c r="DO6" t="n">
-        <v>1.67164179104478</v>
+        <v>1.61194029850746</v>
+      </c>
+      <c r="DP6" t="n">
+        <v>1.78041543026706</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -22496,11 +22661,14 @@
       </c>
       <c r="DO7" t="n">
         <v>5.79710144927535</v>
+      </c>
+      <c r="DP7" t="n">
+        <v>7.22021660649821</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -22854,12 +23022,15 @@
         <v>1.13930605903678</v>
       </c>
       <c r="DO8" t="n">
-        <v>1.59055926115957</v>
+        <v>1.69317598768598</v>
+      </c>
+      <c r="DP8" t="n">
+        <v>1.86868686868686</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -23214,11 +23385,14 @@
       </c>
       <c r="DO9" t="n">
         <v>0.781249999999997</v>
+      </c>
+      <c r="DP9" t="n">
+        <v>0.971817298347911</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -23572,12 +23746,15 @@
         <v>2.49934457747095</v>
       </c>
       <c r="DO10" t="n">
-        <v>1.0015858442534</v>
+        <v>1.52741841248645</v>
+      </c>
+      <c r="DP10" t="n">
+        <v>1.62335000409936</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -23931,12 +24108,15 @@
         <v>0.958772770853294</v>
       </c>
       <c r="DO11" t="n">
-        <v>1.88058298072404</v>
+        <v>1.83356840620593</v>
+      </c>
+      <c r="DP11" t="n">
+        <v>1.81311018131101</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -24290,12 +24470,15 @@
         <v>1.93277310924371</v>
       </c>
       <c r="DO12" t="n">
-        <v>1.5459723352319</v>
+        <v>1.05777054515865</v>
+      </c>
+      <c r="DP12" t="n">
+        <v>1.28514056224899</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -24649,12 +24832,15 @@
         <v>4.91329479768787</v>
       </c>
       <c r="DO13" t="n">
-        <v>4.18994413407821</v>
+        <v>3.91061452513968</v>
+      </c>
+      <c r="DP13" t="n">
+        <v>4.13223140495868</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -24774,10 +24960,11 @@
       <c r="DM14"/>
       <c r="DN14"/>
       <c r="DO14"/>
+      <c r="DP14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -25132,11 +25319,14 @@
       </c>
       <c r="DO15" t="n">
         <v>1.19834710743802</v>
+      </c>
+      <c r="DP15" t="n">
+        <v>1.06404747288725</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -25490,12 +25680,15 @@
         <v>3.6948748510131</v>
       </c>
       <c r="DO16" t="n">
-        <v>3.66213821618428</v>
+        <v>3.63260484347311</v>
+      </c>
+      <c r="DP16" t="n">
+        <v>4.19497784342688</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -25615,10 +25808,11 @@
       <c r="DM17"/>
       <c r="DN17"/>
       <c r="DO17"/>
+      <c r="DP17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -25972,12 +26166,15 @@
         <v>6.4406779661017</v>
       </c>
       <c r="DO18" t="n">
-        <v>5.28846153846155</v>
+        <v>5.12820512820512</v>
+      </c>
+      <c r="DP18" t="n">
+        <v>5.22979397781301</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -26331,12 +26528,15 @@
         <v>4.8272598201609</v>
       </c>
       <c r="DO19" t="n">
-        <v>2.90255701451278</v>
+        <v>2.92559318129463</v>
+      </c>
+      <c r="DP19" t="n">
+        <v>2.054325496462</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -26690,12 +26890,15 @@
         <v>1.17544623421855</v>
       </c>
       <c r="DO20" t="n">
-        <v>0.816852966466026</v>
+        <v>0.730868443680133</v>
+      </c>
+      <c r="DP20" t="n">
+        <v>0.38314176245211</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -27049,12 +27252,15 @@
         <v>2.01874549387167</v>
       </c>
       <c r="DO21" t="n">
-        <v>1.87630298818625</v>
+        <v>1.94579569145239</v>
+      </c>
+      <c r="DP21" t="n">
+        <v>1.92837465564739</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -27408,12 +27614,15 @@
         <v>0.690184049079759</v>
       </c>
       <c r="DO22" t="n">
-        <v>1.4179104477612</v>
+        <v>1.34328358208954</v>
+      </c>
+      <c r="DP22" t="n">
+        <v>1.18343195266274</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -27767,12 +27976,15 @@
         <v>4.92546986390147</v>
       </c>
       <c r="DO23" t="n">
-        <v>4.5338441890166</v>
+        <v>4.40613026819924</v>
+      </c>
+      <c r="DP23" t="n">
+        <v>4.93983533882203</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -28126,12 +28338,15 @@
         <v>0.909727081875425</v>
       </c>
       <c r="DO24" t="n">
-        <v>0.413793103448292</v>
+        <v>0.206896551724146</v>
+      </c>
+      <c r="DP24" t="n">
+        <v>0.891021247429735</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -28486,11 +28701,14 @@
       </c>
       <c r="DO25" t="n">
         <v>1.62271805273833</v>
+      </c>
+      <c r="DP25" t="n">
+        <v>0.201207243460753</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -28845,11 +29063,14 @@
       </c>
       <c r="DO26" t="n">
         <v>1.8232819074334</v>
+      </c>
+      <c r="DP26" t="n">
+        <v>2.03987019007882</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -29203,12 +29424,15 @@
         <v>3.7269869779973</v>
       </c>
       <c r="DO27" t="n">
-        <v>6.14574187884109</v>
+        <v>6.01404741000877</v>
+      </c>
+      <c r="DP27" t="n">
+        <v>6.91605045672032</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -29563,11 +29787,14 @@
       </c>
       <c r="DO28" t="n">
         <v>2.80435499835038</v>
+      </c>
+      <c r="DP28" t="n">
+        <v>3.07390451275343</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -29921,12 +30148,15 @@
         <v>-0.105652403592176</v>
       </c>
       <c r="DO29" t="n">
-        <v>0.500250125062517</v>
+        <v>0.450225112556281</v>
+      </c>
+      <c r="DP29" t="n">
+        <v>0.544015825914933</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -30280,12 +30510,15 @@
         <v>0.0963391136801486</v>
       </c>
       <c r="DO30" t="n">
-        <v>0.0957854406130214</v>
+        <v>0</v>
+      </c>
+      <c r="DP30" t="n">
+        <v>0.0959692898272635</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -30405,10 +30638,11 @@
       <c r="DM31"/>
       <c r="DN31"/>
       <c r="DO31"/>
+      <c r="DP31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -30762,12 +30996,15 @@
         <v>-2.39234449760766</v>
       </c>
       <c r="DO32" t="n">
-        <v>-3.86363636363637</v>
+        <v>-5.00000000000001</v>
+      </c>
+      <c r="DP32" t="n">
+        <v>-4.28893905191872</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -31121,12 +31358,15 @@
         <v>1.66481687014428</v>
       </c>
       <c r="DO33" t="n">
-        <v>2.24839400428265</v>
+        <v>2.03426124197001</v>
+      </c>
+      <c r="DP33" t="n">
+        <v>2.12765957446809</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -31480,12 +31720,15 @@
         <v>-1.68612191958495</v>
       </c>
       <c r="DO34" t="n">
-        <v>-1.03092783505152</v>
+        <v>-0.515463917525762</v>
+      </c>
+      <c r="DP34" t="n">
+        <v>1.80878552971575</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -31839,12 +32082,15 @@
         <v>0.455580865603635</v>
       </c>
       <c r="DO35" t="n">
-        <v>1.76600441501103</v>
+        <v>0</v>
+      </c>
+      <c r="DP35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -32198,12 +32444,15 @@
         <v>3.19001386962554</v>
       </c>
       <c r="DO36" t="n">
-        <v>2.88998357963874</v>
+        <v>2.72577996715926</v>
+      </c>
+      <c r="DP36" t="n">
+        <v>2.8366481904141</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -32558,11 +32807,14 @@
       </c>
       <c r="DO37" t="n">
         <v>2.67737617135209</v>
+      </c>
+      <c r="DP37" t="n">
+        <v>3.31564986737401</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -32916,12 +33168,15 @@
         <v>3.40909090909092</v>
       </c>
       <c r="DO38" t="n">
-        <v>2.76490808548795</v>
+        <v>2.73501718726647</v>
+      </c>
+      <c r="DP38" t="n">
+        <v>2.55728011825572</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -33276,11 +33531,14 @@
       </c>
       <c r="DO39" t="n">
         <v>1.67493796526056</v>
+      </c>
+      <c r="DP39" t="n">
+        <v>2.1659548505186</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -33635,11 +33893,14 @@
       </c>
       <c r="DO40" t="n">
         <v>1.03359173126615</v>
+      </c>
+      <c r="DP40" t="n">
+        <v>1.53452685421995</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -33993,12 +34254,15 @@
         <v>1.3215859030837</v>
       </c>
       <c r="DO41" t="n">
-        <v>4.50134770889489</v>
+        <v>1.7789757412399</v>
+      </c>
+      <c r="DP41" t="n">
+        <v>2.10274154910834</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -34352,12 +34616,15 @@
         <v>-1.39664804469274</v>
       </c>
       <c r="DO42" t="n">
-        <v>-2.17096336499321</v>
+        <v>-2.10312075983716</v>
+      </c>
+      <c r="DP42" t="n">
+        <v>-1.89445196211097</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -34711,12 +34978,15 @@
         <v>3.42809364548496</v>
       </c>
       <c r="DO43" t="n">
-        <v>5.78577013291632</v>
+        <v>5.16028146989835</v>
+      </c>
+      <c r="DP43" t="n">
+        <v>6.33204633204632</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -35070,12 +35340,15 @@
         <v>0.094339622641513</v>
       </c>
       <c r="DO44" t="n">
-        <v>0.616712920135677</v>
+        <v>0.431699044094984</v>
+      </c>
+      <c r="DP44" t="n">
+        <v>0.670936261055196</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -35430,11 +35703,14 @@
       </c>
       <c r="DO45" t="n">
         <v>0</v>
+      </c>
+      <c r="DP45" t="n">
+        <v>0.000000000000012166827667125</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -35788,12 +36064,15 @@
         <v>2.73291925465839</v>
       </c>
       <c r="DO46" t="n">
-        <v>3.34957369062119</v>
+        <v>3.28867235079172</v>
+      </c>
+      <c r="DP46" t="n">
+        <v>3.56495468277946</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -36148,11 +36427,14 @@
       </c>
       <c r="DO47" t="n">
         <v>2.13903743315509</v>
+      </c>
+      <c r="DP47" t="n">
+        <v>2.39361702127659</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -36507,11 +36789,14 @@
       </c>
       <c r="DO48" t="n">
         <v>1.90151145782545</v>
+      </c>
+      <c r="DP48" t="n">
+        <v>2.39374694675135</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -36865,12 +37150,15 @@
         <v>0.603494865789952</v>
       </c>
       <c r="DO49" t="n">
-        <v>1.40671707402849</v>
+        <v>1.30121329347635</v>
+      </c>
+      <c r="DP49" t="n">
+        <v>1.23725712294154</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -37225,11 +37513,14 @@
       </c>
       <c r="DO50" t="n">
         <v>1.05092966855295</v>
+      </c>
+      <c r="DP50" t="n">
+        <v>1.12179487179486</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -37583,12 +37874,15 @@
         <v>5.11945392491469</v>
       </c>
       <c r="DO51" t="n">
-        <v>5.2117263843648</v>
+        <v>4.88599348534202</v>
+      </c>
+      <c r="DP51" t="n">
+        <v>4.20711974110034</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -37942,12 +38236,15 @@
         <v>3.81704508061863</v>
       </c>
       <c r="DO52" t="n">
-        <v>2.37027546444588</v>
+        <v>3.1390134529148</v>
+      </c>
+      <c r="DP52" t="n">
+        <v>3.36401142494445</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -38301,12 +38598,15 @@
         <v>4.02742073693232</v>
       </c>
       <c r="DO53" t="n">
-        <v>6.22964169381107</v>
+        <v>4.64169381107492</v>
+      </c>
+      <c r="DP53" t="n">
+        <v>4.96568429551878</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -38661,11 +38961,14 @@
       </c>
       <c r="DO54" t="n">
         <v>-2.33333333333334</v>
+      </c>
+      <c r="DP54" t="n">
+        <v>-2.45901639344262</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -39019,12 +39322,15 @@
         <v>2.52652854977263</v>
       </c>
       <c r="DO55" t="n">
-        <v>2.66086115142719</v>
+        <v>2.70924044508951</v>
+      </c>
+      <c r="DP55" t="n">
+        <v>2.73775216138329</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -39379,6 +39685,9 @@
       </c>
       <c r="DO56" t="n">
         <v>1.6835016835017</v>
+      </c>
+      <c r="DP56" t="n">
+        <v>1.67224080267559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on April 21st.
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t xml:space="preserve">02/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1311,10 +1314,13 @@
       <c r="EE4" t="s">
         <v>134</v>
       </c>
+      <c r="EF4" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1713,15 +1719,18 @@
         <v>10626.2</v>
       </c>
       <c r="ED5" t="n">
-        <v>10408.5</v>
+        <v>10405.4</v>
       </c>
       <c r="EE5" t="n">
-        <v>10757.6</v>
+        <v>10780.1</v>
+      </c>
+      <c r="EF5" t="n">
+        <v>10823.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2124,11 +2133,14 @@
       </c>
       <c r="EE6" t="n">
         <v>171.1</v>
+      </c>
+      <c r="EF6" t="n">
+        <v>172.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2530,12 +2542,15 @@
         <v>26.9</v>
       </c>
       <c r="EE7" t="n">
-        <v>29.3</v>
+        <v>29.2</v>
+      </c>
+      <c r="EF7" t="n">
+        <v>29.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2937,12 +2952,15 @@
         <v>191.8</v>
       </c>
       <c r="EE8" t="n">
-        <v>197.8</v>
+        <v>198</v>
+      </c>
+      <c r="EF8" t="n">
+        <v>197</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3345,11 +3363,14 @@
       </c>
       <c r="EE9" t="n">
         <v>101.8</v>
+      </c>
+      <c r="EF9" t="n">
+        <v>102.1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3751,12 +3772,15 @@
         <v>1211.5</v>
       </c>
       <c r="EE10" t="n">
-        <v>1225.4</v>
+        <v>1226.7</v>
+      </c>
+      <c r="EF10" t="n">
+        <v>1246.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4158,12 +4182,15 @@
         <v>212.5</v>
       </c>
       <c r="EE11" t="n">
-        <v>223.4</v>
+        <v>223.3</v>
+      </c>
+      <c r="EF11" t="n">
+        <v>225.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4565,12 +4592,15 @@
         <v>123.6</v>
       </c>
       <c r="EE12" t="n">
-        <v>125.2</v>
+        <v>125.6</v>
+      </c>
+      <c r="EF12" t="n">
+        <v>126.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4972,12 +5002,15 @@
         <v>36</v>
       </c>
       <c r="EE13" t="n">
-        <v>37.6</v>
+        <v>38</v>
+      </c>
+      <c r="EF13" t="n">
+        <v>38.8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5113,10 +5146,11 @@
       <c r="EC14"/>
       <c r="ED14"/>
       <c r="EE14"/>
+      <c r="EF14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5518,12 +5552,15 @@
         <v>477.4</v>
       </c>
       <c r="EE15" t="n">
-        <v>488.4</v>
+        <v>489.9</v>
+      </c>
+      <c r="EF15" t="n">
+        <v>489.1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5925,12 +5962,15 @@
         <v>342</v>
       </c>
       <c r="EE16" t="n">
-        <v>346.1</v>
+        <v>346.3</v>
+      </c>
+      <c r="EF16" t="n">
+        <v>347.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6066,10 +6106,11 @@
       <c r="EC17"/>
       <c r="ED17"/>
       <c r="EE17"/>
+      <c r="EF17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6472,11 +6513,14 @@
       </c>
       <c r="EE18" t="n">
         <v>66</v>
+      </c>
+      <c r="EF18" t="n">
+        <v>66.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6878,12 +6922,15 @@
         <v>422</v>
       </c>
       <c r="EE19" t="n">
-        <v>446.5</v>
+        <v>444.3</v>
+      </c>
+      <c r="EF19" t="n">
+        <v>445.7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7285,12 +7332,15 @@
         <v>220.9</v>
       </c>
       <c r="EE20" t="n">
-        <v>224.1</v>
+        <v>229.2</v>
+      </c>
+      <c r="EF20" t="n">
+        <v>229.7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7693,11 +7743,14 @@
       </c>
       <c r="EE21" t="n">
         <v>145.7</v>
+      </c>
+      <c r="EF21" t="n">
+        <v>145.8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8099,12 +8152,15 @@
         <v>132.8</v>
       </c>
       <c r="EE22" t="n">
-        <v>136</v>
+        <v>135.7</v>
+      </c>
+      <c r="EF22" t="n">
+        <v>135.9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8506,12 +8562,15 @@
         <v>152.5</v>
       </c>
       <c r="EE23" t="n">
-        <v>163.6</v>
+        <v>160.6</v>
+      </c>
+      <c r="EF23" t="n">
+        <v>161.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -8914,11 +8973,14 @@
       </c>
       <c r="EE24" t="n">
         <v>150.2</v>
+      </c>
+      <c r="EF24" t="n">
+        <v>149.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9320,12 +9382,15 @@
         <v>49</v>
       </c>
       <c r="EE25" t="n">
-        <v>50.5</v>
+        <v>50.3</v>
+      </c>
+      <c r="EF25" t="n">
+        <v>50.1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9727,12 +9792,15 @@
         <v>203.4</v>
       </c>
       <c r="EE26" t="n">
-        <v>217</v>
+        <v>217.1</v>
+      </c>
+      <c r="EF26" t="n">
+        <v>220.5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10134,12 +10202,15 @@
         <v>234.8</v>
       </c>
       <c r="EE27" t="n">
-        <v>245.6</v>
+        <v>245.2</v>
+      </c>
+      <c r="EF27" t="n">
+        <v>245.9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10541,12 +10612,15 @@
         <v>304.9</v>
       </c>
       <c r="EE28" t="n">
-        <v>323.9</v>
+        <v>323.7</v>
+      </c>
+      <c r="EF28" t="n">
+        <v>323.4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -10948,12 +11022,15 @@
         <v>201.4</v>
       </c>
       <c r="EE29" t="n">
-        <v>207.4</v>
+        <v>207.5</v>
+      </c>
+      <c r="EF29" t="n">
+        <v>205.6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11356,11 +11433,14 @@
       </c>
       <c r="EE30" t="n">
         <v>103.3</v>
+      </c>
+      <c r="EF30" t="n">
+        <v>103.8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11496,10 +11576,11 @@
       <c r="EC31"/>
       <c r="ED31"/>
       <c r="EE31"/>
+      <c r="EF31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -11901,12 +11982,15 @@
         <v>43.2</v>
       </c>
       <c r="EE32" t="n">
-        <v>44</v>
+        <v>43.7</v>
+      </c>
+      <c r="EF32" t="n">
+        <v>44.2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12309,11 +12393,14 @@
       </c>
       <c r="EE33" t="n">
         <v>94.4</v>
+      </c>
+      <c r="EF33" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -12716,11 +12803,14 @@
       </c>
       <c r="EE34" t="n">
         <v>82.8</v>
+      </c>
+      <c r="EF34" t="n">
+        <v>82.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13122,12 +13212,15 @@
         <v>43.6</v>
       </c>
       <c r="EE35" t="n">
-        <v>46.9</v>
+        <v>46.3</v>
+      </c>
+      <c r="EF35" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -13529,12 +13622,15 @@
         <v>305.2</v>
       </c>
       <c r="EE36" t="n">
-        <v>312.2</v>
+        <v>312.6</v>
+      </c>
+      <c r="EF36" t="n">
+        <v>312.1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -13936,12 +14032,15 @@
         <v>73.6</v>
       </c>
       <c r="EE37" t="n">
-        <v>77.7</v>
+        <v>77.6</v>
+      </c>
+      <c r="EF37" t="n">
+        <v>78.2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14343,12 +14442,15 @@
         <v>657.2</v>
       </c>
       <c r="EE38" t="n">
-        <v>677.6</v>
+        <v>678</v>
+      </c>
+      <c r="EF38" t="n">
+        <v>675.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -14751,11 +14853,14 @@
       </c>
       <c r="EE39" t="n">
         <v>324.4</v>
+      </c>
+      <c r="EF39" t="n">
+        <v>333.2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15157,12 +15262,15 @@
         <v>37.4</v>
       </c>
       <c r="EE40" t="n">
-        <v>38.4</v>
+        <v>38.3</v>
+      </c>
+      <c r="EF40" t="n">
+        <v>38.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -15564,12 +15672,15 @@
         <v>378.2</v>
       </c>
       <c r="EE41" t="n">
-        <v>394.9</v>
+        <v>394.7</v>
+      </c>
+      <c r="EF41" t="n">
+        <v>397.6</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -15971,12 +16082,15 @@
         <v>137.6</v>
       </c>
       <c r="EE42" t="n">
-        <v>144.4</v>
+        <v>145.9</v>
+      </c>
+      <c r="EF42" t="n">
+        <v>146.6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -16378,12 +16492,15 @@
         <v>136.5</v>
       </c>
       <c r="EE43" t="n">
-        <v>140.4</v>
+        <v>140.3</v>
+      </c>
+      <c r="EF43" t="n">
+        <v>141.3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -16786,11 +16903,14 @@
       </c>
       <c r="EE44" t="n">
         <v>330</v>
+      </c>
+      <c r="EF44" t="n">
+        <v>331.6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17193,11 +17313,14 @@
       </c>
       <c r="EE45" t="n">
         <v>29.1</v>
+      </c>
+      <c r="EF45" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -17599,12 +17722,15 @@
         <v>159.4</v>
       </c>
       <c r="EE46" t="n">
-        <v>164.5</v>
+        <v>165.3</v>
+      </c>
+      <c r="EF46" t="n">
+        <v>166.7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18007,11 +18133,14 @@
       </c>
       <c r="EE47" t="n">
         <v>38.1</v>
+      </c>
+      <c r="EF47" t="n">
+        <v>38.3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -18413,12 +18542,15 @@
         <v>198.5</v>
       </c>
       <c r="EE48" t="n">
-        <v>205.7</v>
+        <v>207.7</v>
+      </c>
+      <c r="EF48" t="n">
+        <v>208.4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -18820,12 +18952,15 @@
         <v>1148.7</v>
       </c>
       <c r="EE49" t="n">
-        <v>1178.5</v>
+        <v>1178.2</v>
+      </c>
+      <c r="EF49" t="n">
+        <v>1182.3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -19228,11 +19363,14 @@
       </c>
       <c r="EE50" t="n">
         <v>127.3</v>
+      </c>
+      <c r="EF50" t="n">
+        <v>128.1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -19635,11 +19773,14 @@
       </c>
       <c r="EE51" t="n">
         <v>32.4</v>
+      </c>
+      <c r="EF51" t="n">
+        <v>32.1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20042,11 +20183,14 @@
       </c>
       <c r="EE52" t="n">
         <v>322.8</v>
+      </c>
+      <c r="EF52" t="n">
+        <v>323.5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -20448,12 +20592,15 @@
         <v>248.4</v>
       </c>
       <c r="EE53" t="n">
-        <v>252.1</v>
+        <v>251.5</v>
+      </c>
+      <c r="EF53" t="n">
+        <v>251.9</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -20856,11 +21003,14 @@
       </c>
       <c r="EE54" t="n">
         <v>62.3</v>
+      </c>
+      <c r="EF54" t="n">
+        <v>62.7</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -21262,12 +21412,15 @@
         <v>197.6</v>
       </c>
       <c r="EE55" t="n">
-        <v>214.6</v>
+        <v>214.5</v>
+      </c>
+      <c r="EF55" t="n">
+        <v>213.9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -21669,7 +21822,10 @@
         <v>28.7</v>
       </c>
       <c r="EE56" t="n">
-        <v>30.2</v>
+        <v>30.1</v>
+      </c>
+      <c r="EF56" t="n">
+        <v>30.7</v>
       </c>
     </row>
   </sheetData>
@@ -22056,10 +22212,13 @@
       <c r="DS4" t="s">
         <v>134</v>
       </c>
+      <c r="DT4" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -22422,15 +22581,18 @@
         <v>0.880049366307502</v>
       </c>
       <c r="DR5" t="n">
-        <v>1.92819930275373</v>
+        <v>1.89784167025735</v>
       </c>
       <c r="DS5" t="n">
-        <v>2.17211674533901</v>
+        <v>2.38581428259363</v>
+      </c>
+      <c r="DT5" t="n">
+        <v>2.42254480761589</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -22797,11 +22959,14 @@
       </c>
       <c r="DS6" t="n">
         <v>2.27136879856546</v>
+      </c>
+      <c r="DT6" t="n">
+        <v>2.43902439024388</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -23167,12 +23332,15 @@
         <v>-1.82481751824818</v>
       </c>
       <c r="DS7" t="n">
-        <v>3.90070921985816</v>
+        <v>3.54609929078014</v>
+      </c>
+      <c r="DT7" t="n">
+        <v>2.45614035087719</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -23538,12 +23706,15 @@
         <v>0.10438413361167</v>
       </c>
       <c r="DS8" t="n">
-        <v>0.55922724961872</v>
+        <v>0.660904931367571</v>
+      </c>
+      <c r="DT8" t="n">
+        <v>0.767263427109974</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -23910,11 +24081,14 @@
       </c>
       <c r="DS9" t="n">
         <v>0.792079207920789</v>
+      </c>
+      <c r="DT9" t="n">
+        <v>0.789733464955575</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -24280,12 +24454,15 @@
         <v>2.8962119925259</v>
       </c>
       <c r="DS10" t="n">
-        <v>3.39183260209248</v>
+        <v>3.50151873101586</v>
+      </c>
+      <c r="DT10" t="n">
+        <v>3.23755899643951</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -24651,12 +24828,15 @@
         <v>2.21260221260222</v>
       </c>
       <c r="DS11" t="n">
-        <v>3.09183202584217</v>
+        <v>3.04568527918783</v>
+      </c>
+      <c r="DT11" t="n">
+        <v>3.10786106032907</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -25022,12 +25202,15 @@
         <v>1.64473684210527</v>
       </c>
       <c r="DS12" t="n">
-        <v>1.21261115602264</v>
+        <v>1.53597413096201</v>
+      </c>
+      <c r="DT12" t="n">
+        <v>1.44694533762058</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -25393,12 +25576,15 @@
         <v>2.85714285714286</v>
       </c>
       <c r="DS13" t="n">
-        <v>2.45231607629427</v>
+        <v>3.54223433242506</v>
+      </c>
+      <c r="DT13" t="n">
+        <v>3.74331550802137</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -25522,10 +25708,11 @@
       <c r="DQ14"/>
       <c r="DR14"/>
       <c r="DS14"/>
+      <c r="DT14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -25891,12 +26078,15 @@
         <v>0.844951415293621</v>
       </c>
       <c r="DS15" t="n">
-        <v>1.68644597126797</v>
+        <v>1.99875078076204</v>
+      </c>
+      <c r="DT15" t="n">
+        <v>1.85339441899209</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -26262,12 +26452,15 @@
         <v>2.36456150853037</v>
       </c>
       <c r="DS16" t="n">
-        <v>2.7918027918028</v>
+        <v>2.85120285120286</v>
+      </c>
+      <c r="DT16" t="n">
+        <v>3.14726840855106</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -26391,10 +26584,11 @@
       <c r="DQ17"/>
       <c r="DR17"/>
       <c r="DS17"/>
+      <c r="DT17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -26761,11 +26955,14 @@
       </c>
       <c r="DS18" t="n">
         <v>6.28019323671497</v>
+      </c>
+      <c r="DT18" t="n">
+        <v>7.08534621578101</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -27131,12 +27328,15 @@
         <v>0.309008794865703</v>
       </c>
       <c r="DS19" t="n">
-        <v>4.46888160973326</v>
+        <v>3.95414131960692</v>
+      </c>
+      <c r="DT19" t="n">
+        <v>3.67527331937662</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -27502,12 +27702,15 @@
         <v>0.135992747053483</v>
       </c>
       <c r="DS20" t="n">
-        <v>1.58658204895739</v>
+        <v>3.89845874886672</v>
+      </c>
+      <c r="DT20" t="n">
+        <v>2.22518914107699</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -27874,11 +28077,14 @@
       </c>
       <c r="DS21" t="n">
         <v>2.38931834153196</v>
+      </c>
+      <c r="DT21" t="n">
+        <v>2.31578947368422</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -28244,12 +28450,15 @@
         <v>1.06544901065449</v>
       </c>
       <c r="DS22" t="n">
-        <v>0.443131462333822</v>
+        <v>0.2215657311669</v>
+      </c>
+      <c r="DT22" t="n">
+        <v>0.221238938053106</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -28615,12 +28824,15 @@
         <v>-1.73969072164948</v>
       </c>
       <c r="DS23" t="n">
-        <v>3.54430379746835</v>
+        <v>1.64556962025318</v>
+      </c>
+      <c r="DT23" t="n">
+        <v>1.63214061519144</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -28987,11 +29199,14 @@
       </c>
       <c r="DS24" t="n">
         <v>2.94722412611378</v>
+      </c>
+      <c r="DT24" t="n">
+        <v>3.39335180055402</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -29357,12 +29572,15 @@
         <v>1.87110187110188</v>
       </c>
       <c r="DS25" t="n">
-        <v>0.798403193612786</v>
+        <v>0.399201596806393</v>
+      </c>
+      <c r="DT25" t="n">
+        <v>0.400801603206419</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -29728,12 +29946,15 @@
         <v>2.83114256825076</v>
       </c>
       <c r="DS26" t="n">
-        <v>3.43183984747378</v>
+        <v>3.4795042897998</v>
+      </c>
+      <c r="DT26" t="n">
+        <v>3.8135593220339</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -30099,12 +30320,15 @@
         <v>3.57300397000442</v>
       </c>
       <c r="DS27" t="n">
-        <v>3.71621621621622</v>
+        <v>3.54729729729729</v>
+      </c>
+      <c r="DT27" t="n">
+        <v>3.44972654606645</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -30470,12 +30694,15 @@
         <v>5.35590877677954</v>
       </c>
       <c r="DS28" t="n">
-        <v>6.93298118190822</v>
+        <v>6.86695278969959</v>
+      </c>
+      <c r="DT28" t="n">
+        <v>6.20689655172413</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -30841,12 +31068,15 @@
         <v>0.649675162418796</v>
       </c>
       <c r="DS29" t="n">
-        <v>1.26953125</v>
+        <v>1.31835937499999</v>
+      </c>
+      <c r="DT29" t="n">
+        <v>0.636319138521787</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -31213,11 +31443,14 @@
       </c>
       <c r="DS30" t="n">
         <v>0.682261208577015</v>
+      </c>
+      <c r="DT30" t="n">
+        <v>1.07108081791627</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -31341,10 +31574,11 @@
       <c r="DQ31"/>
       <c r="DR31"/>
       <c r="DS31"/>
+      <c r="DT31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -31710,12 +31944,15 @@
         <v>1.17096018735363</v>
       </c>
       <c r="DS32" t="n">
-        <v>0.917431192660547</v>
+        <v>0.229357798165141</v>
+      </c>
+      <c r="DT32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -32082,11 +32319,14 @@
       </c>
       <c r="DS33" t="n">
         <v>1.72413793103448</v>
+      </c>
+      <c r="DT33" t="n">
+        <v>2.04081632653062</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -32453,11 +32693,14 @@
       </c>
       <c r="DS34" t="n">
         <v>4.94296577946767</v>
+      </c>
+      <c r="DT34" t="n">
+        <v>4.2983565107459</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -32823,12 +33066,15 @@
         <v>0.69284064665128</v>
       </c>
       <c r="DS35" t="n">
-        <v>0.860215053763438</v>
+        <v>-0.430107526881727</v>
+      </c>
+      <c r="DT35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -33194,12 +33440,15 @@
         <v>3.24763193504735</v>
       </c>
       <c r="DS36" t="n">
-        <v>1.66069684141974</v>
+        <v>1.7909475740801</v>
+      </c>
+      <c r="DT36" t="n">
+        <v>1.06865284974094</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -33565,12 +33814,15 @@
         <v>2.93706293706293</v>
       </c>
       <c r="DS37" t="n">
-        <v>3.05039787798408</v>
+        <v>2.91777188328911</v>
+      </c>
+      <c r="DT37" t="n">
+        <v>2.49017038007864</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -33936,12 +34188,15 @@
         <v>3.18731355000786</v>
       </c>
       <c r="DS38" t="n">
-        <v>4.08602150537633</v>
+        <v>4.14746543778802</v>
+      </c>
+      <c r="DT38" t="n">
+        <v>3.33537331701346</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -34308,11 +34563,14 @@
       </c>
       <c r="DS39" t="n">
         <v>0.996264009962637</v>
+      </c>
+      <c r="DT39" t="n">
+        <v>0.725513905683185</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -34678,12 +34936,15 @@
         <v>0.808625336927216</v>
       </c>
       <c r="DS40" t="n">
-        <v>1.05263157894736</v>
+        <v>0.789473684210519</v>
+      </c>
+      <c r="DT40" t="n">
+        <v>0.263157894736846</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -35049,12 +35310,15 @@
         <v>0.934080597811583</v>
       </c>
       <c r="DS41" t="n">
-        <v>1.51670951156812</v>
+        <v>1.46529562982006</v>
+      </c>
+      <c r="DT41" t="n">
+        <v>2.84531815830314</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -35420,12 +35684,15 @@
         <v>-2.4113475177305</v>
       </c>
       <c r="DS42" t="n">
-        <v>-2.69541778975741</v>
+        <v>-1.68463611859838</v>
+      </c>
+      <c r="DT42" t="n">
+        <v>-1.47849462365593</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -35791,12 +36058,15 @@
         <v>4.67791411042944</v>
       </c>
       <c r="DS43" t="n">
-        <v>5.01121914734482</v>
+        <v>4.93642483171281</v>
+      </c>
+      <c r="DT43" t="n">
+        <v>4.97771173848441</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -36163,11 +36433,14 @@
       </c>
       <c r="DS44" t="n">
         <v>1.9147621988882</v>
+      </c>
+      <c r="DT44" t="n">
+        <v>1.780233271946</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -36534,11 +36807,14 @@
       </c>
       <c r="DS45" t="n">
         <v>0.344827586206889</v>
+      </c>
+      <c r="DT45" t="n">
+        <v>2.73972602739726</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -36904,12 +37180,15 @@
         <v>3.50649350649351</v>
       </c>
       <c r="DS46" t="n">
-        <v>2.42839352428394</v>
+        <v>2.92652552926527</v>
+      </c>
+      <c r="DT46" t="n">
+        <v>3.0284301606922</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -37276,11 +37555,14 @@
       </c>
       <c r="DS47" t="n">
         <v>1.59999999999998</v>
+      </c>
+      <c r="DT47" t="n">
+        <v>1.32275132275132</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -37646,12 +37928,15 @@
         <v>0.966429298067144</v>
       </c>
       <c r="DS48" t="n">
-        <v>-0.0485908649173928</v>
+        <v>0.923226433430518</v>
+      </c>
+      <c r="DT48" t="n">
+        <v>0.920096852300231</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -38017,12 +38302,15 @@
         <v>2.39793189516849</v>
       </c>
       <c r="DS49" t="n">
-        <v>3.06077831219939</v>
+        <v>3.0345430695234</v>
+      </c>
+      <c r="DT49" t="n">
+        <v>3.21257092972501</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -38389,11 +38677,14 @@
       </c>
       <c r="DS50" t="n">
         <v>2.57856567284448</v>
+      </c>
+      <c r="DT50" t="n">
+        <v>2.89156626506024</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -38760,11 +39051,14 @@
       </c>
       <c r="DS51" t="n">
         <v>2.53164556962027</v>
+      </c>
+      <c r="DT51" t="n">
+        <v>2.22929936305733</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -39131,11 +39425,14 @@
       </c>
       <c r="DS52" t="n">
         <v>3.76084860173577</v>
+      </c>
+      <c r="DT52" t="n">
+        <v>3.38766379034836</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -39501,12 +39798,15 @@
         <v>3.28482328482329</v>
       </c>
       <c r="DS53" t="n">
-        <v>3.06623058053966</v>
+        <v>2.82093213409649</v>
+      </c>
+      <c r="DT53" t="n">
+        <v>2.35676554246239</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -39872,12 +40172,15 @@
         <v>0.511073253833045</v>
       </c>
       <c r="DS54" t="n">
-        <v>1.63132137030994</v>
+        <v>1.63132137030995</v>
+      </c>
+      <c r="DT54" t="n">
+        <v>1.29240710823909</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -40243,12 +40546,15 @@
         <v>2.59605399792314</v>
       </c>
       <c r="DS55" t="n">
-        <v>4.1747572815534</v>
+        <v>4.12621359223301</v>
+      </c>
+      <c r="DT55" t="n">
+        <v>3.18379160636758</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -40614,7 +40920,10 @@
         <v>0.349650349650355</v>
       </c>
       <c r="DS56" t="n">
-        <v>1.34228187919464</v>
+        <v>1.00671140939598</v>
+      </c>
+      <c r="DT56" t="n">
+        <v>1.99335548172757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on May 19th, 2023
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t xml:space="preserve">02/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1311,10 +1317,16 @@
       <c r="EE4" t="s">
         <v>134</v>
       </c>
+      <c r="EF4" t="s">
+        <v>135</v>
+      </c>
+      <c r="EG4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1713,15 +1725,21 @@
         <v>10626.2</v>
       </c>
       <c r="ED5" t="n">
-        <v>10408.5</v>
+        <v>10405.4</v>
       </c>
       <c r="EE5" t="n">
-        <v>10757.6</v>
+        <v>10787.5</v>
+      </c>
+      <c r="EF5" t="n">
+        <v>10819</v>
+      </c>
+      <c r="EG5" t="n">
+        <v>10820.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2124,11 +2142,17 @@
       </c>
       <c r="EE6" t="n">
         <v>171.1</v>
+      </c>
+      <c r="EF6" t="n">
+        <v>171.8</v>
+      </c>
+      <c r="EG6" t="n">
+        <v>171.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2530,12 +2554,18 @@
         <v>26.9</v>
       </c>
       <c r="EE7" t="n">
+        <v>29.2</v>
+      </c>
+      <c r="EF7" t="n">
         <v>29.3</v>
+      </c>
+      <c r="EG7" t="n">
+        <v>29.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2937,12 +2967,18 @@
         <v>191.8</v>
       </c>
       <c r="EE8" t="n">
-        <v>197.8</v>
+        <v>198</v>
+      </c>
+      <c r="EF8" t="n">
+        <v>197</v>
+      </c>
+      <c r="EG8" t="n">
+        <v>199.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3345,11 +3381,17 @@
       </c>
       <c r="EE9" t="n">
         <v>101.8</v>
+      </c>
+      <c r="EF9" t="n">
+        <v>102.1</v>
+      </c>
+      <c r="EG9" t="n">
+        <v>102.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3751,12 +3793,18 @@
         <v>1211.5</v>
       </c>
       <c r="EE10" t="n">
-        <v>1225.4</v>
+        <v>1226.7</v>
+      </c>
+      <c r="EF10" t="n">
+        <v>1244.2</v>
+      </c>
+      <c r="EG10" t="n">
+        <v>1248.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4158,12 +4206,18 @@
         <v>212.5</v>
       </c>
       <c r="EE11" t="n">
-        <v>223.4</v>
+        <v>223.3</v>
+      </c>
+      <c r="EF11" t="n">
+        <v>225.6</v>
+      </c>
+      <c r="EG11" t="n">
+        <v>224.8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4565,12 +4619,18 @@
         <v>123.6</v>
       </c>
       <c r="EE12" t="n">
-        <v>125.2</v>
+        <v>125.6</v>
+      </c>
+      <c r="EF12" t="n">
+        <v>126.3</v>
+      </c>
+      <c r="EG12" t="n">
+        <v>124.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -4972,12 +5032,18 @@
         <v>36</v>
       </c>
       <c r="EE13" t="n">
-        <v>37.6</v>
+        <v>38</v>
+      </c>
+      <c r="EF13" t="n">
+        <v>38.3</v>
+      </c>
+      <c r="EG13" t="n">
+        <v>38.8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5113,10 +5179,12 @@
       <c r="EC14"/>
       <c r="ED14"/>
       <c r="EE14"/>
+      <c r="EF14"/>
+      <c r="EG14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5518,12 +5586,18 @@
         <v>477.4</v>
       </c>
       <c r="EE15" t="n">
-        <v>488.4</v>
+        <v>489.9</v>
+      </c>
+      <c r="EF15" t="n">
+        <v>489.1</v>
+      </c>
+      <c r="EG15" t="n">
+        <v>488.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -5925,12 +5999,18 @@
         <v>342</v>
       </c>
       <c r="EE16" t="n">
-        <v>346.1</v>
+        <v>346.3</v>
+      </c>
+      <c r="EF16" t="n">
+        <v>347.2</v>
+      </c>
+      <c r="EG16" t="n">
+        <v>346.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6066,10 +6146,12 @@
       <c r="EC17"/>
       <c r="ED17"/>
       <c r="EE17"/>
+      <c r="EF17"/>
+      <c r="EG17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6472,11 +6554,17 @@
       </c>
       <c r="EE18" t="n">
         <v>66</v>
+      </c>
+      <c r="EF18" t="n">
+        <v>66.4</v>
+      </c>
+      <c r="EG18" t="n">
+        <v>66.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6878,12 +6966,18 @@
         <v>422</v>
       </c>
       <c r="EE19" t="n">
-        <v>446.5</v>
+        <v>444.3</v>
+      </c>
+      <c r="EF19" t="n">
+        <v>446.1</v>
+      </c>
+      <c r="EG19" t="n">
+        <v>445.9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7285,12 +7379,18 @@
         <v>220.9</v>
       </c>
       <c r="EE20" t="n">
-        <v>224.1</v>
+        <v>229.2</v>
+      </c>
+      <c r="EF20" t="n">
+        <v>229.6</v>
+      </c>
+      <c r="EG20" t="n">
+        <v>228.9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7693,11 +7793,17 @@
       </c>
       <c r="EE21" t="n">
         <v>145.7</v>
+      </c>
+      <c r="EF21" t="n">
+        <v>145.7</v>
+      </c>
+      <c r="EG21" t="n">
+        <v>145.8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8099,12 +8205,18 @@
         <v>132.8</v>
       </c>
       <c r="EE22" t="n">
-        <v>136</v>
+        <v>135.7</v>
+      </c>
+      <c r="EF22" t="n">
+        <v>135.9</v>
+      </c>
+      <c r="EG22" t="n">
+        <v>135.4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8506,12 +8618,18 @@
         <v>152.5</v>
       </c>
       <c r="EE23" t="n">
-        <v>163.6</v>
+        <v>160.6</v>
+      </c>
+      <c r="EF23" t="n">
+        <v>161.4</v>
+      </c>
+      <c r="EG23" t="n">
+        <v>161.1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -8914,11 +9032,17 @@
       </c>
       <c r="EE24" t="n">
         <v>150.2</v>
+      </c>
+      <c r="EF24" t="n">
+        <v>149.3</v>
+      </c>
+      <c r="EG24" t="n">
+        <v>150.4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9320,12 +9444,18 @@
         <v>49</v>
       </c>
       <c r="EE25" t="n">
-        <v>50.5</v>
+        <v>50.3</v>
+      </c>
+      <c r="EF25" t="n">
+        <v>50</v>
+      </c>
+      <c r="EG25" t="n">
+        <v>49.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9727,12 +9857,18 @@
         <v>203.4</v>
       </c>
       <c r="EE26" t="n">
-        <v>217</v>
+        <v>217.1</v>
+      </c>
+      <c r="EF26" t="n">
+        <v>220.5</v>
+      </c>
+      <c r="EG26" t="n">
+        <v>225</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10134,12 +10270,18 @@
         <v>234.8</v>
       </c>
       <c r="EE27" t="n">
-        <v>245.6</v>
+        <v>245.2</v>
+      </c>
+      <c r="EF27" t="n">
+        <v>245.9</v>
+      </c>
+      <c r="EG27" t="n">
+        <v>246.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10541,12 +10683,18 @@
         <v>304.9</v>
       </c>
       <c r="EE28" t="n">
+        <v>323.7</v>
+      </c>
+      <c r="EF28" t="n">
+        <v>323.6</v>
+      </c>
+      <c r="EG28" t="n">
         <v>323.9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -10948,12 +11096,18 @@
         <v>201.4</v>
       </c>
       <c r="EE29" t="n">
-        <v>207.4</v>
+        <v>207.5</v>
+      </c>
+      <c r="EF29" t="n">
+        <v>205.6</v>
+      </c>
+      <c r="EG29" t="n">
+        <v>206</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11356,11 +11510,17 @@
       </c>
       <c r="EE30" t="n">
         <v>103.3</v>
+      </c>
+      <c r="EF30" t="n">
+        <v>103.8</v>
+      </c>
+      <c r="EG30" t="n">
+        <v>103.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11496,10 +11656,12 @@
       <c r="EC31"/>
       <c r="ED31"/>
       <c r="EE31"/>
+      <c r="EF31"/>
+      <c r="EG31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -11901,12 +12063,18 @@
         <v>43.2</v>
       </c>
       <c r="EE32" t="n">
-        <v>44</v>
+        <v>43.7</v>
+      </c>
+      <c r="EF32" t="n">
+        <v>43.6</v>
+      </c>
+      <c r="EG32" t="n">
+        <v>43.5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12309,11 +12477,17 @@
       </c>
       <c r="EE33" t="n">
         <v>94.4</v>
+      </c>
+      <c r="EF33" t="n">
+        <v>95</v>
+      </c>
+      <c r="EG33" t="n">
+        <v>94.7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -12716,11 +12890,17 @@
       </c>
       <c r="EE34" t="n">
         <v>82.8</v>
+      </c>
+      <c r="EF34" t="n">
+        <v>83</v>
+      </c>
+      <c r="EG34" t="n">
+        <v>83.6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13122,12 +13302,18 @@
         <v>43.6</v>
       </c>
       <c r="EE35" t="n">
-        <v>46.9</v>
+        <v>46.3</v>
+      </c>
+      <c r="EF35" t="n">
+        <v>46</v>
+      </c>
+      <c r="EG35" t="n">
+        <v>46.3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -13529,12 +13715,18 @@
         <v>305.2</v>
       </c>
       <c r="EE36" t="n">
-        <v>312.2</v>
+        <v>312.6</v>
+      </c>
+      <c r="EF36" t="n">
+        <v>312.1</v>
+      </c>
+      <c r="EG36" t="n">
+        <v>312.7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -13936,12 +14128,18 @@
         <v>73.6</v>
       </c>
       <c r="EE37" t="n">
+        <v>77.6</v>
+      </c>
+      <c r="EF37" t="n">
+        <v>78.1</v>
+      </c>
+      <c r="EG37" t="n">
         <v>77.7</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14343,12 +14541,18 @@
         <v>657.2</v>
       </c>
       <c r="EE38" t="n">
-        <v>677.6</v>
+        <v>678</v>
+      </c>
+      <c r="EF38" t="n">
+        <v>675.5</v>
+      </c>
+      <c r="EG38" t="n">
+        <v>676.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -14751,11 +14955,17 @@
       </c>
       <c r="EE39" t="n">
         <v>324.4</v>
+      </c>
+      <c r="EF39" t="n">
+        <v>333.2</v>
+      </c>
+      <c r="EG39" t="n">
+        <v>332</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15157,12 +15367,18 @@
         <v>37.4</v>
       </c>
       <c r="EE40" t="n">
-        <v>38.4</v>
+        <v>38.3</v>
+      </c>
+      <c r="EF40" t="n">
+        <v>38.1</v>
+      </c>
+      <c r="EG40" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -15564,12 +15780,18 @@
         <v>378.2</v>
       </c>
       <c r="EE41" t="n">
-        <v>394.9</v>
+        <v>394.7</v>
+      </c>
+      <c r="EF41" t="n">
+        <v>397.5</v>
+      </c>
+      <c r="EG41" t="n">
+        <v>394.4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -15971,12 +16193,18 @@
         <v>137.6</v>
       </c>
       <c r="EE42" t="n">
-        <v>144.4</v>
+        <v>145.9</v>
+      </c>
+      <c r="EF42" t="n">
+        <v>147.2</v>
+      </c>
+      <c r="EG42" t="n">
+        <v>147.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -16378,12 +16606,18 @@
         <v>136.5</v>
       </c>
       <c r="EE43" t="n">
-        <v>140.4</v>
+        <v>140.3</v>
+      </c>
+      <c r="EF43" t="n">
+        <v>141.4</v>
+      </c>
+      <c r="EG43" t="n">
+        <v>141.1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -16786,11 +17020,17 @@
       </c>
       <c r="EE44" t="n">
         <v>330</v>
+      </c>
+      <c r="EF44" t="n">
+        <v>331.4</v>
+      </c>
+      <c r="EG44" t="n">
+        <v>331.9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17193,11 +17433,17 @@
       </c>
       <c r="EE45" t="n">
         <v>29.1</v>
+      </c>
+      <c r="EF45" t="n">
+        <v>30</v>
+      </c>
+      <c r="EG45" t="n">
+        <v>29.4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -17599,12 +17845,18 @@
         <v>159.4</v>
       </c>
       <c r="EE46" t="n">
-        <v>164.5</v>
+        <v>165.3</v>
+      </c>
+      <c r="EF46" t="n">
+        <v>166.7</v>
+      </c>
+      <c r="EG46" t="n">
+        <v>166.3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18007,11 +18259,17 @@
       </c>
       <c r="EE47" t="n">
         <v>38.1</v>
+      </c>
+      <c r="EF47" t="n">
+        <v>38.3</v>
+      </c>
+      <c r="EG47" t="n">
+        <v>38.2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -18413,12 +18671,18 @@
         <v>198.5</v>
       </c>
       <c r="EE48" t="n">
-        <v>205.7</v>
+        <v>207.7</v>
+      </c>
+      <c r="EF48" t="n">
+        <v>208.4</v>
+      </c>
+      <c r="EG48" t="n">
+        <v>209.1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -18820,12 +19084,18 @@
         <v>1148.7</v>
       </c>
       <c r="EE49" t="n">
-        <v>1178.5</v>
+        <v>1178.2</v>
+      </c>
+      <c r="EF49" t="n">
+        <v>1182.3</v>
+      </c>
+      <c r="EG49" t="n">
+        <v>1182.2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -19228,11 +19498,17 @@
       </c>
       <c r="EE50" t="n">
         <v>127.3</v>
+      </c>
+      <c r="EF50" t="n">
+        <v>128.1</v>
+      </c>
+      <c r="EG50" t="n">
+        <v>128.4</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -19635,11 +19911,17 @@
       </c>
       <c r="EE51" t="n">
         <v>32.4</v>
+      </c>
+      <c r="EF51" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="EG51" t="n">
+        <v>32.6</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20042,11 +20324,17 @@
       </c>
       <c r="EE52" t="n">
         <v>322.8</v>
+      </c>
+      <c r="EF52" t="n">
+        <v>323.6</v>
+      </c>
+      <c r="EG52" t="n">
+        <v>323.3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -20448,12 +20736,18 @@
         <v>248.4</v>
       </c>
       <c r="EE53" t="n">
-        <v>252.1</v>
+        <v>251.5</v>
+      </c>
+      <c r="EF53" t="n">
+        <v>252.4</v>
+      </c>
+      <c r="EG53" t="n">
+        <v>252.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -20855,12 +21149,18 @@
         <v>59</v>
       </c>
       <c r="EE54" t="n">
+        <v>62.3</v>
+      </c>
+      <c r="EF54" t="n">
+        <v>62.6</v>
+      </c>
+      <c r="EG54" t="n">
         <v>62.3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -21262,12 +21562,18 @@
         <v>197.6</v>
       </c>
       <c r="EE55" t="n">
-        <v>214.6</v>
+        <v>214.5</v>
+      </c>
+      <c r="EF55" t="n">
+        <v>213.7</v>
+      </c>
+      <c r="EG55" t="n">
+        <v>214.2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -21669,7 +21975,13 @@
         <v>28.7</v>
       </c>
       <c r="EE56" t="n">
-        <v>30.2</v>
+        <v>30.1</v>
+      </c>
+      <c r="EF56" t="n">
+        <v>30.8</v>
+      </c>
+      <c r="EG56" t="n">
+        <v>30.5</v>
       </c>
     </row>
   </sheetData>
@@ -22056,10 +22368,16 @@
       <c r="DS4" t="s">
         <v>134</v>
       </c>
+      <c r="DT4" t="s">
+        <v>135</v>
+      </c>
+      <c r="DU4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -22422,15 +22740,21 @@
         <v>0.880049366307502</v>
       </c>
       <c r="DR5" t="n">
-        <v>1.92819930275373</v>
+        <v>1.89784167025735</v>
       </c>
       <c r="DS5" t="n">
-        <v>2.17211674533901</v>
+        <v>2.45609702817959</v>
+      </c>
+      <c r="DT5" t="n">
+        <v>2.38090731873498</v>
+      </c>
+      <c r="DU5" t="n">
+        <v>2.21416156578251</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -22797,11 +23121,17 @@
       </c>
       <c r="DS6" t="n">
         <v>2.27136879856546</v>
+      </c>
+      <c r="DT6" t="n">
+        <v>2.20107079119571</v>
+      </c>
+      <c r="DU6" t="n">
+        <v>0.999999999999993</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -23167,12 +23497,18 @@
         <v>-1.82481751824818</v>
       </c>
       <c r="DS7" t="n">
-        <v>3.90070921985816</v>
+        <v>3.54609929078014</v>
+      </c>
+      <c r="DT7" t="n">
+        <v>2.80701754385965</v>
+      </c>
+      <c r="DU7" t="n">
+        <v>4.67625899280576</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -23538,12 +23874,18 @@
         <v>0.10438413361167</v>
       </c>
       <c r="DS8" t="n">
-        <v>0.55922724961872</v>
+        <v>0.660904931367571</v>
+      </c>
+      <c r="DT8" t="n">
+        <v>0.767263427109974</v>
+      </c>
+      <c r="DU8" t="n">
+        <v>1.78753830439224</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -23910,11 +24252,17 @@
       </c>
       <c r="DS9" t="n">
         <v>0.792079207920789</v>
+      </c>
+      <c r="DT9" t="n">
+        <v>0.789733464955575</v>
+      </c>
+      <c r="DU9" t="n">
+        <v>0.686947988223738</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -24280,12 +24628,18 @@
         <v>2.8962119925259</v>
       </c>
       <c r="DS10" t="n">
-        <v>3.39183260209248</v>
+        <v>3.50151873101586</v>
+      </c>
+      <c r="DT10" t="n">
+        <v>3.02227374347934</v>
+      </c>
+      <c r="DU10" t="n">
+        <v>2.94287362954415</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -24651,12 +25005,18 @@
         <v>2.21260221260222</v>
       </c>
       <c r="DS11" t="n">
-        <v>3.09183202584217</v>
+        <v>3.04568527918783</v>
+      </c>
+      <c r="DT11" t="n">
+        <v>3.10786106032907</v>
+      </c>
+      <c r="DU11" t="n">
+        <v>2.93040293040293</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -25022,12 +25382,18 @@
         <v>1.64473684210527</v>
       </c>
       <c r="DS12" t="n">
-        <v>1.21261115602264</v>
+        <v>1.53597413096201</v>
+      </c>
+      <c r="DT12" t="n">
+        <v>1.5273311897106</v>
+      </c>
+      <c r="DU12" t="n">
+        <v>0.321802091713601</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -25393,12 +25759,18 @@
         <v>2.85714285714286</v>
       </c>
       <c r="DS13" t="n">
-        <v>2.45231607629427</v>
+        <v>3.54223433242506</v>
+      </c>
+      <c r="DT13" t="n">
+        <v>2.40641711229944</v>
+      </c>
+      <c r="DU13" t="n">
+        <v>2.64550264550265</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -25522,10 +25894,12 @@
       <c r="DQ14"/>
       <c r="DR14"/>
       <c r="DS14"/>
+      <c r="DT14"/>
+      <c r="DU14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -25891,12 +26265,18 @@
         <v>0.844951415293621</v>
       </c>
       <c r="DS15" t="n">
-        <v>1.68644597126797</v>
+        <v>1.99875078076204</v>
+      </c>
+      <c r="DT15" t="n">
+        <v>1.85339441899209</v>
+      </c>
+      <c r="DU15" t="n">
+        <v>1.72772689425479</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -26262,12 +26642,18 @@
         <v>2.36456150853037</v>
       </c>
       <c r="DS16" t="n">
-        <v>2.7918027918028</v>
+        <v>2.85120285120286</v>
+      </c>
+      <c r="DT16" t="n">
+        <v>3.08788598574821</v>
+      </c>
+      <c r="DU16" t="n">
+        <v>2.85035629453681</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -26391,10 +26777,12 @@
       <c r="DQ17"/>
       <c r="DR17"/>
       <c r="DS17"/>
+      <c r="DT17"/>
+      <c r="DU17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -26761,11 +27149,17 @@
       </c>
       <c r="DS18" t="n">
         <v>6.28019323671497</v>
+      </c>
+      <c r="DT18" t="n">
+        <v>6.92431561996781</v>
+      </c>
+      <c r="DU18" t="n">
+        <v>7.60517799352751</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -27131,12 +27525,18 @@
         <v>0.309008794865703</v>
       </c>
       <c r="DS19" t="n">
-        <v>4.46888160973326</v>
+        <v>3.95414131960692</v>
+      </c>
+      <c r="DT19" t="n">
+        <v>3.76831821353804</v>
+      </c>
+      <c r="DU19" t="n">
+        <v>3.8667598416026</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -27502,12 +27902,18 @@
         <v>0.135992747053483</v>
       </c>
       <c r="DS20" t="n">
-        <v>1.58658204895739</v>
+        <v>3.89845874886672</v>
+      </c>
+      <c r="DT20" t="n">
+        <v>2.18068535825547</v>
+      </c>
+      <c r="DU20" t="n">
+        <v>2.14190093708165</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -27874,11 +28280,17 @@
       </c>
       <c r="DS21" t="n">
         <v>2.38931834153196</v>
+      </c>
+      <c r="DT21" t="n">
+        <v>2.24561403508771</v>
+      </c>
+      <c r="DU21" t="n">
+        <v>1.95804195804197</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -28244,12 +28656,18 @@
         <v>1.06544901065449</v>
       </c>
       <c r="DS22" t="n">
-        <v>0.443131462333822</v>
+        <v>0.2215657311669</v>
+      </c>
+      <c r="DT22" t="n">
+        <v>0.221238938053106</v>
+      </c>
+      <c r="DU22" t="n">
+        <v>-0.294550810014732</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -28615,12 +29033,18 @@
         <v>-1.73969072164948</v>
       </c>
       <c r="DS23" t="n">
-        <v>3.54430379746835</v>
+        <v>1.64556962025318</v>
+      </c>
+      <c r="DT23" t="n">
+        <v>1.31826741996233</v>
+      </c>
+      <c r="DU23" t="n">
+        <v>1.76879343019582</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -28987,11 +29411,17 @@
       </c>
       <c r="DS24" t="n">
         <v>2.94722412611378</v>
+      </c>
+      <c r="DT24" t="n">
+        <v>3.39335180055402</v>
+      </c>
+      <c r="DU24" t="n">
+        <v>3.36769759450172</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -29357,12 +29787,18 @@
         <v>1.87110187110188</v>
       </c>
       <c r="DS25" t="n">
-        <v>0.798403193612786</v>
+        <v>0.399201596806393</v>
+      </c>
+      <c r="DT25" t="n">
+        <v>0.200400801603209</v>
+      </c>
+      <c r="DU25" t="n">
+        <v>-1.19760479041916</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -29728,12 +30164,18 @@
         <v>2.83114256825076</v>
       </c>
       <c r="DS26" t="n">
-        <v>3.43183984747378</v>
+        <v>3.4795042897998</v>
+      </c>
+      <c r="DT26" t="n">
+        <v>3.8135593220339</v>
+      </c>
+      <c r="DU26" t="n">
+        <v>3.3532384014699</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -30099,12 +30541,18 @@
         <v>3.57300397000442</v>
       </c>
       <c r="DS27" t="n">
-        <v>3.71621621621622</v>
+        <v>3.54729729729729</v>
+      </c>
+      <c r="DT27" t="n">
+        <v>3.44972654606645</v>
+      </c>
+      <c r="DU27" t="n">
+        <v>3.31098072087174</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -30470,12 +30918,18 @@
         <v>5.35590877677954</v>
       </c>
       <c r="DS28" t="n">
-        <v>6.93298118190822</v>
+        <v>6.86695278969959</v>
+      </c>
+      <c r="DT28" t="n">
+        <v>6.27257799671594</v>
+      </c>
+      <c r="DU28" t="n">
+        <v>5.84967320261437</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -30841,12 +31295,18 @@
         <v>0.649675162418796</v>
       </c>
       <c r="DS29" t="n">
-        <v>1.26953125</v>
+        <v>1.31835937499999</v>
+      </c>
+      <c r="DT29" t="n">
+        <v>0.636319138521787</v>
+      </c>
+      <c r="DU29" t="n">
+        <v>0.340964442279585</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -31213,11 +31673,17 @@
       </c>
       <c r="DS30" t="n">
         <v>0.682261208577015</v>
+      </c>
+      <c r="DT30" t="n">
+        <v>1.07108081791627</v>
+      </c>
+      <c r="DU30" t="n">
+        <v>1.07421874999999</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -31341,10 +31807,12 @@
       <c r="DQ31"/>
       <c r="DR31"/>
       <c r="DS31"/>
+      <c r="DT31"/>
+      <c r="DU31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -31710,12 +32178,18 @@
         <v>1.17096018735363</v>
       </c>
       <c r="DS32" t="n">
-        <v>0.917431192660547</v>
+        <v>0.229357798165141</v>
+      </c>
+      <c r="DT32" t="n">
+        <v>-1.35746606334842</v>
+      </c>
+      <c r="DU32" t="n">
+        <v>-1.58371040723983</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -32082,11 +32556,17 @@
       </c>
       <c r="DS33" t="n">
         <v>1.72413793103448</v>
+      </c>
+      <c r="DT33" t="n">
+        <v>2.04081632653062</v>
+      </c>
+      <c r="DU33" t="n">
+        <v>1.28342245989305</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -32453,11 +32933,17 @@
       </c>
       <c r="DS34" t="n">
         <v>4.94296577946767</v>
+      </c>
+      <c r="DT34" t="n">
+        <v>4.93046776232618</v>
+      </c>
+      <c r="DU34" t="n">
+        <v>4.36953807740325</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -32823,12 +33309,18 @@
         <v>0.69284064665128</v>
       </c>
       <c r="DS35" t="n">
-        <v>0.860215053763438</v>
+        <v>-0.430107526881727</v>
+      </c>
+      <c r="DT35" t="n">
+        <v>0</v>
+      </c>
+      <c r="DU35" t="n">
+        <v>0.216450216450204</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -33194,12 +33686,18 @@
         <v>3.24763193504735</v>
       </c>
       <c r="DS36" t="n">
-        <v>1.66069684141974</v>
+        <v>1.7909475740801</v>
+      </c>
+      <c r="DT36" t="n">
+        <v>1.06865284974094</v>
+      </c>
+      <c r="DU36" t="n">
+        <v>0.838439213157053</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -33565,12 +34063,18 @@
         <v>2.93706293706293</v>
       </c>
       <c r="DS37" t="n">
-        <v>3.05039787798408</v>
+        <v>2.91777188328911</v>
+      </c>
+      <c r="DT37" t="n">
+        <v>2.35910878112713</v>
+      </c>
+      <c r="DU37" t="n">
+        <v>2.50659630606861</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -33936,12 +34440,18 @@
         <v>3.18731355000786</v>
       </c>
       <c r="DS38" t="n">
-        <v>4.08602150537633</v>
+        <v>4.14746543778802</v>
+      </c>
+      <c r="DT38" t="n">
+        <v>3.35067319461444</v>
+      </c>
+      <c r="DU38" t="n">
+        <v>3.56760067370999</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -34308,11 +34818,17 @@
       </c>
       <c r="DS39" t="n">
         <v>0.996264009962637</v>
+      </c>
+      <c r="DT39" t="n">
+        <v>0.725513905683185</v>
+      </c>
+      <c r="DU39" t="n">
+        <v>0.850546780072908</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -34678,12 +35194,18 @@
         <v>0.808625336927216</v>
       </c>
       <c r="DS40" t="n">
-        <v>1.05263157894736</v>
+        <v>0.789473684210519</v>
+      </c>
+      <c r="DT40" t="n">
+        <v>0.263157894736846</v>
+      </c>
+      <c r="DU40" t="n">
+        <v>0.795755968169754</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -35049,12 +35571,18 @@
         <v>0.934080597811583</v>
       </c>
       <c r="DS41" t="n">
-        <v>1.51670951156812</v>
+        <v>1.46529562982006</v>
+      </c>
+      <c r="DT41" t="n">
+        <v>2.8194516295913</v>
+      </c>
+      <c r="DU41" t="n">
+        <v>0.0761228114691587</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -35420,12 +35948,18 @@
         <v>-2.4113475177305</v>
       </c>
       <c r="DS42" t="n">
-        <v>-2.69541778975741</v>
+        <v>-1.68463611859838</v>
+      </c>
+      <c r="DT42" t="n">
+        <v>-1.07526881720432</v>
+      </c>
+      <c r="DU42" t="n">
+        <v>-1.20562625586069</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -35791,12 +36325,18 @@
         <v>4.67791411042944</v>
       </c>
       <c r="DS43" t="n">
-        <v>5.01121914734482</v>
+        <v>4.93642483171281</v>
+      </c>
+      <c r="DT43" t="n">
+        <v>5.05200594353641</v>
+      </c>
+      <c r="DU43" t="n">
+        <v>4.98511904761906</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -36163,11 +36703,17 @@
       </c>
       <c r="DS44" t="n">
         <v>1.9147621988882</v>
+      </c>
+      <c r="DT44" t="n">
+        <v>1.71884591774097</v>
+      </c>
+      <c r="DU44" t="n">
+        <v>1.93488943488944</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -36534,11 +37080,17 @@
       </c>
       <c r="DS45" t="n">
         <v>0.344827586206889</v>
+      </c>
+      <c r="DT45" t="n">
+        <v>2.73972602739726</v>
+      </c>
+      <c r="DU45" t="n">
+        <v>0.684931506849313</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -36904,12 +37456,18 @@
         <v>3.50649350649351</v>
       </c>
       <c r="DS46" t="n">
-        <v>2.42839352428394</v>
+        <v>2.92652552926527</v>
+      </c>
+      <c r="DT46" t="n">
+        <v>3.0284301606922</v>
+      </c>
+      <c r="DU46" t="n">
+        <v>2.78121137206428</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -37276,11 +37834,17 @@
       </c>
       <c r="DS47" t="n">
         <v>1.59999999999998</v>
+      </c>
+      <c r="DT47" t="n">
+        <v>1.32275132275132</v>
+      </c>
+      <c r="DU47" t="n">
+        <v>1.59574468085107</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -37646,12 +38210,18 @@
         <v>0.966429298067144</v>
       </c>
       <c r="DS48" t="n">
-        <v>-0.0485908649173928</v>
+        <v>0.923226433430518</v>
+      </c>
+      <c r="DT48" t="n">
+        <v>0.920096852300231</v>
+      </c>
+      <c r="DU48" t="n">
+        <v>1.21006776379477</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -38017,12 +38587,18 @@
         <v>2.39793189516849</v>
       </c>
       <c r="DS49" t="n">
-        <v>3.06077831219939</v>
+        <v>3.0345430695234</v>
+      </c>
+      <c r="DT49" t="n">
+        <v>3.21257092972501</v>
+      </c>
+      <c r="DU49" t="n">
+        <v>3.0778620629523</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -38389,11 +38965,17 @@
       </c>
       <c r="DS50" t="n">
         <v>2.57856567284448</v>
+      </c>
+      <c r="DT50" t="n">
+        <v>2.89156626506024</v>
+      </c>
+      <c r="DU50" t="n">
+        <v>2.88461538461539</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -38760,11 +39342,17 @@
       </c>
       <c r="DS51" t="n">
         <v>2.53164556962027</v>
+      </c>
+      <c r="DT51" t="n">
+        <v>3.5031847133758</v>
+      </c>
+      <c r="DU51" t="n">
+        <v>4.48717948717949</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -39131,11 +39719,17 @@
       </c>
       <c r="DS52" t="n">
         <v>3.76084860173577</v>
+      </c>
+      <c r="DT52" t="n">
+        <v>3.41962288271015</v>
+      </c>
+      <c r="DU52" t="n">
+        <v>2.7980922098569</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -39501,12 +40095,18 @@
         <v>3.28482328482329</v>
       </c>
       <c r="DS53" t="n">
-        <v>3.06623058053966</v>
+        <v>2.82093213409649</v>
+      </c>
+      <c r="DT53" t="n">
+        <v>2.55993498577813</v>
+      </c>
+      <c r="DU53" t="n">
+        <v>2.27088402270884</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -39872,12 +40472,18 @@
         <v>0.511073253833045</v>
       </c>
       <c r="DS54" t="n">
-        <v>1.63132137030994</v>
+        <v>1.63132137030995</v>
+      </c>
+      <c r="DT54" t="n">
+        <v>1.13085621970919</v>
+      </c>
+      <c r="DU54" t="n">
+        <v>1.13636363636363</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -40243,12 +40849,18 @@
         <v>2.59605399792314</v>
       </c>
       <c r="DS55" t="n">
-        <v>4.1747572815534</v>
+        <v>4.12621359223301</v>
+      </c>
+      <c r="DT55" t="n">
+        <v>3.08731307284128</v>
+      </c>
+      <c r="DU55" t="n">
+        <v>2.88184438040347</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -40614,7 +41226,13 @@
         <v>0.349650349650355</v>
       </c>
       <c r="DS56" t="n">
-        <v>1.34228187919464</v>
+        <v>1.00671140939598</v>
+      </c>
+      <c r="DT56" t="n">
+        <v>2.32558139534883</v>
+      </c>
+      <c r="DU56" t="n">
+        <v>1.66666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on June 16 2023
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t xml:space="preserve">04/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1323,10 +1326,13 @@
       <c r="EG4" t="s">
         <v>136</v>
       </c>
+      <c r="EH4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1731,15 +1737,18 @@
         <v>10787.5</v>
       </c>
       <c r="EF5" t="n">
-        <v>10819</v>
+        <v>10817.6</v>
       </c>
       <c r="EG5" t="n">
-        <v>10820.8</v>
+        <v>10830.7</v>
+      </c>
+      <c r="EH5" t="n">
+        <v>10734.3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2147,12 +2156,15 @@
         <v>171.8</v>
       </c>
       <c r="EG6" t="n">
-        <v>171.7</v>
+        <v>171.6</v>
+      </c>
+      <c r="EH6" t="n">
+        <v>171.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2561,11 +2573,14 @@
       </c>
       <c r="EG7" t="n">
         <v>29.1</v>
+      </c>
+      <c r="EH7" t="n">
+        <v>28.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2973,12 +2988,15 @@
         <v>197</v>
       </c>
       <c r="EG8" t="n">
-        <v>199.3</v>
+        <v>199.4</v>
+      </c>
+      <c r="EH8" t="n">
+        <v>192.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3387,11 +3405,14 @@
       </c>
       <c r="EG9" t="n">
         <v>102.6</v>
+      </c>
+      <c r="EH9" t="n">
+        <v>101.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3800,11 +3821,14 @@
       </c>
       <c r="EG10" t="n">
         <v>1248.8</v>
+      </c>
+      <c r="EH10" t="n">
+        <v>1258</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4213,11 +4237,14 @@
       </c>
       <c r="EG11" t="n">
         <v>224.8</v>
+      </c>
+      <c r="EH11" t="n">
+        <v>225.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4625,12 +4652,15 @@
         <v>126.3</v>
       </c>
       <c r="EG12" t="n">
-        <v>124.7</v>
+        <v>124.8</v>
+      </c>
+      <c r="EH12" t="n">
+        <v>123.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5038,12 +5068,15 @@
         <v>38.3</v>
       </c>
       <c r="EG13" t="n">
-        <v>38.8</v>
+        <v>38.2</v>
+      </c>
+      <c r="EH13" t="n">
+        <v>37.3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5181,10 +5214,11 @@
       <c r="EE14"/>
       <c r="EF14"/>
       <c r="EG14"/>
+      <c r="EH14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5592,12 +5626,15 @@
         <v>489.1</v>
       </c>
       <c r="EG15" t="n">
-        <v>488.7</v>
+        <v>488.9</v>
+      </c>
+      <c r="EH15" t="n">
+        <v>481.1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6005,12 +6042,15 @@
         <v>347.2</v>
       </c>
       <c r="EG16" t="n">
-        <v>346.4</v>
+        <v>346.3</v>
+      </c>
+      <c r="EH16" t="n">
+        <v>342.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6148,10 +6188,11 @@
       <c r="EE17"/>
       <c r="EF17"/>
       <c r="EG17"/>
+      <c r="EH17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6560,11 +6601,14 @@
       </c>
       <c r="EG18" t="n">
         <v>66.5</v>
+      </c>
+      <c r="EH18" t="n">
+        <v>64.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6972,12 +7016,15 @@
         <v>446.1</v>
       </c>
       <c r="EG19" t="n">
-        <v>445.9</v>
+        <v>446</v>
+      </c>
+      <c r="EH19" t="n">
+        <v>444.8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7385,12 +7432,15 @@
         <v>229.6</v>
       </c>
       <c r="EG20" t="n">
-        <v>228.9</v>
+        <v>229</v>
+      </c>
+      <c r="EH20" t="n">
+        <v>230.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7798,12 +7848,15 @@
         <v>145.7</v>
       </c>
       <c r="EG21" t="n">
-        <v>145.8</v>
+        <v>146.2</v>
+      </c>
+      <c r="EH21" t="n">
+        <v>145.5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8211,12 +8264,15 @@
         <v>135.9</v>
       </c>
       <c r="EG22" t="n">
-        <v>135.4</v>
+        <v>135.6</v>
+      </c>
+      <c r="EH22" t="n">
+        <v>135.7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8624,12 +8680,15 @@
         <v>161.4</v>
       </c>
       <c r="EG23" t="n">
-        <v>161.1</v>
+        <v>161</v>
+      </c>
+      <c r="EH23" t="n">
+        <v>160.7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9037,12 +9096,15 @@
         <v>149.3</v>
       </c>
       <c r="EG24" t="n">
-        <v>150.4</v>
+        <v>150.3</v>
+      </c>
+      <c r="EH24" t="n">
+        <v>149.8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9450,12 +9512,15 @@
         <v>50</v>
       </c>
       <c r="EG25" t="n">
-        <v>49.5</v>
+        <v>49.4</v>
+      </c>
+      <c r="EH25" t="n">
+        <v>49.7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9863,12 +9928,15 @@
         <v>220.5</v>
       </c>
       <c r="EG26" t="n">
+        <v>225</v>
+      </c>
+      <c r="EH26" t="n">
         <v>225</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10276,12 +10344,15 @@
         <v>245.9</v>
       </c>
       <c r="EG27" t="n">
-        <v>246.5</v>
+        <v>245.9</v>
+      </c>
+      <c r="EH27" t="n">
+        <v>245.9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10689,12 +10760,15 @@
         <v>323.6</v>
       </c>
       <c r="EG28" t="n">
-        <v>323.9</v>
+        <v>324.6</v>
+      </c>
+      <c r="EH28" t="n">
+        <v>307.1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11102,12 +11176,15 @@
         <v>205.6</v>
       </c>
       <c r="EG29" t="n">
-        <v>206</v>
+        <v>205.9</v>
+      </c>
+      <c r="EH29" t="n">
+        <v>203</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11516,11 +11593,14 @@
       </c>
       <c r="EG30" t="n">
         <v>103.5</v>
+      </c>
+      <c r="EH30" t="n">
+        <v>101.9</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11658,10 +11738,11 @@
       <c r="EE31"/>
       <c r="EF31"/>
       <c r="EG31"/>
+      <c r="EH31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12069,12 +12150,15 @@
         <v>43.6</v>
       </c>
       <c r="EG32" t="n">
-        <v>43.5</v>
+        <v>43.6</v>
+      </c>
+      <c r="EH32" t="n">
+        <v>42.6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12483,11 +12567,14 @@
       </c>
       <c r="EG33" t="n">
         <v>94.7</v>
+      </c>
+      <c r="EH33" t="n">
+        <v>94.9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -12896,11 +12983,14 @@
       </c>
       <c r="EG34" t="n">
         <v>83.6</v>
+      </c>
+      <c r="EH34" t="n">
+        <v>83.8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13308,12 +13398,15 @@
         <v>46</v>
       </c>
       <c r="EG35" t="n">
-        <v>46.3</v>
+        <v>46.4</v>
+      </c>
+      <c r="EH35" t="n">
+        <v>45.5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -13721,12 +13814,15 @@
         <v>312.1</v>
       </c>
       <c r="EG36" t="n">
-        <v>312.7</v>
+        <v>312.6</v>
+      </c>
+      <c r="EH36" t="n">
+        <v>309.9</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14135,11 +14231,14 @@
       </c>
       <c r="EG37" t="n">
         <v>77.7</v>
+      </c>
+      <c r="EH37" t="n">
+        <v>77.3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14547,12 +14646,15 @@
         <v>675.5</v>
       </c>
       <c r="EG38" t="n">
-        <v>676.4</v>
+        <v>676.1</v>
+      </c>
+      <c r="EH38" t="n">
+        <v>672.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -14961,11 +15063,14 @@
       </c>
       <c r="EG39" t="n">
         <v>332</v>
+      </c>
+      <c r="EH39" t="n">
+        <v>333.1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15373,12 +15478,15 @@
         <v>38.1</v>
       </c>
       <c r="EG40" t="n">
-        <v>38</v>
+        <v>38.2</v>
+      </c>
+      <c r="EH40" t="n">
+        <v>38.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -15787,11 +15895,14 @@
       </c>
       <c r="EG41" t="n">
         <v>394.4</v>
+      </c>
+      <c r="EH41" t="n">
+        <v>385.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16199,12 +16310,15 @@
         <v>147.2</v>
       </c>
       <c r="EG42" t="n">
-        <v>147.5</v>
+        <v>147.7</v>
+      </c>
+      <c r="EH42" t="n">
+        <v>146.9</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -16613,11 +16727,14 @@
       </c>
       <c r="EG43" t="n">
         <v>141.1</v>
+      </c>
+      <c r="EH43" t="n">
+        <v>142.6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17025,12 +17142,15 @@
         <v>331.4</v>
       </c>
       <c r="EG44" t="n">
-        <v>331.9</v>
+        <v>332</v>
+      </c>
+      <c r="EH44" t="n">
+        <v>326.7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17438,12 +17558,15 @@
         <v>30</v>
       </c>
       <c r="EG45" t="n">
-        <v>29.4</v>
+        <v>29.5</v>
+      </c>
+      <c r="EH45" t="n">
+        <v>29.8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -17852,11 +17975,14 @@
       </c>
       <c r="EG46" t="n">
         <v>166.3</v>
+      </c>
+      <c r="EH46" t="n">
+        <v>160.8</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18265,11 +18391,14 @@
       </c>
       <c r="EG47" t="n">
         <v>38.2</v>
+      </c>
+      <c r="EH47" t="n">
+        <v>37.7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -18677,12 +18806,15 @@
         <v>208.4</v>
       </c>
       <c r="EG48" t="n">
-        <v>209.1</v>
+        <v>209.4</v>
+      </c>
+      <c r="EH48" t="n">
+        <v>202.9</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -19091,11 +19223,14 @@
       </c>
       <c r="EG49" t="n">
         <v>1182.2</v>
+      </c>
+      <c r="EH49" t="n">
+        <v>1178.1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -19504,11 +19639,14 @@
       </c>
       <c r="EG50" t="n">
         <v>128.4</v>
+      </c>
+      <c r="EH50" t="n">
+        <v>128.6</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -19917,11 +20055,14 @@
       </c>
       <c r="EG51" t="n">
         <v>32.6</v>
+      </c>
+      <c r="EH51" t="n">
+        <v>30.3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20329,12 +20470,15 @@
         <v>323.6</v>
       </c>
       <c r="EG52" t="n">
-        <v>323.3</v>
+        <v>323.7</v>
+      </c>
+      <c r="EH52" t="n">
+        <v>314.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -20742,12 +20886,15 @@
         <v>252.4</v>
       </c>
       <c r="EG53" t="n">
-        <v>252.2</v>
+        <v>252.1</v>
+      </c>
+      <c r="EH53" t="n">
+        <v>249.1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -21156,11 +21303,14 @@
       </c>
       <c r="EG54" t="n">
         <v>62.3</v>
+      </c>
+      <c r="EH54" t="n">
+        <v>61.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -21569,11 +21719,14 @@
       </c>
       <c r="EG55" t="n">
         <v>214.2</v>
+      </c>
+      <c r="EH55" t="n">
+        <v>211.6</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -21981,7 +22134,10 @@
         <v>30.8</v>
       </c>
       <c r="EG56" t="n">
-        <v>30.5</v>
+        <v>30.6</v>
+      </c>
+      <c r="EH56" t="n">
+        <v>30.7</v>
       </c>
     </row>
   </sheetData>
@@ -22374,10 +22530,13 @@
       <c r="DU4" t="s">
         <v>136</v>
       </c>
+      <c r="DV4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -22746,15 +22905,18 @@
         <v>2.45609702817959</v>
       </c>
       <c r="DT5" t="n">
-        <v>2.38090731873498</v>
+        <v>2.36765902681833</v>
       </c>
       <c r="DU5" t="n">
-        <v>2.21416156578251</v>
+        <v>2.30767777525883</v>
+      </c>
+      <c r="DV5" t="n">
+        <v>2.49694446566343</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -23126,12 +23288,15 @@
         <v>2.20107079119571</v>
       </c>
       <c r="DU6" t="n">
-        <v>0.999999999999993</v>
+        <v>0.941176470588232</v>
+      </c>
+      <c r="DV6" t="n">
+        <v>0.764256319811848</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -23504,11 +23669,14 @@
       </c>
       <c r="DU7" t="n">
         <v>4.67625899280576</v>
+      </c>
+      <c r="DV7" t="n">
+        <v>5.99250936329586</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -23880,12 +24048,15 @@
         <v>0.767263427109974</v>
       </c>
       <c r="DU8" t="n">
-        <v>1.78753830439224</v>
+        <v>1.83861082737485</v>
+      </c>
+      <c r="DV8" t="n">
+        <v>1.47523709167544</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -24258,11 +24429,14 @@
       </c>
       <c r="DU9" t="n">
         <v>0.686947988223738</v>
+      </c>
+      <c r="DV9" t="n">
+        <v>0.594059405940588</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -24635,11 +24809,14 @@
       </c>
       <c r="DU10" t="n">
         <v>2.94287362954415</v>
+      </c>
+      <c r="DV10" t="n">
+        <v>2.92914416625756</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -25012,11 +25189,14 @@
       </c>
       <c r="DU11" t="n">
         <v>2.93040293040293</v>
+      </c>
+      <c r="DV11" t="n">
+        <v>3.15500685871058</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -25388,12 +25568,15 @@
         <v>1.5273311897106</v>
       </c>
       <c r="DU12" t="n">
-        <v>0.321802091713601</v>
+        <v>0.402252614641995</v>
+      </c>
+      <c r="DV12" t="n">
+        <v>0.571428571428574</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -25765,12 +25948,15 @@
         <v>2.40641711229944</v>
       </c>
       <c r="DU13" t="n">
-        <v>2.64550264550265</v>
+        <v>1.05820105820107</v>
+      </c>
+      <c r="DV13" t="n">
+        <v>1.08401084010838</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -25896,10 +26082,11 @@
       <c r="DS14"/>
       <c r="DT14"/>
       <c r="DU14"/>
+      <c r="DV14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -26271,12 +26458,15 @@
         <v>1.85339441899209</v>
       </c>
       <c r="DU15" t="n">
-        <v>1.72772689425479</v>
+        <v>1.76935886761032</v>
+      </c>
+      <c r="DV15" t="n">
+        <v>1.64800338051976</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -26648,12 +26838,15 @@
         <v>3.08788598574821</v>
       </c>
       <c r="DU16" t="n">
-        <v>2.85035629453681</v>
+        <v>2.82066508313539</v>
+      </c>
+      <c r="DV16" t="n">
+        <v>1.93509973206311</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -26779,10 +26972,11 @@
       <c r="DS17"/>
       <c r="DT17"/>
       <c r="DU17"/>
+      <c r="DV17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -27155,11 +27349,14 @@
       </c>
       <c r="DU18" t="n">
         <v>7.60517799352751</v>
+      </c>
+      <c r="DV18" t="n">
+        <v>5.73770491803279</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -27531,12 +27728,15 @@
         <v>3.76831821353804</v>
       </c>
       <c r="DU19" t="n">
-        <v>3.8667598416026</v>
+        <v>3.89005357558816</v>
+      </c>
+      <c r="DV19" t="n">
+        <v>3.973819541842</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -27908,12 +28108,15 @@
         <v>2.18068535825547</v>
       </c>
       <c r="DU20" t="n">
-        <v>2.14190093708165</v>
+        <v>2.18652387327086</v>
+      </c>
+      <c r="DV20" t="n">
+        <v>2.54010695187165</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -28285,12 +28488,15 @@
         <v>2.24561403508771</v>
       </c>
       <c r="DU21" t="n">
-        <v>1.95804195804197</v>
+        <v>2.23776223776223</v>
+      </c>
+      <c r="DV21" t="n">
+        <v>1.96215837421164</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -28662,12 +28868,15 @@
         <v>0.221238938053106</v>
       </c>
       <c r="DU22" t="n">
-        <v>-0.294550810014732</v>
+        <v>-0.147275405007376</v>
+      </c>
+      <c r="DV22" t="n">
+        <v>0.147601476014752</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -29039,12 +29248,15 @@
         <v>1.31826741996233</v>
       </c>
       <c r="DU23" t="n">
-        <v>1.76879343019582</v>
+        <v>1.70562223626026</v>
+      </c>
+      <c r="DV23" t="n">
+        <v>1.64452877925363</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -29416,12 +29628,15 @@
         <v>3.39335180055402</v>
       </c>
       <c r="DU24" t="n">
-        <v>3.36769759450172</v>
+        <v>3.29896907216496</v>
+      </c>
+      <c r="DV24" t="n">
+        <v>2.95532646048111</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -29793,12 +30008,15 @@
         <v>0.200400801603209</v>
       </c>
       <c r="DU25" t="n">
-        <v>-1.19760479041916</v>
+        <v>-1.39720558882235</v>
+      </c>
+      <c r="DV25" t="n">
+        <v>1.22199592668026</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -30171,11 +30389,14 @@
       </c>
       <c r="DU26" t="n">
         <v>3.3532384014699</v>
+      </c>
+      <c r="DV26" t="n">
+        <v>2.92772186642268</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -30547,12 +30768,15 @@
         <v>3.44972654606645</v>
       </c>
       <c r="DU27" t="n">
-        <v>3.31098072087174</v>
+        <v>3.05951383067894</v>
+      </c>
+      <c r="DV27" t="n">
+        <v>2.8439983270598</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -30924,12 +31148,15 @@
         <v>6.27257799671594</v>
       </c>
       <c r="DU28" t="n">
-        <v>5.84967320261437</v>
+        <v>6.07843137254903</v>
+      </c>
+      <c r="DV28" t="n">
+        <v>5.89655172413794</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -31301,12 +31528,15 @@
         <v>0.636319138521787</v>
       </c>
       <c r="DU29" t="n">
-        <v>0.340964442279585</v>
+        <v>0.292255236239646</v>
+      </c>
+      <c r="DV29" t="n">
+        <v>0.644521566683198</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -31679,11 +31909,14 @@
       </c>
       <c r="DU30" t="n">
         <v>1.07421874999999</v>
+      </c>
+      <c r="DV30" t="n">
+        <v>1.09126984126985</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -31809,10 +32042,11 @@
       <c r="DS31"/>
       <c r="DT31"/>
       <c r="DU31"/>
+      <c r="DV31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -32184,12 +32418,15 @@
         <v>-1.35746606334842</v>
       </c>
       <c r="DU32" t="n">
-        <v>-1.58371040723983</v>
+        <v>-1.35746606334842</v>
+      </c>
+      <c r="DV32" t="n">
+        <v>-4.48430493273543</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -32562,11 +32799,14 @@
       </c>
       <c r="DU33" t="n">
         <v>1.28342245989305</v>
+      </c>
+      <c r="DV33" t="n">
+        <v>1.60599571734474</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -32939,11 +33179,14 @@
       </c>
       <c r="DU34" t="n">
         <v>4.36953807740325</v>
+      </c>
+      <c r="DV34" t="n">
+        <v>4.61922596754058</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -33315,12 +33558,15 @@
         <v>0</v>
       </c>
       <c r="DU35" t="n">
-        <v>0.216450216450204</v>
+        <v>0.432900432900424</v>
+      </c>
+      <c r="DV35" t="n">
+        <v>0.886917960088689</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -33692,12 +33938,15 @@
         <v>1.06865284974094</v>
       </c>
       <c r="DU36" t="n">
-        <v>0.838439213157053</v>
+        <v>0.806191551112544</v>
+      </c>
+      <c r="DV36" t="n">
+        <v>1.53997378768022</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -34070,11 +34319,14 @@
       </c>
       <c r="DU37" t="n">
         <v>2.50659630606861</v>
+      </c>
+      <c r="DV37" t="n">
+        <v>3.61930294906167</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -34446,12 +34698,15 @@
         <v>3.35067319461444</v>
       </c>
       <c r="DU38" t="n">
-        <v>3.56760067370999</v>
+        <v>3.52166590108712</v>
+      </c>
+      <c r="DV38" t="n">
+        <v>3.49392027089425</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -34824,11 +35079,14 @@
       </c>
       <c r="DU39" t="n">
         <v>0.850546780072908</v>
+      </c>
+      <c r="DV39" t="n">
+        <v>0.725733293014827</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -35200,12 +35458,15 @@
         <v>0.263157894736846</v>
       </c>
       <c r="DU40" t="n">
-        <v>0.795755968169754</v>
+        <v>1.3262599469496</v>
+      </c>
+      <c r="DV40" t="n">
+        <v>1.06100795755968</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -35578,11 +35839,14 @@
       </c>
       <c r="DU41" t="n">
         <v>0.0761228114691587</v>
+      </c>
+      <c r="DV41" t="n">
+        <v>-0.926164136866484</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -35954,12 +36218,15 @@
         <v>-1.07526881720432</v>
       </c>
       <c r="DU42" t="n">
-        <v>-1.20562625586069</v>
+        <v>-1.07166778298729</v>
+      </c>
+      <c r="DV42" t="n">
+        <v>-1.14401076716017</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -36332,11 +36599,14 @@
       </c>
       <c r="DU43" t="n">
         <v>4.98511904761906</v>
+      </c>
+      <c r="DV43" t="n">
+        <v>5.47337278106509</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -36708,12 +36978,15 @@
         <v>1.71884591774097</v>
       </c>
       <c r="DU44" t="n">
-        <v>1.93488943488944</v>
+        <v>1.96560196560196</v>
+      </c>
+      <c r="DV44" t="n">
+        <v>2.02998126171143</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -37085,12 +37358,15 @@
         <v>2.73972602739726</v>
       </c>
       <c r="DU45" t="n">
-        <v>0.684931506849313</v>
+        <v>1.02739726027398</v>
+      </c>
+      <c r="DV45" t="n">
+        <v>2.75862068965516</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -37463,11 +37739,14 @@
       </c>
       <c r="DU46" t="n">
         <v>2.78121137206428</v>
+      </c>
+      <c r="DV46" t="n">
+        <v>-0.0621504039776223</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -37840,11 +38119,14 @@
       </c>
       <c r="DU47" t="n">
         <v>1.59574468085107</v>
+      </c>
+      <c r="DV47" t="n">
+        <v>1.8918918918919</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -38216,12 +38498,15 @@
         <v>0.920096852300231</v>
       </c>
       <c r="DU48" t="n">
-        <v>1.21006776379477</v>
+        <v>1.35527589545014</v>
+      </c>
+      <c r="DV48" t="n">
+        <v>1.29805292061907</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -38594,11 +38879,14 @@
       </c>
       <c r="DU49" t="n">
         <v>3.0778620629523</v>
+      </c>
+      <c r="DV49" t="n">
+        <v>3.07988450433107</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -38971,11 +39259,14 @@
       </c>
       <c r="DU50" t="n">
         <v>2.88461538461539</v>
+      </c>
+      <c r="DV50" t="n">
+        <v>3.04487179487179</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -39348,11 +39639,14 @@
       </c>
       <c r="DU51" t="n">
         <v>4.48717948717949</v>
+      </c>
+      <c r="DV51" t="n">
+        <v>-2.8846153846154</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -39724,12 +40018,15 @@
         <v>3.41962288271015</v>
       </c>
       <c r="DU52" t="n">
-        <v>2.7980922098569</v>
+        <v>2.92527821939586</v>
+      </c>
+      <c r="DV52" t="n">
+        <v>2.2121014964216</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -40101,12 +40398,15 @@
         <v>2.55993498577813</v>
       </c>
       <c r="DU53" t="n">
-        <v>2.27088402270884</v>
+        <v>2.23033252230333</v>
+      </c>
+      <c r="DV53" t="n">
+        <v>0.646464646464656</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -40479,11 +40779,14 @@
       </c>
       <c r="DU54" t="n">
         <v>1.13636363636363</v>
+      </c>
+      <c r="DV54" t="n">
+        <v>0.985221674876838</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -40855,12 +41158,15 @@
         <v>3.08731307284128</v>
       </c>
       <c r="DU55" t="n">
-        <v>2.88184438040347</v>
+        <v>2.88184438040346</v>
+      </c>
+      <c r="DV55" t="n">
+        <v>3.72549019607843</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -41232,7 +41538,10 @@
         <v>2.32558139534883</v>
       </c>
       <c r="DU56" t="n">
-        <v>1.66666666666667</v>
+        <v>2</v>
+      </c>
+      <c r="DV56" t="n">
+        <v>2.33333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on July 21st
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -424,9 +424,6 @@
   </si>
   <si>
     <t xml:space="preserve">04/01/2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1326,13 +1323,10 @@
       <c r="EG4" t="s">
         <v>136</v>
       </c>
-      <c r="EH4" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1737,18 +1731,15 @@
         <v>10787.5</v>
       </c>
       <c r="EF5" t="n">
-        <v>10817.6</v>
+        <v>10819</v>
       </c>
       <c r="EG5" t="n">
-        <v>10830.7</v>
-      </c>
-      <c r="EH5" t="n">
-        <v>10734.3</v>
+        <v>10820.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2156,15 +2147,12 @@
         <v>171.8</v>
       </c>
       <c r="EG6" t="n">
-        <v>171.6</v>
-      </c>
-      <c r="EH6" t="n">
-        <v>171.4</v>
+        <v>171.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2573,14 +2561,11 @@
       </c>
       <c r="EG7" t="n">
         <v>29.1</v>
-      </c>
-      <c r="EH7" t="n">
-        <v>28.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2988,15 +2973,12 @@
         <v>197</v>
       </c>
       <c r="EG8" t="n">
-        <v>199.4</v>
-      </c>
-      <c r="EH8" t="n">
-        <v>192.6</v>
+        <v>199.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3405,14 +3387,11 @@
       </c>
       <c r="EG9" t="n">
         <v>102.6</v>
-      </c>
-      <c r="EH9" t="n">
-        <v>101.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3821,14 +3800,11 @@
       </c>
       <c r="EG10" t="n">
         <v>1248.8</v>
-      </c>
-      <c r="EH10" t="n">
-        <v>1258</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4237,14 +4213,11 @@
       </c>
       <c r="EG11" t="n">
         <v>224.8</v>
-      </c>
-      <c r="EH11" t="n">
-        <v>225.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4652,15 +4625,12 @@
         <v>126.3</v>
       </c>
       <c r="EG12" t="n">
-        <v>124.8</v>
-      </c>
-      <c r="EH12" t="n">
-        <v>123.2</v>
+        <v>124.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5068,15 +5038,12 @@
         <v>38.3</v>
       </c>
       <c r="EG13" t="n">
-        <v>38.2</v>
-      </c>
-      <c r="EH13" t="n">
-        <v>37.3</v>
+        <v>38.8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5214,11 +5181,10 @@
       <c r="EE14"/>
       <c r="EF14"/>
       <c r="EG14"/>
-      <c r="EH14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5626,15 +5592,12 @@
         <v>489.1</v>
       </c>
       <c r="EG15" t="n">
-        <v>488.9</v>
-      </c>
-      <c r="EH15" t="n">
-        <v>481.1</v>
+        <v>488.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6042,15 +6005,12 @@
         <v>347.2</v>
       </c>
       <c r="EG16" t="n">
-        <v>346.3</v>
-      </c>
-      <c r="EH16" t="n">
-        <v>342.4</v>
+        <v>346.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6188,11 +6148,10 @@
       <c r="EE17"/>
       <c r="EF17"/>
       <c r="EG17"/>
-      <c r="EH17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6601,14 +6560,11 @@
       </c>
       <c r="EG18" t="n">
         <v>66.5</v>
-      </c>
-      <c r="EH18" t="n">
-        <v>64.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7016,15 +6972,12 @@
         <v>446.1</v>
       </c>
       <c r="EG19" t="n">
-        <v>446</v>
-      </c>
-      <c r="EH19" t="n">
-        <v>444.8</v>
+        <v>445.9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7432,15 +7385,12 @@
         <v>229.6</v>
       </c>
       <c r="EG20" t="n">
-        <v>229</v>
-      </c>
-      <c r="EH20" t="n">
-        <v>230.1</v>
+        <v>228.9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7848,15 +7798,12 @@
         <v>145.7</v>
       </c>
       <c r="EG21" t="n">
-        <v>146.2</v>
-      </c>
-      <c r="EH21" t="n">
-        <v>145.5</v>
+        <v>145.8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8264,15 +8211,12 @@
         <v>135.9</v>
       </c>
       <c r="EG22" t="n">
-        <v>135.6</v>
-      </c>
-      <c r="EH22" t="n">
-        <v>135.7</v>
+        <v>135.4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8680,15 +8624,12 @@
         <v>161.4</v>
       </c>
       <c r="EG23" t="n">
-        <v>161</v>
-      </c>
-      <c r="EH23" t="n">
-        <v>160.7</v>
+        <v>161.1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9096,15 +9037,12 @@
         <v>149.3</v>
       </c>
       <c r="EG24" t="n">
-        <v>150.3</v>
-      </c>
-      <c r="EH24" t="n">
-        <v>149.8</v>
+        <v>150.4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9512,15 +9450,12 @@
         <v>50</v>
       </c>
       <c r="EG25" t="n">
-        <v>49.4</v>
-      </c>
-      <c r="EH25" t="n">
-        <v>49.7</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9928,15 +9863,12 @@
         <v>220.5</v>
       </c>
       <c r="EG26" t="n">
-        <v>225</v>
-      </c>
-      <c r="EH26" t="n">
         <v>225</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10344,15 +10276,12 @@
         <v>245.9</v>
       </c>
       <c r="EG27" t="n">
-        <v>245.9</v>
-      </c>
-      <c r="EH27" t="n">
-        <v>245.9</v>
+        <v>246.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10760,15 +10689,12 @@
         <v>323.6</v>
       </c>
       <c r="EG28" t="n">
-        <v>324.6</v>
-      </c>
-      <c r="EH28" t="n">
-        <v>307.1</v>
+        <v>323.9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11176,15 +11102,12 @@
         <v>205.6</v>
       </c>
       <c r="EG29" t="n">
-        <v>205.9</v>
-      </c>
-      <c r="EH29" t="n">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11593,14 +11516,11 @@
       </c>
       <c r="EG30" t="n">
         <v>103.5</v>
-      </c>
-      <c r="EH30" t="n">
-        <v>101.9</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11738,11 +11658,10 @@
       <c r="EE31"/>
       <c r="EF31"/>
       <c r="EG31"/>
-      <c r="EH31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12150,15 +12069,12 @@
         <v>43.6</v>
       </c>
       <c r="EG32" t="n">
-        <v>43.6</v>
-      </c>
-      <c r="EH32" t="n">
-        <v>42.6</v>
+        <v>43.5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12567,14 +12483,11 @@
       </c>
       <c r="EG33" t="n">
         <v>94.7</v>
-      </c>
-      <c r="EH33" t="n">
-        <v>94.9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -12983,14 +12896,11 @@
       </c>
       <c r="EG34" t="n">
         <v>83.6</v>
-      </c>
-      <c r="EH34" t="n">
-        <v>83.8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13398,15 +13308,12 @@
         <v>46</v>
       </c>
       <c r="EG35" t="n">
-        <v>46.4</v>
-      </c>
-      <c r="EH35" t="n">
-        <v>45.5</v>
+        <v>46.3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -13814,15 +13721,12 @@
         <v>312.1</v>
       </c>
       <c r="EG36" t="n">
-        <v>312.6</v>
-      </c>
-      <c r="EH36" t="n">
-        <v>309.9</v>
+        <v>312.7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14231,14 +14135,11 @@
       </c>
       <c r="EG37" t="n">
         <v>77.7</v>
-      </c>
-      <c r="EH37" t="n">
-        <v>77.3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14646,15 +14547,12 @@
         <v>675.5</v>
       </c>
       <c r="EG38" t="n">
-        <v>676.1</v>
-      </c>
-      <c r="EH38" t="n">
-        <v>672.4</v>
+        <v>676.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -15063,14 +14961,11 @@
       </c>
       <c r="EG39" t="n">
         <v>332</v>
-      </c>
-      <c r="EH39" t="n">
-        <v>333.1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15478,15 +15373,12 @@
         <v>38.1</v>
       </c>
       <c r="EG40" t="n">
-        <v>38.2</v>
-      </c>
-      <c r="EH40" t="n">
-        <v>38.1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -15895,14 +15787,11 @@
       </c>
       <c r="EG41" t="n">
         <v>394.4</v>
-      </c>
-      <c r="EH41" t="n">
-        <v>385.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16310,15 +16199,12 @@
         <v>147.2</v>
       </c>
       <c r="EG42" t="n">
-        <v>147.7</v>
-      </c>
-      <c r="EH42" t="n">
-        <v>146.9</v>
+        <v>147.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -16727,14 +16613,11 @@
       </c>
       <c r="EG43" t="n">
         <v>141.1</v>
-      </c>
-      <c r="EH43" t="n">
-        <v>142.6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17142,15 +17025,12 @@
         <v>331.4</v>
       </c>
       <c r="EG44" t="n">
-        <v>332</v>
-      </c>
-      <c r="EH44" t="n">
-        <v>326.7</v>
+        <v>331.9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17558,15 +17438,12 @@
         <v>30</v>
       </c>
       <c r="EG45" t="n">
-        <v>29.5</v>
-      </c>
-      <c r="EH45" t="n">
-        <v>29.8</v>
+        <v>29.4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -17975,14 +17852,11 @@
       </c>
       <c r="EG46" t="n">
         <v>166.3</v>
-      </c>
-      <c r="EH46" t="n">
-        <v>160.8</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18391,14 +18265,11 @@
       </c>
       <c r="EG47" t="n">
         <v>38.2</v>
-      </c>
-      <c r="EH47" t="n">
-        <v>37.7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -18806,15 +18677,12 @@
         <v>208.4</v>
       </c>
       <c r="EG48" t="n">
-        <v>209.4</v>
-      </c>
-      <c r="EH48" t="n">
-        <v>202.9</v>
+        <v>209.1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -19223,14 +19091,11 @@
       </c>
       <c r="EG49" t="n">
         <v>1182.2</v>
-      </c>
-      <c r="EH49" t="n">
-        <v>1178.1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -19639,14 +19504,11 @@
       </c>
       <c r="EG50" t="n">
         <v>128.4</v>
-      </c>
-      <c r="EH50" t="n">
-        <v>128.6</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -20055,14 +19917,11 @@
       </c>
       <c r="EG51" t="n">
         <v>32.6</v>
-      </c>
-      <c r="EH51" t="n">
-        <v>30.3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20470,15 +20329,12 @@
         <v>323.6</v>
       </c>
       <c r="EG52" t="n">
-        <v>323.7</v>
-      </c>
-      <c r="EH52" t="n">
-        <v>314.2</v>
+        <v>323.3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -20886,15 +20742,12 @@
         <v>252.4</v>
       </c>
       <c r="EG53" t="n">
-        <v>252.1</v>
-      </c>
-      <c r="EH53" t="n">
-        <v>249.1</v>
+        <v>252.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -21303,14 +21156,11 @@
       </c>
       <c r="EG54" t="n">
         <v>62.3</v>
-      </c>
-      <c r="EH54" t="n">
-        <v>61.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -21719,14 +21569,11 @@
       </c>
       <c r="EG55" t="n">
         <v>214.2</v>
-      </c>
-      <c r="EH55" t="n">
-        <v>211.6</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -22134,10 +21981,7 @@
         <v>30.8</v>
       </c>
       <c r="EG56" t="n">
-        <v>30.6</v>
-      </c>
-      <c r="EH56" t="n">
-        <v>30.7</v>
+        <v>30.5</v>
       </c>
     </row>
   </sheetData>
@@ -22530,13 +22374,10 @@
       <c r="DU4" t="s">
         <v>136</v>
       </c>
-      <c r="DV4" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -22905,18 +22746,15 @@
         <v>2.45609702817959</v>
       </c>
       <c r="DT5" t="n">
-        <v>2.36765902681833</v>
+        <v>2.38090731873498</v>
       </c>
       <c r="DU5" t="n">
-        <v>2.30767777525883</v>
-      </c>
-      <c r="DV5" t="n">
-        <v>2.49694446566343</v>
+        <v>2.21416156578251</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -23288,15 +23126,12 @@
         <v>2.20107079119571</v>
       </c>
       <c r="DU6" t="n">
-        <v>0.941176470588232</v>
-      </c>
-      <c r="DV6" t="n">
-        <v>0.764256319811848</v>
+        <v>0.999999999999993</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -23669,14 +23504,11 @@
       </c>
       <c r="DU7" t="n">
         <v>4.67625899280576</v>
-      </c>
-      <c r="DV7" t="n">
-        <v>5.99250936329586</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -24048,15 +23880,12 @@
         <v>0.767263427109974</v>
       </c>
       <c r="DU8" t="n">
-        <v>1.83861082737485</v>
-      </c>
-      <c r="DV8" t="n">
-        <v>1.47523709167544</v>
+        <v>1.78753830439224</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -24429,14 +24258,11 @@
       </c>
       <c r="DU9" t="n">
         <v>0.686947988223738</v>
-      </c>
-      <c r="DV9" t="n">
-        <v>0.594059405940588</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -24809,14 +24635,11 @@
       </c>
       <c r="DU10" t="n">
         <v>2.94287362954415</v>
-      </c>
-      <c r="DV10" t="n">
-        <v>2.92914416625756</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -25189,14 +25012,11 @@
       </c>
       <c r="DU11" t="n">
         <v>2.93040293040293</v>
-      </c>
-      <c r="DV11" t="n">
-        <v>3.15500685871058</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -25568,15 +25388,12 @@
         <v>1.5273311897106</v>
       </c>
       <c r="DU12" t="n">
-        <v>0.402252614641995</v>
-      </c>
-      <c r="DV12" t="n">
-        <v>0.571428571428574</v>
+        <v>0.321802091713601</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -25948,15 +25765,12 @@
         <v>2.40641711229944</v>
       </c>
       <c r="DU13" t="n">
-        <v>1.05820105820107</v>
-      </c>
-      <c r="DV13" t="n">
-        <v>1.08401084010838</v>
+        <v>2.64550264550265</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -26082,11 +25896,10 @@
       <c r="DS14"/>
       <c r="DT14"/>
       <c r="DU14"/>
-      <c r="DV14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -26458,15 +26271,12 @@
         <v>1.85339441899209</v>
       </c>
       <c r="DU15" t="n">
-        <v>1.76935886761032</v>
-      </c>
-      <c r="DV15" t="n">
-        <v>1.64800338051976</v>
+        <v>1.72772689425479</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -26838,15 +26648,12 @@
         <v>3.08788598574821</v>
       </c>
       <c r="DU16" t="n">
-        <v>2.82066508313539</v>
-      </c>
-      <c r="DV16" t="n">
-        <v>1.93509973206311</v>
+        <v>2.85035629453681</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -26972,11 +26779,10 @@
       <c r="DS17"/>
       <c r="DT17"/>
       <c r="DU17"/>
-      <c r="DV17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -27349,14 +27155,11 @@
       </c>
       <c r="DU18" t="n">
         <v>7.60517799352751</v>
-      </c>
-      <c r="DV18" t="n">
-        <v>5.73770491803279</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -27728,15 +27531,12 @@
         <v>3.76831821353804</v>
       </c>
       <c r="DU19" t="n">
-        <v>3.89005357558816</v>
-      </c>
-      <c r="DV19" t="n">
-        <v>3.973819541842</v>
+        <v>3.8667598416026</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -28108,15 +27908,12 @@
         <v>2.18068535825547</v>
       </c>
       <c r="DU20" t="n">
-        <v>2.18652387327086</v>
-      </c>
-      <c r="DV20" t="n">
-        <v>2.54010695187165</v>
+        <v>2.14190093708165</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -28488,15 +28285,12 @@
         <v>2.24561403508771</v>
       </c>
       <c r="DU21" t="n">
-        <v>2.23776223776223</v>
-      </c>
-      <c r="DV21" t="n">
-        <v>1.96215837421164</v>
+        <v>1.95804195804197</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -28868,15 +28662,12 @@
         <v>0.221238938053106</v>
       </c>
       <c r="DU22" t="n">
-        <v>-0.147275405007376</v>
-      </c>
-      <c r="DV22" t="n">
-        <v>0.147601476014752</v>
+        <v>-0.294550810014732</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -29248,15 +29039,12 @@
         <v>1.31826741996233</v>
       </c>
       <c r="DU23" t="n">
-        <v>1.70562223626026</v>
-      </c>
-      <c r="DV23" t="n">
-        <v>1.64452877925363</v>
+        <v>1.76879343019582</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -29628,15 +29416,12 @@
         <v>3.39335180055402</v>
       </c>
       <c r="DU24" t="n">
-        <v>3.29896907216496</v>
-      </c>
-      <c r="DV24" t="n">
-        <v>2.95532646048111</v>
+        <v>3.36769759450172</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -30008,15 +29793,12 @@
         <v>0.200400801603209</v>
       </c>
       <c r="DU25" t="n">
-        <v>-1.39720558882235</v>
-      </c>
-      <c r="DV25" t="n">
-        <v>1.22199592668026</v>
+        <v>-1.19760479041916</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -30389,14 +30171,11 @@
       </c>
       <c r="DU26" t="n">
         <v>3.3532384014699</v>
-      </c>
-      <c r="DV26" t="n">
-        <v>2.92772186642268</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -30768,15 +30547,12 @@
         <v>3.44972654606645</v>
       </c>
       <c r="DU27" t="n">
-        <v>3.05951383067894</v>
-      </c>
-      <c r="DV27" t="n">
-        <v>2.8439983270598</v>
+        <v>3.31098072087174</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -31148,15 +30924,12 @@
         <v>6.27257799671594</v>
       </c>
       <c r="DU28" t="n">
-        <v>6.07843137254903</v>
-      </c>
-      <c r="DV28" t="n">
-        <v>5.89655172413794</v>
+        <v>5.84967320261437</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -31528,15 +31301,12 @@
         <v>0.636319138521787</v>
       </c>
       <c r="DU29" t="n">
-        <v>0.292255236239646</v>
-      </c>
-      <c r="DV29" t="n">
-        <v>0.644521566683198</v>
+        <v>0.340964442279585</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -31909,14 +31679,11 @@
       </c>
       <c r="DU30" t="n">
         <v>1.07421874999999</v>
-      </c>
-      <c r="DV30" t="n">
-        <v>1.09126984126985</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -32042,11 +31809,10 @@
       <c r="DS31"/>
       <c r="DT31"/>
       <c r="DU31"/>
-      <c r="DV31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -32418,15 +32184,12 @@
         <v>-1.35746606334842</v>
       </c>
       <c r="DU32" t="n">
-        <v>-1.35746606334842</v>
-      </c>
-      <c r="DV32" t="n">
-        <v>-4.48430493273543</v>
+        <v>-1.58371040723983</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -32799,14 +32562,11 @@
       </c>
       <c r="DU33" t="n">
         <v>1.28342245989305</v>
-      </c>
-      <c r="DV33" t="n">
-        <v>1.60599571734474</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -33179,14 +32939,11 @@
       </c>
       <c r="DU34" t="n">
         <v>4.36953807740325</v>
-      </c>
-      <c r="DV34" t="n">
-        <v>4.61922596754058</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -33558,15 +33315,12 @@
         <v>0</v>
       </c>
       <c r="DU35" t="n">
-        <v>0.432900432900424</v>
-      </c>
-      <c r="DV35" t="n">
-        <v>0.886917960088689</v>
+        <v>0.216450216450204</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -33938,15 +33692,12 @@
         <v>1.06865284974094</v>
       </c>
       <c r="DU36" t="n">
-        <v>0.806191551112544</v>
-      </c>
-      <c r="DV36" t="n">
-        <v>1.53997378768022</v>
+        <v>0.838439213157053</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -34319,14 +34070,11 @@
       </c>
       <c r="DU37" t="n">
         <v>2.50659630606861</v>
-      </c>
-      <c r="DV37" t="n">
-        <v>3.61930294906167</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -34698,15 +34446,12 @@
         <v>3.35067319461444</v>
       </c>
       <c r="DU38" t="n">
-        <v>3.52166590108712</v>
-      </c>
-      <c r="DV38" t="n">
-        <v>3.49392027089425</v>
+        <v>3.56760067370999</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -35079,14 +34824,11 @@
       </c>
       <c r="DU39" t="n">
         <v>0.850546780072908</v>
-      </c>
-      <c r="DV39" t="n">
-        <v>0.725733293014827</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -35458,15 +35200,12 @@
         <v>0.263157894736846</v>
       </c>
       <c r="DU40" t="n">
-        <v>1.3262599469496</v>
-      </c>
-      <c r="DV40" t="n">
-        <v>1.06100795755968</v>
+        <v>0.795755968169754</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -35839,14 +35578,11 @@
       </c>
       <c r="DU41" t="n">
         <v>0.0761228114691587</v>
-      </c>
-      <c r="DV41" t="n">
-        <v>-0.926164136866484</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -36218,15 +35954,12 @@
         <v>-1.07526881720432</v>
       </c>
       <c r="DU42" t="n">
-        <v>-1.07166778298729</v>
-      </c>
-      <c r="DV42" t="n">
-        <v>-1.14401076716017</v>
+        <v>-1.20562625586069</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -36599,14 +36332,11 @@
       </c>
       <c r="DU43" t="n">
         <v>4.98511904761906</v>
-      </c>
-      <c r="DV43" t="n">
-        <v>5.47337278106509</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -36978,15 +36708,12 @@
         <v>1.71884591774097</v>
       </c>
       <c r="DU44" t="n">
-        <v>1.96560196560196</v>
-      </c>
-      <c r="DV44" t="n">
-        <v>2.02998126171143</v>
+        <v>1.93488943488944</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -37358,15 +37085,12 @@
         <v>2.73972602739726</v>
       </c>
       <c r="DU45" t="n">
-        <v>1.02739726027398</v>
-      </c>
-      <c r="DV45" t="n">
-        <v>2.75862068965516</v>
+        <v>0.684931506849313</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -37739,14 +37463,11 @@
       </c>
       <c r="DU46" t="n">
         <v>2.78121137206428</v>
-      </c>
-      <c r="DV46" t="n">
-        <v>-0.0621504039776223</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -38119,14 +37840,11 @@
       </c>
       <c r="DU47" t="n">
         <v>1.59574468085107</v>
-      </c>
-      <c r="DV47" t="n">
-        <v>1.8918918918919</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -38498,15 +38216,12 @@
         <v>0.920096852300231</v>
       </c>
       <c r="DU48" t="n">
-        <v>1.35527589545014</v>
-      </c>
-      <c r="DV48" t="n">
-        <v>1.29805292061907</v>
+        <v>1.21006776379477</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -38879,14 +38594,11 @@
       </c>
       <c r="DU49" t="n">
         <v>3.0778620629523</v>
-      </c>
-      <c r="DV49" t="n">
-        <v>3.07988450433107</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -39259,14 +38971,11 @@
       </c>
       <c r="DU50" t="n">
         <v>2.88461538461539</v>
-      </c>
-      <c r="DV50" t="n">
-        <v>3.04487179487179</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -39639,14 +39348,11 @@
       </c>
       <c r="DU51" t="n">
         <v>4.48717948717949</v>
-      </c>
-      <c r="DV51" t="n">
-        <v>-2.8846153846154</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -40018,15 +39724,12 @@
         <v>3.41962288271015</v>
       </c>
       <c r="DU52" t="n">
-        <v>2.92527821939586</v>
-      </c>
-      <c r="DV52" t="n">
-        <v>2.2121014964216</v>
+        <v>2.7980922098569</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -40398,15 +40101,12 @@
         <v>2.55993498577813</v>
       </c>
       <c r="DU53" t="n">
-        <v>2.23033252230333</v>
-      </c>
-      <c r="DV53" t="n">
-        <v>0.646464646464656</v>
+        <v>2.27088402270884</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -40779,14 +40479,11 @@
       </c>
       <c r="DU54" t="n">
         <v>1.13636363636363</v>
-      </c>
-      <c r="DV54" t="n">
-        <v>0.985221674876838</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -41158,15 +40855,12 @@
         <v>3.08731307284128</v>
       </c>
       <c r="DU55" t="n">
-        <v>2.88184438040346</v>
-      </c>
-      <c r="DV55" t="n">
-        <v>3.72549019607843</v>
+        <v>2.88184438040347</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -41538,10 +41232,7 @@
         <v>2.32558139534883</v>
       </c>
       <c r="DU56" t="n">
-        <v>2</v>
-      </c>
-      <c r="DV56" t="n">
-        <v>2.33333333333333</v>
+        <v>1.66666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on July, 21st 2023
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t xml:space="preserve">04/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1323,10 +1329,16 @@
       <c r="EG4" t="s">
         <v>136</v>
       </c>
+      <c r="EH4" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI4" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1731,15 +1743,21 @@
         <v>10787.5</v>
       </c>
       <c r="EF5" t="n">
-        <v>10819</v>
+        <v>10817.6</v>
       </c>
       <c r="EG5" t="n">
-        <v>10820.8</v>
+        <v>10826.6</v>
+      </c>
+      <c r="EH5" t="n">
+        <v>10719.1</v>
+      </c>
+      <c r="EI5" t="n">
+        <v>10154.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2147,12 +2165,18 @@
         <v>171.8</v>
       </c>
       <c r="EG6" t="n">
-        <v>171.7</v>
+        <v>171.6</v>
+      </c>
+      <c r="EH6" t="n">
+        <v>171.5</v>
+      </c>
+      <c r="EI6" t="n">
+        <v>169.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2561,11 +2585,17 @@
       </c>
       <c r="EG7" t="n">
         <v>29.1</v>
+      </c>
+      <c r="EH7" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="EI7" t="n">
+        <v>25.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2973,12 +3003,18 @@
         <v>197</v>
       </c>
       <c r="EG8" t="n">
-        <v>199.3</v>
+        <v>199.4</v>
+      </c>
+      <c r="EH8" t="n">
+        <v>193.5</v>
+      </c>
+      <c r="EI8" t="n">
+        <v>152.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3387,11 +3423,17 @@
       </c>
       <c r="EG9" t="n">
         <v>102.6</v>
+      </c>
+      <c r="EH9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="EI9" t="n">
+        <v>93.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3800,11 +3842,17 @@
       </c>
       <c r="EG10" t="n">
         <v>1248.8</v>
+      </c>
+      <c r="EH10" t="n">
+        <v>1255.9</v>
+      </c>
+      <c r="EI10" t="n">
+        <v>1233.3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4213,11 +4261,17 @@
       </c>
       <c r="EG11" t="n">
         <v>224.8</v>
+      </c>
+      <c r="EH11" t="n">
+        <v>225.6</v>
+      </c>
+      <c r="EI11" t="n">
+        <v>211.3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4625,12 +4679,18 @@
         <v>126.3</v>
       </c>
       <c r="EG12" t="n">
-        <v>124.7</v>
+        <v>124.8</v>
+      </c>
+      <c r="EH12" t="n">
+        <v>123</v>
+      </c>
+      <c r="EI12" t="n">
+        <v>113.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5038,12 +5098,18 @@
         <v>38.3</v>
       </c>
       <c r="EG13" t="n">
-        <v>38.8</v>
+        <v>38.2</v>
+      </c>
+      <c r="EH13" t="n">
+        <v>37.6</v>
+      </c>
+      <c r="EI13" t="n">
+        <v>35.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5181,10 +5247,12 @@
       <c r="EE14"/>
       <c r="EF14"/>
       <c r="EG14"/>
+      <c r="EH14"/>
+      <c r="EI14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5592,12 +5660,18 @@
         <v>489.1</v>
       </c>
       <c r="EG15" t="n">
-        <v>488.7</v>
+        <v>488.9</v>
+      </c>
+      <c r="EH15" t="n">
+        <v>480.4</v>
+      </c>
+      <c r="EI15" t="n">
+        <v>399.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6005,12 +6079,18 @@
         <v>347.2</v>
       </c>
       <c r="EG16" t="n">
-        <v>346.4</v>
+        <v>346.3</v>
+      </c>
+      <c r="EH16" t="n">
+        <v>342.7</v>
+      </c>
+      <c r="EI16" t="n">
+        <v>335.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6148,10 +6228,12 @@
       <c r="EE17"/>
       <c r="EF17"/>
       <c r="EG17"/>
+      <c r="EH17"/>
+      <c r="EI17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6560,11 +6642,17 @@
       </c>
       <c r="EG18" t="n">
         <v>66.5</v>
+      </c>
+      <c r="EH18" t="n">
+        <v>64.5</v>
+      </c>
+      <c r="EI18" t="n">
+        <v>60.9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6972,12 +7060,18 @@
         <v>446.1</v>
       </c>
       <c r="EG19" t="n">
-        <v>445.9</v>
+        <v>446</v>
+      </c>
+      <c r="EH19" t="n">
+        <v>445</v>
+      </c>
+      <c r="EI19" t="n">
+        <v>410.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7385,12 +7479,18 @@
         <v>229.6</v>
       </c>
       <c r="EG20" t="n">
-        <v>228.9</v>
+        <v>229</v>
+      </c>
+      <c r="EH20" t="n">
+        <v>229.5</v>
+      </c>
+      <c r="EI20" t="n">
+        <v>185.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7798,12 +7898,18 @@
         <v>145.7</v>
       </c>
       <c r="EG21" t="n">
-        <v>145.8</v>
+        <v>146.2</v>
+      </c>
+      <c r="EH21" t="n">
+        <v>145.4</v>
+      </c>
+      <c r="EI21" t="n">
+        <v>133.9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8211,12 +8317,18 @@
         <v>135.9</v>
       </c>
       <c r="EG22" t="n">
-        <v>135.4</v>
+        <v>135.6</v>
+      </c>
+      <c r="EH22" t="n">
+        <v>135.3</v>
+      </c>
+      <c r="EI22" t="n">
+        <v>120.2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8624,12 +8736,18 @@
         <v>161.4</v>
       </c>
       <c r="EG23" t="n">
-        <v>161.1</v>
+        <v>161</v>
+      </c>
+      <c r="EH23" t="n">
+        <v>160.7</v>
+      </c>
+      <c r="EI23" t="n">
+        <v>151.1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9037,12 +9155,18 @@
         <v>149.3</v>
       </c>
       <c r="EG24" t="n">
-        <v>150.4</v>
+        <v>150.3</v>
+      </c>
+      <c r="EH24" t="n">
+        <v>149</v>
+      </c>
+      <c r="EI24" t="n">
+        <v>138.9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9450,12 +9574,18 @@
         <v>50</v>
       </c>
       <c r="EG25" t="n">
-        <v>49.5</v>
+        <v>49.4</v>
+      </c>
+      <c r="EH25" t="n">
+        <v>49.7</v>
+      </c>
+      <c r="EI25" t="n">
+        <v>47.6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9864,11 +9994,17 @@
       </c>
       <c r="EG26" t="n">
         <v>225</v>
+      </c>
+      <c r="EH26" t="n">
+        <v>225.2</v>
+      </c>
+      <c r="EI26" t="n">
+        <v>209.7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10276,12 +10412,18 @@
         <v>245.9</v>
       </c>
       <c r="EG27" t="n">
-        <v>246.5</v>
+        <v>245.9</v>
+      </c>
+      <c r="EH27" t="n">
+        <v>245.1</v>
+      </c>
+      <c r="EI27" t="n">
+        <v>239.2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10689,12 +10831,18 @@
         <v>323.6</v>
       </c>
       <c r="EG28" t="n">
-        <v>323.9</v>
+        <v>324.6</v>
+      </c>
+      <c r="EH28" t="n">
+        <v>308.1</v>
+      </c>
+      <c r="EI28" t="n">
+        <v>291.9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11102,12 +11250,18 @@
         <v>205.6</v>
       </c>
       <c r="EG29" t="n">
-        <v>206</v>
+        <v>205.9</v>
+      </c>
+      <c r="EH29" t="n">
+        <v>203</v>
+      </c>
+      <c r="EI29" t="n">
+        <v>198.1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11516,11 +11670,17 @@
       </c>
       <c r="EG30" t="n">
         <v>103.5</v>
+      </c>
+      <c r="EH30" t="n">
+        <v>101.9</v>
+      </c>
+      <c r="EI30" t="n">
+        <v>98.6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11658,10 +11818,12 @@
       <c r="EE31"/>
       <c r="EF31"/>
       <c r="EG31"/>
+      <c r="EH31"/>
+      <c r="EI31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12069,12 +12231,18 @@
         <v>43.6</v>
       </c>
       <c r="EG32" t="n">
-        <v>43.5</v>
+        <v>43.6</v>
+      </c>
+      <c r="EH32" t="n">
+        <v>42.7</v>
+      </c>
+      <c r="EI32" t="n">
+        <v>39.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12483,11 +12651,17 @@
       </c>
       <c r="EG33" t="n">
         <v>94.7</v>
+      </c>
+      <c r="EH33" t="n">
+        <v>94.7</v>
+      </c>
+      <c r="EI33" t="n">
+        <v>91.1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -12896,11 +13070,17 @@
       </c>
       <c r="EG34" t="n">
         <v>83.6</v>
+      </c>
+      <c r="EH34" t="n">
+        <v>83.9</v>
+      </c>
+      <c r="EI34" t="n">
+        <v>76.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13308,12 +13488,18 @@
         <v>46</v>
       </c>
       <c r="EG35" t="n">
-        <v>46.3</v>
+        <v>46.4</v>
+      </c>
+      <c r="EH35" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="EI35" t="n">
+        <v>38.8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -13721,12 +13907,18 @@
         <v>312.1</v>
       </c>
       <c r="EG36" t="n">
-        <v>312.7</v>
+        <v>312.6</v>
+      </c>
+      <c r="EH36" t="n">
+        <v>310</v>
+      </c>
+      <c r="EI36" t="n">
+        <v>304.4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14135,11 +14327,17 @@
       </c>
       <c r="EG37" t="n">
         <v>77.7</v>
+      </c>
+      <c r="EH37" t="n">
+        <v>77.1</v>
+      </c>
+      <c r="EI37" t="n">
+        <v>72.7</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14547,12 +14745,18 @@
         <v>675.5</v>
       </c>
       <c r="EG38" t="n">
-        <v>676.4</v>
+        <v>676.1</v>
+      </c>
+      <c r="EH38" t="n">
+        <v>672.4</v>
+      </c>
+      <c r="EI38" t="n">
+        <v>661.3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -14961,11 +15165,17 @@
       </c>
       <c r="EG39" t="n">
         <v>332</v>
+      </c>
+      <c r="EH39" t="n">
+        <v>333.1</v>
+      </c>
+      <c r="EI39" t="n">
+        <v>293.8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15373,12 +15583,18 @@
         <v>38.1</v>
       </c>
       <c r="EG40" t="n">
-        <v>38</v>
+        <v>38.2</v>
+      </c>
+      <c r="EH40" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="EI40" t="n">
+        <v>32.5</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -15787,11 +16003,17 @@
       </c>
       <c r="EG41" t="n">
         <v>394.4</v>
+      </c>
+      <c r="EH41" t="n">
+        <v>385.3</v>
+      </c>
+      <c r="EI41" t="n">
+        <v>354.3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16199,12 +16421,18 @@
         <v>147.2</v>
       </c>
       <c r="EG42" t="n">
-        <v>147.5</v>
+        <v>147.7</v>
+      </c>
+      <c r="EH42" t="n">
+        <v>146.8</v>
+      </c>
+      <c r="EI42" t="n">
+        <v>133.6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -16613,11 +16841,17 @@
       </c>
       <c r="EG43" t="n">
         <v>141.1</v>
+      </c>
+      <c r="EH43" t="n">
+        <v>142.2</v>
+      </c>
+      <c r="EI43" t="n">
+        <v>142.1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17025,12 +17259,18 @@
         <v>331.4</v>
       </c>
       <c r="EG44" t="n">
-        <v>331.9</v>
+        <v>332</v>
+      </c>
+      <c r="EH44" t="n">
+        <v>326.7</v>
+      </c>
+      <c r="EI44" t="n">
+        <v>303.2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17438,12 +17678,18 @@
         <v>30</v>
       </c>
       <c r="EG45" t="n">
-        <v>29.4</v>
+        <v>29.5</v>
+      </c>
+      <c r="EH45" t="n">
+        <v>29.8</v>
+      </c>
+      <c r="EI45" t="n">
+        <v>27.5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -17852,11 +18098,17 @@
       </c>
       <c r="EG46" t="n">
         <v>166.3</v>
+      </c>
+      <c r="EH46" t="n">
+        <v>160.9</v>
+      </c>
+      <c r="EI46" t="n">
+        <v>155.5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18265,11 +18517,17 @@
       </c>
       <c r="EG47" t="n">
         <v>38.2</v>
+      </c>
+      <c r="EH47" t="n">
+        <v>37.7</v>
+      </c>
+      <c r="EI47" t="n">
+        <v>34.1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -18677,12 +18935,18 @@
         <v>208.4</v>
       </c>
       <c r="EG48" t="n">
-        <v>209.1</v>
+        <v>209.4</v>
+      </c>
+      <c r="EH48" t="n">
+        <v>205.8</v>
+      </c>
+      <c r="EI48" t="n">
+        <v>194</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -19091,11 +19355,17 @@
       </c>
       <c r="EG49" t="n">
         <v>1182.2</v>
+      </c>
+      <c r="EH49" t="n">
+        <v>1178.1</v>
+      </c>
+      <c r="EI49" t="n">
+        <v>1132.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -19504,11 +19774,17 @@
       </c>
       <c r="EG50" t="n">
         <v>128.4</v>
+      </c>
+      <c r="EH50" t="n">
+        <v>128.6</v>
+      </c>
+      <c r="EI50" t="n">
+        <v>119.4</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -19917,11 +20193,17 @@
       </c>
       <c r="EG51" t="n">
         <v>32.6</v>
+      </c>
+      <c r="EH51" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="EI51" t="n">
+        <v>29.3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20329,12 +20611,18 @@
         <v>323.6</v>
       </c>
       <c r="EG52" t="n">
-        <v>323.3</v>
+        <v>323.7</v>
+      </c>
+      <c r="EH52" t="n">
+        <v>313.6</v>
+      </c>
+      <c r="EI52" t="n">
+        <v>305.7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -20742,12 +21030,18 @@
         <v>252.4</v>
       </c>
       <c r="EG53" t="n">
-        <v>252.2</v>
+        <v>252.1</v>
+      </c>
+      <c r="EH53" t="n">
+        <v>252.7</v>
+      </c>
+      <c r="EI53" t="n">
+        <v>247.4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -21156,11 +21450,17 @@
       </c>
       <c r="EG54" t="n">
         <v>62.3</v>
+      </c>
+      <c r="EH54" t="n">
+        <v>61.6</v>
+      </c>
+      <c r="EI54" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -21569,11 +21869,17 @@
       </c>
       <c r="EG55" t="n">
         <v>214.2</v>
+      </c>
+      <c r="EH55" t="n">
+        <v>211.4</v>
+      </c>
+      <c r="EI55" t="n">
+        <v>191</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -21981,7 +22287,13 @@
         <v>30.8</v>
       </c>
       <c r="EG56" t="n">
-        <v>30.5</v>
+        <v>30.6</v>
+      </c>
+      <c r="EH56" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="EI56" t="n">
+        <v>28.2</v>
       </c>
     </row>
   </sheetData>
@@ -22374,10 +22686,16 @@
       <c r="DU4" t="s">
         <v>136</v>
       </c>
+      <c r="DV4" t="s">
+        <v>137</v>
+      </c>
+      <c r="DW4" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -22746,15 +23064,21 @@
         <v>2.45609702817959</v>
       </c>
       <c r="DT5" t="n">
-        <v>2.38090731873498</v>
+        <v>2.36765902681833</v>
       </c>
       <c r="DU5" t="n">
-        <v>2.21416156578251</v>
+        <v>2.26894884002117</v>
+      </c>
+      <c r="DV5" t="n">
+        <v>2.35180658467651</v>
+      </c>
+      <c r="DW5" t="n">
+        <v>2.82199270959904</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -23126,12 +23450,18 @@
         <v>2.20107079119571</v>
       </c>
       <c r="DU6" t="n">
-        <v>0.999999999999993</v>
+        <v>0.941176470588232</v>
+      </c>
+      <c r="DV6" t="n">
+        <v>0.823045267489698</v>
+      </c>
+      <c r="DW6" t="n">
+        <v>0.832342449464926</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -23504,11 +23834,17 @@
       </c>
       <c r="DU7" t="n">
         <v>4.67625899280576</v>
+      </c>
+      <c r="DV7" t="n">
+        <v>5.99250936329586</v>
+      </c>
+      <c r="DW7" t="n">
+        <v>14.5454545454546</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -23880,12 +24216,18 @@
         <v>0.767263427109974</v>
       </c>
       <c r="DU8" t="n">
-        <v>1.78753830439224</v>
+        <v>1.83861082737485</v>
+      </c>
+      <c r="DV8" t="n">
+        <v>1.94942044257112</v>
+      </c>
+      <c r="DW8" t="n">
+        <v>1.39906728847435</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -24258,11 +24600,17 @@
       </c>
       <c r="DU9" t="n">
         <v>0.686947988223738</v>
+      </c>
+      <c r="DV9" t="n">
+        <v>0.594059405940588</v>
+      </c>
+      <c r="DW9" t="n">
+        <v>0.755124056094948</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -24635,11 +24983,17 @@
       </c>
       <c r="DU10" t="n">
         <v>2.94287362954415</v>
+      </c>
+      <c r="DV10" t="n">
+        <v>2.75732286041565</v>
+      </c>
+      <c r="DW10" t="n">
+        <v>2.61253016057909</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -25012,11 +25366,17 @@
       </c>
       <c r="DU11" t="n">
         <v>2.93040293040293</v>
+      </c>
+      <c r="DV11" t="n">
+        <v>3.15500685871058</v>
+      </c>
+      <c r="DW11" t="n">
+        <v>3.3757338551859</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -25388,12 +25748,18 @@
         <v>1.5273311897106</v>
       </c>
       <c r="DU12" t="n">
-        <v>0.321802091713601</v>
+        <v>0.402252614641995</v>
+      </c>
+      <c r="DV12" t="n">
+        <v>0.408163265306122</v>
+      </c>
+      <c r="DW12" t="n">
+        <v>1.79372197309417</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -25765,12 +26131,18 @@
         <v>2.40641711229944</v>
       </c>
       <c r="DU13" t="n">
-        <v>2.64550264550265</v>
+        <v>1.05820105820107</v>
+      </c>
+      <c r="DV13" t="n">
+        <v>1.89701897018969</v>
+      </c>
+      <c r="DW13" t="n">
+        <v>2.00000000000001</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -25896,10 +26268,12 @@
       <c r="DS14"/>
       <c r="DT14"/>
       <c r="DU14"/>
+      <c r="DV14"/>
+      <c r="DW14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -26271,12 +26645,18 @@
         <v>1.85339441899209</v>
       </c>
       <c r="DU15" t="n">
-        <v>1.72772689425479</v>
+        <v>1.76935886761032</v>
+      </c>
+      <c r="DV15" t="n">
+        <v>1.50010564124233</v>
+      </c>
+      <c r="DW15" t="n">
+        <v>1.91473066122032</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -26648,12 +27028,18 @@
         <v>3.08788598574821</v>
       </c>
       <c r="DU16" t="n">
-        <v>2.85035629453681</v>
+        <v>2.82066508313539</v>
+      </c>
+      <c r="DV16" t="n">
+        <v>2.02441202738911</v>
+      </c>
+      <c r="DW16" t="n">
+        <v>3.45785736338377</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -26779,10 +27165,12 @@
       <c r="DS17"/>
       <c r="DT17"/>
       <c r="DU17"/>
+      <c r="DV17"/>
+      <c r="DW17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -27155,11 +27543,17 @@
       </c>
       <c r="DU18" t="n">
         <v>7.60517799352751</v>
+      </c>
+      <c r="DV18" t="n">
+        <v>5.73770491803279</v>
+      </c>
+      <c r="DW18" t="n">
+        <v>4.81927710843374</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -27531,12 +27925,18 @@
         <v>3.76831821353804</v>
       </c>
       <c r="DU19" t="n">
-        <v>3.8667598416026</v>
+        <v>3.89005357558816</v>
+      </c>
+      <c r="DV19" t="n">
+        <v>4.02057035998131</v>
+      </c>
+      <c r="DW19" t="n">
+        <v>4.1085467917829</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -27908,12 +28308,18 @@
         <v>2.18068535825547</v>
       </c>
       <c r="DU20" t="n">
-        <v>2.14190093708165</v>
+        <v>2.18652387327086</v>
+      </c>
+      <c r="DV20" t="n">
+        <v>2.27272727272727</v>
+      </c>
+      <c r="DW20" t="n">
+        <v>-3.0890052356021</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -28285,12 +28691,18 @@
         <v>2.24561403508771</v>
       </c>
       <c r="DU21" t="n">
-        <v>1.95804195804197</v>
+        <v>2.23776223776223</v>
+      </c>
+      <c r="DV21" t="n">
+        <v>1.89208128941837</v>
+      </c>
+      <c r="DW21" t="n">
+        <v>1.67046317388004</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -28662,12 +29074,18 @@
         <v>0.221238938053106</v>
       </c>
       <c r="DU22" t="n">
-        <v>-0.294550810014732</v>
+        <v>-0.147275405007376</v>
+      </c>
+      <c r="DV22" t="n">
+        <v>-0.147601476014773</v>
+      </c>
+      <c r="DW22" t="n">
+        <v>-0.331674958540623</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -29039,12 +29457,18 @@
         <v>1.31826741996233</v>
       </c>
       <c r="DU23" t="n">
-        <v>1.76879343019582</v>
+        <v>1.70562223626026</v>
+      </c>
+      <c r="DV23" t="n">
+        <v>1.64452877925363</v>
+      </c>
+      <c r="DW23" t="n">
+        <v>1.75084175084175</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -29416,12 +29840,18 @@
         <v>3.39335180055402</v>
       </c>
       <c r="DU24" t="n">
-        <v>3.36769759450172</v>
+        <v>3.29896907216496</v>
+      </c>
+      <c r="DV24" t="n">
+        <v>2.40549828178694</v>
+      </c>
+      <c r="DW24" t="n">
+        <v>3.19465081723624</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -29793,12 +30223,18 @@
         <v>0.200400801603209</v>
       </c>
       <c r="DU25" t="n">
-        <v>-1.19760479041916</v>
+        <v>-1.39720558882235</v>
+      </c>
+      <c r="DV25" t="n">
+        <v>1.22199592668026</v>
+      </c>
+      <c r="DW25" t="n">
+        <v>0.421940928270033</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -30171,11 +30607,17 @@
       </c>
       <c r="DU26" t="n">
         <v>3.3532384014699</v>
+      </c>
+      <c r="DV26" t="n">
+        <v>3.01921317474838</v>
+      </c>
+      <c r="DW26" t="n">
+        <v>2.04379562043796</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -30547,12 +30989,18 @@
         <v>3.44972654606645</v>
       </c>
       <c r="DU27" t="n">
-        <v>3.31098072087174</v>
+        <v>3.05951383067894</v>
+      </c>
+      <c r="DV27" t="n">
+        <v>2.50941028858217</v>
+      </c>
+      <c r="DW27" t="n">
+        <v>2.22222222222222</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -30924,12 +31372,18 @@
         <v>6.27257799671594</v>
       </c>
       <c r="DU28" t="n">
-        <v>5.84967320261437</v>
+        <v>6.07843137254903</v>
+      </c>
+      <c r="DV28" t="n">
+        <v>6.24137931034484</v>
+      </c>
+      <c r="DW28" t="n">
+        <v>5.6842867487328</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -31301,12 +31755,18 @@
         <v>0.636319138521787</v>
       </c>
       <c r="DU29" t="n">
-        <v>0.340964442279585</v>
+        <v>0.292255236239646</v>
+      </c>
+      <c r="DV29" t="n">
+        <v>0.644521566683198</v>
+      </c>
+      <c r="DW29" t="n">
+        <v>1.27811860940695</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -31679,11 +32139,17 @@
       </c>
       <c r="DU30" t="n">
         <v>1.07421874999999</v>
+      </c>
+      <c r="DV30" t="n">
+        <v>1.09126984126985</v>
+      </c>
+      <c r="DW30" t="n">
+        <v>1.54479917610711</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -31809,10 +32275,12 @@
       <c r="DS31"/>
       <c r="DT31"/>
       <c r="DU31"/>
+      <c r="DV31"/>
+      <c r="DW31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -32184,12 +32652,18 @@
         <v>-1.35746606334842</v>
       </c>
       <c r="DU32" t="n">
-        <v>-1.58371040723983</v>
+        <v>-1.35746606334842</v>
+      </c>
+      <c r="DV32" t="n">
+        <v>-4.26008968609865</v>
+      </c>
+      <c r="DW32" t="n">
+        <v>-6.9047619047619</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -32562,11 +33036,17 @@
       </c>
       <c r="DU33" t="n">
         <v>1.28342245989305</v>
+      </c>
+      <c r="DV33" t="n">
+        <v>1.39186295503212</v>
+      </c>
+      <c r="DW33" t="n">
+        <v>3.6405005688282</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -32939,11 +33419,17 @@
       </c>
       <c r="DU34" t="n">
         <v>4.36953807740325</v>
+      </c>
+      <c r="DV34" t="n">
+        <v>4.74406991260925</v>
+      </c>
+      <c r="DW34" t="n">
+        <v>7.74647887323944</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -33315,12 +33801,18 @@
         <v>0</v>
       </c>
       <c r="DU35" t="n">
-        <v>0.216450216450204</v>
+        <v>0.432900432900424</v>
+      </c>
+      <c r="DV35" t="n">
+        <v>0.886917960088689</v>
+      </c>
+      <c r="DW35" t="n">
+        <v>-0.51282051282052</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -33692,12 +34184,18 @@
         <v>1.06865284974094</v>
       </c>
       <c r="DU36" t="n">
-        <v>0.838439213157053</v>
+        <v>0.806191551112544</v>
+      </c>
+      <c r="DV36" t="n">
+        <v>1.57273918741809</v>
+      </c>
+      <c r="DW36" t="n">
+        <v>0.99535500995355</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -34070,11 +34568,17 @@
       </c>
       <c r="DU37" t="n">
         <v>2.50659630606861</v>
+      </c>
+      <c r="DV37" t="n">
+        <v>3.35120643431635</v>
+      </c>
+      <c r="DW37" t="n">
+        <v>14.3081761006289</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -34446,12 +34950,18 @@
         <v>3.35067319461444</v>
       </c>
       <c r="DU38" t="n">
-        <v>3.56760067370999</v>
+        <v>3.52166590108712</v>
+      </c>
+      <c r="DV38" t="n">
+        <v>3.49392027089425</v>
+      </c>
+      <c r="DW38" t="n">
+        <v>3.57086922474551</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -34824,11 +35334,17 @@
       </c>
       <c r="DU39" t="n">
         <v>0.850546780072908</v>
+      </c>
+      <c r="DV39" t="n">
+        <v>0.725733293014827</v>
+      </c>
+      <c r="DW39" t="n">
+        <v>0.789022298456265</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -35200,12 +35716,18 @@
         <v>0.263157894736846</v>
       </c>
       <c r="DU40" t="n">
-        <v>0.795755968169754</v>
+        <v>1.3262599469496</v>
+      </c>
+      <c r="DV40" t="n">
+        <v>0.530503978779829</v>
+      </c>
+      <c r="DW40" t="n">
+        <v>-2.40240240240239</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -35578,11 +36100,17 @@
       </c>
       <c r="DU41" t="n">
         <v>0.0761228114691587</v>
+      </c>
+      <c r="DV41" t="n">
+        <v>-0.874710573707223</v>
+      </c>
+      <c r="DW41" t="n">
+        <v>-0.393590104020251</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -35954,12 +36482,18 @@
         <v>-1.07526881720432</v>
       </c>
       <c r="DU42" t="n">
-        <v>-1.20562625586069</v>
+        <v>-1.07166778298729</v>
+      </c>
+      <c r="DV42" t="n">
+        <v>-1.21130551816957</v>
+      </c>
+      <c r="DW42" t="n">
+        <v>0.830188679245279</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -36332,11 +36866,17 @@
       </c>
       <c r="DU43" t="n">
         <v>4.98511904761906</v>
+      </c>
+      <c r="DV43" t="n">
+        <v>5.17751479289943</v>
+      </c>
+      <c r="DW43" t="n">
+        <v>7.57002271006813</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -36708,12 +37248,18 @@
         <v>1.71884591774097</v>
       </c>
       <c r="DU44" t="n">
-        <v>1.93488943488944</v>
+        <v>1.96560196560196</v>
+      </c>
+      <c r="DV44" t="n">
+        <v>2.02998126171143</v>
+      </c>
+      <c r="DW44" t="n">
+        <v>1.40468227424749</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -37085,12 +37631,18 @@
         <v>2.73972602739726</v>
       </c>
       <c r="DU45" t="n">
-        <v>0.684931506849313</v>
+        <v>1.02739726027398</v>
+      </c>
+      <c r="DV45" t="n">
+        <v>2.75862068965516</v>
+      </c>
+      <c r="DW45" t="n">
+        <v>2.23048327137547</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -37463,11 +38015,17 @@
       </c>
       <c r="DU46" t="n">
         <v>2.78121137206428</v>
+      </c>
+      <c r="DV46" t="n">
+        <v>0</v>
+      </c>
+      <c r="DW46" t="n">
+        <v>0.0643500643500607</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -37840,11 +38398,17 @@
       </c>
       <c r="DU47" t="n">
         <v>1.59574468085107</v>
+      </c>
+      <c r="DV47" t="n">
+        <v>1.8918918918919</v>
+      </c>
+      <c r="DW47" t="n">
+        <v>2.40240240240242</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -38216,12 +38780,18 @@
         <v>0.920096852300231</v>
       </c>
       <c r="DU48" t="n">
-        <v>1.21006776379477</v>
+        <v>1.35527589545014</v>
+      </c>
+      <c r="DV48" t="n">
+        <v>2.74588117823265</v>
+      </c>
+      <c r="DW48" t="n">
+        <v>1.2526096033403</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -38594,11 +39164,17 @@
       </c>
       <c r="DU49" t="n">
         <v>3.0778620629523</v>
+      </c>
+      <c r="DV49" t="n">
+        <v>3.07988450433107</v>
+      </c>
+      <c r="DW49" t="n">
+        <v>2.24729241877257</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -38971,11 +39547,17 @@
       </c>
       <c r="DU50" t="n">
         <v>2.88461538461539</v>
+      </c>
+      <c r="DV50" t="n">
+        <v>3.04487179487179</v>
+      </c>
+      <c r="DW50" t="n">
+        <v>3.10880829015544</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -39348,11 +39930,17 @@
       </c>
       <c r="DU51" t="n">
         <v>4.48717948717949</v>
+      </c>
+      <c r="DV51" t="n">
+        <v>-5.12820512820513</v>
+      </c>
+      <c r="DW51" t="n">
+        <v>7.72058823529411</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -39724,12 +40312,18 @@
         <v>3.41962288271015</v>
       </c>
       <c r="DU52" t="n">
-        <v>2.7980922098569</v>
+        <v>2.92527821939586</v>
+      </c>
+      <c r="DV52" t="n">
+        <v>2.01691607026677</v>
+      </c>
+      <c r="DW52" t="n">
+        <v>2.24080267558528</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -40101,12 +40695,18 @@
         <v>2.55993498577813</v>
       </c>
       <c r="DU53" t="n">
-        <v>2.27088402270884</v>
+        <v>2.23033252230333</v>
+      </c>
+      <c r="DV53" t="n">
+        <v>2.10101010101011</v>
+      </c>
+      <c r="DW53" t="n">
+        <v>2.48550124275062</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -40479,11 +41079,17 @@
       </c>
       <c r="DU54" t="n">
         <v>1.13636363636363</v>
+      </c>
+      <c r="DV54" t="n">
+        <v>1.14942528735631</v>
+      </c>
+      <c r="DW54" t="n">
+        <v>-0.17825311942958</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -40855,12 +41461,18 @@
         <v>3.08731307284128</v>
       </c>
       <c r="DU55" t="n">
-        <v>2.88184438040347</v>
+        <v>2.88184438040346</v>
+      </c>
+      <c r="DV55" t="n">
+        <v>3.62745098039216</v>
+      </c>
+      <c r="DW55" t="n">
+        <v>2.46781115879828</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -41232,7 +41844,13 @@
         <v>2.32558139534883</v>
       </c>
       <c r="DU56" t="n">
-        <v>1.66666666666667</v>
+        <v>2</v>
+      </c>
+      <c r="DV56" t="n">
+        <v>2.33333333333333</v>
+      </c>
+      <c r="DW56" t="n">
+        <v>3.2967032967033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on August 18
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -424,6 +424,15 @@
   </si>
   <si>
     <t xml:space="preserve">04/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1323,10 +1332,19 @@
       <c r="EG4" t="s">
         <v>136</v>
       </c>
+      <c r="EH4" t="s">
+        <v>137</v>
+      </c>
+      <c r="EI4" t="s">
+        <v>138</v>
+      </c>
+      <c r="EJ4" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1731,15 +1749,24 @@
         <v>10787.5</v>
       </c>
       <c r="EF5" t="n">
-        <v>10819</v>
+        <v>10817.6</v>
       </c>
       <c r="EG5" t="n">
-        <v>10820.8</v>
+        <v>10826.6</v>
+      </c>
+      <c r="EH5" t="n">
+        <v>10720.3</v>
+      </c>
+      <c r="EI5" t="n">
+        <v>10139.8</v>
+      </c>
+      <c r="EJ5" t="n">
+        <v>9046.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2147,12 +2174,21 @@
         <v>171.8</v>
       </c>
       <c r="EG6" t="n">
-        <v>171.7</v>
+        <v>171.6</v>
+      </c>
+      <c r="EH6" t="n">
+        <v>171.5</v>
+      </c>
+      <c r="EI6" t="n">
+        <v>169.2</v>
+      </c>
+      <c r="EJ6" t="n">
+        <v>160.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2561,11 +2597,20 @@
       </c>
       <c r="EG7" t="n">
         <v>29.1</v>
+      </c>
+      <c r="EH7" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="EI7" t="n">
+        <v>22.9</v>
+      </c>
+      <c r="EJ7" t="n">
+        <v>19.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -2973,12 +3018,21 @@
         <v>197</v>
       </c>
       <c r="EG8" t="n">
-        <v>199.3</v>
+        <v>199.4</v>
+      </c>
+      <c r="EH8" t="n">
+        <v>193.5</v>
+      </c>
+      <c r="EI8" t="n">
+        <v>152.7</v>
+      </c>
+      <c r="EJ8" t="n">
+        <v>151.9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3387,11 +3441,20 @@
       </c>
       <c r="EG9" t="n">
         <v>102.6</v>
+      </c>
+      <c r="EH9" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="EI9" t="n">
+        <v>93.4</v>
+      </c>
+      <c r="EJ9" t="n">
+        <v>82.2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3800,11 +3863,20 @@
       </c>
       <c r="EG10" t="n">
         <v>1248.8</v>
+      </c>
+      <c r="EH10" t="n">
+        <v>1255.9</v>
+      </c>
+      <c r="EI10" t="n">
+        <v>1234.6</v>
+      </c>
+      <c r="EJ10" t="n">
+        <v>1074.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4213,11 +4285,20 @@
       </c>
       <c r="EG11" t="n">
         <v>224.8</v>
+      </c>
+      <c r="EH11" t="n">
+        <v>225.6</v>
+      </c>
+      <c r="EI11" t="n">
+        <v>211.2</v>
+      </c>
+      <c r="EJ11" t="n">
+        <v>197</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4625,12 +4706,21 @@
         <v>126.3</v>
       </c>
       <c r="EG12" t="n">
-        <v>124.7</v>
+        <v>124.8</v>
+      </c>
+      <c r="EH12" t="n">
+        <v>123</v>
+      </c>
+      <c r="EI12" t="n">
+        <v>114.2</v>
+      </c>
+      <c r="EJ12" t="n">
+        <v>96.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5038,12 +5128,21 @@
         <v>38.3</v>
       </c>
       <c r="EG13" t="n">
-        <v>38.8</v>
+        <v>38.2</v>
+      </c>
+      <c r="EH13" t="n">
+        <v>37.6</v>
+      </c>
+      <c r="EI13" t="n">
+        <v>35.2</v>
+      </c>
+      <c r="EJ13" t="n">
+        <v>34.1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5181,10 +5280,13 @@
       <c r="EE14"/>
       <c r="EF14"/>
       <c r="EG14"/>
+      <c r="EH14"/>
+      <c r="EI14"/>
+      <c r="EJ14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5592,12 +5694,21 @@
         <v>489.1</v>
       </c>
       <c r="EG15" t="n">
-        <v>488.7</v>
+        <v>488.9</v>
+      </c>
+      <c r="EH15" t="n">
+        <v>480.4</v>
+      </c>
+      <c r="EI15" t="n">
+        <v>399.2</v>
+      </c>
+      <c r="EJ15" t="n">
+        <v>393</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6005,12 +6116,21 @@
         <v>347.2</v>
       </c>
       <c r="EG16" t="n">
-        <v>346.4</v>
+        <v>346.3</v>
+      </c>
+      <c r="EH16" t="n">
+        <v>342.7</v>
+      </c>
+      <c r="EI16" t="n">
+        <v>335.3</v>
+      </c>
+      <c r="EJ16" t="n">
+        <v>320</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6148,10 +6268,13 @@
       <c r="EE17"/>
       <c r="EF17"/>
       <c r="EG17"/>
+      <c r="EH17"/>
+      <c r="EI17"/>
+      <c r="EJ17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6560,11 +6683,20 @@
       </c>
       <c r="EG18" t="n">
         <v>66.5</v>
+      </c>
+      <c r="EH18" t="n">
+        <v>64.5</v>
+      </c>
+      <c r="EI18" t="n">
+        <v>61.4</v>
+      </c>
+      <c r="EJ18" t="n">
+        <v>54.9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -6972,12 +7104,21 @@
         <v>446.1</v>
       </c>
       <c r="EG19" t="n">
-        <v>445.9</v>
+        <v>446</v>
+      </c>
+      <c r="EH19" t="n">
+        <v>445</v>
+      </c>
+      <c r="EI19" t="n">
+        <v>408.7</v>
+      </c>
+      <c r="EJ19" t="n">
+        <v>380.6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7385,12 +7526,21 @@
         <v>229.6</v>
       </c>
       <c r="EG20" t="n">
-        <v>228.9</v>
+        <v>229</v>
+      </c>
+      <c r="EH20" t="n">
+        <v>229.5</v>
+      </c>
+      <c r="EI20" t="n">
+        <v>185.5</v>
+      </c>
+      <c r="EJ20" t="n">
+        <v>167.8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7798,12 +7948,21 @@
         <v>145.7</v>
       </c>
       <c r="EG21" t="n">
-        <v>145.8</v>
+        <v>146.2</v>
+      </c>
+      <c r="EH21" t="n">
+        <v>145.4</v>
+      </c>
+      <c r="EI21" t="n">
+        <v>132.2</v>
+      </c>
+      <c r="EJ21" t="n">
+        <v>114.6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8211,12 +8370,21 @@
         <v>135.9</v>
       </c>
       <c r="EG22" t="n">
-        <v>135.4</v>
+        <v>135.6</v>
+      </c>
+      <c r="EH22" t="n">
+        <v>135.3</v>
+      </c>
+      <c r="EI22" t="n">
+        <v>119.9</v>
+      </c>
+      <c r="EJ22" t="n">
+        <v>102.6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8624,12 +8792,21 @@
         <v>161.4</v>
       </c>
       <c r="EG23" t="n">
-        <v>161.1</v>
+        <v>161</v>
+      </c>
+      <c r="EH23" t="n">
+        <v>160.7</v>
+      </c>
+      <c r="EI23" t="n">
+        <v>151.1</v>
+      </c>
+      <c r="EJ23" t="n">
+        <v>126.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9037,12 +9214,21 @@
         <v>149.3</v>
       </c>
       <c r="EG24" t="n">
-        <v>150.4</v>
+        <v>150.3</v>
+      </c>
+      <c r="EH24" t="n">
+        <v>149</v>
+      </c>
+      <c r="EI24" t="n">
+        <v>139.1</v>
+      </c>
+      <c r="EJ24" t="n">
+        <v>131.9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9450,12 +9636,21 @@
         <v>50</v>
       </c>
       <c r="EG25" t="n">
-        <v>49.5</v>
+        <v>49.4</v>
+      </c>
+      <c r="EH25" t="n">
+        <v>49.7</v>
+      </c>
+      <c r="EI25" t="n">
+        <v>47.7</v>
+      </c>
+      <c r="EJ25" t="n">
+        <v>40.7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -9864,11 +10059,20 @@
       </c>
       <c r="EG26" t="n">
         <v>225</v>
+      </c>
+      <c r="EH26" t="n">
+        <v>225.2</v>
+      </c>
+      <c r="EI26" t="n">
+        <v>209.7</v>
+      </c>
+      <c r="EJ26" t="n">
+        <v>196.1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10276,12 +10480,21 @@
         <v>245.9</v>
       </c>
       <c r="EG27" t="n">
-        <v>246.5</v>
+        <v>245.9</v>
+      </c>
+      <c r="EH27" t="n">
+        <v>245.1</v>
+      </c>
+      <c r="EI27" t="n">
+        <v>239.7</v>
+      </c>
+      <c r="EJ27" t="n">
+        <v>212.6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10689,12 +10902,21 @@
         <v>323.6</v>
       </c>
       <c r="EG28" t="n">
-        <v>323.9</v>
+        <v>324.6</v>
+      </c>
+      <c r="EH28" t="n">
+        <v>308.1</v>
+      </c>
+      <c r="EI28" t="n">
+        <v>291.9</v>
+      </c>
+      <c r="EJ28" t="n">
+        <v>263.6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11102,12 +11324,21 @@
         <v>205.6</v>
       </c>
       <c r="EG29" t="n">
-        <v>206</v>
+        <v>205.9</v>
+      </c>
+      <c r="EH29" t="n">
+        <v>203</v>
+      </c>
+      <c r="EI29" t="n">
+        <v>197.7</v>
+      </c>
+      <c r="EJ29" t="n">
+        <v>167.5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11516,11 +11747,20 @@
       </c>
       <c r="EG30" t="n">
         <v>103.5</v>
+      </c>
+      <c r="EH30" t="n">
+        <v>101.9</v>
+      </c>
+      <c r="EI30" t="n">
+        <v>98.7</v>
+      </c>
+      <c r="EJ30" t="n">
+        <v>93.3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11658,10 +11898,13 @@
       <c r="EE31"/>
       <c r="EF31"/>
       <c r="EG31"/>
+      <c r="EH31"/>
+      <c r="EI31"/>
+      <c r="EJ31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12069,12 +12312,21 @@
         <v>43.6</v>
       </c>
       <c r="EG32" t="n">
-        <v>43.5</v>
+        <v>43.6</v>
+      </c>
+      <c r="EH32" t="n">
+        <v>42.7</v>
+      </c>
+      <c r="EI32" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="EJ32" t="n">
+        <v>32.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12483,11 +12735,20 @@
       </c>
       <c r="EG33" t="n">
         <v>94.7</v>
+      </c>
+      <c r="EH33" t="n">
+        <v>94.7</v>
+      </c>
+      <c r="EI33" t="n">
+        <v>90.5</v>
+      </c>
+      <c r="EJ33" t="n">
+        <v>78.7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -12896,11 +13157,20 @@
       </c>
       <c r="EG34" t="n">
         <v>83.6</v>
+      </c>
+      <c r="EH34" t="n">
+        <v>83.9</v>
+      </c>
+      <c r="EI34" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="EJ34" t="n">
+        <v>70.6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13308,12 +13578,21 @@
         <v>46</v>
       </c>
       <c r="EG35" t="n">
-        <v>46.3</v>
+        <v>46.4</v>
+      </c>
+      <c r="EH35" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="EI35" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="EJ35" t="n">
+        <v>32.3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -13721,12 +14000,21 @@
         <v>312.1</v>
       </c>
       <c r="EG36" t="n">
-        <v>312.7</v>
+        <v>312.6</v>
+      </c>
+      <c r="EH36" t="n">
+        <v>310</v>
+      </c>
+      <c r="EI36" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="EJ36" t="n">
+        <v>257.1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14135,11 +14423,20 @@
       </c>
       <c r="EG37" t="n">
         <v>77.7</v>
+      </c>
+      <c r="EH37" t="n">
+        <v>77.1</v>
+      </c>
+      <c r="EI37" t="n">
+        <v>71</v>
+      </c>
+      <c r="EJ37" t="n">
+        <v>65.3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14547,12 +14844,21 @@
         <v>675.5</v>
       </c>
       <c r="EG38" t="n">
-        <v>676.4</v>
+        <v>676.1</v>
+      </c>
+      <c r="EH38" t="n">
+        <v>672.4</v>
+      </c>
+      <c r="EI38" t="n">
+        <v>659.8</v>
+      </c>
+      <c r="EJ38" t="n">
+        <v>538.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -14961,11 +15267,20 @@
       </c>
       <c r="EG39" t="n">
         <v>332</v>
+      </c>
+      <c r="EH39" t="n">
+        <v>333.1</v>
+      </c>
+      <c r="EI39" t="n">
+        <v>293.8</v>
+      </c>
+      <c r="EJ39" t="n">
+        <v>237.3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15373,12 +15688,21 @@
         <v>38.1</v>
       </c>
       <c r="EG40" t="n">
-        <v>38</v>
+        <v>38.2</v>
+      </c>
+      <c r="EH40" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="EI40" t="n">
+        <v>32.4</v>
+      </c>
+      <c r="EJ40" t="n">
+        <v>26.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -15787,11 +16111,20 @@
       </c>
       <c r="EG41" t="n">
         <v>394.4</v>
+      </c>
+      <c r="EH41" t="n">
+        <v>385.3</v>
+      </c>
+      <c r="EI41" t="n">
+        <v>357.7</v>
+      </c>
+      <c r="EJ41" t="n">
+        <v>348.9</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16199,12 +16532,21 @@
         <v>147.2</v>
       </c>
       <c r="EG42" t="n">
-        <v>147.5</v>
+        <v>147.7</v>
+      </c>
+      <c r="EH42" t="n">
+        <v>146.8</v>
+      </c>
+      <c r="EI42" t="n">
+        <v>134.8</v>
+      </c>
+      <c r="EJ42" t="n">
+        <v>125.6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -16613,11 +16955,20 @@
       </c>
       <c r="EG43" t="n">
         <v>141.1</v>
+      </c>
+      <c r="EH43" t="n">
+        <v>142.2</v>
+      </c>
+      <c r="EI43" t="n">
+        <v>141.6</v>
+      </c>
+      <c r="EJ43" t="n">
+        <v>111.3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17025,12 +17376,21 @@
         <v>331.4</v>
       </c>
       <c r="EG44" t="n">
-        <v>331.9</v>
+        <v>332</v>
+      </c>
+      <c r="EH44" t="n">
+        <v>326.7</v>
+      </c>
+      <c r="EI44" t="n">
+        <v>302.2</v>
+      </c>
+      <c r="EJ44" t="n">
+        <v>271.3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17438,12 +17798,21 @@
         <v>30</v>
       </c>
       <c r="EG45" t="n">
-        <v>29.4</v>
+        <v>29.5</v>
+      </c>
+      <c r="EH45" t="n">
+        <v>29.8</v>
+      </c>
+      <c r="EI45" t="n">
+        <v>27.3</v>
+      </c>
+      <c r="EJ45" t="n">
+        <v>22.9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -17852,11 +18221,20 @@
       </c>
       <c r="EG46" t="n">
         <v>166.3</v>
+      </c>
+      <c r="EH46" t="n">
+        <v>160.9</v>
+      </c>
+      <c r="EI46" t="n">
+        <v>155.8</v>
+      </c>
+      <c r="EJ46" t="n">
+        <v>147.1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18265,11 +18643,20 @@
       </c>
       <c r="EG47" t="n">
         <v>38.2</v>
+      </c>
+      <c r="EH47" t="n">
+        <v>37.7</v>
+      </c>
+      <c r="EI47" t="n">
+        <v>34</v>
+      </c>
+      <c r="EJ47" t="n">
+        <v>28.4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -18677,12 +19064,21 @@
         <v>208.4</v>
       </c>
       <c r="EG48" t="n">
-        <v>209.1</v>
+        <v>209.4</v>
+      </c>
+      <c r="EH48" t="n">
+        <v>205.8</v>
+      </c>
+      <c r="EI48" t="n">
+        <v>192.8</v>
+      </c>
+      <c r="EJ48" t="n">
+        <v>168.2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -19091,11 +19487,20 @@
       </c>
       <c r="EG49" t="n">
         <v>1182.2</v>
+      </c>
+      <c r="EH49" t="n">
+        <v>1178.1</v>
+      </c>
+      <c r="EI49" t="n">
+        <v>1133.6</v>
+      </c>
+      <c r="EJ49" t="n">
+        <v>1061</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -19504,11 +19909,20 @@
       </c>
       <c r="EG50" t="n">
         <v>128.4</v>
+      </c>
+      <c r="EH50" t="n">
+        <v>128.6</v>
+      </c>
+      <c r="EI50" t="n">
+        <v>119.4</v>
+      </c>
+      <c r="EJ50" t="n">
+        <v>107.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -19917,11 +20331,20 @@
       </c>
       <c r="EG51" t="n">
         <v>32.6</v>
+      </c>
+      <c r="EH51" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="EI51" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="EJ51" t="n">
+        <v>26.1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20329,12 +20752,21 @@
         <v>323.6</v>
       </c>
       <c r="EG52" t="n">
-        <v>323.3</v>
+        <v>323.7</v>
+      </c>
+      <c r="EH52" t="n">
+        <v>313.6</v>
+      </c>
+      <c r="EI52" t="n">
+        <v>305.8</v>
+      </c>
+      <c r="EJ52" t="n">
+        <v>273.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -20742,12 +21174,21 @@
         <v>252.4</v>
       </c>
       <c r="EG53" t="n">
-        <v>252.2</v>
+        <v>252.1</v>
+      </c>
+      <c r="EH53" t="n">
+        <v>252.7</v>
+      </c>
+      <c r="EI53" t="n">
+        <v>249.5</v>
+      </c>
+      <c r="EJ53" t="n">
+        <v>230.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -21156,11 +21597,20 @@
       </c>
       <c r="EG54" t="n">
         <v>62.3</v>
+      </c>
+      <c r="EH54" t="n">
+        <v>61.6</v>
+      </c>
+      <c r="EI54" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="EJ54" t="n">
+        <v>51.7</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -21569,11 +22019,20 @@
       </c>
       <c r="EG55" t="n">
         <v>214.2</v>
+      </c>
+      <c r="EH55" t="n">
+        <v>211.4</v>
+      </c>
+      <c r="EI55" t="n">
+        <v>189.7</v>
+      </c>
+      <c r="EJ55" t="n">
+        <v>168.1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -21981,7 +22440,16 @@
         <v>30.8</v>
       </c>
       <c r="EG56" t="n">
-        <v>30.5</v>
+        <v>30.6</v>
+      </c>
+      <c r="EH56" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="EI56" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="EJ56" t="n">
+        <v>24.1</v>
       </c>
     </row>
   </sheetData>
@@ -22374,10 +22842,19 @@
       <c r="DU4" t="s">
         <v>136</v>
       </c>
+      <c r="DV4" t="s">
+        <v>137</v>
+      </c>
+      <c r="DW4" t="s">
+        <v>138</v>
+      </c>
+      <c r="DX4" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -22746,15 +23223,24 @@
         <v>2.45609702817959</v>
       </c>
       <c r="DT5" t="n">
-        <v>2.38090731873498</v>
+        <v>2.36765902681833</v>
       </c>
       <c r="DU5" t="n">
-        <v>2.21416156578251</v>
+        <v>2.26894884002117</v>
+      </c>
+      <c r="DV5" t="n">
+        <v>2.36326483843862</v>
+      </c>
+      <c r="DW5" t="n">
+        <v>2.67112191170514</v>
+      </c>
+      <c r="DX5" t="n">
+        <v>1.785573645068</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -23126,12 +23612,21 @@
         <v>2.20107079119571</v>
       </c>
       <c r="DU6" t="n">
-        <v>0.999999999999993</v>
+        <v>0.941176470588232</v>
+      </c>
+      <c r="DV6" t="n">
+        <v>0.823045267489698</v>
+      </c>
+      <c r="DW6" t="n">
+        <v>0.594530321046373</v>
+      </c>
+      <c r="DX6" t="n">
+        <v>0.06222775357811</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -23504,11 +23999,20 @@
       </c>
       <c r="DU7" t="n">
         <v>4.67625899280576</v>
+      </c>
+      <c r="DV7" t="n">
+        <v>5.99250936329586</v>
+      </c>
+      <c r="DW7" t="n">
+        <v>4.09090909090908</v>
+      </c>
+      <c r="DX7" t="n">
+        <v>2.11640211640213</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -23880,12 +24384,21 @@
         <v>0.767263427109974</v>
       </c>
       <c r="DU8" t="n">
-        <v>1.78753830439224</v>
+        <v>1.83861082737485</v>
+      </c>
+      <c r="DV8" t="n">
+        <v>1.94942044257112</v>
+      </c>
+      <c r="DW8" t="n">
+        <v>1.73217854763491</v>
+      </c>
+      <c r="DX8" t="n">
+        <v>3.47411444141689</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -24258,11 +24771,20 @@
       </c>
       <c r="DU9" t="n">
         <v>0.686947988223738</v>
+      </c>
+      <c r="DV9" t="n">
+        <v>0.594059405940588</v>
+      </c>
+      <c r="DW9" t="n">
+        <v>0.755124056094948</v>
+      </c>
+      <c r="DX9" t="n">
+        <v>0.611995104039185</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -24635,11 +25157,20 @@
       </c>
       <c r="DU10" t="n">
         <v>2.94287362954415</v>
+      </c>
+      <c r="DV10" t="n">
+        <v>2.75732286041565</v>
+      </c>
+      <c r="DW10" t="n">
+        <v>2.72069223729094</v>
+      </c>
+      <c r="DX10" t="n">
+        <v>3.08932169241102</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -25012,11 +25543,20 @@
       </c>
       <c r="DU11" t="n">
         <v>2.93040293040293</v>
+      </c>
+      <c r="DV11" t="n">
+        <v>3.15500685871058</v>
+      </c>
+      <c r="DW11" t="n">
+        <v>3.32681017612524</v>
+      </c>
+      <c r="DX11" t="n">
+        <v>5.74342458400429</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -25388,12 +25928,21 @@
         <v>1.5273311897106</v>
       </c>
       <c r="DU12" t="n">
-        <v>0.321802091713601</v>
+        <v>0.402252614641995</v>
+      </c>
+      <c r="DV12" t="n">
+        <v>0.408163265306122</v>
+      </c>
+      <c r="DW12" t="n">
+        <v>2.42152466367713</v>
+      </c>
+      <c r="DX12" t="n">
+        <v>-0.309278350515461</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -25765,12 +26314,21 @@
         <v>2.40641711229944</v>
       </c>
       <c r="DU13" t="n">
-        <v>2.64550264550265</v>
+        <v>1.05820105820107</v>
+      </c>
+      <c r="DV13" t="n">
+        <v>1.89701897018969</v>
+      </c>
+      <c r="DW13" t="n">
+        <v>0.57142857142858</v>
+      </c>
+      <c r="DX13" t="n">
+        <v>0.887573964497054</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -25896,10 +26454,13 @@
       <c r="DS14"/>
       <c r="DT14"/>
       <c r="DU14"/>
+      <c r="DV14"/>
+      <c r="DW14"/>
+      <c r="DX14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -26271,12 +26832,21 @@
         <v>1.85339441899209</v>
       </c>
       <c r="DU15" t="n">
-        <v>1.72772689425479</v>
+        <v>1.76935886761032</v>
+      </c>
+      <c r="DV15" t="n">
+        <v>1.50010564124233</v>
+      </c>
+      <c r="DW15" t="n">
+        <v>1.91473066122032</v>
+      </c>
+      <c r="DX15" t="n">
+        <v>1.83985488468516</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -26648,12 +27218,21 @@
         <v>3.08788598574821</v>
       </c>
       <c r="DU16" t="n">
-        <v>2.85035629453681</v>
+        <v>2.82066508313539</v>
+      </c>
+      <c r="DV16" t="n">
+        <v>2.02441202738911</v>
+      </c>
+      <c r="DW16" t="n">
+        <v>3.51960481630134</v>
+      </c>
+      <c r="DX16" t="n">
+        <v>3.55987055016181</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -26779,10 +27358,13 @@
       <c r="DS17"/>
       <c r="DT17"/>
       <c r="DU17"/>
+      <c r="DV17"/>
+      <c r="DW17"/>
+      <c r="DX17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -27155,11 +27737,20 @@
       </c>
       <c r="DU18" t="n">
         <v>7.60517799352751</v>
+      </c>
+      <c r="DV18" t="n">
+        <v>5.73770491803279</v>
+      </c>
+      <c r="DW18" t="n">
+        <v>5.67986230636834</v>
+      </c>
+      <c r="DX18" t="n">
+        <v>6.60194174757281</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -27531,12 +28122,21 @@
         <v>3.76831821353804</v>
       </c>
       <c r="DU19" t="n">
-        <v>3.8667598416026</v>
+        <v>3.89005357558816</v>
+      </c>
+      <c r="DV19" t="n">
+        <v>4.02057035998131</v>
+      </c>
+      <c r="DW19" t="n">
+        <v>3.65204159269591</v>
+      </c>
+      <c r="DX19" t="n">
+        <v>3.42391304347827</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -27908,12 +28508,21 @@
         <v>2.18068535825547</v>
       </c>
       <c r="DU20" t="n">
-        <v>2.14190093708165</v>
+        <v>2.18652387327086</v>
+      </c>
+      <c r="DV20" t="n">
+        <v>2.27272727272727</v>
+      </c>
+      <c r="DW20" t="n">
+        <v>-2.87958115183246</v>
+      </c>
+      <c r="DX20" t="n">
+        <v>-1.46799765120376</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -28285,12 +28894,21 @@
         <v>2.24561403508771</v>
       </c>
       <c r="DU21" t="n">
-        <v>1.95804195804197</v>
+        <v>2.23776223776223</v>
+      </c>
+      <c r="DV21" t="n">
+        <v>1.89208128941837</v>
+      </c>
+      <c r="DW21" t="n">
+        <v>0.379650721336371</v>
+      </c>
+      <c r="DX21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -28662,12 +29280,21 @@
         <v>0.221238938053106</v>
       </c>
       <c r="DU22" t="n">
-        <v>-0.294550810014732</v>
+        <v>-0.147275405007376</v>
+      </c>
+      <c r="DV22" t="n">
+        <v>-0.147601476014773</v>
+      </c>
+      <c r="DW22" t="n">
+        <v>-0.580431177446093</v>
+      </c>
+      <c r="DX22" t="n">
+        <v>0.686947988223738</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -29039,12 +29666,21 @@
         <v>1.31826741996233</v>
       </c>
       <c r="DU23" t="n">
-        <v>1.76879343019582</v>
+        <v>1.70562223626026</v>
+      </c>
+      <c r="DV23" t="n">
+        <v>1.64452877925363</v>
+      </c>
+      <c r="DW23" t="n">
+        <v>1.75084175084175</v>
+      </c>
+      <c r="DX23" t="n">
+        <v>3.42298288508559</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -29416,12 +30052,21 @@
         <v>3.39335180055402</v>
       </c>
       <c r="DU24" t="n">
-        <v>3.36769759450172</v>
+        <v>3.29896907216496</v>
+      </c>
+      <c r="DV24" t="n">
+        <v>2.40549828178694</v>
+      </c>
+      <c r="DW24" t="n">
+        <v>3.34323922734027</v>
+      </c>
+      <c r="DX24" t="n">
+        <v>2.08978328173376</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -29793,12 +30438,21 @@
         <v>0.200400801603209</v>
       </c>
       <c r="DU25" t="n">
-        <v>-1.19760479041916</v>
+        <v>-1.39720558882235</v>
+      </c>
+      <c r="DV25" t="n">
+        <v>1.22199592668026</v>
+      </c>
+      <c r="DW25" t="n">
+        <v>0.632911392405072</v>
+      </c>
+      <c r="DX25" t="n">
+        <v>0.742574257425753</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -30171,11 +30825,20 @@
       </c>
       <c r="DU26" t="n">
         <v>3.3532384014699</v>
+      </c>
+      <c r="DV26" t="n">
+        <v>3.01921317474838</v>
+      </c>
+      <c r="DW26" t="n">
+        <v>2.04379562043796</v>
+      </c>
+      <c r="DX26" t="n">
+        <v>2.56276150627615</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -30547,12 +31210,21 @@
         <v>3.44972654606645</v>
       </c>
       <c r="DU27" t="n">
-        <v>3.31098072087174</v>
+        <v>3.05951383067894</v>
+      </c>
+      <c r="DV27" t="n">
+        <v>2.50941028858217</v>
+      </c>
+      <c r="DW27" t="n">
+        <v>2.43589743589743</v>
+      </c>
+      <c r="DX27" t="n">
+        <v>2.70531400966183</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -30924,12 +31596,21 @@
         <v>6.27257799671594</v>
       </c>
       <c r="DU28" t="n">
-        <v>5.84967320261437</v>
+        <v>6.07843137254903</v>
+      </c>
+      <c r="DV28" t="n">
+        <v>6.24137931034484</v>
+      </c>
+      <c r="DW28" t="n">
+        <v>5.6842867487328</v>
+      </c>
+      <c r="DX28" t="n">
+        <v>5.73606097071801</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -31301,12 +31982,21 @@
         <v>0.636319138521787</v>
       </c>
       <c r="DU29" t="n">
-        <v>0.340964442279585</v>
+        <v>0.292255236239646</v>
+      </c>
+      <c r="DV29" t="n">
+        <v>0.644521566683198</v>
+      </c>
+      <c r="DW29" t="n">
+        <v>1.07361963190182</v>
+      </c>
+      <c r="DX29" t="n">
+        <v>-0.475341651812247</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -31679,11 +32369,20 @@
       </c>
       <c r="DU30" t="n">
         <v>1.07421874999999</v>
+      </c>
+      <c r="DV30" t="n">
+        <v>1.09126984126985</v>
+      </c>
+      <c r="DW30" t="n">
+        <v>1.64778578784757</v>
+      </c>
+      <c r="DX30" t="n">
+        <v>-1.06044538706257</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -31809,10 +32508,13 @@
       <c r="DS31"/>
       <c r="DT31"/>
       <c r="DU31"/>
+      <c r="DV31"/>
+      <c r="DW31"/>
+      <c r="DX31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -32184,12 +32886,21 @@
         <v>-1.35746606334842</v>
       </c>
       <c r="DU32" t="n">
-        <v>-1.58371040723983</v>
+        <v>-1.35746606334842</v>
+      </c>
+      <c r="DV32" t="n">
+        <v>-4.26008968609865</v>
+      </c>
+      <c r="DW32" t="n">
+        <v>-6.9047619047619</v>
+      </c>
+      <c r="DX32" t="n">
+        <v>-7.49279538904899</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -32562,11 +33273,20 @@
       </c>
       <c r="DU33" t="n">
         <v>1.28342245989305</v>
+      </c>
+      <c r="DV33" t="n">
+        <v>1.39186295503212</v>
+      </c>
+      <c r="DW33" t="n">
+        <v>2.95790671217292</v>
+      </c>
+      <c r="DX33" t="n">
+        <v>1.94300518134717</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -32939,11 +33659,20 @@
       </c>
       <c r="DU34" t="n">
         <v>4.36953807740325</v>
+      </c>
+      <c r="DV34" t="n">
+        <v>4.74406991260925</v>
+      </c>
+      <c r="DW34" t="n">
+        <v>7.74647887323944</v>
+      </c>
+      <c r="DX34" t="n">
+        <v>5.68862275449101</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -33315,12 +34044,21 @@
         <v>0</v>
       </c>
       <c r="DU35" t="n">
-        <v>0.216450216450204</v>
+        <v>0.432900432900424</v>
+      </c>
+      <c r="DV35" t="n">
+        <v>0.886917960088689</v>
+      </c>
+      <c r="DW35" t="n">
+        <v>0.25641025641026</v>
+      </c>
+      <c r="DX35" t="n">
+        <v>-0.0000000000000219982271133158</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -33692,12 +34430,21 @@
         <v>1.06865284974094</v>
       </c>
       <c r="DU36" t="n">
-        <v>0.838439213157053</v>
+        <v>0.806191551112544</v>
+      </c>
+      <c r="DV36" t="n">
+        <v>1.57273918741809</v>
+      </c>
+      <c r="DW36" t="n">
+        <v>0.729927007299285</v>
+      </c>
+      <c r="DX36" t="n">
+        <v>3.66935483870969</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -34070,11 +34817,20 @@
       </c>
       <c r="DU37" t="n">
         <v>2.50659630606861</v>
+      </c>
+      <c r="DV37" t="n">
+        <v>3.35120643431635</v>
+      </c>
+      <c r="DW37" t="n">
+        <v>11.6352201257862</v>
+      </c>
+      <c r="DX37" t="n">
+        <v>7.75577557755775</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -34446,12 +35202,21 @@
         <v>3.35067319461444</v>
       </c>
       <c r="DU38" t="n">
-        <v>3.56760067370999</v>
+        <v>3.52166590108712</v>
+      </c>
+      <c r="DV38" t="n">
+        <v>3.49392027089425</v>
+      </c>
+      <c r="DW38" t="n">
+        <v>3.33594361785436</v>
+      </c>
+      <c r="DX38" t="n">
+        <v>1.7961807525052</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -34824,11 +35589,20 @@
       </c>
       <c r="DU39" t="n">
         <v>0.850546780072908</v>
+      </c>
+      <c r="DV39" t="n">
+        <v>0.725733293014827</v>
+      </c>
+      <c r="DW39" t="n">
+        <v>0.789022298456265</v>
+      </c>
+      <c r="DX39" t="n">
+        <v>0.721561969439736</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -35200,12 +35974,21 @@
         <v>0.263157894736846</v>
       </c>
       <c r="DU40" t="n">
-        <v>0.795755968169754</v>
+        <v>1.3262599469496</v>
+      </c>
+      <c r="DV40" t="n">
+        <v>0.530503978779829</v>
+      </c>
+      <c r="DW40" t="n">
+        <v>-2.7027027027027</v>
+      </c>
+      <c r="DX40" t="n">
+        <v>-6.4516129032258</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -35578,11 +36361,20 @@
       </c>
       <c r="DU41" t="n">
         <v>0.0761228114691587</v>
+      </c>
+      <c r="DV41" t="n">
+        <v>-0.874710573707223</v>
+      </c>
+      <c r="DW41" t="n">
+        <v>0.562271577171774</v>
+      </c>
+      <c r="DX41" t="n">
+        <v>1.39494333042719</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -35954,12 +36746,21 @@
         <v>-1.07526881720432</v>
       </c>
       <c r="DU42" t="n">
-        <v>-1.20562625586069</v>
+        <v>-1.07166778298729</v>
+      </c>
+      <c r="DV42" t="n">
+        <v>-1.21130551816957</v>
+      </c>
+      <c r="DW42" t="n">
+        <v>1.73584905660378</v>
+      </c>
+      <c r="DX42" t="n">
+        <v>2.61437908496731</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -36332,11 +37133,20 @@
       </c>
       <c r="DU43" t="n">
         <v>4.98511904761906</v>
+      </c>
+      <c r="DV43" t="n">
+        <v>5.17751479289943</v>
+      </c>
+      <c r="DW43" t="n">
+        <v>7.19152157456472</v>
+      </c>
+      <c r="DX43" t="n">
+        <v>2.39190432382705</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -36708,12 +37518,21 @@
         <v>1.71884591774097</v>
       </c>
       <c r="DU44" t="n">
-        <v>1.93488943488944</v>
+        <v>1.96560196560196</v>
+      </c>
+      <c r="DV44" t="n">
+        <v>2.02998126171143</v>
+      </c>
+      <c r="DW44" t="n">
+        <v>1.07023411371237</v>
+      </c>
+      <c r="DX44" t="n">
+        <v>0.930059523809524</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -37085,12 +37904,21 @@
         <v>2.73972602739726</v>
       </c>
       <c r="DU45" t="n">
-        <v>0.684931506849313</v>
+        <v>1.02739726027398</v>
+      </c>
+      <c r="DV45" t="n">
+        <v>2.75862068965516</v>
+      </c>
+      <c r="DW45" t="n">
+        <v>1.48698884758365</v>
+      </c>
+      <c r="DX45" t="n">
+        <v>-2.13675213675214</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -37463,11 +38291,20 @@
       </c>
       <c r="DU46" t="n">
         <v>2.78121137206428</v>
+      </c>
+      <c r="DV46" t="n">
+        <v>0</v>
+      </c>
+      <c r="DW46" t="n">
+        <v>0.257400257400261</v>
+      </c>
+      <c r="DX46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -37840,11 +38677,20 @@
       </c>
       <c r="DU47" t="n">
         <v>1.59574468085107</v>
+      </c>
+      <c r="DV47" t="n">
+        <v>1.8918918918919</v>
+      </c>
+      <c r="DW47" t="n">
+        <v>2.10210210210211</v>
+      </c>
+      <c r="DX47" t="n">
+        <v>1.06761565836298</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -38216,12 +39062,21 @@
         <v>0.920096852300231</v>
       </c>
       <c r="DU48" t="n">
-        <v>1.21006776379477</v>
+        <v>1.35527589545014</v>
+      </c>
+      <c r="DV48" t="n">
+        <v>2.74588117823265</v>
+      </c>
+      <c r="DW48" t="n">
+        <v>0.626304801670155</v>
+      </c>
+      <c r="DX48" t="n">
+        <v>0.899820035992801</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -38594,11 +39449,20 @@
       </c>
       <c r="DU49" t="n">
         <v>3.0778620629523</v>
+      </c>
+      <c r="DV49" t="n">
+        <v>3.07988450433107</v>
+      </c>
+      <c r="DW49" t="n">
+        <v>2.31046931407941</v>
+      </c>
+      <c r="DX49" t="n">
+        <v>1.50196115947575</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -38971,11 +39835,20 @@
       </c>
       <c r="DU50" t="n">
         <v>2.88461538461539</v>
+      </c>
+      <c r="DV50" t="n">
+        <v>3.04487179487179</v>
+      </c>
+      <c r="DW50" t="n">
+        <v>3.10880829015544</v>
+      </c>
+      <c r="DX50" t="n">
+        <v>6.01577909270216</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -39348,11 +40221,20 @@
       </c>
       <c r="DU51" t="n">
         <v>4.48717948717949</v>
+      </c>
+      <c r="DV51" t="n">
+        <v>-5.12820512820513</v>
+      </c>
+      <c r="DW51" t="n">
+        <v>8.08823529411764</v>
+      </c>
+      <c r="DX51" t="n">
+        <v>5.24193548387099</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -39724,12 +40606,21 @@
         <v>3.41962288271015</v>
       </c>
       <c r="DU52" t="n">
-        <v>2.7980922098569</v>
+        <v>2.92527821939586</v>
+      </c>
+      <c r="DV52" t="n">
+        <v>2.01691607026677</v>
+      </c>
+      <c r="DW52" t="n">
+        <v>2.27424749163878</v>
+      </c>
+      <c r="DX52" t="n">
+        <v>3.09433962264151</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -40101,12 +40992,21 @@
         <v>2.55993498577813</v>
       </c>
       <c r="DU53" t="n">
-        <v>2.27088402270884</v>
+        <v>2.23033252230333</v>
+      </c>
+      <c r="DV53" t="n">
+        <v>2.10101010101011</v>
+      </c>
+      <c r="DW53" t="n">
+        <v>3.35542667771334</v>
+      </c>
+      <c r="DX53" t="n">
+        <v>0.43630017452007</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -40479,11 +41379,20 @@
       </c>
       <c r="DU54" t="n">
         <v>1.13636363636363</v>
+      </c>
+      <c r="DV54" t="n">
+        <v>1.14942528735631</v>
+      </c>
+      <c r="DW54" t="n">
+        <v>-0.356506238859172</v>
+      </c>
+      <c r="DX54" t="n">
+        <v>1.57170923379176</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -40855,12 +41764,21 @@
         <v>3.08731307284128</v>
       </c>
       <c r="DU55" t="n">
-        <v>2.88184438040347</v>
+        <v>2.88184438040346</v>
+      </c>
+      <c r="DV55" t="n">
+        <v>3.62745098039216</v>
+      </c>
+      <c r="DW55" t="n">
+        <v>1.77038626609441</v>
+      </c>
+      <c r="DX55" t="n">
+        <v>-1.05944673337256</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -41232,7 +42150,16 @@
         <v>2.32558139534883</v>
       </c>
       <c r="DU56" t="n">
-        <v>1.66666666666667</v>
+        <v>2</v>
+      </c>
+      <c r="DV56" t="n">
+        <v>2.33333333333333</v>
+      </c>
+      <c r="DW56" t="n">
+        <v>2.93040293040293</v>
+      </c>
+      <c r="DX56" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023-09-19 :: SEM Update for September
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t xml:space="preserve">07/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1341,10 +1344,13 @@
       <c r="EJ4" t="s">
         <v>139</v>
       </c>
+      <c r="EK4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1758,15 +1764,18 @@
         <v>10720.3</v>
       </c>
       <c r="EI5" t="n">
-        <v>10139.8</v>
+        <v>10121.8</v>
       </c>
       <c r="EJ5" t="n">
-        <v>9046.6</v>
+        <v>9035.6</v>
+      </c>
+      <c r="EK5" t="n">
+        <v>9318.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2183,12 +2192,15 @@
         <v>169.2</v>
       </c>
       <c r="EJ6" t="n">
-        <v>160.8</v>
+        <v>160.7</v>
+      </c>
+      <c r="EK6" t="n">
+        <v>163.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2606,11 +2618,14 @@
       </c>
       <c r="EJ7" t="n">
         <v>19.3</v>
+      </c>
+      <c r="EK7" t="n">
+        <v>21.4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3027,12 +3042,15 @@
         <v>152.7</v>
       </c>
       <c r="EJ8" t="n">
-        <v>151.9</v>
+        <v>151</v>
+      </c>
+      <c r="EK8" t="n">
+        <v>182.9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3450,11 +3468,14 @@
       </c>
       <c r="EJ9" t="n">
         <v>82.2</v>
+      </c>
+      <c r="EK9" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3871,12 +3892,15 @@
         <v>1234.6</v>
       </c>
       <c r="EJ10" t="n">
-        <v>1074.5</v>
+        <v>1065.7</v>
+      </c>
+      <c r="EK10" t="n">
+        <v>1115.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4293,12 +4317,15 @@
         <v>211.2</v>
       </c>
       <c r="EJ11" t="n">
-        <v>197</v>
+        <v>197.5</v>
+      </c>
+      <c r="EK11" t="n">
+        <v>203.4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4716,11 +4743,14 @@
       </c>
       <c r="EJ12" t="n">
         <v>96.7</v>
+      </c>
+      <c r="EK12" t="n">
+        <v>97.9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5137,12 +5167,15 @@
         <v>35.2</v>
       </c>
       <c r="EJ13" t="n">
-        <v>34.1</v>
+        <v>33.8</v>
+      </c>
+      <c r="EK13" t="n">
+        <v>32.9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5283,10 +5316,11 @@
       <c r="EH14"/>
       <c r="EI14"/>
       <c r="EJ14"/>
+      <c r="EK14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5703,12 +5737,15 @@
         <v>399.2</v>
       </c>
       <c r="EJ15" t="n">
-        <v>393</v>
+        <v>392.9</v>
+      </c>
+      <c r="EK15" t="n">
+        <v>461.9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6125,12 +6162,15 @@
         <v>335.3</v>
       </c>
       <c r="EJ16" t="n">
-        <v>320</v>
+        <v>321.8</v>
+      </c>
+      <c r="EK16" t="n">
+        <v>343.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6271,10 +6311,11 @@
       <c r="EH17"/>
       <c r="EI17"/>
       <c r="EJ17"/>
+      <c r="EK17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6692,11 +6733,14 @@
       </c>
       <c r="EJ18" t="n">
         <v>54.9</v>
+      </c>
+      <c r="EK18" t="n">
+        <v>54.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7113,12 +7157,15 @@
         <v>408.7</v>
       </c>
       <c r="EJ19" t="n">
-        <v>380.6</v>
+        <v>380.8</v>
+      </c>
+      <c r="EK19" t="n">
+        <v>384</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7535,12 +7582,15 @@
         <v>185.5</v>
       </c>
       <c r="EJ20" t="n">
-        <v>167.8</v>
+        <v>171.2</v>
+      </c>
+      <c r="EK20" t="n">
+        <v>207.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7957,12 +8007,15 @@
         <v>132.2</v>
       </c>
       <c r="EJ21" t="n">
-        <v>114.6</v>
+        <v>115.4</v>
+      </c>
+      <c r="EK21" t="n">
+        <v>120.4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8379,12 +8432,15 @@
         <v>119.9</v>
       </c>
       <c r="EJ22" t="n">
-        <v>102.6</v>
+        <v>103.3</v>
+      </c>
+      <c r="EK22" t="n">
+        <v>110.8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8801,12 +8857,15 @@
         <v>151.1</v>
       </c>
       <c r="EJ23" t="n">
-        <v>126.9</v>
+        <v>127.7</v>
+      </c>
+      <c r="EK23" t="n">
+        <v>150.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9223,12 +9282,15 @@
         <v>139.1</v>
       </c>
       <c r="EJ24" t="n">
-        <v>131.9</v>
+        <v>132.1</v>
+      </c>
+      <c r="EK24" t="n">
+        <v>139.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9646,11 +9708,14 @@
       </c>
       <c r="EJ25" t="n">
         <v>40.7</v>
+      </c>
+      <c r="EK25" t="n">
+        <v>39.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10068,11 +10133,14 @@
       </c>
       <c r="EJ26" t="n">
         <v>196.1</v>
+      </c>
+      <c r="EK26" t="n">
+        <v>198.1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10489,12 +10557,15 @@
         <v>239.7</v>
       </c>
       <c r="EJ27" t="n">
-        <v>212.6</v>
+        <v>210.8</v>
+      </c>
+      <c r="EK27" t="n">
+        <v>207.6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10912,11 +10983,14 @@
       </c>
       <c r="EJ28" t="n">
         <v>263.6</v>
+      </c>
+      <c r="EK28" t="n">
+        <v>274.6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11333,12 +11407,15 @@
         <v>197.7</v>
       </c>
       <c r="EJ29" t="n">
-        <v>167.5</v>
+        <v>168.1</v>
+      </c>
+      <c r="EK29" t="n">
+        <v>163.3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11755,12 +11832,15 @@
         <v>98.7</v>
       </c>
       <c r="EJ30" t="n">
-        <v>93.3</v>
+        <v>94.5</v>
+      </c>
+      <c r="EK30" t="n">
+        <v>97.8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11901,10 +11981,11 @@
       <c r="EH31"/>
       <c r="EI31"/>
       <c r="EJ31"/>
+      <c r="EK31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12321,12 +12402,15 @@
         <v>39.1</v>
       </c>
       <c r="EJ32" t="n">
-        <v>32.1</v>
+        <v>32.3</v>
+      </c>
+      <c r="EK32" t="n">
+        <v>33.4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12743,12 +12827,15 @@
         <v>90.5</v>
       </c>
       <c r="EJ33" t="n">
-        <v>78.7</v>
+        <v>78.8</v>
+      </c>
+      <c r="EK33" t="n">
+        <v>80.6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -13166,11 +13253,14 @@
       </c>
       <c r="EJ34" t="n">
         <v>70.6</v>
+      </c>
+      <c r="EK34" t="n">
+        <v>73.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13587,12 +13677,15 @@
         <v>39.1</v>
       </c>
       <c r="EJ35" t="n">
-        <v>32.3</v>
+        <v>33.1</v>
+      </c>
+      <c r="EK35" t="n">
+        <v>33.8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14010,11 +14103,14 @@
       </c>
       <c r="EJ36" t="n">
         <v>257.1</v>
+      </c>
+      <c r="EK36" t="n">
+        <v>259.8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14431,12 +14527,15 @@
         <v>71</v>
       </c>
       <c r="EJ37" t="n">
-        <v>65.3</v>
+        <v>65.7</v>
+      </c>
+      <c r="EK37" t="n">
+        <v>70.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14853,12 +14952,15 @@
         <v>659.8</v>
       </c>
       <c r="EJ38" t="n">
-        <v>538.4</v>
+        <v>546.1</v>
+      </c>
+      <c r="EK38" t="n">
+        <v>542.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -15276,11 +15378,14 @@
       </c>
       <c r="EJ39" t="n">
         <v>237.3</v>
+      </c>
+      <c r="EK39" t="n">
+        <v>286.3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15698,11 +15803,14 @@
       </c>
       <c r="EJ40" t="n">
         <v>26.1</v>
+      </c>
+      <c r="EK40" t="n">
+        <v>28.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -16119,12 +16227,15 @@
         <v>357.7</v>
       </c>
       <c r="EJ41" t="n">
-        <v>348.9</v>
+        <v>349.3</v>
+      </c>
+      <c r="EK41" t="n">
+        <v>353.4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16541,12 +16652,15 @@
         <v>134.8</v>
       </c>
       <c r="EJ42" t="n">
-        <v>125.6</v>
+        <v>122.3</v>
+      </c>
+      <c r="EK42" t="n">
+        <v>127.2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -16963,12 +17077,15 @@
         <v>141.6</v>
       </c>
       <c r="EJ43" t="n">
-        <v>111.3</v>
+        <v>110.8</v>
+      </c>
+      <c r="EK43" t="n">
+        <v>112.7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17386,11 +17503,14 @@
       </c>
       <c r="EJ44" t="n">
         <v>271.3</v>
+      </c>
+      <c r="EK44" t="n">
+        <v>277.9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17807,12 +17927,15 @@
         <v>27.3</v>
       </c>
       <c r="EJ45" t="n">
-        <v>22.9</v>
+        <v>23</v>
+      </c>
+      <c r="EK45" t="n">
+        <v>22.6</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -18229,12 +18352,15 @@
         <v>155.8</v>
       </c>
       <c r="EJ46" t="n">
-        <v>147.1</v>
+        <v>146</v>
+      </c>
+      <c r="EK46" t="n">
+        <v>147.8</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18651,12 +18777,15 @@
         <v>34</v>
       </c>
       <c r="EJ47" t="n">
-        <v>28.4</v>
+        <v>28.2</v>
+      </c>
+      <c r="EK47" t="n">
+        <v>29.2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -19073,12 +19202,15 @@
         <v>192.8</v>
       </c>
       <c r="EJ48" t="n">
-        <v>168.2</v>
+        <v>168.6</v>
+      </c>
+      <c r="EK48" t="n">
+        <v>182.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -19495,12 +19627,15 @@
         <v>1133.6</v>
       </c>
       <c r="EJ49" t="n">
-        <v>1061</v>
+        <v>1060.3</v>
+      </c>
+      <c r="EK49" t="n">
+        <v>1082.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -19918,11 +20053,14 @@
       </c>
       <c r="EJ50" t="n">
         <v>107.5</v>
+      </c>
+      <c r="EK50" t="n">
+        <v>113.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -20339,12 +20477,15 @@
         <v>29.4</v>
       </c>
       <c r="EJ51" t="n">
-        <v>26.1</v>
+        <v>26.3</v>
+      </c>
+      <c r="EK51" t="n">
+        <v>26.5</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20761,12 +20902,15 @@
         <v>305.8</v>
       </c>
       <c r="EJ52" t="n">
-        <v>273.2</v>
+        <v>275.1</v>
+      </c>
+      <c r="EK52" t="n">
+        <v>295.4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -21183,12 +21327,15 @@
         <v>249.5</v>
       </c>
       <c r="EJ53" t="n">
-        <v>230.2</v>
+        <v>230</v>
+      </c>
+      <c r="EK53" t="n">
+        <v>216.1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -21606,11 +21753,14 @@
       </c>
       <c r="EJ54" t="n">
         <v>51.7</v>
+      </c>
+      <c r="EK54" t="n">
+        <v>54.8</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -22027,12 +22177,15 @@
         <v>189.7</v>
       </c>
       <c r="EJ55" t="n">
-        <v>168.1</v>
+        <v>169.9</v>
+      </c>
+      <c r="EK55" t="n">
+        <v>165.9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -22449,7 +22602,10 @@
         <v>28.1</v>
       </c>
       <c r="EJ56" t="n">
-        <v>24.1</v>
+        <v>23.9</v>
+      </c>
+      <c r="EK56" t="n">
+        <v>24.6</v>
       </c>
     </row>
   </sheetData>
@@ -22851,10 +23007,13 @@
       <c r="DX4" t="s">
         <v>139</v>
       </c>
+      <c r="DY4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -23232,15 +23391,18 @@
         <v>2.36326483843862</v>
       </c>
       <c r="DW5" t="n">
-        <v>2.67112191170514</v>
+        <v>2.4888618874038</v>
       </c>
       <c r="DX5" t="n">
-        <v>1.785573645068</v>
+        <v>1.66180987634875</v>
+      </c>
+      <c r="DY5" t="n">
+        <v>0.572039157699323</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -23621,12 +23783,15 @@
         <v>0.594530321046373</v>
       </c>
       <c r="DX6" t="n">
-        <v>0.06222775357811</v>
+        <v>0</v>
+      </c>
+      <c r="DY6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -24008,11 +24173,14 @@
       </c>
       <c r="DX7" t="n">
         <v>2.11640211640213</v>
+      </c>
+      <c r="DY7" t="n">
+        <v>0.0000000000000166014657887874</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -24393,12 +24561,15 @@
         <v>1.73217854763491</v>
       </c>
       <c r="DX8" t="n">
-        <v>3.47411444141689</v>
+        <v>2.86103542234332</v>
+      </c>
+      <c r="DY8" t="n">
+        <v>2.46498599439775</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -24780,11 +24951,14 @@
       </c>
       <c r="DX9" t="n">
         <v>0.611995104039185</v>
+      </c>
+      <c r="DY9" t="n">
+        <v>0.578034682080925</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -25165,12 +25339,15 @@
         <v>2.72069223729094</v>
       </c>
       <c r="DX10" t="n">
-        <v>3.08932169241102</v>
+        <v>2.24503501870863</v>
+      </c>
+      <c r="DY10" t="n">
+        <v>2.78341013824885</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -25551,12 +25728,15 @@
         <v>3.32681017612524</v>
       </c>
       <c r="DX11" t="n">
-        <v>5.74342458400429</v>
+        <v>6.01180891035963</v>
+      </c>
+      <c r="DY11" t="n">
+        <v>2.57186081694401</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -25938,11 +26118,14 @@
       </c>
       <c r="DX12" t="n">
         <v>-0.309278350515461</v>
+      </c>
+      <c r="DY12" t="n">
+        <v>-0.305498981670058</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -26323,12 +26506,15 @@
         <v>0.57142857142858</v>
       </c>
       <c r="DX13" t="n">
-        <v>0.887573964497054</v>
+        <v>0</v>
+      </c>
+      <c r="DY13" t="n">
+        <v>0.611620795107042</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -26457,10 +26643,11 @@
       <c r="DV14"/>
       <c r="DW14"/>
       <c r="DX14"/>
+      <c r="DY14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -26841,12 +27028,15 @@
         <v>1.91473066122032</v>
       </c>
       <c r="DX15" t="n">
-        <v>1.83985488468516</v>
+        <v>1.81394143560509</v>
+      </c>
+      <c r="DY15" t="n">
+        <v>1.98719364098035</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -27227,12 +27417,15 @@
         <v>3.51960481630134</v>
       </c>
       <c r="DX16" t="n">
-        <v>3.55987055016181</v>
+        <v>4.14239482200648</v>
+      </c>
+      <c r="DY16" t="n">
+        <v>2.4179104477612</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -27361,10 +27554,11 @@
       <c r="DV17"/>
       <c r="DW17"/>
       <c r="DX17"/>
+      <c r="DY17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -27746,11 +27940,14 @@
       </c>
       <c r="DX18" t="n">
         <v>6.60194174757281</v>
+      </c>
+      <c r="DY18" t="n">
+        <v>3.79506641366223</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -28131,12 +28328,15 @@
         <v>3.65204159269591</v>
       </c>
       <c r="DX19" t="n">
-        <v>3.42391304347827</v>
+        <v>3.4782608695652</v>
+      </c>
+      <c r="DY19" t="n">
+        <v>2.92146877512732</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -28517,12 +28717,15 @@
         <v>-2.87958115183246</v>
       </c>
       <c r="DX20" t="n">
-        <v>-1.46799765120376</v>
+        <v>0.528479154433339</v>
+      </c>
+      <c r="DY20" t="n">
+        <v>-0.62260536398468</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -28903,12 +29106,15 @@
         <v>0.379650721336371</v>
       </c>
       <c r="DX21" t="n">
-        <v>0</v>
+        <v>0.698080279232122</v>
+      </c>
+      <c r="DY21" t="n">
+        <v>1.34680134680134</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -29289,12 +29495,15 @@
         <v>-0.580431177446093</v>
       </c>
       <c r="DX22" t="n">
-        <v>0.686947988223738</v>
+        <v>1.37389597644749</v>
+      </c>
+      <c r="DY22" t="n">
+        <v>0.362318840579702</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -29675,12 +29884,15 @@
         <v>1.75084175084175</v>
       </c>
       <c r="DX23" t="n">
-        <v>3.42298288508559</v>
+        <v>4.07497962510188</v>
+      </c>
+      <c r="DY23" t="n">
+        <v>3.07377049180326</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -30061,12 +30273,15 @@
         <v>3.34323922734027</v>
       </c>
       <c r="DX24" t="n">
-        <v>2.08978328173376</v>
+        <v>2.24458204334366</v>
+      </c>
+      <c r="DY24" t="n">
+        <v>1.52838427947598</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -30448,11 +30663,14 @@
       </c>
       <c r="DX25" t="n">
         <v>0.742574257425753</v>
+      </c>
+      <c r="DY25" t="n">
+        <v>0.50890585241731</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -30834,11 +31052,14 @@
       </c>
       <c r="DX26" t="n">
         <v>2.56276150627615</v>
+      </c>
+      <c r="DY26" t="n">
+        <v>4.42804428044281</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -31219,12 +31440,15 @@
         <v>2.43589743589743</v>
       </c>
       <c r="DX27" t="n">
-        <v>2.70531400966183</v>
+        <v>1.83574879227054</v>
+      </c>
+      <c r="DY27" t="n">
+        <v>1.96463654223967</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -31606,11 +31830,14 @@
       </c>
       <c r="DX28" t="n">
         <v>5.73606097071801</v>
+      </c>
+      <c r="DY28" t="n">
+        <v>5.90050134978789</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -31991,12 +32218,15 @@
         <v>1.07361963190182</v>
       </c>
       <c r="DX29" t="n">
-        <v>-0.475341651812247</v>
+        <v>-0.11883541295307</v>
+      </c>
+      <c r="DY29" t="n">
+        <v>-0.366076876143987</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -32377,12 +32607,15 @@
         <v>1.64778578784757</v>
       </c>
       <c r="DX30" t="n">
-        <v>-1.06044538706257</v>
+        <v>0.212089077412516</v>
+      </c>
+      <c r="DY30" t="n">
+        <v>0.410677618069836</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -32511,10 +32744,11 @@
       <c r="DV31"/>
       <c r="DW31"/>
       <c r="DX31"/>
+      <c r="DY31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -32895,12 +33129,15 @@
         <v>-6.9047619047619</v>
       </c>
       <c r="DX32" t="n">
-        <v>-7.49279538904899</v>
+        <v>-6.91642651296832</v>
+      </c>
+      <c r="DY32" t="n">
+        <v>-3.18840579710145</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -33281,12 +33518,15 @@
         <v>2.95790671217292</v>
       </c>
       <c r="DX33" t="n">
-        <v>1.94300518134717</v>
+        <v>2.07253886010364</v>
+      </c>
+      <c r="DY33" t="n">
+        <v>0.876095118898609</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -33668,11 +33908,14 @@
       </c>
       <c r="DX34" t="n">
         <v>5.68862275449101</v>
+      </c>
+      <c r="DY34" t="n">
+        <v>5.60344827586208</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -34053,12 +34296,15 @@
         <v>0.25641025641026</v>
       </c>
       <c r="DX35" t="n">
-        <v>-0.0000000000000219982271133158</v>
+        <v>2.4767801857585</v>
+      </c>
+      <c r="DY35" t="n">
+        <v>2.73556231003039</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -34440,11 +34686,14 @@
       </c>
       <c r="DX36" t="n">
         <v>3.66935483870969</v>
+      </c>
+      <c r="DY36" t="n">
+        <v>4.17000801924619</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -34825,12 +35074,15 @@
         <v>11.6352201257862</v>
       </c>
       <c r="DX37" t="n">
-        <v>7.75577557755775</v>
+        <v>8.41584158415842</v>
+      </c>
+      <c r="DY37" t="n">
+        <v>1.88133140376268</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -35211,12 +35463,15 @@
         <v>3.33594361785436</v>
       </c>
       <c r="DX38" t="n">
-        <v>1.7961807525052</v>
+        <v>3.25203252032521</v>
+      </c>
+      <c r="DY38" t="n">
+        <v>2.45561012466944</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -35598,11 +35853,14 @@
       </c>
       <c r="DX39" t="n">
         <v>0.721561969439736</v>
+      </c>
+      <c r="DY39" t="n">
+        <v>0.632688927943745</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -35984,11 +36242,14 @@
       </c>
       <c r="DX40" t="n">
         <v>-6.4516129032258</v>
+      </c>
+      <c r="DY40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -36369,12 +36630,15 @@
         <v>0.562271577171774</v>
       </c>
       <c r="DX41" t="n">
-        <v>1.39494333042719</v>
+        <v>1.5111886079628</v>
+      </c>
+      <c r="DY41" t="n">
+        <v>1.90311418685122</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -36755,12 +37019,15 @@
         <v>1.73584905660378</v>
       </c>
       <c r="DX42" t="n">
-        <v>2.61437908496731</v>
+        <v>-0.0816993464052357</v>
+      </c>
+      <c r="DY42" t="n">
+        <v>0.952380952380943</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -37141,12 +37408,15 @@
         <v>7.19152157456472</v>
       </c>
       <c r="DX43" t="n">
-        <v>2.39190432382705</v>
+        <v>1.93192272309108</v>
+      </c>
+      <c r="DY43" t="n">
+        <v>1.806684733514</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -37528,11 +37798,14 @@
       </c>
       <c r="DX44" t="n">
         <v>0.930059523809524</v>
+      </c>
+      <c r="DY44" t="n">
+        <v>2.05655526992287</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -37913,12 +38186,15 @@
         <v>1.48698884758365</v>
       </c>
       <c r="DX45" t="n">
-        <v>-2.13675213675214</v>
+        <v>-1.7094017094017</v>
+      </c>
+      <c r="DY45" t="n">
+        <v>-4.64135021097046</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -38299,12 +38575,15 @@
         <v>0.257400257400261</v>
       </c>
       <c r="DX46" t="n">
-        <v>0</v>
+        <v>-0.747790618626781</v>
+      </c>
+      <c r="DY46" t="n">
+        <v>-1.00468854655057</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -38685,12 +38964,15 @@
         <v>2.10210210210211</v>
       </c>
       <c r="DX47" t="n">
-        <v>1.06761565836298</v>
+        <v>0.355871886121001</v>
+      </c>
+      <c r="DY47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -39071,12 +39353,15 @@
         <v>0.626304801670155</v>
       </c>
       <c r="DX48" t="n">
-        <v>0.899820035992801</v>
+        <v>1.13977204559089</v>
+      </c>
+      <c r="DY48" t="n">
+        <v>0.773053561568182</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -39457,12 +39742,15 @@
         <v>2.31046931407941</v>
       </c>
       <c r="DX49" t="n">
-        <v>1.50196115947575</v>
+        <v>1.43499473835263</v>
+      </c>
+      <c r="DY49" t="n">
+        <v>1.77631578947369</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -39844,11 +40132,14 @@
       </c>
       <c r="DX50" t="n">
         <v>6.01577909270216</v>
+      </c>
+      <c r="DY50" t="n">
+        <v>5.28756957328386</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -40229,12 +40520,15 @@
         <v>8.08823529411764</v>
       </c>
       <c r="DX51" t="n">
-        <v>5.24193548387099</v>
+        <v>6.04838709677421</v>
+      </c>
+      <c r="DY51" t="n">
+        <v>5.57768924302788</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -40615,12 +40909,15 @@
         <v>2.27424749163878</v>
       </c>
       <c r="DX52" t="n">
-        <v>3.09433962264151</v>
+        <v>3.81132075471699</v>
+      </c>
+      <c r="DY52" t="n">
+        <v>4.67753366406803</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -41001,12 +41298,15 @@
         <v>3.35542667771334</v>
       </c>
       <c r="DX53" t="n">
-        <v>0.43630017452007</v>
+        <v>0.349040139616061</v>
+      </c>
+      <c r="DY53" t="n">
+        <v>-2.52593594948128</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -41388,11 +41688,14 @@
       </c>
       <c r="DX54" t="n">
         <v>1.57170923379176</v>
+      </c>
+      <c r="DY54" t="n">
+        <v>1.48148148148149</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -41773,12 +42076,15 @@
         <v>1.77038626609441</v>
       </c>
       <c r="DX55" t="n">
-        <v>-1.05944673337256</v>
+        <v>0.0000000000000167284928960589</v>
+      </c>
+      <c r="DY55" t="n">
+        <v>-0.777511961722495</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -42159,7 +42465,10 @@
         <v>2.93040293040293</v>
       </c>
       <c r="DX56" t="n">
-        <v>0</v>
+        <v>-0.829875518672211</v>
+      </c>
+      <c r="DY56" t="n">
+        <v>-0.0000000000000144419255235793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023-10-20 :: SEM Update for October
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t xml:space="preserve">08/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1347,10 +1350,13 @@
       <c r="EK4" t="s">
         <v>140</v>
       </c>
+      <c r="EL4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1767,15 +1773,18 @@
         <v>10121.8</v>
       </c>
       <c r="EJ5" t="n">
-        <v>9035.6</v>
+        <v>9039</v>
       </c>
       <c r="EK5" t="n">
-        <v>9318.1</v>
+        <v>9474.7</v>
+      </c>
+      <c r="EL5" t="n">
+        <v>10620.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2195,12 +2204,15 @@
         <v>160.7</v>
       </c>
       <c r="EK6" t="n">
-        <v>163.9</v>
+        <v>165</v>
+      </c>
+      <c r="EL6" t="n">
+        <v>171.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2621,11 +2633,14 @@
       </c>
       <c r="EK7" t="n">
         <v>21.4</v>
+      </c>
+      <c r="EL7" t="n">
+        <v>27.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3045,12 +3060,15 @@
         <v>151</v>
       </c>
       <c r="EK8" t="n">
-        <v>182.9</v>
+        <v>185.5</v>
+      </c>
+      <c r="EL8" t="n">
+        <v>201.7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3471,11 +3489,14 @@
       </c>
       <c r="EK9" t="n">
         <v>87</v>
+      </c>
+      <c r="EL9" t="n">
+        <v>100.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3895,12 +3916,15 @@
         <v>1065.7</v>
       </c>
       <c r="EK10" t="n">
-        <v>1115.2</v>
+        <v>1111</v>
+      </c>
+      <c r="EL10" t="n">
+        <v>1187.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4320,12 +4344,15 @@
         <v>197.5</v>
       </c>
       <c r="EK11" t="n">
-        <v>203.4</v>
+        <v>206.3</v>
+      </c>
+      <c r="EL11" t="n">
+        <v>224.4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4745,12 +4772,15 @@
         <v>96.7</v>
       </c>
       <c r="EK12" t="n">
-        <v>97.9</v>
+        <v>97.8</v>
+      </c>
+      <c r="EL12" t="n">
+        <v>124.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5170,12 +5200,15 @@
         <v>33.8</v>
       </c>
       <c r="EK13" t="n">
-        <v>32.9</v>
+        <v>33.2</v>
+      </c>
+      <c r="EL13" t="n">
+        <v>36.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5317,10 +5350,11 @@
       <c r="EI14"/>
       <c r="EJ14"/>
       <c r="EK14"/>
+      <c r="EL14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5740,12 +5774,15 @@
         <v>392.9</v>
       </c>
       <c r="EK15" t="n">
-        <v>461.9</v>
+        <v>459.2</v>
+      </c>
+      <c r="EL15" t="n">
+        <v>487.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6165,12 +6202,15 @@
         <v>321.8</v>
       </c>
       <c r="EK16" t="n">
-        <v>343.1</v>
+        <v>344.2</v>
+      </c>
+      <c r="EL16" t="n">
+        <v>350.8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6312,10 +6352,11 @@
       <c r="EI17"/>
       <c r="EJ17"/>
       <c r="EK17"/>
+      <c r="EL17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6735,12 +6776,15 @@
         <v>54.9</v>
       </c>
       <c r="EK18" t="n">
-        <v>54.7</v>
+        <v>57.1</v>
+      </c>
+      <c r="EL18" t="n">
+        <v>66.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7160,12 +7204,15 @@
         <v>380.8</v>
       </c>
       <c r="EK19" t="n">
-        <v>384</v>
+        <v>384.8</v>
+      </c>
+      <c r="EL19" t="n">
+        <v>445.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7585,12 +7632,15 @@
         <v>171.2</v>
       </c>
       <c r="EK20" t="n">
-        <v>207.5</v>
+        <v>206.5</v>
+      </c>
+      <c r="EL20" t="n">
+        <v>229.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8010,12 +8060,15 @@
         <v>115.4</v>
       </c>
       <c r="EK21" t="n">
-        <v>120.4</v>
+        <v>119.2</v>
+      </c>
+      <c r="EL21" t="n">
+        <v>142.1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8435,12 +8488,15 @@
         <v>103.3</v>
       </c>
       <c r="EK22" t="n">
-        <v>110.8</v>
+        <v>112.2</v>
+      </c>
+      <c r="EL22" t="n">
+        <v>132.6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8861,11 +8917,14 @@
       </c>
       <c r="EK23" t="n">
         <v>150.9</v>
+      </c>
+      <c r="EL23" t="n">
+        <v>161.2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9285,12 +9344,15 @@
         <v>132.1</v>
       </c>
       <c r="EK24" t="n">
-        <v>139.5</v>
+        <v>140.5</v>
+      </c>
+      <c r="EL24" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9711,11 +9773,14 @@
       </c>
       <c r="EK25" t="n">
         <v>39.5</v>
+      </c>
+      <c r="EL25" t="n">
+        <v>49.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10135,12 +10200,15 @@
         <v>196.1</v>
       </c>
       <c r="EK26" t="n">
-        <v>198.1</v>
+        <v>197.7</v>
+      </c>
+      <c r="EL26" t="n">
+        <v>220.4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10560,12 +10628,15 @@
         <v>210.8</v>
       </c>
       <c r="EK27" t="n">
-        <v>207.6</v>
+        <v>207.5</v>
+      </c>
+      <c r="EL27" t="n">
+        <v>239.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10985,12 +11056,15 @@
         <v>263.6</v>
       </c>
       <c r="EK28" t="n">
-        <v>274.6</v>
+        <v>272.7</v>
+      </c>
+      <c r="EL28" t="n">
+        <v>324</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11410,12 +11484,15 @@
         <v>168.1</v>
       </c>
       <c r="EK29" t="n">
-        <v>163.3</v>
+        <v>164.3</v>
+      </c>
+      <c r="EL29" t="n">
+        <v>194.3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11835,12 +11912,15 @@
         <v>94.5</v>
       </c>
       <c r="EK30" t="n">
-        <v>97.8</v>
+        <v>99.6</v>
+      </c>
+      <c r="EL30" t="n">
+        <v>104.6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11982,10 +12062,11 @@
       <c r="EI31"/>
       <c r="EJ31"/>
       <c r="EK31"/>
+      <c r="EL31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12406,11 +12487,14 @@
       </c>
       <c r="EK32" t="n">
         <v>33.4</v>
+      </c>
+      <c r="EL32" t="n">
+        <v>39.8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12830,12 +12914,15 @@
         <v>78.8</v>
       </c>
       <c r="EK33" t="n">
-        <v>80.6</v>
+        <v>81</v>
+      </c>
+      <c r="EL33" t="n">
+        <v>92.6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -13255,12 +13342,15 @@
         <v>70.6</v>
       </c>
       <c r="EK34" t="n">
-        <v>73.5</v>
+        <v>69</v>
+      </c>
+      <c r="EL34" t="n">
+        <v>78.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13680,12 +13770,15 @@
         <v>33.1</v>
       </c>
       <c r="EK35" t="n">
-        <v>33.8</v>
+        <v>33.1</v>
+      </c>
+      <c r="EL35" t="n">
+        <v>45.6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14105,12 +14198,15 @@
         <v>257.1</v>
       </c>
       <c r="EK36" t="n">
-        <v>259.8</v>
+        <v>259.6</v>
+      </c>
+      <c r="EL36" t="n">
+        <v>303.3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14530,12 +14626,15 @@
         <v>65.7</v>
       </c>
       <c r="EK37" t="n">
-        <v>70.4</v>
+        <v>71.6</v>
+      </c>
+      <c r="EL37" t="n">
+        <v>78.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14955,12 +15054,15 @@
         <v>546.1</v>
       </c>
       <c r="EK38" t="n">
-        <v>542.4</v>
+        <v>532.9</v>
+      </c>
+      <c r="EL38" t="n">
+        <v>651.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -15381,11 +15483,14 @@
       </c>
       <c r="EK39" t="n">
         <v>286.3</v>
+      </c>
+      <c r="EL39" t="n">
+        <v>319</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15806,11 +15911,14 @@
       </c>
       <c r="EK40" t="n">
         <v>28.8</v>
+      </c>
+      <c r="EL40" t="n">
+        <v>37.9</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -16230,12 +16338,15 @@
         <v>349.3</v>
       </c>
       <c r="EK41" t="n">
-        <v>353.4</v>
+        <v>349.8</v>
+      </c>
+      <c r="EL41" t="n">
+        <v>383.4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16655,12 +16766,15 @@
         <v>122.3</v>
       </c>
       <c r="EK42" t="n">
-        <v>127.2</v>
+        <v>129.1</v>
+      </c>
+      <c r="EL42" t="n">
+        <v>148.1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -17080,12 +17194,15 @@
         <v>110.8</v>
       </c>
       <c r="EK43" t="n">
-        <v>112.7</v>
+        <v>112.5</v>
+      </c>
+      <c r="EL43" t="n">
+        <v>127.3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17505,12 +17622,15 @@
         <v>271.3</v>
       </c>
       <c r="EK44" t="n">
-        <v>277.9</v>
+        <v>278</v>
+      </c>
+      <c r="EL44" t="n">
+        <v>319.9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17930,12 +18050,15 @@
         <v>23</v>
       </c>
       <c r="EK45" t="n">
-        <v>22.6</v>
+        <v>23.2</v>
+      </c>
+      <c r="EL45" t="n">
+        <v>28.4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -18355,12 +18478,15 @@
         <v>146</v>
       </c>
       <c r="EK46" t="n">
-        <v>147.8</v>
+        <v>150.8</v>
+      </c>
+      <c r="EL46" t="n">
+        <v>161.1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18780,12 +18906,15 @@
         <v>28.2</v>
       </c>
       <c r="EK47" t="n">
-        <v>29.2</v>
+        <v>29.9</v>
+      </c>
+      <c r="EL47" t="n">
+        <v>37.9</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -19205,12 +19334,15 @@
         <v>168.6</v>
       </c>
       <c r="EK48" t="n">
-        <v>182.5</v>
+        <v>182.1</v>
+      </c>
+      <c r="EL48" t="n">
+        <v>206.7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -19630,12 +19762,15 @@
         <v>1060.3</v>
       </c>
       <c r="EK49" t="n">
-        <v>1082.9</v>
+        <v>1087.7</v>
+      </c>
+      <c r="EL49" t="n">
+        <v>1154.2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -20056,11 +20191,14 @@
       </c>
       <c r="EK50" t="n">
         <v>113.5</v>
+      </c>
+      <c r="EL50" t="n">
+        <v>128.2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -20481,11 +20619,14 @@
       </c>
       <c r="EK51" t="n">
         <v>26.5</v>
+      </c>
+      <c r="EL51" t="n">
+        <v>32.3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20905,12 +21046,15 @@
         <v>275.1</v>
       </c>
       <c r="EK52" t="n">
-        <v>295.4</v>
+        <v>292.2</v>
+      </c>
+      <c r="EL52" t="n">
+        <v>318.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -21330,12 +21474,15 @@
         <v>230</v>
       </c>
       <c r="EK53" t="n">
-        <v>216.1</v>
+        <v>218.8</v>
+      </c>
+      <c r="EL53" t="n">
+        <v>230.7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -21755,12 +21902,15 @@
         <v>51.7</v>
       </c>
       <c r="EK54" t="n">
-        <v>54.8</v>
+        <v>54.9</v>
+      </c>
+      <c r="EL54" t="n">
+        <v>59.4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -22180,12 +22330,15 @@
         <v>169.9</v>
       </c>
       <c r="EK55" t="n">
-        <v>165.9</v>
+        <v>166.8</v>
+      </c>
+      <c r="EL55" t="n">
+        <v>206.8</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -22605,7 +22758,10 @@
         <v>23.9</v>
       </c>
       <c r="EK56" t="n">
-        <v>24.6</v>
+        <v>24.5</v>
+      </c>
+      <c r="EL56" t="n">
+        <v>29.4</v>
       </c>
     </row>
   </sheetData>
@@ -23010,10 +23166,13 @@
       <c r="DY4" t="s">
         <v>140</v>
       </c>
+      <c r="DZ4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -23394,15 +23553,18 @@
         <v>2.4888618874038</v>
       </c>
       <c r="DX5" t="n">
-        <v>1.66180987634875</v>
+        <v>1.7000641321347</v>
       </c>
       <c r="DY5" t="n">
-        <v>0.572039157699323</v>
+        <v>2.26225297082601</v>
+      </c>
+      <c r="DZ5" t="n">
+        <v>2.69590778989711</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -23786,12 +23948,15 @@
         <v>0</v>
       </c>
       <c r="DY6" t="n">
-        <v>0</v>
+        <v>0.671140939597312</v>
+      </c>
+      <c r="DZ6" t="n">
+        <v>0.999412110523232</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -24176,11 +24341,14 @@
       </c>
       <c r="DY7" t="n">
         <v>0.0000000000000166014657887874</v>
+      </c>
+      <c r="DZ7" t="n">
+        <v>0.740740740740751</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -24564,12 +24732,15 @@
         <v>2.86103542234332</v>
       </c>
       <c r="DY8" t="n">
-        <v>2.46498599439775</v>
+        <v>3.92156862745098</v>
+      </c>
+      <c r="DZ8" t="n">
+        <v>5.32637075718015</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -24954,11 +25125,14 @@
       </c>
       <c r="DY9" t="n">
         <v>0.578034682080925</v>
+      </c>
+      <c r="DZ9" t="n">
+        <v>0.599999999999994</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -25342,12 +25516,15 @@
         <v>2.24503501870863</v>
       </c>
       <c r="DY10" t="n">
-        <v>2.78341013824885</v>
+        <v>2.3963133640553</v>
+      </c>
+      <c r="DZ10" t="n">
+        <v>2.34422132207188</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -25731,12 +25908,15 @@
         <v>6.01180891035963</v>
       </c>
       <c r="DY11" t="n">
-        <v>2.57186081694401</v>
+        <v>4.03429147755925</v>
+      </c>
+      <c r="DZ11" t="n">
+        <v>2.79431974347227</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -26120,12 +26300,15 @@
         <v>-0.309278350515461</v>
       </c>
       <c r="DY12" t="n">
-        <v>-0.305498981670058</v>
+        <v>-0.407331975560073</v>
+      </c>
+      <c r="DZ12" t="n">
+        <v>2.55354200988467</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -26509,12 +26692,15 @@
         <v>0</v>
       </c>
       <c r="DY13" t="n">
-        <v>0.611620795107042</v>
+        <v>1.52905198776758</v>
+      </c>
+      <c r="DZ13" t="n">
+        <v>0.54794520547946</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -26644,10 +26830,11 @@
       <c r="DW14"/>
       <c r="DX14"/>
       <c r="DY14"/>
+      <c r="DZ14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -27031,12 +27218,15 @@
         <v>1.81394143560509</v>
       </c>
       <c r="DY15" t="n">
-        <v>1.98719364098035</v>
+        <v>1.39103554868625</v>
+      </c>
+      <c r="DZ15" t="n">
+        <v>2.22408728493495</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -27420,12 +27610,15 @@
         <v>4.14239482200648</v>
       </c>
       <c r="DY16" t="n">
-        <v>2.4179104477612</v>
+        <v>2.74626865671641</v>
+      </c>
+      <c r="DZ16" t="n">
+        <v>3.35886859163229</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -27555,10 +27748,11 @@
       <c r="DW17"/>
       <c r="DX17"/>
       <c r="DY17"/>
+      <c r="DZ17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -27942,12 +28136,15 @@
         <v>6.60194174757281</v>
       </c>
       <c r="DY18" t="n">
-        <v>3.79506641366223</v>
+        <v>8.34914611005691</v>
+      </c>
+      <c r="DZ18" t="n">
+        <v>8.88157894736841</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -28331,12 +28528,15 @@
         <v>3.4782608695652</v>
       </c>
       <c r="DY19" t="n">
-        <v>2.92146877512732</v>
+        <v>3.13588850174216</v>
+      </c>
+      <c r="DZ19" t="n">
+        <v>3.68040996971815</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -28720,12 +28920,15 @@
         <v>0.528479154433339</v>
       </c>
       <c r="DY20" t="n">
-        <v>-0.62260536398468</v>
+        <v>-1.10153256704981</v>
+      </c>
+      <c r="DZ20" t="n">
+        <v>2.40963855421686</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -29109,12 +29312,15 @@
         <v>0.698080279232122</v>
       </c>
       <c r="DY21" t="n">
-        <v>1.34680134680134</v>
+        <v>0.336700336700341</v>
+      </c>
+      <c r="DZ21" t="n">
+        <v>0.995024875621895</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -29498,12 +29704,15 @@
         <v>1.37389597644749</v>
       </c>
       <c r="DY22" t="n">
-        <v>0.362318840579702</v>
+        <v>1.63043478260869</v>
+      </c>
+      <c r="DZ22" t="n">
+        <v>1.22137404580152</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -29888,11 +30097,14 @@
       </c>
       <c r="DY23" t="n">
         <v>3.07377049180326</v>
+      </c>
+      <c r="DZ23" t="n">
+        <v>2.21940393151554</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -30276,12 +30488,15 @@
         <v>2.24458204334366</v>
       </c>
       <c r="DY24" t="n">
-        <v>1.52838427947598</v>
+        <v>2.25618631732168</v>
+      </c>
+      <c r="DZ24" t="n">
+        <v>3.09278350515464</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -30666,11 +30881,14 @@
       </c>
       <c r="DY25" t="n">
         <v>0.50890585241731</v>
+      </c>
+      <c r="DZ25" t="n">
+        <v>-0.201612903225809</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -31054,12 +31272,15 @@
         <v>2.56276150627615</v>
       </c>
       <c r="DY26" t="n">
-        <v>4.42804428044281</v>
+        <v>4.21718502899313</v>
+      </c>
+      <c r="DZ26" t="n">
+        <v>3.57142857142856</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -31443,12 +31664,15 @@
         <v>1.83574879227054</v>
       </c>
       <c r="DY27" t="n">
-        <v>1.96463654223967</v>
+        <v>1.91552062868368</v>
+      </c>
+      <c r="DZ27" t="n">
+        <v>0.587248322147665</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -31832,12 +32056,15 @@
         <v>5.73606097071801</v>
       </c>
       <c r="DY28" t="n">
-        <v>5.90050134978789</v>
+        <v>5.1677593521018</v>
+      </c>
+      <c r="DZ28" t="n">
+        <v>5.43442889684347</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -32221,12 +32448,15 @@
         <v>-0.11883541295307</v>
       </c>
       <c r="DY29" t="n">
-        <v>-0.366076876143987</v>
+        <v>0.244051250762664</v>
+      </c>
+      <c r="DZ29" t="n">
+        <v>1.67451596023025</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -32610,12 +32840,15 @@
         <v>0.212089077412516</v>
       </c>
       <c r="DY30" t="n">
-        <v>0.410677618069836</v>
+        <v>2.25872689938399</v>
+      </c>
+      <c r="DZ30" t="n">
+        <v>0.965250965250951</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -32745,10 +32978,11 @@
       <c r="DW31"/>
       <c r="DX31"/>
       <c r="DY31"/>
+      <c r="DZ31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -33133,11 +33367,14 @@
       </c>
       <c r="DY32" t="n">
         <v>-3.18840579710145</v>
+      </c>
+      <c r="DZ32" t="n">
+        <v>-6.57276995305165</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -33521,12 +33758,15 @@
         <v>2.07253886010364</v>
       </c>
       <c r="DY33" t="n">
-        <v>0.876095118898609</v>
+        <v>1.3767209011264</v>
+      </c>
+      <c r="DZ33" t="n">
+        <v>1.64654226125137</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -33910,12 +34150,15 @@
         <v>5.68862275449101</v>
       </c>
       <c r="DY34" t="n">
-        <v>5.60344827586208</v>
+        <v>-0.862068965517233</v>
+      </c>
+      <c r="DZ34" t="n">
+        <v>-1.13924050632912</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -34299,12 +34542,15 @@
         <v>2.4767801857585</v>
       </c>
       <c r="DY35" t="n">
-        <v>2.73556231003039</v>
+        <v>0.607902735562319</v>
+      </c>
+      <c r="DZ35" t="n">
+        <v>2.70270270270269</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -34688,12 +34934,15 @@
         <v>3.66935483870969</v>
       </c>
       <c r="DY36" t="n">
-        <v>4.17000801924619</v>
+        <v>4.08981555733762</v>
+      </c>
+      <c r="DZ36" t="n">
+        <v>3.72777017783857</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -35077,12 +35326,15 @@
         <v>8.41584158415842</v>
       </c>
       <c r="DY37" t="n">
-        <v>1.88133140376268</v>
+        <v>3.61794500723589</v>
+      </c>
+      <c r="DZ37" t="n">
+        <v>4.95314591700136</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -35466,12 +35718,15 @@
         <v>3.25203252032521</v>
       </c>
       <c r="DY38" t="n">
-        <v>2.45561012466944</v>
+        <v>0.661125802795618</v>
+      </c>
+      <c r="DZ38" t="n">
+        <v>3.25087218522042</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -35856,11 +36111,14 @@
       </c>
       <c r="DY39" t="n">
         <v>0.632688927943745</v>
+      </c>
+      <c r="DZ39" t="n">
+        <v>0.726239343227032</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -36245,11 +36503,14 @@
       </c>
       <c r="DY40" t="n">
         <v>0</v>
+      </c>
+      <c r="DZ40" t="n">
+        <v>3.55191256830602</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -36633,12 +36894,15 @@
         <v>1.5111886079628</v>
       </c>
       <c r="DY41" t="n">
-        <v>1.90311418685122</v>
+        <v>0.865051903114187</v>
+      </c>
+      <c r="DZ41" t="n">
+        <v>1.32135306553913</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -37022,12 +37286,15 @@
         <v>-0.0816993464052357</v>
       </c>
       <c r="DY42" t="n">
-        <v>0.952380952380943</v>
+        <v>2.46031746031746</v>
+      </c>
+      <c r="DZ42" t="n">
+        <v>2.70457697642164</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -37411,12 +37678,15 @@
         <v>1.93192272309108</v>
       </c>
       <c r="DY43" t="n">
-        <v>1.806684733514</v>
+        <v>1.6260162601626</v>
+      </c>
+      <c r="DZ43" t="n">
+        <v>2.24899598393575</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -37800,12 +38070,15 @@
         <v>0.930059523809524</v>
       </c>
       <c r="DY44" t="n">
-        <v>2.05655526992287</v>
+        <v>2.0932794711715</v>
+      </c>
+      <c r="DZ44" t="n">
+        <v>-0.621310966138552</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -38189,12 +38462,15 @@
         <v>-1.7094017094017</v>
       </c>
       <c r="DY45" t="n">
-        <v>-4.64135021097046</v>
+        <v>-2.1097046413502</v>
+      </c>
+      <c r="DZ45" t="n">
+        <v>1.79211469534049</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -38578,12 +38854,15 @@
         <v>-0.747790618626781</v>
       </c>
       <c r="DY46" t="n">
-        <v>-1.00468854655057</v>
+        <v>1.00468854655057</v>
+      </c>
+      <c r="DZ46" t="n">
+        <v>-0.0620347394540908</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -38967,12 +39246,15 @@
         <v>0.355871886121001</v>
       </c>
       <c r="DY47" t="n">
-        <v>0</v>
+        <v>2.39726027397259</v>
+      </c>
+      <c r="DZ47" t="n">
+        <v>3.83561643835616</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -39356,12 +39638,15 @@
         <v>1.13977204559089</v>
       </c>
       <c r="DY48" t="n">
-        <v>0.773053561568182</v>
+        <v>0.552181115405853</v>
+      </c>
+      <c r="DZ48" t="n">
+        <v>0.632911392405055</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -39745,12 +40030,15 @@
         <v>1.43499473835263</v>
       </c>
       <c r="DY49" t="n">
-        <v>1.77631578947369</v>
+        <v>2.22744360902256</v>
+      </c>
+      <c r="DZ49" t="n">
+        <v>2.03323903818953</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -40135,11 +40423,14 @@
       </c>
       <c r="DY50" t="n">
         <v>5.28756957328386</v>
+      </c>
+      <c r="DZ50" t="n">
+        <v>4.56769983686785</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -40524,11 +40815,14 @@
       </c>
       <c r="DY51" t="n">
         <v>5.57768924302788</v>
+      </c>
+      <c r="DZ51" t="n">
+        <v>5.2117263843648</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -40912,12 +41206,15 @@
         <v>3.81132075471699</v>
       </c>
       <c r="DY52" t="n">
-        <v>4.67753366406803</v>
+        <v>3.54358610914245</v>
+      </c>
+      <c r="DZ52" t="n">
+        <v>1.75887432043492</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -41301,12 +41598,15 @@
         <v>0.349040139616061</v>
       </c>
       <c r="DY53" t="n">
-        <v>-2.52593594948128</v>
+        <v>-1.30807397383851</v>
+      </c>
+      <c r="DZ53" t="n">
+        <v>-1.82978723404256</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -41690,12 +41990,15 @@
         <v>1.57170923379176</v>
       </c>
       <c r="DY54" t="n">
-        <v>1.48148148148149</v>
+        <v>1.66666666666668</v>
+      </c>
+      <c r="DZ54" t="n">
+        <v>-0.834724540901491</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -42079,12 +42382,15 @@
         <v>0.0000000000000167284928960589</v>
       </c>
       <c r="DY55" t="n">
-        <v>-0.777511961722495</v>
+        <v>-0.239234449760752</v>
+      </c>
+      <c r="DZ55" t="n">
+        <v>2.02269363591516</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -42468,7 +42774,10 @@
         <v>-0.829875518672211</v>
       </c>
       <c r="DY56" t="n">
-        <v>-0.0000000000000144419255235793</v>
+        <v>-0.406504065040656</v>
+      </c>
+      <c r="DZ56" t="n">
+        <v>1.37931034482758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023-11-17 :: SEM Update for November
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t xml:space="preserve">08/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1347,10 +1353,16 @@
       <c r="EK4" t="s">
         <v>140</v>
       </c>
+      <c r="EL4" t="s">
+        <v>141</v>
+      </c>
+      <c r="EM4" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1767,15 +1779,21 @@
         <v>10121.8</v>
       </c>
       <c r="EJ5" t="n">
-        <v>9035.6</v>
+        <v>9039</v>
       </c>
       <c r="EK5" t="n">
-        <v>9318.1</v>
+        <v>9484.3</v>
+      </c>
+      <c r="EL5" t="n">
+        <v>10584.9</v>
+      </c>
+      <c r="EM5" t="n">
+        <v>10929</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2195,12 +2213,18 @@
         <v>160.7</v>
       </c>
       <c r="EK6" t="n">
-        <v>163.9</v>
+        <v>165</v>
+      </c>
+      <c r="EL6" t="n">
+        <v>171.5</v>
+      </c>
+      <c r="EM6" t="n">
+        <v>174.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2621,11 +2645,17 @@
       </c>
       <c r="EK7" t="n">
         <v>21.4</v>
+      </c>
+      <c r="EL7" t="n">
+        <v>27.2</v>
+      </c>
+      <c r="EM7" t="n">
+        <v>28.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3045,12 +3075,18 @@
         <v>151</v>
       </c>
       <c r="EK8" t="n">
-        <v>182.9</v>
+        <v>185.5</v>
+      </c>
+      <c r="EL8" t="n">
+        <v>200.6</v>
+      </c>
+      <c r="EM8" t="n">
+        <v>202.7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3471,11 +3507,17 @@
       </c>
       <c r="EK9" t="n">
         <v>87</v>
+      </c>
+      <c r="EL9" t="n">
+        <v>100.6</v>
+      </c>
+      <c r="EM9" t="n">
+        <v>102.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3895,12 +3937,18 @@
         <v>1065.7</v>
       </c>
       <c r="EK10" t="n">
-        <v>1115.2</v>
+        <v>1111</v>
+      </c>
+      <c r="EL10" t="n">
+        <v>1184.1</v>
+      </c>
+      <c r="EM10" t="n">
+        <v>1234.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4320,12 +4368,18 @@
         <v>197.5</v>
       </c>
       <c r="EK11" t="n">
-        <v>203.4</v>
+        <v>206.3</v>
+      </c>
+      <c r="EL11" t="n">
+        <v>224.2</v>
+      </c>
+      <c r="EM11" t="n">
+        <v>231.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4745,12 +4799,18 @@
         <v>96.7</v>
       </c>
       <c r="EK12" t="n">
-        <v>97.9</v>
+        <v>97.8</v>
+      </c>
+      <c r="EL12" t="n">
+        <v>123.5</v>
+      </c>
+      <c r="EM12" t="n">
+        <v>127.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5170,12 +5230,18 @@
         <v>33.8</v>
       </c>
       <c r="EK13" t="n">
-        <v>32.9</v>
+        <v>33.2</v>
+      </c>
+      <c r="EL13" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="EM13" t="n">
+        <v>39.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5317,10 +5383,12 @@
       <c r="EI14"/>
       <c r="EJ14"/>
       <c r="EK14"/>
+      <c r="EL14"/>
+      <c r="EM14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5740,12 +5808,18 @@
         <v>392.9</v>
       </c>
       <c r="EK15" t="n">
-        <v>461.9</v>
+        <v>459.2</v>
+      </c>
+      <c r="EL15" t="n">
+        <v>484</v>
+      </c>
+      <c r="EM15" t="n">
+        <v>491.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6165,12 +6239,18 @@
         <v>321.8</v>
       </c>
       <c r="EK16" t="n">
-        <v>343.1</v>
+        <v>344.2</v>
+      </c>
+      <c r="EL16" t="n">
+        <v>350.4</v>
+      </c>
+      <c r="EM16" t="n">
+        <v>352.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6312,10 +6392,12 @@
       <c r="EI17"/>
       <c r="EJ17"/>
       <c r="EK17"/>
+      <c r="EL17"/>
+      <c r="EM17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6735,12 +6817,18 @@
         <v>54.9</v>
       </c>
       <c r="EK18" t="n">
-        <v>54.7</v>
+        <v>57.1</v>
+      </c>
+      <c r="EL18" t="n">
+        <v>64</v>
+      </c>
+      <c r="EM18" t="n">
+        <v>67.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7160,12 +7248,18 @@
         <v>380.8</v>
       </c>
       <c r="EK19" t="n">
-        <v>384</v>
+        <v>384.8</v>
+      </c>
+      <c r="EL19" t="n">
+        <v>445</v>
+      </c>
+      <c r="EM19" t="n">
+        <v>456.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7585,12 +7679,18 @@
         <v>171.2</v>
       </c>
       <c r="EK20" t="n">
-        <v>207.5</v>
+        <v>206.5</v>
+      </c>
+      <c r="EL20" t="n">
+        <v>229.5</v>
+      </c>
+      <c r="EM20" t="n">
+        <v>235.3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8010,12 +8110,18 @@
         <v>115.4</v>
       </c>
       <c r="EK21" t="n">
-        <v>120.4</v>
+        <v>119.2</v>
+      </c>
+      <c r="EL21" t="n">
+        <v>142.1</v>
+      </c>
+      <c r="EM21" t="n">
+        <v>147.9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8435,12 +8541,18 @@
         <v>103.3</v>
       </c>
       <c r="EK22" t="n">
-        <v>110.8</v>
+        <v>112.2</v>
+      </c>
+      <c r="EL22" t="n">
+        <v>132.9</v>
+      </c>
+      <c r="EM22" t="n">
+        <v>138.6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8861,11 +8973,17 @@
       </c>
       <c r="EK23" t="n">
         <v>150.9</v>
+      </c>
+      <c r="EL23" t="n">
+        <v>161.2</v>
+      </c>
+      <c r="EM23" t="n">
+        <v>163.4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9285,12 +9403,18 @@
         <v>132.1</v>
       </c>
       <c r="EK24" t="n">
-        <v>139.5</v>
+        <v>140.5</v>
+      </c>
+      <c r="EL24" t="n">
+        <v>150.1</v>
+      </c>
+      <c r="EM24" t="n">
+        <v>151.8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9711,11 +9835,17 @@
       </c>
       <c r="EK25" t="n">
         <v>39.5</v>
+      </c>
+      <c r="EL25" t="n">
+        <v>50</v>
+      </c>
+      <c r="EM25" t="n">
+        <v>51.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10135,12 +10265,18 @@
         <v>196.1</v>
       </c>
       <c r="EK26" t="n">
-        <v>198.1</v>
+        <v>197.7</v>
+      </c>
+      <c r="EL26" t="n">
+        <v>219.8</v>
+      </c>
+      <c r="EM26" t="n">
+        <v>224.9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10560,12 +10696,18 @@
         <v>210.8</v>
       </c>
       <c r="EK27" t="n">
-        <v>207.6</v>
+        <v>207.5</v>
+      </c>
+      <c r="EL27" t="n">
+        <v>240</v>
+      </c>
+      <c r="EM27" t="n">
+        <v>247.9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10985,12 +11127,18 @@
         <v>263.6</v>
       </c>
       <c r="EK28" t="n">
-        <v>274.6</v>
+        <v>272.7</v>
+      </c>
+      <c r="EL28" t="n">
+        <v>324</v>
+      </c>
+      <c r="EM28" t="n">
+        <v>334.1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11410,12 +11558,18 @@
         <v>168.1</v>
       </c>
       <c r="EK29" t="n">
-        <v>163.3</v>
+        <v>164.3</v>
+      </c>
+      <c r="EL29" t="n">
+        <v>194</v>
+      </c>
+      <c r="EM29" t="n">
+        <v>207.3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11835,12 +11989,18 @@
         <v>94.5</v>
       </c>
       <c r="EK30" t="n">
-        <v>97.8</v>
+        <v>99.6</v>
+      </c>
+      <c r="EL30" t="n">
+        <v>104.6</v>
+      </c>
+      <c r="EM30" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11982,10 +12142,12 @@
       <c r="EI31"/>
       <c r="EJ31"/>
       <c r="EK31"/>
+      <c r="EL31"/>
+      <c r="EM31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12406,11 +12568,17 @@
       </c>
       <c r="EK32" t="n">
         <v>33.4</v>
+      </c>
+      <c r="EL32" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="EM32" t="n">
+        <v>42.4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12830,12 +12998,18 @@
         <v>78.8</v>
       </c>
       <c r="EK33" t="n">
-        <v>80.6</v>
+        <v>81</v>
+      </c>
+      <c r="EL33" t="n">
+        <v>92.7</v>
+      </c>
+      <c r="EM33" t="n">
+        <v>96</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -13255,12 +13429,18 @@
         <v>70.6</v>
       </c>
       <c r="EK34" t="n">
-        <v>73.5</v>
+        <v>69</v>
+      </c>
+      <c r="EL34" t="n">
+        <v>82.7</v>
+      </c>
+      <c r="EM34" t="n">
+        <v>85.2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13680,12 +13860,18 @@
         <v>33.1</v>
       </c>
       <c r="EK35" t="n">
-        <v>33.8</v>
+        <v>33.1</v>
+      </c>
+      <c r="EL35" t="n">
+        <v>45.3</v>
+      </c>
+      <c r="EM35" t="n">
+        <v>46.6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14105,12 +14291,18 @@
         <v>257.1</v>
       </c>
       <c r="EK36" t="n">
-        <v>259.8</v>
+        <v>259.6</v>
+      </c>
+      <c r="EL36" t="n">
+        <v>303.8</v>
+      </c>
+      <c r="EM36" t="n">
+        <v>323.7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14530,12 +14722,18 @@
         <v>65.7</v>
       </c>
       <c r="EK37" t="n">
-        <v>70.4</v>
+        <v>71.6</v>
+      </c>
+      <c r="EL37" t="n">
+        <v>78.6</v>
+      </c>
+      <c r="EM37" t="n">
+        <v>81.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14955,12 +15153,18 @@
         <v>546.1</v>
       </c>
       <c r="EK38" t="n">
-        <v>542.4</v>
+        <v>532.9</v>
+      </c>
+      <c r="EL38" t="n">
+        <v>651.1</v>
+      </c>
+      <c r="EM38" t="n">
+        <v>675.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -15381,11 +15585,17 @@
       </c>
       <c r="EK39" t="n">
         <v>286.3</v>
+      </c>
+      <c r="EL39" t="n">
+        <v>319</v>
+      </c>
+      <c r="EM39" t="n">
+        <v>327.3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15806,11 +16016,17 @@
       </c>
       <c r="EK40" t="n">
         <v>28.8</v>
+      </c>
+      <c r="EL40" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="EM40" t="n">
+        <v>39.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -16230,12 +16446,18 @@
         <v>349.3</v>
       </c>
       <c r="EK41" t="n">
-        <v>353.4</v>
+        <v>349.8</v>
+      </c>
+      <c r="EL41" t="n">
+        <v>383.8</v>
+      </c>
+      <c r="EM41" t="n">
+        <v>394.5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16655,12 +16877,18 @@
         <v>122.3</v>
       </c>
       <c r="EK42" t="n">
-        <v>127.2</v>
+        <v>129.1</v>
+      </c>
+      <c r="EL42" t="n">
+        <v>149.6</v>
+      </c>
+      <c r="EM42" t="n">
+        <v>153.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -17080,12 +17308,18 @@
         <v>110.8</v>
       </c>
       <c r="EK43" t="n">
-        <v>112.7</v>
+        <v>112.5</v>
+      </c>
+      <c r="EL43" t="n">
+        <v>126.9</v>
+      </c>
+      <c r="EM43" t="n">
+        <v>137.6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17505,12 +17739,18 @@
         <v>271.3</v>
       </c>
       <c r="EK44" t="n">
-        <v>277.9</v>
+        <v>278</v>
+      </c>
+      <c r="EL44" t="n">
+        <v>319.4</v>
+      </c>
+      <c r="EM44" t="n">
+        <v>327.8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17930,12 +18170,18 @@
         <v>23</v>
       </c>
       <c r="EK45" t="n">
-        <v>22.6</v>
+        <v>23.2</v>
+      </c>
+      <c r="EL45" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="EM45" t="n">
+        <v>29.7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -18355,12 +18601,18 @@
         <v>146</v>
       </c>
       <c r="EK46" t="n">
-        <v>147.8</v>
+        <v>150.8</v>
+      </c>
+      <c r="EL46" t="n">
+        <v>161</v>
+      </c>
+      <c r="EM46" t="n">
+        <v>164.2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18780,12 +19032,18 @@
         <v>28.2</v>
       </c>
       <c r="EK47" t="n">
-        <v>29.2</v>
+        <v>29.9</v>
+      </c>
+      <c r="EL47" t="n">
+        <v>37.3</v>
+      </c>
+      <c r="EM47" t="n">
+        <v>38.7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -19205,12 +19463,18 @@
         <v>168.6</v>
       </c>
       <c r="EK48" t="n">
-        <v>182.5</v>
+        <v>182.1</v>
+      </c>
+      <c r="EL48" t="n">
+        <v>206.7</v>
+      </c>
+      <c r="EM48" t="n">
+        <v>212.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -19630,12 +19894,18 @@
         <v>1060.3</v>
       </c>
       <c r="EK49" t="n">
-        <v>1082.9</v>
+        <v>1087.7</v>
+      </c>
+      <c r="EL49" t="n">
+        <v>1156.5</v>
+      </c>
+      <c r="EM49" t="n">
+        <v>1191.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -20056,11 +20326,17 @@
       </c>
       <c r="EK50" t="n">
         <v>113.5</v>
+      </c>
+      <c r="EL50" t="n">
+        <v>128.2</v>
+      </c>
+      <c r="EM50" t="n">
+        <v>132</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -20481,11 +20757,17 @@
       </c>
       <c r="EK51" t="n">
         <v>26.5</v>
+      </c>
+      <c r="EL51" t="n">
+        <v>32.8</v>
+      </c>
+      <c r="EM51" t="n">
+        <v>34.1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20905,12 +21187,18 @@
         <v>275.1</v>
       </c>
       <c r="EK52" t="n">
-        <v>295.4</v>
+        <v>292.2</v>
+      </c>
+      <c r="EL52" t="n">
+        <v>324.4</v>
+      </c>
+      <c r="EM52" t="n">
+        <v>328.6</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -21330,12 +21618,18 @@
         <v>230</v>
       </c>
       <c r="EK53" t="n">
-        <v>216.1</v>
+        <v>218.8</v>
+      </c>
+      <c r="EL53" t="n">
+        <v>228.8</v>
+      </c>
+      <c r="EM53" t="n">
+        <v>248.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -21755,12 +22049,18 @@
         <v>51.7</v>
       </c>
       <c r="EK54" t="n">
-        <v>54.8</v>
+        <v>54.9</v>
+      </c>
+      <c r="EL54" t="n">
+        <v>59.4</v>
+      </c>
+      <c r="EM54" t="n">
+        <v>61.3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -22180,12 +22480,18 @@
         <v>169.9</v>
       </c>
       <c r="EK55" t="n">
-        <v>165.9</v>
+        <v>166.8</v>
+      </c>
+      <c r="EL55" t="n">
+        <v>207</v>
+      </c>
+      <c r="EM55" t="n">
+        <v>216.9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -22605,7 +22911,13 @@
         <v>23.9</v>
       </c>
       <c r="EK56" t="n">
-        <v>24.6</v>
+        <v>24.5</v>
+      </c>
+      <c r="EL56" t="n">
+        <v>29.2</v>
+      </c>
+      <c r="EM56" t="n">
+        <v>30.3</v>
       </c>
     </row>
   </sheetData>
@@ -23010,10 +23322,16 @@
       <c r="DY4" t="s">
         <v>140</v>
       </c>
+      <c r="DZ4" t="s">
+        <v>141</v>
+      </c>
+      <c r="EA4" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -23394,15 +23712,21 @@
         <v>2.4888618874038</v>
       </c>
       <c r="DX5" t="n">
-        <v>1.66180987634875</v>
+        <v>1.7000641321347</v>
       </c>
       <c r="DY5" t="n">
-        <v>0.572039157699323</v>
+        <v>2.36586761071115</v>
+      </c>
+      <c r="DZ5" t="n">
+        <v>2.35263402181482</v>
+      </c>
+      <c r="EA5" t="n">
+        <v>2.60719348811883</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -23786,12 +24110,18 @@
         <v>0</v>
       </c>
       <c r="DY6" t="n">
-        <v>0</v>
+        <v>0.671140939597312</v>
+      </c>
+      <c r="DZ6" t="n">
+        <v>0.823045267489715</v>
+      </c>
+      <c r="EA6" t="n">
+        <v>0.694042799305951</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -24176,11 +24506,17 @@
       </c>
       <c r="DY7" t="n">
         <v>0.0000000000000166014657887874</v>
+      </c>
+      <c r="DZ7" t="n">
+        <v>0.740740740740751</v>
+      </c>
+      <c r="EA7" t="n">
+        <v>0.714285714285724</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -24564,12 +24900,18 @@
         <v>2.86103542234332</v>
       </c>
       <c r="DY8" t="n">
-        <v>2.46498599439775</v>
+        <v>3.92156862745098</v>
+      </c>
+      <c r="DZ8" t="n">
+        <v>4.75195822454308</v>
+      </c>
+      <c r="EA8" t="n">
+        <v>4.26954732510289</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -24954,11 +25296,17 @@
       </c>
       <c r="DY9" t="n">
         <v>0.578034682080925</v>
+      </c>
+      <c r="DZ9" t="n">
+        <v>0.599999999999994</v>
+      </c>
+      <c r="EA9" t="n">
+        <v>0.293255131964821</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -25342,12 +25690,18 @@
         <v>2.24503501870863</v>
       </c>
       <c r="DY10" t="n">
-        <v>2.78341013824885</v>
+        <v>2.3963133640553</v>
+      </c>
+      <c r="DZ10" t="n">
+        <v>2.05119365681289</v>
+      </c>
+      <c r="EA10" t="n">
+        <v>1.76451187335093</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -25731,12 +26085,18 @@
         <v>6.01180891035963</v>
       </c>
       <c r="DY11" t="n">
-        <v>2.57186081694401</v>
+        <v>4.03429147755925</v>
+      </c>
+      <c r="DZ11" t="n">
+        <v>2.70270270270269</v>
+      </c>
+      <c r="EA11" t="n">
+        <v>3.75838926174497</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -26120,12 +26480,18 @@
         <v>-0.309278350515461</v>
       </c>
       <c r="DY12" t="n">
-        <v>-0.305498981670058</v>
+        <v>-0.407331975560073</v>
+      </c>
+      <c r="DZ12" t="n">
+        <v>1.72981878088962</v>
+      </c>
+      <c r="EA12" t="n">
+        <v>2.08333333333334</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -26509,12 +26875,18 @@
         <v>0</v>
       </c>
       <c r="DY13" t="n">
-        <v>0.611620795107042</v>
+        <v>1.52905198776758</v>
+      </c>
+      <c r="DZ13" t="n">
+        <v>3.83561643835616</v>
+      </c>
+      <c r="EA13" t="n">
+        <v>5.61497326203209</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -26644,10 +27016,12 @@
       <c r="DW14"/>
       <c r="DX14"/>
       <c r="DY14"/>
+      <c r="DZ14"/>
+      <c r="EA14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -27031,12 +27405,18 @@
         <v>1.81394143560509</v>
       </c>
       <c r="DY15" t="n">
-        <v>1.98719364098035</v>
+        <v>1.39103554868625</v>
+      </c>
+      <c r="DZ15" t="n">
+        <v>1.55266470835081</v>
+      </c>
+      <c r="EA15" t="n">
+        <v>1.80310880829015</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -27420,12 +27800,18 @@
         <v>4.14239482200648</v>
       </c>
       <c r="DY16" t="n">
-        <v>2.4179104477612</v>
+        <v>2.74626865671641</v>
+      </c>
+      <c r="DZ16" t="n">
+        <v>3.24101355332941</v>
+      </c>
+      <c r="EA16" t="n">
+        <v>3.09669880222026</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -27555,10 +27941,12 @@
       <c r="DW17"/>
       <c r="DX17"/>
       <c r="DY17"/>
+      <c r="DZ17"/>
+      <c r="EA17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -27942,12 +28330,18 @@
         <v>6.60194174757281</v>
       </c>
       <c r="DY18" t="n">
-        <v>3.79506641366223</v>
+        <v>8.34914611005691</v>
+      </c>
+      <c r="DZ18" t="n">
+        <v>5.26315789473685</v>
+      </c>
+      <c r="EA18" t="n">
+        <v>6.61417322834646</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -28331,12 +28725,18 @@
         <v>3.4782608695652</v>
       </c>
       <c r="DY19" t="n">
-        <v>2.92146877512732</v>
+        <v>3.13588850174216</v>
+      </c>
+      <c r="DZ19" t="n">
+        <v>3.65711623573259</v>
+      </c>
+      <c r="EA19" t="n">
+        <v>3.65576748410536</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -28720,12 +29120,18 @@
         <v>0.528479154433339</v>
       </c>
       <c r="DY20" t="n">
-        <v>-0.62260536398468</v>
+        <v>-1.10153256704981</v>
+      </c>
+      <c r="DZ20" t="n">
+        <v>2.40963855421686</v>
+      </c>
+      <c r="EA20" t="n">
+        <v>4.1611332447986</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -29109,12 +29515,18 @@
         <v>0.698080279232122</v>
       </c>
       <c r="DY21" t="n">
-        <v>1.34680134680134</v>
+        <v>0.336700336700341</v>
+      </c>
+      <c r="DZ21" t="n">
+        <v>0.995024875621895</v>
+      </c>
+      <c r="EA21" t="n">
+        <v>1.37080191912269</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -29498,12 +29910,18 @@
         <v>1.37389597644749</v>
       </c>
       <c r="DY22" t="n">
-        <v>0.362318840579702</v>
+        <v>1.63043478260869</v>
+      </c>
+      <c r="DZ22" t="n">
+        <v>1.45038167938932</v>
+      </c>
+      <c r="EA22" t="n">
+        <v>2.28782287822878</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -29888,11 +30306,17 @@
       </c>
       <c r="DY23" t="n">
         <v>3.07377049180326</v>
+      </c>
+      <c r="DZ23" t="n">
+        <v>2.21940393151554</v>
+      </c>
+      <c r="EA23" t="n">
+        <v>2.31684408265499</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -30276,12 +30700,18 @@
         <v>2.24458204334366</v>
       </c>
       <c r="DY24" t="n">
-        <v>1.52838427947598</v>
+        <v>2.25618631732168</v>
+      </c>
+      <c r="DZ24" t="n">
+        <v>3.1615120274914</v>
+      </c>
+      <c r="EA24" t="n">
+        <v>2.22222222222223</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -30666,11 +31096,17 @@
       </c>
       <c r="DY25" t="n">
         <v>0.50890585241731</v>
+      </c>
+      <c r="DZ25" t="n">
+        <v>0.806451612903223</v>
+      </c>
+      <c r="EA25" t="n">
+        <v>1.17878192534381</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -31054,12 +31490,18 @@
         <v>2.56276150627615</v>
       </c>
       <c r="DY26" t="n">
-        <v>4.42804428044281</v>
+        <v>4.21718502899313</v>
+      </c>
+      <c r="DZ26" t="n">
+        <v>3.28947368421053</v>
+      </c>
+      <c r="EA26" t="n">
+        <v>3.68833563854311</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -31443,12 +31885,18 @@
         <v>1.83574879227054</v>
       </c>
       <c r="DY27" t="n">
-        <v>1.96463654223967</v>
+        <v>1.91552062868368</v>
+      </c>
+      <c r="DZ27" t="n">
+        <v>0.671140939597325</v>
+      </c>
+      <c r="EA27" t="n">
+        <v>0.731409995936604</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -31832,12 +32280,18 @@
         <v>5.73606097071801</v>
       </c>
       <c r="DY28" t="n">
-        <v>5.90050134978789</v>
+        <v>5.1677593521018</v>
+      </c>
+      <c r="DZ28" t="n">
+        <v>5.43442889684347</v>
+      </c>
+      <c r="EA28" t="n">
+        <v>4.47154471544716</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -32221,12 +32675,18 @@
         <v>-0.11883541295307</v>
       </c>
       <c r="DY29" t="n">
-        <v>-0.366076876143987</v>
+        <v>0.244051250762664</v>
+      </c>
+      <c r="DZ29" t="n">
+        <v>1.51753008895866</v>
+      </c>
+      <c r="EA29" t="n">
+        <v>1.76730486008838</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -32610,12 +33070,18 @@
         <v>0.212089077412516</v>
       </c>
       <c r="DY30" t="n">
-        <v>0.410677618069836</v>
+        <v>2.25872689938399</v>
+      </c>
+      <c r="DZ30" t="n">
+        <v>0.965250965250951</v>
+      </c>
+      <c r="EA30" t="n">
+        <v>0.767754318618053</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -32745,10 +33211,12 @@
       <c r="DW31"/>
       <c r="DX31"/>
       <c r="DY31"/>
+      <c r="DZ31"/>
+      <c r="EA31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -33133,11 +33601,17 @@
       </c>
       <c r="DY32" t="n">
         <v>-3.18840579710145</v>
+      </c>
+      <c r="DZ32" t="n">
+        <v>-4.46009389671361</v>
+      </c>
+      <c r="EA32" t="n">
+        <v>-2.97482837528605</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -33521,12 +33995,18 @@
         <v>2.07253886010364</v>
       </c>
       <c r="DY33" t="n">
-        <v>0.876095118898609</v>
+        <v>1.3767209011264</v>
+      </c>
+      <c r="DZ33" t="n">
+        <v>1.75631174533479</v>
+      </c>
+      <c r="EA33" t="n">
+        <v>1.15911485774499</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -33910,12 +34390,18 @@
         <v>5.68862275449101</v>
       </c>
       <c r="DY34" t="n">
-        <v>5.60344827586208</v>
+        <v>-0.862068965517233</v>
+      </c>
+      <c r="DZ34" t="n">
+        <v>4.68354430379747</v>
+      </c>
+      <c r="EA34" t="n">
+        <v>5.97014925373134</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -34299,12 +34785,18 @@
         <v>2.4767801857585</v>
       </c>
       <c r="DY35" t="n">
-        <v>2.73556231003039</v>
+        <v>0.607902735562319</v>
+      </c>
+      <c r="DZ35" t="n">
+        <v>2.02702702702702</v>
+      </c>
+      <c r="EA35" t="n">
+        <v>1.96936542669582</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -34688,12 +35180,18 @@
         <v>3.66935483870969</v>
       </c>
       <c r="DY36" t="n">
-        <v>4.17000801924619</v>
+        <v>4.08981555733762</v>
+      </c>
+      <c r="DZ36" t="n">
+        <v>3.89876880984951</v>
+      </c>
+      <c r="EA36" t="n">
+        <v>5.19987000324994</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -35077,12 +35575,18 @@
         <v>8.41584158415842</v>
       </c>
       <c r="DY37" t="n">
-        <v>1.88133140376268</v>
+        <v>3.61794500723589</v>
+      </c>
+      <c r="DZ37" t="n">
+        <v>5.22088353413655</v>
+      </c>
+      <c r="EA37" t="n">
+        <v>7.67195767195769</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -35466,12 +35970,18 @@
         <v>3.25203252032521</v>
       </c>
       <c r="DY38" t="n">
-        <v>2.45561012466944</v>
+        <v>0.661125802795618</v>
+      </c>
+      <c r="DZ38" t="n">
+        <v>3.25087218522042</v>
+      </c>
+      <c r="EA38" t="n">
+        <v>0.640739085084183</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -35856,11 +36366,17 @@
       </c>
       <c r="DY39" t="n">
         <v>0.632688927943745</v>
+      </c>
+      <c r="DZ39" t="n">
+        <v>0.726239343227032</v>
+      </c>
+      <c r="EA39" t="n">
+        <v>1.48837209302326</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -36245,11 +36761,17 @@
       </c>
       <c r="DY40" t="n">
         <v>0</v>
+      </c>
+      <c r="DZ40" t="n">
+        <v>3.55191256830602</v>
+      </c>
+      <c r="EA40" t="n">
+        <v>3.64583333333333</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -36633,12 +37155,18 @@
         <v>1.5111886079628</v>
       </c>
       <c r="DY41" t="n">
-        <v>1.90311418685122</v>
+        <v>0.865051903114187</v>
+      </c>
+      <c r="DZ41" t="n">
+        <v>1.42706131078225</v>
+      </c>
+      <c r="EA41" t="n">
+        <v>1.15384615384615</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -37022,12 +37550,18 @@
         <v>-0.0816993464052357</v>
       </c>
       <c r="DY42" t="n">
-        <v>0.952380952380943</v>
+        <v>2.46031746031746</v>
+      </c>
+      <c r="DZ42" t="n">
+        <v>3.74479889042996</v>
+      </c>
+      <c r="EA42" t="n">
+        <v>4.70668485675307</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -37411,12 +37945,18 @@
         <v>1.93192272309108</v>
       </c>
       <c r="DY43" t="n">
-        <v>1.806684733514</v>
+        <v>1.6260162601626</v>
+      </c>
+      <c r="DZ43" t="n">
+        <v>1.9277108433735</v>
+      </c>
+      <c r="EA43" t="n">
+        <v>1.54981549815498</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -37800,12 +38340,18 @@
         <v>0.930059523809524</v>
       </c>
       <c r="DY44" t="n">
-        <v>2.05655526992287</v>
+        <v>2.0932794711715</v>
+      </c>
+      <c r="DZ44" t="n">
+        <v>-0.77663870767319</v>
+      </c>
+      <c r="EA44" t="n">
+        <v>-0.485731633272641</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -38189,12 +38735,18 @@
         <v>-1.7094017094017</v>
       </c>
       <c r="DY45" t="n">
-        <v>-4.64135021097046</v>
+        <v>-2.1097046413502</v>
+      </c>
+      <c r="DZ45" t="n">
+        <v>1.4336917562724</v>
+      </c>
+      <c r="EA45" t="n">
+        <v>3.12500000000001</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -38578,12 +39130,18 @@
         <v>-0.747790618626781</v>
       </c>
       <c r="DY46" t="n">
-        <v>-1.00468854655057</v>
+        <v>1.00468854655057</v>
+      </c>
+      <c r="DZ46" t="n">
+        <v>-0.124069478908182</v>
+      </c>
+      <c r="EA46" t="n">
+        <v>0.121951219512188</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -38967,12 +39525,18 @@
         <v>0.355871886121001</v>
       </c>
       <c r="DY47" t="n">
-        <v>0</v>
+        <v>2.39726027397259</v>
+      </c>
+      <c r="DZ47" t="n">
+        <v>2.1917808219178</v>
+      </c>
+      <c r="EA47" t="n">
+        <v>1.8421052631579</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -39356,12 +39920,18 @@
         <v>1.13977204559089</v>
       </c>
       <c r="DY48" t="n">
-        <v>0.773053561568182</v>
+        <v>0.552181115405853</v>
+      </c>
+      <c r="DZ48" t="n">
+        <v>0.632911392405055</v>
+      </c>
+      <c r="EA48" t="n">
+        <v>1.9664268585132</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -39745,12 +40315,18 @@
         <v>1.43499473835263</v>
       </c>
       <c r="DY49" t="n">
-        <v>1.77631578947369</v>
+        <v>2.22744360902256</v>
+      </c>
+      <c r="DZ49" t="n">
+        <v>2.23656294200848</v>
+      </c>
+      <c r="EA49" t="n">
+        <v>1.86308862490387</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -40135,11 +40711,17 @@
       </c>
       <c r="DY50" t="n">
         <v>5.28756957328386</v>
+      </c>
+      <c r="DZ50" t="n">
+        <v>4.56769983686785</v>
+      </c>
+      <c r="EA50" t="n">
+        <v>4.5958795562599</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -40524,11 +41106,17 @@
       </c>
       <c r="DY51" t="n">
         <v>5.57768924302788</v>
+      </c>
+      <c r="DZ51" t="n">
+        <v>6.84039087947881</v>
+      </c>
+      <c r="EA51" t="n">
+        <v>6.23052959501558</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -40912,12 +41500,18 @@
         <v>3.81132075471699</v>
       </c>
       <c r="DY52" t="n">
-        <v>4.67753366406803</v>
+        <v>3.54358610914245</v>
+      </c>
+      <c r="DZ52" t="n">
+        <v>3.74160537256156</v>
+      </c>
+      <c r="EA52" t="n">
+        <v>3.92156862745099</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -41301,12 +41895,18 @@
         <v>0.349040139616061</v>
       </c>
       <c r="DY53" t="n">
-        <v>-2.52593594948128</v>
+        <v>-1.30807397383851</v>
+      </c>
+      <c r="DZ53" t="n">
+        <v>-2.63829787234042</v>
+      </c>
+      <c r="EA53" t="n">
+        <v>-0.241157556270094</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -41690,12 +42290,18 @@
         <v>1.57170923379176</v>
       </c>
       <c r="DY54" t="n">
-        <v>1.48148148148149</v>
+        <v>1.66666666666668</v>
+      </c>
+      <c r="DZ54" t="n">
+        <v>-0.834724540901491</v>
+      </c>
+      <c r="EA54" t="n">
+        <v>-0.648298217179912</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -42079,12 +42685,18 @@
         <v>0.0000000000000167284928960589</v>
       </c>
       <c r="DY55" t="n">
-        <v>-0.777511961722495</v>
+        <v>-0.239234449760752</v>
+      </c>
+      <c r="DZ55" t="n">
+        <v>2.12136161815491</v>
+      </c>
+      <c r="EA55" t="n">
+        <v>2.26308345120227</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -42468,7 +43080,13 @@
         <v>-0.829875518672211</v>
       </c>
       <c r="DY56" t="n">
-        <v>-0.0000000000000144419255235793</v>
+        <v>-0.406504065040656</v>
+      </c>
+      <c r="DZ56" t="n">
+        <v>0.689655172413803</v>
+      </c>
+      <c r="EA56" t="n">
+        <v>0.664451827242522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on November 17th, 2023
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -433,6 +433,15 @@
   </si>
   <si>
     <t xml:space="preserve">07/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1341,10 +1350,19 @@
       <c r="EJ4" t="s">
         <v>139</v>
       </c>
+      <c r="EK4" t="s">
+        <v>140</v>
+      </c>
+      <c r="EL4" t="s">
+        <v>141</v>
+      </c>
+      <c r="EM4" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1758,15 +1776,24 @@
         <v>10720.3</v>
       </c>
       <c r="EI5" t="n">
-        <v>10139.8</v>
+        <v>10121.8</v>
       </c>
       <c r="EJ5" t="n">
-        <v>9046.6</v>
+        <v>9039</v>
+      </c>
+      <c r="EK5" t="n">
+        <v>9484.3</v>
+      </c>
+      <c r="EL5" t="n">
+        <v>10584.9</v>
+      </c>
+      <c r="EM5" t="n">
+        <v>10929</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2183,12 +2210,21 @@
         <v>169.2</v>
       </c>
       <c r="EJ6" t="n">
-        <v>160.8</v>
+        <v>160.7</v>
+      </c>
+      <c r="EK6" t="n">
+        <v>165</v>
+      </c>
+      <c r="EL6" t="n">
+        <v>171.5</v>
+      </c>
+      <c r="EM6" t="n">
+        <v>174.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2606,11 +2642,20 @@
       </c>
       <c r="EJ7" t="n">
         <v>19.3</v>
+      </c>
+      <c r="EK7" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="EL7" t="n">
+        <v>27.2</v>
+      </c>
+      <c r="EM7" t="n">
+        <v>28.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3027,12 +3072,21 @@
         <v>152.7</v>
       </c>
       <c r="EJ8" t="n">
-        <v>151.9</v>
+        <v>151</v>
+      </c>
+      <c r="EK8" t="n">
+        <v>185.5</v>
+      </c>
+      <c r="EL8" t="n">
+        <v>200.6</v>
+      </c>
+      <c r="EM8" t="n">
+        <v>202.7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3450,11 +3504,20 @@
       </c>
       <c r="EJ9" t="n">
         <v>82.2</v>
+      </c>
+      <c r="EK9" t="n">
+        <v>87</v>
+      </c>
+      <c r="EL9" t="n">
+        <v>100.6</v>
+      </c>
+      <c r="EM9" t="n">
+        <v>102.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3871,12 +3934,21 @@
         <v>1234.6</v>
       </c>
       <c r="EJ10" t="n">
-        <v>1074.5</v>
+        <v>1065.7</v>
+      </c>
+      <c r="EK10" t="n">
+        <v>1111</v>
+      </c>
+      <c r="EL10" t="n">
+        <v>1184.1</v>
+      </c>
+      <c r="EM10" t="n">
+        <v>1234.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4293,12 +4365,21 @@
         <v>211.2</v>
       </c>
       <c r="EJ11" t="n">
-        <v>197</v>
+        <v>197.5</v>
+      </c>
+      <c r="EK11" t="n">
+        <v>206.3</v>
+      </c>
+      <c r="EL11" t="n">
+        <v>224.2</v>
+      </c>
+      <c r="EM11" t="n">
+        <v>231.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4716,11 +4797,20 @@
       </c>
       <c r="EJ12" t="n">
         <v>96.7</v>
+      </c>
+      <c r="EK12" t="n">
+        <v>97.8</v>
+      </c>
+      <c r="EL12" t="n">
+        <v>123.5</v>
+      </c>
+      <c r="EM12" t="n">
+        <v>127.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5137,12 +5227,21 @@
         <v>35.2</v>
       </c>
       <c r="EJ13" t="n">
-        <v>34.1</v>
+        <v>33.8</v>
+      </c>
+      <c r="EK13" t="n">
+        <v>33.2</v>
+      </c>
+      <c r="EL13" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="EM13" t="n">
+        <v>39.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5283,10 +5382,13 @@
       <c r="EH14"/>
       <c r="EI14"/>
       <c r="EJ14"/>
+      <c r="EK14"/>
+      <c r="EL14"/>
+      <c r="EM14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5703,12 +5805,21 @@
         <v>399.2</v>
       </c>
       <c r="EJ15" t="n">
-        <v>393</v>
+        <v>392.9</v>
+      </c>
+      <c r="EK15" t="n">
+        <v>459.2</v>
+      </c>
+      <c r="EL15" t="n">
+        <v>484</v>
+      </c>
+      <c r="EM15" t="n">
+        <v>491.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6125,12 +6236,21 @@
         <v>335.3</v>
       </c>
       <c r="EJ16" t="n">
-        <v>320</v>
+        <v>321.8</v>
+      </c>
+      <c r="EK16" t="n">
+        <v>344.2</v>
+      </c>
+      <c r="EL16" t="n">
+        <v>350.4</v>
+      </c>
+      <c r="EM16" t="n">
+        <v>352.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6271,10 +6391,13 @@
       <c r="EH17"/>
       <c r="EI17"/>
       <c r="EJ17"/>
+      <c r="EK17"/>
+      <c r="EL17"/>
+      <c r="EM17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6692,11 +6815,20 @@
       </c>
       <c r="EJ18" t="n">
         <v>54.9</v>
+      </c>
+      <c r="EK18" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="EL18" t="n">
+        <v>64</v>
+      </c>
+      <c r="EM18" t="n">
+        <v>67.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7113,12 +7245,21 @@
         <v>408.7</v>
       </c>
       <c r="EJ19" t="n">
-        <v>380.6</v>
+        <v>380.8</v>
+      </c>
+      <c r="EK19" t="n">
+        <v>384.8</v>
+      </c>
+      <c r="EL19" t="n">
+        <v>445</v>
+      </c>
+      <c r="EM19" t="n">
+        <v>456.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7535,12 +7676,21 @@
         <v>185.5</v>
       </c>
       <c r="EJ20" t="n">
-        <v>167.8</v>
+        <v>171.2</v>
+      </c>
+      <c r="EK20" t="n">
+        <v>206.5</v>
+      </c>
+      <c r="EL20" t="n">
+        <v>229.5</v>
+      </c>
+      <c r="EM20" t="n">
+        <v>235.3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -7957,12 +8107,21 @@
         <v>132.2</v>
       </c>
       <c r="EJ21" t="n">
-        <v>114.6</v>
+        <v>115.4</v>
+      </c>
+      <c r="EK21" t="n">
+        <v>119.2</v>
+      </c>
+      <c r="EL21" t="n">
+        <v>142.1</v>
+      </c>
+      <c r="EM21" t="n">
+        <v>147.9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8379,12 +8538,21 @@
         <v>119.9</v>
       </c>
       <c r="EJ22" t="n">
-        <v>102.6</v>
+        <v>103.3</v>
+      </c>
+      <c r="EK22" t="n">
+        <v>112.2</v>
+      </c>
+      <c r="EL22" t="n">
+        <v>132.9</v>
+      </c>
+      <c r="EM22" t="n">
+        <v>138.6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8801,12 +8969,21 @@
         <v>151.1</v>
       </c>
       <c r="EJ23" t="n">
-        <v>126.9</v>
+        <v>127.7</v>
+      </c>
+      <c r="EK23" t="n">
+        <v>150.9</v>
+      </c>
+      <c r="EL23" t="n">
+        <v>161.2</v>
+      </c>
+      <c r="EM23" t="n">
+        <v>163.4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9223,12 +9400,21 @@
         <v>139.1</v>
       </c>
       <c r="EJ24" t="n">
-        <v>131.9</v>
+        <v>132.1</v>
+      </c>
+      <c r="EK24" t="n">
+        <v>140.5</v>
+      </c>
+      <c r="EL24" t="n">
+        <v>150.1</v>
+      </c>
+      <c r="EM24" t="n">
+        <v>151.8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9646,11 +9832,20 @@
       </c>
       <c r="EJ25" t="n">
         <v>40.7</v>
+      </c>
+      <c r="EK25" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="EL25" t="n">
+        <v>50</v>
+      </c>
+      <c r="EM25" t="n">
+        <v>51.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10068,11 +10263,20 @@
       </c>
       <c r="EJ26" t="n">
         <v>196.1</v>
+      </c>
+      <c r="EK26" t="n">
+        <v>197.7</v>
+      </c>
+      <c r="EL26" t="n">
+        <v>219.8</v>
+      </c>
+      <c r="EM26" t="n">
+        <v>224.9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10489,12 +10693,21 @@
         <v>239.7</v>
       </c>
       <c r="EJ27" t="n">
-        <v>212.6</v>
+        <v>210.8</v>
+      </c>
+      <c r="EK27" t="n">
+        <v>207.5</v>
+      </c>
+      <c r="EL27" t="n">
+        <v>240</v>
+      </c>
+      <c r="EM27" t="n">
+        <v>247.9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -10912,11 +11125,20 @@
       </c>
       <c r="EJ28" t="n">
         <v>263.6</v>
+      </c>
+      <c r="EK28" t="n">
+        <v>272.7</v>
+      </c>
+      <c r="EL28" t="n">
+        <v>324</v>
+      </c>
+      <c r="EM28" t="n">
+        <v>334.1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11333,12 +11555,21 @@
         <v>197.7</v>
       </c>
       <c r="EJ29" t="n">
-        <v>167.5</v>
+        <v>168.1</v>
+      </c>
+      <c r="EK29" t="n">
+        <v>164.3</v>
+      </c>
+      <c r="EL29" t="n">
+        <v>194</v>
+      </c>
+      <c r="EM29" t="n">
+        <v>207.3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11755,12 +11986,21 @@
         <v>98.7</v>
       </c>
       <c r="EJ30" t="n">
-        <v>93.3</v>
+        <v>94.5</v>
+      </c>
+      <c r="EK30" t="n">
+        <v>99.6</v>
+      </c>
+      <c r="EL30" t="n">
+        <v>104.6</v>
+      </c>
+      <c r="EM30" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -11901,10 +12141,13 @@
       <c r="EH31"/>
       <c r="EI31"/>
       <c r="EJ31"/>
+      <c r="EK31"/>
+      <c r="EL31"/>
+      <c r="EM31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12321,12 +12564,21 @@
         <v>39.1</v>
       </c>
       <c r="EJ32" t="n">
-        <v>32.1</v>
+        <v>32.3</v>
+      </c>
+      <c r="EK32" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="EL32" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="EM32" t="n">
+        <v>42.4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -12743,12 +12995,21 @@
         <v>90.5</v>
       </c>
       <c r="EJ33" t="n">
-        <v>78.7</v>
+        <v>78.8</v>
+      </c>
+      <c r="EK33" t="n">
+        <v>81</v>
+      </c>
+      <c r="EL33" t="n">
+        <v>92.7</v>
+      </c>
+      <c r="EM33" t="n">
+        <v>96</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -13166,11 +13427,20 @@
       </c>
       <c r="EJ34" t="n">
         <v>70.6</v>
+      </c>
+      <c r="EK34" t="n">
+        <v>69</v>
+      </c>
+      <c r="EL34" t="n">
+        <v>82.7</v>
+      </c>
+      <c r="EM34" t="n">
+        <v>85.2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13587,12 +13857,21 @@
         <v>39.1</v>
       </c>
       <c r="EJ35" t="n">
-        <v>32.3</v>
+        <v>33.1</v>
+      </c>
+      <c r="EK35" t="n">
+        <v>33.1</v>
+      </c>
+      <c r="EL35" t="n">
+        <v>45.3</v>
+      </c>
+      <c r="EM35" t="n">
+        <v>46.6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14010,11 +14289,20 @@
       </c>
       <c r="EJ36" t="n">
         <v>257.1</v>
+      </c>
+      <c r="EK36" t="n">
+        <v>259.6</v>
+      </c>
+      <c r="EL36" t="n">
+        <v>303.8</v>
+      </c>
+      <c r="EM36" t="n">
+        <v>323.7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14431,12 +14719,21 @@
         <v>71</v>
       </c>
       <c r="EJ37" t="n">
-        <v>65.3</v>
+        <v>65.7</v>
+      </c>
+      <c r="EK37" t="n">
+        <v>71.6</v>
+      </c>
+      <c r="EL37" t="n">
+        <v>78.6</v>
+      </c>
+      <c r="EM37" t="n">
+        <v>81.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -14853,12 +15150,21 @@
         <v>659.8</v>
       </c>
       <c r="EJ38" t="n">
-        <v>538.4</v>
+        <v>546.1</v>
+      </c>
+      <c r="EK38" t="n">
+        <v>532.9</v>
+      </c>
+      <c r="EL38" t="n">
+        <v>651.1</v>
+      </c>
+      <c r="EM38" t="n">
+        <v>675.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -15276,11 +15582,20 @@
       </c>
       <c r="EJ39" t="n">
         <v>237.3</v>
+      </c>
+      <c r="EK39" t="n">
+        <v>286.3</v>
+      </c>
+      <c r="EL39" t="n">
+        <v>319</v>
+      </c>
+      <c r="EM39" t="n">
+        <v>327.3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -15698,11 +16013,20 @@
       </c>
       <c r="EJ40" t="n">
         <v>26.1</v>
+      </c>
+      <c r="EK40" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="EL40" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="EM40" t="n">
+        <v>39.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -16119,12 +16443,21 @@
         <v>357.7</v>
       </c>
       <c r="EJ41" t="n">
-        <v>348.9</v>
+        <v>349.3</v>
+      </c>
+      <c r="EK41" t="n">
+        <v>349.8</v>
+      </c>
+      <c r="EL41" t="n">
+        <v>383.8</v>
+      </c>
+      <c r="EM41" t="n">
+        <v>394.5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16541,12 +16874,21 @@
         <v>134.8</v>
       </c>
       <c r="EJ42" t="n">
-        <v>125.6</v>
+        <v>122.3</v>
+      </c>
+      <c r="EK42" t="n">
+        <v>129.1</v>
+      </c>
+      <c r="EL42" t="n">
+        <v>149.6</v>
+      </c>
+      <c r="EM42" t="n">
+        <v>153.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -16963,12 +17305,21 @@
         <v>141.6</v>
       </c>
       <c r="EJ43" t="n">
-        <v>111.3</v>
+        <v>110.8</v>
+      </c>
+      <c r="EK43" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="EL43" t="n">
+        <v>126.9</v>
+      </c>
+      <c r="EM43" t="n">
+        <v>137.6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17386,11 +17737,20 @@
       </c>
       <c r="EJ44" t="n">
         <v>271.3</v>
+      </c>
+      <c r="EK44" t="n">
+        <v>278</v>
+      </c>
+      <c r="EL44" t="n">
+        <v>319.4</v>
+      </c>
+      <c r="EM44" t="n">
+        <v>327.8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -17807,12 +18167,21 @@
         <v>27.3</v>
       </c>
       <c r="EJ45" t="n">
-        <v>22.9</v>
+        <v>23</v>
+      </c>
+      <c r="EK45" t="n">
+        <v>23.2</v>
+      </c>
+      <c r="EL45" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="EM45" t="n">
+        <v>29.7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -18229,12 +18598,21 @@
         <v>155.8</v>
       </c>
       <c r="EJ46" t="n">
-        <v>147.1</v>
+        <v>146</v>
+      </c>
+      <c r="EK46" t="n">
+        <v>150.8</v>
+      </c>
+      <c r="EL46" t="n">
+        <v>161</v>
+      </c>
+      <c r="EM46" t="n">
+        <v>164.2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -18651,12 +19029,21 @@
         <v>34</v>
       </c>
       <c r="EJ47" t="n">
-        <v>28.4</v>
+        <v>28.2</v>
+      </c>
+      <c r="EK47" t="n">
+        <v>29.9</v>
+      </c>
+      <c r="EL47" t="n">
+        <v>37.3</v>
+      </c>
+      <c r="EM47" t="n">
+        <v>38.7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -19073,12 +19460,21 @@
         <v>192.8</v>
       </c>
       <c r="EJ48" t="n">
-        <v>168.2</v>
+        <v>168.6</v>
+      </c>
+      <c r="EK48" t="n">
+        <v>182.1</v>
+      </c>
+      <c r="EL48" t="n">
+        <v>206.7</v>
+      </c>
+      <c r="EM48" t="n">
+        <v>212.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -19495,12 +19891,21 @@
         <v>1133.6</v>
       </c>
       <c r="EJ49" t="n">
-        <v>1061</v>
+        <v>1060.3</v>
+      </c>
+      <c r="EK49" t="n">
+        <v>1087.7</v>
+      </c>
+      <c r="EL49" t="n">
+        <v>1156.5</v>
+      </c>
+      <c r="EM49" t="n">
+        <v>1191.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -19918,11 +20323,20 @@
       </c>
       <c r="EJ50" t="n">
         <v>107.5</v>
+      </c>
+      <c r="EK50" t="n">
+        <v>113.5</v>
+      </c>
+      <c r="EL50" t="n">
+        <v>128.2</v>
+      </c>
+      <c r="EM50" t="n">
+        <v>132</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -20339,12 +20753,21 @@
         <v>29.4</v>
       </c>
       <c r="EJ51" t="n">
-        <v>26.1</v>
+        <v>26.3</v>
+      </c>
+      <c r="EK51" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="EL51" t="n">
+        <v>32.8</v>
+      </c>
+      <c r="EM51" t="n">
+        <v>34.1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -20761,12 +21184,21 @@
         <v>305.8</v>
       </c>
       <c r="EJ52" t="n">
-        <v>273.2</v>
+        <v>275.1</v>
+      </c>
+      <c r="EK52" t="n">
+        <v>292.2</v>
+      </c>
+      <c r="EL52" t="n">
+        <v>324.4</v>
+      </c>
+      <c r="EM52" t="n">
+        <v>328.6</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -21183,12 +21615,21 @@
         <v>249.5</v>
       </c>
       <c r="EJ53" t="n">
-        <v>230.2</v>
+        <v>230</v>
+      </c>
+      <c r="EK53" t="n">
+        <v>218.8</v>
+      </c>
+      <c r="EL53" t="n">
+        <v>228.8</v>
+      </c>
+      <c r="EM53" t="n">
+        <v>248.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -21606,11 +22047,20 @@
       </c>
       <c r="EJ54" t="n">
         <v>51.7</v>
+      </c>
+      <c r="EK54" t="n">
+        <v>54.9</v>
+      </c>
+      <c r="EL54" t="n">
+        <v>59.4</v>
+      </c>
+      <c r="EM54" t="n">
+        <v>61.3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -22027,12 +22477,21 @@
         <v>189.7</v>
       </c>
       <c r="EJ55" t="n">
-        <v>168.1</v>
+        <v>169.9</v>
+      </c>
+      <c r="EK55" t="n">
+        <v>166.8</v>
+      </c>
+      <c r="EL55" t="n">
+        <v>207</v>
+      </c>
+      <c r="EM55" t="n">
+        <v>216.9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -22449,7 +22908,16 @@
         <v>28.1</v>
       </c>
       <c r="EJ56" t="n">
-        <v>24.1</v>
+        <v>23.9</v>
+      </c>
+      <c r="EK56" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="EL56" t="n">
+        <v>29.2</v>
+      </c>
+      <c r="EM56" t="n">
+        <v>30.3</v>
       </c>
     </row>
   </sheetData>
@@ -22851,10 +23319,19 @@
       <c r="DX4" t="s">
         <v>139</v>
       </c>
+      <c r="DY4" t="s">
+        <v>140</v>
+      </c>
+      <c r="DZ4" t="s">
+        <v>141</v>
+      </c>
+      <c r="EA4" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -23232,15 +23709,24 @@
         <v>2.36326483843862</v>
       </c>
       <c r="DW5" t="n">
-        <v>2.67112191170514</v>
+        <v>2.4888618874038</v>
       </c>
       <c r="DX5" t="n">
-        <v>1.785573645068</v>
+        <v>1.7000641321347</v>
+      </c>
+      <c r="DY5" t="n">
+        <v>2.36586761071115</v>
+      </c>
+      <c r="DZ5" t="n">
+        <v>2.35263402181482</v>
+      </c>
+      <c r="EA5" t="n">
+        <v>2.60719348811883</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -23621,12 +24107,21 @@
         <v>0.594530321046373</v>
       </c>
       <c r="DX6" t="n">
-        <v>0.06222775357811</v>
+        <v>0</v>
+      </c>
+      <c r="DY6" t="n">
+        <v>0.671140939597312</v>
+      </c>
+      <c r="DZ6" t="n">
+        <v>0.823045267489715</v>
+      </c>
+      <c r="EA6" t="n">
+        <v>0.694042799305951</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -24008,11 +24503,20 @@
       </c>
       <c r="DX7" t="n">
         <v>2.11640211640213</v>
+      </c>
+      <c r="DY7" t="n">
+        <v>0.0000000000000166014657887874</v>
+      </c>
+      <c r="DZ7" t="n">
+        <v>0.740740740740751</v>
+      </c>
+      <c r="EA7" t="n">
+        <v>0.714285714285724</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -24393,12 +24897,21 @@
         <v>1.73217854763491</v>
       </c>
       <c r="DX8" t="n">
-        <v>3.47411444141689</v>
+        <v>2.86103542234332</v>
+      </c>
+      <c r="DY8" t="n">
+        <v>3.92156862745098</v>
+      </c>
+      <c r="DZ8" t="n">
+        <v>4.75195822454308</v>
+      </c>
+      <c r="EA8" t="n">
+        <v>4.26954732510289</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -24780,11 +25293,20 @@
       </c>
       <c r="DX9" t="n">
         <v>0.611995104039185</v>
+      </c>
+      <c r="DY9" t="n">
+        <v>0.578034682080925</v>
+      </c>
+      <c r="DZ9" t="n">
+        <v>0.599999999999994</v>
+      </c>
+      <c r="EA9" t="n">
+        <v>0.293255131964821</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -25165,12 +25687,21 @@
         <v>2.72069223729094</v>
       </c>
       <c r="DX10" t="n">
-        <v>3.08932169241102</v>
+        <v>2.24503501870863</v>
+      </c>
+      <c r="DY10" t="n">
+        <v>2.3963133640553</v>
+      </c>
+      <c r="DZ10" t="n">
+        <v>2.05119365681289</v>
+      </c>
+      <c r="EA10" t="n">
+        <v>1.76451187335093</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -25551,12 +26082,21 @@
         <v>3.32681017612524</v>
       </c>
       <c r="DX11" t="n">
-        <v>5.74342458400429</v>
+        <v>6.01180891035963</v>
+      </c>
+      <c r="DY11" t="n">
+        <v>4.03429147755925</v>
+      </c>
+      <c r="DZ11" t="n">
+        <v>2.70270270270269</v>
+      </c>
+      <c r="EA11" t="n">
+        <v>3.75838926174497</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -25938,11 +26478,20 @@
       </c>
       <c r="DX12" t="n">
         <v>-0.309278350515461</v>
+      </c>
+      <c r="DY12" t="n">
+        <v>-0.407331975560073</v>
+      </c>
+      <c r="DZ12" t="n">
+        <v>1.72981878088962</v>
+      </c>
+      <c r="EA12" t="n">
+        <v>2.08333333333334</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -26323,12 +26872,21 @@
         <v>0.57142857142858</v>
       </c>
       <c r="DX13" t="n">
-        <v>0.887573964497054</v>
+        <v>0</v>
+      </c>
+      <c r="DY13" t="n">
+        <v>1.52905198776758</v>
+      </c>
+      <c r="DZ13" t="n">
+        <v>3.83561643835616</v>
+      </c>
+      <c r="EA13" t="n">
+        <v>5.61497326203209</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -26457,10 +27015,13 @@
       <c r="DV14"/>
       <c r="DW14"/>
       <c r="DX14"/>
+      <c r="DY14"/>
+      <c r="DZ14"/>
+      <c r="EA14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -26841,12 +27402,21 @@
         <v>1.91473066122032</v>
       </c>
       <c r="DX15" t="n">
-        <v>1.83985488468516</v>
+        <v>1.81394143560509</v>
+      </c>
+      <c r="DY15" t="n">
+        <v>1.39103554868625</v>
+      </c>
+      <c r="DZ15" t="n">
+        <v>1.55266470835081</v>
+      </c>
+      <c r="EA15" t="n">
+        <v>1.80310880829015</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -27227,12 +27797,21 @@
         <v>3.51960481630134</v>
       </c>
       <c r="DX16" t="n">
-        <v>3.55987055016181</v>
+        <v>4.14239482200648</v>
+      </c>
+      <c r="DY16" t="n">
+        <v>2.74626865671641</v>
+      </c>
+      <c r="DZ16" t="n">
+        <v>3.24101355332941</v>
+      </c>
+      <c r="EA16" t="n">
+        <v>3.09669880222026</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -27361,10 +27940,13 @@
       <c r="DV17"/>
       <c r="DW17"/>
       <c r="DX17"/>
+      <c r="DY17"/>
+      <c r="DZ17"/>
+      <c r="EA17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -27746,11 +28328,20 @@
       </c>
       <c r="DX18" t="n">
         <v>6.60194174757281</v>
+      </c>
+      <c r="DY18" t="n">
+        <v>8.34914611005691</v>
+      </c>
+      <c r="DZ18" t="n">
+        <v>5.26315789473685</v>
+      </c>
+      <c r="EA18" t="n">
+        <v>6.61417322834646</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -28131,12 +28722,21 @@
         <v>3.65204159269591</v>
       </c>
       <c r="DX19" t="n">
-        <v>3.42391304347827</v>
+        <v>3.4782608695652</v>
+      </c>
+      <c r="DY19" t="n">
+        <v>3.13588850174216</v>
+      </c>
+      <c r="DZ19" t="n">
+        <v>3.65711623573259</v>
+      </c>
+      <c r="EA19" t="n">
+        <v>3.65576748410536</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -28517,12 +29117,21 @@
         <v>-2.87958115183246</v>
       </c>
       <c r="DX20" t="n">
-        <v>-1.46799765120376</v>
+        <v>0.528479154433339</v>
+      </c>
+      <c r="DY20" t="n">
+        <v>-1.10153256704981</v>
+      </c>
+      <c r="DZ20" t="n">
+        <v>2.40963855421686</v>
+      </c>
+      <c r="EA20" t="n">
+        <v>4.1611332447986</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -28903,12 +29512,21 @@
         <v>0.379650721336371</v>
       </c>
       <c r="DX21" t="n">
-        <v>0</v>
+        <v>0.698080279232122</v>
+      </c>
+      <c r="DY21" t="n">
+        <v>0.336700336700341</v>
+      </c>
+      <c r="DZ21" t="n">
+        <v>0.995024875621895</v>
+      </c>
+      <c r="EA21" t="n">
+        <v>1.37080191912269</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -29289,12 +29907,21 @@
         <v>-0.580431177446093</v>
       </c>
       <c r="DX22" t="n">
-        <v>0.686947988223738</v>
+        <v>1.37389597644749</v>
+      </c>
+      <c r="DY22" t="n">
+        <v>1.63043478260869</v>
+      </c>
+      <c r="DZ22" t="n">
+        <v>1.45038167938932</v>
+      </c>
+      <c r="EA22" t="n">
+        <v>2.28782287822878</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -29675,12 +30302,21 @@
         <v>1.75084175084175</v>
       </c>
       <c r="DX23" t="n">
-        <v>3.42298288508559</v>
+        <v>4.07497962510188</v>
+      </c>
+      <c r="DY23" t="n">
+        <v>3.07377049180326</v>
+      </c>
+      <c r="DZ23" t="n">
+        <v>2.21940393151554</v>
+      </c>
+      <c r="EA23" t="n">
+        <v>2.31684408265499</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -30061,12 +30697,21 @@
         <v>3.34323922734027</v>
       </c>
       <c r="DX24" t="n">
-        <v>2.08978328173376</v>
+        <v>2.24458204334366</v>
+      </c>
+      <c r="DY24" t="n">
+        <v>2.25618631732168</v>
+      </c>
+      <c r="DZ24" t="n">
+        <v>3.1615120274914</v>
+      </c>
+      <c r="EA24" t="n">
+        <v>2.22222222222223</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -30448,11 +31093,20 @@
       </c>
       <c r="DX25" t="n">
         <v>0.742574257425753</v>
+      </c>
+      <c r="DY25" t="n">
+        <v>0.50890585241731</v>
+      </c>
+      <c r="DZ25" t="n">
+        <v>0.806451612903223</v>
+      </c>
+      <c r="EA25" t="n">
+        <v>1.17878192534381</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -30834,11 +31488,20 @@
       </c>
       <c r="DX26" t="n">
         <v>2.56276150627615</v>
+      </c>
+      <c r="DY26" t="n">
+        <v>4.21718502899313</v>
+      </c>
+      <c r="DZ26" t="n">
+        <v>3.28947368421053</v>
+      </c>
+      <c r="EA26" t="n">
+        <v>3.68833563854311</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -31219,12 +31882,21 @@
         <v>2.43589743589743</v>
       </c>
       <c r="DX27" t="n">
-        <v>2.70531400966183</v>
+        <v>1.83574879227054</v>
+      </c>
+      <c r="DY27" t="n">
+        <v>1.91552062868368</v>
+      </c>
+      <c r="DZ27" t="n">
+        <v>0.671140939597325</v>
+      </c>
+      <c r="EA27" t="n">
+        <v>0.731409995936604</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -31606,11 +32278,20 @@
       </c>
       <c r="DX28" t="n">
         <v>5.73606097071801</v>
+      </c>
+      <c r="DY28" t="n">
+        <v>5.1677593521018</v>
+      </c>
+      <c r="DZ28" t="n">
+        <v>5.43442889684347</v>
+      </c>
+      <c r="EA28" t="n">
+        <v>4.47154471544716</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -31991,12 +32672,21 @@
         <v>1.07361963190182</v>
       </c>
       <c r="DX29" t="n">
-        <v>-0.475341651812247</v>
+        <v>-0.11883541295307</v>
+      </c>
+      <c r="DY29" t="n">
+        <v>0.244051250762664</v>
+      </c>
+      <c r="DZ29" t="n">
+        <v>1.51753008895866</v>
+      </c>
+      <c r="EA29" t="n">
+        <v>1.76730486008838</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -32377,12 +33067,21 @@
         <v>1.64778578784757</v>
       </c>
       <c r="DX30" t="n">
-        <v>-1.06044538706257</v>
+        <v>0.212089077412516</v>
+      </c>
+      <c r="DY30" t="n">
+        <v>2.25872689938399</v>
+      </c>
+      <c r="DZ30" t="n">
+        <v>0.965250965250951</v>
+      </c>
+      <c r="EA30" t="n">
+        <v>0.767754318618053</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -32511,10 +33210,13 @@
       <c r="DV31"/>
       <c r="DW31"/>
       <c r="DX31"/>
+      <c r="DY31"/>
+      <c r="DZ31"/>
+      <c r="EA31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -32895,12 +33597,21 @@
         <v>-6.9047619047619</v>
       </c>
       <c r="DX32" t="n">
-        <v>-7.49279538904899</v>
+        <v>-6.91642651296832</v>
+      </c>
+      <c r="DY32" t="n">
+        <v>-3.18840579710145</v>
+      </c>
+      <c r="DZ32" t="n">
+        <v>-4.46009389671361</v>
+      </c>
+      <c r="EA32" t="n">
+        <v>-2.97482837528605</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -33281,12 +33992,21 @@
         <v>2.95790671217292</v>
       </c>
       <c r="DX33" t="n">
-        <v>1.94300518134717</v>
+        <v>2.07253886010364</v>
+      </c>
+      <c r="DY33" t="n">
+        <v>1.3767209011264</v>
+      </c>
+      <c r="DZ33" t="n">
+        <v>1.75631174533479</v>
+      </c>
+      <c r="EA33" t="n">
+        <v>1.15911485774499</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -33668,11 +34388,20 @@
       </c>
       <c r="DX34" t="n">
         <v>5.68862275449101</v>
+      </c>
+      <c r="DY34" t="n">
+        <v>-0.862068965517233</v>
+      </c>
+      <c r="DZ34" t="n">
+        <v>4.68354430379747</v>
+      </c>
+      <c r="EA34" t="n">
+        <v>5.97014925373134</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -34053,12 +34782,21 @@
         <v>0.25641025641026</v>
       </c>
       <c r="DX35" t="n">
-        <v>-0.0000000000000219982271133158</v>
+        <v>2.4767801857585</v>
+      </c>
+      <c r="DY35" t="n">
+        <v>0.607902735562319</v>
+      </c>
+      <c r="DZ35" t="n">
+        <v>2.02702702702702</v>
+      </c>
+      <c r="EA35" t="n">
+        <v>1.96936542669582</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -34440,11 +35178,20 @@
       </c>
       <c r="DX36" t="n">
         <v>3.66935483870969</v>
+      </c>
+      <c r="DY36" t="n">
+        <v>4.08981555733762</v>
+      </c>
+      <c r="DZ36" t="n">
+        <v>3.89876880984951</v>
+      </c>
+      <c r="EA36" t="n">
+        <v>5.19987000324994</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -34825,12 +35572,21 @@
         <v>11.6352201257862</v>
       </c>
       <c r="DX37" t="n">
-        <v>7.75577557755775</v>
+        <v>8.41584158415842</v>
+      </c>
+      <c r="DY37" t="n">
+        <v>3.61794500723589</v>
+      </c>
+      <c r="DZ37" t="n">
+        <v>5.22088353413655</v>
+      </c>
+      <c r="EA37" t="n">
+        <v>7.67195767195769</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -35211,12 +35967,21 @@
         <v>3.33594361785436</v>
       </c>
       <c r="DX38" t="n">
-        <v>1.7961807525052</v>
+        <v>3.25203252032521</v>
+      </c>
+      <c r="DY38" t="n">
+        <v>0.661125802795618</v>
+      </c>
+      <c r="DZ38" t="n">
+        <v>3.25087218522042</v>
+      </c>
+      <c r="EA38" t="n">
+        <v>0.640739085084183</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -35598,11 +36363,20 @@
       </c>
       <c r="DX39" t="n">
         <v>0.721561969439736</v>
+      </c>
+      <c r="DY39" t="n">
+        <v>0.632688927943745</v>
+      </c>
+      <c r="DZ39" t="n">
+        <v>0.726239343227032</v>
+      </c>
+      <c r="EA39" t="n">
+        <v>1.48837209302326</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -35984,11 +36758,20 @@
       </c>
       <c r="DX40" t="n">
         <v>-6.4516129032258</v>
+      </c>
+      <c r="DY40" t="n">
+        <v>0</v>
+      </c>
+      <c r="DZ40" t="n">
+        <v>3.55191256830602</v>
+      </c>
+      <c r="EA40" t="n">
+        <v>3.64583333333333</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -36369,12 +37152,21 @@
         <v>0.562271577171774</v>
       </c>
       <c r="DX41" t="n">
-        <v>1.39494333042719</v>
+        <v>1.5111886079628</v>
+      </c>
+      <c r="DY41" t="n">
+        <v>0.865051903114187</v>
+      </c>
+      <c r="DZ41" t="n">
+        <v>1.42706131078225</v>
+      </c>
+      <c r="EA41" t="n">
+        <v>1.15384615384615</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -36755,12 +37547,21 @@
         <v>1.73584905660378</v>
       </c>
       <c r="DX42" t="n">
-        <v>2.61437908496731</v>
+        <v>-0.0816993464052357</v>
+      </c>
+      <c r="DY42" t="n">
+        <v>2.46031746031746</v>
+      </c>
+      <c r="DZ42" t="n">
+        <v>3.74479889042996</v>
+      </c>
+      <c r="EA42" t="n">
+        <v>4.70668485675307</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -37141,12 +37942,21 @@
         <v>7.19152157456472</v>
       </c>
       <c r="DX43" t="n">
-        <v>2.39190432382705</v>
+        <v>1.93192272309108</v>
+      </c>
+      <c r="DY43" t="n">
+        <v>1.6260162601626</v>
+      </c>
+      <c r="DZ43" t="n">
+        <v>1.9277108433735</v>
+      </c>
+      <c r="EA43" t="n">
+        <v>1.54981549815498</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -37528,11 +38338,20 @@
       </c>
       <c r="DX44" t="n">
         <v>0.930059523809524</v>
+      </c>
+      <c r="DY44" t="n">
+        <v>2.0932794711715</v>
+      </c>
+      <c r="DZ44" t="n">
+        <v>-0.77663870767319</v>
+      </c>
+      <c r="EA44" t="n">
+        <v>-0.485731633272641</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -37913,12 +38732,21 @@
         <v>1.48698884758365</v>
       </c>
       <c r="DX45" t="n">
-        <v>-2.13675213675214</v>
+        <v>-1.7094017094017</v>
+      </c>
+      <c r="DY45" t="n">
+        <v>-2.1097046413502</v>
+      </c>
+      <c r="DZ45" t="n">
+        <v>1.4336917562724</v>
+      </c>
+      <c r="EA45" t="n">
+        <v>3.12500000000001</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -38299,12 +39127,21 @@
         <v>0.257400257400261</v>
       </c>
       <c r="DX46" t="n">
-        <v>0</v>
+        <v>-0.747790618626781</v>
+      </c>
+      <c r="DY46" t="n">
+        <v>1.00468854655057</v>
+      </c>
+      <c r="DZ46" t="n">
+        <v>-0.124069478908182</v>
+      </c>
+      <c r="EA46" t="n">
+        <v>0.121951219512188</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -38685,12 +39522,21 @@
         <v>2.10210210210211</v>
       </c>
       <c r="DX47" t="n">
-        <v>1.06761565836298</v>
+        <v>0.355871886121001</v>
+      </c>
+      <c r="DY47" t="n">
+        <v>2.39726027397259</v>
+      </c>
+      <c r="DZ47" t="n">
+        <v>2.1917808219178</v>
+      </c>
+      <c r="EA47" t="n">
+        <v>1.8421052631579</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -39071,12 +39917,21 @@
         <v>0.626304801670155</v>
       </c>
       <c r="DX48" t="n">
-        <v>0.899820035992801</v>
+        <v>1.13977204559089</v>
+      </c>
+      <c r="DY48" t="n">
+        <v>0.552181115405853</v>
+      </c>
+      <c r="DZ48" t="n">
+        <v>0.632911392405055</v>
+      </c>
+      <c r="EA48" t="n">
+        <v>1.9664268585132</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -39457,12 +40312,21 @@
         <v>2.31046931407941</v>
       </c>
       <c r="DX49" t="n">
-        <v>1.50196115947575</v>
+        <v>1.43499473835263</v>
+      </c>
+      <c r="DY49" t="n">
+        <v>2.22744360902256</v>
+      </c>
+      <c r="DZ49" t="n">
+        <v>2.23656294200848</v>
+      </c>
+      <c r="EA49" t="n">
+        <v>1.86308862490387</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -39844,11 +40708,20 @@
       </c>
       <c r="DX50" t="n">
         <v>6.01577909270216</v>
+      </c>
+      <c r="DY50" t="n">
+        <v>5.28756957328386</v>
+      </c>
+      <c r="DZ50" t="n">
+        <v>4.56769983686785</v>
+      </c>
+      <c r="EA50" t="n">
+        <v>4.5958795562599</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -40229,12 +41102,21 @@
         <v>8.08823529411764</v>
       </c>
       <c r="DX51" t="n">
-        <v>5.24193548387099</v>
+        <v>6.04838709677421</v>
+      </c>
+      <c r="DY51" t="n">
+        <v>5.57768924302788</v>
+      </c>
+      <c r="DZ51" t="n">
+        <v>6.84039087947881</v>
+      </c>
+      <c r="EA51" t="n">
+        <v>6.23052959501558</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -40615,12 +41497,21 @@
         <v>2.27424749163878</v>
       </c>
       <c r="DX52" t="n">
-        <v>3.09433962264151</v>
+        <v>3.81132075471699</v>
+      </c>
+      <c r="DY52" t="n">
+        <v>3.54358610914245</v>
+      </c>
+      <c r="DZ52" t="n">
+        <v>3.74160537256156</v>
+      </c>
+      <c r="EA52" t="n">
+        <v>3.92156862745099</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -41001,12 +41892,21 @@
         <v>3.35542667771334</v>
       </c>
       <c r="DX53" t="n">
-        <v>0.43630017452007</v>
+        <v>0.349040139616061</v>
+      </c>
+      <c r="DY53" t="n">
+        <v>-1.30807397383851</v>
+      </c>
+      <c r="DZ53" t="n">
+        <v>-2.63829787234042</v>
+      </c>
+      <c r="EA53" t="n">
+        <v>-0.241157556270094</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -41388,11 +42288,20 @@
       </c>
       <c r="DX54" t="n">
         <v>1.57170923379176</v>
+      </c>
+      <c r="DY54" t="n">
+        <v>1.66666666666668</v>
+      </c>
+      <c r="DZ54" t="n">
+        <v>-0.834724540901491</v>
+      </c>
+      <c r="EA54" t="n">
+        <v>-0.648298217179912</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -41773,12 +42682,21 @@
         <v>1.77038626609441</v>
       </c>
       <c r="DX55" t="n">
-        <v>-1.05944673337256</v>
+        <v>0.0000000000000167284928960589</v>
+      </c>
+      <c r="DY55" t="n">
+        <v>-0.239234449760752</v>
+      </c>
+      <c r="DZ55" t="n">
+        <v>2.12136161815491</v>
+      </c>
+      <c r="EA55" t="n">
+        <v>2.26308345120227</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -42159,7 +43077,16 @@
         <v>2.93040293040293</v>
       </c>
       <c r="DX56" t="n">
-        <v>0</v>
+        <v>-0.829875518672211</v>
+      </c>
+      <c r="DY56" t="n">
+        <v>-0.406504065040656</v>
+      </c>
+      <c r="DZ56" t="n">
+        <v>0.689655172413803</v>
+      </c>
+      <c r="EA56" t="n">
+        <v>0.664451827242522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023-12-22 :: SEM Update for December
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -442,6 +442,9 @@
   </si>
   <si>
     <t xml:space="preserve">10/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1359,10 +1362,13 @@
       <c r="EM4" t="s">
         <v>142</v>
       </c>
+      <c r="EN4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1785,15 +1791,18 @@
         <v>9484.3</v>
       </c>
       <c r="EL5" t="n">
-        <v>10584.9</v>
+        <v>10596.8</v>
       </c>
       <c r="EM5" t="n">
-        <v>10929</v>
+        <v>10957.3</v>
+      </c>
+      <c r="EN5" t="n">
+        <v>11085.3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2220,11 +2229,14 @@
       </c>
       <c r="EM6" t="n">
         <v>174.1</v>
+      </c>
+      <c r="EN6" t="n">
+        <v>174.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2650,12 +2662,15 @@
         <v>27.2</v>
       </c>
       <c r="EM7" t="n">
-        <v>28.2</v>
+        <v>28.3</v>
+      </c>
+      <c r="EN7" t="n">
+        <v>28.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3081,12 +3096,15 @@
         <v>200.6</v>
       </c>
       <c r="EM8" t="n">
-        <v>202.7</v>
+        <v>203.6</v>
+      </c>
+      <c r="EN8" t="n">
+        <v>204.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3512,12 +3530,15 @@
         <v>100.6</v>
       </c>
       <c r="EM9" t="n">
+        <v>102.6</v>
+      </c>
+      <c r="EN9" t="n">
         <v>102.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3943,12 +3964,15 @@
         <v>1184.1</v>
       </c>
       <c r="EM10" t="n">
-        <v>1234.2</v>
+        <v>1234.8</v>
+      </c>
+      <c r="EN10" t="n">
+        <v>1250.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4374,12 +4398,15 @@
         <v>224.2</v>
       </c>
       <c r="EM11" t="n">
-        <v>231.9</v>
+        <v>231.6</v>
+      </c>
+      <c r="EN11" t="n">
+        <v>234.2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4805,12 +4832,15 @@
         <v>123.5</v>
       </c>
       <c r="EM12" t="n">
-        <v>127.4</v>
+        <v>127.5</v>
+      </c>
+      <c r="EN12" t="n">
+        <v>128.8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5236,12 +5266,15 @@
         <v>37.9</v>
       </c>
       <c r="EM13" t="n">
-        <v>39.5</v>
+        <v>39</v>
+      </c>
+      <c r="EN13" t="n">
+        <v>39.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5385,10 +5418,11 @@
       <c r="EK14"/>
       <c r="EL14"/>
       <c r="EM14"/>
+      <c r="EN14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5814,12 +5848,15 @@
         <v>484</v>
       </c>
       <c r="EM15" t="n">
-        <v>491.2</v>
+        <v>490</v>
+      </c>
+      <c r="EN15" t="n">
+        <v>494.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6245,12 +6282,15 @@
         <v>350.4</v>
       </c>
       <c r="EM16" t="n">
-        <v>352.9</v>
+        <v>352.5</v>
+      </c>
+      <c r="EN16" t="n">
+        <v>353.7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6394,10 +6434,11 @@
       <c r="EK17"/>
       <c r="EL17"/>
       <c r="EM17"/>
+      <c r="EN17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6823,12 +6864,15 @@
         <v>64</v>
       </c>
       <c r="EM18" t="n">
-        <v>67.7</v>
+        <v>66.8</v>
+      </c>
+      <c r="EN18" t="n">
+        <v>67.4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7254,12 +7298,15 @@
         <v>445</v>
       </c>
       <c r="EM19" t="n">
-        <v>456.5</v>
+        <v>456.8</v>
+      </c>
+      <c r="EN19" t="n">
+        <v>460</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7685,12 +7732,15 @@
         <v>229.5</v>
       </c>
       <c r="EM20" t="n">
-        <v>235.3</v>
+        <v>233</v>
+      </c>
+      <c r="EN20" t="n">
+        <v>235.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8116,12 +8166,15 @@
         <v>142.1</v>
       </c>
       <c r="EM21" t="n">
-        <v>147.9</v>
+        <v>148.1</v>
+      </c>
+      <c r="EN21" t="n">
+        <v>149.1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8548,11 +8601,14 @@
       </c>
       <c r="EM22" t="n">
         <v>138.6</v>
+      </c>
+      <c r="EN22" t="n">
+        <v>140.2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -8978,12 +9034,15 @@
         <v>161.2</v>
       </c>
       <c r="EM23" t="n">
-        <v>163.4</v>
+        <v>163.8</v>
+      </c>
+      <c r="EN23" t="n">
+        <v>165.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9409,12 +9468,15 @@
         <v>150.1</v>
       </c>
       <c r="EM24" t="n">
-        <v>151.8</v>
+        <v>152.8</v>
+      </c>
+      <c r="EN24" t="n">
+        <v>154</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9840,12 +9902,15 @@
         <v>50</v>
       </c>
       <c r="EM25" t="n">
-        <v>51.5</v>
+        <v>51.6</v>
+      </c>
+      <c r="EN25" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10272,11 +10337,14 @@
       </c>
       <c r="EM26" t="n">
         <v>224.9</v>
+      </c>
+      <c r="EN26" t="n">
+        <v>226.3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10702,12 +10770,15 @@
         <v>240</v>
       </c>
       <c r="EM27" t="n">
-        <v>247.9</v>
+        <v>247.5</v>
+      </c>
+      <c r="EN27" t="n">
+        <v>251.2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11134,11 +11205,14 @@
       </c>
       <c r="EM28" t="n">
         <v>334.1</v>
+      </c>
+      <c r="EN28" t="n">
+        <v>335.8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11564,12 +11638,15 @@
         <v>194</v>
       </c>
       <c r="EM29" t="n">
-        <v>207.3</v>
+        <v>207</v>
+      </c>
+      <c r="EN29" t="n">
+        <v>210.8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -11995,12 +12072,15 @@
         <v>104.6</v>
       </c>
       <c r="EM30" t="n">
-        <v>105</v>
+        <v>105.1</v>
+      </c>
+      <c r="EN30" t="n">
+        <v>105.4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -12144,10 +12224,11 @@
       <c r="EK31"/>
       <c r="EL31"/>
       <c r="EM31"/>
+      <c r="EN31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12574,11 +12655,14 @@
       </c>
       <c r="EM32" t="n">
         <v>42.4</v>
+      </c>
+      <c r="EN32" t="n">
+        <v>42.7</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13004,12 +13088,15 @@
         <v>92.7</v>
       </c>
       <c r="EM33" t="n">
-        <v>96</v>
+        <v>95.3</v>
+      </c>
+      <c r="EN33" t="n">
+        <v>96.8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -13435,12 +13522,15 @@
         <v>82.7</v>
       </c>
       <c r="EM34" t="n">
-        <v>85.2</v>
+        <v>84.5</v>
+      </c>
+      <c r="EN34" t="n">
+        <v>84.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13867,11 +13957,14 @@
       </c>
       <c r="EM35" t="n">
         <v>46.6</v>
+      </c>
+      <c r="EN35" t="n">
+        <v>46.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14298,11 +14391,14 @@
       </c>
       <c r="EM36" t="n">
         <v>323.7</v>
+      </c>
+      <c r="EN36" t="n">
+        <v>327.9</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14728,12 +14824,15 @@
         <v>78.6</v>
       </c>
       <c r="EM37" t="n">
-        <v>81.4</v>
+        <v>81.5</v>
+      </c>
+      <c r="EN37" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -15160,11 +15259,14 @@
       </c>
       <c r="EM38" t="n">
         <v>675.4</v>
+      </c>
+      <c r="EN38" t="n">
+        <v>683.3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -15591,11 +15693,14 @@
       </c>
       <c r="EM39" t="n">
         <v>327.3</v>
+      </c>
+      <c r="EN39" t="n">
+        <v>331.8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -16021,12 +16126,15 @@
         <v>37.9</v>
       </c>
       <c r="EM40" t="n">
+        <v>39.8</v>
+      </c>
+      <c r="EN40" t="n">
         <v>39.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -16452,12 +16560,15 @@
         <v>383.8</v>
       </c>
       <c r="EM41" t="n">
-        <v>394.5</v>
+        <v>393</v>
+      </c>
+      <c r="EN41" t="n">
+        <v>396.3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16883,12 +16994,15 @@
         <v>149.6</v>
       </c>
       <c r="EM42" t="n">
-        <v>153.5</v>
+        <v>152.6</v>
+      </c>
+      <c r="EN42" t="n">
+        <v>153.2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -17314,12 +17428,15 @@
         <v>126.9</v>
       </c>
       <c r="EM43" t="n">
-        <v>137.6</v>
+        <v>138.4</v>
+      </c>
+      <c r="EN43" t="n">
+        <v>140.8</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17745,12 +17862,15 @@
         <v>319.4</v>
       </c>
       <c r="EM44" t="n">
-        <v>327.8</v>
+        <v>327.3</v>
+      </c>
+      <c r="EN44" t="n">
+        <v>332.3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -18176,12 +18296,15 @@
         <v>28.3</v>
       </c>
       <c r="EM45" t="n">
-        <v>29.7</v>
+        <v>29.8</v>
+      </c>
+      <c r="EN45" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -18607,12 +18730,15 @@
         <v>161</v>
       </c>
       <c r="EM46" t="n">
-        <v>164.2</v>
+        <v>164</v>
+      </c>
+      <c r="EN46" t="n">
+        <v>165</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -19038,12 +19164,15 @@
         <v>37.3</v>
       </c>
       <c r="EM47" t="n">
-        <v>38.7</v>
+        <v>38.8</v>
+      </c>
+      <c r="EN47" t="n">
+        <v>39.3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -19469,12 +19598,15 @@
         <v>206.7</v>
       </c>
       <c r="EM48" t="n">
-        <v>212.6</v>
+        <v>210.2</v>
+      </c>
+      <c r="EN48" t="n">
+        <v>211.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -19900,12 +20032,15 @@
         <v>1156.5</v>
       </c>
       <c r="EM49" t="n">
-        <v>1191.9</v>
+        <v>1191.4</v>
+      </c>
+      <c r="EN49" t="n">
+        <v>1200.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -20332,11 +20467,14 @@
       </c>
       <c r="EM50" t="n">
         <v>132</v>
+      </c>
+      <c r="EN50" t="n">
+        <v>133</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -20762,12 +20900,15 @@
         <v>32.8</v>
       </c>
       <c r="EM51" t="n">
-        <v>34.1</v>
+        <v>34.2</v>
+      </c>
+      <c r="EN51" t="n">
+        <v>34.6</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -21194,11 +21335,14 @@
       </c>
       <c r="EM52" t="n">
         <v>328.6</v>
+      </c>
+      <c r="EN52" t="n">
+        <v>333.6</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -21624,12 +21768,15 @@
         <v>228.8</v>
       </c>
       <c r="EM53" t="n">
-        <v>248.2</v>
+        <v>244.1</v>
+      </c>
+      <c r="EN53" t="n">
+        <v>246.1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -22055,12 +22202,15 @@
         <v>59.4</v>
       </c>
       <c r="EM54" t="n">
-        <v>61.3</v>
+        <v>61.6</v>
+      </c>
+      <c r="EN54" t="n">
+        <v>62.4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -22486,12 +22636,15 @@
         <v>207</v>
       </c>
       <c r="EM55" t="n">
-        <v>216.9</v>
+        <v>216.5</v>
+      </c>
+      <c r="EN55" t="n">
+        <v>217.7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -22917,7 +23070,10 @@
         <v>29.2</v>
       </c>
       <c r="EM56" t="n">
-        <v>30.3</v>
+        <v>30.4</v>
+      </c>
+      <c r="EN56" t="n">
+        <v>30.6</v>
       </c>
     </row>
   </sheetData>
@@ -23328,10 +23484,13 @@
       <c r="EA4" t="s">
         <v>142</v>
       </c>
+      <c r="EB4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -23718,15 +23877,18 @@
         <v>2.36586761071115</v>
       </c>
       <c r="DZ5" t="n">
-        <v>2.35263402181482</v>
+        <v>2.46770325674943</v>
       </c>
       <c r="EA5" t="n">
-        <v>2.60719348811883</v>
+        <v>2.8728887553632</v>
+      </c>
+      <c r="EB5" t="n">
+        <v>2.92948801277647</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -24117,11 +24279,14 @@
       </c>
       <c r="EA6" t="n">
         <v>0.694042799305951</v>
+      </c>
+      <c r="EB6" t="n">
+        <v>0.286861732644865</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -24511,12 +24676,15 @@
         <v>0.740740740740751</v>
       </c>
       <c r="EA7" t="n">
-        <v>0.714285714285724</v>
+        <v>1.07142857142856</v>
+      </c>
+      <c r="EB7" t="n">
+        <v>0.350877192982461</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -24906,12 +25074,15 @@
         <v>4.75195822454308</v>
       </c>
       <c r="EA8" t="n">
-        <v>4.26954732510289</v>
+        <v>4.73251028806585</v>
+      </c>
+      <c r="EB8" t="n">
+        <v>3.54251012145749</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -25302,11 +25473,14 @@
       </c>
       <c r="EA9" t="n">
         <v>0.293255131964821</v>
+      </c>
+      <c r="EB9" t="n">
+        <v>0.195312499999989</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -25696,12 +25870,15 @@
         <v>2.05119365681289</v>
       </c>
       <c r="EA10" t="n">
-        <v>1.76451187335093</v>
+        <v>1.81398416886544</v>
+      </c>
+      <c r="EB10" t="n">
+        <v>1.21408336705787</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -26091,12 +26268,15 @@
         <v>2.70270270270269</v>
       </c>
       <c r="EA11" t="n">
-        <v>3.75838926174497</v>
+        <v>3.6241610738255</v>
+      </c>
+      <c r="EB11" t="n">
+        <v>3.95028850421659</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -26486,12 +26666,15 @@
         <v>1.72981878088962</v>
       </c>
       <c r="EA12" t="n">
-        <v>2.08333333333334</v>
+        <v>2.16346153846154</v>
+      </c>
+      <c r="EB12" t="n">
+        <v>1.57728706624607</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -26881,12 +27064,15 @@
         <v>3.83561643835616</v>
       </c>
       <c r="EA13" t="n">
-        <v>5.61497326203209</v>
+        <v>4.27807486631016</v>
+      </c>
+      <c r="EB13" t="n">
+        <v>3.70370370370372</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -27018,10 +27204,11 @@
       <c r="DY14"/>
       <c r="DZ14"/>
       <c r="EA14"/>
+      <c r="EB14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -27411,12 +27598,15 @@
         <v>1.55266470835081</v>
       </c>
       <c r="EA15" t="n">
-        <v>1.80310880829015</v>
+        <v>1.55440414507772</v>
+      </c>
+      <c r="EB15" t="n">
+        <v>1.62351006987258</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -27806,12 +27996,15 @@
         <v>3.24101355332941</v>
       </c>
       <c r="EA16" t="n">
-        <v>3.09669880222026</v>
+        <v>2.97984224364592</v>
+      </c>
+      <c r="EB16" t="n">
+        <v>2.78988666085441</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -27943,10 +28136,11 @@
       <c r="DY17"/>
       <c r="DZ17"/>
       <c r="EA17"/>
+      <c r="EB17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -28336,12 +28530,15 @@
         <v>5.26315789473685</v>
       </c>
       <c r="EA18" t="n">
-        <v>6.61417322834646</v>
+        <v>5.19685039370078</v>
+      </c>
+      <c r="EB18" t="n">
+        <v>4.82115085536549</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -28731,12 +28928,15 @@
         <v>3.65711623573259</v>
       </c>
       <c r="EA19" t="n">
-        <v>3.65576748410536</v>
+        <v>3.72388737511353</v>
+      </c>
+      <c r="EB19" t="n">
+        <v>3.51035103510352</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -29126,12 +29326,15 @@
         <v>2.40963855421686</v>
       </c>
       <c r="EA20" t="n">
-        <v>4.1611332447986</v>
+        <v>3.14298362107128</v>
+      </c>
+      <c r="EB20" t="n">
+        <v>3.01837270341208</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -29521,12 +29724,15 @@
         <v>0.995024875621895</v>
       </c>
       <c r="EA21" t="n">
-        <v>1.37080191912269</v>
+        <v>1.50788211103495</v>
+      </c>
+      <c r="EB21" t="n">
+        <v>1.42857142857142</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -29917,11 +30123,14 @@
       </c>
       <c r="EA22" t="n">
         <v>2.28782287822878</v>
+      </c>
+      <c r="EB22" t="n">
+        <v>2.6354319180088</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -30311,12 +30520,15 @@
         <v>2.21940393151554</v>
       </c>
       <c r="EA23" t="n">
-        <v>2.31684408265499</v>
+        <v>2.56731371321229</v>
+      </c>
+      <c r="EB23" t="n">
+        <v>2.16049382716049</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -30706,12 +30918,15 @@
         <v>3.1615120274914</v>
       </c>
       <c r="EA24" t="n">
-        <v>2.22222222222223</v>
+        <v>2.8956228956229</v>
+      </c>
+      <c r="EB24" t="n">
+        <v>2.59826782145237</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -31101,12 +31316,15 @@
         <v>0.806451612903223</v>
       </c>
       <c r="EA25" t="n">
-        <v>1.17878192534381</v>
+        <v>1.37524557956779</v>
+      </c>
+      <c r="EB25" t="n">
+        <v>1.76125244618395</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -31497,11 +31715,14 @@
       </c>
       <c r="EA26" t="n">
         <v>3.68833563854311</v>
+      </c>
+      <c r="EB26" t="n">
+        <v>3.23905109489052</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -31891,12 +32112,15 @@
         <v>0.671140939597325</v>
       </c>
       <c r="EA27" t="n">
-        <v>0.731409995936604</v>
+        <v>0.568874441284022</v>
+      </c>
+      <c r="EB27" t="n">
+        <v>0.88353413654618</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -32287,11 +32511,14 @@
       </c>
       <c r="EA28" t="n">
         <v>4.47154471544716</v>
+      </c>
+      <c r="EB28" t="n">
+        <v>3.96284829721363</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -32681,12 +32908,15 @@
         <v>1.51753008895866</v>
       </c>
       <c r="EA29" t="n">
-        <v>1.76730486008838</v>
+        <v>1.62002945508101</v>
+      </c>
+      <c r="EB29" t="n">
+        <v>2.33009708737865</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -33076,12 +33306,15 @@
         <v>0.965250965250951</v>
       </c>
       <c r="EA30" t="n">
-        <v>0.767754318618053</v>
+        <v>0.863723608445303</v>
+      </c>
+      <c r="EB30" t="n">
+        <v>0.764818355640546</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -33213,10 +33446,11 @@
       <c r="DY31"/>
       <c r="DZ31"/>
       <c r="EA31"/>
+      <c r="EB31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -33607,11 +33841,14 @@
       </c>
       <c r="EA32" t="n">
         <v>-2.97482837528605</v>
+      </c>
+      <c r="EB32" t="n">
+        <v>-3.39366515837104</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -34001,12 +34238,15 @@
         <v>1.75631174533479</v>
       </c>
       <c r="EA33" t="n">
-        <v>1.15911485774499</v>
+        <v>0.421496311907277</v>
+      </c>
+      <c r="EB33" t="n">
+        <v>1.36125654450263</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -34396,12 +34636,15 @@
         <v>4.68354430379747</v>
       </c>
       <c r="EA34" t="n">
-        <v>5.97014925373134</v>
+        <v>5.09950248756218</v>
+      </c>
+      <c r="EB34" t="n">
+        <v>3.93603936039359</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -34792,11 +35035,14 @@
       </c>
       <c r="EA35" t="n">
         <v>1.96936542669582</v>
+      </c>
+      <c r="EB35" t="n">
+        <v>1.52173913043479</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -35187,11 +35433,14 @@
       </c>
       <c r="EA36" t="n">
         <v>5.19987000324994</v>
+      </c>
+      <c r="EB36" t="n">
+        <v>5.60386473429951</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -35581,12 +35830,15 @@
         <v>5.22088353413655</v>
       </c>
       <c r="EA37" t="n">
-        <v>7.67195767195769</v>
+        <v>7.80423280423281</v>
+      </c>
+      <c r="EB37" t="n">
+        <v>8.07291666666667</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -35977,11 +36229,14 @@
       </c>
       <c r="EA38" t="n">
         <v>0.640739085084183</v>
+      </c>
+      <c r="EB38" t="n">
+        <v>0.633284241531658</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -36372,11 +36627,14 @@
       </c>
       <c r="EA39" t="n">
         <v>1.48837209302326</v>
+      </c>
+      <c r="EB39" t="n">
+        <v>1.81037127953359</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -36767,11 +37025,14 @@
       </c>
       <c r="EA40" t="n">
         <v>3.64583333333333</v>
+      </c>
+      <c r="EB40" t="n">
+        <v>2.8423772609819</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -37161,12 +37422,15 @@
         <v>1.42706131078225</v>
       </c>
       <c r="EA41" t="n">
-        <v>1.15384615384615</v>
+        <v>0.769230769230769</v>
+      </c>
+      <c r="EB41" t="n">
+        <v>0.303720577069108</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -37556,12 +37820,15 @@
         <v>3.74479889042996</v>
       </c>
       <c r="EA42" t="n">
-        <v>4.70668485675307</v>
+        <v>4.09276944065484</v>
+      </c>
+      <c r="EB42" t="n">
+        <v>3.7237643872715</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -37951,12 +38218,15 @@
         <v>1.9277108433735</v>
       </c>
       <c r="EA43" t="n">
-        <v>1.54981549815498</v>
+        <v>2.14022140221403</v>
+      </c>
+      <c r="EB43" t="n">
+        <v>1.80766449746929</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -38346,12 +38616,15 @@
         <v>-0.77663870767319</v>
       </c>
       <c r="EA44" t="n">
-        <v>-0.485731633272641</v>
+        <v>-0.637522768670334</v>
+      </c>
+      <c r="EB44" t="n">
+        <v>-0.329934013197367</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -38741,12 +39014,15 @@
         <v>1.4336917562724</v>
       </c>
       <c r="EA45" t="n">
-        <v>3.12500000000001</v>
+        <v>3.47222222222221</v>
+      </c>
+      <c r="EB45" t="n">
+        <v>3.44827586206897</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -39136,12 +39412,15 @@
         <v>-0.124069478908182</v>
       </c>
       <c r="EA46" t="n">
-        <v>0.121951219512188</v>
+        <v>0</v>
+      </c>
+      <c r="EB46" t="n">
+        <v>-0.482509047044639</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -39531,12 +39810,15 @@
         <v>2.1917808219178</v>
       </c>
       <c r="EA47" t="n">
-        <v>1.8421052631579</v>
+        <v>2.10526315789473</v>
+      </c>
+      <c r="EB47" t="n">
+        <v>2.61096605744125</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -39926,12 +40208,15 @@
         <v>0.632911392405055</v>
       </c>
       <c r="EA48" t="n">
-        <v>1.9664268585132</v>
+        <v>0.815347721822537</v>
+      </c>
+      <c r="EB48" t="n">
+        <v>1.29248444231689</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -40321,12 +40606,15 @@
         <v>2.23656294200848</v>
       </c>
       <c r="EA49" t="n">
-        <v>1.86308862490387</v>
+        <v>1.82035723442442</v>
+      </c>
+      <c r="EB49" t="n">
+        <v>1.82296082753943</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -40717,11 +41005,14 @@
       </c>
       <c r="EA50" t="n">
         <v>4.5958795562599</v>
+      </c>
+      <c r="EB50" t="n">
+        <v>4.4776119402985</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -41111,12 +41402,15 @@
         <v>6.84039087947881</v>
       </c>
       <c r="EA51" t="n">
-        <v>6.23052959501558</v>
+        <v>6.54205607476636</v>
+      </c>
+      <c r="EB51" t="n">
+        <v>7.12074303405574</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -41507,11 +41801,14 @@
       </c>
       <c r="EA52" t="n">
         <v>3.92156862745099</v>
+      </c>
+      <c r="EB52" t="n">
+        <v>4.47854682117132</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -41901,12 +42198,15 @@
         <v>-2.63829787234042</v>
       </c>
       <c r="EA53" t="n">
-        <v>-0.241157556270094</v>
+        <v>-1.88906752411576</v>
+      </c>
+      <c r="EB53" t="n">
+        <v>-1.20433560818947</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -42296,12 +42596,15 @@
         <v>-0.834724540901491</v>
       </c>
       <c r="EA54" t="n">
-        <v>-0.648298217179912</v>
+        <v>-0.162074554294978</v>
+      </c>
+      <c r="EB54" t="n">
+        <v>-0.319488817891378</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -42691,12 +42994,15 @@
         <v>2.12136161815491</v>
       </c>
       <c r="EA55" t="n">
-        <v>2.26308345120227</v>
+        <v>2.07449316360208</v>
+      </c>
+      <c r="EB55" t="n">
+        <v>2.1586109807602</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -43086,7 +43392,10 @@
         <v>0.689655172413803</v>
       </c>
       <c r="EA56" t="n">
-        <v>0.664451827242522</v>
+        <v>0.996677740863778</v>
+      </c>
+      <c r="EB56" t="n">
+        <v>0.990099009900993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Updat on january 23rd 2024
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t xml:space="preserve">11/01/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1365,10 +1368,13 @@
       <c r="EN4" t="s">
         <v>143</v>
       </c>
+      <c r="EO4" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1794,15 +1800,18 @@
         <v>10596.8</v>
       </c>
       <c r="EM5" t="n">
-        <v>10957.3</v>
+        <v>10951.6</v>
       </c>
       <c r="EN5" t="n">
-        <v>11085.3</v>
+        <v>11070.5</v>
+      </c>
+      <c r="EO5" t="n">
+        <v>10981.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2231,12 +2240,15 @@
         <v>174.1</v>
       </c>
       <c r="EN6" t="n">
-        <v>174.8</v>
+        <v>175</v>
+      </c>
+      <c r="EO6" t="n">
+        <v>173.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2666,11 +2678,14 @@
       </c>
       <c r="EN7" t="n">
         <v>28.6</v>
+      </c>
+      <c r="EO7" t="n">
+        <v>28.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3099,12 +3114,15 @@
         <v>203.6</v>
       </c>
       <c r="EN8" t="n">
-        <v>204.6</v>
+        <v>205.1</v>
+      </c>
+      <c r="EO8" t="n">
+        <v>202.9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3534,11 +3552,14 @@
       </c>
       <c r="EN9" t="n">
         <v>102.6</v>
+      </c>
+      <c r="EO9" t="n">
+        <v>102.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -3968,11 +3989,14 @@
       </c>
       <c r="EN10" t="n">
         <v>1250.5</v>
+      </c>
+      <c r="EO10" t="n">
+        <v>1248.7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4401,12 +4425,15 @@
         <v>231.6</v>
       </c>
       <c r="EN11" t="n">
-        <v>234.2</v>
+        <v>234</v>
+      </c>
+      <c r="EO11" t="n">
+        <v>232.4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4836,11 +4863,14 @@
       </c>
       <c r="EN12" t="n">
         <v>128.8</v>
+      </c>
+      <c r="EO12" t="n">
+        <v>127.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5269,12 +5299,15 @@
         <v>39</v>
       </c>
       <c r="EN13" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="EO13" t="n">
         <v>39.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5419,10 +5452,11 @@
       <c r="EL14"/>
       <c r="EM14"/>
       <c r="EN14"/>
+      <c r="EO14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5851,12 +5885,15 @@
         <v>490</v>
       </c>
       <c r="EN15" t="n">
-        <v>494.5</v>
+        <v>490.5</v>
+      </c>
+      <c r="EO15" t="n">
+        <v>484</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6285,12 +6322,15 @@
         <v>352.5</v>
       </c>
       <c r="EN16" t="n">
-        <v>353.7</v>
+        <v>353.9</v>
+      </c>
+      <c r="EO16" t="n">
+        <v>353</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6435,10 +6475,11 @@
       <c r="EL17"/>
       <c r="EM17"/>
       <c r="EN17"/>
+      <c r="EO17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6868,11 +6909,14 @@
       </c>
       <c r="EN18" t="n">
         <v>67.4</v>
+      </c>
+      <c r="EO18" t="n">
+        <v>66.3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7301,12 +7345,15 @@
         <v>456.8</v>
       </c>
       <c r="EN19" t="n">
-        <v>460</v>
+        <v>461.3</v>
+      </c>
+      <c r="EO19" t="n">
+        <v>453.7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7736,11 +7783,14 @@
       </c>
       <c r="EN20" t="n">
         <v>235.5</v>
+      </c>
+      <c r="EO20" t="n">
+        <v>235.9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8170,11 +8220,14 @@
       </c>
       <c r="EN21" t="n">
         <v>149.1</v>
+      </c>
+      <c r="EO21" t="n">
+        <v>146.3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8604,11 +8657,14 @@
       </c>
       <c r="EN22" t="n">
         <v>140.2</v>
+      </c>
+      <c r="EO22" t="n">
+        <v>137.1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9037,12 +9093,15 @@
         <v>163.8</v>
       </c>
       <c r="EN23" t="n">
-        <v>165.5</v>
+        <v>165.2</v>
+      </c>
+      <c r="EO23" t="n">
+        <v>164.6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9471,12 +9530,15 @@
         <v>152.8</v>
       </c>
       <c r="EN24" t="n">
-        <v>154</v>
+        <v>153.7</v>
+      </c>
+      <c r="EO24" t="n">
+        <v>152.9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -9905,12 +9967,15 @@
         <v>51.6</v>
       </c>
       <c r="EN25" t="n">
-        <v>52</v>
+        <v>51.9</v>
+      </c>
+      <c r="EO25" t="n">
+        <v>49.6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10339,12 +10404,15 @@
         <v>224.9</v>
       </c>
       <c r="EN26" t="n">
-        <v>226.3</v>
+        <v>226.2</v>
+      </c>
+      <c r="EO26" t="n">
+        <v>225.3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10773,12 +10841,15 @@
         <v>247.5</v>
       </c>
       <c r="EN27" t="n">
-        <v>251.2</v>
+        <v>251.4</v>
+      </c>
+      <c r="EO27" t="n">
+        <v>249.9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11207,12 +11278,15 @@
         <v>334.1</v>
       </c>
       <c r="EN28" t="n">
-        <v>335.8</v>
+        <v>337.2</v>
+      </c>
+      <c r="EO28" t="n">
+        <v>331.7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11642,11 +11716,14 @@
       </c>
       <c r="EN29" t="n">
         <v>210.8</v>
+      </c>
+      <c r="EO29" t="n">
+        <v>205.5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12076,11 +12153,14 @@
       </c>
       <c r="EN30" t="n">
         <v>105.4</v>
+      </c>
+      <c r="EO30" t="n">
+        <v>101.8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -12225,10 +12305,11 @@
       <c r="EL31"/>
       <c r="EM31"/>
       <c r="EN31"/>
+      <c r="EO31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12658,11 +12739,14 @@
       </c>
       <c r="EN32" t="n">
         <v>42.7</v>
+      </c>
+      <c r="EO32" t="n">
+        <v>42.9</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13091,12 +13175,15 @@
         <v>95.3</v>
       </c>
       <c r="EN33" t="n">
-        <v>96.8</v>
+        <v>96.6</v>
+      </c>
+      <c r="EO33" t="n">
+        <v>95.6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -13526,11 +13613,14 @@
       </c>
       <c r="EN34" t="n">
         <v>84.5</v>
+      </c>
+      <c r="EO34" t="n">
+        <v>84.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -13960,11 +14050,14 @@
       </c>
       <c r="EN35" t="n">
         <v>46.7</v>
+      </c>
+      <c r="EO35" t="n">
+        <v>46.5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14393,12 +14486,15 @@
         <v>323.7</v>
       </c>
       <c r="EN36" t="n">
-        <v>327.9</v>
+        <v>328</v>
+      </c>
+      <c r="EO36" t="n">
+        <v>328</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -14827,12 +14923,15 @@
         <v>81.5</v>
       </c>
       <c r="EN37" t="n">
-        <v>83</v>
+        <v>82.9</v>
+      </c>
+      <c r="EO37" t="n">
+        <v>80.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -15262,11 +15361,14 @@
       </c>
       <c r="EN38" t="n">
         <v>683.3</v>
+      </c>
+      <c r="EO38" t="n">
+        <v>686.8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -15696,11 +15798,14 @@
       </c>
       <c r="EN39" t="n">
         <v>331.8</v>
+      </c>
+      <c r="EO39" t="n">
+        <v>328.5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -16130,11 +16235,14 @@
       </c>
       <c r="EN40" t="n">
         <v>39.8</v>
+      </c>
+      <c r="EO40" t="n">
+        <v>40.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -16564,11 +16672,14 @@
       </c>
       <c r="EN41" t="n">
         <v>396.3</v>
+      </c>
+      <c r="EO41" t="n">
+        <v>390.6</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -16998,11 +17109,14 @@
       </c>
       <c r="EN42" t="n">
         <v>153.2</v>
+      </c>
+      <c r="EO42" t="n">
+        <v>152.8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -17431,12 +17545,15 @@
         <v>138.4</v>
       </c>
       <c r="EN43" t="n">
-        <v>140.8</v>
+        <v>140.6</v>
+      </c>
+      <c r="EO43" t="n">
+        <v>139.9</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -17865,12 +17982,15 @@
         <v>327.3</v>
       </c>
       <c r="EN44" t="n">
-        <v>332.3</v>
+        <v>332.1</v>
+      </c>
+      <c r="EO44" t="n">
+        <v>329</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -18300,11 +18420,14 @@
       </c>
       <c r="EN45" t="n">
         <v>30</v>
+      </c>
+      <c r="EO45" t="n">
+        <v>30.2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -18734,11 +18857,14 @@
       </c>
       <c r="EN46" t="n">
         <v>165</v>
+      </c>
+      <c r="EO46" t="n">
+        <v>163.1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -19168,11 +19294,14 @@
       </c>
       <c r="EN47" t="n">
         <v>39.3</v>
+      </c>
+      <c r="EO47" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -19602,11 +19731,14 @@
       </c>
       <c r="EN48" t="n">
         <v>211.6</v>
+      </c>
+      <c r="EO48" t="n">
+        <v>209.9</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -20035,12 +20167,15 @@
         <v>1191.4</v>
       </c>
       <c r="EN49" t="n">
-        <v>1200.9</v>
+        <v>1200.7</v>
+      </c>
+      <c r="EO49" t="n">
+        <v>1197.7</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -20470,11 +20605,14 @@
       </c>
       <c r="EN50" t="n">
         <v>133</v>
+      </c>
+      <c r="EO50" t="n">
+        <v>132.7</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -20903,12 +21041,15 @@
         <v>34.2</v>
       </c>
       <c r="EN51" t="n">
-        <v>34.6</v>
+        <v>34.4</v>
+      </c>
+      <c r="EO51" t="n">
+        <v>34.2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -21337,12 +21478,15 @@
         <v>328.6</v>
       </c>
       <c r="EN52" t="n">
-        <v>333.6</v>
+        <v>333.1</v>
+      </c>
+      <c r="EO52" t="n">
+        <v>327.7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -21771,12 +21915,15 @@
         <v>244.1</v>
       </c>
       <c r="EN53" t="n">
-        <v>246.1</v>
+        <v>246.5</v>
+      </c>
+      <c r="EO53" t="n">
+        <v>245.6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -22205,12 +22352,15 @@
         <v>61.6</v>
       </c>
       <c r="EN54" t="n">
-        <v>62.4</v>
+        <v>62.2</v>
+      </c>
+      <c r="EO54" t="n">
+        <v>61.6</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -22639,12 +22789,15 @@
         <v>216.5</v>
       </c>
       <c r="EN55" t="n">
-        <v>217.7</v>
+        <v>217.4</v>
+      </c>
+      <c r="EO55" t="n">
+        <v>215</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -23073,6 +23226,9 @@
         <v>30.4</v>
       </c>
       <c r="EN56" t="n">
+        <v>30.6</v>
+      </c>
+      <c r="EO56" t="n">
         <v>30.6</v>
       </c>
     </row>
@@ -23487,10 +23643,13 @@
       <c r="EB4" t="s">
         <v>143</v>
       </c>
+      <c r="EC4" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -23880,15 +24039,18 @@
         <v>2.46770325674943</v>
       </c>
       <c r="EA5" t="n">
-        <v>2.8728887553632</v>
+        <v>2.81937416090056</v>
       </c>
       <c r="EB5" t="n">
-        <v>2.92948801277647</v>
+        <v>2.7920667050456</v>
+      </c>
+      <c r="EC5" t="n">
+        <v>3.34550450772619</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -24281,12 +24443,15 @@
         <v>0.694042799305951</v>
       </c>
       <c r="EB6" t="n">
-        <v>0.286861732644865</v>
+        <v>0.401606425702805</v>
+      </c>
+      <c r="EC6" t="n">
+        <v>0.636942675159249</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -24680,11 +24845,14 @@
       </c>
       <c r="EB7" t="n">
         <v>0.350877192982461</v>
+      </c>
+      <c r="EC7" t="n">
+        <v>1.76678445229682</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -25077,12 +25245,15 @@
         <v>4.73251028806585</v>
       </c>
       <c r="EB8" t="n">
-        <v>3.54251012145749</v>
+        <v>3.79554655870447</v>
+      </c>
+      <c r="EC8" t="n">
+        <v>7.35449735449736</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -25476,11 +25647,14 @@
       </c>
       <c r="EB9" t="n">
         <v>0.195312499999989</v>
+      </c>
+      <c r="EC9" t="n">
+        <v>0.195694716242678</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -25874,11 +26048,14 @@
       </c>
       <c r="EB10" t="n">
         <v>1.21408336705787</v>
+      </c>
+      <c r="EC10" t="n">
+        <v>4.8710842361636</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -26271,12 +26448,15 @@
         <v>3.6241610738255</v>
       </c>
       <c r="EB11" t="n">
-        <v>3.95028850421659</v>
+        <v>3.86151797603195</v>
+      </c>
+      <c r="EC11" t="n">
+        <v>4.26200089726336</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -26670,11 +26850,14 @@
       </c>
       <c r="EB12" t="n">
         <v>1.57728706624607</v>
+      </c>
+      <c r="EC12" t="n">
+        <v>1.75718849840257</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -27068,11 +27251,14 @@
       </c>
       <c r="EB13" t="n">
         <v>3.70370370370372</v>
+      </c>
+      <c r="EC13" t="n">
+        <v>2.61780104712042</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -27205,10 +27391,11 @@
       <c r="DZ14"/>
       <c r="EA14"/>
       <c r="EB14"/>
+      <c r="EC14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -27601,12 +27788,15 @@
         <v>1.55440414507772</v>
       </c>
       <c r="EB15" t="n">
-        <v>1.62351006987258</v>
+        <v>0.801479654747221</v>
+      </c>
+      <c r="EC15" t="n">
+        <v>0.665557404326121</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -27999,12 +28189,15 @@
         <v>2.97984224364592</v>
       </c>
       <c r="EB16" t="n">
-        <v>2.78988666085441</v>
+        <v>2.84800929962219</v>
+      </c>
+      <c r="EC16" t="n">
+        <v>2.88545613523753</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -28137,10 +28330,11 @@
       <c r="DZ17"/>
       <c r="EA17"/>
       <c r="EB17"/>
+      <c r="EC17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -28534,11 +28728,14 @@
       </c>
       <c r="EB18" t="n">
         <v>4.82115085536549</v>
+      </c>
+      <c r="EC18" t="n">
+        <v>6.24999999999999</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -28931,12 +29128,15 @@
         <v>3.72388737511353</v>
       </c>
       <c r="EB19" t="n">
-        <v>3.51035103510352</v>
+        <v>3.80288028802881</v>
+      </c>
+      <c r="EC19" t="n">
+        <v>3.67915904936015</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -29330,11 +29530,14 @@
       </c>
       <c r="EB20" t="n">
         <v>3.01837270341208</v>
+      </c>
+      <c r="EC20" t="n">
+        <v>4.56560283687942</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -29728,11 +29931,14 @@
       </c>
       <c r="EB21" t="n">
         <v>1.42857142857142</v>
+      </c>
+      <c r="EC21" t="n">
+        <v>0.688231245698555</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -30126,11 +30332,14 @@
       </c>
       <c r="EB22" t="n">
         <v>2.6354319180088</v>
+      </c>
+      <c r="EC22" t="n">
+        <v>2.61976047904192</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -30523,12 +30732,15 @@
         <v>2.56731371321229</v>
       </c>
       <c r="EB23" t="n">
-        <v>2.16049382716049</v>
+        <v>1.9753086419753</v>
+      </c>
+      <c r="EC23" t="n">
+        <v>3.52201257861635</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -30921,12 +31133,15 @@
         <v>2.8956228956229</v>
       </c>
       <c r="EB24" t="n">
-        <v>2.59826782145237</v>
+        <v>2.39840106595603</v>
+      </c>
+      <c r="EC24" t="n">
+        <v>2.54862508383636</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -31319,12 +31534,15 @@
         <v>1.37524557956779</v>
       </c>
       <c r="EB25" t="n">
-        <v>1.76125244618395</v>
+        <v>1.5655577299413</v>
+      </c>
+      <c r="EC25" t="n">
+        <v>1.84804928131417</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -31717,12 +31935,15 @@
         <v>3.68833563854311</v>
       </c>
       <c r="EB26" t="n">
-        <v>3.23905109489052</v>
+        <v>3.19343065693431</v>
+      </c>
+      <c r="EC26" t="n">
+        <v>3.15934065934066</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -32115,12 +32336,15 @@
         <v>0.568874441284022</v>
       </c>
       <c r="EB27" t="n">
-        <v>0.88353413654618</v>
+        <v>0.963855421686749</v>
+      </c>
+      <c r="EC27" t="n">
+        <v>1.54408776919952</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -32513,12 +32737,15 @@
         <v>4.47154471544716</v>
       </c>
       <c r="EB28" t="n">
-        <v>3.96284829721363</v>
+        <v>4.39628482972136</v>
+      </c>
+      <c r="EC28" t="n">
+        <v>4.17713567839196</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -32912,11 +33139,14 @@
       </c>
       <c r="EB29" t="n">
         <v>2.33009708737865</v>
+      </c>
+      <c r="EC29" t="n">
+        <v>1.78306092124815</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -33310,11 +33540,14 @@
       </c>
       <c r="EB30" t="n">
         <v>0.764818355640546</v>
+      </c>
+      <c r="EC30" t="n">
+        <v>1.19284294234594</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -33447,10 +33680,11 @@
       <c r="DZ31"/>
       <c r="EA31"/>
       <c r="EB31"/>
+      <c r="EC31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -33844,11 +34078,14 @@
       </c>
       <c r="EB32" t="n">
         <v>-3.39366515837104</v>
+      </c>
+      <c r="EC32" t="n">
+        <v>-2.27790432801822</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -34241,12 +34478,15 @@
         <v>0.421496311907277</v>
       </c>
       <c r="EB33" t="n">
-        <v>1.36125654450263</v>
+        <v>1.15183246073298</v>
+      </c>
+      <c r="EC33" t="n">
+        <v>-0.20876826722337</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -34640,11 +34880,14 @@
       </c>
       <c r="EB34" t="n">
         <v>3.93603936039359</v>
+      </c>
+      <c r="EC34" t="n">
+        <v>3.3169533169533</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -35038,11 +35281,14 @@
       </c>
       <c r="EB35" t="n">
         <v>1.52173913043479</v>
+      </c>
+      <c r="EC35" t="n">
+        <v>2.42290748898679</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -35435,12 +35681,15 @@
         <v>5.19987000324994</v>
       </c>
       <c r="EB36" t="n">
-        <v>5.60386473429951</v>
+        <v>5.63607085346216</v>
+      </c>
+      <c r="EC36" t="n">
+        <v>5.26315789473685</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -35833,12 +36082,15 @@
         <v>7.80423280423281</v>
       </c>
       <c r="EB37" t="n">
-        <v>8.07291666666667</v>
+        <v>7.94270833333335</v>
+      </c>
+      <c r="EC37" t="n">
+        <v>5.23560209424084</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -36232,11 +36484,14 @@
       </c>
       <c r="EB38" t="n">
         <v>0.633284241531658</v>
+      </c>
+      <c r="EC38" t="n">
+        <v>1.65778567199527</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -36630,11 +36885,14 @@
       </c>
       <c r="EB39" t="n">
         <v>1.81037127953359</v>
+      </c>
+      <c r="EC39" t="n">
+        <v>1.79733498605516</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -37028,11 +37286,14 @@
       </c>
       <c r="EB40" t="n">
         <v>2.8423772609819</v>
+      </c>
+      <c r="EC40" t="n">
+        <v>3.8860103626943</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -37426,11 +37687,14 @@
       </c>
       <c r="EB41" t="n">
         <v>0.303720577069108</v>
+      </c>
+      <c r="EC41" t="n">
+        <v>0.878099173553728</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -37824,11 +38088,14 @@
       </c>
       <c r="EB42" t="n">
         <v>3.7237643872715</v>
+      </c>
+      <c r="EC42" t="n">
+        <v>3.66350067842608</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -38221,12 +38488,15 @@
         <v>2.14022140221403</v>
       </c>
       <c r="EB43" t="n">
-        <v>1.80766449746929</v>
+        <v>1.66305133767174</v>
+      </c>
+      <c r="EC43" t="n">
+        <v>1.52394775036284</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -38619,12 +38889,15 @@
         <v>-0.637522768670334</v>
       </c>
       <c r="EB44" t="n">
-        <v>-0.329934013197367</v>
+        <v>-0.389922015596884</v>
+      </c>
+      <c r="EC44" t="n">
+        <v>-0.0911023382933357</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -39018,11 +39291,14 @@
       </c>
       <c r="EB45" t="n">
         <v>3.44827586206897</v>
+      </c>
+      <c r="EC45" t="n">
+        <v>4.13793103448276</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -39416,11 +39692,14 @@
       </c>
       <c r="EB46" t="n">
         <v>-0.482509047044639</v>
+      </c>
+      <c r="EC46" t="n">
+        <v>-0.548780487804864</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -39814,11 +40093,14 @@
       </c>
       <c r="EB47" t="n">
         <v>2.61096605744125</v>
+      </c>
+      <c r="EC47" t="n">
+        <v>3.17460317460318</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -40212,11 +40494,14 @@
       </c>
       <c r="EB48" t="n">
         <v>1.29248444231689</v>
+      </c>
+      <c r="EC48" t="n">
+        <v>0.768122899663944</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -40609,12 +40894,15 @@
         <v>1.82035723442442</v>
       </c>
       <c r="EB49" t="n">
-        <v>1.82296082753943</v>
+        <v>1.80600305239952</v>
+      </c>
+      <c r="EC49" t="n">
+        <v>1.97530864197531</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -41008,11 +41296,14 @@
       </c>
       <c r="EB50" t="n">
         <v>4.4776119402985</v>
+      </c>
+      <c r="EC50" t="n">
+        <v>4.32389937106918</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -41405,12 +41696,15 @@
         <v>6.54205607476636</v>
       </c>
       <c r="EB51" t="n">
-        <v>7.12074303405574</v>
+        <v>6.5015479876161</v>
+      </c>
+      <c r="EC51" t="n">
+        <v>6.2111801242236</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -41803,12 +42097,15 @@
         <v>3.92156862745099</v>
       </c>
       <c r="EB52" t="n">
-        <v>4.47854682117132</v>
+        <v>4.32195427497651</v>
+      </c>
+      <c r="EC52" t="n">
+        <v>2.53441802252817</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -42201,12 +42498,15 @@
         <v>-1.88906752411576</v>
       </c>
       <c r="EB53" t="n">
-        <v>-1.20433560818947</v>
+        <v>-1.04375752709755</v>
+      </c>
+      <c r="EC53" t="n">
+        <v>-1.2464817048653</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -42599,12 +42899,15 @@
         <v>-0.162074554294978</v>
       </c>
       <c r="EB54" t="n">
-        <v>-0.319488817891378</v>
+        <v>-0.638977635782757</v>
+      </c>
+      <c r="EC54" t="n">
+        <v>-0.484652665589668</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -42997,12 +43300,15 @@
         <v>2.07449316360208</v>
       </c>
       <c r="EB55" t="n">
-        <v>2.1586109807602</v>
+        <v>2.01783200375411</v>
+      </c>
+      <c r="EC55" t="n">
+        <v>1.99240986717267</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -43396,6 +43702,9 @@
       </c>
       <c r="EB56" t="n">
         <v>0.990099009900993</v>
+      </c>
+      <c r="EC56" t="n">
+        <v>0.990099009900981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on April 19, 2024
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t xml:space="preserve">02/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1383,10 +1386,13 @@
       <c r="EQ4" t="s">
         <v>146</v>
       </c>
+      <c r="ER4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1821,15 +1827,18 @@
         <v>11046.7</v>
       </c>
       <c r="EP5" t="n">
-        <v>10725.7</v>
+        <v>10720.4</v>
       </c>
       <c r="EQ5" t="n">
-        <v>11104.8</v>
+        <v>11103.8</v>
+      </c>
+      <c r="ER5" t="n">
+        <v>11161.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2267,12 +2276,15 @@
         <v>172.2</v>
       </c>
       <c r="EQ6" t="n">
-        <v>174.5</v>
+        <v>174.3</v>
+      </c>
+      <c r="ER6" t="n">
+        <v>175.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2710,12 +2722,15 @@
         <v>27.2</v>
       </c>
       <c r="EQ7" t="n">
-        <v>29</v>
+        <v>28.9</v>
+      </c>
+      <c r="ER7" t="n">
+        <v>28.9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3153,12 +3168,15 @@
         <v>197.2</v>
       </c>
       <c r="EQ8" t="n">
-        <v>203</v>
+        <v>203.1</v>
+      </c>
+      <c r="ER8" t="n">
+        <v>202.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3597,11 +3615,14 @@
       </c>
       <c r="EQ9" t="n">
         <v>102.9</v>
+      </c>
+      <c r="ER9" t="n">
+        <v>103.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4039,12 +4060,15 @@
         <v>1253.8</v>
       </c>
       <c r="EQ10" t="n">
-        <v>1264</v>
+        <v>1266.2</v>
+      </c>
+      <c r="ER10" t="n">
+        <v>1284.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4482,12 +4506,15 @@
         <v>226.2</v>
       </c>
       <c r="EQ11" t="n">
-        <v>236.8</v>
+        <v>236.7</v>
+      </c>
+      <c r="ER11" t="n">
+        <v>239.8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4926,11 +4953,14 @@
       </c>
       <c r="EQ12" t="n">
         <v>125.1</v>
+      </c>
+      <c r="ER12" t="n">
+        <v>125.6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5368,12 +5398,15 @@
         <v>37.8</v>
       </c>
       <c r="EQ13" t="n">
-        <v>39.8</v>
+        <v>40.3</v>
+      </c>
+      <c r="ER13" t="n">
+        <v>41.1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5521,10 +5554,11 @@
       <c r="EO14"/>
       <c r="EP14"/>
       <c r="EQ14"/>
+      <c r="ER14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -5962,12 +5996,15 @@
         <v>489</v>
       </c>
       <c r="EQ15" t="n">
+        <v>499.5</v>
+      </c>
+      <c r="ER15" t="n">
         <v>499.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6405,12 +6442,15 @@
         <v>351.6</v>
       </c>
       <c r="EQ16" t="n">
-        <v>354.7</v>
+        <v>354.8</v>
+      </c>
+      <c r="ER16" t="n">
+        <v>355.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6558,10 +6598,11 @@
       <c r="EO17"/>
       <c r="EP17"/>
       <c r="EQ17"/>
+      <c r="ER17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -6999,12 +7040,15 @@
         <v>63.9</v>
       </c>
       <c r="EQ18" t="n">
-        <v>66.5</v>
+        <v>66.6</v>
+      </c>
+      <c r="ER18" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7442,12 +7486,15 @@
         <v>431.2</v>
       </c>
       <c r="EQ19" t="n">
-        <v>456.6</v>
+        <v>458.3</v>
+      </c>
+      <c r="ER19" t="n">
+        <v>461.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7886,11 +7933,14 @@
       </c>
       <c r="EQ20" t="n">
         <v>235.1</v>
+      </c>
+      <c r="ER20" t="n">
+        <v>236</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8328,12 +8378,15 @@
         <v>142.6</v>
       </c>
       <c r="EQ21" t="n">
-        <v>147.4</v>
+        <v>148</v>
+      </c>
+      <c r="ER21" t="n">
+        <v>148.6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8772,11 +8825,14 @@
       </c>
       <c r="EQ22" t="n">
         <v>137.3</v>
+      </c>
+      <c r="ER22" t="n">
+        <v>137.9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9215,11 +9271,14 @@
       </c>
       <c r="EQ23" t="n">
         <v>164.6</v>
+      </c>
+      <c r="ER23" t="n">
+        <v>165.6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9657,12 +9716,15 @@
         <v>145.6</v>
       </c>
       <c r="EQ24" t="n">
-        <v>146.4</v>
+        <v>147</v>
+      </c>
+      <c r="ER24" t="n">
+        <v>147.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10100,12 +10162,15 @@
         <v>49.6</v>
       </c>
       <c r="EQ25" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="ER25" t="n">
         <v>50.3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10544,11 +10609,14 @@
       </c>
       <c r="EQ26" t="n">
         <v>221.9</v>
+      </c>
+      <c r="ER26" t="n">
+        <v>224.6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -10987,11 +11055,14 @@
       </c>
       <c r="EQ27" t="n">
         <v>246.3</v>
+      </c>
+      <c r="ER27" t="n">
+        <v>247.1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11429,12 +11500,15 @@
         <v>306.5</v>
       </c>
       <c r="EQ28" t="n">
-        <v>327.8</v>
+        <v>328.7</v>
+      </c>
+      <c r="ER28" t="n">
+        <v>329.5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11873,11 +11947,14 @@
       </c>
       <c r="EQ29" t="n">
         <v>219.2</v>
+      </c>
+      <c r="ER29" t="n">
+        <v>219.1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12315,12 +12392,15 @@
         <v>102</v>
       </c>
       <c r="EQ30" t="n">
-        <v>104.9</v>
+        <v>104.8</v>
+      </c>
+      <c r="ER30" t="n">
+        <v>105.1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -12468,10 +12548,11 @@
       <c r="EO31"/>
       <c r="EP31"/>
       <c r="EQ31"/>
+      <c r="ER31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12910,11 +12991,14 @@
       </c>
       <c r="EQ32" t="n">
         <v>44.6</v>
+      </c>
+      <c r="ER32" t="n">
+        <v>44.8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13353,11 +13437,14 @@
       </c>
       <c r="EQ33" t="n">
         <v>94</v>
+      </c>
+      <c r="ER33" t="n">
+        <v>94.8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -13795,12 +13882,15 @@
         <v>77.3</v>
       </c>
       <c r="EQ34" t="n">
-        <v>85</v>
+        <v>85.2</v>
+      </c>
+      <c r="ER34" t="n">
+        <v>85.4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -14238,12 +14328,15 @@
         <v>43</v>
       </c>
       <c r="EQ35" t="n">
-        <v>46.2</v>
+        <v>46.3</v>
+      </c>
+      <c r="ER35" t="n">
+        <v>46.5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14681,12 +14774,15 @@
         <v>309.9</v>
       </c>
       <c r="EQ36" t="n">
-        <v>321.2</v>
+        <v>321.1</v>
+      </c>
+      <c r="ER36" t="n">
+        <v>322.8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -15124,12 +15220,15 @@
         <v>76.7</v>
       </c>
       <c r="EQ37" t="n">
-        <v>80.7</v>
+        <v>80.8</v>
+      </c>
+      <c r="ER37" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -15568,11 +15667,14 @@
       </c>
       <c r="EQ38" t="n">
         <v>680.7</v>
+      </c>
+      <c r="ER38" t="n">
+        <v>683.7</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16011,11 +16113,14 @@
       </c>
       <c r="EQ39" t="n">
         <v>340.1</v>
+      </c>
+      <c r="ER39" t="n">
+        <v>343.3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -16454,11 +16559,14 @@
       </c>
       <c r="EQ40" t="n">
         <v>39.5</v>
+      </c>
+      <c r="ER40" t="n">
+        <v>39.2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -16896,12 +17004,15 @@
         <v>378.7</v>
       </c>
       <c r="EQ41" t="n">
-        <v>393</v>
+        <v>392</v>
+      </c>
+      <c r="ER41" t="n">
+        <v>395.7</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -17339,12 +17450,15 @@
         <v>141.3</v>
       </c>
       <c r="EQ42" t="n">
-        <v>149.5</v>
+        <v>152.5</v>
+      </c>
+      <c r="ER42" t="n">
+        <v>153.3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -17782,12 +17896,15 @@
         <v>138.1</v>
       </c>
       <c r="EQ43" t="n">
-        <v>142.2</v>
+        <v>142.1</v>
+      </c>
+      <c r="ER43" t="n">
+        <v>143.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -18226,11 +18343,14 @@
       </c>
       <c r="EQ44" t="n">
         <v>334.9</v>
+      </c>
+      <c r="ER44" t="n">
+        <v>336.1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -18669,11 +18789,14 @@
       </c>
       <c r="EQ45" t="n">
         <v>29.6</v>
+      </c>
+      <c r="ER45" t="n">
+        <v>29.9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -19111,12 +19234,15 @@
         <v>158.8</v>
       </c>
       <c r="EQ46" t="n">
-        <v>163.9</v>
+        <v>164.3</v>
+      </c>
+      <c r="ER46" t="n">
+        <v>164.6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -19554,12 +19680,15 @@
         <v>37.5</v>
       </c>
       <c r="EQ47" t="n">
-        <v>38.9</v>
+        <v>38.8</v>
+      </c>
+      <c r="ER47" t="n">
+        <v>39.1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -19997,12 +20126,15 @@
         <v>198.2</v>
       </c>
       <c r="EQ48" t="n">
-        <v>208.2</v>
+        <v>207.8</v>
+      </c>
+      <c r="ER48" t="n">
+        <v>208.9</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -20440,12 +20572,15 @@
         <v>1170.5</v>
       </c>
       <c r="EQ49" t="n">
-        <v>1204</v>
+        <v>1205</v>
+      </c>
+      <c r="ER49" t="n">
+        <v>1206.6</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -20884,11 +21019,14 @@
       </c>
       <c r="EQ50" t="n">
         <v>135</v>
+      </c>
+      <c r="ER50" t="n">
+        <v>135.3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -21326,12 +21464,15 @@
         <v>31.8</v>
       </c>
       <c r="EQ51" t="n">
-        <v>33.3</v>
+        <v>33.2</v>
+      </c>
+      <c r="ER51" t="n">
+        <v>32.9</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -21770,11 +21911,14 @@
       </c>
       <c r="EQ52" t="n">
         <v>332</v>
+      </c>
+      <c r="ER52" t="n">
+        <v>334.1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -22212,12 +22356,15 @@
         <v>253.8</v>
       </c>
       <c r="EQ53" t="n">
-        <v>255.5</v>
+        <v>255.8</v>
+      </c>
+      <c r="ER53" t="n">
+        <v>257.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -22656,11 +22803,14 @@
       </c>
       <c r="EQ54" t="n">
         <v>63.6</v>
+      </c>
+      <c r="ER54" t="n">
+        <v>64.2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -23098,12 +23248,15 @@
         <v>198.6</v>
       </c>
       <c r="EQ55" t="n">
+        <v>216.6</v>
+      </c>
+      <c r="ER55" t="n">
         <v>216.5</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -23542,6 +23695,9 @@
       </c>
       <c r="EQ56" t="n">
         <v>31.2</v>
+      </c>
+      <c r="ER56" t="n">
+        <v>31.6</v>
       </c>
     </row>
   </sheetData>
@@ -23964,10 +24120,13 @@
       <c r="EE4" t="s">
         <v>146</v>
       </c>
+      <c r="EF4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -24366,15 +24525,18 @@
         <v>3.4499873575382</v>
       </c>
       <c r="ED5" t="n">
-        <v>2.50879272115605</v>
+        <v>2.4581390014527</v>
       </c>
       <c r="EE5" t="n">
-        <v>2.33895493502902</v>
+        <v>2.32973919454429</v>
+      </c>
+      <c r="EF5" t="n">
+        <v>2.52048352132858</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -24776,12 +24938,15 @@
         <v>1.11567821491484</v>
       </c>
       <c r="EE6" t="n">
-        <v>1.1008111239861</v>
+        <v>0.984936268829674</v>
+      </c>
+      <c r="EF6" t="n">
+        <v>1.09383995394358</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -25183,12 +25348,15 @@
         <v>-0.366300366300346</v>
       </c>
       <c r="EE7" t="n">
-        <v>0.34602076124568</v>
+        <v>0</v>
+      </c>
+      <c r="EF7" t="n">
+        <v>0.347222222222215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -25590,12 +25758,15 @@
         <v>0.869565217391299</v>
       </c>
       <c r="EE8" t="n">
-        <v>0.644521566683198</v>
+        <v>0.694100148735763</v>
+      </c>
+      <c r="EF8" t="n">
+        <v>1.19940029985006</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -25998,11 +26169,14 @@
       </c>
       <c r="EE9" t="n">
         <v>0.98135426889107</v>
+      </c>
+      <c r="EF9" t="n">
+        <v>1.07421874999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -26404,12 +26578,15 @@
         <v>3.00690108445612</v>
       </c>
       <c r="EE10" t="n">
-        <v>3.05748063595597</v>
+        <v>3.23685283326539</v>
+      </c>
+      <c r="EF10" t="n">
+        <v>3.11571508873363</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -26811,12 +26988,15 @@
         <v>4.77072718851319</v>
       </c>
       <c r="EE11" t="n">
-        <v>5.99820948970457</v>
+        <v>5.95344673231872</v>
+      </c>
+      <c r="EF11" t="n">
+        <v>6.15316511730855</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -27219,11 +27399,14 @@
       </c>
       <c r="EE12" t="n">
         <v>-0.318725099601598</v>
+      </c>
+      <c r="EF12" t="n">
+        <v>-0.475435816164824</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -27625,12 +27808,15 @@
         <v>3.27868852459015</v>
       </c>
       <c r="EE13" t="n">
-        <v>2.8423772609819</v>
+        <v>4.13436692506458</v>
+      </c>
+      <c r="EF13" t="n">
+        <v>4.31472081218271</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -27766,10 +27952,11 @@
       <c r="EC14"/>
       <c r="ED14"/>
       <c r="EE14"/>
+      <c r="EF14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -28172,11 +28359,14 @@
       </c>
       <c r="EE15" t="n">
         <v>1.17480251164674</v>
+      </c>
+      <c r="EF15" t="n">
+        <v>1.40073081607796</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -28578,12 +28768,15 @@
         <v>2.5371828521435</v>
       </c>
       <c r="EE16" t="n">
-        <v>2.42564250649725</v>
+        <v>2.45451920300318</v>
+      </c>
+      <c r="EF16" t="n">
+        <v>2.33227756982435</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -28719,10 +28912,11 @@
       <c r="EC17"/>
       <c r="ED17"/>
       <c r="EE17"/>
+      <c r="EF17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -29124,12 +29318,15 @@
         <v>4.58265139116202</v>
       </c>
       <c r="EE18" t="n">
-        <v>3.58255451713395</v>
+        <v>3.73831775700933</v>
+      </c>
+      <c r="EF18" t="n">
+        <v>5.34591194968553</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -29531,12 +29728,15 @@
         <v>1.12570356472796</v>
       </c>
       <c r="EE19" t="n">
-        <v>3.30316742081447</v>
+        <v>3.68778280542985</v>
+      </c>
+      <c r="EF19" t="n">
+        <v>3.59469782071443</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -29938,12 +30138,15 @@
         <v>1.52877697841727</v>
       </c>
       <c r="EE20" t="n">
-        <v>2.5294374182294</v>
+        <v>2.52943741822939</v>
+      </c>
+      <c r="EF20" t="n">
+        <v>1.1139674378749</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -30345,12 +30548,15 @@
         <v>0.706214689265537</v>
       </c>
       <c r="EE21" t="n">
-        <v>0.683060109289617</v>
+        <v>1.09289617486338</v>
+      </c>
+      <c r="EF21" t="n">
+        <v>1.43344709897611</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -30753,11 +30959,14 @@
       </c>
       <c r="EE22" t="n">
         <v>0.218978102189789</v>
+      </c>
+      <c r="EF22" t="n">
+        <v>0.877834674469654</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -31160,11 +31369,14 @@
       </c>
       <c r="EE23" t="n">
         <v>1.04358502148557</v>
+      </c>
+      <c r="EF23" t="n">
+        <v>0.79123554473523</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -31566,12 +31778,15 @@
         <v>-0.884955752212378</v>
       </c>
       <c r="EE24" t="n">
-        <v>-1.74496644295304</v>
+        <v>-1.34228187919463</v>
+      </c>
+      <c r="EF24" t="n">
+        <v>-0.40567951318458</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -31973,12 +32188,15 @@
         <v>3.11850311850312</v>
       </c>
       <c r="EE25" t="n">
-        <v>3.07377049180329</v>
+        <v>3.27868852459018</v>
+      </c>
+      <c r="EF25" t="n">
+        <v>2.65306122448979</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -32381,11 +32599,14 @@
       </c>
       <c r="EE26" t="n">
         <v>2.92207792207793</v>
+      </c>
+      <c r="EF26" t="n">
+        <v>2.41678066575467</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -32788,11 +33009,14 @@
       </c>
       <c r="EE27" t="n">
         <v>1.39975298476738</v>
+      </c>
+      <c r="EF27" t="n">
+        <v>1.3120131201312</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -33194,12 +33418,15 @@
         <v>3.58229131463333</v>
       </c>
       <c r="EE28" t="n">
-        <v>4.96317643291707</v>
+        <v>5.2513608709574</v>
+      </c>
+      <c r="EF28" t="n">
+        <v>5.7784911717496</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -33602,11 +33829,14 @@
       </c>
       <c r="EE29" t="n">
         <v>5.33397405093703</v>
+      </c>
+      <c r="EF29" t="n">
+        <v>5.3872053872054</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -34008,12 +34238,15 @@
         <v>1.49253731343284</v>
       </c>
       <c r="EE30" t="n">
-        <v>1.15718418514949</v>
+        <v>1.06075216972037</v>
+      </c>
+      <c r="EF30" t="n">
+        <v>1.0576923076923</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -34149,10 +34382,11 @@
       <c r="EC31"/>
       <c r="ED31"/>
       <c r="EE31"/>
+      <c r="EF31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -34555,11 +34789,14 @@
       </c>
       <c r="EE32" t="n">
         <v>1.82648401826485</v>
+      </c>
+      <c r="EF32" t="n">
+        <v>1.81818181818181</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -34962,11 +35199,14 @@
       </c>
       <c r="EE33" t="n">
         <v>-0.212314225053082</v>
+      </c>
+      <c r="EF33" t="n">
+        <v>0.105596620908125</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -35368,12 +35608,15 @@
         <v>4.88466757123473</v>
       </c>
       <c r="EE34" t="n">
-        <v>4.16666666666667</v>
+        <v>4.41176470588235</v>
+      </c>
+      <c r="EF34" t="n">
+        <v>4.40097799511002</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -35775,12 +36018,15 @@
         <v>0.233100233100236</v>
       </c>
       <c r="EE35" t="n">
-        <v>0.87336244541486</v>
+        <v>1.09170305676856</v>
+      </c>
+      <c r="EF35" t="n">
+        <v>1.52838427947597</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -36182,12 +36428,15 @@
         <v>2.7860696517413</v>
       </c>
       <c r="EE36" t="n">
-        <v>2.06545916746107</v>
+        <v>2.03368287257707</v>
+      </c>
+      <c r="EF36" t="n">
+        <v>2.24897054165346</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -36589,12 +36838,15 @@
         <v>3.23014804845223</v>
       </c>
       <c r="EE37" t="n">
-        <v>3.86100386100386</v>
+        <v>3.989703989704</v>
+      </c>
+      <c r="EF37" t="n">
+        <v>3.97946084724004</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -36997,11 +37249,14 @@
       </c>
       <c r="EE38" t="n">
         <v>2.51506024096386</v>
+      </c>
+      <c r="EF38" t="n">
+        <v>2.50374812593704</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -37404,11 +37659,14 @@
       </c>
       <c r="EE39" t="n">
         <v>2.04020402040204</v>
+      </c>
+      <c r="EF39" t="n">
+        <v>2.08147487362472</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -37811,11 +38069,14 @@
       </c>
       <c r="EE40" t="n">
         <v>1.54241645244216</v>
+      </c>
+      <c r="EF40" t="n">
+        <v>0.771208226221091</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -38217,12 +38478,15 @@
         <v>-0.525348043078525</v>
       </c>
       <c r="EE41" t="n">
-        <v>-1.52843898772238</v>
+        <v>-1.77900275620146</v>
+      </c>
+      <c r="EF41" t="n">
+        <v>-0.100984599848532</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -38624,12 +38888,15 @@
         <v>1.21776504297995</v>
       </c>
       <c r="EE42" t="n">
-        <v>1.01351351351351</v>
+        <v>3.04054054054054</v>
+      </c>
+      <c r="EF42" t="n">
+        <v>2.8169014084507</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -39031,12 +39298,15 @@
         <v>2.37212750185326</v>
       </c>
       <c r="EE43" t="n">
-        <v>2.52343186733958</v>
+        <v>2.45133381398703</v>
+      </c>
+      <c r="EF43" t="n">
+        <v>2.79369627507162</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -39439,11 +39709,14 @@
       </c>
       <c r="EE44" t="n">
         <v>1.60800970873788</v>
+      </c>
+      <c r="EF44" t="n">
+        <v>1.60217654171704</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -39846,11 +40119,14 @@
       </c>
       <c r="EE45" t="n">
         <v>0.338983050847462</v>
+      </c>
+      <c r="EF45" t="n">
+        <v>-0.993377483443711</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -40252,12 +40528,15 @@
         <v>0.889453621346909</v>
       </c>
       <c r="EE46" t="n">
-        <v>0.490496627835691</v>
+        <v>0.735744941753536</v>
+      </c>
+      <c r="EF46" t="n">
+        <v>0.365853658536582</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -40659,12 +40938,15 @@
         <v>2.73972602739726</v>
       </c>
       <c r="EE47" t="n">
-        <v>2.09973753280841</v>
+        <v>1.83727034120736</v>
+      </c>
+      <c r="EF47" t="n">
+        <v>2.08877284595301</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -41066,12 +41348,15 @@
         <v>-1.34395221503233</v>
       </c>
       <c r="EE48" t="n">
-        <v>-1.18652112007592</v>
+        <v>-1.37636449928808</v>
+      </c>
+      <c r="EF48" t="n">
+        <v>-1.0421601136902</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -41473,12 +41758,15 @@
         <v>2.12895907861444</v>
       </c>
       <c r="EE49" t="n">
-        <v>2.80932456664675</v>
+        <v>2.8947143711041</v>
+      </c>
+      <c r="EF49" t="n">
+        <v>2.83814881104576</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -41881,11 +42169,14 @@
       </c>
       <c r="EE50" t="n">
         <v>4.8951048951049</v>
+      </c>
+      <c r="EF50" t="n">
+        <v>4.88372093023257</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -42287,12 +42578,15 @@
         <v>2.9126213592233</v>
       </c>
       <c r="EE51" t="n">
-        <v>3.09597523219814</v>
+        <v>2.78637770897835</v>
+      </c>
+      <c r="EF51" t="n">
+        <v>2.49221183800627</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -42695,11 +42989,14 @@
       </c>
       <c r="EE52" t="n">
         <v>2.85006195786865</v>
+      </c>
+      <c r="EF52" t="n">
+        <v>3.08546744831842</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -43101,12 +43398,15 @@
         <v>1.72344689378758</v>
       </c>
       <c r="EE53" t="n">
-        <v>1.10803324099723</v>
+        <v>1.22675108824694</v>
+      </c>
+      <c r="EF53" t="n">
+        <v>1.49960536700871</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -43509,11 +43809,14 @@
       </c>
       <c r="EE54" t="n">
         <v>1.27388535031848</v>
+      </c>
+      <c r="EF54" t="n">
+        <v>1.26182965299685</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -43915,12 +44218,15 @@
         <v>1.95071868583161</v>
       </c>
       <c r="EE55" t="n">
-        <v>1.93032015065913</v>
+        <v>1.9774011299435</v>
+      </c>
+      <c r="EF55" t="n">
+        <v>1.73872180451127</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -44323,6 +44629,9 @@
       </c>
       <c r="EE56" t="n">
         <v>2.97029702970298</v>
+      </c>
+      <c r="EF56" t="n">
+        <v>2.5974025974026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on May 17, 2024
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -457,6 +457,9 @@
   </si>
   <si>
     <t xml:space="preserve">03/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1389,10 +1392,13 @@
       <c r="ER4" t="s">
         <v>147</v>
       </c>
+      <c r="ES4" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1830,15 +1836,18 @@
         <v>10720.4</v>
       </c>
       <c r="EQ5" t="n">
-        <v>11103.8</v>
+        <v>11113.4</v>
       </c>
       <c r="ER5" t="n">
-        <v>11161.2</v>
+        <v>11168.8</v>
+      </c>
+      <c r="ES5" t="n">
+        <v>11161.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2279,12 +2288,15 @@
         <v>174.3</v>
       </c>
       <c r="ER6" t="n">
-        <v>175.6</v>
+        <v>175.5</v>
+      </c>
+      <c r="ES6" t="n">
+        <v>175.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2725,12 +2737,15 @@
         <v>28.9</v>
       </c>
       <c r="ER7" t="n">
+        <v>29</v>
+      </c>
+      <c r="ES7" t="n">
         <v>28.9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3171,12 +3186,15 @@
         <v>203.1</v>
       </c>
       <c r="ER8" t="n">
-        <v>202.5</v>
+        <v>202.1</v>
+      </c>
+      <c r="ES8" t="n">
+        <v>203.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3618,11 +3636,14 @@
       </c>
       <c r="ER9" t="n">
         <v>103.5</v>
+      </c>
+      <c r="ES9" t="n">
+        <v>104.1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4063,12 +4084,15 @@
         <v>1266.2</v>
       </c>
       <c r="ER10" t="n">
-        <v>1284.1</v>
+        <v>1283.8</v>
+      </c>
+      <c r="ES10" t="n">
+        <v>1290</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4509,12 +4533,15 @@
         <v>236.7</v>
       </c>
       <c r="ER11" t="n">
-        <v>239.8</v>
+        <v>239.7</v>
+      </c>
+      <c r="ES11" t="n">
+        <v>239.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4955,12 +4982,15 @@
         <v>125.1</v>
       </c>
       <c r="ER12" t="n">
-        <v>125.6</v>
+        <v>125.5</v>
+      </c>
+      <c r="ES12" t="n">
+        <v>125.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5401,12 +5431,15 @@
         <v>40.3</v>
       </c>
       <c r="ER13" t="n">
-        <v>41.1</v>
+        <v>40.6</v>
+      </c>
+      <c r="ES13" t="n">
+        <v>40.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5555,10 +5588,11 @@
       <c r="EP14"/>
       <c r="EQ14"/>
       <c r="ER14"/>
+      <c r="ES14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6000,11 +6034,14 @@
       </c>
       <c r="ER15" t="n">
         <v>499.5</v>
+      </c>
+      <c r="ES15" t="n">
+        <v>500.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6445,12 +6482,15 @@
         <v>354.8</v>
       </c>
       <c r="ER16" t="n">
-        <v>355.4</v>
+        <v>355.5</v>
+      </c>
+      <c r="ES16" t="n">
+        <v>354.8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6599,10 +6639,11 @@
       <c r="EP17"/>
       <c r="EQ17"/>
       <c r="ER17"/>
+      <c r="ES17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7043,12 +7084,15 @@
         <v>66.6</v>
       </c>
       <c r="ER18" t="n">
+        <v>67</v>
+      </c>
+      <c r="ES18" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7489,12 +7533,15 @@
         <v>458.3</v>
       </c>
       <c r="ER19" t="n">
-        <v>461.1</v>
+        <v>461.2</v>
+      </c>
+      <c r="ES19" t="n">
+        <v>458.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7935,12 +7982,15 @@
         <v>235.1</v>
       </c>
       <c r="ER20" t="n">
-        <v>236</v>
+        <v>235.7</v>
+      </c>
+      <c r="ES20" t="n">
+        <v>234.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8382,11 +8432,14 @@
       </c>
       <c r="ER21" t="n">
         <v>148.6</v>
+      </c>
+      <c r="ES21" t="n">
+        <v>148.5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8828,11 +8881,14 @@
       </c>
       <c r="ER22" t="n">
         <v>137.9</v>
+      </c>
+      <c r="ES22" t="n">
+        <v>137.7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9273,12 +9329,15 @@
         <v>164.6</v>
       </c>
       <c r="ER23" t="n">
-        <v>165.6</v>
+        <v>166</v>
+      </c>
+      <c r="ES23" t="n">
+        <v>165.9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9719,12 +9778,15 @@
         <v>147</v>
       </c>
       <c r="ER24" t="n">
-        <v>147.3</v>
+        <v>147.4</v>
+      </c>
+      <c r="ES24" t="n">
+        <v>147.1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10165,12 +10227,15 @@
         <v>50.4</v>
       </c>
       <c r="ER25" t="n">
-        <v>50.3</v>
+        <v>50.2</v>
+      </c>
+      <c r="ES25" t="n">
+        <v>49.8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10612,11 +10677,14 @@
       </c>
       <c r="ER26" t="n">
         <v>224.6</v>
+      </c>
+      <c r="ES26" t="n">
+        <v>228.2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11058,11 +11126,14 @@
       </c>
       <c r="ER27" t="n">
         <v>247.1</v>
+      </c>
+      <c r="ES27" t="n">
+        <v>246.2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11503,12 +11574,15 @@
         <v>328.7</v>
       </c>
       <c r="ER28" t="n">
-        <v>329.5</v>
+        <v>328.9</v>
+      </c>
+      <c r="ES28" t="n">
+        <v>329.1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -11950,11 +12024,14 @@
       </c>
       <c r="ER29" t="n">
         <v>219.1</v>
+      </c>
+      <c r="ES29" t="n">
+        <v>217.8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12396,11 +12473,14 @@
       </c>
       <c r="ER30" t="n">
         <v>105.1</v>
+      </c>
+      <c r="ES30" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -12549,10 +12629,11 @@
       <c r="EP31"/>
       <c r="EQ31"/>
       <c r="ER31"/>
+      <c r="ES31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -12994,11 +13075,14 @@
       </c>
       <c r="ER32" t="n">
         <v>44.8</v>
+      </c>
+      <c r="ES32" t="n">
+        <v>45.4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13439,12 +13523,15 @@
         <v>94</v>
       </c>
       <c r="ER33" t="n">
-        <v>94.8</v>
+        <v>95</v>
+      </c>
+      <c r="ES33" t="n">
+        <v>94.7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -13885,12 +13972,15 @@
         <v>85.2</v>
       </c>
       <c r="ER34" t="n">
-        <v>85.4</v>
+        <v>85.5</v>
+      </c>
+      <c r="ES34" t="n">
+        <v>85.2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -14331,12 +14421,15 @@
         <v>46.3</v>
       </c>
       <c r="ER35" t="n">
-        <v>46.5</v>
+        <v>46.4</v>
+      </c>
+      <c r="ES35" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14777,12 +14870,15 @@
         <v>321.1</v>
       </c>
       <c r="ER36" t="n">
-        <v>322.8</v>
+        <v>322.7</v>
+      </c>
+      <c r="ES36" t="n">
+        <v>323.4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -15224,11 +15320,14 @@
       </c>
       <c r="ER37" t="n">
         <v>81</v>
+      </c>
+      <c r="ES37" t="n">
+        <v>80.6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -15670,11 +15769,14 @@
       </c>
       <c r="ER38" t="n">
         <v>683.7</v>
+      </c>
+      <c r="ES38" t="n">
+        <v>682.3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16116,11 +16218,14 @@
       </c>
       <c r="ER39" t="n">
         <v>343.3</v>
+      </c>
+      <c r="ES39" t="n">
+        <v>343.7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -16561,12 +16666,15 @@
         <v>39.5</v>
       </c>
       <c r="ER40" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="ES40" t="n">
         <v>39.2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -17007,12 +17115,15 @@
         <v>392</v>
       </c>
       <c r="ER41" t="n">
-        <v>395.7</v>
+        <v>395.8</v>
+      </c>
+      <c r="ES41" t="n">
+        <v>391.5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -17453,12 +17564,15 @@
         <v>152.5</v>
       </c>
       <c r="ER42" t="n">
-        <v>153.3</v>
+        <v>154</v>
+      </c>
+      <c r="ES42" t="n">
+        <v>153.9</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -17899,12 +18013,15 @@
         <v>142.1</v>
       </c>
       <c r="ER43" t="n">
+        <v>143.6</v>
+      </c>
+      <c r="ES43" t="n">
         <v>143.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -18346,11 +18463,14 @@
       </c>
       <c r="ER44" t="n">
         <v>336.1</v>
+      </c>
+      <c r="ES44" t="n">
+        <v>336.5</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -18791,12 +18911,15 @@
         <v>29.6</v>
       </c>
       <c r="ER45" t="n">
+        <v>29.9</v>
+      </c>
+      <c r="ES45" t="n">
         <v>29.9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -19238,11 +19361,14 @@
       </c>
       <c r="ER46" t="n">
         <v>164.6</v>
+      </c>
+      <c r="ES46" t="n">
+        <v>165.5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -19683,12 +19809,15 @@
         <v>38.8</v>
       </c>
       <c r="ER47" t="n">
-        <v>39.1</v>
+        <v>39</v>
+      </c>
+      <c r="ES47" t="n">
+        <v>38.8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -20129,12 +20258,15 @@
         <v>207.8</v>
       </c>
       <c r="ER48" t="n">
-        <v>208.9</v>
+        <v>209</v>
+      </c>
+      <c r="ES48" t="n">
+        <v>209.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -20575,12 +20707,15 @@
         <v>1205</v>
       </c>
       <c r="ER49" t="n">
-        <v>1206.6</v>
+        <v>1206.8</v>
+      </c>
+      <c r="ES49" t="n">
+        <v>1207.2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -21021,12 +21156,15 @@
         <v>135</v>
       </c>
       <c r="ER50" t="n">
+        <v>135.3</v>
+      </c>
+      <c r="ES50" t="n">
         <v>135.3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -21467,12 +21605,15 @@
         <v>33.2</v>
       </c>
       <c r="ER51" t="n">
-        <v>32.9</v>
+        <v>33.2</v>
+      </c>
+      <c r="ES51" t="n">
+        <v>33.1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -21913,12 +22054,15 @@
         <v>332</v>
       </c>
       <c r="ER52" t="n">
-        <v>334.1</v>
+        <v>333.9</v>
+      </c>
+      <c r="ES52" t="n">
+        <v>331.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -22359,12 +22503,15 @@
         <v>255.8</v>
       </c>
       <c r="ER53" t="n">
-        <v>257.2</v>
+        <v>259</v>
+      </c>
+      <c r="ES53" t="n">
+        <v>259</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -22806,11 +22953,14 @@
       </c>
       <c r="ER54" t="n">
         <v>64.2</v>
+      </c>
+      <c r="ES54" t="n">
+        <v>63.7</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -23252,11 +23402,14 @@
       </c>
       <c r="ER55" t="n">
         <v>216.5</v>
+      </c>
+      <c r="ES55" t="n">
+        <v>215.4</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -23697,6 +23850,9 @@
         <v>31.2</v>
       </c>
       <c r="ER56" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="ES56" t="n">
         <v>31.6</v>
       </c>
     </row>
@@ -24123,10 +24279,13 @@
       <c r="EF4" t="s">
         <v>147</v>
       </c>
+      <c r="EG4" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -24528,15 +24687,18 @@
         <v>2.4581390014527</v>
       </c>
       <c r="EE5" t="n">
-        <v>2.32973919454429</v>
+        <v>2.41821030319786</v>
       </c>
       <c r="EF5" t="n">
-        <v>2.52048352132858</v>
+        <v>2.59029283168606</v>
+      </c>
+      <c r="EG5" t="n">
+        <v>2.43477143617558</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -24941,12 +25103,15 @@
         <v>0.984936268829674</v>
       </c>
       <c r="EF6" t="n">
-        <v>1.09383995394358</v>
+        <v>1.03626943005182</v>
+      </c>
+      <c r="EG6" t="n">
+        <v>1.09447004608294</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -25351,12 +25516,15 @@
         <v>0</v>
       </c>
       <c r="EF7" t="n">
-        <v>0.347222222222215</v>
+        <v>0.694444444444442</v>
+      </c>
+      <c r="EG7" t="n">
+        <v>-0.0000000000000122931269162647</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -25761,12 +25929,15 @@
         <v>0.694100148735763</v>
       </c>
       <c r="EF8" t="n">
-        <v>1.19940029985006</v>
+        <v>0.999500249875062</v>
+      </c>
+      <c r="EG8" t="n">
+        <v>0.0491400491400603</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -26172,11 +26343,14 @@
       </c>
       <c r="EF9" t="n">
         <v>1.07421874999999</v>
+      </c>
+      <c r="EG9" t="n">
+        <v>1.06796116504854</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -26581,12 +26755,15 @@
         <v>3.23685283326539</v>
       </c>
       <c r="EF10" t="n">
-        <v>3.11571508873363</v>
+        <v>3.09162450815066</v>
+      </c>
+      <c r="EG10" t="n">
+        <v>3.05160568780956</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -26991,12 +27168,15 @@
         <v>5.95344673231872</v>
       </c>
       <c r="EF11" t="n">
-        <v>6.15316511730855</v>
+        <v>6.10889774236388</v>
+      </c>
+      <c r="EG11" t="n">
+        <v>4.99561787905346</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -27401,12 +27581,15 @@
         <v>-0.318725099601598</v>
       </c>
       <c r="EF12" t="n">
-        <v>-0.475435816164824</v>
+        <v>-0.554675118858956</v>
+      </c>
+      <c r="EG12" t="n">
+        <v>1.20967741935484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -27811,12 +27994,15 @@
         <v>4.13436692506458</v>
       </c>
       <c r="EF13" t="n">
-        <v>4.31472081218271</v>
+        <v>3.04568527918779</v>
+      </c>
+      <c r="EG13" t="n">
+        <v>3.8265306122449</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -27953,10 +28139,11 @@
       <c r="ED14"/>
       <c r="EE14"/>
       <c r="EF14"/>
+      <c r="EG14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -28362,11 +28549,14 @@
       </c>
       <c r="EF15" t="n">
         <v>1.40073081607796</v>
+      </c>
+      <c r="EG15" t="n">
+        <v>1.45896656534954</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -28771,12 +28961,15 @@
         <v>2.45451920300318</v>
       </c>
       <c r="EF16" t="n">
-        <v>2.33227756982435</v>
+        <v>2.3610711200691</v>
+      </c>
+      <c r="EG16" t="n">
+        <v>3.0796048808832</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -28913,10 +29106,11 @@
       <c r="ED17"/>
       <c r="EE17"/>
       <c r="EF17"/>
+      <c r="EG17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -29322,11 +29516,14 @@
       </c>
       <c r="EF18" t="n">
         <v>5.34591194968553</v>
+      </c>
+      <c r="EG18" t="n">
+        <v>6.0126582278481</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -29731,12 +29928,15 @@
         <v>3.68778280542985</v>
       </c>
       <c r="EF19" t="n">
-        <v>3.59469782071443</v>
+        <v>3.6171646820939</v>
+      </c>
+      <c r="EG19" t="n">
+        <v>3.64253393665159</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -30141,12 +30341,15 @@
         <v>2.52943741822939</v>
       </c>
       <c r="EF20" t="n">
-        <v>1.1139674378749</v>
+        <v>0.985432733504718</v>
+      </c>
+      <c r="EG20" t="n">
+        <v>1.38588133391079</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -30552,11 +30755,14 @@
       </c>
       <c r="EF21" t="n">
         <v>1.43344709897611</v>
+      </c>
+      <c r="EG21" t="n">
+        <v>1.43442622950819</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -30962,11 +31168,14 @@
       </c>
       <c r="EF22" t="n">
         <v>0.877834674469654</v>
+      </c>
+      <c r="EG22" t="n">
+        <v>0.510948905109481</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -31371,12 +31580,15 @@
         <v>1.04358502148557</v>
       </c>
       <c r="EF23" t="n">
-        <v>0.79123554473523</v>
+        <v>1.034692635423</v>
+      </c>
+      <c r="EG23" t="n">
+        <v>2.02952029520296</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -31781,12 +31993,15 @@
         <v>-1.34228187919463</v>
       </c>
       <c r="EF24" t="n">
-        <v>-0.40567951318458</v>
+        <v>-0.338066260987153</v>
+      </c>
+      <c r="EG24" t="n">
+        <v>-1.07599193006052</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -32191,12 +32406,15 @@
         <v>3.27868852459018</v>
       </c>
       <c r="EF25" t="n">
-        <v>2.65306122448979</v>
+        <v>2.44897959183674</v>
+      </c>
+      <c r="EG25" t="n">
+        <v>2.46913580246914</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -32602,11 +32820,14 @@
       </c>
       <c r="EF26" t="n">
         <v>2.41678066575467</v>
+      </c>
+      <c r="EG26" t="n">
+        <v>3.21121664405245</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -33012,11 +33233,14 @@
       </c>
       <c r="EF27" t="n">
         <v>1.3120131201312</v>
+      </c>
+      <c r="EG27" t="n">
+        <v>1.35858377933305</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -33421,12 +33645,15 @@
         <v>5.2513608709574</v>
       </c>
       <c r="EF28" t="n">
-        <v>5.7784911717496</v>
+        <v>5.58587479935794</v>
+      </c>
+      <c r="EG28" t="n">
+        <v>5.51458800897725</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -33832,11 +34059,14 @@
       </c>
       <c r="EF29" t="n">
         <v>5.3872053872054</v>
+      </c>
+      <c r="EG29" t="n">
+        <v>4.81231953801732</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -34242,11 +34472,14 @@
       </c>
       <c r="EF30" t="n">
         <v>1.0576923076923</v>
+      </c>
+      <c r="EG30" t="n">
+        <v>1.25361620057859</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -34383,10 +34616,11 @@
       <c r="ED31"/>
       <c r="EE31"/>
       <c r="EF31"/>
+      <c r="EG31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -34792,11 +35026,14 @@
       </c>
       <c r="EF32" t="n">
         <v>1.81818181818181</v>
+      </c>
+      <c r="EG32" t="n">
+        <v>1.79372197309416</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -35201,12 +35438,15 @@
         <v>-0.212314225053082</v>
       </c>
       <c r="EF33" t="n">
-        <v>0.105596620908125</v>
+        <v>0.31678986272439</v>
+      </c>
+      <c r="EG33" t="n">
+        <v>-0.0000000000000150061823814171</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -35611,12 +35851,15 @@
         <v>4.41176470588235</v>
       </c>
       <c r="EF34" t="n">
-        <v>4.40097799511002</v>
+        <v>4.52322738386307</v>
+      </c>
+      <c r="EG34" t="n">
+        <v>4.02930402930403</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -36021,12 +36264,15 @@
         <v>1.09170305676856</v>
       </c>
       <c r="EF35" t="n">
-        <v>1.52838427947597</v>
+        <v>1.31004366812226</v>
+      </c>
+      <c r="EG35" t="n">
+        <v>0.877192982456137</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -36431,12 +36677,15 @@
         <v>2.03368287257707</v>
       </c>
       <c r="EF36" t="n">
-        <v>2.24897054165346</v>
+        <v>2.21729490022173</v>
+      </c>
+      <c r="EG36" t="n">
+        <v>2.53646163601774</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -36842,11 +37091,14 @@
       </c>
       <c r="EF37" t="n">
         <v>3.97946084724004</v>
+      </c>
+      <c r="EG37" t="n">
+        <v>3.59897172236504</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -37252,11 +37504,14 @@
       </c>
       <c r="EF38" t="n">
         <v>2.50374812593704</v>
+      </c>
+      <c r="EG38" t="n">
+        <v>2.49361574282712</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -37662,11 +37917,14 @@
       </c>
       <c r="EF39" t="n">
         <v>2.08147487362472</v>
+      </c>
+      <c r="EG39" t="n">
+        <v>2.1093285799168</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -38072,11 +38330,14 @@
       </c>
       <c r="EF40" t="n">
         <v>0.771208226221091</v>
+      </c>
+      <c r="EG40" t="n">
+        <v>2.34986945169714</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -38481,12 +38742,15 @@
         <v>-1.77900275620146</v>
       </c>
       <c r="EF41" t="n">
-        <v>-0.100984599848532</v>
+        <v>-0.0757384498864095</v>
+      </c>
+      <c r="EG41" t="n">
+        <v>-1.85510152920531</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -38891,12 +39155,15 @@
         <v>3.04054054054054</v>
       </c>
       <c r="EF42" t="n">
-        <v>2.8169014084507</v>
+        <v>3.28638497652581</v>
+      </c>
+      <c r="EG42" t="n">
+        <v>3.35795836131632</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -39301,12 +39568,15 @@
         <v>2.45133381398703</v>
       </c>
       <c r="EF43" t="n">
-        <v>2.79369627507162</v>
+        <v>2.86532951289398</v>
+      </c>
+      <c r="EG43" t="n">
+        <v>2.64663805436337</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -39712,11 +39982,14 @@
       </c>
       <c r="EF44" t="n">
         <v>1.60217654171704</v>
+      </c>
+      <c r="EG44" t="n">
+        <v>1.90793458509993</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -40122,11 +40395,14 @@
       </c>
       <c r="EF45" t="n">
         <v>-0.993377483443711</v>
+      </c>
+      <c r="EG45" t="n">
+        <v>1.35593220338984</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -40532,11 +40808,14 @@
       </c>
       <c r="EF46" t="n">
         <v>0.365853658536582</v>
+      </c>
+      <c r="EG46" t="n">
+        <v>0.485731633272624</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -40941,12 +41220,15 @@
         <v>1.83727034120736</v>
       </c>
       <c r="EF47" t="n">
-        <v>2.08877284595301</v>
+        <v>1.82767624020888</v>
+      </c>
+      <c r="EG47" t="n">
+        <v>1.57068062827224</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -41351,12 +41633,15 @@
         <v>-1.37636449928808</v>
       </c>
       <c r="EF48" t="n">
-        <v>-1.0421601136902</v>
+        <v>-0.99478919943156</v>
+      </c>
+      <c r="EG48" t="n">
+        <v>-1.36470588235294</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -41761,12 +42046,15 @@
         <v>2.8947143711041</v>
       </c>
       <c r="EF49" t="n">
-        <v>2.83814881104576</v>
+        <v>2.85519474985085</v>
+      </c>
+      <c r="EG49" t="n">
+        <v>2.99462503199385</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -42171,12 +42459,15 @@
         <v>4.8951048951049</v>
       </c>
       <c r="EF50" t="n">
+        <v>4.88372093023257</v>
+      </c>
+      <c r="EG50" t="n">
         <v>4.88372093023257</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -42581,12 +42872,15 @@
         <v>2.78637770897835</v>
       </c>
       <c r="EF51" t="n">
-        <v>2.49221183800627</v>
+        <v>3.42679127725859</v>
+      </c>
+      <c r="EG51" t="n">
+        <v>2.1604938271605</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -42991,12 +43285,15 @@
         <v>2.85006195786865</v>
       </c>
       <c r="EF52" t="n">
-        <v>3.08546744831842</v>
+        <v>3.02375809935204</v>
+      </c>
+      <c r="EG52" t="n">
+        <v>2.19068188830607</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -43401,12 +43698,15 @@
         <v>1.22675108824694</v>
       </c>
       <c r="EF53" t="n">
-        <v>1.49960536700871</v>
+        <v>2.20994475138122</v>
+      </c>
+      <c r="EG53" t="n">
+        <v>0.154679040989937</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -43812,11 +44112,14 @@
       </c>
       <c r="EF54" t="n">
         <v>1.26182965299685</v>
+      </c>
+      <c r="EG54" t="n">
+        <v>1.11111111111112</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -44222,11 +44525,14 @@
       </c>
       <c r="EF55" t="n">
         <v>1.73872180451127</v>
+      </c>
+      <c r="EG55" t="n">
+        <v>1.12676056338028</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -44632,6 +44938,9 @@
       </c>
       <c r="EF56" t="n">
         <v>2.5974025974026</v>
+      </c>
+      <c r="EG56" t="n">
+        <v>3.26797385620916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on June25, 2024
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -460,6 +460,9 @@
   </si>
   <si>
     <t xml:space="preserve">04/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1395,10 +1398,13 @@
       <c r="ES4" t="s">
         <v>148</v>
       </c>
+      <c r="ET4" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1839,15 +1845,18 @@
         <v>11113.4</v>
       </c>
       <c r="ER5" t="n">
-        <v>11168.8</v>
+        <v>11169.1</v>
       </c>
       <c r="ES5" t="n">
-        <v>11161.6</v>
+        <v>11158</v>
+      </c>
+      <c r="ET5" t="n">
+        <v>11036</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2291,12 +2300,15 @@
         <v>175.5</v>
       </c>
       <c r="ES6" t="n">
-        <v>175.5</v>
+        <v>175.6</v>
+      </c>
+      <c r="ET6" t="n">
+        <v>175.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2740,12 +2752,15 @@
         <v>29</v>
       </c>
       <c r="ES7" t="n">
-        <v>28.9</v>
+        <v>28.8</v>
+      </c>
+      <c r="ET7" t="n">
+        <v>27.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3190,11 +3205,14 @@
       </c>
       <c r="ES8" t="n">
         <v>203.6</v>
+      </c>
+      <c r="ET8" t="n">
+        <v>195.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3639,11 +3657,14 @@
       </c>
       <c r="ES9" t="n">
         <v>104.1</v>
+      </c>
+      <c r="ET9" t="n">
+        <v>103.1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4087,12 +4108,15 @@
         <v>1283.8</v>
       </c>
       <c r="ES10" t="n">
-        <v>1290</v>
+        <v>1292.2</v>
+      </c>
+      <c r="ET10" t="n">
+        <v>1303.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4536,12 +4560,15 @@
         <v>239.7</v>
       </c>
       <c r="ES11" t="n">
-        <v>239.6</v>
+        <v>239.7</v>
+      </c>
+      <c r="ET11" t="n">
+        <v>240.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -4985,12 +5012,15 @@
         <v>125.5</v>
       </c>
       <c r="ES12" t="n">
-        <v>125.5</v>
+        <v>125.4</v>
+      </c>
+      <c r="ET12" t="n">
+        <v>126.1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5434,12 +5464,15 @@
         <v>40.6</v>
       </c>
       <c r="ES13" t="n">
-        <v>40.7</v>
+        <v>40.4</v>
+      </c>
+      <c r="ET13" t="n">
+        <v>39.6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5589,10 +5622,11 @@
       <c r="EQ14"/>
       <c r="ER14"/>
       <c r="ES14"/>
+      <c r="ET14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6036,12 +6070,15 @@
         <v>499.5</v>
       </c>
       <c r="ES15" t="n">
-        <v>500.7</v>
+        <v>501</v>
+      </c>
+      <c r="ET15" t="n">
+        <v>489</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6485,12 +6522,15 @@
         <v>355.5</v>
       </c>
       <c r="ES16" t="n">
-        <v>354.8</v>
+        <v>354.9</v>
+      </c>
+      <c r="ET16" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6640,10 +6680,11 @@
       <c r="EQ17"/>
       <c r="ER17"/>
       <c r="ES17"/>
+      <c r="ET17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7087,12 +7128,15 @@
         <v>67</v>
       </c>
       <c r="ES18" t="n">
-        <v>67</v>
+        <v>66.8</v>
+      </c>
+      <c r="ET18" t="n">
+        <v>65.8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7536,12 +7580,15 @@
         <v>461.2</v>
       </c>
       <c r="ES19" t="n">
-        <v>458.1</v>
+        <v>458.6</v>
+      </c>
+      <c r="ET19" t="n">
+        <v>459</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -7985,12 +8032,15 @@
         <v>235.7</v>
       </c>
       <c r="ES20" t="n">
-        <v>234.1</v>
+        <v>234.3</v>
+      </c>
+      <c r="ET20" t="n">
+        <v>232.3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8435,11 +8485,14 @@
       </c>
       <c r="ES21" t="n">
         <v>148.5</v>
+      </c>
+      <c r="ET21" t="n">
+        <v>148</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8884,11 +8937,14 @@
       </c>
       <c r="ES22" t="n">
         <v>137.7</v>
+      </c>
+      <c r="ET22" t="n">
+        <v>137</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9332,12 +9388,15 @@
         <v>166</v>
       </c>
       <c r="ES23" t="n">
-        <v>165.9</v>
+        <v>165.1</v>
+      </c>
+      <c r="ET23" t="n">
+        <v>164.7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9781,12 +9840,15 @@
         <v>147.4</v>
       </c>
       <c r="ES24" t="n">
-        <v>147.1</v>
+        <v>148.4</v>
+      </c>
+      <c r="ET24" t="n">
+        <v>147.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10230,12 +10292,15 @@
         <v>50.2</v>
       </c>
       <c r="ES25" t="n">
-        <v>49.8</v>
+        <v>49.7</v>
+      </c>
+      <c r="ET25" t="n">
+        <v>49.7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10679,12 +10744,15 @@
         <v>224.6</v>
       </c>
       <c r="ES26" t="n">
-        <v>228.2</v>
+        <v>228.3</v>
+      </c>
+      <c r="ET26" t="n">
+        <v>229</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11129,11 +11197,14 @@
       </c>
       <c r="ES27" t="n">
         <v>246.2</v>
+      </c>
+      <c r="ET27" t="n">
+        <v>244.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11577,12 +11648,15 @@
         <v>328.9</v>
       </c>
       <c r="ES28" t="n">
-        <v>329.1</v>
+        <v>328.9</v>
+      </c>
+      <c r="ET28" t="n">
+        <v>310.9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12026,12 +12100,15 @@
         <v>219.1</v>
       </c>
       <c r="ES29" t="n">
-        <v>217.8</v>
+        <v>218</v>
+      </c>
+      <c r="ET29" t="n">
+        <v>215.9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12476,11 +12553,14 @@
       </c>
       <c r="ES30" t="n">
         <v>105</v>
+      </c>
+      <c r="ET30" t="n">
+        <v>103.4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -12630,10 +12710,11 @@
       <c r="EQ31"/>
       <c r="ER31"/>
       <c r="ES31"/>
+      <c r="ET31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -13078,11 +13159,14 @@
       </c>
       <c r="ES32" t="n">
         <v>45.4</v>
+      </c>
+      <c r="ET32" t="n">
+        <v>46.3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13527,11 +13611,14 @@
       </c>
       <c r="ES33" t="n">
         <v>94.7</v>
+      </c>
+      <c r="ET33" t="n">
+        <v>95.5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -13976,11 +14063,14 @@
       </c>
       <c r="ES34" t="n">
         <v>85.2</v>
+      </c>
+      <c r="ET34" t="n">
+        <v>85.8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -14425,11 +14515,14 @@
       </c>
       <c r="ES35" t="n">
         <v>46</v>
+      </c>
+      <c r="ET35" t="n">
+        <v>45.4</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14873,12 +14966,15 @@
         <v>322.7</v>
       </c>
       <c r="ES36" t="n">
-        <v>323.4</v>
+        <v>323.7</v>
+      </c>
+      <c r="ET36" t="n">
+        <v>320</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -15322,12 +15418,15 @@
         <v>81</v>
       </c>
       <c r="ES37" t="n">
-        <v>80.6</v>
+        <v>80.4</v>
+      </c>
+      <c r="ET37" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -15772,11 +15871,14 @@
       </c>
       <c r="ES38" t="n">
         <v>682.3</v>
+      </c>
+      <c r="ET38" t="n">
+        <v>682.9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16221,11 +16323,14 @@
       </c>
       <c r="ES39" t="n">
         <v>343.7</v>
+      </c>
+      <c r="ET39" t="n">
+        <v>343.5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -16669,12 +16774,15 @@
         <v>39.2</v>
       </c>
       <c r="ES40" t="n">
-        <v>39.2</v>
+        <v>39.3</v>
+      </c>
+      <c r="ET40" t="n">
+        <v>38.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -17118,12 +17226,15 @@
         <v>395.8</v>
       </c>
       <c r="ES41" t="n">
-        <v>391.5</v>
+        <v>391.8</v>
+      </c>
+      <c r="ET41" t="n">
+        <v>381.7</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -17567,12 +17678,15 @@
         <v>154</v>
       </c>
       <c r="ES42" t="n">
-        <v>153.9</v>
+        <v>153.8</v>
+      </c>
+      <c r="ET42" t="n">
+        <v>153.2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -18016,12 +18130,15 @@
         <v>143.6</v>
       </c>
       <c r="ES43" t="n">
-        <v>143.5</v>
+        <v>143.3</v>
+      </c>
+      <c r="ET43" t="n">
+        <v>144</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -18466,11 +18583,14 @@
       </c>
       <c r="ES44" t="n">
         <v>336.5</v>
+      </c>
+      <c r="ET44" t="n">
+        <v>333.4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -18915,11 +19035,14 @@
       </c>
       <c r="ES45" t="n">
         <v>29.9</v>
+      </c>
+      <c r="ET45" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -19363,12 +19486,15 @@
         <v>164.6</v>
       </c>
       <c r="ES46" t="n">
-        <v>165.5</v>
+        <v>165.3</v>
+      </c>
+      <c r="ET46" t="n">
+        <v>161.4</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -19813,11 +19939,14 @@
       </c>
       <c r="ES47" t="n">
         <v>38.8</v>
+      </c>
+      <c r="ET47" t="n">
+        <v>38.4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -20261,12 +20390,15 @@
         <v>209</v>
       </c>
       <c r="ES48" t="n">
-        <v>209.6</v>
+        <v>209.1</v>
+      </c>
+      <c r="ET48" t="n">
+        <v>202.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -20711,11 +20843,14 @@
       </c>
       <c r="ES49" t="n">
         <v>1207.2</v>
+      </c>
+      <c r="ET49" t="n">
+        <v>1205.2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -21160,11 +21295,14 @@
       </c>
       <c r="ES50" t="n">
         <v>135.3</v>
+      </c>
+      <c r="ET50" t="n">
+        <v>135.2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -21609,11 +21747,14 @@
       </c>
       <c r="ES51" t="n">
         <v>33.1</v>
+      </c>
+      <c r="ET51" t="n">
+        <v>30.2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -22057,12 +22198,15 @@
         <v>333.9</v>
       </c>
       <c r="ES52" t="n">
-        <v>331.2</v>
+        <v>333.3</v>
+      </c>
+      <c r="ET52" t="n">
+        <v>325.9</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -22506,12 +22650,15 @@
         <v>259</v>
       </c>
       <c r="ES53" t="n">
-        <v>259</v>
+        <v>259.2</v>
+      </c>
+      <c r="ET53" t="n">
+        <v>258.5</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -22956,11 +23103,14 @@
       </c>
       <c r="ES54" t="n">
         <v>63.7</v>
+      </c>
+      <c r="ET54" t="n">
+        <v>61.2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -23405,11 +23555,14 @@
       </c>
       <c r="ES55" t="n">
         <v>215.4</v>
+      </c>
+      <c r="ET55" t="n">
+        <v>206.7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -23854,6 +24007,9 @@
       </c>
       <c r="ES56" t="n">
         <v>31.6</v>
+      </c>
+      <c r="ET56" t="n">
+        <v>31.7</v>
       </c>
     </row>
   </sheetData>
@@ -24282,10 +24438,13 @@
       <c r="EG4" t="s">
         <v>148</v>
       </c>
+      <c r="EH4" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -24690,15 +24849,18 @@
         <v>2.41821030319786</v>
       </c>
       <c r="EF5" t="n">
-        <v>2.59029283168606</v>
+        <v>2.59304846235806</v>
       </c>
       <c r="EG5" t="n">
-        <v>2.43477143617558</v>
+        <v>2.40173269825538</v>
+      </c>
+      <c r="EH5" t="n">
+        <v>2.29031689977663</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -25106,12 +25268,15 @@
         <v>1.03626943005182</v>
       </c>
       <c r="EG6" t="n">
-        <v>1.09447004608294</v>
+        <v>1.15207373271888</v>
+      </c>
+      <c r="EH6" t="n">
+        <v>1.0938399539436</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -25519,12 +25684,15 @@
         <v>0.694444444444442</v>
       </c>
       <c r="EG7" t="n">
-        <v>-0.0000000000000122931269162647</v>
+        <v>-0.34602076124568</v>
+      </c>
+      <c r="EH7" t="n">
+        <v>-1.06761565836298</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -25933,11 +26101,14 @@
       </c>
       <c r="EG8" t="n">
         <v>0.0491400491400603</v>
+      </c>
+      <c r="EH8" t="n">
+        <v>-1.21273370389084</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -26346,11 +26517,14 @@
       </c>
       <c r="EG9" t="n">
         <v>1.06796116504854</v>
+      </c>
+      <c r="EH9" t="n">
+        <v>1.07843137254901</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -26758,12 +26932,15 @@
         <v>3.09162450815066</v>
       </c>
       <c r="EG10" t="n">
-        <v>3.05160568780956</v>
+        <v>3.22735261223837</v>
+      </c>
+      <c r="EH10" t="n">
+        <v>3.01161963481147</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -27171,12 +27348,15 @@
         <v>6.10889774236388</v>
       </c>
       <c r="EG11" t="n">
-        <v>4.99561787905346</v>
+        <v>5.03943908851886</v>
+      </c>
+      <c r="EH11" t="n">
+        <v>5.66534914361002</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -27584,12 +27764,15 @@
         <v>-0.554675118858956</v>
       </c>
       <c r="EG12" t="n">
-        <v>1.20967741935484</v>
+        <v>1.12903225806452</v>
+      </c>
+      <c r="EH12" t="n">
+        <v>1.12269446672012</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -27997,12 +28180,15 @@
         <v>3.04568527918779</v>
       </c>
       <c r="EG13" t="n">
-        <v>3.8265306122449</v>
+        <v>3.06122448979593</v>
+      </c>
+      <c r="EH13" t="n">
+        <v>2.85714285714284</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -28140,10 +28326,11 @@
       <c r="EE14"/>
       <c r="EF14"/>
       <c r="EG14"/>
+      <c r="EH14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -28551,12 +28738,15 @@
         <v>1.40073081607796</v>
       </c>
       <c r="EG15" t="n">
-        <v>1.45896656534954</v>
+        <v>1.51975683890578</v>
+      </c>
+      <c r="EH15" t="n">
+        <v>1.38917686087498</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -28964,12 +29154,15 @@
         <v>2.3610711200691</v>
       </c>
       <c r="EG16" t="n">
-        <v>3.0796048808832</v>
+        <v>3.10865775711795</v>
+      </c>
+      <c r="EH16" t="n">
+        <v>1.77377144518756</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -29107,10 +29300,11 @@
       <c r="EE17"/>
       <c r="EF17"/>
       <c r="EG17"/>
+      <c r="EH17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -29518,12 +29712,15 @@
         <v>5.34591194968553</v>
       </c>
       <c r="EG18" t="n">
-        <v>6.0126582278481</v>
+        <v>5.69620253164556</v>
+      </c>
+      <c r="EH18" t="n">
+        <v>6.30048465266561</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -29931,12 +30128,15 @@
         <v>3.6171646820939</v>
       </c>
       <c r="EG19" t="n">
-        <v>3.64253393665159</v>
+        <v>3.75565610859729</v>
+      </c>
+      <c r="EH19" t="n">
+        <v>3.47159603246167</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -30344,12 +30544,15 @@
         <v>0.985432733504718</v>
       </c>
       <c r="EG20" t="n">
-        <v>1.38588133391079</v>
+        <v>1.47249891728022</v>
+      </c>
+      <c r="EH20" t="n">
+        <v>0.912250217202443</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -30758,11 +30961,14 @@
       </c>
       <c r="EG21" t="n">
         <v>1.43442622950819</v>
+      </c>
+      <c r="EH21" t="n">
+        <v>1.09289617486338</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -31171,11 +31377,14 @@
       </c>
       <c r="EG22" t="n">
         <v>0.510948905109481</v>
+      </c>
+      <c r="EH22" t="n">
+        <v>0.146198830409348</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -31583,12 +31792,15 @@
         <v>1.034692635423</v>
       </c>
       <c r="EG23" t="n">
-        <v>2.02952029520296</v>
+        <v>1.53751537515375</v>
+      </c>
+      <c r="EH23" t="n">
+        <v>1.16707616707615</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -31996,12 +32208,15 @@
         <v>-0.338066260987153</v>
       </c>
       <c r="EG24" t="n">
-        <v>-1.07599193006052</v>
+        <v>-0.201748486886356</v>
+      </c>
+      <c r="EH24" t="n">
+        <v>-0.203252032520314</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -32409,12 +32624,15 @@
         <v>2.44897959183674</v>
       </c>
       <c r="EG25" t="n">
-        <v>2.46913580246914</v>
+        <v>2.26337448559673</v>
+      </c>
+      <c r="EH25" t="n">
+        <v>1.63599182004091</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -32822,12 +33040,15 @@
         <v>2.41678066575467</v>
       </c>
       <c r="EG26" t="n">
-        <v>3.21121664405245</v>
+        <v>3.25644504748982</v>
+      </c>
+      <c r="EH26" t="n">
+        <v>2.78276481149012</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -33236,11 +33457,14 @@
       </c>
       <c r="EG27" t="n">
         <v>1.35858377933305</v>
+      </c>
+      <c r="EH27" t="n">
+        <v>1.32450331125827</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -33648,12 +33872,15 @@
         <v>5.58587479935794</v>
       </c>
       <c r="EG28" t="n">
-        <v>5.51458800897725</v>
+        <v>5.45046489259378</v>
+      </c>
+      <c r="EH28" t="n">
+        <v>2.40447957839261</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -34061,12 +34288,15 @@
         <v>5.3872053872054</v>
       </c>
       <c r="EG29" t="n">
-        <v>4.81231953801732</v>
+        <v>4.90856592877766</v>
+      </c>
+      <c r="EH29" t="n">
+        <v>5.26572403705509</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -34475,11 +34705,14 @@
       </c>
       <c r="EG30" t="n">
         <v>1.25361620057859</v>
+      </c>
+      <c r="EH30" t="n">
+        <v>0.779727095516553</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -34617,10 +34850,11 @@
       <c r="EE31"/>
       <c r="EF31"/>
       <c r="EG31"/>
+      <c r="EH31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -35029,11 +35263,14 @@
       </c>
       <c r="EG32" t="n">
         <v>1.79372197309416</v>
+      </c>
+      <c r="EH32" t="n">
+        <v>1.75824175824175</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -35442,11 +35679,14 @@
       </c>
       <c r="EG33" t="n">
         <v>-0.0000000000000150061823814171</v>
+      </c>
+      <c r="EH33" t="n">
+        <v>0.844772967265044</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -35855,11 +36095,14 @@
       </c>
       <c r="EG34" t="n">
         <v>4.02930402930403</v>
+      </c>
+      <c r="EH34" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -36268,11 +36511,14 @@
       </c>
       <c r="EG35" t="n">
         <v>0.877192982456137</v>
+      </c>
+      <c r="EH35" t="n">
+        <v>0.442477876106201</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -36680,12 +36926,15 @@
         <v>2.21729490022173</v>
       </c>
       <c r="EG36" t="n">
-        <v>2.53646163601774</v>
+        <v>2.63157894736841</v>
+      </c>
+      <c r="EH36" t="n">
+        <v>2.59698621352997</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -37093,12 +37342,15 @@
         <v>3.97946084724004</v>
       </c>
       <c r="EG37" t="n">
-        <v>3.59897172236504</v>
+        <v>3.34190231362469</v>
+      </c>
+      <c r="EH37" t="n">
+        <v>3.09278350515465</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -37507,11 +37759,14 @@
       </c>
       <c r="EG38" t="n">
         <v>2.49361574282712</v>
+      </c>
+      <c r="EH38" t="n">
+        <v>2.47599039615848</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -37920,11 +38175,14 @@
       </c>
       <c r="EG39" t="n">
         <v>2.1093285799168</v>
+      </c>
+      <c r="EH39" t="n">
+        <v>2.08023774145617</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -38332,12 +38590,15 @@
         <v>0.771208226221091</v>
       </c>
       <c r="EG40" t="n">
-        <v>2.34986945169714</v>
+        <v>2.61096605744125</v>
+      </c>
+      <c r="EH40" t="n">
+        <v>1.83727034120736</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -38745,12 +39006,15 @@
         <v>-0.0757384498864095</v>
       </c>
       <c r="EG41" t="n">
-        <v>-1.85510152920531</v>
+        <v>-1.77989471045375</v>
+      </c>
+      <c r="EH41" t="n">
+        <v>-2.99872935196951</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -39158,12 +39422,15 @@
         <v>3.28638497652581</v>
       </c>
       <c r="EG42" t="n">
-        <v>3.35795836131632</v>
+        <v>3.29079919409</v>
+      </c>
+      <c r="EH42" t="n">
+        <v>3.304113283884</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -39571,12 +39838,15 @@
         <v>2.86532951289398</v>
       </c>
       <c r="EG43" t="n">
-        <v>2.64663805436337</v>
+        <v>2.5035765379113</v>
+      </c>
+      <c r="EH43" t="n">
+        <v>2.49110320284698</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -39985,11 +40255,14 @@
       </c>
       <c r="EG44" t="n">
         <v>1.90793458509993</v>
+      </c>
+      <c r="EH44" t="n">
+        <v>4.48135380758383</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -40398,11 +40671,14 @@
       </c>
       <c r="EG45" t="n">
         <v>1.35593220338984</v>
+      </c>
+      <c r="EH45" t="n">
+        <v>-2.68456375838925</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -40810,12 +41086,15 @@
         <v>0.365853658536582</v>
       </c>
       <c r="EG46" t="n">
-        <v>0.485731633272624</v>
+        <v>0.364298724954477</v>
+      </c>
+      <c r="EH46" t="n">
+        <v>1.12781954887219</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -41224,11 +41503,14 @@
       </c>
       <c r="EG47" t="n">
         <v>1.57068062827224</v>
+      </c>
+      <c r="EH47" t="n">
+        <v>1.58730158730159</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -41636,12 +41918,15 @@
         <v>-0.99478919943156</v>
       </c>
       <c r="EG48" t="n">
-        <v>-1.36470588235294</v>
+        <v>-1.6</v>
+      </c>
+      <c r="EH48" t="n">
+        <v>-2.87631831255991</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -42050,11 +42335,14 @@
       </c>
       <c r="EG49" t="n">
         <v>2.99462503199385</v>
+      </c>
+      <c r="EH49" t="n">
+        <v>2.92058070025619</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -42463,11 +42751,14 @@
       </c>
       <c r="EG50" t="n">
         <v>4.88372093023257</v>
+      </c>
+      <c r="EH50" t="n">
+        <v>4.88750969743986</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -42876,11 +43167,14 @@
       </c>
       <c r="EG51" t="n">
         <v>2.1604938271605</v>
+      </c>
+      <c r="EH51" t="n">
+        <v>-7.07692307692308</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -43288,12 +43582,15 @@
         <v>3.02375809935204</v>
       </c>
       <c r="EG52" t="n">
-        <v>2.19068188830607</v>
+        <v>2.83863005245294</v>
+      </c>
+      <c r="EH52" t="n">
+        <v>2.90495737290811</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -43701,12 +43998,15 @@
         <v>2.20994475138122</v>
       </c>
       <c r="EG53" t="n">
-        <v>0.154679040989937</v>
+        <v>0.232018561484906</v>
+      </c>
+      <c r="EH53" t="n">
+        <v>-0.615148019992319</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -44115,11 +44415,14 @@
       </c>
       <c r="EG54" t="n">
         <v>1.11111111111112</v>
+      </c>
+      <c r="EH54" t="n">
+        <v>-1.60771704180064</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -44528,11 +44831,14 @@
       </c>
       <c r="EG55" t="n">
         <v>1.12676056338028</v>
+      </c>
+      <c r="EH55" t="n">
+        <v>-1.28939828080227</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -44941,6 +45247,9 @@
       </c>
       <c r="EG56" t="n">
         <v>3.26797385620916</v>
+      </c>
+      <c r="EH56" t="n">
+        <v>2.92207792207793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on july 19th 2024
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t xml:space="preserve">05/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1401,10 +1404,13 @@
       <c r="ET4" t="s">
         <v>149</v>
       </c>
+      <c r="EU4" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1848,15 +1854,18 @@
         <v>11169.1</v>
       </c>
       <c r="ES5" t="n">
-        <v>11158</v>
+        <v>11158.9</v>
       </c>
       <c r="ET5" t="n">
-        <v>11036</v>
+        <v>10998.9</v>
+      </c>
+      <c r="EU5" t="n">
+        <v>10401.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2303,12 +2312,15 @@
         <v>175.6</v>
       </c>
       <c r="ET6" t="n">
-        <v>175.6</v>
+        <v>175.9</v>
+      </c>
+      <c r="EU6" t="n">
+        <v>173</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2755,12 +2767,15 @@
         <v>28.8</v>
       </c>
       <c r="ET7" t="n">
-        <v>27.8</v>
+        <v>27.5</v>
+      </c>
+      <c r="EU7" t="n">
+        <v>21.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3207,12 +3222,15 @@
         <v>203.6</v>
       </c>
       <c r="ET8" t="n">
-        <v>195.5</v>
+        <v>195.2</v>
+      </c>
+      <c r="EU8" t="n">
+        <v>158.9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3660,11 +3678,14 @@
       </c>
       <c r="ET9" t="n">
         <v>103.1</v>
+      </c>
+      <c r="EU9" t="n">
+        <v>94.8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4112,11 +4133,14 @@
       </c>
       <c r="ET10" t="n">
         <v>1303.2</v>
+      </c>
+      <c r="EU10" t="n">
+        <v>1287.4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4564,11 +4588,14 @@
       </c>
       <c r="ET11" t="n">
         <v>240.6</v>
+      </c>
+      <c r="EU11" t="n">
+        <v>224.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5016,11 +5043,14 @@
       </c>
       <c r="ET12" t="n">
         <v>126.1</v>
+      </c>
+      <c r="EU12" t="n">
+        <v>118.9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5467,12 +5497,15 @@
         <v>40.4</v>
       </c>
       <c r="ET13" t="n">
-        <v>39.6</v>
+        <v>40.1</v>
+      </c>
+      <c r="EU13" t="n">
+        <v>37.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5623,10 +5656,11 @@
       <c r="ER14"/>
       <c r="ES14"/>
       <c r="ET14"/>
+      <c r="EU14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6073,12 +6107,15 @@
         <v>501</v>
       </c>
       <c r="ET15" t="n">
-        <v>489</v>
+        <v>489.1</v>
+      </c>
+      <c r="EU15" t="n">
+        <v>409.1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6526,11 +6563,14 @@
       </c>
       <c r="ET16" t="n">
         <v>350</v>
+      </c>
+      <c r="EU16" t="n">
+        <v>340</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6681,10 +6721,11 @@
       <c r="ER17"/>
       <c r="ES17"/>
       <c r="ET17"/>
+      <c r="EU17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7132,11 +7173,14 @@
       </c>
       <c r="ET18" t="n">
         <v>65.8</v>
+      </c>
+      <c r="EU18" t="n">
+        <v>62.1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7584,11 +7628,14 @@
       </c>
       <c r="ET19" t="n">
         <v>459</v>
+      </c>
+      <c r="EU19" t="n">
+        <v>419.6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8035,12 +8082,15 @@
         <v>234.3</v>
       </c>
       <c r="ET20" t="n">
-        <v>232.3</v>
+        <v>232.4</v>
+      </c>
+      <c r="EU20" t="n">
+        <v>190.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8487,12 +8537,15 @@
         <v>148.5</v>
       </c>
       <c r="ET21" t="n">
-        <v>148</v>
+        <v>147.4</v>
+      </c>
+      <c r="EU21" t="n">
+        <v>133</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8939,12 +8992,15 @@
         <v>137.7</v>
       </c>
       <c r="ET22" t="n">
-        <v>137</v>
+        <v>130.8</v>
+      </c>
+      <c r="EU22" t="n">
+        <v>119.2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9391,12 +9447,15 @@
         <v>165.1</v>
       </c>
       <c r="ET23" t="n">
-        <v>164.7</v>
+        <v>164.5</v>
+      </c>
+      <c r="EU23" t="n">
+        <v>154.7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9844,11 +9903,14 @@
       </c>
       <c r="ET24" t="n">
         <v>147.3</v>
+      </c>
+      <c r="EU24" t="n">
+        <v>137.1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10295,12 +10357,15 @@
         <v>49.7</v>
       </c>
       <c r="ET25" t="n">
-        <v>49.7</v>
+        <v>49.9</v>
+      </c>
+      <c r="EU25" t="n">
+        <v>48.1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10748,11 +10813,14 @@
       </c>
       <c r="ET26" t="n">
         <v>229</v>
+      </c>
+      <c r="EU26" t="n">
+        <v>215.7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11200,11 +11268,14 @@
       </c>
       <c r="ET27" t="n">
         <v>244.8</v>
+      </c>
+      <c r="EU27" t="n">
+        <v>240.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11651,12 +11722,15 @@
         <v>328.9</v>
       </c>
       <c r="ET28" t="n">
-        <v>310.9</v>
+        <v>314.5</v>
+      </c>
+      <c r="EU28" t="n">
+        <v>294.7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12103,12 +12177,15 @@
         <v>218</v>
       </c>
       <c r="ET29" t="n">
-        <v>215.9</v>
+        <v>216.3</v>
+      </c>
+      <c r="EU29" t="n">
+        <v>205.8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12555,12 +12632,15 @@
         <v>105</v>
       </c>
       <c r="ET30" t="n">
-        <v>103.4</v>
+        <v>103.3</v>
+      </c>
+      <c r="EU30" t="n">
+        <v>99.9</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -12711,10 +12791,11 @@
       <c r="ER31"/>
       <c r="ES31"/>
       <c r="ET31"/>
+      <c r="EU31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -13162,11 +13243,14 @@
       </c>
       <c r="ET32" t="n">
         <v>46.3</v>
+      </c>
+      <c r="EU32" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13613,12 +13697,15 @@
         <v>94.7</v>
       </c>
       <c r="ET33" t="n">
-        <v>95.5</v>
+        <v>95.3</v>
+      </c>
+      <c r="EU33" t="n">
+        <v>87.9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -14065,12 +14152,15 @@
         <v>85.2</v>
       </c>
       <c r="ET34" t="n">
-        <v>85.8</v>
+        <v>86.3</v>
+      </c>
+      <c r="EU34" t="n">
+        <v>73.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -14517,12 +14607,15 @@
         <v>46</v>
       </c>
       <c r="ET35" t="n">
-        <v>45.4</v>
+        <v>43.9</v>
+      </c>
+      <c r="EU35" t="n">
+        <v>40.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -14969,12 +15062,15 @@
         <v>323.7</v>
       </c>
       <c r="ET36" t="n">
-        <v>320</v>
+        <v>319.5</v>
+      </c>
+      <c r="EU36" t="n">
+        <v>316.1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -15422,11 +15518,14 @@
       </c>
       <c r="ET37" t="n">
         <v>80</v>
+      </c>
+      <c r="EU37" t="n">
+        <v>72.7</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -15874,11 +15973,14 @@
       </c>
       <c r="ET38" t="n">
         <v>682.9</v>
+      </c>
+      <c r="EU38" t="n">
+        <v>670.5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16326,11 +16428,14 @@
       </c>
       <c r="ET39" t="n">
         <v>343.5</v>
+      </c>
+      <c r="EU39" t="n">
+        <v>319.3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -16778,11 +16883,14 @@
       </c>
       <c r="ET40" t="n">
         <v>38.8</v>
+      </c>
+      <c r="EU40" t="n">
+        <v>34.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -17229,12 +17337,15 @@
         <v>391.8</v>
       </c>
       <c r="ET41" t="n">
-        <v>381.7</v>
+        <v>379.6</v>
+      </c>
+      <c r="EU41" t="n">
+        <v>360</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -17681,12 +17792,15 @@
         <v>153.8</v>
       </c>
       <c r="ET42" t="n">
-        <v>153.2</v>
+        <v>153.6</v>
+      </c>
+      <c r="EU42" t="n">
+        <v>139.8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -18133,12 +18247,15 @@
         <v>143.3</v>
       </c>
       <c r="ET43" t="n">
-        <v>144</v>
+        <v>143.2</v>
+      </c>
+      <c r="EU43" t="n">
+        <v>141.6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -18585,12 +18702,15 @@
         <v>336.5</v>
       </c>
       <c r="ET44" t="n">
-        <v>333.4</v>
+        <v>333.5</v>
+      </c>
+      <c r="EU44" t="n">
+        <v>304.8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -19038,11 +19158,14 @@
       </c>
       <c r="ET45" t="n">
         <v>29</v>
+      </c>
+      <c r="EU45" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -19489,12 +19612,15 @@
         <v>165.3</v>
       </c>
       <c r="ET46" t="n">
-        <v>161.4</v>
+        <v>161.6</v>
+      </c>
+      <c r="EU46" t="n">
+        <v>156.9</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -19941,12 +20067,15 @@
         <v>38.8</v>
       </c>
       <c r="ET47" t="n">
-        <v>38.4</v>
+        <v>38.3</v>
+      </c>
+      <c r="EU47" t="n">
+        <v>34.6</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -20393,12 +20522,15 @@
         <v>209.1</v>
       </c>
       <c r="ET48" t="n">
-        <v>202.6</v>
+        <v>202</v>
+      </c>
+      <c r="EU48" t="n">
+        <v>189.3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -20845,12 +20977,15 @@
         <v>1207.2</v>
       </c>
       <c r="ET49" t="n">
-        <v>1205.2</v>
+        <v>1204.6</v>
+      </c>
+      <c r="EU49" t="n">
+        <v>1164.1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -21298,11 +21433,14 @@
       </c>
       <c r="ET50" t="n">
         <v>135.2</v>
+      </c>
+      <c r="EU50" t="n">
+        <v>127.3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -21750,11 +21888,14 @@
       </c>
       <c r="ET51" t="n">
         <v>30.2</v>
+      </c>
+      <c r="EU51" t="n">
+        <v>28.9</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -22201,12 +22342,15 @@
         <v>333.3</v>
       </c>
       <c r="ET52" t="n">
-        <v>325.9</v>
+        <v>328.6</v>
+      </c>
+      <c r="EU52" t="n">
+        <v>320.1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -22653,12 +22797,15 @@
         <v>259.2</v>
       </c>
       <c r="ET53" t="n">
-        <v>258.5</v>
+        <v>260.4</v>
+      </c>
+      <c r="EU53" t="n">
+        <v>256.5</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -23106,11 +23253,14 @@
       </c>
       <c r="ET54" t="n">
         <v>61.2</v>
+      </c>
+      <c r="EU54" t="n">
+        <v>57.4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -23558,11 +23708,14 @@
       </c>
       <c r="ET55" t="n">
         <v>206.7</v>
+      </c>
+      <c r="EU55" t="n">
+        <v>188.3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -24009,7 +24162,10 @@
         <v>31.6</v>
       </c>
       <c r="ET56" t="n">
-        <v>31.7</v>
+        <v>31.6</v>
+      </c>
+      <c r="EU56" t="n">
+        <v>29.1</v>
       </c>
     </row>
   </sheetData>
@@ -24441,10 +24597,13 @@
       <c r="EH4" t="s">
         <v>149</v>
       </c>
+      <c r="EI4" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -24852,15 +25011,18 @@
         <v>2.59304846235806</v>
       </c>
       <c r="EG5" t="n">
-        <v>2.40173269825538</v>
+        <v>2.40999238273543</v>
       </c>
       <c r="EH5" t="n">
-        <v>2.29031689977663</v>
+        <v>1.94644495731726</v>
+      </c>
+      <c r="EI5" t="n">
+        <v>2.12469317623958</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -25271,12 +25433,15 @@
         <v>1.15207373271888</v>
       </c>
       <c r="EH6" t="n">
-        <v>1.0938399539436</v>
+        <v>1.26655152561889</v>
+      </c>
+      <c r="EI6" t="n">
+        <v>1.11046171829338</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -25687,12 +25852,15 @@
         <v>-0.34602076124568</v>
       </c>
       <c r="EH7" t="n">
-        <v>-1.06761565836298</v>
+        <v>-2.13523131672597</v>
+      </c>
+      <c r="EI7" t="n">
+        <v>-4.40528634361234</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -26103,12 +26271,15 @@
         <v>0.0491400491400603</v>
       </c>
       <c r="EH8" t="n">
-        <v>-1.21273370389084</v>
+        <v>-1.36432541687719</v>
+      </c>
+      <c r="EI8" t="n">
+        <v>2.64857881136951</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -26520,11 +26691,14 @@
       </c>
       <c r="EH9" t="n">
         <v>1.07843137254901</v>
+      </c>
+      <c r="EI9" t="n">
+        <v>1.17395944503736</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -26936,11 +27110,14 @@
       </c>
       <c r="EH10" t="n">
         <v>3.01161963481147</v>
+      </c>
+      <c r="EI10" t="n">
+        <v>3.03321328531413</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -27352,11 +27529,14 @@
       </c>
       <c r="EH11" t="n">
         <v>5.66534914361002</v>
+      </c>
+      <c r="EI11" t="n">
+        <v>4.46719404374129</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -27768,11 +27948,14 @@
       </c>
       <c r="EH12" t="n">
         <v>1.12269446672012</v>
+      </c>
+      <c r="EI12" t="n">
+        <v>2.06008583690988</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -28183,12 +28366,15 @@
         <v>3.06122448979593</v>
       </c>
       <c r="EH13" t="n">
-        <v>2.85714285714284</v>
+        <v>4.15584415584416</v>
+      </c>
+      <c r="EI13" t="n">
+        <v>4.45682451253482</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -28327,10 +28513,11 @@
       <c r="EF14"/>
       <c r="EG14"/>
       <c r="EH14"/>
+      <c r="EI14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -28741,12 +28928,15 @@
         <v>1.51975683890578</v>
       </c>
       <c r="EH15" t="n">
-        <v>1.38917686087498</v>
+        <v>1.40991084387312</v>
+      </c>
+      <c r="EI15" t="n">
+        <v>1.21227115289459</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -29158,11 +29348,14 @@
       </c>
       <c r="EH16" t="n">
         <v>1.77377144518756</v>
+      </c>
+      <c r="EI16" t="n">
+        <v>2.44049412473637</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -29301,10 +29494,11 @@
       <c r="EF17"/>
       <c r="EG17"/>
       <c r="EH17"/>
+      <c r="EI17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -29716,11 +29910,14 @@
       </c>
       <c r="EH18" t="n">
         <v>6.30048465266561</v>
+      </c>
+      <c r="EI18" t="n">
+        <v>5.0761421319797</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -30132,11 +30329,14 @@
       </c>
       <c r="EH19" t="n">
         <v>3.47159603246167</v>
+      </c>
+      <c r="EI19" t="n">
+        <v>0.623501199040773</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -30547,12 +30747,15 @@
         <v>1.47249891728022</v>
       </c>
       <c r="EH20" t="n">
-        <v>0.912250217202443</v>
+        <v>0.955690703735889</v>
+      </c>
+      <c r="EI20" t="n">
+        <v>0.741525423728801</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -30963,12 +31166,15 @@
         <v>1.43442622950819</v>
       </c>
       <c r="EH21" t="n">
-        <v>1.09289617486338</v>
+        <v>0.683060109289598</v>
+      </c>
+      <c r="EI21" t="n">
+        <v>-0.374531835205993</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -31379,12 +31585,15 @@
         <v>0.510948905109481</v>
       </c>
       <c r="EH22" t="n">
-        <v>0.146198830409348</v>
+        <v>-4.3859649122807</v>
+      </c>
+      <c r="EI22" t="n">
+        <v>0.252312867956251</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -31795,12 +32004,15 @@
         <v>1.53751537515375</v>
       </c>
       <c r="EH23" t="n">
-        <v>1.16707616707615</v>
+        <v>1.04422604422604</v>
+      </c>
+      <c r="EI23" t="n">
+        <v>0.847457627118633</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -32212,11 +32424,14 @@
       </c>
       <c r="EH24" t="n">
         <v>-0.203252032520314</v>
+      </c>
+      <c r="EI24" t="n">
+        <v>-0.21834061135372</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -32627,12 +32842,15 @@
         <v>2.26337448559673</v>
       </c>
       <c r="EH25" t="n">
-        <v>1.63599182004091</v>
+        <v>2.04498977505112</v>
+      </c>
+      <c r="EI25" t="n">
+        <v>1.90677966101695</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -33044,11 +33262,14 @@
       </c>
       <c r="EH26" t="n">
         <v>2.78276481149012</v>
+      </c>
+      <c r="EI26" t="n">
+        <v>3.75180375180377</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -33460,11 +33681,14 @@
       </c>
       <c r="EH27" t="n">
         <v>1.32450331125827</v>
+      </c>
+      <c r="EI27" t="n">
+        <v>1.34850400337127</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -33875,12 +34099,15 @@
         <v>5.45046489259378</v>
       </c>
       <c r="EH28" t="n">
-        <v>2.40447957839261</v>
+        <v>3.59025032938076</v>
+      </c>
+      <c r="EI28" t="n">
+        <v>4.02400282386164</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -34291,12 +34518,15 @@
         <v>4.90856592877766</v>
       </c>
       <c r="EH29" t="n">
-        <v>5.26572403705509</v>
+        <v>5.46075085324232</v>
+      </c>
+      <c r="EI29" t="n">
+        <v>3.05458187280921</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -34707,12 +34937,15 @@
         <v>1.25361620057859</v>
       </c>
       <c r="EH30" t="n">
-        <v>0.779727095516553</v>
+        <v>0.682261208576987</v>
+      </c>
+      <c r="EI30" t="n">
+        <v>2.0429009193054</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -34851,10 +35084,11 @@
       <c r="EF31"/>
       <c r="EG31"/>
       <c r="EH31"/>
+      <c r="EI31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -35266,11 +35500,14 @@
       </c>
       <c r="EH32" t="n">
         <v>1.75824175824175</v>
+      </c>
+      <c r="EI32" t="n">
+        <v>1.89573459715639</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -35681,12 +35918,15 @@
         <v>-0.0000000000000150061823814171</v>
       </c>
       <c r="EH33" t="n">
-        <v>0.844772967265044</v>
+        <v>0.63357972544878</v>
+      </c>
+      <c r="EI33" t="n">
+        <v>-2.98013245033111</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -36097,12 +36337,15 @@
         <v>4.02930402930403</v>
       </c>
       <c r="EH34" t="n">
-        <v>4</v>
+        <v>4.6060606060606</v>
+      </c>
+      <c r="EI34" t="n">
+        <v>1.24653739612187</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -36513,12 +36756,15 @@
         <v>0.877192982456137</v>
       </c>
       <c r="EH35" t="n">
-        <v>0.442477876106201</v>
+        <v>-2.87610619469024</v>
+      </c>
+      <c r="EI35" t="n">
+        <v>5.44041450777202</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -36929,12 +37175,15 @@
         <v>2.63157894736841</v>
       </c>
       <c r="EH36" t="n">
-        <v>2.59698621352997</v>
+        <v>2.43667842257133</v>
+      </c>
+      <c r="EI36" t="n">
+        <v>2.69655620532814</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -37346,11 +37595,14 @@
       </c>
       <c r="EH37" t="n">
         <v>3.09278350515465</v>
+      </c>
+      <c r="EI37" t="n">
+        <v>4.60431654676259</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -37762,11 +38014,14 @@
       </c>
       <c r="EH38" t="n">
         <v>2.47599039615848</v>
+      </c>
+      <c r="EI38" t="n">
+        <v>2.47592847317743</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -38178,11 +38433,14 @@
       </c>
       <c r="EH39" t="n">
         <v>2.08023774145617</v>
+      </c>
+      <c r="EI39" t="n">
+        <v>1.85007974481659</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -38594,11 +38852,14 @@
       </c>
       <c r="EH40" t="n">
         <v>1.83727034120736</v>
+      </c>
+      <c r="EI40" t="n">
+        <v>5.90062111801242</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -39009,12 +39270,15 @@
         <v>-1.77989471045375</v>
       </c>
       <c r="EH41" t="n">
-        <v>-2.99872935196951</v>
+        <v>-3.53240152477763</v>
+      </c>
+      <c r="EI41" t="n">
+        <v>-0.826446280991736</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -39425,12 +39689,15 @@
         <v>3.29079919409</v>
       </c>
       <c r="EH42" t="n">
-        <v>3.304113283884</v>
+        <v>3.57383681726231</v>
+      </c>
+      <c r="EI42" t="n">
+        <v>2.64317180616742</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -39841,12 +40108,15 @@
         <v>2.5035765379113</v>
       </c>
       <c r="EH43" t="n">
-        <v>2.49110320284698</v>
+        <v>1.92170818505339</v>
+      </c>
+      <c r="EI43" t="n">
+        <v>0.926585887384165</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -40257,12 +40527,15 @@
         <v>1.90793458509993</v>
       </c>
       <c r="EH44" t="n">
-        <v>4.48135380758383</v>
+        <v>4.51269194609841</v>
+      </c>
+      <c r="EI44" t="n">
+        <v>1.83762111593719</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -40674,11 +40947,14 @@
       </c>
       <c r="EH45" t="n">
         <v>-2.68456375838925</v>
+      </c>
+      <c r="EI45" t="n">
+        <v>2.94117647058824</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -41089,12 +41365,15 @@
         <v>0.364298724954477</v>
       </c>
       <c r="EH46" t="n">
-        <v>1.12781954887219</v>
+        <v>1.2531328320802</v>
+      </c>
+      <c r="EI46" t="n">
+        <v>1.42210730446026</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -41505,12 +41784,15 @@
         <v>1.57068062827224</v>
       </c>
       <c r="EH47" t="n">
-        <v>1.58730158730159</v>
+        <v>1.32275132275132</v>
+      </c>
+      <c r="EI47" t="n">
+        <v>1.46627565982405</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -41921,12 +42203,15 @@
         <v>-1.6</v>
       </c>
       <c r="EH48" t="n">
-        <v>-2.87631831255991</v>
+        <v>-3.16395014381591</v>
+      </c>
+      <c r="EI48" t="n">
+        <v>-2.87326834273985</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -42337,12 +42622,15 @@
         <v>2.99462503199385</v>
       </c>
       <c r="EH49" t="n">
-        <v>2.92058070025619</v>
+        <v>2.86934244235695</v>
+      </c>
+      <c r="EI49" t="n">
+        <v>3.0085833112114</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -42754,11 +43042,14 @@
       </c>
       <c r="EH50" t="n">
         <v>4.88750969743986</v>
+      </c>
+      <c r="EI50" t="n">
+        <v>3.83360522022838</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -43170,11 +43461,14 @@
       </c>
       <c r="EH51" t="n">
         <v>-7.07692307692308</v>
+      </c>
+      <c r="EI51" t="n">
+        <v>-0.687285223367707</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -43585,12 +43879,15 @@
         <v>2.83863005245294</v>
       </c>
       <c r="EH52" t="n">
-        <v>2.90495737290811</v>
+        <v>3.75749921060942</v>
+      </c>
+      <c r="EI52" t="n">
+        <v>4.19921875000001</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -44001,12 +44298,15 @@
         <v>0.232018561484906</v>
       </c>
       <c r="EH53" t="n">
-        <v>-0.615148019992319</v>
+        <v>0.115340253748541</v>
+      </c>
+      <c r="EI53" t="n">
+        <v>-0.0779119594857766</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -44417,12 +44717,15 @@
         <v>1.11111111111112</v>
       </c>
       <c r="EH54" t="n">
-        <v>-1.60771704180064</v>
+        <v>-1.60771704180065</v>
+      </c>
+      <c r="EI54" t="n">
+        <v>-0.692041522491347</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -44834,11 +45137,14 @@
       </c>
       <c r="EH55" t="n">
         <v>-1.28939828080227</v>
+      </c>
+      <c r="EI55" t="n">
+        <v>-0.475687103594068</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -45249,7 +45555,10 @@
         <v>3.26797385620916</v>
       </c>
       <c r="EH56" t="n">
-        <v>2.92207792207793</v>
+        <v>2.5974025974026</v>
+      </c>
+      <c r="EI56" t="n">
+        <v>3.19148936170214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on August 16
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -466,6 +466,9 @@
   </si>
   <si>
     <t xml:space="preserve">06/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1407,10 +1410,13 @@
       <c r="EU4" t="s">
         <v>150</v>
       </c>
+      <c r="EV4" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1857,15 +1863,18 @@
         <v>11158.9</v>
       </c>
       <c r="ET5" t="n">
-        <v>10998.9</v>
+        <v>10987.9</v>
       </c>
       <c r="EU5" t="n">
-        <v>10401.4</v>
+        <v>10350.2</v>
+      </c>
+      <c r="EV5" t="n">
+        <v>9275.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2316,11 +2325,14 @@
       </c>
       <c r="EU6" t="n">
         <v>173</v>
+      </c>
+      <c r="EV6" t="n">
+        <v>163.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2770,12 +2782,15 @@
         <v>27.5</v>
       </c>
       <c r="EU7" t="n">
-        <v>21.7</v>
+        <v>21.5</v>
+      </c>
+      <c r="EV7" t="n">
+        <v>18.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3225,12 +3240,15 @@
         <v>195.2</v>
       </c>
       <c r="EU8" t="n">
-        <v>158.9</v>
+        <v>155.6</v>
+      </c>
+      <c r="EV8" t="n">
+        <v>151</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3681,11 +3699,14 @@
       </c>
       <c r="EU9" t="n">
         <v>94.8</v>
+      </c>
+      <c r="EV9" t="n">
+        <v>83.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4135,12 +4156,15 @@
         <v>1303.2</v>
       </c>
       <c r="EU10" t="n">
-        <v>1287.4</v>
+        <v>1277.9</v>
+      </c>
+      <c r="EV10" t="n">
+        <v>1119.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4590,12 +4614,15 @@
         <v>240.6</v>
       </c>
       <c r="EU11" t="n">
-        <v>224.5</v>
+        <v>224.4</v>
+      </c>
+      <c r="EV11" t="n">
+        <v>210.8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5045,12 +5072,15 @@
         <v>126.1</v>
       </c>
       <c r="EU12" t="n">
-        <v>118.9</v>
+        <v>119.2</v>
+      </c>
+      <c r="EV12" t="n">
+        <v>99.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5500,12 +5530,15 @@
         <v>40.1</v>
       </c>
       <c r="EU13" t="n">
-        <v>37.5</v>
+        <v>36.9</v>
+      </c>
+      <c r="EV13" t="n">
+        <v>35.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5657,10 +5690,11 @@
       <c r="ES14"/>
       <c r="ET14"/>
       <c r="EU14"/>
+      <c r="EV14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6110,12 +6144,15 @@
         <v>489.1</v>
       </c>
       <c r="EU15" t="n">
-        <v>409.1</v>
+        <v>409.2</v>
+      </c>
+      <c r="EV15" t="n">
+        <v>401.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6565,12 +6602,15 @@
         <v>350</v>
       </c>
       <c r="EU16" t="n">
-        <v>340</v>
+        <v>340.6</v>
+      </c>
+      <c r="EV16" t="n">
+        <v>329</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6722,10 +6762,11 @@
       <c r="ES17"/>
       <c r="ET17"/>
       <c r="EU17"/>
+      <c r="EV17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7175,12 +7216,15 @@
         <v>65.8</v>
       </c>
       <c r="EU18" t="n">
-        <v>62.1</v>
+        <v>62.5</v>
+      </c>
+      <c r="EV18" t="n">
+        <v>55.4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7630,12 +7674,15 @@
         <v>459</v>
       </c>
       <c r="EU19" t="n">
-        <v>419.6</v>
+        <v>424.4</v>
+      </c>
+      <c r="EV19" t="n">
+        <v>406.2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8085,12 +8132,15 @@
         <v>232.4</v>
       </c>
       <c r="EU20" t="n">
-        <v>190.2</v>
+        <v>185.1</v>
+      </c>
+      <c r="EV20" t="n">
+        <v>173.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8540,12 +8590,15 @@
         <v>147.4</v>
       </c>
       <c r="EU21" t="n">
-        <v>133</v>
+        <v>131.9</v>
+      </c>
+      <c r="EV21" t="n">
+        <v>114.9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -8996,11 +9049,14 @@
       </c>
       <c r="EU22" t="n">
         <v>119.2</v>
+      </c>
+      <c r="EV22" t="n">
+        <v>96.5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9450,12 +9506,15 @@
         <v>164.5</v>
       </c>
       <c r="EU23" t="n">
-        <v>154.7</v>
+        <v>154.3</v>
+      </c>
+      <c r="EV23" t="n">
+        <v>129.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9906,11 +9965,14 @@
       </c>
       <c r="EU24" t="n">
         <v>137.1</v>
+      </c>
+      <c r="EV24" t="n">
+        <v>130.4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10360,12 +10422,15 @@
         <v>49.9</v>
       </c>
       <c r="EU25" t="n">
-        <v>48.1</v>
+        <v>46.8</v>
+      </c>
+      <c r="EV25" t="n">
+        <v>40.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10816,11 +10881,14 @@
       </c>
       <c r="EU26" t="n">
         <v>215.7</v>
+      </c>
+      <c r="EV26" t="n">
+        <v>202.2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11271,11 +11339,14 @@
       </c>
       <c r="EU27" t="n">
         <v>240.5</v>
+      </c>
+      <c r="EV27" t="n">
+        <v>214.7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11726,11 +11797,14 @@
       </c>
       <c r="EU28" t="n">
         <v>294.7</v>
+      </c>
+      <c r="EV28" t="n">
+        <v>267</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12180,12 +12254,15 @@
         <v>216.3</v>
       </c>
       <c r="EU29" t="n">
-        <v>205.8</v>
+        <v>205.5</v>
+      </c>
+      <c r="EV29" t="n">
+        <v>176</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12635,12 +12712,15 @@
         <v>103.3</v>
       </c>
       <c r="EU30" t="n">
-        <v>99.9</v>
+        <v>99.8</v>
+      </c>
+      <c r="EV30" t="n">
+        <v>95.4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -12792,10 +12872,11 @@
       <c r="ES31"/>
       <c r="ET31"/>
       <c r="EU31"/>
+      <c r="EV31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -13246,11 +13327,14 @@
       </c>
       <c r="EU32" t="n">
         <v>43</v>
+      </c>
+      <c r="EV32" t="n">
+        <v>35.5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13700,12 +13784,15 @@
         <v>95.3</v>
       </c>
       <c r="EU33" t="n">
-        <v>87.9</v>
+        <v>87.6</v>
+      </c>
+      <c r="EV33" t="n">
+        <v>78.6</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -14156,11 +14243,14 @@
       </c>
       <c r="EU34" t="n">
         <v>73.1</v>
+      </c>
+      <c r="EV34" t="n">
+        <v>67.7</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -14610,12 +14700,15 @@
         <v>43.9</v>
       </c>
       <c r="EU35" t="n">
-        <v>40.7</v>
+        <v>39.7</v>
+      </c>
+      <c r="EV35" t="n">
+        <v>32.3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -15065,12 +15158,15 @@
         <v>319.5</v>
       </c>
       <c r="EU36" t="n">
-        <v>316.1</v>
+        <v>315.6</v>
+      </c>
+      <c r="EV36" t="n">
+        <v>264</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -15520,12 +15616,15 @@
         <v>80</v>
       </c>
       <c r="EU37" t="n">
-        <v>72.7</v>
+        <v>71.2</v>
+      </c>
+      <c r="EV37" t="n">
+        <v>63.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -15976,11 +16075,14 @@
       </c>
       <c r="EU38" t="n">
         <v>670.5</v>
+      </c>
+      <c r="EV38" t="n">
+        <v>563.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16431,11 +16533,14 @@
       </c>
       <c r="EU39" t="n">
         <v>319.3</v>
+      </c>
+      <c r="EV39" t="n">
+        <v>261.1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -16885,12 +16990,15 @@
         <v>38.8</v>
       </c>
       <c r="EU40" t="n">
-        <v>34.1</v>
+        <v>33.9</v>
+      </c>
+      <c r="EV40" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -17340,12 +17448,15 @@
         <v>379.6</v>
       </c>
       <c r="EU41" t="n">
-        <v>360</v>
+        <v>359</v>
+      </c>
+      <c r="EV41" t="n">
+        <v>347.8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -17795,12 +17906,15 @@
         <v>153.6</v>
       </c>
       <c r="EU42" t="n">
-        <v>139.8</v>
+        <v>137.8</v>
+      </c>
+      <c r="EV42" t="n">
+        <v>124.8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -18250,12 +18364,15 @@
         <v>143.2</v>
       </c>
       <c r="EU43" t="n">
-        <v>141.6</v>
+        <v>141.3</v>
+      </c>
+      <c r="EV43" t="n">
+        <v>111</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -18705,12 +18822,15 @@
         <v>333.5</v>
       </c>
       <c r="EU44" t="n">
-        <v>304.8</v>
+        <v>305.2</v>
+      </c>
+      <c r="EV44" t="n">
+        <v>277.3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -19161,11 +19281,14 @@
       </c>
       <c r="EU45" t="n">
         <v>28</v>
+      </c>
+      <c r="EV45" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -19615,12 +19738,15 @@
         <v>161.6</v>
       </c>
       <c r="EU46" t="n">
-        <v>156.9</v>
+        <v>156.8</v>
+      </c>
+      <c r="EV46" t="n">
+        <v>146.5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -20070,12 +20196,15 @@
         <v>38.3</v>
       </c>
       <c r="EU47" t="n">
-        <v>34.6</v>
+        <v>34.3</v>
+      </c>
+      <c r="EV47" t="n">
+        <v>28.8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -20526,11 +20655,14 @@
       </c>
       <c r="EU48" t="n">
         <v>189.3</v>
+      </c>
+      <c r="EV48" t="n">
+        <v>164.1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -20980,12 +21112,15 @@
         <v>1204.6</v>
       </c>
       <c r="EU49" t="n">
-        <v>1164.1</v>
+        <v>1159.2</v>
+      </c>
+      <c r="EV49" t="n">
+        <v>1088</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -21435,12 +21570,15 @@
         <v>135.2</v>
       </c>
       <c r="EU50" t="n">
-        <v>127.3</v>
+        <v>127.8</v>
+      </c>
+      <c r="EV50" t="n">
+        <v>112.7</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -21891,11 +22029,14 @@
       </c>
       <c r="EU51" t="n">
         <v>28.9</v>
+      </c>
+      <c r="EV51" t="n">
+        <v>25.4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -22345,12 +22486,15 @@
         <v>328.6</v>
       </c>
       <c r="EU52" t="n">
-        <v>320.1</v>
+        <v>315.2</v>
+      </c>
+      <c r="EV52" t="n">
+        <v>283.7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -22800,12 +22944,15 @@
         <v>260.4</v>
       </c>
       <c r="EU53" t="n">
-        <v>256.5</v>
+        <v>253.3</v>
+      </c>
+      <c r="EV53" t="n">
+        <v>234.4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -23255,12 +23402,15 @@
         <v>61.2</v>
       </c>
       <c r="EU54" t="n">
-        <v>57.4</v>
+        <v>56.1</v>
+      </c>
+      <c r="EV54" t="n">
+        <v>51.6</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -23710,12 +23860,15 @@
         <v>206.7</v>
       </c>
       <c r="EU55" t="n">
-        <v>188.3</v>
+        <v>187.3</v>
+      </c>
+      <c r="EV55" t="n">
+        <v>170.6</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -24165,7 +24318,10 @@
         <v>31.6</v>
       </c>
       <c r="EU56" t="n">
-        <v>29.1</v>
+        <v>28.9</v>
+      </c>
+      <c r="EV56" t="n">
+        <v>24.2</v>
       </c>
     </row>
   </sheetData>
@@ -24600,10 +24756,13 @@
       <c r="EI4" t="s">
         <v>150</v>
       </c>
+      <c r="EJ4" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -25014,15 +25173,18 @@
         <v>2.40999238273543</v>
       </c>
       <c r="EH5" t="n">
-        <v>1.94644495731726</v>
+        <v>1.84448831669588</v>
       </c>
       <c r="EI5" t="n">
-        <v>2.12469317623958</v>
+        <v>1.62199312714777</v>
+      </c>
+      <c r="EJ5" t="n">
+        <v>1.97557194841744</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -25437,11 +25599,14 @@
       </c>
       <c r="EI6" t="n">
         <v>1.11046171829338</v>
+      </c>
+      <c r="EJ6" t="n">
+        <v>0.491400491400498</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -25855,12 +26020,15 @@
         <v>-2.13523131672597</v>
       </c>
       <c r="EI7" t="n">
-        <v>-4.40528634361234</v>
+        <v>-5.2863436123348</v>
+      </c>
+      <c r="EJ7" t="n">
+        <v>-2.08333333333333</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -26274,12 +26442,15 @@
         <v>-1.36432541687719</v>
       </c>
       <c r="EI8" t="n">
-        <v>2.64857881136951</v>
+        <v>0.516795865633064</v>
+      </c>
+      <c r="EJ8" t="n">
+        <v>0.132625994694953</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -26694,11 +26865,14 @@
       </c>
       <c r="EI9" t="n">
         <v>1.17395944503736</v>
+      </c>
+      <c r="EJ9" t="n">
+        <v>1.21065375302663</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -27112,12 +27286,15 @@
         <v>3.01161963481147</v>
       </c>
       <c r="EI10" t="n">
-        <v>3.03321328531413</v>
+        <v>2.27290916366547</v>
+      </c>
+      <c r="EJ10" t="n">
+        <v>4.24501954943213</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -27531,12 +27708,15 @@
         <v>5.66534914361002</v>
       </c>
       <c r="EI11" t="n">
-        <v>4.46719404374129</v>
+        <v>4.4206607724523</v>
+      </c>
+      <c r="EJ11" t="n">
+        <v>4.82347090999502</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -27950,12 +28130,15 @@
         <v>1.12269446672012</v>
       </c>
       <c r="EI12" t="n">
-        <v>2.06008583690988</v>
+        <v>2.31759656652361</v>
+      </c>
+      <c r="EJ12" t="n">
+        <v>1.94274028629857</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -28369,12 +28552,15 @@
         <v>4.15584415584416</v>
       </c>
       <c r="EI13" t="n">
-        <v>4.45682451253482</v>
+        <v>2.78551532033426</v>
+      </c>
+      <c r="EJ13" t="n">
+        <v>3.19767441860466</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -28514,10 +28700,11 @@
       <c r="EG14"/>
       <c r="EH14"/>
       <c r="EI14"/>
+      <c r="EJ14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -28931,12 +29118,15 @@
         <v>1.40991084387312</v>
       </c>
       <c r="EI15" t="n">
-        <v>1.21227115289459</v>
+        <v>1.23701138050469</v>
+      </c>
+      <c r="EJ15" t="n">
+        <v>0.904749937170149</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -29350,12 +29540,15 @@
         <v>1.77377144518756</v>
       </c>
       <c r="EI16" t="n">
-        <v>2.44049412473637</v>
+        <v>2.62127146730944</v>
+      </c>
+      <c r="EJ16" t="n">
+        <v>4.24588086185044</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -29495,10 +29688,11 @@
       <c r="EG17"/>
       <c r="EH17"/>
       <c r="EI17"/>
+      <c r="EJ17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -29912,12 +30106,15 @@
         <v>6.30048465266561</v>
       </c>
       <c r="EI18" t="n">
-        <v>5.0761421319797</v>
+        <v>5.75296108291032</v>
+      </c>
+      <c r="EJ18" t="n">
+        <v>7.15667311411993</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -30331,12 +30528,15 @@
         <v>3.47159603246167</v>
       </c>
       <c r="EI19" t="n">
-        <v>0.623501199040773</v>
+        <v>1.77458033573141</v>
+      </c>
+      <c r="EJ19" t="n">
+        <v>5.80880437613962</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -30750,12 +30950,15 @@
         <v>0.955690703735889</v>
       </c>
       <c r="EI20" t="n">
-        <v>0.741525423728801</v>
+        <v>-1.95974576271186</v>
+      </c>
+      <c r="EJ20" t="n">
+        <v>2.48520710059171</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -31169,12 +31372,15 @@
         <v>0.683060109289598</v>
       </c>
       <c r="EI21" t="n">
-        <v>-0.374531835205993</v>
+        <v>-1.19850187265919</v>
+      </c>
+      <c r="EJ21" t="n">
+        <v>-1.7948717948718</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -31589,11 +31795,14 @@
       </c>
       <c r="EI22" t="n">
         <v>0.252312867956251</v>
+      </c>
+      <c r="EJ22" t="n">
+        <v>-0.309917355371898</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -32007,12 +32216,15 @@
         <v>1.04422604422604</v>
       </c>
       <c r="EI23" t="n">
-        <v>0.847457627118633</v>
+        <v>0.586701434159065</v>
+      </c>
+      <c r="EJ23" t="n">
+        <v>1.09289617486339</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -32427,11 +32639,14 @@
       </c>
       <c r="EI24" t="n">
         <v>-0.21834061135372</v>
+      </c>
+      <c r="EJ24" t="n">
+        <v>0.539707016191224</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -32845,12 +33060,15 @@
         <v>2.04498977505112</v>
       </c>
       <c r="EI25" t="n">
-        <v>1.90677966101695</v>
+        <v>-0.847457627118656</v>
+      </c>
+      <c r="EJ25" t="n">
+        <v>0.997506234413979</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -33265,11 +33483,14 @@
       </c>
       <c r="EI26" t="n">
         <v>3.75180375180377</v>
+      </c>
+      <c r="EJ26" t="n">
+        <v>3.63915940543309</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -33684,11 +33905,14 @@
       </c>
       <c r="EI27" t="n">
         <v>1.34850400337127</v>
+      </c>
+      <c r="EJ27" t="n">
+        <v>1.36921624173748</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -34103,11 +34327,14 @@
       </c>
       <c r="EI28" t="n">
         <v>4.02400282386164</v>
+      </c>
+      <c r="EJ28" t="n">
+        <v>3.44827586206896</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -34521,12 +34748,15 @@
         <v>5.46075085324232</v>
       </c>
       <c r="EI29" t="n">
-        <v>3.05458187280921</v>
+        <v>2.90435653480219</v>
+      </c>
+      <c r="EJ29" t="n">
+        <v>2.92397660818713</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -34940,12 +35170,15 @@
         <v>0.682261208576987</v>
       </c>
       <c r="EI30" t="n">
-        <v>2.0429009193054</v>
+        <v>1.94075587334013</v>
+      </c>
+      <c r="EJ30" t="n">
+        <v>1.59744408945685</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -35085,10 +35318,11 @@
       <c r="EG31"/>
       <c r="EH31"/>
       <c r="EI31"/>
+      <c r="EJ31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -35503,11 +35737,14 @@
       </c>
       <c r="EI32" t="n">
         <v>1.89573459715639</v>
+      </c>
+      <c r="EJ32" t="n">
+        <v>1.71919770773637</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -35921,12 +36158,15 @@
         <v>0.63357972544878</v>
       </c>
       <c r="EI33" t="n">
-        <v>-2.98013245033111</v>
+        <v>-3.3112582781457</v>
+      </c>
+      <c r="EJ33" t="n">
+        <v>-0.506329113924058</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -36341,11 +36581,14 @@
       </c>
       <c r="EI34" t="n">
         <v>1.24653739612187</v>
+      </c>
+      <c r="EJ34" t="n">
+        <v>1.80451127819549</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -36759,12 +37002,15 @@
         <v>-2.87610619469024</v>
       </c>
       <c r="EI35" t="n">
-        <v>5.44041450777202</v>
+        <v>2.84974093264247</v>
+      </c>
+      <c r="EJ35" t="n">
+        <v>-1.22324159021404</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -37178,12 +37424,15 @@
         <v>2.43667842257133</v>
       </c>
       <c r="EI36" t="n">
-        <v>2.69655620532814</v>
+        <v>2.53411306042885</v>
+      </c>
+      <c r="EJ36" t="n">
+        <v>2.60396424407306</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -37597,12 +37846,15 @@
         <v>3.09278350515465</v>
       </c>
       <c r="EI37" t="n">
-        <v>4.60431654676259</v>
+        <v>2.44604316546763</v>
+      </c>
+      <c r="EJ37" t="n">
+        <v>-0.626959247648901</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -38017,11 +38269,14 @@
       </c>
       <c r="EI38" t="n">
         <v>2.47592847317743</v>
+      </c>
+      <c r="EJ38" t="n">
+        <v>2.53095411507647</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -38436,11 +38691,14 @@
       </c>
       <c r="EI39" t="n">
         <v>1.85007974481659</v>
+      </c>
+      <c r="EJ39" t="n">
+        <v>1.95236235845373</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -38854,12 +39112,15 @@
         <v>1.83727034120736</v>
       </c>
       <c r="EI40" t="n">
-        <v>5.90062111801242</v>
+        <v>5.27950310559005</v>
+      </c>
+      <c r="EJ40" t="n">
+        <v>6.22710622710622</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -39273,12 +39534,15 @@
         <v>-3.53240152477763</v>
       </c>
       <c r="EI41" t="n">
-        <v>-0.826446280991736</v>
+        <v>-1.10192837465565</v>
+      </c>
+      <c r="EJ41" t="n">
+        <v>-1.19318181818183</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -39692,12 +39956,15 @@
         <v>3.57383681726231</v>
       </c>
       <c r="EI42" t="n">
-        <v>2.64317180616742</v>
+        <v>1.17474302496331</v>
+      </c>
+      <c r="EJ42" t="n">
+        <v>1.05263157894738</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -40111,12 +40378,15 @@
         <v>1.92170818505339</v>
       </c>
       <c r="EI43" t="n">
-        <v>0.926585887384165</v>
+        <v>0.712758374910905</v>
+      </c>
+      <c r="EJ43" t="n">
+        <v>1.00090991810737</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -40530,12 +40800,15 @@
         <v>4.51269194609841</v>
       </c>
       <c r="EI44" t="n">
-        <v>1.83762111593719</v>
+        <v>1.97126628800534</v>
+      </c>
+      <c r="EJ44" t="n">
+        <v>1.093693036821</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -40950,11 +41223,14 @@
       </c>
       <c r="EI45" t="n">
         <v>2.94117647058824</v>
+      </c>
+      <c r="EJ45" t="n">
+        <v>5.26315789473685</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -41368,12 +41644,15 @@
         <v>1.2531328320802</v>
       </c>
       <c r="EI46" t="n">
-        <v>1.42210730446026</v>
+        <v>1.35746606334843</v>
+      </c>
+      <c r="EJ46" t="n">
+        <v>1.03448275862069</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -41787,12 +42066,15 @@
         <v>1.32275132275132</v>
       </c>
       <c r="EI47" t="n">
-        <v>1.46627565982405</v>
+        <v>0.586510263929627</v>
+      </c>
+      <c r="EJ47" t="n">
+        <v>2.12765957446808</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -42207,11 +42489,14 @@
       </c>
       <c r="EI48" t="n">
         <v>-2.87326834273985</v>
+      </c>
+      <c r="EJ48" t="n">
+        <v>-2.66903914590747</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -42625,12 +42910,15 @@
         <v>2.86934244235695</v>
       </c>
       <c r="EI49" t="n">
-        <v>3.0085833112114</v>
+        <v>2.57499336341918</v>
+      </c>
+      <c r="EJ49" t="n">
+        <v>2.98154283009938</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -43044,12 +43332,15 @@
         <v>4.88750969743986</v>
       </c>
       <c r="EI50" t="n">
-        <v>3.83360522022838</v>
+        <v>4.24143556280586</v>
+      </c>
+      <c r="EJ50" t="n">
+        <v>5.22875816993464</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -43464,11 +43755,14 @@
       </c>
       <c r="EI51" t="n">
         <v>-0.687285223367707</v>
+      </c>
+      <c r="EJ51" t="n">
+        <v>-0.000000000000013987061727561</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -43882,12 +44176,15 @@
         <v>3.75749921060942</v>
       </c>
       <c r="EI52" t="n">
-        <v>4.19921875000001</v>
+        <v>2.60416666666667</v>
+      </c>
+      <c r="EJ52" t="n">
+        <v>2.45576020223908</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -44301,12 +44598,15 @@
         <v>0.115340253748541</v>
       </c>
       <c r="EI53" t="n">
-        <v>-0.0779119594857766</v>
+        <v>-1.32450331125827</v>
+      </c>
+      <c r="EJ53" t="n">
+        <v>0.55770055770055</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -44720,12 +45020,15 @@
         <v>-1.60771704180065</v>
       </c>
       <c r="EI54" t="n">
-        <v>-0.692041522491347</v>
+        <v>-2.94117647058823</v>
+      </c>
+      <c r="EJ54" t="n">
+        <v>-0.578034682080947</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -45139,12 +45442,15 @@
         <v>-1.28939828080227</v>
       </c>
       <c r="EI55" t="n">
-        <v>-0.475687103594068</v>
+        <v>-1.00422832980973</v>
+      </c>
+      <c r="EJ55" t="n">
+        <v>0.293944738389166</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -45558,7 +45864,10 @@
         <v>2.5974025974026</v>
       </c>
       <c r="EI56" t="n">
-        <v>3.19148936170214</v>
+        <v>2.4822695035461</v>
+      </c>
+      <c r="EJ56" t="n">
+        <v>1.255230125523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on Sept 20 2024
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t xml:space="preserve">07/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1413,10 +1416,13 @@
       <c r="EV4" t="s">
         <v>151</v>
       </c>
+      <c r="EW4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1866,15 +1872,18 @@
         <v>10987.9</v>
       </c>
       <c r="EU5" t="n">
-        <v>10350.2</v>
+        <v>10338.6</v>
       </c>
       <c r="EV5" t="n">
-        <v>9275.8</v>
+        <v>9260.6</v>
+      </c>
+      <c r="EW5" t="n">
+        <v>9631.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2327,12 +2336,15 @@
         <v>173</v>
       </c>
       <c r="EV6" t="n">
-        <v>163.6</v>
+        <v>163.5</v>
+      </c>
+      <c r="EW6" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2786,11 +2798,14 @@
       </c>
       <c r="EV7" t="n">
         <v>18.8</v>
+      </c>
+      <c r="EW7" t="n">
+        <v>20.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3243,12 +3258,15 @@
         <v>155.6</v>
       </c>
       <c r="EV8" t="n">
-        <v>151</v>
+        <v>150.8</v>
+      </c>
+      <c r="EW8" t="n">
+        <v>178.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3702,11 +3720,14 @@
       </c>
       <c r="EV9" t="n">
         <v>83.6</v>
+      </c>
+      <c r="EW9" t="n">
+        <v>88.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4159,12 +4180,15 @@
         <v>1277.9</v>
       </c>
       <c r="EV10" t="n">
-        <v>1119.8</v>
+        <v>1124.6</v>
+      </c>
+      <c r="EW10" t="n">
+        <v>1178.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4617,12 +4641,15 @@
         <v>224.4</v>
       </c>
       <c r="EV11" t="n">
-        <v>210.8</v>
+        <v>210.4</v>
+      </c>
+      <c r="EW11" t="n">
+        <v>218.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5075,12 +5102,15 @@
         <v>119.2</v>
       </c>
       <c r="EV12" t="n">
-        <v>99.7</v>
+        <v>99</v>
+      </c>
+      <c r="EW12" t="n">
+        <v>99.6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5533,12 +5563,15 @@
         <v>36.9</v>
       </c>
       <c r="EV13" t="n">
-        <v>35.5</v>
+        <v>35.4</v>
+      </c>
+      <c r="EW13" t="n">
+        <v>34.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5691,10 +5724,11 @@
       <c r="ET14"/>
       <c r="EU14"/>
       <c r="EV14"/>
+      <c r="EW14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6147,12 +6181,15 @@
         <v>409.2</v>
       </c>
       <c r="EV15" t="n">
-        <v>401.5</v>
+        <v>400.7</v>
+      </c>
+      <c r="EW15" t="n">
+        <v>471.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6605,12 +6642,15 @@
         <v>340.6</v>
       </c>
       <c r="EV16" t="n">
-        <v>329</v>
+        <v>329.6</v>
+      </c>
+      <c r="EW16" t="n">
+        <v>353.7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6763,10 +6803,11 @@
       <c r="ET17"/>
       <c r="EU17"/>
       <c r="EV17"/>
+      <c r="EW17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7219,12 +7260,15 @@
         <v>62.5</v>
       </c>
       <c r="EV18" t="n">
-        <v>55.4</v>
+        <v>55.8</v>
+      </c>
+      <c r="EW18" t="n">
+        <v>57.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7677,12 +7721,15 @@
         <v>424.4</v>
       </c>
       <c r="EV19" t="n">
-        <v>406.2</v>
+        <v>407.1</v>
+      </c>
+      <c r="EW19" t="n">
+        <v>407.9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8135,12 +8182,15 @@
         <v>185.1</v>
       </c>
       <c r="EV20" t="n">
-        <v>173.2</v>
+        <v>169.3</v>
+      </c>
+      <c r="EW20" t="n">
+        <v>210.7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8593,12 +8643,15 @@
         <v>131.9</v>
       </c>
       <c r="EV21" t="n">
-        <v>114.9</v>
+        <v>115.3</v>
+      </c>
+      <c r="EW21" t="n">
+        <v>121.5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9052,11 +9105,14 @@
       </c>
       <c r="EV22" t="n">
         <v>96.5</v>
+      </c>
+      <c r="EW22" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9509,12 +9565,15 @@
         <v>154.3</v>
       </c>
       <c r="EV23" t="n">
-        <v>129.5</v>
+        <v>129.8</v>
+      </c>
+      <c r="EW23" t="n">
+        <v>153.6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -9968,11 +10027,14 @@
       </c>
       <c r="EV24" t="n">
         <v>130.4</v>
+      </c>
+      <c r="EW24" t="n">
+        <v>137.9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10425,12 +10487,15 @@
         <v>46.8</v>
       </c>
       <c r="EV25" t="n">
-        <v>40.5</v>
+        <v>40.2</v>
+      </c>
+      <c r="EW25" t="n">
+        <v>40.3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10883,12 +10948,15 @@
         <v>215.7</v>
       </c>
       <c r="EV26" t="n">
-        <v>202.2</v>
+        <v>199.4</v>
+      </c>
+      <c r="EW26" t="n">
+        <v>200.7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11342,11 +11410,14 @@
       </c>
       <c r="EV27" t="n">
         <v>214.7</v>
+      </c>
+      <c r="EW27" t="n">
+        <v>212.8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11800,11 +11871,14 @@
       </c>
       <c r="EV28" t="n">
         <v>267</v>
+      </c>
+      <c r="EW28" t="n">
+        <v>272.4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12258,11 +12332,14 @@
       </c>
       <c r="EV29" t="n">
         <v>176</v>
+      </c>
+      <c r="EW29" t="n">
+        <v>173</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12715,12 +12792,15 @@
         <v>99.8</v>
       </c>
       <c r="EV30" t="n">
-        <v>95.4</v>
+        <v>95.5</v>
+      </c>
+      <c r="EW30" t="n">
+        <v>99.6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -12873,10 +12953,11 @@
       <c r="ET31"/>
       <c r="EU31"/>
       <c r="EV31"/>
+      <c r="EW31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -13330,11 +13411,14 @@
       </c>
       <c r="EV32" t="n">
         <v>35.5</v>
+      </c>
+      <c r="EW32" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13787,12 +13871,15 @@
         <v>87.6</v>
       </c>
       <c r="EV33" t="n">
-        <v>78.6</v>
+        <v>78.7</v>
+      </c>
+      <c r="EW33" t="n">
+        <v>80.4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -14245,12 +14332,15 @@
         <v>73.1</v>
       </c>
       <c r="EV34" t="n">
-        <v>67.7</v>
+        <v>70.1</v>
+      </c>
+      <c r="EW34" t="n">
+        <v>74.7</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -14703,12 +14793,15 @@
         <v>39.7</v>
       </c>
       <c r="EV35" t="n">
-        <v>32.3</v>
+        <v>32.2</v>
+      </c>
+      <c r="EW35" t="n">
+        <v>32.1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -15162,11 +15255,14 @@
       </c>
       <c r="EV36" t="n">
         <v>264</v>
+      </c>
+      <c r="EW36" t="n">
+        <v>261.5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -15620,11 +15716,14 @@
       </c>
       <c r="EV37" t="n">
         <v>63.4</v>
+      </c>
+      <c r="EW37" t="n">
+        <v>72.1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -16078,11 +16177,14 @@
       </c>
       <c r="EV38" t="n">
         <v>563.1</v>
+      </c>
+      <c r="EW38" t="n">
+        <v>556.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16536,11 +16638,14 @@
       </c>
       <c r="EV39" t="n">
         <v>261.1</v>
+      </c>
+      <c r="EW39" t="n">
+        <v>310</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -16993,12 +17098,15 @@
         <v>33.9</v>
       </c>
       <c r="EV40" t="n">
-        <v>29</v>
+        <v>28.7</v>
+      </c>
+      <c r="EW40" t="n">
+        <v>30.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -17451,12 +17559,15 @@
         <v>359</v>
       </c>
       <c r="EV41" t="n">
-        <v>347.8</v>
+        <v>348.2</v>
+      </c>
+      <c r="EW41" t="n">
+        <v>350.8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -17909,12 +18020,15 @@
         <v>137.8</v>
       </c>
       <c r="EV42" t="n">
-        <v>124.8</v>
+        <v>126.1</v>
+      </c>
+      <c r="EW42" t="n">
+        <v>130.1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -18367,12 +18481,15 @@
         <v>141.3</v>
       </c>
       <c r="EV43" t="n">
-        <v>111</v>
+        <v>113.1</v>
+      </c>
+      <c r="EW43" t="n">
+        <v>113.8</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -18825,12 +18942,15 @@
         <v>305.2</v>
       </c>
       <c r="EV44" t="n">
-        <v>277.3</v>
+        <v>278.1</v>
+      </c>
+      <c r="EW44" t="n">
+        <v>284.5</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -19283,12 +19403,15 @@
         <v>28</v>
       </c>
       <c r="EV45" t="n">
-        <v>24</v>
+        <v>23.7</v>
+      </c>
+      <c r="EW45" t="n">
+        <v>23.7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -19741,12 +19864,15 @@
         <v>156.8</v>
       </c>
       <c r="EV46" t="n">
-        <v>146.5</v>
+        <v>146.3</v>
+      </c>
+      <c r="EW46" t="n">
+        <v>151.6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -20200,11 +20326,14 @@
       </c>
       <c r="EV47" t="n">
         <v>28.8</v>
+      </c>
+      <c r="EW47" t="n">
+        <v>30.1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -20658,11 +20787,14 @@
       </c>
       <c r="EV48" t="n">
         <v>164.1</v>
+      </c>
+      <c r="EW48" t="n">
+        <v>177.2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -21115,12 +21247,15 @@
         <v>1159.2</v>
       </c>
       <c r="EV49" t="n">
-        <v>1088</v>
+        <v>1085.5</v>
+      </c>
+      <c r="EW49" t="n">
+        <v>1100.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -21574,11 +21709,14 @@
       </c>
       <c r="EV50" t="n">
         <v>112.7</v>
+      </c>
+      <c r="EW50" t="n">
+        <v>120.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -22031,12 +22169,15 @@
         <v>28.9</v>
       </c>
       <c r="EV51" t="n">
-        <v>25.4</v>
+        <v>25.7</v>
+      </c>
+      <c r="EW51" t="n">
+        <v>25.9</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -22489,12 +22630,15 @@
         <v>315.2</v>
       </c>
       <c r="EV52" t="n">
-        <v>283.7</v>
+        <v>279.9</v>
+      </c>
+      <c r="EW52" t="n">
+        <v>294.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -22947,12 +23091,15 @@
         <v>253.3</v>
       </c>
       <c r="EV53" t="n">
-        <v>234.4</v>
+        <v>233.8</v>
+      </c>
+      <c r="EW53" t="n">
+        <v>218.3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -23406,11 +23553,14 @@
       </c>
       <c r="EV54" t="n">
         <v>51.6</v>
+      </c>
+      <c r="EW54" t="n">
+        <v>53.9</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -23864,11 +24014,14 @@
       </c>
       <c r="EV55" t="n">
         <v>170.6</v>
+      </c>
+      <c r="EW55" t="n">
+        <v>173.9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -24321,7 +24474,10 @@
         <v>28.9</v>
       </c>
       <c r="EV56" t="n">
-        <v>24.2</v>
+        <v>24.3</v>
+      </c>
+      <c r="EW56" t="n">
+        <v>24.7</v>
       </c>
     </row>
   </sheetData>
@@ -24759,10 +24915,13 @@
       <c r="EJ4" t="s">
         <v>151</v>
       </c>
+      <c r="EK4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -25176,15 +25335,18 @@
         <v>1.84448831669588</v>
       </c>
       <c r="EI5" t="n">
-        <v>1.62199312714777</v>
+        <v>1.50810014727539</v>
       </c>
       <c r="EJ5" t="n">
-        <v>1.97557194841744</v>
+        <v>1.80846736513451</v>
+      </c>
+      <c r="EK5" t="n">
+        <v>0.907328828120892</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -25601,12 +25763,15 @@
         <v>1.11046171829338</v>
       </c>
       <c r="EJ6" t="n">
-        <v>0.491400491400498</v>
+        <v>0.429975429975423</v>
+      </c>
+      <c r="EK6" t="n">
+        <v>0.478468899521538</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -26024,11 +26189,14 @@
       </c>
       <c r="EJ7" t="n">
         <v>-2.08333333333333</v>
+      </c>
+      <c r="EK7" t="n">
+        <v>-2.803738317757</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -26445,12 +26613,15 @@
         <v>0.516795865633064</v>
       </c>
       <c r="EJ8" t="n">
-        <v>0.132625994694953</v>
+        <v>0</v>
+      </c>
+      <c r="EK8" t="n">
+        <v>-3.09446254071661</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -26868,11 +27039,14 @@
       </c>
       <c r="EJ9" t="n">
         <v>1.21065375302663</v>
+      </c>
+      <c r="EK9" t="n">
+        <v>1.1441647597254</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -27289,12 +27463,15 @@
         <v>2.27290916366547</v>
       </c>
       <c r="EJ10" t="n">
-        <v>4.24501954943213</v>
+        <v>4.69186371253024</v>
+      </c>
+      <c r="EK10" t="n">
+        <v>5.11241970021415</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -27711,12 +27888,15 @@
         <v>4.4206607724523</v>
       </c>
       <c r="EJ11" t="n">
-        <v>4.82347090999502</v>
+        <v>4.62456489308802</v>
+      </c>
+      <c r="EK11" t="n">
+        <v>4.13891531874406</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -28133,12 +28313,15 @@
         <v>2.31759656652361</v>
       </c>
       <c r="EJ12" t="n">
-        <v>1.94274028629857</v>
+        <v>1.22699386503068</v>
+      </c>
+      <c r="EK12" t="n">
+        <v>-0.895522388059707</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -28555,12 +28738,15 @@
         <v>2.78551532033426</v>
       </c>
       <c r="EJ13" t="n">
-        <v>3.19767441860466</v>
+        <v>2.90697674418605</v>
+      </c>
+      <c r="EK13" t="n">
+        <v>2.66272189349114</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -28701,10 +28887,11 @@
       <c r="EH14"/>
       <c r="EI14"/>
       <c r="EJ14"/>
+      <c r="EK14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -29121,12 +29308,15 @@
         <v>1.23701138050469</v>
       </c>
       <c r="EJ15" t="n">
-        <v>0.904749937170149</v>
+        <v>0.703694395576795</v>
+      </c>
+      <c r="EK15" t="n">
+        <v>1.1810178226326</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -29543,12 +29733,15 @@
         <v>2.62127146730944</v>
       </c>
       <c r="EJ16" t="n">
-        <v>4.24588086185044</v>
+        <v>4.43599493029151</v>
+      </c>
+      <c r="EK16" t="n">
+        <v>2.81976744186046</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -29689,10 +29882,11 @@
       <c r="EH17"/>
       <c r="EI17"/>
       <c r="EJ17"/>
+      <c r="EK17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -30109,12 +30303,15 @@
         <v>5.75296108291032</v>
       </c>
       <c r="EJ18" t="n">
-        <v>7.15667311411993</v>
+        <v>7.93036750483559</v>
+      </c>
+      <c r="EK18" t="n">
+        <v>7.27611940298507</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -30531,12 +30728,15 @@
         <v>1.77458033573141</v>
       </c>
       <c r="EJ19" t="n">
-        <v>5.80880437613962</v>
+        <v>6.04324042719459</v>
+      </c>
+      <c r="EK19" t="n">
+        <v>6.08582574772431</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -30953,12 +31153,15 @@
         <v>-1.95974576271186</v>
       </c>
       <c r="EJ20" t="n">
-        <v>2.48520710059171</v>
+        <v>0.177514792899415</v>
+      </c>
+      <c r="EK20" t="n">
+        <v>1.83663605606572</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -31375,12 +31578,15 @@
         <v>-1.19850187265919</v>
       </c>
       <c r="EJ21" t="n">
-        <v>-1.7948717948718</v>
+        <v>-1.45299145299146</v>
+      </c>
+      <c r="EK21" t="n">
+        <v>-0.0822368421052585</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -31798,11 +32004,14 @@
       </c>
       <c r="EJ22" t="n">
         <v>-0.309917355371898</v>
+      </c>
+      <c r="EK22" t="n">
+        <v>-0.379506641366229</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -32219,12 +32428,15 @@
         <v>0.586701434159065</v>
       </c>
       <c r="EJ23" t="n">
-        <v>1.09289617486339</v>
+        <v>1.32708821233413</v>
+      </c>
+      <c r="EK23" t="n">
+        <v>0.986193293885602</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -32642,11 +32854,14 @@
       </c>
       <c r="EJ24" t="n">
         <v>0.539707016191224</v>
+      </c>
+      <c r="EK24" t="n">
+        <v>0.290909090909095</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -33063,12 +33278,15 @@
         <v>-0.847457627118656</v>
       </c>
       <c r="EJ25" t="n">
-        <v>0.997506234413979</v>
+        <v>0.249376558603513</v>
+      </c>
+      <c r="EK25" t="n">
+        <v>4.40414507772021</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -33485,12 +33703,15 @@
         <v>3.75180375180377</v>
       </c>
       <c r="EJ26" t="n">
-        <v>3.63915940543309</v>
+        <v>2.20399794976933</v>
+      </c>
+      <c r="EK26" t="n">
+        <v>2.03355363497711</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -33908,11 +34129,14 @@
       </c>
       <c r="EJ27" t="n">
         <v>1.36921624173748</v>
+      </c>
+      <c r="EK27" t="n">
+        <v>1.38161029061458</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -34330,11 +34554,14 @@
       </c>
       <c r="EJ28" t="n">
         <v>3.44827586206896</v>
+      </c>
+      <c r="EK28" t="n">
+        <v>4.00916380297824</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -34752,11 +34979,14 @@
       </c>
       <c r="EJ29" t="n">
         <v>2.92397660818713</v>
+      </c>
+      <c r="EK29" t="n">
+        <v>2.91493158834028</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -35173,12 +35403,15 @@
         <v>1.94075587334013</v>
       </c>
       <c r="EJ30" t="n">
-        <v>1.59744408945685</v>
+        <v>1.70394036208732</v>
+      </c>
+      <c r="EK30" t="n">
+        <v>1.63265306122448</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -35319,10 +35552,11 @@
       <c r="EH31"/>
       <c r="EI31"/>
       <c r="EJ31"/>
+      <c r="EK31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -35740,11 +35974,14 @@
       </c>
       <c r="EJ32" t="n">
         <v>1.71919770773637</v>
+      </c>
+      <c r="EK32" t="n">
+        <v>1.64835164835163</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -36161,12 +36398,15 @@
         <v>-3.3112582781457</v>
       </c>
       <c r="EJ33" t="n">
-        <v>-0.506329113924058</v>
+        <v>-0.379746835443052</v>
+      </c>
+      <c r="EK33" t="n">
+        <v>-0.863131935881614</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -36583,12 +36823,15 @@
         <v>1.24653739612187</v>
       </c>
       <c r="EJ34" t="n">
-        <v>1.80451127819549</v>
+        <v>5.41353383458646</v>
+      </c>
+      <c r="EK34" t="n">
+        <v>12.6696832579186</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -37005,12 +37248,15 @@
         <v>2.84974093264247</v>
       </c>
       <c r="EJ35" t="n">
-        <v>-1.22324159021404</v>
+        <v>-1.52905198776756</v>
+      </c>
+      <c r="EK35" t="n">
+        <v>-1.23076923076923</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -37428,11 +37674,14 @@
       </c>
       <c r="EJ36" t="n">
         <v>2.60396424407306</v>
+      </c>
+      <c r="EK36" t="n">
+        <v>2.26828314430974</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -37850,11 +38099,14 @@
       </c>
       <c r="EJ37" t="n">
         <v>-0.626959247648901</v>
+      </c>
+      <c r="EK37" t="n">
+        <v>2.41477272727271</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -38272,11 +38524,14 @@
       </c>
       <c r="EJ38" t="n">
         <v>2.53095411507647</v>
+      </c>
+      <c r="EK38" t="n">
+        <v>2.50552689756817</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -38694,11 +38949,14 @@
       </c>
       <c r="EJ39" t="n">
         <v>1.95236235845373</v>
+      </c>
+      <c r="EK39" t="n">
+        <v>1.90664036817881</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -39115,12 +39373,15 @@
         <v>5.27950310559005</v>
       </c>
       <c r="EJ40" t="n">
-        <v>6.22710622710622</v>
+        <v>5.12820512820512</v>
+      </c>
+      <c r="EK40" t="n">
+        <v>9.60854092526689</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -39537,12 +39798,15 @@
         <v>-1.10192837465565</v>
       </c>
       <c r="EJ41" t="n">
-        <v>-1.19318181818183</v>
+        <v>-1.07954545454546</v>
+      </c>
+      <c r="EK41" t="n">
+        <v>-0.707613925842061</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -39959,12 +40223,15 @@
         <v>1.17474302496331</v>
       </c>
       <c r="EJ42" t="n">
-        <v>1.05263157894738</v>
+        <v>2.10526315789473</v>
+      </c>
+      <c r="EK42" t="n">
+        <v>-0.230061349693238</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -40381,12 +40648,15 @@
         <v>0.712758374910905</v>
       </c>
       <c r="EJ43" t="n">
-        <v>1.00090991810737</v>
+        <v>2.91173794358507</v>
+      </c>
+      <c r="EK43" t="n">
+        <v>1.51650312221231</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -40803,12 +41073,15 @@
         <v>1.97126628800534</v>
       </c>
       <c r="EJ44" t="n">
-        <v>1.093693036821</v>
+        <v>1.3853445133066</v>
+      </c>
+      <c r="EK44" t="n">
+        <v>0.779312787814378</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -41225,12 +41498,15 @@
         <v>2.94117647058824</v>
       </c>
       <c r="EJ45" t="n">
-        <v>5.26315789473685</v>
+        <v>3.94736842105264</v>
+      </c>
+      <c r="EK45" t="n">
+        <v>3.49344978165941</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -41647,12 +41923,15 @@
         <v>1.35746606334843</v>
       </c>
       <c r="EJ46" t="n">
-        <v>1.03448275862069</v>
+        <v>0.896551724137939</v>
+      </c>
+      <c r="EK46" t="n">
+        <v>1.20160213618158</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -42070,11 +42349,14 @@
       </c>
       <c r="EJ47" t="n">
         <v>2.12765957446808</v>
+      </c>
+      <c r="EK47" t="n">
+        <v>1.00671140939599</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -42492,11 +42774,14 @@
       </c>
       <c r="EJ48" t="n">
         <v>-2.66903914590747</v>
+      </c>
+      <c r="EK48" t="n">
+        <v>-2.47660979636764</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -42913,12 +43198,15 @@
         <v>2.57499336341918</v>
       </c>
       <c r="EJ49" t="n">
-        <v>2.98154283009938</v>
+        <v>2.74491244675816</v>
+      </c>
+      <c r="EK49" t="n">
+        <v>1.0741828865222</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -43336,11 +43624,14 @@
       </c>
       <c r="EJ50" t="n">
         <v>5.22875816993464</v>
+      </c>
+      <c r="EK50" t="n">
+        <v>4.60069444444445</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -43757,12 +44048,15 @@
         <v>-0.687285223367707</v>
       </c>
       <c r="EJ51" t="n">
-        <v>-0.000000000000013987061727561</v>
+        <v>1.18110236220471</v>
+      </c>
+      <c r="EK51" t="n">
+        <v>1.171875</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -44179,12 +44473,15 @@
         <v>2.60416666666667</v>
       </c>
       <c r="EJ52" t="n">
-        <v>2.45576020223908</v>
+        <v>1.08342361863489</v>
+      </c>
+      <c r="EK52" t="n">
+        <v>1.37835975189524</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -44601,12 +44898,15 @@
         <v>-1.32450331125827</v>
       </c>
       <c r="EJ53" t="n">
-        <v>0.55770055770055</v>
+        <v>0.300300300300295</v>
+      </c>
+      <c r="EK53" t="n">
+        <v>-1.62235241099594</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -45024,11 +45324,14 @@
       </c>
       <c r="EJ54" t="n">
         <v>-0.578034682080947</v>
+      </c>
+      <c r="EK54" t="n">
+        <v>-2.70758122743682</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -45446,11 +45749,14 @@
       </c>
       <c r="EJ55" t="n">
         <v>0.293944738389166</v>
+      </c>
+      <c r="EK55" t="n">
+        <v>4.00717703349282</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -45867,7 +46173,10 @@
         <v>2.4822695035461</v>
       </c>
       <c r="EJ56" t="n">
-        <v>1.255230125523</v>
+        <v>1.67364016736401</v>
+      </c>
+      <c r="EK56" t="n">
+        <v>-1.98412698412698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on October 22, 2024
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t xml:space="preserve">08/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1419,10 +1422,13 @@
       <c r="EW4" t="s">
         <v>152</v>
       </c>
+      <c r="EX4" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1875,15 +1881,18 @@
         <v>10338.6</v>
       </c>
       <c r="EV5" t="n">
-        <v>9260.6</v>
+        <v>9272.6</v>
       </c>
       <c r="EW5" t="n">
-        <v>9631.1</v>
+        <v>9723.2</v>
+      </c>
+      <c r="EX5" t="n">
+        <v>10832.9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2340,11 +2349,14 @@
       </c>
       <c r="EW6" t="n">
         <v>168</v>
+      </c>
+      <c r="EX6" t="n">
+        <v>174.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2801,11 +2813,14 @@
       </c>
       <c r="EW7" t="n">
         <v>20.8</v>
+      </c>
+      <c r="EX7" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3261,12 +3276,15 @@
         <v>150.8</v>
       </c>
       <c r="EW8" t="n">
-        <v>178.5</v>
+        <v>179.6</v>
+      </c>
+      <c r="EX8" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3723,11 +3741,14 @@
       </c>
       <c r="EW9" t="n">
         <v>88.4</v>
+      </c>
+      <c r="EX9" t="n">
+        <v>102.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4183,12 +4204,15 @@
         <v>1124.6</v>
       </c>
       <c r="EW10" t="n">
-        <v>1178.1</v>
+        <v>1173.7</v>
+      </c>
+      <c r="EX10" t="n">
+        <v>1242</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4644,12 +4668,15 @@
         <v>210.4</v>
       </c>
       <c r="EW11" t="n">
-        <v>218.9</v>
+        <v>219.4</v>
+      </c>
+      <c r="EX11" t="n">
+        <v>238.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5106,11 +5133,14 @@
       </c>
       <c r="EW12" t="n">
         <v>99.6</v>
+      </c>
+      <c r="EX12" t="n">
+        <v>121.9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5566,12 +5596,15 @@
         <v>35.4</v>
       </c>
       <c r="EW13" t="n">
-        <v>34.7</v>
+        <v>34.8</v>
+      </c>
+      <c r="EX13" t="n">
+        <v>39.6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5725,10 +5758,11 @@
       <c r="EU14"/>
       <c r="EV14"/>
       <c r="EW14"/>
+      <c r="EX14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6184,12 +6218,15 @@
         <v>400.7</v>
       </c>
       <c r="EW15" t="n">
-        <v>471.2</v>
+        <v>471</v>
+      </c>
+      <c r="EX15" t="n">
+        <v>499.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6645,12 +6682,15 @@
         <v>329.6</v>
       </c>
       <c r="EW16" t="n">
-        <v>353.7</v>
+        <v>353</v>
+      </c>
+      <c r="EX16" t="n">
+        <v>357.2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6804,10 +6844,11 @@
       <c r="EU17"/>
       <c r="EV17"/>
       <c r="EW17"/>
+      <c r="EX17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7263,12 +7304,15 @@
         <v>55.8</v>
       </c>
       <c r="EW18" t="n">
-        <v>57.5</v>
+        <v>58.4</v>
+      </c>
+      <c r="EX18" t="n">
+        <v>66.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7724,12 +7768,15 @@
         <v>407.1</v>
       </c>
       <c r="EW19" t="n">
-        <v>407.9</v>
+        <v>417.1</v>
+      </c>
+      <c r="EX19" t="n">
+        <v>478</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8185,12 +8232,15 @@
         <v>169.3</v>
       </c>
       <c r="EW20" t="n">
-        <v>210.7</v>
+        <v>212</v>
+      </c>
+      <c r="EX20" t="n">
+        <v>232.7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8646,12 +8696,15 @@
         <v>115.3</v>
       </c>
       <c r="EW21" t="n">
-        <v>121.5</v>
+        <v>120.6</v>
+      </c>
+      <c r="EX21" t="n">
+        <v>141.8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9108,11 +9161,14 @@
       </c>
       <c r="EW22" t="n">
         <v>105</v>
+      </c>
+      <c r="EX22" t="n">
+        <v>132.7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9569,11 +9625,14 @@
       </c>
       <c r="EW23" t="n">
         <v>153.6</v>
+      </c>
+      <c r="EX23" t="n">
+        <v>164.3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10030,11 +10089,14 @@
       </c>
       <c r="EW24" t="n">
         <v>137.9</v>
+      </c>
+      <c r="EX24" t="n">
+        <v>146.4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10490,12 +10552,15 @@
         <v>40.2</v>
       </c>
       <c r="EW25" t="n">
-        <v>40.3</v>
+        <v>40.4</v>
+      </c>
+      <c r="EX25" t="n">
+        <v>50.7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -10952,11 +11017,14 @@
       </c>
       <c r="EW26" t="n">
         <v>200.7</v>
+      </c>
+      <c r="EX26" t="n">
+        <v>222.2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11413,11 +11481,14 @@
       </c>
       <c r="EW27" t="n">
         <v>212.8</v>
+      </c>
+      <c r="EX27" t="n">
+        <v>244.6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11874,11 +11945,14 @@
       </c>
       <c r="EW28" t="n">
         <v>272.4</v>
+      </c>
+      <c r="EX28" t="n">
+        <v>322.7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12335,11 +12409,14 @@
       </c>
       <c r="EW29" t="n">
         <v>173</v>
+      </c>
+      <c r="EX29" t="n">
+        <v>204.4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12795,12 +12872,15 @@
         <v>95.5</v>
       </c>
       <c r="EW30" t="n">
-        <v>99.6</v>
+        <v>100.1</v>
+      </c>
+      <c r="EX30" t="n">
+        <v>105.3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -12954,10 +13034,11 @@
       <c r="EU31"/>
       <c r="EV31"/>
       <c r="EW31"/>
+      <c r="EX31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -13414,11 +13495,14 @@
       </c>
       <c r="EW32" t="n">
         <v>37</v>
+      </c>
+      <c r="EX32" t="n">
+        <v>43.3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13874,12 +13958,15 @@
         <v>78.7</v>
       </c>
       <c r="EW33" t="n">
-        <v>80.4</v>
+        <v>80.5</v>
+      </c>
+      <c r="EX33" t="n">
+        <v>93.3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -14335,12 +14422,15 @@
         <v>70.1</v>
       </c>
       <c r="EW34" t="n">
-        <v>74.7</v>
+        <v>75.2</v>
+      </c>
+      <c r="EX34" t="n">
+        <v>87.8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -14796,12 +14886,15 @@
         <v>32.2</v>
       </c>
       <c r="EW35" t="n">
-        <v>32.1</v>
+        <v>33.9</v>
+      </c>
+      <c r="EX35" t="n">
+        <v>44.5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -15258,11 +15351,14 @@
       </c>
       <c r="EW36" t="n">
         <v>261.5</v>
+      </c>
+      <c r="EX36" t="n">
+        <v>306</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -15718,12 +15814,15 @@
         <v>63.4</v>
       </c>
       <c r="EW37" t="n">
-        <v>72.1</v>
+        <v>71.9</v>
+      </c>
+      <c r="EX37" t="n">
+        <v>79.9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -16180,11 +16279,14 @@
       </c>
       <c r="EW38" t="n">
         <v>556.4</v>
+      </c>
+      <c r="EX38" t="n">
+        <v>663.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16641,11 +16743,14 @@
       </c>
       <c r="EW39" t="n">
         <v>310</v>
+      </c>
+      <c r="EX39" t="n">
+        <v>337.6</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -17101,12 +17206,15 @@
         <v>28.7</v>
       </c>
       <c r="EW40" t="n">
-        <v>30.8</v>
+        <v>31</v>
+      </c>
+      <c r="EX40" t="n">
+        <v>40.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -17562,12 +17670,15 @@
         <v>348.2</v>
       </c>
       <c r="EW41" t="n">
-        <v>350.8</v>
+        <v>352.5</v>
+      </c>
+      <c r="EX41" t="n">
+        <v>389.8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -18023,12 +18134,15 @@
         <v>126.1</v>
       </c>
       <c r="EW42" t="n">
-        <v>130.1</v>
+        <v>131.9</v>
+      </c>
+      <c r="EX42" t="n">
+        <v>151.2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -18484,12 +18598,15 @@
         <v>113.1</v>
       </c>
       <c r="EW43" t="n">
-        <v>113.8</v>
+        <v>114.6</v>
+      </c>
+      <c r="EX43" t="n">
+        <v>128</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -18945,12 +19062,15 @@
         <v>278.1</v>
       </c>
       <c r="EW44" t="n">
-        <v>284.5</v>
+        <v>283.2</v>
+      </c>
+      <c r="EX44" t="n">
+        <v>330.5</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -19406,12 +19526,15 @@
         <v>23.7</v>
       </c>
       <c r="EW45" t="n">
-        <v>23.7</v>
+        <v>23.6</v>
+      </c>
+      <c r="EX45" t="n">
+        <v>29.4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -19867,12 +19990,15 @@
         <v>146.3</v>
       </c>
       <c r="EW46" t="n">
-        <v>151.6</v>
+        <v>152.3</v>
+      </c>
+      <c r="EX46" t="n">
+        <v>163.2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -20328,12 +20454,15 @@
         <v>28.8</v>
       </c>
       <c r="EW47" t="n">
-        <v>30.1</v>
+        <v>29.9</v>
+      </c>
+      <c r="EX47" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -20790,11 +20919,14 @@
       </c>
       <c r="EW48" t="n">
         <v>177.2</v>
+      </c>
+      <c r="EX48" t="n">
+        <v>200.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -21250,12 +21382,15 @@
         <v>1085.5</v>
       </c>
       <c r="EW49" t="n">
-        <v>1100.9</v>
+        <v>1108.3</v>
+      </c>
+      <c r="EX49" t="n">
+        <v>1159.7</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -21712,11 +21847,14 @@
       </c>
       <c r="EW50" t="n">
         <v>120.5</v>
+      </c>
+      <c r="EX50" t="n">
+        <v>134.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -22173,11 +22311,14 @@
       </c>
       <c r="EW51" t="n">
         <v>25.9</v>
+      </c>
+      <c r="EX51" t="n">
+        <v>31.4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -22633,12 +22774,15 @@
         <v>279.9</v>
       </c>
       <c r="EW52" t="n">
-        <v>294.2</v>
+        <v>292.7</v>
+      </c>
+      <c r="EX52" t="n">
+        <v>325.1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -23094,12 +23238,15 @@
         <v>233.8</v>
       </c>
       <c r="EW53" t="n">
-        <v>218.3</v>
+        <v>222.3</v>
+      </c>
+      <c r="EX53" t="n">
+        <v>233.1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -23555,12 +23702,15 @@
         <v>51.6</v>
       </c>
       <c r="EW54" t="n">
-        <v>53.9</v>
+        <v>53.8</v>
+      </c>
+      <c r="EX54" t="n">
+        <v>59.4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -24017,11 +24167,14 @@
       </c>
       <c r="EW55" t="n">
         <v>173.9</v>
+      </c>
+      <c r="EX55" t="n">
+        <v>206.2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -24477,7 +24630,10 @@
         <v>24.3</v>
       </c>
       <c r="EW56" t="n">
-        <v>24.7</v>
+        <v>25.6</v>
+      </c>
+      <c r="EX56" t="n">
+        <v>29.6</v>
       </c>
     </row>
   </sheetData>
@@ -24918,10 +25074,13 @@
       <c r="EK4" t="s">
         <v>152</v>
       </c>
+      <c r="EL4" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -25338,15 +25497,18 @@
         <v>1.50810014727539</v>
       </c>
       <c r="EJ5" t="n">
-        <v>1.80846736513451</v>
+        <v>1.94039203614734</v>
       </c>
       <c r="EK5" t="n">
-        <v>0.907328828120892</v>
+        <v>1.87228246634188</v>
+      </c>
+      <c r="EL5" t="n">
+        <v>1.58859661461996</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -25767,11 +25929,14 @@
       </c>
       <c r="EK6" t="n">
         <v>0.478468899521538</v>
+      </c>
+      <c r="EL6" t="n">
+        <v>0.577367205542725</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -26192,11 +26357,14 @@
       </c>
       <c r="EK7" t="n">
         <v>-2.803738317757</v>
+      </c>
+      <c r="EL7" t="n">
+        <v>-4.76190476190476</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -26616,12 +26784,15 @@
         <v>0</v>
       </c>
       <c r="EK8" t="n">
-        <v>-3.09446254071661</v>
+        <v>-2.49728555917481</v>
+      </c>
+      <c r="EL8" t="n">
+        <v>0.857286938981336</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -27042,11 +27213,14 @@
       </c>
       <c r="EK9" t="n">
         <v>1.1441647597254</v>
+      </c>
+      <c r="EL9" t="n">
+        <v>1.18694362017804</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -27466,12 +27640,15 @@
         <v>4.69186371253024</v>
       </c>
       <c r="EK10" t="n">
-        <v>5.11241970021415</v>
+        <v>4.71984296930765</v>
+      </c>
+      <c r="EL10" t="n">
+        <v>3.47413146713322</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -27891,12 +28068,15 @@
         <v>4.62456489308802</v>
       </c>
       <c r="EK11" t="n">
-        <v>4.13891531874406</v>
+        <v>4.37678401522361</v>
+      </c>
+      <c r="EL11" t="n">
+        <v>4.23765836609874</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -28317,11 +28497,14 @@
       </c>
       <c r="EK12" t="n">
         <v>-0.895522388059707</v>
+      </c>
+      <c r="EL12" t="n">
+        <v>-0.651996740016309</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -28741,12 +28924,15 @@
         <v>2.90697674418605</v>
       </c>
       <c r="EK13" t="n">
-        <v>2.66272189349114</v>
+        <v>2.95857988165681</v>
+      </c>
+      <c r="EL13" t="n">
+        <v>2.32558139534882</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -28888,10 +29074,11 @@
       <c r="EI14"/>
       <c r="EJ14"/>
       <c r="EK14"/>
+      <c r="EL14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -29311,12 +29498,15 @@
         <v>0.703694395576795</v>
       </c>
       <c r="EK15" t="n">
-        <v>1.1810178226326</v>
+        <v>1.13807171999141</v>
+      </c>
+      <c r="EL15" t="n">
+        <v>2.10504802779482</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -29736,12 +29926,15 @@
         <v>4.43599493029151</v>
       </c>
       <c r="EK16" t="n">
-        <v>2.81976744186046</v>
+        <v>2.61627906976744</v>
+      </c>
+      <c r="EL16" t="n">
+        <v>1.85343598517251</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -29883,10 +30076,11 @@
       <c r="EI17"/>
       <c r="EJ17"/>
       <c r="EK17"/>
+      <c r="EL17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -30306,12 +30500,15 @@
         <v>7.93036750483559</v>
       </c>
       <c r="EK18" t="n">
-        <v>7.27611940298507</v>
+        <v>8.95522388059701</v>
+      </c>
+      <c r="EL18" t="n">
+        <v>7.25806451612903</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -30731,12 +30928,15 @@
         <v>6.04324042719459</v>
       </c>
       <c r="EK19" t="n">
-        <v>6.08582574772431</v>
+        <v>8.47854356306891</v>
+      </c>
+      <c r="EL19" t="n">
+        <v>8.43920145190562</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -31156,12 +31356,15 @@
         <v>0.177514792899415</v>
       </c>
       <c r="EK20" t="n">
-        <v>1.83663605606572</v>
+        <v>2.46495891735137</v>
+      </c>
+      <c r="EL20" t="n">
+        <v>1.26196692776328</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -31581,12 +31784,15 @@
         <v>-1.45299145299146</v>
       </c>
       <c r="EK21" t="n">
-        <v>-0.0822368421052585</v>
+        <v>-0.822368421052632</v>
+      </c>
+      <c r="EL21" t="n">
+        <v>-0.839160839160831</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -32007,11 +32213,14 @@
       </c>
       <c r="EK22" t="n">
         <v>-0.379506641366229</v>
+      </c>
+      <c r="EL22" t="n">
+        <v>0.22658610271902</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -32432,11 +32641,14 @@
       </c>
       <c r="EK23" t="n">
         <v>0.986193293885602</v>
+      </c>
+      <c r="EL23" t="n">
+        <v>0.366524129505206</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -32857,11 +33069,14 @@
       </c>
       <c r="EK24" t="n">
         <v>0.290909090909095</v>
+      </c>
+      <c r="EL24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -33281,12 +33496,15 @@
         <v>0.249376558603513</v>
       </c>
       <c r="EK25" t="n">
-        <v>4.40414507772021</v>
+        <v>4.66321243523315</v>
+      </c>
+      <c r="EL25" t="n">
+        <v>4.53608247422681</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -33707,11 +33925,14 @@
       </c>
       <c r="EK26" t="n">
         <v>2.03355363497711</v>
+      </c>
+      <c r="EL26" t="n">
+        <v>1.55393053016454</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -34132,11 +34353,14 @@
       </c>
       <c r="EK27" t="n">
         <v>1.38161029061458</v>
+      </c>
+      <c r="EL27" t="n">
+        <v>1.40961857379768</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -34557,11 +34781,14 @@
       </c>
       <c r="EK28" t="n">
         <v>4.00916380297824</v>
+      </c>
+      <c r="EL28" t="n">
+        <v>4.13036463375283</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -34982,11 +35209,14 @@
       </c>
       <c r="EK29" t="n">
         <v>2.91493158834028</v>
+      </c>
+      <c r="EL29" t="n">
+        <v>2.8169014084507</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -35406,12 +35636,15 @@
         <v>1.70394036208732</v>
       </c>
       <c r="EK30" t="n">
-        <v>1.63265306122448</v>
+        <v>2.14285714285714</v>
+      </c>
+      <c r="EL30" t="n">
+        <v>0.765550239234447</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -35553,10 +35786,11 @@
       <c r="EI31"/>
       <c r="EJ31"/>
       <c r="EK31"/>
+      <c r="EL31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -35977,11 +36211,14 @@
       </c>
       <c r="EK32" t="n">
         <v>1.64835164835163</v>
+      </c>
+      <c r="EL32" t="n">
+        <v>2.12264150943396</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -36401,12 +36638,15 @@
         <v>-0.379746835443052</v>
       </c>
       <c r="EK33" t="n">
-        <v>-0.863131935881614</v>
+        <v>-0.739827373612817</v>
+      </c>
+      <c r="EL33" t="n">
+        <v>0.430570505920351</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -36826,12 +37066,15 @@
         <v>5.41353383458646</v>
       </c>
       <c r="EK34" t="n">
-        <v>12.6696832579186</v>
+        <v>13.4238310708899</v>
+      </c>
+      <c r="EL34" t="n">
+        <v>6.03864734299519</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -37251,12 +37494,15 @@
         <v>-1.52905198776756</v>
       </c>
       <c r="EK35" t="n">
-        <v>-1.23076923076923</v>
+        <v>4.3076923076923</v>
+      </c>
+      <c r="EL35" t="n">
+        <v>0.451467268623031</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -37677,11 +37923,14 @@
       </c>
       <c r="EK36" t="n">
         <v>2.26828314430974</v>
+      </c>
+      <c r="EL36" t="n">
+        <v>2.44392366923335</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -38101,12 +38350,15 @@
         <v>-0.626959247648901</v>
       </c>
       <c r="EK37" t="n">
-        <v>2.41477272727271</v>
+        <v>2.13068181818182</v>
+      </c>
+      <c r="EL37" t="n">
+        <v>3.36351875808539</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -38527,11 +38779,14 @@
       </c>
       <c r="EK38" t="n">
         <v>2.50552689756817</v>
+      </c>
+      <c r="EL38" t="n">
+        <v>2.44090838869148</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -38952,11 +39207,14 @@
       </c>
       <c r="EK39" t="n">
         <v>1.90664036817881</v>
+      </c>
+      <c r="EL39" t="n">
+        <v>1.93236714975846</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -39376,12 +39634,15 @@
         <v>5.12820512820512</v>
       </c>
       <c r="EK40" t="n">
-        <v>9.60854092526689</v>
+        <v>10.3202846975089</v>
+      </c>
+      <c r="EL40" t="n">
+        <v>10.2702702702703</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -39801,12 +40062,15 @@
         <v>-1.07954545454546</v>
       </c>
       <c r="EK41" t="n">
-        <v>-0.707613925842061</v>
+        <v>-0.226436456269463</v>
+      </c>
+      <c r="EL41" t="n">
+        <v>1.32570834416427</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -40226,12 +40490,15 @@
         <v>2.10526315789473</v>
       </c>
       <c r="EK42" t="n">
-        <v>-0.230061349693238</v>
+        <v>1.15030674846628</v>
+      </c>
+      <c r="EL42" t="n">
+        <v>0.799999999999992</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -40651,12 +40918,15 @@
         <v>2.91173794358507</v>
       </c>
       <c r="EK43" t="n">
-        <v>1.51650312221231</v>
+        <v>2.23015165031222</v>
+      </c>
+      <c r="EL43" t="n">
+        <v>1.10584518167457</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -41076,12 +41346,15 @@
         <v>1.3853445133066</v>
       </c>
       <c r="EK44" t="n">
-        <v>0.779312787814378</v>
+        <v>0.318809776833148</v>
+      </c>
+      <c r="EL44" t="n">
+        <v>1.19412124923455</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -41501,12 +41774,15 @@
         <v>3.94736842105264</v>
       </c>
       <c r="EK45" t="n">
-        <v>3.49344978165941</v>
+        <v>3.05676855895198</v>
+      </c>
+      <c r="EL45" t="n">
+        <v>5.37634408602151</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -41926,12 +42202,15 @@
         <v>0.896551724137939</v>
       </c>
       <c r="EK46" t="n">
-        <v>1.20160213618158</v>
+        <v>1.66889185580774</v>
+      </c>
+      <c r="EL46" t="n">
+        <v>2.06378986866793</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -42351,12 +42630,15 @@
         <v>2.12765957446808</v>
       </c>
       <c r="EK47" t="n">
-        <v>1.00671140939599</v>
+        <v>0.335570469798663</v>
+      </c>
+      <c r="EL47" t="n">
+        <v>-0.537634408602158</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -42777,11 +43059,14 @@
       </c>
       <c r="EK48" t="n">
         <v>-2.47660979636764</v>
+      </c>
+      <c r="EL48" t="n">
+        <v>-2.38558909444986</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -43201,12 +43486,15 @@
         <v>2.74491244675816</v>
       </c>
       <c r="EK49" t="n">
-        <v>1.0741828865222</v>
+        <v>1.75358060962173</v>
+      </c>
+      <c r="EL49" t="n">
+        <v>-0.00862217623727445</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -43627,11 +43915,14 @@
       </c>
       <c r="EK50" t="n">
         <v>4.60069444444445</v>
+      </c>
+      <c r="EL50" t="n">
+        <v>4.10216718266255</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -44052,11 +44343,14 @@
       </c>
       <c r="EK51" t="n">
         <v>1.171875</v>
+      </c>
+      <c r="EL51" t="n">
+        <v>0.641025641025627</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -44476,12 +44770,15 @@
         <v>1.08342361863489</v>
       </c>
       <c r="EK52" t="n">
-        <v>1.37835975189524</v>
+        <v>0.861474844934528</v>
+      </c>
+      <c r="EL52" t="n">
+        <v>1.84837092731829</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -44901,12 +45198,15 @@
         <v>0.300300300300295</v>
       </c>
       <c r="EK53" t="n">
-        <v>-1.62235241099594</v>
+        <v>0.180261378999552</v>
+      </c>
+      <c r="EL53" t="n">
+        <v>-0.427167876975651</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -45326,12 +45626,15 @@
         <v>-0.578034682080947</v>
       </c>
       <c r="EK54" t="n">
-        <v>-2.70758122743682</v>
+        <v>-2.88808664259929</v>
+      </c>
+      <c r="EL54" t="n">
+        <v>-2.78232405891979</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -45752,11 +46055,14 @@
       </c>
       <c r="EK55" t="n">
         <v>4.00717703349282</v>
+      </c>
+      <c r="EL55" t="n">
+        <v>0.145701796988835</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -46176,7 +46482,10 @@
         <v>1.67364016736401</v>
       </c>
       <c r="EK56" t="n">
-        <v>-1.98412698412698</v>
+        <v>1.58730158730158</v>
+      </c>
+      <c r="EL56" t="n">
+        <v>-1.33333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on November 19, 2024
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -475,6 +475,9 @@
   </si>
   <si>
     <t xml:space="preserve">09/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1425,10 +1428,13 @@
       <c r="EX4" t="s">
         <v>153</v>
       </c>
+      <c r="EY4" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1884,15 +1890,18 @@
         <v>9272.6</v>
       </c>
       <c r="EW5" t="n">
-        <v>9723.2</v>
+        <v>9729.9</v>
       </c>
       <c r="EX5" t="n">
-        <v>10832.9</v>
+        <v>10806</v>
+      </c>
+      <c r="EY5" t="n">
+        <v>11178.9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2351,12 +2360,15 @@
         <v>168</v>
       </c>
       <c r="EX6" t="n">
-        <v>174.2</v>
+        <v>174.1</v>
+      </c>
+      <c r="EY6" t="n">
+        <v>177.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2816,11 +2828,14 @@
       </c>
       <c r="EX7" t="n">
         <v>26</v>
+      </c>
+      <c r="EY7" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3279,12 +3294,15 @@
         <v>179.6</v>
       </c>
       <c r="EX8" t="n">
-        <v>200</v>
+        <v>200.1</v>
+      </c>
+      <c r="EY8" t="n">
+        <v>201.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3744,11 +3762,14 @@
       </c>
       <c r="EX9" t="n">
         <v>102.3</v>
+      </c>
+      <c r="EY9" t="n">
+        <v>104.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4207,12 +4228,15 @@
         <v>1173.7</v>
       </c>
       <c r="EX10" t="n">
-        <v>1242</v>
+        <v>1241.7</v>
+      </c>
+      <c r="EY10" t="n">
+        <v>1283.9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4671,12 +4695,15 @@
         <v>219.4</v>
       </c>
       <c r="EX11" t="n">
-        <v>238.6</v>
+        <v>239</v>
+      </c>
+      <c r="EY11" t="n">
+        <v>245.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5136,11 +5163,14 @@
       </c>
       <c r="EX12" t="n">
         <v>121.9</v>
+      </c>
+      <c r="EY12" t="n">
+        <v>123.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5599,12 +5629,15 @@
         <v>34.8</v>
       </c>
       <c r="EX13" t="n">
-        <v>39.6</v>
+        <v>39.7</v>
+      </c>
+      <c r="EY13" t="n">
+        <v>40.8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5759,10 +5792,11 @@
       <c r="EV14"/>
       <c r="EW14"/>
       <c r="EX14"/>
+      <c r="EY14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6222,11 +6256,14 @@
       </c>
       <c r="EX15" t="n">
         <v>499.6</v>
+      </c>
+      <c r="EY15" t="n">
+        <v>503.1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6685,12 +6722,15 @@
         <v>353</v>
       </c>
       <c r="EX16" t="n">
-        <v>357.2</v>
+        <v>355.7</v>
+      </c>
+      <c r="EY16" t="n">
+        <v>357.8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6845,10 +6885,11 @@
       <c r="EV17"/>
       <c r="EW17"/>
       <c r="EX17"/>
+      <c r="EY17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7307,12 +7348,15 @@
         <v>58.4</v>
       </c>
       <c r="EX18" t="n">
-        <v>66.5</v>
+        <v>65.6</v>
+      </c>
+      <c r="EY18" t="n">
+        <v>69.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7771,12 +7815,15 @@
         <v>417.1</v>
       </c>
       <c r="EX19" t="n">
-        <v>478</v>
+        <v>459.4</v>
+      </c>
+      <c r="EY19" t="n">
+        <v>473</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8235,12 +8282,15 @@
         <v>212</v>
       </c>
       <c r="EX20" t="n">
-        <v>232.7</v>
+        <v>232.4</v>
+      </c>
+      <c r="EY20" t="n">
+        <v>238.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8699,12 +8749,15 @@
         <v>120.6</v>
       </c>
       <c r="EX21" t="n">
-        <v>141.8</v>
+        <v>144.3</v>
+      </c>
+      <c r="EY21" t="n">
+        <v>149.8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9164,11 +9217,14 @@
       </c>
       <c r="EX22" t="n">
         <v>132.7</v>
+      </c>
+      <c r="EY22" t="n">
+        <v>138.4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9628,11 +9684,14 @@
       </c>
       <c r="EX23" t="n">
         <v>164.3</v>
+      </c>
+      <c r="EY23" t="n">
+        <v>165.6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10091,12 +10150,15 @@
         <v>137.9</v>
       </c>
       <c r="EX24" t="n">
-        <v>146.4</v>
+        <v>148.2</v>
+      </c>
+      <c r="EY24" t="n">
+        <v>151.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10556,11 +10618,14 @@
       </c>
       <c r="EX25" t="n">
         <v>50.7</v>
+      </c>
+      <c r="EY25" t="n">
+        <v>51.2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11020,11 +11085,14 @@
       </c>
       <c r="EX26" t="n">
         <v>222.2</v>
+      </c>
+      <c r="EY26" t="n">
+        <v>223.2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11484,11 +11552,14 @@
       </c>
       <c r="EX27" t="n">
         <v>244.6</v>
+      </c>
+      <c r="EY27" t="n">
+        <v>248.4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -11948,11 +12019,14 @@
       </c>
       <c r="EX28" t="n">
         <v>322.7</v>
+      </c>
+      <c r="EY28" t="n">
+        <v>333.4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12412,11 +12486,14 @@
       </c>
       <c r="EX29" t="n">
         <v>204.4</v>
+      </c>
+      <c r="EY29" t="n">
+        <v>217.6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12876,11 +12953,14 @@
       </c>
       <c r="EX30" t="n">
         <v>105.3</v>
+      </c>
+      <c r="EY30" t="n">
+        <v>105.7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -13035,10 +13115,11 @@
       <c r="EV31"/>
       <c r="EW31"/>
       <c r="EX31"/>
+      <c r="EY31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -13498,11 +13579,14 @@
       </c>
       <c r="EX32" t="n">
         <v>43.3</v>
+      </c>
+      <c r="EY32" t="n">
+        <v>43.6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -13961,12 +14045,15 @@
         <v>80.5</v>
       </c>
       <c r="EX33" t="n">
-        <v>93.3</v>
+        <v>93.4</v>
+      </c>
+      <c r="EY33" t="n">
+        <v>97.4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -14425,12 +14512,15 @@
         <v>75.2</v>
       </c>
       <c r="EX34" t="n">
-        <v>87.8</v>
+        <v>86.4</v>
+      </c>
+      <c r="EY34" t="n">
+        <v>87.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -14889,12 +14979,15 @@
         <v>33.9</v>
       </c>
       <c r="EX35" t="n">
-        <v>44.5</v>
+        <v>44.2</v>
+      </c>
+      <c r="EY35" t="n">
+        <v>45.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -15354,11 +15447,14 @@
       </c>
       <c r="EX36" t="n">
         <v>306</v>
+      </c>
+      <c r="EY36" t="n">
+        <v>324.2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -15818,11 +15914,14 @@
       </c>
       <c r="EX37" t="n">
         <v>79.9</v>
+      </c>
+      <c r="EY37" t="n">
+        <v>81.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -16282,11 +16381,14 @@
       </c>
       <c r="EX38" t="n">
         <v>663.1</v>
+      </c>
+      <c r="EY38" t="n">
+        <v>690.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16746,11 +16848,14 @@
       </c>
       <c r="EX39" t="n">
         <v>337.6</v>
+      </c>
+      <c r="EY39" t="n">
+        <v>342.1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -17210,11 +17315,14 @@
       </c>
       <c r="EX40" t="n">
         <v>40.8</v>
+      </c>
+      <c r="EY40" t="n">
+        <v>42.7</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -17673,12 +17781,15 @@
         <v>352.5</v>
       </c>
       <c r="EX41" t="n">
-        <v>389.8</v>
+        <v>389.4</v>
+      </c>
+      <c r="EY41" t="n">
+        <v>396.8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -18137,12 +18248,15 @@
         <v>131.9</v>
       </c>
       <c r="EX42" t="n">
-        <v>151.2</v>
+        <v>153.1</v>
+      </c>
+      <c r="EY42" t="n">
+        <v>156.3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -18601,12 +18715,15 @@
         <v>114.6</v>
       </c>
       <c r="EX43" t="n">
-        <v>128</v>
+        <v>128.2</v>
+      </c>
+      <c r="EY43" t="n">
+        <v>142.1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -19066,11 +19183,14 @@
       </c>
       <c r="EX44" t="n">
         <v>330.5</v>
+      </c>
+      <c r="EY44" t="n">
+        <v>336.3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -19530,11 +19650,14 @@
       </c>
       <c r="EX45" t="n">
         <v>29.4</v>
+      </c>
+      <c r="EY45" t="n">
+        <v>30.1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -19993,12 +20116,15 @@
         <v>152.3</v>
       </c>
       <c r="EX46" t="n">
-        <v>163.2</v>
+        <v>162.8</v>
+      </c>
+      <c r="EY46" t="n">
+        <v>164.4</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -20457,12 +20583,15 @@
         <v>29.9</v>
       </c>
       <c r="EX47" t="n">
-        <v>37</v>
+        <v>37.9</v>
+      </c>
+      <c r="EY47" t="n">
+        <v>39.9</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -20921,12 +21050,15 @@
         <v>177.2</v>
       </c>
       <c r="EX48" t="n">
-        <v>200.5</v>
+        <v>200.8</v>
+      </c>
+      <c r="EY48" t="n">
+        <v>206.1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -21385,12 +21517,15 @@
         <v>1108.3</v>
       </c>
       <c r="EX49" t="n">
-        <v>1159.7</v>
+        <v>1163.8</v>
+      </c>
+      <c r="EY49" t="n">
+        <v>1202.4</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -21849,12 +21984,15 @@
         <v>120.5</v>
       </c>
       <c r="EX50" t="n">
-        <v>134.5</v>
+        <v>135.7</v>
+      </c>
+      <c r="EY50" t="n">
+        <v>140</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -22313,12 +22451,15 @@
         <v>25.9</v>
       </c>
       <c r="EX51" t="n">
-        <v>31.4</v>
+        <v>32</v>
+      </c>
+      <c r="EY51" t="n">
+        <v>33.8</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -22777,12 +22918,15 @@
         <v>292.7</v>
       </c>
       <c r="EX52" t="n">
-        <v>325.1</v>
+        <v>333.3</v>
+      </c>
+      <c r="EY52" t="n">
+        <v>339.7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -23241,12 +23385,15 @@
         <v>222.3</v>
       </c>
       <c r="EX53" t="n">
-        <v>233.1</v>
+        <v>233.5</v>
+      </c>
+      <c r="EY53" t="n">
+        <v>251.9</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -23705,12 +23852,15 @@
         <v>53.8</v>
       </c>
       <c r="EX54" t="n">
-        <v>59.4</v>
+        <v>59.3</v>
+      </c>
+      <c r="EY54" t="n">
+        <v>61.4</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -24169,12 +24319,15 @@
         <v>173.9</v>
       </c>
       <c r="EX55" t="n">
-        <v>206.2</v>
+        <v>206.5</v>
+      </c>
+      <c r="EY55" t="n">
+        <v>214.7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -24633,7 +24786,10 @@
         <v>25.6</v>
       </c>
       <c r="EX56" t="n">
-        <v>29.6</v>
+        <v>29.9</v>
+      </c>
+      <c r="EY56" t="n">
+        <v>31.2</v>
       </c>
     </row>
   </sheetData>
@@ -25077,10 +25233,13 @@
       <c r="EL4" t="s">
         <v>153</v>
       </c>
+      <c r="EM4" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -25500,15 +25659,18 @@
         <v>1.94039203614734</v>
       </c>
       <c r="EK5" t="n">
-        <v>1.87228246634188</v>
+        <v>1.94247996228194</v>
       </c>
       <c r="EL5" t="n">
-        <v>1.58859661461996</v>
+        <v>1.33633422422282</v>
+      </c>
+      <c r="EM5" t="n">
+        <v>1.43732135565537</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -25931,12 +26093,15 @@
         <v>0.478468899521538</v>
       </c>
       <c r="EL6" t="n">
-        <v>0.577367205542725</v>
+        <v>0.519630484988472</v>
+      </c>
+      <c r="EM6" t="n">
+        <v>0.854214123006817</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -26360,11 +26525,14 @@
       </c>
       <c r="EL7" t="n">
         <v>-4.76190476190476</v>
+      </c>
+      <c r="EM7" t="n">
+        <v>-4.59363957597172</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -26787,12 +26955,15 @@
         <v>-2.49728555917481</v>
       </c>
       <c r="EL8" t="n">
-        <v>0.857286938981336</v>
+        <v>0.907715582450823</v>
+      </c>
+      <c r="EM8" t="n">
+        <v>0.149105367793246</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -27216,11 +27387,14 @@
       </c>
       <c r="EL9" t="n">
         <v>1.18694362017804</v>
+      </c>
+      <c r="EM9" t="n">
+        <v>1.16166505324297</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -27643,12 +27817,15 @@
         <v>4.71984296930765</v>
       </c>
       <c r="EL10" t="n">
-        <v>3.47413146713322</v>
+        <v>3.44913771557112</v>
+      </c>
+      <c r="EM10" t="n">
+        <v>2.52335702307755</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -28071,12 +28248,15 @@
         <v>4.37678401522361</v>
       </c>
       <c r="EL11" t="n">
-        <v>4.23765836609874</v>
+        <v>4.41240716470074</v>
+      </c>
+      <c r="EM11" t="n">
+        <v>4.20918367346939</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -28500,11 +28680,14 @@
       </c>
       <c r="EL12" t="n">
         <v>-0.651996740016309</v>
+      </c>
+      <c r="EM12" t="n">
+        <v>-1.82829888712241</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -28927,12 +29110,15 @@
         <v>2.95857988165681</v>
       </c>
       <c r="EL13" t="n">
-        <v>2.32558139534882</v>
+        <v>2.58397932816537</v>
+      </c>
+      <c r="EM13" t="n">
+        <v>2.77078085642316</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -29075,10 +29261,11 @@
       <c r="EJ14"/>
       <c r="EK14"/>
       <c r="EL14"/>
+      <c r="EM14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -29502,11 +29689,14 @@
       </c>
       <c r="EL15" t="n">
         <v>2.10504802779482</v>
+      </c>
+      <c r="EM15" t="n">
+        <v>1.32930513595167</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -29929,12 +30119,15 @@
         <v>2.61627906976744</v>
       </c>
       <c r="EL16" t="n">
-        <v>1.85343598517251</v>
+        <v>1.42571998859424</v>
+      </c>
+      <c r="EM16" t="n">
+        <v>1.41723356009069</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -30077,10 +30270,11 @@
       <c r="EJ17"/>
       <c r="EK17"/>
       <c r="EL17"/>
+      <c r="EM17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -30503,12 +30697,15 @@
         <v>8.95522388059701</v>
       </c>
       <c r="EL18" t="n">
-        <v>7.25806451612903</v>
+        <v>5.80645161290322</v>
+      </c>
+      <c r="EM18" t="n">
+        <v>7.56172839506174</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -30931,12 +31128,15 @@
         <v>8.47854356306891</v>
       </c>
       <c r="EL19" t="n">
-        <v>8.43920145190562</v>
+        <v>4.21960072595281</v>
+      </c>
+      <c r="EM19" t="n">
+        <v>4.6691745961496</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -31359,12 +31559,15 @@
         <v>2.46495891735137</v>
       </c>
       <c r="EL20" t="n">
-        <v>1.26196692776328</v>
+        <v>1.13141862489121</v>
+      </c>
+      <c r="EM20" t="n">
+        <v>2.18884120171675</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -31787,12 +31990,15 @@
         <v>-0.822368421052632</v>
       </c>
       <c r="EL21" t="n">
-        <v>-0.839160839160831</v>
+        <v>0.909090909090917</v>
+      </c>
+      <c r="EM21" t="n">
+        <v>0.807537012113067</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -32216,11 +32422,14 @@
       </c>
       <c r="EL22" t="n">
         <v>0.22658610271902</v>
+      </c>
+      <c r="EM22" t="n">
+        <v>1.16959064327485</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -32644,11 +32853,14 @@
       </c>
       <c r="EL23" t="n">
         <v>0.366524129505206</v>
+      </c>
+      <c r="EM23" t="n">
+        <v>0.424499696785924</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -33071,12 +33283,15 @@
         <v>0.290909090909095</v>
       </c>
       <c r="EL24" t="n">
-        <v>0</v>
+        <v>1.2295081967213</v>
+      </c>
+      <c r="EM24" t="n">
+        <v>2.50338294993233</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -33500,11 +33715,14 @@
       </c>
       <c r="EL25" t="n">
         <v>4.53608247422681</v>
+      </c>
+      <c r="EM25" t="n">
+        <v>2.19560878243513</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -33928,11 +34146,14 @@
       </c>
       <c r="EL26" t="n">
         <v>1.55393053016454</v>
+      </c>
+      <c r="EM26" t="n">
+        <v>0.904159132007233</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -34356,11 +34577,14 @@
       </c>
       <c r="EL27" t="n">
         <v>1.40961857379768</v>
+      </c>
+      <c r="EM27" t="n">
+        <v>1.42915475704369</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -34784,11 +35008,14 @@
       </c>
       <c r="EL28" t="n">
         <v>4.13036463375283</v>
+      </c>
+      <c r="EM28" t="n">
+        <v>4.05742821473159</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -35212,11 +35439,14 @@
       </c>
       <c r="EL29" t="n">
         <v>2.8169014084507</v>
+      </c>
+      <c r="EM29" t="n">
+        <v>2.30371415138693</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -35640,11 +35870,14 @@
       </c>
       <c r="EL30" t="n">
         <v>0.765550239234447</v>
+      </c>
+      <c r="EM30" t="n">
+        <v>0.189573459715643</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -35787,10 +36020,11 @@
       <c r="EJ31"/>
       <c r="EK31"/>
       <c r="EL31"/>
+      <c r="EM31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -36214,11 +36448,14 @@
       </c>
       <c r="EL32" t="n">
         <v>2.12264150943396</v>
+      </c>
+      <c r="EM32" t="n">
+        <v>0.69284064665128</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -36641,12 +36878,15 @@
         <v>-0.739827373612817</v>
       </c>
       <c r="EL33" t="n">
-        <v>0.430570505920351</v>
+        <v>0.538213132400431</v>
+      </c>
+      <c r="EM33" t="n">
+        <v>1.88284518828452</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -37069,12 +37309,15 @@
         <v>13.4238310708899</v>
       </c>
       <c r="EL34" t="n">
-        <v>6.03864734299519</v>
+        <v>4.34782608695653</v>
+      </c>
+      <c r="EM34" t="n">
+        <v>3.79596678529063</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -37497,12 +37740,15 @@
         <v>4.3076923076923</v>
       </c>
       <c r="EL35" t="n">
-        <v>0.451467268623031</v>
+        <v>-0.2257336343115</v>
+      </c>
+      <c r="EM35" t="n">
+        <v>-0.218340611353699</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -37926,11 +38172,14 @@
       </c>
       <c r="EL36" t="n">
         <v>2.44392366923335</v>
+      </c>
+      <c r="EM36" t="n">
+        <v>2.14240705734088</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -38354,11 +38603,14 @@
       </c>
       <c r="EL37" t="n">
         <v>3.36351875808539</v>
+      </c>
+      <c r="EM37" t="n">
+        <v>3.03797468354431</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -38782,11 +39034,14 @@
       </c>
       <c r="EL38" t="n">
         <v>2.44090838869148</v>
+      </c>
+      <c r="EM38" t="n">
+        <v>2.51039809863339</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -39210,11 +39465,14 @@
       </c>
       <c r="EL39" t="n">
         <v>1.93236714975846</v>
+      </c>
+      <c r="EM39" t="n">
+        <v>1.48323939483833</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -39638,11 +39896,14 @@
       </c>
       <c r="EL40" t="n">
         <v>10.2702702702703</v>
+      </c>
+      <c r="EM40" t="n">
+        <v>9.48717948717949</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -40065,12 +40326,15 @@
         <v>-0.226436456269463</v>
       </c>
       <c r="EL41" t="n">
-        <v>1.32570834416427</v>
+        <v>1.22173121913179</v>
+      </c>
+      <c r="EM41" t="n">
+        <v>0.761808024377871</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -40493,12 +40757,15 @@
         <v>1.15030674846628</v>
       </c>
       <c r="EL42" t="n">
-        <v>0.799999999999992</v>
+        <v>2.06666666666668</v>
+      </c>
+      <c r="EM42" t="n">
+        <v>2.09013716525148</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -40921,12 +41188,15 @@
         <v>2.23015165031222</v>
       </c>
       <c r="EL43" t="n">
-        <v>1.10584518167457</v>
+        <v>1.26382306477095</v>
+      </c>
+      <c r="EM43" t="n">
+        <v>1.93687230989958</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -41350,11 +41620,14 @@
       </c>
       <c r="EL44" t="n">
         <v>1.19412124923455</v>
+      </c>
+      <c r="EM44" t="n">
+        <v>0.508069336521216</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -41778,11 +42051,14 @@
       </c>
       <c r="EL45" t="n">
         <v>5.37634408602151</v>
+      </c>
+      <c r="EM45" t="n">
+        <v>2.38095238095238</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -42205,12 +42481,15 @@
         <v>1.66889185580774</v>
       </c>
       <c r="EL46" t="n">
-        <v>2.06378986866793</v>
+        <v>1.81363352095062</v>
+      </c>
+      <c r="EM46" t="n">
+        <v>0.920810313075506</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -42633,12 +42912,15 @@
         <v>0.335570469798663</v>
       </c>
       <c r="EL47" t="n">
-        <v>-0.537634408602158</v>
+        <v>1.88172043010752</v>
+      </c>
+      <c r="EM47" t="n">
+        <v>3.10077519379844</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -43061,12 +43343,15 @@
         <v>-2.47660979636764</v>
       </c>
       <c r="EL48" t="n">
-        <v>-2.38558909444986</v>
+        <v>-2.23953261927945</v>
+      </c>
+      <c r="EM48" t="n">
+        <v>-1.34035423647679</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -43489,12 +43774,15 @@
         <v>1.75358060962173</v>
       </c>
       <c r="EL49" t="n">
-        <v>-0.00862217623727445</v>
+        <v>0.344887049491292</v>
+      </c>
+      <c r="EM49" t="n">
+        <v>0.610827545812081</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -43917,12 +44205,15 @@
         <v>4.60069444444445</v>
       </c>
       <c r="EL50" t="n">
-        <v>4.10216718266255</v>
+        <v>5.03095975232198</v>
+      </c>
+      <c r="EM50" t="n">
+        <v>5.26315789473684</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -44345,12 +44636,15 @@
         <v>1.171875</v>
       </c>
       <c r="EL51" t="n">
-        <v>0.641025641025627</v>
+        <v>2.56410256410255</v>
+      </c>
+      <c r="EM51" t="n">
+        <v>3.99999999999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -44773,12 +45067,15 @@
         <v>0.861474844934528</v>
       </c>
       <c r="EL52" t="n">
-        <v>1.84837092731829</v>
+        <v>4.4172932330827</v>
+      </c>
+      <c r="EM52" t="n">
+        <v>3.82029339853301</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -45201,12 +45498,15 @@
         <v>0.180261378999552</v>
       </c>
       <c r="EL53" t="n">
-        <v>-0.427167876975651</v>
+        <v>-0.256300726185401</v>
+      </c>
+      <c r="EM53" t="n">
+        <v>0.921474358974352</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -45629,12 +45929,15 @@
         <v>-2.88808664259929</v>
       </c>
       <c r="EL54" t="n">
-        <v>-2.78232405891979</v>
+        <v>-2.94599018003272</v>
+      </c>
+      <c r="EM54" t="n">
+        <v>-3.15457413249211</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -46057,12 +46360,15 @@
         <v>4.00717703349282</v>
       </c>
       <c r="EL55" t="n">
-        <v>0.145701796988835</v>
+        <v>0.29140359397767</v>
+      </c>
+      <c r="EM55" t="n">
+        <v>-0.278680910357651</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -46485,7 +46791,10 @@
         <v>1.58730158730158</v>
       </c>
       <c r="EL56" t="n">
-        <v>-1.33333333333333</v>
+        <v>-0.333333333333338</v>
+      </c>
+      <c r="EM56" t="n">
+        <v>-0.319488817891356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on December, 20 2024
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -478,6 +478,9 @@
   </si>
   <si>
     <t xml:space="preserve">10/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1431,10 +1434,13 @@
       <c r="EY4" t="s">
         <v>154</v>
       </c>
+      <c r="EZ4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1893,15 +1899,18 @@
         <v>9729.9</v>
       </c>
       <c r="EX5" t="n">
-        <v>10806</v>
+        <v>10818.4</v>
       </c>
       <c r="EY5" t="n">
-        <v>11178.9</v>
+        <v>11180.8</v>
+      </c>
+      <c r="EZ5" t="n">
+        <v>11301.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2363,12 +2372,15 @@
         <v>174.1</v>
       </c>
       <c r="EY6" t="n">
-        <v>177.1</v>
+        <v>176.5</v>
+      </c>
+      <c r="EZ6" t="n">
+        <v>177.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2830,12 +2842,15 @@
         <v>26</v>
       </c>
       <c r="EY7" t="n">
-        <v>27</v>
+        <v>27.1</v>
+      </c>
+      <c r="EZ7" t="n">
+        <v>27.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3297,12 +3312,15 @@
         <v>200.1</v>
       </c>
       <c r="EY8" t="n">
-        <v>201.5</v>
+        <v>202.9</v>
+      </c>
+      <c r="EZ8" t="n">
+        <v>206.4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3765,11 +3783,14 @@
       </c>
       <c r="EY9" t="n">
         <v>104.5</v>
+      </c>
+      <c r="EZ9" t="n">
+        <v>104.7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4231,12 +4252,15 @@
         <v>1241.7</v>
       </c>
       <c r="EY10" t="n">
-        <v>1283.9</v>
+        <v>1291.2</v>
+      </c>
+      <c r="EZ10" t="n">
+        <v>1307.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4698,12 +4722,15 @@
         <v>239</v>
       </c>
       <c r="EY11" t="n">
-        <v>245.1</v>
+        <v>244.9</v>
+      </c>
+      <c r="EZ11" t="n">
+        <v>247.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5166,11 +5193,14 @@
       </c>
       <c r="EY12" t="n">
         <v>123.5</v>
+      </c>
+      <c r="EZ12" t="n">
+        <v>124.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5633,11 +5663,14 @@
       </c>
       <c r="EY13" t="n">
         <v>40.8</v>
+      </c>
+      <c r="EZ13" t="n">
+        <v>41.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5793,10 +5826,11 @@
       <c r="EW14"/>
       <c r="EX14"/>
       <c r="EY14"/>
+      <c r="EZ14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6259,11 +6293,14 @@
       </c>
       <c r="EY15" t="n">
         <v>503.1</v>
+      </c>
+      <c r="EZ15" t="n">
+        <v>506.4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6725,12 +6762,15 @@
         <v>355.7</v>
       </c>
       <c r="EY16" t="n">
-        <v>357.8</v>
+        <v>357.7</v>
+      </c>
+      <c r="EZ16" t="n">
+        <v>358.8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6886,10 +6926,11 @@
       <c r="EW17"/>
       <c r="EX17"/>
       <c r="EY17"/>
+      <c r="EZ17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7351,12 +7392,15 @@
         <v>65.6</v>
       </c>
       <c r="EY18" t="n">
-        <v>69.7</v>
+        <v>69.2</v>
+      </c>
+      <c r="EZ18" t="n">
+        <v>69.3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7818,12 +7862,15 @@
         <v>459.4</v>
       </c>
       <c r="EY19" t="n">
-        <v>473</v>
+        <v>472.4</v>
+      </c>
+      <c r="EZ19" t="n">
+        <v>474.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8285,12 +8332,15 @@
         <v>232.4</v>
       </c>
       <c r="EY20" t="n">
-        <v>238.1</v>
+        <v>235.7</v>
+      </c>
+      <c r="EZ20" t="n">
+        <v>240.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8752,12 +8802,15 @@
         <v>144.3</v>
       </c>
       <c r="EY21" t="n">
-        <v>149.8</v>
+        <v>149.7</v>
+      </c>
+      <c r="EZ21" t="n">
+        <v>151.1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9220,11 +9273,14 @@
       </c>
       <c r="EY22" t="n">
         <v>138.4</v>
+      </c>
+      <c r="EZ22" t="n">
+        <v>139.8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9686,12 +9742,15 @@
         <v>164.3</v>
       </c>
       <c r="EY23" t="n">
-        <v>165.6</v>
+        <v>165.3</v>
+      </c>
+      <c r="EZ23" t="n">
+        <v>167.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10153,12 +10212,15 @@
         <v>148.2</v>
       </c>
       <c r="EY24" t="n">
-        <v>151.5</v>
+        <v>151.6</v>
+      </c>
+      <c r="EZ24" t="n">
+        <v>153.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10620,12 +10682,15 @@
         <v>50.7</v>
       </c>
       <c r="EY25" t="n">
-        <v>51.2</v>
+        <v>52</v>
+      </c>
+      <c r="EZ25" t="n">
+        <v>52.2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11087,12 +11152,15 @@
         <v>222.2</v>
       </c>
       <c r="EY26" t="n">
-        <v>223.2</v>
+        <v>226</v>
+      </c>
+      <c r="EZ26" t="n">
+        <v>228.8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11555,11 +11623,14 @@
       </c>
       <c r="EY27" t="n">
         <v>248.4</v>
+      </c>
+      <c r="EZ27" t="n">
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -12022,11 +12093,14 @@
       </c>
       <c r="EY28" t="n">
         <v>333.4</v>
+      </c>
+      <c r="EZ28" t="n">
+        <v>336.6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12489,11 +12563,14 @@
       </c>
       <c r="EY29" t="n">
         <v>217.6</v>
+      </c>
+      <c r="EZ29" t="n">
+        <v>221.1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -12955,12 +13032,15 @@
         <v>105.3</v>
       </c>
       <c r="EY30" t="n">
-        <v>105.7</v>
+        <v>106</v>
+      </c>
+      <c r="EZ30" t="n">
+        <v>106.3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -13116,10 +13196,11 @@
       <c r="EW31"/>
       <c r="EX31"/>
       <c r="EY31"/>
+      <c r="EZ31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -13582,11 +13663,14 @@
       </c>
       <c r="EY32" t="n">
         <v>43.6</v>
+      </c>
+      <c r="EZ32" t="n">
+        <v>44.3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -14048,12 +14132,15 @@
         <v>93.4</v>
       </c>
       <c r="EY33" t="n">
-        <v>97.4</v>
+        <v>97.5</v>
+      </c>
+      <c r="EZ33" t="n">
+        <v>97.7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -14515,12 +14602,15 @@
         <v>86.4</v>
       </c>
       <c r="EY34" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="EZ34" t="n">
         <v>87.5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -14982,12 +15072,15 @@
         <v>44.2</v>
       </c>
       <c r="EY35" t="n">
-        <v>45.7</v>
+        <v>45.5</v>
+      </c>
+      <c r="EZ35" t="n">
+        <v>45.6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -15449,12 +15542,15 @@
         <v>306</v>
       </c>
       <c r="EY36" t="n">
-        <v>324.2</v>
+        <v>324.8</v>
+      </c>
+      <c r="EZ36" t="n">
+        <v>328.6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -15917,11 +16013,14 @@
       </c>
       <c r="EY37" t="n">
         <v>81.4</v>
+      </c>
+      <c r="EZ37" t="n">
+        <v>82.4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -16384,11 +16483,14 @@
       </c>
       <c r="EY38" t="n">
         <v>690.1</v>
+      </c>
+      <c r="EZ38" t="n">
+        <v>693.8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16850,12 +16952,15 @@
         <v>337.6</v>
       </c>
       <c r="EY39" t="n">
-        <v>342.1</v>
+        <v>343.6</v>
+      </c>
+      <c r="EZ39" t="n">
+        <v>347.7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -17318,11 +17423,14 @@
       </c>
       <c r="EY40" t="n">
         <v>42.7</v>
+      </c>
+      <c r="EZ40" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -17784,12 +17892,15 @@
         <v>389.4</v>
       </c>
       <c r="EY41" t="n">
-        <v>396.8</v>
+        <v>396.4</v>
+      </c>
+      <c r="EZ41" t="n">
+        <v>403</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -18252,11 +18363,14 @@
       </c>
       <c r="EY42" t="n">
         <v>156.3</v>
+      </c>
+      <c r="EZ42" t="n">
+        <v>157</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -18718,12 +18832,15 @@
         <v>128.2</v>
       </c>
       <c r="EY43" t="n">
-        <v>142.1</v>
+        <v>140.9</v>
+      </c>
+      <c r="EZ43" t="n">
+        <v>143.3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -19185,12 +19302,15 @@
         <v>330.5</v>
       </c>
       <c r="EY44" t="n">
-        <v>336.3</v>
+        <v>338.6</v>
+      </c>
+      <c r="EZ44" t="n">
+        <v>343.6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -19653,11 +19773,14 @@
       </c>
       <c r="EY45" t="n">
         <v>30.1</v>
+      </c>
+      <c r="EZ45" t="n">
+        <v>30.4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -20119,12 +20242,15 @@
         <v>162.8</v>
       </c>
       <c r="EY46" t="n">
-        <v>164.4</v>
+        <v>164.2</v>
+      </c>
+      <c r="EZ46" t="n">
+        <v>166</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -20586,12 +20712,15 @@
         <v>37.9</v>
       </c>
       <c r="EY47" t="n">
-        <v>39.9</v>
+        <v>39.5</v>
+      </c>
+      <c r="EZ47" t="n">
+        <v>39.8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -21054,11 +21183,14 @@
       </c>
       <c r="EY48" t="n">
         <v>206.1</v>
+      </c>
+      <c r="EZ48" t="n">
+        <v>207.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -21520,12 +21652,15 @@
         <v>1163.8</v>
       </c>
       <c r="EY49" t="n">
-        <v>1202.4</v>
+        <v>1200.6</v>
+      </c>
+      <c r="EZ49" t="n">
+        <v>1210.4</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -21988,11 +22123,14 @@
       </c>
       <c r="EY50" t="n">
         <v>140</v>
+      </c>
+      <c r="EZ50" t="n">
+        <v>141.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -22454,12 +22592,15 @@
         <v>32</v>
       </c>
       <c r="EY51" t="n">
-        <v>33.8</v>
+        <v>34.1</v>
+      </c>
+      <c r="EZ51" t="n">
+        <v>34.4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -22921,12 +23062,15 @@
         <v>333.3</v>
       </c>
       <c r="EY52" t="n">
-        <v>339.7</v>
+        <v>341.7</v>
+      </c>
+      <c r="EZ52" t="n">
+        <v>345.3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -23388,12 +23532,15 @@
         <v>233.5</v>
       </c>
       <c r="EY53" t="n">
-        <v>251.9</v>
+        <v>249.6</v>
+      </c>
+      <c r="EZ53" t="n">
+        <v>253.1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -23856,11 +24003,14 @@
       </c>
       <c r="EY54" t="n">
         <v>61.4</v>
+      </c>
+      <c r="EZ54" t="n">
+        <v>61.9</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -24323,11 +24473,14 @@
       </c>
       <c r="EY55" t="n">
         <v>214.7</v>
+      </c>
+      <c r="EZ55" t="n">
+        <v>215.6</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -24789,7 +24942,10 @@
         <v>29.9</v>
       </c>
       <c r="EY56" t="n">
-        <v>31.2</v>
+        <v>31.1</v>
+      </c>
+      <c r="EZ56" t="n">
+        <v>31.4</v>
       </c>
     </row>
   </sheetData>
@@ -25236,10 +25392,13 @@
       <c r="EM4" t="s">
         <v>154</v>
       </c>
+      <c r="EN4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -25662,15 +25821,18 @@
         <v>1.94247996228194</v>
       </c>
       <c r="EL5" t="n">
-        <v>1.33633422422282</v>
+        <v>1.45261874619027</v>
       </c>
       <c r="EM5" t="n">
-        <v>1.43732135565537</v>
+        <v>1.45456195272446</v>
+      </c>
+      <c r="EN5" t="n">
+        <v>1.44973070017953</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -26096,12 +26258,15 @@
         <v>0.519630484988472</v>
       </c>
       <c r="EM6" t="n">
-        <v>0.854214123006817</v>
+        <v>0.512528473804087</v>
+      </c>
+      <c r="EN6" t="n">
+        <v>0.509626274065672</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -26527,12 +26692,15 @@
         <v>-4.76190476190476</v>
       </c>
       <c r="EM7" t="n">
-        <v>-4.59363957597172</v>
+        <v>-4.24028268551235</v>
+      </c>
+      <c r="EN7" t="n">
+        <v>-4.18118466898956</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -26958,12 +27126,15 @@
         <v>0.907715582450823</v>
       </c>
       <c r="EM8" t="n">
-        <v>0.149105367793246</v>
+        <v>0.844930417495024</v>
+      </c>
+      <c r="EN8" t="n">
+        <v>1.67487684729064</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -27390,11 +27561,14 @@
       </c>
       <c r="EM9" t="n">
         <v>1.16166505324297</v>
+      </c>
+      <c r="EN9" t="n">
+        <v>1.06177606177606</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -27820,12 +27994,15 @@
         <v>3.44913771557112</v>
       </c>
       <c r="EM10" t="n">
-        <v>2.52335702307755</v>
+        <v>3.1062844366366</v>
+      </c>
+      <c r="EN10" t="n">
+        <v>2.68530150753771</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -28251,12 +28428,15 @@
         <v>4.41240716470074</v>
       </c>
       <c r="EM11" t="n">
-        <v>4.20918367346939</v>
+        <v>4.12414965986395</v>
+      </c>
+      <c r="EN11" t="n">
+        <v>4.07905803195963</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -28683,11 +28863,14 @@
       </c>
       <c r="EM12" t="n">
         <v>-1.82829888712241</v>
+      </c>
+      <c r="EN12" t="n">
+        <v>-1.81102362204724</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -29114,11 +29297,14 @@
       </c>
       <c r="EM13" t="n">
         <v>2.77078085642316</v>
+      </c>
+      <c r="EN13" t="n">
+        <v>2.23325062034741</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -29262,10 +29448,11 @@
       <c r="EK14"/>
       <c r="EL14"/>
       <c r="EM14"/>
+      <c r="EN14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -29692,11 +29879,14 @@
       </c>
       <c r="EM15" t="n">
         <v>1.32930513595167</v>
+      </c>
+      <c r="EN15" t="n">
+        <v>1.82988135934044</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -30122,12 +30312,15 @@
         <v>1.42571998859424</v>
       </c>
       <c r="EM16" t="n">
-        <v>1.41723356009069</v>
+        <v>1.38888888888888</v>
+      </c>
+      <c r="EN16" t="n">
+        <v>1.32730866986727</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -30271,10 +30464,11 @@
       <c r="EK17"/>
       <c r="EL17"/>
       <c r="EM17"/>
+      <c r="EN17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -30700,12 +30894,15 @@
         <v>5.80645161290322</v>
       </c>
       <c r="EM18" t="n">
-        <v>7.56172839506174</v>
+        <v>6.79012345679011</v>
+      </c>
+      <c r="EN18" t="n">
+        <v>6.28834355828222</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -31131,12 +31328,15 @@
         <v>4.21960072595281</v>
       </c>
       <c r="EM19" t="n">
-        <v>4.6691745961496</v>
+        <v>4.53640185881834</v>
+      </c>
+      <c r="EN19" t="n">
+        <v>3.988603988604</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -31562,12 +31762,15 @@
         <v>1.13141862489121</v>
       </c>
       <c r="EM20" t="n">
-        <v>2.18884120171675</v>
+        <v>1.1587982832618</v>
+      </c>
+      <c r="EN20" t="n">
+        <v>1.86598812553011</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -31993,12 +32196,15 @@
         <v>0.909090909090917</v>
       </c>
       <c r="EM21" t="n">
-        <v>0.807537012113067</v>
+        <v>0.74024226110363</v>
+      </c>
+      <c r="EN21" t="n">
+        <v>0.935203740814967</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -32425,11 +32631,14 @@
       </c>
       <c r="EM22" t="n">
         <v>1.16959064327485</v>
+      </c>
+      <c r="EN22" t="n">
+        <v>1.08459869848156</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -32855,12 +33064,15 @@
         <v>0.366524129505206</v>
       </c>
       <c r="EM23" t="n">
-        <v>0.424499696785924</v>
+        <v>0.24257125530625</v>
+      </c>
+      <c r="EN23" t="n">
+        <v>0.661057692307706</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -33286,12 +33498,15 @@
         <v>1.2295081967213</v>
       </c>
       <c r="EM24" t="n">
-        <v>2.50338294993233</v>
+        <v>2.57104194857915</v>
+      </c>
+      <c r="EN24" t="n">
+        <v>3.0241935483871</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -33717,12 +33932,15 @@
         <v>4.53608247422681</v>
       </c>
       <c r="EM25" t="n">
-        <v>2.19560878243513</v>
+        <v>3.79241516966068</v>
+      </c>
+      <c r="EN25" t="n">
+        <v>3.77733598409541</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -34148,12 +34366,15 @@
         <v>1.55393053016454</v>
       </c>
       <c r="EM26" t="n">
-        <v>0.904159132007233</v>
+        <v>2.16998191681737</v>
+      </c>
+      <c r="EN26" t="n">
+        <v>2.37136465324385</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -34580,11 +34801,14 @@
       </c>
       <c r="EM27" t="n">
         <v>1.42915475704369</v>
+      </c>
+      <c r="EN27" t="n">
+        <v>2.53317249698431</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -35011,11 +35235,14 @@
       </c>
       <c r="EM28" t="n">
         <v>4.05742821473159</v>
+      </c>
+      <c r="EN28" t="n">
+        <v>4.11382616764615</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -35442,11 +35669,14 @@
       </c>
       <c r="EM29" t="n">
         <v>2.30371415138693</v>
+      </c>
+      <c r="EN29" t="n">
+        <v>1.88940092165898</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -35872,12 +36102,15 @@
         <v>0.765550239234447</v>
       </c>
       <c r="EM30" t="n">
-        <v>0.189573459715643</v>
+        <v>0.4739336492891</v>
+      </c>
+      <c r="EN30" t="n">
+        <v>0.472589792060492</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -36021,10 +36254,11 @@
       <c r="EK31"/>
       <c r="EL31"/>
       <c r="EM31"/>
+      <c r="EN31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -36451,11 +36685,14 @@
       </c>
       <c r="EM32" t="n">
         <v>0.69284064665128</v>
+      </c>
+      <c r="EN32" t="n">
+        <v>1.14155251141553</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -36881,12 +37118,15 @@
         <v>0.538213132400431</v>
       </c>
       <c r="EM33" t="n">
-        <v>1.88284518828452</v>
+        <v>1.98744769874478</v>
+      </c>
+      <c r="EN33" t="n">
+        <v>1.6649323621228</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -37313,11 +37553,14 @@
       </c>
       <c r="EM34" t="n">
         <v>3.79596678529063</v>
+      </c>
+      <c r="EN34" t="n">
+        <v>3.06242638398115</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -37743,12 +37986,15 @@
         <v>-0.2257336343115</v>
       </c>
       <c r="EM35" t="n">
-        <v>-0.218340611353699</v>
+        <v>-0.655021834061129</v>
+      </c>
+      <c r="EN35" t="n">
+        <v>-0.653594771241839</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -38174,12 +38420,15 @@
         <v>2.44392366923335</v>
       </c>
       <c r="EM36" t="n">
-        <v>2.14240705734088</v>
+        <v>2.33144297416508</v>
+      </c>
+      <c r="EN36" t="n">
+        <v>2.20839813374806</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -38606,11 +38855,14 @@
       </c>
       <c r="EM37" t="n">
         <v>3.03797468354431</v>
+      </c>
+      <c r="EN37" t="n">
+        <v>2.87141073657929</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -39037,11 +39289,14 @@
       </c>
       <c r="EM38" t="n">
         <v>2.51039809863339</v>
+      </c>
+      <c r="EN38" t="n">
+        <v>2.42102155299675</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -39467,12 +39722,15 @@
         <v>1.93236714975846</v>
       </c>
       <c r="EM39" t="n">
-        <v>1.48323939483833</v>
+        <v>1.92821121328982</v>
+      </c>
+      <c r="EN39" t="n">
+        <v>1.99471985919625</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -39899,11 +40157,14 @@
       </c>
       <c r="EM40" t="n">
         <v>9.48717948717949</v>
+      </c>
+      <c r="EN40" t="n">
+        <v>10.2564102564103</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -40329,12 +40590,15 @@
         <v>1.22173121913179</v>
       </c>
       <c r="EM41" t="n">
-        <v>0.761808024377871</v>
+        <v>0.660233621127482</v>
+      </c>
+      <c r="EN41" t="n">
+        <v>1.00250626566416</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -40761,11 +41025,14 @@
       </c>
       <c r="EM42" t="n">
         <v>2.09013716525148</v>
+      </c>
+      <c r="EN42" t="n">
+        <v>1.8818948734588</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -41191,12 +41458,15 @@
         <v>1.26382306477095</v>
       </c>
       <c r="EM43" t="n">
-        <v>1.93687230989958</v>
+        <v>1.07604017216641</v>
+      </c>
+      <c r="EN43" t="n">
+        <v>1.27208480565372</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -41622,12 +41892,15 @@
         <v>1.19412124923455</v>
       </c>
       <c r="EM44" t="n">
-        <v>0.508069336521216</v>
+        <v>1.19545726240287</v>
+      </c>
+      <c r="EN44" t="n">
+        <v>1.506646971935</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -42054,11 +42327,14 @@
       </c>
       <c r="EM45" t="n">
         <v>2.38095238095238</v>
+      </c>
+      <c r="EN45" t="n">
+        <v>2.7027027027027</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -42484,12 +42760,15 @@
         <v>1.81363352095062</v>
       </c>
       <c r="EM46" t="n">
-        <v>0.920810313075506</v>
+        <v>0.798035604665428</v>
+      </c>
+      <c r="EN46" t="n">
+        <v>1.28126906650396</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -42915,12 +43194,15 @@
         <v>1.88172043010752</v>
       </c>
       <c r="EM47" t="n">
-        <v>3.10077519379844</v>
+        <v>2.06718346253229</v>
+      </c>
+      <c r="EN47" t="n">
+        <v>1.53061224489794</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -43347,11 +43629,14 @@
       </c>
       <c r="EM48" t="n">
         <v>-1.34035423647679</v>
+      </c>
+      <c r="EN48" t="n">
+        <v>-1.37832699619771</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -43777,12 +44062,15 @@
         <v>0.344887049491292</v>
       </c>
       <c r="EM49" t="n">
-        <v>0.610827545812081</v>
+        <v>0.46021253451594</v>
+      </c>
+      <c r="EN49" t="n">
+        <v>0.456469416549091</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -44209,11 +44497,14 @@
       </c>
       <c r="EM50" t="n">
         <v>5.26315789473684</v>
+      </c>
+      <c r="EN50" t="n">
+        <v>5.43964232488824</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -44639,12 +44930,15 @@
         <v>2.56410256410255</v>
       </c>
       <c r="EM51" t="n">
-        <v>3.99999999999999</v>
+        <v>4.92307692307693</v>
+      </c>
+      <c r="EN51" t="n">
+        <v>5.19877675840977</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -45070,12 +45364,15 @@
         <v>4.4172932330827</v>
       </c>
       <c r="EM52" t="n">
-        <v>3.82029339853301</v>
+        <v>4.43154034229829</v>
+      </c>
+      <c r="EN52" t="n">
+        <v>4.10009044317155</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -45501,12 +45798,15 @@
         <v>-0.256300726185401</v>
       </c>
       <c r="EM53" t="n">
-        <v>0.921474358974352</v>
+        <v>0</v>
+      </c>
+      <c r="EN53" t="n">
+        <v>0.476379515680821</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -45933,11 +46233,14 @@
       </c>
       <c r="EM54" t="n">
         <v>-3.15457413249211</v>
+      </c>
+      <c r="EN54" t="n">
+        <v>-3.4321372854914</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -46364,11 +46667,14 @@
       </c>
       <c r="EM55" t="n">
         <v>-0.278680910357651</v>
+      </c>
+      <c r="EN55" t="n">
+        <v>-0.185185185185188</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -46794,7 +47100,10 @@
         <v>-0.333333333333338</v>
       </c>
       <c r="EM56" t="n">
-        <v>-0.319488817891356</v>
+        <v>-0.638977635782734</v>
+      </c>
+      <c r="EN56" t="n">
+        <v>0.319488817891378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on jan 28, 2025
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="209">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t xml:space="preserve">11/01/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/01/2024</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1437,10 +1440,13 @@
       <c r="EZ4" t="s">
         <v>155</v>
       </c>
+      <c r="FA4" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1902,15 +1908,18 @@
         <v>10818.4</v>
       </c>
       <c r="EY5" t="n">
-        <v>11180.8</v>
+        <v>11177</v>
       </c>
       <c r="EZ5" t="n">
-        <v>11301.5</v>
+        <v>11288.5</v>
+      </c>
+      <c r="FA5" t="n">
+        <v>11183.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2375,12 +2384,15 @@
         <v>176.5</v>
       </c>
       <c r="EZ6" t="n">
-        <v>177.5</v>
+        <v>177.6</v>
+      </c>
+      <c r="FA6" t="n">
+        <v>177.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2845,12 +2857,15 @@
         <v>27.1</v>
       </c>
       <c r="EZ7" t="n">
-        <v>27.5</v>
+        <v>27.4</v>
+      </c>
+      <c r="FA7" t="n">
+        <v>27.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3315,12 +3330,15 @@
         <v>202.9</v>
       </c>
       <c r="EZ8" t="n">
-        <v>206.4</v>
+        <v>205.4</v>
+      </c>
+      <c r="FA8" t="n">
+        <v>200.4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3786,11 +3804,14 @@
       </c>
       <c r="EZ9" t="n">
         <v>104.7</v>
+      </c>
+      <c r="FA9" t="n">
+        <v>104.1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4255,12 +4276,15 @@
         <v>1291.2</v>
       </c>
       <c r="EZ10" t="n">
-        <v>1307.8</v>
+        <v>1311.4</v>
+      </c>
+      <c r="FA10" t="n">
+        <v>1303.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4726,11 +4750,14 @@
       </c>
       <c r="EZ11" t="n">
         <v>247.5</v>
+      </c>
+      <c r="FA11" t="n">
+        <v>245.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5196,11 +5223,14 @@
       </c>
       <c r="EZ12" t="n">
         <v>124.7</v>
+      </c>
+      <c r="FA12" t="n">
+        <v>124.3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B13" t="n">
         <v>30.9</v>
@@ -5665,12 +5695,15 @@
         <v>40.8</v>
       </c>
       <c r="EZ13" t="n">
-        <v>41.2</v>
+        <v>41.3</v>
+      </c>
+      <c r="FA13" t="n">
+        <v>41.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5827,10 +5860,11 @@
       <c r="EX14"/>
       <c r="EY14"/>
       <c r="EZ14"/>
+      <c r="FA14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6296,11 +6330,14 @@
       </c>
       <c r="EZ15" t="n">
         <v>506.4</v>
+      </c>
+      <c r="FA15" t="n">
+        <v>498.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6765,12 +6802,15 @@
         <v>357.7</v>
       </c>
       <c r="EZ16" t="n">
-        <v>358.8</v>
+        <v>358.7</v>
+      </c>
+      <c r="FA16" t="n">
+        <v>356.2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -6927,10 +6967,11 @@
       <c r="EX17"/>
       <c r="EY17"/>
       <c r="EZ17"/>
+      <c r="FA17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7395,12 +7436,15 @@
         <v>69.2</v>
       </c>
       <c r="EZ18" t="n">
-        <v>69.3</v>
+        <v>69.4</v>
+      </c>
+      <c r="FA18" t="n">
+        <v>67.1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -7865,12 +7909,15 @@
         <v>472.4</v>
       </c>
       <c r="EZ19" t="n">
-        <v>474.5</v>
+        <v>474.8</v>
+      </c>
+      <c r="FA19" t="n">
+        <v>473.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8335,12 +8382,15 @@
         <v>235.7</v>
       </c>
       <c r="EZ20" t="n">
-        <v>240.2</v>
+        <v>240.9</v>
+      </c>
+      <c r="FA20" t="n">
+        <v>240.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8805,12 +8855,15 @@
         <v>149.7</v>
       </c>
       <c r="EZ21" t="n">
-        <v>151.1</v>
+        <v>151.2</v>
+      </c>
+      <c r="FA21" t="n">
+        <v>150.1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9276,11 +9329,14 @@
       </c>
       <c r="EZ22" t="n">
         <v>139.8</v>
+      </c>
+      <c r="FA22" t="n">
+        <v>137.2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9746,11 +9802,14 @@
       </c>
       <c r="EZ23" t="n">
         <v>167.5</v>
+      </c>
+      <c r="FA23" t="n">
+        <v>166.8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10216,11 +10275,14 @@
       </c>
       <c r="EZ24" t="n">
         <v>153.3</v>
+      </c>
+      <c r="FA24" t="n">
+        <v>153.2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10685,12 +10747,15 @@
         <v>52</v>
       </c>
       <c r="EZ25" t="n">
-        <v>52.2</v>
+        <v>52.4</v>
+      </c>
+      <c r="FA25" t="n">
+        <v>52.4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11155,12 +11220,15 @@
         <v>226</v>
       </c>
       <c r="EZ26" t="n">
-        <v>228.8</v>
+        <v>228.6</v>
+      </c>
+      <c r="FA26" t="n">
+        <v>228.6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11626,11 +11694,14 @@
       </c>
       <c r="EZ27" t="n">
         <v>255</v>
+      </c>
+      <c r="FA27" t="n">
+        <v>251.9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -12095,12 +12166,15 @@
         <v>333.4</v>
       </c>
       <c r="EZ28" t="n">
-        <v>336.6</v>
+        <v>336.4</v>
+      </c>
+      <c r="FA28" t="n">
+        <v>332.7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12566,11 +12640,14 @@
       </c>
       <c r="EZ29" t="n">
         <v>221.1</v>
+      </c>
+      <c r="FA29" t="n">
+        <v>216.2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -13035,12 +13112,15 @@
         <v>106</v>
       </c>
       <c r="EZ30" t="n">
-        <v>106.3</v>
+        <v>106.4</v>
+      </c>
+      <c r="FA30" t="n">
+        <v>102.7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -13197,10 +13277,11 @@
       <c r="EX31"/>
       <c r="EY31"/>
       <c r="EZ31"/>
+      <c r="FA31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -13666,11 +13747,14 @@
       </c>
       <c r="EZ32" t="n">
         <v>44.3</v>
+      </c>
+      <c r="FA32" t="n">
+        <v>44.6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -14135,12 +14219,15 @@
         <v>97.5</v>
       </c>
       <c r="EZ33" t="n">
+        <v>97.7</v>
+      </c>
+      <c r="FA33" t="n">
         <v>97.7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -14605,12 +14692,15 @@
         <v>87.5</v>
       </c>
       <c r="EZ34" t="n">
-        <v>87.5</v>
+        <v>88.7</v>
+      </c>
+      <c r="FA34" t="n">
+        <v>89.2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -15075,12 +15165,15 @@
         <v>45.5</v>
       </c>
       <c r="EZ35" t="n">
-        <v>45.6</v>
+        <v>45.5</v>
+      </c>
+      <c r="FA35" t="n">
+        <v>45.2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B36" t="n">
         <v>307.9</v>
@@ -15545,12 +15638,15 @@
         <v>324.8</v>
       </c>
       <c r="EZ36" t="n">
-        <v>328.6</v>
+        <v>328.7</v>
+      </c>
+      <c r="FA36" t="n">
+        <v>326.7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -16016,11 +16112,14 @@
       </c>
       <c r="EZ37" t="n">
         <v>82.4</v>
+      </c>
+      <c r="FA37" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -16486,11 +16585,14 @@
       </c>
       <c r="EZ38" t="n">
         <v>693.8</v>
+      </c>
+      <c r="FA38" t="n">
+        <v>696.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -16956,11 +17058,14 @@
       </c>
       <c r="EZ39" t="n">
         <v>347.7</v>
+      </c>
+      <c r="FA39" t="n">
+        <v>344.7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -17426,11 +17531,14 @@
       </c>
       <c r="EZ40" t="n">
         <v>43</v>
+      </c>
+      <c r="FA40" t="n">
+        <v>42.8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -17895,12 +18003,15 @@
         <v>396.4</v>
       </c>
       <c r="EZ41" t="n">
-        <v>403</v>
+        <v>401.8</v>
+      </c>
+      <c r="FA41" t="n">
+        <v>396.9</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -18365,12 +18476,15 @@
         <v>156.3</v>
       </c>
       <c r="EZ42" t="n">
-        <v>157</v>
+        <v>157.2</v>
+      </c>
+      <c r="FA42" t="n">
+        <v>157.1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -18835,12 +18949,15 @@
         <v>140.9</v>
       </c>
       <c r="EZ43" t="n">
-        <v>143.3</v>
+        <v>143.5</v>
+      </c>
+      <c r="FA43" t="n">
+        <v>142.7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -19306,11 +19423,14 @@
       </c>
       <c r="EZ44" t="n">
         <v>343.6</v>
+      </c>
+      <c r="FA44" t="n">
+        <v>339.7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B45" t="n">
         <v>31</v>
@@ -19776,11 +19896,14 @@
       </c>
       <c r="EZ45" t="n">
         <v>30.4</v>
+      </c>
+      <c r="FA45" t="n">
+        <v>30.5</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B46" t="n">
         <v>158.2</v>
@@ -20246,11 +20369,14 @@
       </c>
       <c r="EZ46" t="n">
         <v>166</v>
+      </c>
+      <c r="FA46" t="n">
+        <v>164.1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -20716,11 +20842,14 @@
       </c>
       <c r="EZ47" t="n">
         <v>39.8</v>
+      </c>
+      <c r="FA47" t="n">
+        <v>39.5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -21185,12 +21314,15 @@
         <v>206.1</v>
       </c>
       <c r="EZ48" t="n">
-        <v>207.5</v>
+        <v>207.4</v>
+      </c>
+      <c r="FA48" t="n">
+        <v>206.3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -21655,12 +21787,15 @@
         <v>1200.6</v>
       </c>
       <c r="EZ49" t="n">
-        <v>1210.4</v>
+        <v>1209.8</v>
+      </c>
+      <c r="FA49" t="n">
+        <v>1208.1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -22126,11 +22261,14 @@
       </c>
       <c r="EZ50" t="n">
         <v>141.5</v>
+      </c>
+      <c r="FA50" t="n">
+        <v>141.3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -22596,11 +22734,14 @@
       </c>
       <c r="EZ51" t="n">
         <v>34.4</v>
+      </c>
+      <c r="FA51" t="n">
+        <v>34.1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -23065,12 +23206,15 @@
         <v>341.7</v>
       </c>
       <c r="EZ52" t="n">
-        <v>345.3</v>
+        <v>345.4</v>
+      </c>
+      <c r="FA52" t="n">
+        <v>341.1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -23535,12 +23679,15 @@
         <v>249.6</v>
       </c>
       <c r="EZ53" t="n">
-        <v>253.1</v>
+        <v>254.1</v>
+      </c>
+      <c r="FA53" t="n">
+        <v>250.4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -24005,12 +24152,15 @@
         <v>61.4</v>
       </c>
       <c r="EZ54" t="n">
-        <v>61.9</v>
+        <v>62.1</v>
+      </c>
+      <c r="FA54" t="n">
+        <v>61.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -24475,12 +24625,15 @@
         <v>214.7</v>
       </c>
       <c r="EZ55" t="n">
-        <v>215.6</v>
+        <v>215.5</v>
+      </c>
+      <c r="FA55" t="n">
+        <v>212.1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -24946,6 +25099,9 @@
       </c>
       <c r="EZ56" t="n">
         <v>31.4</v>
+      </c>
+      <c r="FA56" t="n">
+        <v>31.3</v>
       </c>
     </row>
   </sheetData>
@@ -25395,10 +25551,13 @@
       <c r="EN4" t="s">
         <v>155</v>
       </c>
+      <c r="EO4" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -25824,15 +25983,18 @@
         <v>1.45261874619027</v>
       </c>
       <c r="EM5" t="n">
-        <v>1.45456195272446</v>
+        <v>1.42008075858627</v>
       </c>
       <c r="EN5" t="n">
-        <v>1.44973070017953</v>
+        <v>1.33303411131059</v>
+      </c>
+      <c r="EO5" t="n">
+        <v>1.234757891497</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -26261,12 +26423,15 @@
         <v>0.512528473804087</v>
       </c>
       <c r="EN6" t="n">
-        <v>0.509626274065672</v>
+        <v>0.566251415628523</v>
+      </c>
+      <c r="EO6" t="n">
+        <v>0.453001132502838</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -26695,12 +26860,15 @@
         <v>-4.24028268551235</v>
       </c>
       <c r="EN7" t="n">
-        <v>-4.18118466898956</v>
+        <v>-4.52961672473869</v>
+      </c>
+      <c r="EO7" t="n">
+        <v>-5.20833333333332</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -27129,12 +27297,15 @@
         <v>0.844930417495024</v>
       </c>
       <c r="EN8" t="n">
-        <v>1.67487684729064</v>
+        <v>1.18226600985222</v>
+      </c>
+      <c r="EO8" t="n">
+        <v>2.40163515585079</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -27564,11 +27735,14 @@
       </c>
       <c r="EN9" t="n">
         <v>1.06177606177606</v>
+      </c>
+      <c r="EO9" t="n">
+        <v>1.16618075801748</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -27997,12 +28171,15 @@
         <v>3.1062844366366</v>
       </c>
       <c r="EN10" t="n">
-        <v>2.68530150753771</v>
+        <v>2.96796482412062</v>
+      </c>
+      <c r="EO10" t="n">
+        <v>2.78347263838511</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -28432,11 +28609,14 @@
       </c>
       <c r="EN11" t="n">
         <v>4.07905803195963</v>
+      </c>
+      <c r="EO11" t="n">
+        <v>3.84778012684989</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -28866,11 +29046,14 @@
       </c>
       <c r="EN12" t="n">
         <v>-1.81102362204724</v>
+      </c>
+      <c r="EO12" t="n">
+        <v>-1.6613924050633</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B13" t="n">
         <v>-1.61812297734628</v>
@@ -29299,12 +29482,15 @@
         <v>2.77078085642316</v>
       </c>
       <c r="EN13" t="n">
-        <v>2.23325062034741</v>
+        <v>2.48138957816377</v>
+      </c>
+      <c r="EO13" t="n">
+        <v>2.2167487684729</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -29449,10 +29635,11 @@
       <c r="EL14"/>
       <c r="EM14"/>
       <c r="EN14"/>
+      <c r="EO14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -29882,11 +30069,14 @@
       </c>
       <c r="EN15" t="n">
         <v>1.82988135934044</v>
+      </c>
+      <c r="EO15" t="n">
+        <v>1.58891831330211</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -30315,12 +30505,15 @@
         <v>1.38888888888888</v>
       </c>
       <c r="EN16" t="n">
-        <v>1.32730866986727</v>
+        <v>1.29906805987008</v>
+      </c>
+      <c r="EO16" t="n">
+        <v>0.849377123442809</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -30465,10 +30658,11 @@
       <c r="EL17"/>
       <c r="EM17"/>
       <c r="EN17"/>
+      <c r="EO17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -30897,12 +31091,15 @@
         <v>6.79012345679011</v>
       </c>
       <c r="EN18" t="n">
-        <v>6.28834355828222</v>
+        <v>6.44171779141107</v>
+      </c>
+      <c r="EO18" t="n">
+        <v>5.17241379310344</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -31331,12 +31528,15 @@
         <v>4.53640185881834</v>
       </c>
       <c r="EN19" t="n">
-        <v>3.988603988604</v>
+        <v>4.05435020819636</v>
+      </c>
+      <c r="EO19" t="n">
+        <v>5.46143557735176</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -31765,12 +31965,15 @@
         <v>1.1587982832618</v>
       </c>
       <c r="EN20" t="n">
-        <v>1.86598812553011</v>
+        <v>2.16284987277353</v>
+      </c>
+      <c r="EO20" t="n">
+        <v>3.13573883161511</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -32199,12 +32402,15 @@
         <v>0.74024226110363</v>
       </c>
       <c r="EN21" t="n">
-        <v>0.935203740814967</v>
+        <v>1.00200400801603</v>
+      </c>
+      <c r="EO21" t="n">
+        <v>1.28205128205129</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -32634,11 +32840,14 @@
       </c>
       <c r="EN22" t="n">
         <v>1.08459869848156</v>
+      </c>
+      <c r="EO22" t="n">
+        <v>1.62962962962962</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -33068,11 +33277,14 @@
       </c>
       <c r="EN23" t="n">
         <v>0.661057692307706</v>
+      </c>
+      <c r="EO23" t="n">
+        <v>0.66385033192518</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -33502,11 +33714,14 @@
       </c>
       <c r="EN24" t="n">
         <v>3.0241935483871</v>
+      </c>
+      <c r="EO24" t="n">
+        <v>3.16498316498316</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -33935,12 +34150,15 @@
         <v>3.79241516966068</v>
       </c>
       <c r="EN25" t="n">
-        <v>3.77733598409541</v>
+        <v>4.17495029821072</v>
+      </c>
+      <c r="EO25" t="n">
+        <v>4.3824701195219</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -34369,12 +34587,15 @@
         <v>2.16998191681737</v>
       </c>
       <c r="EN26" t="n">
-        <v>2.37136465324385</v>
+        <v>2.28187919463088</v>
+      </c>
+      <c r="EO26" t="n">
+        <v>2.14477211796246</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -34804,11 +35025,14 @@
       </c>
       <c r="EN27" t="n">
         <v>2.53317249698431</v>
+      </c>
+      <c r="EO27" t="n">
+        <v>1.61355385235982</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -35237,12 +35461,15 @@
         <v>4.05742821473159</v>
       </c>
       <c r="EN28" t="n">
-        <v>4.11382616764615</v>
+        <v>4.05196412001236</v>
+      </c>
+      <c r="EO28" t="n">
+        <v>4.13145539906105</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -35672,11 +35899,14 @@
       </c>
       <c r="EN29" t="n">
         <v>1.88940092165898</v>
+      </c>
+      <c r="EO29" t="n">
+        <v>2.46445497630333</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -36105,12 +36335,15 @@
         <v>0.4739336492891</v>
       </c>
       <c r="EN30" t="n">
-        <v>0.472589792060492</v>
+        <v>0.567107750472584</v>
+      </c>
+      <c r="EO30" t="n">
+        <v>0.785083415112839</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -36255,10 +36488,11 @@
       <c r="EL31"/>
       <c r="EM31"/>
       <c r="EN31"/>
+      <c r="EO31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -36688,11 +36922,14 @@
       </c>
       <c r="EN32" t="n">
         <v>1.14155251141553</v>
+      </c>
+      <c r="EO32" t="n">
+        <v>0.904977375565592</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -37122,11 +37359,14 @@
       </c>
       <c r="EN33" t="n">
         <v>1.6649323621228</v>
+      </c>
+      <c r="EO33" t="n">
+        <v>2.51836306400839</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -37555,12 +37795,15 @@
         <v>3.79596678529063</v>
       </c>
       <c r="EN34" t="n">
-        <v>3.06242638398115</v>
+        <v>4.47585394581861</v>
+      </c>
+      <c r="EO34" t="n">
+        <v>5.18867924528301</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -37989,12 +38232,15 @@
         <v>-0.655021834061129</v>
       </c>
       <c r="EN35" t="n">
-        <v>-0.653594771241839</v>
+        <v>-0.871459694989104</v>
+      </c>
+      <c r="EO35" t="n">
+        <v>-0.220750551876383</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B36" t="n">
         <v>2.5657681065281</v>
@@ -38423,12 +38669,15 @@
         <v>2.33144297416508</v>
       </c>
       <c r="EN36" t="n">
-        <v>2.20839813374806</v>
+        <v>2.23950233281494</v>
+      </c>
+      <c r="EO36" t="n">
+        <v>1.68067226890756</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -38858,11 +39107,14 @@
       </c>
       <c r="EN37" t="n">
         <v>2.87141073657929</v>
+      </c>
+      <c r="EO37" t="n">
+        <v>2.01511335012594</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -39292,11 +39544,14 @@
       </c>
       <c r="EN38" t="n">
         <v>2.42102155299675</v>
+      </c>
+      <c r="EO38" t="n">
+        <v>2.35259520658727</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -39726,11 +39981,14 @@
       </c>
       <c r="EN39" t="n">
         <v>1.99471985919625</v>
+      </c>
+      <c r="EO39" t="n">
+        <v>1.95208518189884</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -40160,11 +40418,14 @@
       </c>
       <c r="EN40" t="n">
         <v>10.2564102564103</v>
+      </c>
+      <c r="EO40" t="n">
+        <v>8.9058524173028</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -40593,12 +40854,15 @@
         <v>0.660233621127482</v>
       </c>
       <c r="EN41" t="n">
-        <v>1.00250626566416</v>
+        <v>0.701754385964901</v>
+      </c>
+      <c r="EO41" t="n">
+        <v>1.09526235354052</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -41027,12 +41291,15 @@
         <v>2.09013716525148</v>
       </c>
       <c r="EN42" t="n">
-        <v>1.8818948734588</v>
+        <v>2.01168072680078</v>
+      </c>
+      <c r="EO42" t="n">
+        <v>2.61267145656434</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -41461,12 +41728,15 @@
         <v>1.07604017216641</v>
       </c>
       <c r="EN43" t="n">
-        <v>1.27208480565372</v>
+        <v>1.41342756183746</v>
+      </c>
+      <c r="EO43" t="n">
+        <v>1.34943181818182</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -41896,11 +42166,14 @@
       </c>
       <c r="EN44" t="n">
         <v>1.506646971935</v>
+      </c>
+      <c r="EO44" t="n">
+        <v>1.40298507462686</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B45" t="n">
         <v>0.322580645161295</v>
@@ -42330,11 +42603,14 @@
       </c>
       <c r="EN45" t="n">
         <v>2.7027027027027</v>
+      </c>
+      <c r="EO45" t="n">
+        <v>2.6936026936027</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B46" t="n">
         <v>0.758533501896345</v>
@@ -42764,11 +43040,14 @@
       </c>
       <c r="EN46" t="n">
         <v>1.28126906650396</v>
+      </c>
+      <c r="EO46" t="n">
+        <v>1.23380629241211</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -43198,11 +43477,14 @@
       </c>
       <c r="EN47" t="n">
         <v>1.53061224489794</v>
+      </c>
+      <c r="EO47" t="n">
+        <v>1.54241645244214</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -43631,12 +43913,15 @@
         <v>-1.34035423647679</v>
       </c>
       <c r="EN48" t="n">
-        <v>-1.37832699619771</v>
+        <v>-1.42585551330798</v>
+      </c>
+      <c r="EO48" t="n">
+        <v>-1.14997604216579</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -44065,12 +44350,15 @@
         <v>0.46021253451594</v>
       </c>
       <c r="EN49" t="n">
-        <v>0.456469416549091</v>
+        <v>0.406672752925543</v>
+      </c>
+      <c r="EO49" t="n">
+        <v>0.215678141849847</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -44500,11 +44788,14 @@
       </c>
       <c r="EN50" t="n">
         <v>5.43964232488824</v>
+      </c>
+      <c r="EO50" t="n">
+        <v>5.52651232262885</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -44934,11 +45225,14 @@
       </c>
       <c r="EN51" t="n">
         <v>5.19877675840977</v>
+      </c>
+      <c r="EO51" t="n">
+        <v>4.60122699386501</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -45367,12 +45661,15 @@
         <v>4.43154034229829</v>
       </c>
       <c r="EN52" t="n">
-        <v>4.10009044317155</v>
+        <v>4.13023816701839</v>
+      </c>
+      <c r="EO52" t="n">
+        <v>4.59981600735971</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -45801,12 +46098,15 @@
         <v>0</v>
       </c>
       <c r="EN53" t="n">
-        <v>0.476379515680821</v>
+        <v>0.873362445414843</v>
+      </c>
+      <c r="EO53" t="n">
+        <v>-0.278773397052974</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -46235,12 +46535,15 @@
         <v>-3.15457413249211</v>
       </c>
       <c r="EN54" t="n">
-        <v>-3.4321372854914</v>
+        <v>-3.1201248049922</v>
+      </c>
+      <c r="EO54" t="n">
+        <v>-3.1496062992126</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -46669,12 +46972,15 @@
         <v>-0.278680910357651</v>
       </c>
       <c r="EN55" t="n">
-        <v>-0.185185185185188</v>
+        <v>-0.231481481481481</v>
+      </c>
+      <c r="EO55" t="n">
+        <v>-0.934142923867352</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -47104,6 +47410,9 @@
       </c>
       <c r="EN56" t="n">
         <v>0.319488817891378</v>
+      </c>
+      <c r="EO56" t="n">
+        <v>0.320512820512825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update, Apr 18
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t xml:space="preserve">02/01/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/01/2025</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1455,10 +1458,13 @@
       <c r="FC4" t="s">
         <v>158</v>
       </c>
+      <c r="FD4" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1929,15 +1935,18 @@
         <v>11184.6</v>
       </c>
       <c r="FB5" t="n">
-        <v>10898.3</v>
+        <v>10902.9</v>
       </c>
       <c r="FC5" t="n">
-        <v>11241.8</v>
+        <v>11231.6</v>
+      </c>
+      <c r="FD5" t="n">
+        <v>11290.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2411,12 +2420,15 @@
         <v>177.1</v>
       </c>
       <c r="FC6" t="n">
-        <v>179.6</v>
+        <v>179.7</v>
+      </c>
+      <c r="FD6" t="n">
+        <v>180.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2890,12 +2902,15 @@
         <v>28.2</v>
       </c>
       <c r="FC7" t="n">
+        <v>29</v>
+      </c>
+      <c r="FD7" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3369,12 +3384,15 @@
         <v>195.9</v>
       </c>
       <c r="FC8" t="n">
-        <v>203.5</v>
+        <v>204</v>
+      </c>
+      <c r="FD8" t="n">
+        <v>202.9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3849,11 +3867,14 @@
       </c>
       <c r="FC9" t="n">
         <v>102.8</v>
+      </c>
+      <c r="FD9" t="n">
+        <v>103.1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4327,12 +4348,15 @@
         <v>1293.2</v>
       </c>
       <c r="FC10" t="n">
-        <v>1304.1</v>
+        <v>1301.5</v>
+      </c>
+      <c r="FD10" t="n">
+        <v>1322</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4806,12 +4830,15 @@
         <v>232.9</v>
       </c>
       <c r="FC11" t="n">
-        <v>241.9</v>
+        <v>241.7</v>
+      </c>
+      <c r="FD11" t="n">
+        <v>243.7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5285,12 +5312,15 @@
         <v>123.2</v>
       </c>
       <c r="FC12" t="n">
-        <v>124.6</v>
+        <v>124.5</v>
+      </c>
+      <c r="FD12" t="n">
+        <v>125.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B13" t="n">
         <v>30.2</v>
@@ -5764,12 +5794,15 @@
         <v>37.8</v>
       </c>
       <c r="FC13" t="n">
-        <v>39.8</v>
+        <v>39.2</v>
+      </c>
+      <c r="FD13" t="n">
+        <v>40.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5929,10 +5962,11 @@
       <c r="FA14"/>
       <c r="FB14"/>
       <c r="FC14"/>
+      <c r="FD14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6406,12 +6440,15 @@
         <v>495.5</v>
       </c>
       <c r="FC15" t="n">
-        <v>503.5</v>
+        <v>504.1</v>
+      </c>
+      <c r="FD15" t="n">
+        <v>505.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6886,11 +6923,14 @@
       </c>
       <c r="FC16" t="n">
         <v>357.3</v>
+      </c>
+      <c r="FD16" t="n">
+        <v>357.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -7050,10 +7090,11 @@
       <c r="FA17"/>
       <c r="FB17"/>
       <c r="FC17"/>
+      <c r="FD17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7528,11 +7569,14 @@
       </c>
       <c r="FC18" t="n">
         <v>63.9</v>
+      </c>
+      <c r="FD18" t="n">
+        <v>64.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -8006,12 +8050,15 @@
         <v>448.6</v>
       </c>
       <c r="FC19" t="n">
-        <v>464.8</v>
+        <v>469.2</v>
+      </c>
+      <c r="FD19" t="n">
+        <v>475.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8485,12 +8532,15 @@
         <v>224.8</v>
       </c>
       <c r="FC20" t="n">
-        <v>229.6</v>
+        <v>239.7</v>
+      </c>
+      <c r="FD20" t="n">
+        <v>243.7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -8964,12 +9014,15 @@
         <v>147.5</v>
       </c>
       <c r="FC21" t="n">
-        <v>150.2</v>
+        <v>150.4</v>
+      </c>
+      <c r="FD21" t="n">
+        <v>149.6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9443,12 +9496,15 @@
         <v>130</v>
       </c>
       <c r="FC22" t="n">
-        <v>137.9</v>
+        <v>137.5</v>
+      </c>
+      <c r="FD22" t="n">
+        <v>138.3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9922,12 +9978,15 @@
         <v>159.1</v>
       </c>
       <c r="FC23" t="n">
-        <v>163.6</v>
+        <v>166</v>
+      </c>
+      <c r="FD23" t="n">
+        <v>166.8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10401,12 +10460,15 @@
         <v>150</v>
       </c>
       <c r="FC24" t="n">
-        <v>151.8</v>
+        <v>152.4</v>
+      </c>
+      <c r="FD24" t="n">
+        <v>150.6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10880,12 +10942,15 @@
         <v>48.2</v>
       </c>
       <c r="FC25" t="n">
-        <v>49.5</v>
+        <v>49</v>
+      </c>
+      <c r="FD25" t="n">
+        <v>49.3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11360,11 +11425,14 @@
       </c>
       <c r="FC26" t="n">
         <v>232.2</v>
+      </c>
+      <c r="FD26" t="n">
+        <v>235.7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11838,12 +11906,15 @@
         <v>238.8</v>
       </c>
       <c r="FC27" t="n">
-        <v>246.4</v>
+        <v>246.2</v>
+      </c>
+      <c r="FD27" t="n">
+        <v>248.1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -12318,11 +12389,14 @@
       </c>
       <c r="FC28" t="n">
         <v>324.5</v>
+      </c>
+      <c r="FD28" t="n">
+        <v>325.2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12796,12 +12870,15 @@
         <v>210.5</v>
       </c>
       <c r="FC29" t="n">
-        <v>214.4</v>
+        <v>214.3</v>
+      </c>
+      <c r="FD29" t="n">
+        <v>213.8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -13275,12 +13352,15 @@
         <v>102.1</v>
       </c>
       <c r="FC30" t="n">
-        <v>105.6</v>
+        <v>105.4</v>
+      </c>
+      <c r="FD30" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -13440,10 +13520,11 @@
       <c r="FA31"/>
       <c r="FB31"/>
       <c r="FC31"/>
+      <c r="FD31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -13918,11 +13999,14 @@
       </c>
       <c r="FC32" t="n">
         <v>43</v>
+      </c>
+      <c r="FD32" t="n">
+        <v>43.2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -14397,11 +14481,14 @@
       </c>
       <c r="FC33" t="n">
         <v>97.1</v>
+      </c>
+      <c r="FD33" t="n">
+        <v>96.9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -14876,11 +14963,14 @@
       </c>
       <c r="FC34" t="n">
         <v>89.9</v>
+      </c>
+      <c r="FD34" t="n">
+        <v>90.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -15355,11 +15445,14 @@
       </c>
       <c r="FC35" t="n">
         <v>45.7</v>
+      </c>
+      <c r="FD35" t="n">
+        <v>45.6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B36" t="n">
         <v>314.2</v>
@@ -15833,12 +15926,15 @@
         <v>321.7</v>
       </c>
       <c r="FC36" t="n">
-        <v>339.2</v>
+        <v>338.9</v>
+      </c>
+      <c r="FD36" t="n">
+        <v>338.5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -16313,11 +16409,14 @@
       </c>
       <c r="FC37" t="n">
         <v>81.6</v>
+      </c>
+      <c r="FD37" t="n">
+        <v>82.1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -16792,11 +16891,14 @@
       </c>
       <c r="FC38" t="n">
         <v>679.3</v>
+      </c>
+      <c r="FD38" t="n">
+        <v>678.8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -17271,11 +17373,14 @@
       </c>
       <c r="FC39" t="n">
         <v>348.8</v>
+      </c>
+      <c r="FD39" t="n">
+        <v>350.7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -17750,11 +17855,14 @@
       </c>
       <c r="FC40" t="n">
         <v>40.3</v>
+      </c>
+      <c r="FD40" t="n">
+        <v>40.2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -18228,12 +18336,15 @@
         <v>378.5</v>
       </c>
       <c r="FC41" t="n">
-        <v>390.4</v>
+        <v>392.2</v>
+      </c>
+      <c r="FD41" t="n">
+        <v>394.9</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -18707,12 +18818,15 @@
         <v>146.2</v>
       </c>
       <c r="FC42" t="n">
-        <v>154</v>
+        <v>154.5</v>
+      </c>
+      <c r="FD42" t="n">
+        <v>155.6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -19186,12 +19300,15 @@
         <v>142.6</v>
       </c>
       <c r="FC43" t="n">
-        <v>146.4</v>
+        <v>146.1</v>
+      </c>
+      <c r="FD43" t="n">
+        <v>146.6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -19666,11 +19783,14 @@
       </c>
       <c r="FC44" t="n">
         <v>339.8</v>
+      </c>
+      <c r="FD44" t="n">
+        <v>341.5</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B45" t="n">
         <v>31.3</v>
@@ -20145,11 +20265,14 @@
       </c>
       <c r="FC45" t="n">
         <v>30.1</v>
+      </c>
+      <c r="FD45" t="n">
+        <v>30.3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B46" t="n">
         <v>159.1</v>
@@ -20623,12 +20746,15 @@
         <v>166.1</v>
       </c>
       <c r="FC46" t="n">
-        <v>169.3</v>
+        <v>170.1</v>
+      </c>
+      <c r="FD46" t="n">
+        <v>170.5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -21103,11 +21229,14 @@
       </c>
       <c r="FC47" t="n">
         <v>39</v>
+      </c>
+      <c r="FD47" t="n">
+        <v>39.2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -21581,12 +21710,15 @@
         <v>205.3</v>
       </c>
       <c r="FC48" t="n">
-        <v>215.6</v>
+        <v>215.9</v>
+      </c>
+      <c r="FD48" t="n">
+        <v>216.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -22060,12 +22192,15 @@
         <v>1192.3</v>
       </c>
       <c r="FC49" t="n">
-        <v>1222.2</v>
+        <v>1222</v>
+      </c>
+      <c r="FD49" t="n">
+        <v>1226.8</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -22540,11 +22675,14 @@
       </c>
       <c r="FC50" t="n">
         <v>138.5</v>
+      </c>
+      <c r="FD50" t="n">
+        <v>138.9</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -23018,12 +23156,15 @@
         <v>32</v>
       </c>
       <c r="FC51" t="n">
-        <v>33.7</v>
+        <v>33.2</v>
+      </c>
+      <c r="FD51" t="n">
+        <v>33.4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -23497,12 +23638,15 @@
         <v>323.6</v>
       </c>
       <c r="FC52" t="n">
-        <v>337.1</v>
+        <v>338</v>
+      </c>
+      <c r="FD52" t="n">
+        <v>340.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -23976,12 +24120,15 @@
         <v>266.9</v>
       </c>
       <c r="FC53" t="n">
-        <v>268.2</v>
+        <v>269</v>
+      </c>
+      <c r="FD53" t="n">
+        <v>267.4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -24455,12 +24602,15 @@
         <v>57.6</v>
       </c>
       <c r="FC54" t="n">
-        <v>61.8</v>
+        <v>62.1</v>
+      </c>
+      <c r="FD54" t="n">
+        <v>62.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -24934,12 +25084,15 @@
         <v>204.5</v>
       </c>
       <c r="FC55" t="n">
-        <v>214.2</v>
+        <v>213.8</v>
+      </c>
+      <c r="FD55" t="n">
+        <v>213.4</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -25413,7 +25566,10 @@
         <v>29.3</v>
       </c>
       <c r="FC56" t="n">
-        <v>31.1</v>
+        <v>31.3</v>
+      </c>
+      <c r="FD56" t="n">
+        <v>31.7</v>
       </c>
     </row>
   </sheetData>
@@ -25872,10 +26028,13 @@
       <c r="EQ4" t="s">
         <v>158</v>
       </c>
+      <c r="ER4" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -26310,15 +26469,18 @@
         <v>1.30427694147057</v>
       </c>
       <c r="EP5" t="n">
-        <v>1.72587600574981</v>
+        <v>1.76881288853214</v>
       </c>
       <c r="EQ5" t="n">
-        <v>1.22458535179816</v>
+        <v>1.13274145041329</v>
+      </c>
+      <c r="ER5" t="n">
+        <v>1.16389506128594</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -26756,12 +26918,15 @@
         <v>1.08447488584475</v>
       </c>
       <c r="EQ6" t="n">
-        <v>0.785634118967471</v>
+        <v>0.841750841750842</v>
+      </c>
+      <c r="ER6" t="n">
+        <v>0.612131329994448</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -27200,11 +27365,14 @@
       </c>
       <c r="EQ7" t="n">
         <v>-0.343642611683854</v>
+      </c>
+      <c r="ER7" t="n">
+        <v>-0.684931506849313</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -27642,12 +27810,15 @@
         <v>-3.63994097393015</v>
       </c>
       <c r="EQ8" t="n">
-        <v>-2.5849688846338</v>
+        <v>-2.34561991383437</v>
+      </c>
+      <c r="ER8" t="n">
+        <v>-1.83841315916787</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -28086,11 +28257,14 @@
       </c>
       <c r="EQ9" t="n">
         <v>0.784313725490207</v>
+      </c>
+      <c r="ER9" t="n">
+        <v>0.683593750000003</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -28528,12 +28702,15 @@
         <v>3.38983050847458</v>
       </c>
       <c r="EQ10" t="n">
-        <v>3.59043609500356</v>
+        <v>3.38390658511398</v>
+      </c>
+      <c r="ER10" t="n">
+        <v>3.29739021722144</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -28971,12 +29148,15 @@
         <v>5.00450856627592</v>
       </c>
       <c r="EQ11" t="n">
-        <v>4.58279290964116</v>
+        <v>4.49632511889321</v>
+      </c>
+      <c r="ER11" t="n">
+        <v>4.23438836612488</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -29414,12 +29594,15 @@
         <v>-1.36108887109687</v>
       </c>
       <c r="EQ12" t="n">
-        <v>-1.11111111111112</v>
+        <v>-1.19047619047619</v>
+      </c>
+      <c r="ER12" t="n">
+        <v>-1.10410094637223</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B13" t="n">
         <v>-1.98675496688743</v>
@@ -29857,12 +30040,15 @@
         <v>4.70914127423822</v>
       </c>
       <c r="EQ13" t="n">
-        <v>4.18848167539266</v>
+        <v>2.61780104712042</v>
+      </c>
+      <c r="ER13" t="n">
+        <v>2.29007633587788</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -30010,10 +30196,11 @@
       <c r="EO14"/>
       <c r="EP14"/>
       <c r="EQ14"/>
+      <c r="ER14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -30451,12 +30638,15 @@
         <v>0.364593882924855</v>
       </c>
       <c r="EQ15" t="n">
-        <v>0.639616230261852</v>
+        <v>0.759544273435952</v>
+      </c>
+      <c r="ER15" t="n">
+        <v>0.978434504792328</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -30895,11 +31085,14 @@
       </c>
       <c r="EQ16" t="n">
         <v>1.73690205011389</v>
+      </c>
+      <c r="ER16" t="n">
+        <v>1.93677015095413</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -31047,10 +31240,11 @@
       <c r="EO17"/>
       <c r="EP17"/>
       <c r="EQ17"/>
+      <c r="ER17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -31489,11 +31683,14 @@
       </c>
       <c r="EQ18" t="n">
         <v>-0.930232558139526</v>
+      </c>
+      <c r="ER18" t="n">
+        <v>-0.772797527047913</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -31931,12 +32128,15 @@
         <v>2.49029015307289</v>
       </c>
       <c r="EQ19" t="n">
-        <v>2.28873239436621</v>
+        <v>3.25704225352113</v>
+      </c>
+      <c r="ER19" t="n">
+        <v>3.59790667248147</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -32374,12 +32574,15 @@
         <v>-1.48992112182296</v>
       </c>
       <c r="EQ20" t="n">
-        <v>-1.88034188034188</v>
+        <v>2.43589743589743</v>
+      </c>
+      <c r="ER20" t="n">
+        <v>2.43799915931065</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -32817,12 +33020,15 @@
         <v>2.28848821081832</v>
       </c>
       <c r="EQ21" t="n">
-        <v>0.940860215053748</v>
+        <v>1.0752688172043</v>
+      </c>
+      <c r="ER21" t="n">
+        <v>0.133868808567596</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -33260,12 +33466,15 @@
         <v>-2.32907588279489</v>
       </c>
       <c r="EQ22" t="n">
-        <v>0.0725689404934853</v>
+        <v>-0.217706821480394</v>
+      </c>
+      <c r="ER22" t="n">
+        <v>0.508720930232571</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -33703,12 +33912,15 @@
         <v>-0.624609618988132</v>
       </c>
       <c r="EQ23" t="n">
-        <v>-0.365408038976854</v>
+        <v>1.09622411693058</v>
+      </c>
+      <c r="ER23" t="n">
+        <v>0.724637681159431</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -34146,12 +34358,15 @@
         <v>0.671140939597315</v>
       </c>
       <c r="EQ24" t="n">
-        <v>0.729927007299285</v>
+        <v>1.1280690112807</v>
+      </c>
+      <c r="ER24" t="n">
+        <v>0.266311584553951</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -34589,12 +34804,15 @@
         <v>-1.43149284253579</v>
       </c>
       <c r="EQ25" t="n">
-        <v>-0.602409638554211</v>
+        <v>-1.60642570281124</v>
+      </c>
+      <c r="ER25" t="n">
+        <v>-1.20240480961923</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -35033,11 +35251,14 @@
       </c>
       <c r="EQ26" t="n">
         <v>4.03225806451612</v>
+      </c>
+      <c r="ER26" t="n">
+        <v>3.97000441111601</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -35475,12 +35696,15 @@
         <v>0.420521446593776</v>
       </c>
       <c r="EQ27" t="n">
-        <v>0</v>
+        <v>-0.0811688311688265</v>
+      </c>
+      <c r="ER27" t="n">
+        <v>-0.201126307321009</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -35919,11 +36143,14 @@
       </c>
       <c r="EQ28" t="n">
         <v>1.43794935917475</v>
+      </c>
+      <c r="ER28" t="n">
+        <v>1.37157107231919</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -36361,12 +36588,15 @@
         <v>0.765916706558173</v>
       </c>
       <c r="EQ29" t="n">
-        <v>0.657276995305167</v>
+        <v>0.610328638497658</v>
+      </c>
+      <c r="ER29" t="n">
+        <v>-0.511865984178685</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -36804,12 +37034,15 @@
         <v>0.889328063241112</v>
       </c>
       <c r="EQ30" t="n">
-        <v>1.05263157894738</v>
+        <v>0.861244019138761</v>
+      </c>
+      <c r="ER30" t="n">
+        <v>0.286532951289396</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -36957,10 +37190,11 @@
       <c r="EO31"/>
       <c r="EP31"/>
       <c r="EQ31"/>
+      <c r="ER31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -37399,11 +37633,14 @@
       </c>
       <c r="EQ32" t="n">
         <v>-1.82648401826483</v>
+      </c>
+      <c r="ER32" t="n">
+        <v>-1.59453302961275</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -37842,11 +38079,14 @@
       </c>
       <c r="EQ33" t="n">
         <v>2.64270613107824</v>
+      </c>
+      <c r="ER33" t="n">
+        <v>1.46596858638744</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -38285,11 +38525,14 @@
       </c>
       <c r="EQ34" t="n">
         <v>4.292343387471</v>
+      </c>
+      <c r="ER34" t="n">
+        <v>3.92156862745099</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -38728,11 +38971,14 @@
       </c>
       <c r="EQ35" t="n">
         <v>-0.652173913043472</v>
+      </c>
+      <c r="ER35" t="n">
+        <v>-1.51187904967605</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B36" t="n">
         <v>2.80076384468492</v>
@@ -39170,12 +39416,15 @@
         <v>2.48486779229054</v>
       </c>
       <c r="EQ36" t="n">
-        <v>1.5264890751272</v>
+        <v>1.43669560011971</v>
+      </c>
+      <c r="ER36" t="n">
+        <v>1.43841774048547</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -39614,11 +39863,14 @@
       </c>
       <c r="EQ37" t="n">
         <v>1.49253731343282</v>
+      </c>
+      <c r="ER37" t="n">
+        <v>1.4833127317676</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -40057,11 +40309,14 @@
       </c>
       <c r="EQ38" t="n">
         <v>0.726571767497031</v>
+      </c>
+      <c r="ER38" t="n">
+        <v>0.727110847306702</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -40500,11 +40755,14 @@
       </c>
       <c r="EQ39" t="n">
         <v>1.5725101921957</v>
+      </c>
+      <c r="ER39" t="n">
+        <v>1.47569444444445</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -40943,11 +41201,14 @@
       </c>
       <c r="EQ40" t="n">
         <v>1.00250626566414</v>
+      </c>
+      <c r="ER40" t="n">
+        <v>0.751879699248131</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -41385,12 +41646,15 @@
         <v>-1.68831168831169</v>
       </c>
       <c r="EQ41" t="n">
-        <v>-2.35117558779389</v>
+        <v>-1.90095047523761</v>
+      </c>
+      <c r="ER41" t="n">
+        <v>-0.0506200961781799</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -41828,12 +42092,15 @@
         <v>2.81293952180028</v>
       </c>
       <c r="EQ42" t="n">
-        <v>0.456621004566203</v>
+        <v>0.782778864970638</v>
+      </c>
+      <c r="ER42" t="n">
+        <v>0.646830530401035</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -42271,12 +42538,15 @@
         <v>3.48330914368651</v>
       </c>
       <c r="EQ43" t="n">
-        <v>3.24400564174894</v>
+        <v>3.0324400564175</v>
+      </c>
+      <c r="ER43" t="n">
+        <v>2.44584206848358</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -42715,11 +42985,14 @@
       </c>
       <c r="EQ44" t="n">
         <v>1.52375261428145</v>
+      </c>
+      <c r="ER44" t="n">
+        <v>1.60666468313003</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B45" t="n">
         <v>0.638977635782745</v>
@@ -43158,11 +43431,14 @@
       </c>
       <c r="EQ45" t="n">
         <v>-1.95439739413681</v>
+      </c>
+      <c r="ER45" t="n">
+        <v>-2.25806451612904</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B46" t="n">
         <v>0.817096165933364</v>
@@ -43600,12 +43876,15 @@
         <v>2.15252152521525</v>
       </c>
       <c r="EQ46" t="n">
-        <v>0.474777448071223</v>
+        <v>0.94955489614243</v>
+      </c>
+      <c r="ER46" t="n">
+        <v>0.827912477823759</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -44044,11 +44323,14 @@
       </c>
       <c r="EQ47" t="n">
         <v>0.257069408740364</v>
+      </c>
+      <c r="ER47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -44486,12 +44768,15 @@
         <v>1.63366336633664</v>
       </c>
       <c r="EQ48" t="n">
-        <v>1.50659133709981</v>
+        <v>1.64783427495292</v>
+      </c>
+      <c r="ER48" t="n">
+        <v>1.26286248830682</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -44929,12 +45214,15 @@
         <v>0.862871161492264</v>
       </c>
       <c r="EQ49" t="n">
-        <v>1.09181141439206</v>
+        <v>1.0752688172043</v>
+      </c>
+      <c r="ER49" t="n">
+        <v>1.27125639755653</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -45373,11 +45661,14 @@
       </c>
       <c r="EQ50" t="n">
         <v>3.59012715033658</v>
+      </c>
+      <c r="ER50" t="n">
+        <v>3.5022354694486</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -45815,12 +46106,15 @@
         <v>2.23642172523961</v>
       </c>
       <c r="EQ51" t="n">
-        <v>1.50602409638554</v>
+        <v>0</v>
+      </c>
+      <c r="ER51" t="n">
+        <v>1.5197568389058</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -46258,12 +46552,15 @@
         <v>1.88916876574307</v>
       </c>
       <c r="EQ52" t="n">
-        <v>1.32251277427113</v>
+        <v>1.59302675082657</v>
+      </c>
+      <c r="ER52" t="n">
+        <v>1.67364016736401</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -46701,12 +46998,15 @@
         <v>3.16969462698105</v>
       </c>
       <c r="EQ53" t="n">
-        <v>0.713481036425076</v>
+        <v>1.01389410439354</v>
+      </c>
+      <c r="ER53" t="n">
+        <v>-0.298284862043256</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -47144,12 +47444,15 @@
         <v>-4.3189368770764</v>
       </c>
       <c r="EQ54" t="n">
-        <v>-1.74880763116057</v>
+        <v>-1.2718600953895</v>
+      </c>
+      <c r="ER54" t="n">
+        <v>-1.88383045525903</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -47587,12 +47890,15 @@
         <v>3.59675785207701</v>
       </c>
       <c r="EQ55" t="n">
-        <v>-0.325732899022796</v>
+        <v>-0.511865984178685</v>
+      </c>
+      <c r="ER55" t="n">
+        <v>-1.52284263959391</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -48030,7 +48336,10 @@
         <v>-2.33333333333334</v>
       </c>
       <c r="EQ56" t="n">
-        <v>0.322580645161295</v>
+        <v>0.967741935483862</v>
+      </c>
+      <c r="ER56" t="n">
+        <v>1.6025641025641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update May 21, 2025
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="213">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -493,6 +493,9 @@
   </si>
   <si>
     <t xml:space="preserve">03/01/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/01/2025</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1461,10 +1464,13 @@
       <c r="FD4" t="s">
         <v>159</v>
       </c>
+      <c r="FE4" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1938,15 +1944,18 @@
         <v>10902.9</v>
       </c>
       <c r="FC5" t="n">
-        <v>11231.6</v>
+        <v>11230.5</v>
       </c>
       <c r="FD5" t="n">
-        <v>11290.7</v>
+        <v>11272.2</v>
+      </c>
+      <c r="FE5" t="n">
+        <v>11269</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2423,12 +2432,15 @@
         <v>179.7</v>
       </c>
       <c r="FD6" t="n">
-        <v>180.8</v>
+        <v>180.7</v>
+      </c>
+      <c r="FE6" t="n">
+        <v>180.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2906,11 +2918,14 @@
       </c>
       <c r="FD7" t="n">
         <v>29</v>
+      </c>
+      <c r="FE7" t="n">
+        <v>28.9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3387,12 +3402,15 @@
         <v>204</v>
       </c>
       <c r="FD8" t="n">
-        <v>202.9</v>
+        <v>202.3</v>
+      </c>
+      <c r="FE8" t="n">
+        <v>203.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3870,11 +3888,14 @@
       </c>
       <c r="FD9" t="n">
         <v>103.1</v>
+      </c>
+      <c r="FE9" t="n">
+        <v>103.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4351,12 +4372,15 @@
         <v>1301.5</v>
       </c>
       <c r="FD10" t="n">
-        <v>1322</v>
+        <v>1323</v>
+      </c>
+      <c r="FE10" t="n">
+        <v>1328.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4833,12 +4857,15 @@
         <v>241.7</v>
       </c>
       <c r="FD11" t="n">
-        <v>243.7</v>
+        <v>243.6</v>
+      </c>
+      <c r="FE11" t="n">
+        <v>242.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5316,11 +5343,14 @@
       </c>
       <c r="FD12" t="n">
         <v>125.4</v>
+      </c>
+      <c r="FE12" t="n">
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B13" t="n">
         <v>30.2</v>
@@ -5797,12 +5827,15 @@
         <v>39.2</v>
       </c>
       <c r="FD13" t="n">
+        <v>39.7</v>
+      </c>
+      <c r="FE13" t="n">
         <v>40.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5963,10 +5996,11 @@
       <c r="FB14"/>
       <c r="FC14"/>
       <c r="FD14"/>
+      <c r="FE14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6443,12 +6477,15 @@
         <v>504.1</v>
       </c>
       <c r="FD15" t="n">
-        <v>505.7</v>
+        <v>505.8</v>
+      </c>
+      <c r="FE15" t="n">
+        <v>504.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6925,12 +6962,15 @@
         <v>357.3</v>
       </c>
       <c r="FD16" t="n">
-        <v>357.9</v>
+        <v>358</v>
+      </c>
+      <c r="FE16" t="n">
+        <v>357</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -7091,10 +7131,11 @@
       <c r="FB17"/>
       <c r="FC17"/>
       <c r="FD17"/>
+      <c r="FE17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7572,11 +7613,14 @@
       </c>
       <c r="FD18" t="n">
         <v>64.2</v>
+      </c>
+      <c r="FE18" t="n">
+        <v>64.1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -8053,12 +8097,15 @@
         <v>469.2</v>
       </c>
       <c r="FD19" t="n">
-        <v>475.1</v>
+        <v>470.4</v>
+      </c>
+      <c r="FE19" t="n">
+        <v>469.6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8536,11 +8583,14 @@
       </c>
       <c r="FD20" t="n">
         <v>243.7</v>
+      </c>
+      <c r="FE20" t="n">
+        <v>239.7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -9017,12 +9067,15 @@
         <v>150.4</v>
       </c>
       <c r="FD21" t="n">
-        <v>149.6</v>
+        <v>149.7</v>
+      </c>
+      <c r="FE21" t="n">
+        <v>150.1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9499,12 +9552,15 @@
         <v>137.5</v>
       </c>
       <c r="FD22" t="n">
-        <v>138.3</v>
+        <v>138.2</v>
+      </c>
+      <c r="FE22" t="n">
+        <v>137.7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -9981,12 +10037,15 @@
         <v>166</v>
       </c>
       <c r="FD23" t="n">
-        <v>166.8</v>
+        <v>166.7</v>
+      </c>
+      <c r="FE23" t="n">
+        <v>165.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10463,12 +10522,15 @@
         <v>152.4</v>
       </c>
       <c r="FD24" t="n">
-        <v>150.6</v>
+        <v>151.9</v>
+      </c>
+      <c r="FE24" t="n">
+        <v>152</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -10946,11 +11008,14 @@
       </c>
       <c r="FD25" t="n">
         <v>49.3</v>
+      </c>
+      <c r="FE25" t="n">
+        <v>49.6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11428,11 +11493,14 @@
       </c>
       <c r="FD26" t="n">
         <v>235.7</v>
+      </c>
+      <c r="FE26" t="n">
+        <v>238.3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11909,12 +11977,15 @@
         <v>246.2</v>
       </c>
       <c r="FD27" t="n">
-        <v>248.1</v>
+        <v>247.8</v>
+      </c>
+      <c r="FE27" t="n">
+        <v>246.3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -12392,11 +12463,14 @@
       </c>
       <c r="FD28" t="n">
         <v>325.2</v>
+      </c>
+      <c r="FE28" t="n">
+        <v>325.4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12873,12 +12947,15 @@
         <v>214.3</v>
       </c>
       <c r="FD29" t="n">
-        <v>213.8</v>
+        <v>213.9</v>
+      </c>
+      <c r="FE29" t="n">
+        <v>212.9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -13355,12 +13432,15 @@
         <v>105.4</v>
       </c>
       <c r="FD30" t="n">
+        <v>105.1</v>
+      </c>
+      <c r="FE30" t="n">
         <v>105</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -13521,10 +13601,11 @@
       <c r="FB31"/>
       <c r="FC31"/>
       <c r="FD31"/>
+      <c r="FE31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -14002,11 +14083,14 @@
       </c>
       <c r="FD32" t="n">
         <v>43.2</v>
+      </c>
+      <c r="FE32" t="n">
+        <v>43.9</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -14483,12 +14567,15 @@
         <v>97.1</v>
       </c>
       <c r="FD33" t="n">
+        <v>96.7</v>
+      </c>
+      <c r="FE33" t="n">
         <v>96.9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -14966,11 +15053,14 @@
       </c>
       <c r="FD34" t="n">
         <v>90.1</v>
+      </c>
+      <c r="FE34" t="n">
+        <v>89.8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -15448,11 +15538,14 @@
       </c>
       <c r="FD35" t="n">
         <v>45.6</v>
+      </c>
+      <c r="FE35" t="n">
+        <v>44.8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B36" t="n">
         <v>314.2</v>
@@ -15929,12 +16022,15 @@
         <v>338.9</v>
       </c>
       <c r="FD36" t="n">
-        <v>338.5</v>
+        <v>338.6</v>
+      </c>
+      <c r="FE36" t="n">
+        <v>340.9</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -16411,12 +16507,15 @@
         <v>81.6</v>
       </c>
       <c r="FD37" t="n">
-        <v>82.1</v>
+        <v>81.6</v>
+      </c>
+      <c r="FE37" t="n">
+        <v>81.6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -16894,11 +16993,14 @@
       </c>
       <c r="FD38" t="n">
         <v>678.8</v>
+      </c>
+      <c r="FE38" t="n">
+        <v>678.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -17376,11 +17478,14 @@
       </c>
       <c r="FD39" t="n">
         <v>350.7</v>
+      </c>
+      <c r="FE39" t="n">
+        <v>353.5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -17858,11 +17963,14 @@
       </c>
       <c r="FD40" t="n">
         <v>40.2</v>
+      </c>
+      <c r="FE40" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -18339,12 +18447,15 @@
         <v>392.2</v>
       </c>
       <c r="FD41" t="n">
-        <v>394.9</v>
+        <v>395.1</v>
+      </c>
+      <c r="FE41" t="n">
+        <v>391.9</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -18822,11 +18933,14 @@
       </c>
       <c r="FD42" t="n">
         <v>155.6</v>
+      </c>
+      <c r="FE42" t="n">
+        <v>155.5</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -19303,12 +19417,15 @@
         <v>146.1</v>
       </c>
       <c r="FD43" t="n">
-        <v>146.6</v>
+        <v>146.7</v>
+      </c>
+      <c r="FE43" t="n">
+        <v>145.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -19786,11 +19903,14 @@
       </c>
       <c r="FD44" t="n">
         <v>341.5</v>
+      </c>
+      <c r="FE44" t="n">
+        <v>340.6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B45" t="n">
         <v>31.3</v>
@@ -20268,11 +20388,14 @@
       </c>
       <c r="FD45" t="n">
         <v>30.3</v>
+      </c>
+      <c r="FE45" t="n">
+        <v>29.9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B46" t="n">
         <v>159.1</v>
@@ -20750,11 +20873,14 @@
       </c>
       <c r="FD46" t="n">
         <v>170.5</v>
+      </c>
+      <c r="FE46" t="n">
+        <v>170.6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -21231,12 +21357,15 @@
         <v>39</v>
       </c>
       <c r="FD47" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="FE47" t="n">
         <v>39.2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -21713,12 +21842,15 @@
         <v>215.9</v>
       </c>
       <c r="FD48" t="n">
-        <v>216.5</v>
+        <v>217.8</v>
+      </c>
+      <c r="FE48" t="n">
+        <v>218.9</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -22195,12 +22327,15 @@
         <v>1222</v>
       </c>
       <c r="FD49" t="n">
-        <v>1226.8</v>
+        <v>1225.2</v>
+      </c>
+      <c r="FE49" t="n">
+        <v>1225.9</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -22678,11 +22813,14 @@
       </c>
       <c r="FD50" t="n">
         <v>138.9</v>
+      </c>
+      <c r="FE50" t="n">
+        <v>138</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -23159,12 +23297,15 @@
         <v>33.2</v>
       </c>
       <c r="FD51" t="n">
-        <v>33.4</v>
+        <v>33.1</v>
+      </c>
+      <c r="FE51" t="n">
+        <v>33.2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -23641,12 +23782,15 @@
         <v>338</v>
       </c>
       <c r="FD52" t="n">
-        <v>340.2</v>
+        <v>339.8</v>
+      </c>
+      <c r="FE52" t="n">
+        <v>338.4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -24123,12 +24267,15 @@
         <v>269</v>
       </c>
       <c r="FD53" t="n">
-        <v>267.4</v>
+        <v>269.8</v>
+      </c>
+      <c r="FE53" t="n">
+        <v>267.7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -24606,11 +24753,14 @@
       </c>
       <c r="FD54" t="n">
         <v>62.5</v>
+      </c>
+      <c r="FE54" t="n">
+        <v>63.1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -25088,11 +25238,14 @@
       </c>
       <c r="FD55" t="n">
         <v>213.4</v>
+      </c>
+      <c r="FE55" t="n">
+        <v>213.6</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -25570,6 +25723,9 @@
       </c>
       <c r="FD56" t="n">
         <v>31.7</v>
+      </c>
+      <c r="FE56" t="n">
+        <v>31.5</v>
       </c>
     </row>
   </sheetData>
@@ -26031,10 +26187,13 @@
       <c r="ER4" t="s">
         <v>159</v>
       </c>
+      <c r="ES4" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -26472,15 +26631,18 @@
         <v>1.76881288853214</v>
       </c>
       <c r="EQ5" t="n">
-        <v>1.13274145041329</v>
+        <v>1.12283671595023</v>
       </c>
       <c r="ER5" t="n">
-        <v>1.16389506128594</v>
+        <v>0.998136334312966</v>
+      </c>
+      <c r="ES5" t="n">
+        <v>1.06273261288731</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -26921,12 +27083,15 @@
         <v>0.841750841750842</v>
       </c>
       <c r="ER6" t="n">
-        <v>0.612131329994448</v>
+        <v>0.556483027267668</v>
+      </c>
+      <c r="ES6" t="n">
+        <v>1.00671140939598</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -27368,11 +27533,14 @@
       </c>
       <c r="ER7" t="n">
         <v>-0.684931506849313</v>
+      </c>
+      <c r="ES7" t="n">
+        <v>-0.687285223367683</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -27813,12 +27981,15 @@
         <v>-2.34561991383437</v>
       </c>
       <c r="ER8" t="n">
-        <v>-1.83841315916787</v>
+        <v>-2.12868892114174</v>
+      </c>
+      <c r="ES8" t="n">
+        <v>-1.97780993728896</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -28260,11 +28431,14 @@
       </c>
       <c r="ER9" t="n">
         <v>0.683593750000003</v>
+      </c>
+      <c r="ES9" t="n">
+        <v>0.678294573643414</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -28705,12 +28879,15 @@
         <v>3.38390658511398</v>
       </c>
       <c r="ER10" t="n">
-        <v>3.29739021722144</v>
+        <v>3.37552742616034</v>
+      </c>
+      <c r="ES10" t="n">
+        <v>3.32996187660468</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -29151,12 +29328,15 @@
         <v>4.49632511889321</v>
       </c>
       <c r="ER11" t="n">
-        <v>4.23438836612488</v>
+        <v>4.19161676646707</v>
+      </c>
+      <c r="ES11" t="n">
+        <v>4.33848797250859</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -29598,11 +29778,14 @@
       </c>
       <c r="ER12" t="n">
         <v>-1.10410094637223</v>
+      </c>
+      <c r="ES12" t="n">
+        <v>-0.158478605388275</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B13" t="n">
         <v>-1.98675496688743</v>
@@ -30043,12 +30226,15 @@
         <v>2.61780104712042</v>
       </c>
       <c r="ER13" t="n">
-        <v>2.29007633587788</v>
+        <v>1.01781170483462</v>
+      </c>
+      <c r="ES13" t="n">
+        <v>2.03045685279189</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -30197,10 +30383,11 @@
       <c r="EP14"/>
       <c r="EQ14"/>
       <c r="ER14"/>
+      <c r="ES14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -30641,12 +30828,15 @@
         <v>0.759544273435952</v>
       </c>
       <c r="ER15" t="n">
-        <v>0.978434504792328</v>
+        <v>0.998402555910532</v>
+      </c>
+      <c r="ES15" t="n">
+        <v>0.397851601352695</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -31087,12 +31277,15 @@
         <v>1.73690205011389</v>
       </c>
       <c r="ER16" t="n">
-        <v>1.93677015095413</v>
+        <v>1.96525206493876</v>
+      </c>
+      <c r="ES16" t="n">
+        <v>1.70940170940171</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -31241,10 +31434,11 @@
       <c r="EP17"/>
       <c r="EQ17"/>
       <c r="ER17"/>
+      <c r="ES17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -31686,11 +31880,14 @@
       </c>
       <c r="ER18" t="n">
         <v>-0.772797527047913</v>
+      </c>
+      <c r="ES18" t="n">
+        <v>-0.311041990668745</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -32131,12 +32328,15 @@
         <v>3.25704225352113</v>
       </c>
       <c r="ER19" t="n">
-        <v>3.59790667248147</v>
+        <v>2.57304840819886</v>
+      </c>
+      <c r="ES19" t="n">
+        <v>3.14078629475073</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -32578,11 +32778,14 @@
       </c>
       <c r="ER20" t="n">
         <v>2.43799915931065</v>
+      </c>
+      <c r="ES20" t="n">
+        <v>1.31022823330515</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -33023,12 +33226,15 @@
         <v>1.0752688172043</v>
       </c>
       <c r="ER21" t="n">
-        <v>0.133868808567596</v>
+        <v>0.200803212851394</v>
+      </c>
+      <c r="ES21" t="n">
+        <v>0.805910006715909</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -33469,12 +33675,15 @@
         <v>-0.217706821480394</v>
       </c>
       <c r="ER22" t="n">
-        <v>0.508720930232571</v>
+        <v>0.436046511627903</v>
+      </c>
+      <c r="ES22" t="n">
+        <v>-0.505780346820822</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -33915,12 +34124,15 @@
         <v>1.09622411693058</v>
       </c>
       <c r="ER23" t="n">
-        <v>0.724637681159431</v>
+        <v>0.664251207729465</v>
+      </c>
+      <c r="ES23" t="n">
+        <v>0.791717417783198</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -34361,12 +34573,15 @@
         <v>1.1280690112807</v>
       </c>
       <c r="ER24" t="n">
-        <v>0.266311584553951</v>
+        <v>1.13182423435421</v>
+      </c>
+      <c r="ES24" t="n">
+        <v>0.929614873837985</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -34808,11 +35023,14 @@
       </c>
       <c r="ER25" t="n">
         <v>-1.20240480961923</v>
+      </c>
+      <c r="ES25" t="n">
+        <v>-0.401606425702803</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -35254,11 +35472,14 @@
       </c>
       <c r="ER26" t="n">
         <v>3.97000441111601</v>
+      </c>
+      <c r="ES26" t="n">
+        <v>3.92498909725251</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -35699,12 +35920,15 @@
         <v>-0.0811688311688265</v>
       </c>
       <c r="ER27" t="n">
-        <v>-0.201126307321009</v>
+        <v>-0.321802091713601</v>
+      </c>
+      <c r="ES27" t="n">
+        <v>-0.243013365735113</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -36146,11 +36370,14 @@
       </c>
       <c r="ER28" t="n">
         <v>1.37157107231919</v>
+      </c>
+      <c r="ES28" t="n">
+        <v>1.43391521197006</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -36591,12 +36818,15 @@
         <v>0.610328638497658</v>
       </c>
       <c r="ER29" t="n">
-        <v>-0.511865984178685</v>
+        <v>-0.465332712889716</v>
+      </c>
+      <c r="ES29" t="n">
+        <v>0.0940291490361959</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -37037,12 +37267,15 @@
         <v>0.861244019138761</v>
       </c>
       <c r="ER30" t="n">
-        <v>0.286532951289396</v>
+        <v>0.382043935052536</v>
+      </c>
+      <c r="ES30" t="n">
+        <v>0.671140939597318</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -37191,10 +37424,11 @@
       <c r="EP31"/>
       <c r="EQ31"/>
       <c r="ER31"/>
+      <c r="ES31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -37636,11 +37870,14 @@
       </c>
       <c r="ER32" t="n">
         <v>-1.59453302961275</v>
+      </c>
+      <c r="ES32" t="n">
+        <v>-1.56950672645739</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -38081,12 +38318,15 @@
         <v>2.64270613107824</v>
       </c>
       <c r="ER33" t="n">
+        <v>1.25654450261779</v>
+      </c>
+      <c r="ES33" t="n">
         <v>1.46596858638744</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -38528,11 +38768,14 @@
       </c>
       <c r="ER34" t="n">
         <v>3.92156862745099</v>
+      </c>
+      <c r="ES34" t="n">
+        <v>4.17633410672853</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -38974,11 +39217,14 @@
       </c>
       <c r="ER35" t="n">
         <v>-1.51187904967605</v>
+      </c>
+      <c r="ES35" t="n">
+        <v>-0.884955752212402</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B36" t="n">
         <v>2.80076384468492</v>
@@ -39419,12 +39665,15 @@
         <v>1.43669560011971</v>
       </c>
       <c r="ER36" t="n">
-        <v>1.43841774048547</v>
+        <v>1.46838477674559</v>
+      </c>
+      <c r="ES36" t="n">
+        <v>2.06586826347305</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -39865,12 +40114,15 @@
         <v>1.49253731343282</v>
       </c>
       <c r="ER37" t="n">
-        <v>1.4833127317676</v>
+        <v>0.865265760197761</v>
+      </c>
+      <c r="ES37" t="n">
+        <v>0.990099009900987</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -40312,11 +40564,14 @@
       </c>
       <c r="ER38" t="n">
         <v>0.727110847306702</v>
+      </c>
+      <c r="ES38" t="n">
+        <v>0.727866904337506</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -40758,11 +41013,14 @@
       </c>
       <c r="ER39" t="n">
         <v>1.47569444444445</v>
+      </c>
+      <c r="ES39" t="n">
+        <v>1.43472022955524</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -41204,11 +41462,14 @@
       </c>
       <c r="ER40" t="n">
         <v>0.751879699248131</v>
+      </c>
+      <c r="ES40" t="n">
+        <v>0.502512562814078</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -41649,12 +41910,15 @@
         <v>-1.90095047523761</v>
       </c>
       <c r="ER41" t="n">
-        <v>-0.0506200961781799</v>
+        <v>0</v>
+      </c>
+      <c r="ES41" t="n">
+        <v>-1.95146359769829</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -42096,11 +42360,14 @@
       </c>
       <c r="ER42" t="n">
         <v>0.646830530401035</v>
+      </c>
+      <c r="ES42" t="n">
+        <v>0.777705767984438</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -42541,12 +42808,15 @@
         <v>3.0324400564175</v>
       </c>
       <c r="ER43" t="n">
-        <v>2.44584206848358</v>
+        <v>2.51572327044025</v>
+      </c>
+      <c r="ES43" t="n">
+        <v>1.67714884696015</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -42988,11 +43258,14 @@
       </c>
       <c r="ER44" t="n">
         <v>1.60666468313003</v>
+      </c>
+      <c r="ES44" t="n">
+        <v>1.61097852028637</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B45" t="n">
         <v>0.638977635782745</v>
@@ -43434,11 +43707,14 @@
       </c>
       <c r="ER45" t="n">
         <v>-2.25806451612904</v>
+      </c>
+      <c r="ES45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B46" t="n">
         <v>0.817096165933364</v>
@@ -43880,11 +44156,14 @@
       </c>
       <c r="ER46" t="n">
         <v>0.827912477823759</v>
+      </c>
+      <c r="ES46" t="n">
+        <v>0.117370892018789</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -44326,11 +44605,14 @@
       </c>
       <c r="ER47" t="n">
         <v>0</v>
+      </c>
+      <c r="ES47" t="n">
+        <v>1.29198966408269</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -44771,12 +45053,15 @@
         <v>1.64783427495292</v>
       </c>
       <c r="ER48" t="n">
-        <v>1.26286248830682</v>
+        <v>1.87090739008418</v>
+      </c>
+      <c r="ES48" t="n">
+        <v>1.95621797857475</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -45217,12 +45502,15 @@
         <v>1.0752688172043</v>
       </c>
       <c r="ER49" t="n">
-        <v>1.27125639755653</v>
+        <v>1.13917781079742</v>
+      </c>
+      <c r="ES49" t="n">
+        <v>1.38946323711853</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -45664,11 +45952,14 @@
       </c>
       <c r="ER50" t="n">
         <v>3.5022354694486</v>
+      </c>
+      <c r="ES50" t="n">
+        <v>3.52588147036758</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -46109,12 +46400,15 @@
         <v>0</v>
       </c>
       <c r="ER51" t="n">
-        <v>1.5197568389058</v>
+        <v>0.607902735562319</v>
+      </c>
+      <c r="ES51" t="n">
+        <v>0.606060606060615</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -46555,12 +46849,15 @@
         <v>1.59302675082657</v>
       </c>
       <c r="ER52" t="n">
-        <v>1.67364016736401</v>
+        <v>1.55409444112373</v>
+      </c>
+      <c r="ES52" t="n">
+        <v>1.77443609022556</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -47001,12 +47298,15 @@
         <v>1.01389410439354</v>
       </c>
       <c r="ER53" t="n">
-        <v>-0.298284862043256</v>
+        <v>0.596569724086511</v>
+      </c>
+      <c r="ES53" t="n">
+        <v>-0.260804769001486</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -47448,11 +47748,14 @@
       </c>
       <c r="ER54" t="n">
         <v>-1.88383045525903</v>
+      </c>
+      <c r="ES54" t="n">
+        <v>-0.315955766192726</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -47894,11 +48197,14 @@
       </c>
       <c r="ER55" t="n">
         <v>-1.52284263959391</v>
+      </c>
+      <c r="ES55" t="n">
+        <v>-0.789595912679989</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -48340,6 +48646,9 @@
       </c>
       <c r="ER56" t="n">
         <v>1.6025641025641</v>
+      </c>
+      <c r="ES56" t="n">
+        <v>1.28617363344051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on June 24, 2025
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -496,6 +496,9 @@
   </si>
   <si>
     <t xml:space="preserve">04/01/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/01/2025</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1467,10 +1470,13 @@
       <c r="FE4" t="s">
         <v>160</v>
       </c>
+      <c r="FF4" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1947,15 +1953,18 @@
         <v>11230.5</v>
       </c>
       <c r="FD5" t="n">
-        <v>11272.2</v>
+        <v>11274.6</v>
       </c>
       <c r="FE5" t="n">
-        <v>11269</v>
+        <v>11273.9</v>
+      </c>
+      <c r="FF5" t="n">
+        <v>11088.6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2435,12 +2444,15 @@
         <v>180.7</v>
       </c>
       <c r="FE6" t="n">
+        <v>180.6</v>
+      </c>
+      <c r="FF6" t="n">
         <v>180.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2920,12 +2932,15 @@
         <v>29</v>
       </c>
       <c r="FE7" t="n">
-        <v>28.9</v>
+        <v>28.7</v>
+      </c>
+      <c r="FF7" t="n">
+        <v>27.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3405,12 +3420,15 @@
         <v>202.3</v>
       </c>
       <c r="FE8" t="n">
-        <v>203.2</v>
+        <v>203.4</v>
+      </c>
+      <c r="FF8" t="n">
+        <v>194</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3891,11 +3909,14 @@
       </c>
       <c r="FE9" t="n">
         <v>103.9</v>
+      </c>
+      <c r="FF9" t="n">
+        <v>102.8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4375,12 +4396,15 @@
         <v>1323</v>
       </c>
       <c r="FE10" t="n">
-        <v>1328.1</v>
+        <v>1327.3</v>
+      </c>
+      <c r="FF10" t="n">
+        <v>1337.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4860,12 +4884,15 @@
         <v>243.6</v>
       </c>
       <c r="FE11" t="n">
-        <v>242.9</v>
+        <v>243</v>
+      </c>
+      <c r="FF11" t="n">
+        <v>244.2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5345,12 +5372,15 @@
         <v>125.4</v>
       </c>
       <c r="FE12" t="n">
-        <v>126</v>
+        <v>125.8</v>
+      </c>
+      <c r="FF12" t="n">
+        <v>124.2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B13" t="n">
         <v>30.2</v>
@@ -5830,12 +5860,15 @@
         <v>39.7</v>
       </c>
       <c r="FE13" t="n">
-        <v>40.2</v>
+        <v>39.6</v>
+      </c>
+      <c r="FF13" t="n">
+        <v>38.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -5997,10 +6030,11 @@
       <c r="FC14"/>
       <c r="FD14"/>
       <c r="FE14"/>
+      <c r="FF14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6480,12 +6514,15 @@
         <v>505.8</v>
       </c>
       <c r="FE15" t="n">
-        <v>504.7</v>
+        <v>504.9</v>
+      </c>
+      <c r="FF15" t="n">
+        <v>490.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -6965,12 +7002,15 @@
         <v>358</v>
       </c>
       <c r="FE16" t="n">
-        <v>357</v>
+        <v>357.3</v>
+      </c>
+      <c r="FF16" t="n">
+        <v>355</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -7132,10 +7172,11 @@
       <c r="FC17"/>
       <c r="FD17"/>
       <c r="FE17"/>
+      <c r="FF17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7616,11 +7657,14 @@
       </c>
       <c r="FE18" t="n">
         <v>64.1</v>
+      </c>
+      <c r="FF18" t="n">
+        <v>61.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -8100,12 +8144,15 @@
         <v>470.4</v>
       </c>
       <c r="FE19" t="n">
-        <v>469.6</v>
+        <v>469.5</v>
+      </c>
+      <c r="FF19" t="n">
+        <v>464.4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8585,12 +8632,15 @@
         <v>243.7</v>
       </c>
       <c r="FE20" t="n">
-        <v>239.7</v>
+        <v>238.7</v>
+      </c>
+      <c r="FF20" t="n">
+        <v>234.4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -9070,12 +9120,15 @@
         <v>149.7</v>
       </c>
       <c r="FE21" t="n">
-        <v>150.1</v>
+        <v>149.6</v>
+      </c>
+      <c r="FF21" t="n">
+        <v>151.1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9555,12 +9608,15 @@
         <v>138.2</v>
       </c>
       <c r="FE22" t="n">
-        <v>137.7</v>
+        <v>137.8</v>
+      </c>
+      <c r="FF22" t="n">
+        <v>134.8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -10040,12 +10096,15 @@
         <v>166.7</v>
       </c>
       <c r="FE23" t="n">
-        <v>165.5</v>
+        <v>166.1</v>
+      </c>
+      <c r="FF23" t="n">
+        <v>166.1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10526,11 +10585,14 @@
       </c>
       <c r="FE24" t="n">
         <v>152</v>
+      </c>
+      <c r="FF24" t="n">
+        <v>151</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -11010,12 +11072,15 @@
         <v>49.3</v>
       </c>
       <c r="FE25" t="n">
-        <v>49.6</v>
+        <v>49.4</v>
+      </c>
+      <c r="FF25" t="n">
+        <v>49.3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11496,11 +11561,14 @@
       </c>
       <c r="FE26" t="n">
         <v>238.3</v>
+      </c>
+      <c r="FF26" t="n">
+        <v>239</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -11981,11 +12049,14 @@
       </c>
       <c r="FE27" t="n">
         <v>246.3</v>
+      </c>
+      <c r="FF27" t="n">
+        <v>245.9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -12466,11 +12537,14 @@
       </c>
       <c r="FE28" t="n">
         <v>325.4</v>
+      </c>
+      <c r="FF28" t="n">
+        <v>309.5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -12951,11 +13025,14 @@
       </c>
       <c r="FE29" t="n">
         <v>212.9</v>
+      </c>
+      <c r="FF29" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -13435,12 +13512,15 @@
         <v>105.1</v>
       </c>
       <c r="FE30" t="n">
-        <v>105</v>
+        <v>104.9</v>
+      </c>
+      <c r="FF30" t="n">
+        <v>103.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -13602,10 +13682,11 @@
       <c r="FC31"/>
       <c r="FD31"/>
       <c r="FE31"/>
+      <c r="FF31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -14086,11 +14167,14 @@
       </c>
       <c r="FE32" t="n">
         <v>43.9</v>
+      </c>
+      <c r="FF32" t="n">
+        <v>44.8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -14571,11 +14655,14 @@
       </c>
       <c r="FE33" t="n">
         <v>96.9</v>
+      </c>
+      <c r="FF33" t="n">
+        <v>98</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -15055,12 +15142,15 @@
         <v>90.1</v>
       </c>
       <c r="FE34" t="n">
-        <v>89.8</v>
+        <v>90.3</v>
+      </c>
+      <c r="FF34" t="n">
+        <v>91</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -15541,11 +15631,14 @@
       </c>
       <c r="FE35" t="n">
         <v>44.8</v>
+      </c>
+      <c r="FF35" t="n">
+        <v>44.5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B36" t="n">
         <v>314.2</v>
@@ -16025,12 +16118,15 @@
         <v>338.6</v>
       </c>
       <c r="FE36" t="n">
-        <v>340.9</v>
+        <v>341</v>
+      </c>
+      <c r="FF36" t="n">
+        <v>333.4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -16510,12 +16606,15 @@
         <v>81.6</v>
       </c>
       <c r="FE37" t="n">
-        <v>81.6</v>
+        <v>81.7</v>
+      </c>
+      <c r="FF37" t="n">
+        <v>81.5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -16996,11 +17095,14 @@
       </c>
       <c r="FE38" t="n">
         <v>678.1</v>
+      </c>
+      <c r="FF38" t="n">
+        <v>673.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -17481,11 +17583,14 @@
       </c>
       <c r="FE39" t="n">
         <v>353.5</v>
+      </c>
+      <c r="FF39" t="n">
+        <v>353.3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -17966,11 +18071,14 @@
       </c>
       <c r="FE40" t="n">
         <v>40</v>
+      </c>
+      <c r="FF40" t="n">
+        <v>39.7</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -18450,12 +18558,15 @@
         <v>395.1</v>
       </c>
       <c r="FE41" t="n">
-        <v>391.9</v>
+        <v>391.8</v>
+      </c>
+      <c r="FF41" t="n">
+        <v>382.8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -18935,12 +19046,15 @@
         <v>155.6</v>
       </c>
       <c r="FE42" t="n">
-        <v>155.5</v>
+        <v>155.9</v>
+      </c>
+      <c r="FF42" t="n">
+        <v>155.3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -19420,12 +19534,15 @@
         <v>146.7</v>
       </c>
       <c r="FE43" t="n">
-        <v>145.5</v>
+        <v>145.7</v>
+      </c>
+      <c r="FF43" t="n">
+        <v>146.6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -19906,11 +20023,14 @@
       </c>
       <c r="FE44" t="n">
         <v>340.6</v>
+      </c>
+      <c r="FF44" t="n">
+        <v>336.4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B45" t="n">
         <v>31.3</v>
@@ -20390,12 +20510,15 @@
         <v>30.3</v>
       </c>
       <c r="FE45" t="n">
-        <v>29.9</v>
+        <v>30</v>
+      </c>
+      <c r="FF45" t="n">
+        <v>28.8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B46" t="n">
         <v>159.1</v>
@@ -20875,12 +20998,15 @@
         <v>170.5</v>
       </c>
       <c r="FE46" t="n">
-        <v>170.6</v>
+        <v>170.5</v>
+      </c>
+      <c r="FF46" t="n">
+        <v>166.8</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -21361,11 +21487,14 @@
       </c>
       <c r="FE47" t="n">
         <v>39.2</v>
+      </c>
+      <c r="FF47" t="n">
+        <v>38.8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -21845,12 +21974,15 @@
         <v>217.8</v>
       </c>
       <c r="FE48" t="n">
-        <v>218.9</v>
+        <v>218</v>
+      </c>
+      <c r="FF48" t="n">
+        <v>210.2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -22330,12 +22462,15 @@
         <v>1225.2</v>
       </c>
       <c r="FE49" t="n">
-        <v>1225.9</v>
+        <v>1225.8</v>
+      </c>
+      <c r="FF49" t="n">
+        <v>1223.3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -22816,11 +22951,14 @@
       </c>
       <c r="FE50" t="n">
         <v>138</v>
+      </c>
+      <c r="FF50" t="n">
+        <v>137.4</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -23300,12 +23438,15 @@
         <v>33.1</v>
       </c>
       <c r="FE51" t="n">
-        <v>33.2</v>
+        <v>32.9</v>
+      </c>
+      <c r="FF51" t="n">
+        <v>30.7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -23786,11 +23927,14 @@
       </c>
       <c r="FE52" t="n">
         <v>338.4</v>
+      </c>
+      <c r="FF52" t="n">
+        <v>330.3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -24270,12 +24414,15 @@
         <v>269.8</v>
       </c>
       <c r="FE53" t="n">
-        <v>267.7</v>
+        <v>269.7</v>
+      </c>
+      <c r="FF53" t="n">
+        <v>266</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -24755,12 +24902,15 @@
         <v>62.5</v>
       </c>
       <c r="FE54" t="n">
-        <v>63.1</v>
+        <v>62.7</v>
+      </c>
+      <c r="FF54" t="n">
+        <v>62.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -25241,11 +25391,14 @@
       </c>
       <c r="FE55" t="n">
         <v>213.6</v>
+      </c>
+      <c r="FF55" t="n">
+        <v>204.9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -25725,7 +25878,10 @@
         <v>31.7</v>
       </c>
       <c r="FE56" t="n">
-        <v>31.5</v>
+        <v>31.6</v>
+      </c>
+      <c r="FF56" t="n">
+        <v>31.6</v>
       </c>
     </row>
   </sheetData>
@@ -26190,10 +26346,13 @@
       <c r="ES4" t="s">
         <v>160</v>
       </c>
+      <c r="ET4" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -26634,15 +26793,18 @@
         <v>1.12283671595023</v>
       </c>
       <c r="ER5" t="n">
-        <v>0.998136334312966</v>
+        <v>1.01964016916351</v>
       </c>
       <c r="ES5" t="n">
-        <v>1.06273261288731</v>
+        <v>1.10667683063539</v>
+      </c>
+      <c r="ET5" t="n">
+        <v>0.956889880274961</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -27086,12 +27248,15 @@
         <v>0.556483027267668</v>
       </c>
       <c r="ES6" t="n">
-        <v>1.00671140939598</v>
+        <v>1.00671140939596</v>
+      </c>
+      <c r="ET6" t="n">
+        <v>1.1198208286674</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -27535,12 +27700,15 @@
         <v>-0.684931506849313</v>
       </c>
       <c r="ES7" t="n">
-        <v>-0.687285223367683</v>
+        <v>-1.37457044673539</v>
+      </c>
+      <c r="ET7" t="n">
+        <v>-1.76678445229681</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -27984,12 +28152,15 @@
         <v>-2.12868892114174</v>
       </c>
       <c r="ES8" t="n">
-        <v>-1.97780993728896</v>
+        <v>-1.88133140376268</v>
+      </c>
+      <c r="ET8" t="n">
+        <v>-1.12130479102956</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -28434,11 +28605,14 @@
       </c>
       <c r="ES9" t="n">
         <v>0.678294573643414</v>
+      </c>
+      <c r="ET9" t="n">
+        <v>0.587084148727993</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -28882,12 +29056,15 @@
         <v>3.37552742616034</v>
       </c>
       <c r="ES10" t="n">
-        <v>3.32996187660468</v>
+        <v>3.26771959853729</v>
+      </c>
+      <c r="ET10" t="n">
+        <v>3.29059168855246</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -29331,12 +29508,15 @@
         <v>4.19161676646707</v>
       </c>
       <c r="ES11" t="n">
-        <v>4.33848797250859</v>
+        <v>4.38144329896908</v>
+      </c>
+      <c r="ET11" t="n">
+        <v>4.49293966623878</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -29780,12 +29960,15 @@
         <v>-1.10410094637223</v>
       </c>
       <c r="ES12" t="n">
-        <v>-0.158478605388275</v>
+        <v>-0.316957210776538</v>
+      </c>
+      <c r="ET12" t="n">
+        <v>-1.11464968152868</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B13" t="n">
         <v>-1.98675496688743</v>
@@ -30229,12 +30412,15 @@
         <v>1.01781170483462</v>
       </c>
       <c r="ES13" t="n">
-        <v>2.03045685279189</v>
+        <v>0.507614213197959</v>
+      </c>
+      <c r="ET13" t="n">
+        <v>0.781249999999992</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -30384,10 +30570,11 @@
       <c r="EQ14"/>
       <c r="ER14"/>
       <c r="ES14"/>
+      <c r="ET14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -30831,12 +31018,15 @@
         <v>0.998402555910532</v>
       </c>
       <c r="ES15" t="n">
-        <v>0.397851601352695</v>
+        <v>0.437636761487963</v>
+      </c>
+      <c r="ET15" t="n">
+        <v>0.102103328568523</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -31280,12 +31470,15 @@
         <v>1.96525206493876</v>
       </c>
       <c r="ES16" t="n">
-        <v>1.70940170940171</v>
+        <v>1.7948717948718</v>
+      </c>
+      <c r="ET16" t="n">
+        <v>1.31278538812786</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -31435,10 +31628,11 @@
       <c r="EQ17"/>
       <c r="ER17"/>
       <c r="ES17"/>
+      <c r="ET17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -31883,11 +32077,14 @@
       </c>
       <c r="ES18" t="n">
         <v>-0.311041990668745</v>
+      </c>
+      <c r="ET18" t="n">
+        <v>-0.323624595469249</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -32331,12 +32528,15 @@
         <v>2.57304840819886</v>
       </c>
       <c r="ES19" t="n">
-        <v>3.14078629475073</v>
+        <v>3.11882275422799</v>
+      </c>
+      <c r="ET19" t="n">
+        <v>2.69792127377265</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -32780,12 +32980,15 @@
         <v>2.43799915931065</v>
       </c>
       <c r="ES20" t="n">
-        <v>1.31022823330515</v>
+        <v>0.887573964497039</v>
+      </c>
+      <c r="ET20" t="n">
+        <v>-1.42977291841885</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -33229,12 +33432,15 @@
         <v>0.200803212851394</v>
       </c>
       <c r="ES21" t="n">
-        <v>0.805910006715909</v>
+        <v>0.470114170584277</v>
+      </c>
+      <c r="ET21" t="n">
+        <v>2.02565833896018</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -33678,12 +33884,15 @@
         <v>0.436046511627903</v>
       </c>
       <c r="ES22" t="n">
-        <v>-0.505780346820822</v>
+        <v>-0.43352601156069</v>
+      </c>
+      <c r="ET22" t="n">
+        <v>1.8896447467876</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -34127,12 +34336,15 @@
         <v>0.664251207729465</v>
       </c>
       <c r="ES23" t="n">
-        <v>0.791717417783198</v>
+        <v>1.15712545676005</v>
+      </c>
+      <c r="ET23" t="n">
+        <v>1.40415140415139</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -34577,11 +34789,14 @@
       </c>
       <c r="ES24" t="n">
         <v>0.929614873837985</v>
+      </c>
+      <c r="ET24" t="n">
+        <v>0.801068090787709</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -35025,12 +35240,15 @@
         <v>-1.20240480961923</v>
       </c>
       <c r="ES25" t="n">
-        <v>-0.401606425702803</v>
+        <v>-0.803212851405605</v>
+      </c>
+      <c r="ET25" t="n">
+        <v>-0.202429149797574</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -35475,11 +35693,14 @@
       </c>
       <c r="ES26" t="n">
         <v>3.92498909725251</v>
+      </c>
+      <c r="ET26" t="n">
+        <v>3.91304347826087</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -35924,11 +36145,14 @@
       </c>
       <c r="ES27" t="n">
         <v>-0.243013365735113</v>
+      </c>
+      <c r="ET27" t="n">
+        <v>-0.121852152721369</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -36373,11 +36597,14 @@
       </c>
       <c r="ES28" t="n">
         <v>1.43391521197006</v>
+      </c>
+      <c r="ET28" t="n">
+        <v>1.37569603668522</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -36822,11 +37049,14 @@
       </c>
       <c r="ES29" t="n">
         <v>0.0940291490361959</v>
+      </c>
+      <c r="ET29" t="n">
+        <v>-0.332225913621271</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -37270,12 +37500,15 @@
         <v>0.382043935052536</v>
       </c>
       <c r="ES30" t="n">
-        <v>0.671140939597318</v>
+        <v>0.575263662511993</v>
+      </c>
+      <c r="ET30" t="n">
+        <v>0.877192982456146</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -37425,10 +37658,11 @@
       <c r="EQ31"/>
       <c r="ER31"/>
       <c r="ES31"/>
+      <c r="ET31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -37873,11 +38107,14 @@
       </c>
       <c r="ES32" t="n">
         <v>-1.56950672645739</v>
+      </c>
+      <c r="ET32" t="n">
+        <v>-1.53846153846154</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -38322,11 +38559,14 @@
       </c>
       <c r="ES33" t="n">
         <v>1.46596858638744</v>
+      </c>
+      <c r="ET33" t="n">
+        <v>1.87110187110187</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -38770,12 +39010,15 @@
         <v>3.92156862745099</v>
       </c>
       <c r="ES34" t="n">
-        <v>4.17633410672853</v>
+        <v>4.75638051044083</v>
+      </c>
+      <c r="ET34" t="n">
+        <v>4.83870967741934</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -39220,11 +39463,14 @@
       </c>
       <c r="ES35" t="n">
         <v>-0.884955752212402</v>
+      </c>
+      <c r="ET35" t="n">
+        <v>3.48837209302326</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B36" t="n">
         <v>2.80076384468492</v>
@@ -39668,12 +39914,15 @@
         <v>1.46838477674559</v>
       </c>
       <c r="ES36" t="n">
-        <v>2.06586826347305</v>
+        <v>2.09580838323353</v>
+      </c>
+      <c r="ET36" t="n">
+        <v>1.86373357775742</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -40117,12 +40366,15 @@
         <v>0.865265760197761</v>
       </c>
       <c r="ES37" t="n">
-        <v>0.990099009900987</v>
+        <v>1.11386138613862</v>
+      </c>
+      <c r="ET37" t="n">
+        <v>0.991325898389092</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -40567,11 +40819,14 @@
       </c>
       <c r="ES38" t="n">
         <v>0.727866904337506</v>
+      </c>
+      <c r="ET38" t="n">
+        <v>0.748055056852167</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -41016,11 +41271,14 @@
       </c>
       <c r="ES39" t="n">
         <v>1.43472022955524</v>
+      </c>
+      <c r="ET39" t="n">
+        <v>1.43554407120297</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -41465,11 +41723,14 @@
       </c>
       <c r="ES40" t="n">
         <v>0.502512562814078</v>
+      </c>
+      <c r="ET40" t="n">
+        <v>1.01781170483462</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -41913,12 +42174,15 @@
         <v>0</v>
       </c>
       <c r="ES41" t="n">
-        <v>-1.95146359769829</v>
+        <v>-1.97648236177134</v>
+      </c>
+      <c r="ET41" t="n">
+        <v>-1.66966349858722</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -42362,12 +42626,15 @@
         <v>0.646830530401035</v>
       </c>
       <c r="ES42" t="n">
-        <v>0.777705767984438</v>
+        <v>1.03694102397926</v>
+      </c>
+      <c r="ET42" t="n">
+        <v>0.778715120051907</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -42811,12 +43078,15 @@
         <v>2.51572327044025</v>
       </c>
       <c r="ES43" t="n">
-        <v>1.67714884696015</v>
+        <v>1.81691125087351</v>
+      </c>
+      <c r="ET43" t="n">
+        <v>2.30286113049549</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -43261,11 +43531,14 @@
       </c>
       <c r="ES44" t="n">
         <v>1.61097852028637</v>
+      </c>
+      <c r="ET44" t="n">
+        <v>1.50875075437536</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B45" t="n">
         <v>0.638977635782745</v>
@@ -43709,12 +43982,15 @@
         <v>-2.25806451612904</v>
       </c>
       <c r="ES45" t="n">
-        <v>0</v>
+        <v>0.334448160535122</v>
+      </c>
+      <c r="ET45" t="n">
+        <v>-2.04081632653062</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B46" t="n">
         <v>0.817096165933364</v>
@@ -44158,12 +44434,15 @@
         <v>0.827912477823759</v>
       </c>
       <c r="ES46" t="n">
-        <v>0.117370892018789</v>
+        <v>0.058685446009403</v>
+      </c>
+      <c r="ET46" t="n">
+        <v>0.421432871764008</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -44608,11 +44887,14 @@
       </c>
       <c r="ES47" t="n">
         <v>1.29198966408269</v>
+      </c>
+      <c r="ET47" t="n">
+        <v>1.04166666666666</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -45056,12 +45338,15 @@
         <v>1.87090739008418</v>
       </c>
       <c r="ES48" t="n">
-        <v>1.95621797857475</v>
+        <v>1.53702841173731</v>
+      </c>
+      <c r="ET48" t="n">
+        <v>1.35004821600772</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -45505,12 +45790,15 @@
         <v>1.13917781079742</v>
       </c>
       <c r="ES49" t="n">
-        <v>1.38946323711853</v>
+        <v>1.38119262261186</v>
+      </c>
+      <c r="ET49" t="n">
+        <v>1.24141355623603</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -45955,11 +46243,14 @@
       </c>
       <c r="ES50" t="n">
         <v>3.52588147036758</v>
+      </c>
+      <c r="ET50" t="n">
+        <v>3.46385542168672</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -46403,12 +46694,15 @@
         <v>0.607902735562319</v>
       </c>
       <c r="ES51" t="n">
-        <v>0.606060606060615</v>
+        <v>-0.303030303030307</v>
+      </c>
+      <c r="ET51" t="n">
+        <v>-6.11620795107034</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -46853,11 +47147,14 @@
       </c>
       <c r="ES52" t="n">
         <v>1.77443609022556</v>
+      </c>
+      <c r="ET52" t="n">
+        <v>1.59950784374038</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -47301,12 +47598,15 @@
         <v>0.596569724086511</v>
       </c>
       <c r="ES53" t="n">
-        <v>-0.260804769001486</v>
+        <v>0.484351713859915</v>
+      </c>
+      <c r="ET53" t="n">
+        <v>-1.59082500924899</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -47750,12 +48050,15 @@
         <v>-1.88383045525903</v>
       </c>
       <c r="ES54" t="n">
-        <v>-0.315955766192726</v>
+        <v>-0.94786729857819</v>
+      </c>
+      <c r="ET54" t="n">
+        <v>-1.72955974842766</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -48200,11 +48503,14 @@
       </c>
       <c r="ES55" t="n">
         <v>-0.789595912679989</v>
+      </c>
+      <c r="ET55" t="n">
+        <v>0.195599022004879</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -48648,7 +48954,10 @@
         <v>1.6025641025641</v>
       </c>
       <c r="ES56" t="n">
-        <v>1.28617363344051</v>
+        <v>1.60771704180063</v>
+      </c>
+      <c r="ET56" t="n">
+        <v>1.28205128205127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on August 19th, 2025
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -499,6 +499,12 @@
   </si>
   <si>
     <t xml:space="preserve">05/01/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/01/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/01/2025</t>
   </si>
   <si>
     <t xml:space="preserve">United States</t>
@@ -1473,10 +1479,16 @@
       <c r="FF4" t="s">
         <v>161</v>
       </c>
+      <c r="FG4" t="s">
+        <v>162</v>
+      </c>
+      <c r="FH4" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1956,15 +1968,21 @@
         <v>11274.6</v>
       </c>
       <c r="FE5" t="n">
-        <v>11273.9</v>
+        <v>11267.9</v>
       </c>
       <c r="FF5" t="n">
-        <v>11088.6</v>
+        <v>11093.6</v>
+      </c>
+      <c r="FG5" t="n">
+        <v>10506.5</v>
+      </c>
+      <c r="FH5" t="n">
+        <v>9339.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2447,12 +2465,18 @@
         <v>180.6</v>
       </c>
       <c r="FF6" t="n">
-        <v>180.6</v>
+        <v>180.5</v>
+      </c>
+      <c r="FG6" t="n">
+        <v>177.3</v>
+      </c>
+      <c r="FH6" t="n">
+        <v>167.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2936,11 +2960,17 @@
       </c>
       <c r="FF7" t="n">
         <v>27.8</v>
+      </c>
+      <c r="FG7" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="FH7" t="n">
+        <v>18.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3423,12 +3453,18 @@
         <v>203.4</v>
       </c>
       <c r="FF8" t="n">
-        <v>194</v>
+        <v>192.5</v>
+      </c>
+      <c r="FG8" t="n">
+        <v>150.8</v>
+      </c>
+      <c r="FH8" t="n">
+        <v>147.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3912,11 +3948,17 @@
       </c>
       <c r="FF9" t="n">
         <v>102.8</v>
+      </c>
+      <c r="FG9" t="n">
+        <v>94.5</v>
+      </c>
+      <c r="FH9" t="n">
+        <v>83.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4400,11 +4442,17 @@
       </c>
       <c r="FF10" t="n">
         <v>1337.2</v>
+      </c>
+      <c r="FG10" t="n">
+        <v>1315.5</v>
+      </c>
+      <c r="FH10" t="n">
+        <v>1151.9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4887,12 +4935,18 @@
         <v>243</v>
       </c>
       <c r="FF11" t="n">
-        <v>244.2</v>
+        <v>243.8</v>
+      </c>
+      <c r="FG11" t="n">
+        <v>228.4</v>
+      </c>
+      <c r="FH11" t="n">
+        <v>214.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5376,11 +5430,17 @@
       </c>
       <c r="FF12" t="n">
         <v>124.2</v>
+      </c>
+      <c r="FG12" t="n">
+        <v>117.9</v>
+      </c>
+      <c r="FH12" t="n">
+        <v>99.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B13" t="n">
         <v>30.2</v>
@@ -5864,11 +5924,17 @@
       </c>
       <c r="FF13" t="n">
         <v>38.7</v>
+      </c>
+      <c r="FG13" t="n">
+        <v>35.7</v>
+      </c>
+      <c r="FH13" t="n">
+        <v>33.9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -6031,10 +6097,12 @@
       <c r="FD14"/>
       <c r="FE14"/>
       <c r="FF14"/>
+      <c r="FG14"/>
+      <c r="FH14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6517,12 +6585,18 @@
         <v>504.9</v>
       </c>
       <c r="FF15" t="n">
-        <v>490.2</v>
+        <v>489.9</v>
+      </c>
+      <c r="FG15" t="n">
+        <v>409.2</v>
+      </c>
+      <c r="FH15" t="n">
+        <v>400.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -7005,12 +7079,18 @@
         <v>357.3</v>
       </c>
       <c r="FF16" t="n">
-        <v>355</v>
+        <v>354.9</v>
+      </c>
+      <c r="FG16" t="n">
+        <v>342.2</v>
+      </c>
+      <c r="FH16" t="n">
+        <v>328.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -7173,10 +7253,12 @@
       <c r="FD17"/>
       <c r="FE17"/>
       <c r="FF17"/>
+      <c r="FG17"/>
+      <c r="FH17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7659,12 +7741,18 @@
         <v>64.1</v>
       </c>
       <c r="FF18" t="n">
-        <v>61.6</v>
+        <v>61.5</v>
+      </c>
+      <c r="FG18" t="n">
+        <v>59.2</v>
+      </c>
+      <c r="FH18" t="n">
+        <v>53.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -8148,11 +8236,17 @@
       </c>
       <c r="FF19" t="n">
         <v>464.4</v>
+      </c>
+      <c r="FG19" t="n">
+        <v>430</v>
+      </c>
+      <c r="FH19" t="n">
+        <v>396.8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8635,12 +8729,18 @@
         <v>238.7</v>
       </c>
       <c r="FF20" t="n">
-        <v>234.4</v>
+        <v>234.3</v>
+      </c>
+      <c r="FG20" t="n">
+        <v>196.6</v>
+      </c>
+      <c r="FH20" t="n">
+        <v>181</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -9123,12 +9223,18 @@
         <v>149.6</v>
       </c>
       <c r="FF21" t="n">
-        <v>151.1</v>
+        <v>149.8</v>
+      </c>
+      <c r="FG21" t="n">
+        <v>137.1</v>
+      </c>
+      <c r="FH21" t="n">
+        <v>117</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9611,12 +9717,18 @@
         <v>137.8</v>
       </c>
       <c r="FF22" t="n">
-        <v>134.8</v>
+        <v>134.7</v>
+      </c>
+      <c r="FG22" t="n">
+        <v>120</v>
+      </c>
+      <c r="FH22" t="n">
+        <v>98.2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -10099,12 +10211,18 @@
         <v>166.1</v>
       </c>
       <c r="FF23" t="n">
-        <v>166.1</v>
+        <v>165.9</v>
+      </c>
+      <c r="FG23" t="n">
+        <v>155.9</v>
+      </c>
+      <c r="FH23" t="n">
+        <v>131.2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10588,11 +10706,17 @@
       </c>
       <c r="FF24" t="n">
         <v>151</v>
+      </c>
+      <c r="FG24" t="n">
+        <v>140.5</v>
+      </c>
+      <c r="FH24" t="n">
+        <v>133.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -11076,11 +11200,17 @@
       </c>
       <c r="FF25" t="n">
         <v>49.3</v>
+      </c>
+      <c r="FG25" t="n">
+        <v>47.2</v>
+      </c>
+      <c r="FH25" t="n">
+        <v>39.7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11564,11 +11694,17 @@
       </c>
       <c r="FF26" t="n">
         <v>239</v>
+      </c>
+      <c r="FG26" t="n">
+        <v>225.5</v>
+      </c>
+      <c r="FH26" t="n">
+        <v>213.2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -12052,11 +12188,17 @@
       </c>
       <c r="FF27" t="n">
         <v>245.9</v>
+      </c>
+      <c r="FG27" t="n">
+        <v>241</v>
+      </c>
+      <c r="FH27" t="n">
+        <v>213.9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -12540,11 +12682,17 @@
       </c>
       <c r="FF28" t="n">
         <v>309.5</v>
+      </c>
+      <c r="FG28" t="n">
+        <v>293.4</v>
+      </c>
+      <c r="FH28" t="n">
+        <v>265.8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -13027,12 +13175,18 @@
         <v>212.9</v>
       </c>
       <c r="FF29" t="n">
-        <v>210</v>
+        <v>210.4</v>
+      </c>
+      <c r="FG29" t="n">
+        <v>202.3</v>
+      </c>
+      <c r="FH29" t="n">
+        <v>168.9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -13516,11 +13670,17 @@
       </c>
       <c r="FF30" t="n">
         <v>103.5</v>
+      </c>
+      <c r="FG30" t="n">
+        <v>99.2</v>
+      </c>
+      <c r="FH30" t="n">
+        <v>93.7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -13683,10 +13843,12 @@
       <c r="FD31"/>
       <c r="FE31"/>
       <c r="FF31"/>
+      <c r="FG31"/>
+      <c r="FH31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -14170,11 +14332,17 @@
       </c>
       <c r="FF32" t="n">
         <v>44.8</v>
+      </c>
+      <c r="FG32" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="FH32" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -14657,12 +14825,18 @@
         <v>96.9</v>
       </c>
       <c r="FF33" t="n">
-        <v>98</v>
+        <v>97.8</v>
+      </c>
+      <c r="FG33" t="n">
+        <v>90.8</v>
+      </c>
+      <c r="FH33" t="n">
+        <v>80.5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -15145,12 +15319,18 @@
         <v>90.3</v>
       </c>
       <c r="FF34" t="n">
-        <v>91</v>
+        <v>90.8</v>
+      </c>
+      <c r="FG34" t="n">
+        <v>75.9</v>
+      </c>
+      <c r="FH34" t="n">
+        <v>73.1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -15633,12 +15813,18 @@
         <v>44.8</v>
       </c>
       <c r="FF35" t="n">
-        <v>44.5</v>
+        <v>44.4</v>
+      </c>
+      <c r="FG35" t="n">
+        <v>40.3</v>
+      </c>
+      <c r="FH35" t="n">
+        <v>33.1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B36" t="n">
         <v>314.2</v>
@@ -16121,12 +16307,18 @@
         <v>341</v>
       </c>
       <c r="FF36" t="n">
-        <v>333.4</v>
+        <v>332.7</v>
+      </c>
+      <c r="FG36" t="n">
+        <v>325.8</v>
+      </c>
+      <c r="FH36" t="n">
+        <v>263.6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -16610,11 +16802,17 @@
       </c>
       <c r="FF37" t="n">
         <v>81.5</v>
+      </c>
+      <c r="FG37" t="n">
+        <v>73.9</v>
+      </c>
+      <c r="FH37" t="n">
+        <v>65.6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -17098,11 +17296,17 @@
       </c>
       <c r="FF38" t="n">
         <v>673.4</v>
+      </c>
+      <c r="FG38" t="n">
+        <v>662.3</v>
+      </c>
+      <c r="FH38" t="n">
+        <v>555.1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -17586,11 +17790,17 @@
       </c>
       <c r="FF39" t="n">
         <v>353.3</v>
+      </c>
+      <c r="FG39" t="n">
+        <v>324.6</v>
+      </c>
+      <c r="FH39" t="n">
+        <v>267.1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -18074,11 +18284,17 @@
       </c>
       <c r="FF40" t="n">
         <v>39.7</v>
+      </c>
+      <c r="FG40" t="n">
+        <v>35.2</v>
+      </c>
+      <c r="FH40" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -18561,12 +18777,18 @@
         <v>391.8</v>
       </c>
       <c r="FF41" t="n">
-        <v>382.8</v>
+        <v>382.4</v>
+      </c>
+      <c r="FG41" t="n">
+        <v>358</v>
+      </c>
+      <c r="FH41" t="n">
+        <v>349.5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -19050,11 +19272,17 @@
       </c>
       <c r="FF42" t="n">
         <v>155.3</v>
+      </c>
+      <c r="FG42" t="n">
+        <v>142.4</v>
+      </c>
+      <c r="FH42" t="n">
+        <v>129.2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -19538,11 +19766,17 @@
       </c>
       <c r="FF43" t="n">
         <v>146.6</v>
+      </c>
+      <c r="FG43" t="n">
+        <v>143.6</v>
+      </c>
+      <c r="FH43" t="n">
+        <v>112.2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -20026,11 +20260,17 @@
       </c>
       <c r="FF44" t="n">
         <v>336.4</v>
+      </c>
+      <c r="FG44" t="n">
+        <v>307.1</v>
+      </c>
+      <c r="FH44" t="n">
+        <v>279.8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B45" t="n">
         <v>31.3</v>
@@ -20514,11 +20754,17 @@
       </c>
       <c r="FF45" t="n">
         <v>28.8</v>
+      </c>
+      <c r="FG45" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="FH45" t="n">
+        <v>23.1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B46" t="n">
         <v>159.1</v>
@@ -21001,12 +21247,18 @@
         <v>170.5</v>
       </c>
       <c r="FF46" t="n">
-        <v>166.8</v>
+        <v>166.9</v>
+      </c>
+      <c r="FG46" t="n">
+        <v>161.4</v>
+      </c>
+      <c r="FH46" t="n">
+        <v>151.7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -21490,11 +21742,17 @@
       </c>
       <c r="FF47" t="n">
         <v>38.8</v>
+      </c>
+      <c r="FG47" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="FH47" t="n">
+        <v>28.5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -21977,12 +22235,18 @@
         <v>218</v>
       </c>
       <c r="FF48" t="n">
-        <v>210.2</v>
+        <v>214.3</v>
+      </c>
+      <c r="FG48" t="n">
+        <v>201.1</v>
+      </c>
+      <c r="FH48" t="n">
+        <v>176.2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -22465,12 +22729,18 @@
         <v>1225.8</v>
       </c>
       <c r="FF49" t="n">
-        <v>1223.3</v>
+        <v>1223.5</v>
+      </c>
+      <c r="FG49" t="n">
+        <v>1175.5</v>
+      </c>
+      <c r="FH49" t="n">
+        <v>1094.2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -22954,11 +23224,17 @@
       </c>
       <c r="FF50" t="n">
         <v>137.4</v>
+      </c>
+      <c r="FG50" t="n">
+        <v>130.7</v>
+      </c>
+      <c r="FH50" t="n">
+        <v>114.8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -23442,11 +23718,17 @@
       </c>
       <c r="FF51" t="n">
         <v>30.7</v>
+      </c>
+      <c r="FG51" t="n">
+        <v>30</v>
+      </c>
+      <c r="FH51" t="n">
+        <v>25.7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -23930,11 +24212,17 @@
       </c>
       <c r="FF52" t="n">
         <v>330.3</v>
+      </c>
+      <c r="FG52" t="n">
+        <v>322.2</v>
+      </c>
+      <c r="FH52" t="n">
+        <v>294</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -24417,12 +24705,18 @@
         <v>269.7</v>
       </c>
       <c r="FF53" t="n">
-        <v>266</v>
+        <v>266.2</v>
+      </c>
+      <c r="FG53" t="n">
+        <v>261.2</v>
+      </c>
+      <c r="FH53" t="n">
+        <v>239.5</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -24906,11 +25200,17 @@
       </c>
       <c r="FF54" t="n">
         <v>62.5</v>
+      </c>
+      <c r="FG54" t="n">
+        <v>57</v>
+      </c>
+      <c r="FH54" t="n">
+        <v>52.1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -25393,12 +25693,18 @@
         <v>213.6</v>
       </c>
       <c r="FF55" t="n">
-        <v>204.9</v>
+        <v>205.5</v>
+      </c>
+      <c r="FG55" t="n">
+        <v>187.8</v>
+      </c>
+      <c r="FH55" t="n">
+        <v>173.1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -25882,6 +26188,12 @@
       </c>
       <c r="FF56" t="n">
         <v>31.6</v>
+      </c>
+      <c r="FG56" t="n">
+        <v>29</v>
+      </c>
+      <c r="FH56" t="n">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -26349,10 +26661,16 @@
       <c r="ET4" t="s">
         <v>161</v>
       </c>
+      <c r="EU4" t="s">
+        <v>162</v>
+      </c>
+      <c r="EV4" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -26796,15 +27114,21 @@
         <v>1.01964016916351</v>
       </c>
       <c r="ES5" t="n">
-        <v>1.10667683063539</v>
+        <v>1.05286758441327</v>
       </c>
       <c r="ET5" t="n">
-        <v>0.956889880274961</v>
+        <v>1.00241270997406</v>
+      </c>
+      <c r="EU5" t="n">
+        <v>1.59453082695134</v>
+      </c>
+      <c r="EV5" t="n">
+        <v>0.733438315680499</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -27251,12 +27575,18 @@
         <v>1.00671140939596</v>
       </c>
       <c r="ET6" t="n">
-        <v>1.1198208286674</v>
+        <v>1.06382978723403</v>
+      </c>
+      <c r="EU6" t="n">
+        <v>0.853242320819113</v>
+      </c>
+      <c r="EV6" t="n">
+        <v>1.08630054315028</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -27704,11 +28034,17 @@
       </c>
       <c r="ET7" t="n">
         <v>-1.76678445229681</v>
+      </c>
+      <c r="EU7" t="n">
+        <v>2.70270270270271</v>
+      </c>
+      <c r="EV7" t="n">
+        <v>-3.09278350515463</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -28155,12 +28491,18 @@
         <v>-1.88133140376268</v>
       </c>
       <c r="ET8" t="n">
-        <v>-1.12130479102956</v>
+        <v>-1.88583078491335</v>
+      </c>
+      <c r="EU8" t="n">
+        <v>-3.33333333333333</v>
+      </c>
+      <c r="EV8" t="n">
+        <v>-2.77227722772276</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -28608,11 +28950,17 @@
       </c>
       <c r="ET9" t="n">
         <v>0.587084148727993</v>
+      </c>
+      <c r="EU9" t="n">
+        <v>0.638977635782741</v>
+      </c>
+      <c r="EV9" t="n">
+        <v>0.60313630880579</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -29060,11 +29408,17 @@
       </c>
       <c r="ET10" t="n">
         <v>3.29059168855246</v>
+      </c>
+      <c r="EU10" t="n">
+        <v>2.82163514147256</v>
+      </c>
+      <c r="EV10" t="n">
+        <v>3.44858554108667</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -29511,12 +29865,18 @@
         <v>4.38144329896908</v>
       </c>
       <c r="ET11" t="n">
-        <v>4.49293966623878</v>
+        <v>4.32178005990587</v>
+      </c>
+      <c r="EU11" t="n">
+        <v>4.53089244851259</v>
+      </c>
+      <c r="EV11" t="n">
+        <v>4.78515624999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -29964,11 +30324,17 @@
       </c>
       <c r="ET12" t="n">
         <v>-1.11464968152868</v>
+      </c>
+      <c r="EU12" t="n">
+        <v>0.16992353440953</v>
+      </c>
+      <c r="EV12" t="n">
+        <v>0.402819738167147</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B13" t="n">
         <v>-1.98675496688743</v>
@@ -30416,11 +30782,17 @@
       </c>
       <c r="ET13" t="n">
         <v>0.781249999999992</v>
+      </c>
+      <c r="EU13" t="n">
+        <v>-1.65289256198346</v>
+      </c>
+      <c r="EV13" t="n">
+        <v>-0.294117647058828</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -30571,10 +30943,12 @@
       <c r="ER14"/>
       <c r="ES14"/>
       <c r="ET14"/>
+      <c r="EU14"/>
+      <c r="EV14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -31021,12 +31395,18 @@
         <v>0.437636761487963</v>
       </c>
       <c r="ET15" t="n">
-        <v>0.102103328568523</v>
+        <v>0.0408413314274138</v>
+      </c>
+      <c r="EU15" t="n">
+        <v>0.0488997555012336</v>
+      </c>
+      <c r="EV15" t="n">
+        <v>0.124937531234369</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -31473,12 +31853,18 @@
         <v>1.7948717948718</v>
       </c>
       <c r="ET16" t="n">
-        <v>1.31278538812786</v>
+        <v>1.28424657534248</v>
+      </c>
+      <c r="EU16" t="n">
+        <v>2.39377618192697</v>
+      </c>
+      <c r="EV16" t="n">
+        <v>2.65957446808511</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -31629,10 +32015,12 @@
       <c r="ER17"/>
       <c r="ES17"/>
       <c r="ET17"/>
+      <c r="EU17"/>
+      <c r="EV17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -32079,12 +32467,18 @@
         <v>-0.311041990668745</v>
       </c>
       <c r="ET18" t="n">
-        <v>-0.323624595469249</v>
+        <v>-0.485436893203879</v>
+      </c>
+      <c r="EU18" t="n">
+        <v>-0.504201680672264</v>
+      </c>
+      <c r="EV18" t="n">
+        <v>0.188323917137466</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -32532,11 +32926,17 @@
       </c>
       <c r="ET19" t="n">
         <v>2.69792127377265</v>
+      </c>
+      <c r="EU19" t="n">
+        <v>2.8462090408993</v>
+      </c>
+      <c r="EV19" t="n">
+        <v>-0.800000000000011</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -32983,12 +33383,18 @@
         <v>0.887573964497039</v>
       </c>
       <c r="ET20" t="n">
-        <v>-1.42977291841885</v>
+        <v>-1.47182506307822</v>
+      </c>
+      <c r="EU20" t="n">
+        <v>-1.15635997988938</v>
+      </c>
+      <c r="EV20" t="n">
+        <v>5.72429906542057</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -33435,12 +33841,18 @@
         <v>0.470114170584277</v>
       </c>
       <c r="ET21" t="n">
-        <v>2.02565833896018</v>
+        <v>1.1478730587441</v>
+      </c>
+      <c r="EU21" t="n">
+        <v>3.54984894259822</v>
+      </c>
+      <c r="EV21" t="n">
+        <v>1.38648180242634</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -33887,12 +34299,18 @@
         <v>-0.43352601156069</v>
       </c>
       <c r="ET22" t="n">
-        <v>1.8896447467876</v>
+        <v>1.81405895691608</v>
+      </c>
+      <c r="EU22" t="n">
+        <v>1.09519797809605</v>
+      </c>
+      <c r="EV22" t="n">
+        <v>0.61475409836065</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -34339,12 +34757,18 @@
         <v>1.15712545676005</v>
       </c>
       <c r="ET23" t="n">
-        <v>1.40415140415139</v>
+        <v>1.28205128205126</v>
+      </c>
+      <c r="EU23" t="n">
+        <v>1.16807268007788</v>
+      </c>
+      <c r="EV23" t="n">
+        <v>1.46945088940447</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -34792,11 +35216,17 @@
       </c>
       <c r="ET24" t="n">
         <v>0.801068090787709</v>
+      </c>
+      <c r="EU24" t="n">
+        <v>0.861450107681255</v>
+      </c>
+      <c r="EV24" t="n">
+        <v>0.755857898715041</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -35244,11 +35674,17 @@
       </c>
       <c r="ET25" t="n">
         <v>-0.202429149797574</v>
+      </c>
+      <c r="EU25" t="n">
+        <v>1.50537634408603</v>
+      </c>
+      <c r="EV25" t="n">
+        <v>0.761421319796965</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -35696,11 +36132,17 @@
       </c>
       <c r="ET26" t="n">
         <v>3.91304347826087</v>
+      </c>
+      <c r="EU26" t="n">
+        <v>3.72585096596137</v>
+      </c>
+      <c r="EV26" t="n">
+        <v>3.79746835443039</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -36148,11 +36590,17 @@
       </c>
       <c r="ET27" t="n">
         <v>-0.121852152721369</v>
+      </c>
+      <c r="EU27" t="n">
+        <v>-0.248344370860937</v>
+      </c>
+      <c r="EV27" t="n">
+        <v>-0.418994413407824</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -36600,11 +37048,17 @@
       </c>
       <c r="ET28" t="n">
         <v>1.37569603668522</v>
+      </c>
+      <c r="EU28" t="n">
+        <v>0.548320767649063</v>
+      </c>
+      <c r="EV28" t="n">
+        <v>1.5666794038976</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -37051,12 +37505,18 @@
         <v>0.0940291490361959</v>
       </c>
       <c r="ET29" t="n">
-        <v>-0.332225913621271</v>
+        <v>-0.142382534409118</v>
+      </c>
+      <c r="EU29" t="n">
+        <v>1.14999999999999</v>
+      </c>
+      <c r="EV29" t="n">
+        <v>-1.57342657342657</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -37504,11 +37964,17 @@
       </c>
       <c r="ET30" t="n">
         <v>0.877192982456146</v>
+      </c>
+      <c r="EU30" t="n">
+        <v>1.43149284253576</v>
+      </c>
+      <c r="EV30" t="n">
+        <v>-1.57563025210086</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -37659,10 +38125,12 @@
       <c r="ER31"/>
       <c r="ES31"/>
       <c r="ET31"/>
+      <c r="EU31"/>
+      <c r="EV31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -38110,11 +38578,17 @@
       </c>
       <c r="ET32" t="n">
         <v>-1.53846153846154</v>
+      </c>
+      <c r="EU32" t="n">
+        <v>-1.41509433962264</v>
+      </c>
+      <c r="EV32" t="n">
+        <v>-1.9607843137255</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -38561,12 +39035,18 @@
         <v>1.46596858638744</v>
       </c>
       <c r="ET33" t="n">
-        <v>1.87110187110187</v>
+        <v>1.66320166320167</v>
+      </c>
+      <c r="EU33" t="n">
+        <v>2.83125707814269</v>
+      </c>
+      <c r="EV33" t="n">
+        <v>1.64141414141416</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -39013,12 +39493,18 @@
         <v>4.75638051044083</v>
       </c>
       <c r="ET34" t="n">
-        <v>4.83870967741934</v>
+        <v>4.60829493087558</v>
+      </c>
+      <c r="EU34" t="n">
+        <v>3.54706684856752</v>
+      </c>
+      <c r="EV34" t="n">
+        <v>3.68794326241134</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -39465,12 +39951,18 @@
         <v>-0.884955752212402</v>
       </c>
       <c r="ET35" t="n">
-        <v>3.48837209302326</v>
+        <v>3.25581395348839</v>
+      </c>
+      <c r="EU35" t="n">
+        <v>2.8061224489796</v>
+      </c>
+      <c r="EV35" t="n">
+        <v>3.11526479750779</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B36" t="n">
         <v>2.80076384468492</v>
@@ -39917,12 +40409,18 @@
         <v>2.09580838323353</v>
       </c>
       <c r="ET36" t="n">
-        <v>1.86373357775742</v>
+        <v>1.64986251145739</v>
+      </c>
+      <c r="EU36" t="n">
+        <v>1.84432635198501</v>
+      </c>
+      <c r="EV36" t="n">
+        <v>-0.715630885122402</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -40370,11 +40868,17 @@
       </c>
       <c r="ET37" t="n">
         <v>0.991325898389092</v>
+      </c>
+      <c r="EU37" t="n">
+        <v>3.35664335664336</v>
+      </c>
+      <c r="EV37" t="n">
+        <v>3.63349131121643</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -40822,11 +41326,17 @@
       </c>
       <c r="ET38" t="n">
         <v>0.748055056852167</v>
+      </c>
+      <c r="EU38" t="n">
+        <v>0.760687661646145</v>
+      </c>
+      <c r="EV38" t="n">
+        <v>1.01910828025478</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -41274,11 +41784,17 @@
       </c>
       <c r="ET39" t="n">
         <v>1.43554407120297</v>
+      </c>
+      <c r="EU39" t="n">
+        <v>1.43750000000001</v>
+      </c>
+      <c r="EV39" t="n">
+        <v>1.71363290175171</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -41726,11 +42242,17 @@
       </c>
       <c r="ET40" t="n">
         <v>1.01781170483462</v>
+      </c>
+      <c r="EU40" t="n">
+        <v>2.32558139534885</v>
+      </c>
+      <c r="EV40" t="n">
+        <v>0.34602076124568</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -42177,12 +42699,18 @@
         <v>-1.97648236177134</v>
       </c>
       <c r="ET41" t="n">
-        <v>-1.66966349858722</v>
+        <v>-1.7724120215772</v>
+      </c>
+      <c r="EU41" t="n">
+        <v>-1.18686171680928</v>
+      </c>
+      <c r="EV41" t="n">
+        <v>0.402183280666469</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -42630,11 +43158,17 @@
       </c>
       <c r="ET42" t="n">
         <v>0.778715120051907</v>
+      </c>
+      <c r="EU42" t="n">
+        <v>2.89017341040465</v>
+      </c>
+      <c r="EV42" t="n">
+        <v>2.05371248025276</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -43082,11 +43616,17 @@
       </c>
       <c r="ET43" t="n">
         <v>2.30286113049549</v>
+      </c>
+      <c r="EU43" t="n">
+        <v>1.41242937853109</v>
+      </c>
+      <c r="EV43" t="n">
+        <v>-1.49253731343284</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -43534,11 +44074,17 @@
       </c>
       <c r="ET44" t="n">
         <v>1.50875075437536</v>
+      </c>
+      <c r="EU44" t="n">
+        <v>1.85737976782754</v>
+      </c>
+      <c r="EV44" t="n">
+        <v>1.56079854809438</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B45" t="n">
         <v>0.638977635782745</v>
@@ -43986,11 +44532,17 @@
       </c>
       <c r="ET45" t="n">
         <v>-2.04081632653062</v>
+      </c>
+      <c r="EU45" t="n">
+        <v>-5.33807829181494</v>
+      </c>
+      <c r="EV45" t="n">
+        <v>-2.53164556962026</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B46" t="n">
         <v>0.817096165933364</v>
@@ -44437,12 +44989,18 @@
         <v>0.058685446009403</v>
       </c>
       <c r="ET46" t="n">
-        <v>0.421432871764008</v>
+        <v>0.481637567730273</v>
+      </c>
+      <c r="EU46" t="n">
+        <v>0.560747663551405</v>
+      </c>
+      <c r="EV46" t="n">
+        <v>1.47157190635451</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -44890,11 +45448,17 @@
       </c>
       <c r="ET47" t="n">
         <v>1.04166666666666</v>
+      </c>
+      <c r="EU47" t="n">
+        <v>1.16618075801749</v>
+      </c>
+      <c r="EV47" t="n">
+        <v>-0.696864111498255</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -45341,12 +45905,18 @@
         <v>1.53702841173731</v>
       </c>
       <c r="ET48" t="n">
-        <v>1.35004821600772</v>
+        <v>3.32690453230474</v>
+      </c>
+      <c r="EU48" t="n">
+        <v>3.07534597642233</v>
+      </c>
+      <c r="EV48" t="n">
+        <v>3.52526439482961</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -45793,12 +46363,18 @@
         <v>1.38119262261186</v>
       </c>
       <c r="ET49" t="n">
-        <v>1.24141355623603</v>
+        <v>1.25796573698585</v>
+      </c>
+      <c r="EU49" t="n">
+        <v>1.24020325553355</v>
+      </c>
+      <c r="EV49" t="n">
+        <v>0.82004975582789</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -46246,11 +46822,17 @@
       </c>
       <c r="ET50" t="n">
         <v>3.46385542168672</v>
+      </c>
+      <c r="EU50" t="n">
+        <v>3.64789849325931</v>
+      </c>
+      <c r="EV50" t="n">
+        <v>4.26884650317894</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -46698,11 +47280,17 @@
       </c>
       <c r="ET51" t="n">
         <v>-6.11620795107034</v>
+      </c>
+      <c r="EU51" t="n">
+        <v>0</v>
+      </c>
+      <c r="EV51" t="n">
+        <v>-0.387596899224798</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -47150,11 +47738,17 @@
       </c>
       <c r="ET52" t="n">
         <v>1.59950784374038</v>
+      </c>
+      <c r="EU52" t="n">
+        <v>1.8975332068311</v>
+      </c>
+      <c r="EV52" t="n">
+        <v>4.62633451957295</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -47601,12 +48195,18 @@
         <v>0.484351713859915</v>
       </c>
       <c r="ET53" t="n">
-        <v>-1.59082500924899</v>
+        <v>-1.51683314835367</v>
+      </c>
+      <c r="EU53" t="n">
+        <v>-0.985595147839259</v>
+      </c>
+      <c r="EV53" t="n">
+        <v>-2.20498162515313</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -48054,11 +48654,17 @@
       </c>
       <c r="ET54" t="n">
         <v>-1.72955974842766</v>
+      </c>
+      <c r="EU54" t="n">
+        <v>1.24333925399645</v>
+      </c>
+      <c r="EV54" t="n">
+        <v>1.16504854368931</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -48505,12 +49111,18 @@
         <v>-0.789595912679989</v>
       </c>
       <c r="ET55" t="n">
-        <v>0.195599022004879</v>
+        <v>0.488997555012225</v>
+      </c>
+      <c r="EU55" t="n">
+        <v>0.374131480491725</v>
+      </c>
+      <c r="EV55" t="n">
+        <v>1.10981308411215</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -48958,6 +49570,12 @@
       </c>
       <c r="ET56" t="n">
         <v>1.28205128205127</v>
+      </c>
+      <c r="EU56" t="n">
+        <v>1.39860139860139</v>
+      </c>
+      <c r="EV56" t="n">
+        <v>3.73443983402491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on Sept. 19 2025
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -507,6 +507,9 @@
     <t xml:space="preserve">07/01/2025</t>
   </si>
   <si>
+    <t xml:space="preserve">08/01/2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">United States</t>
   </si>
   <si>
@@ -1485,10 +1488,13 @@
       <c r="FH4" t="s">
         <v>163</v>
       </c>
+      <c r="FI4" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1974,15 +1980,18 @@
         <v>11093.6</v>
       </c>
       <c r="FG5" t="n">
-        <v>10506.5</v>
+        <v>10497.9</v>
       </c>
       <c r="FH5" t="n">
-        <v>9339.4</v>
+        <v>9366.5</v>
+      </c>
+      <c r="FI5" t="n">
+        <v>9793.9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2471,12 +2480,15 @@
         <v>177.3</v>
       </c>
       <c r="FH6" t="n">
-        <v>167.5</v>
+        <v>167.7</v>
+      </c>
+      <c r="FI6" t="n">
+        <v>172.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2965,12 +2977,15 @@
         <v>22.8</v>
       </c>
       <c r="FH7" t="n">
-        <v>18.8</v>
+        <v>19</v>
+      </c>
+      <c r="FI7" t="n">
+        <v>21.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3459,12 +3474,15 @@
         <v>150.8</v>
       </c>
       <c r="FH8" t="n">
-        <v>147.3</v>
+        <v>148.5</v>
+      </c>
+      <c r="FI8" t="n">
+        <v>174</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3954,11 +3972,14 @@
       </c>
       <c r="FH9" t="n">
         <v>83.4</v>
+      </c>
+      <c r="FI9" t="n">
+        <v>88.2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4447,12 +4468,15 @@
         <v>1315.5</v>
       </c>
       <c r="FH10" t="n">
-        <v>1151.9</v>
+        <v>1141.6</v>
+      </c>
+      <c r="FI10" t="n">
+        <v>1192.3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4941,12 +4965,15 @@
         <v>228.4</v>
       </c>
       <c r="FH11" t="n">
-        <v>214.6</v>
+        <v>215.2</v>
+      </c>
+      <c r="FI11" t="n">
+        <v>221.7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5436,11 +5463,14 @@
       </c>
       <c r="FH12" t="n">
         <v>99.7</v>
+      </c>
+      <c r="FI12" t="n">
+        <v>100.3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B13" t="n">
         <v>30.2</v>
@@ -5929,12 +5959,15 @@
         <v>35.7</v>
       </c>
       <c r="FH13" t="n">
-        <v>33.9</v>
+        <v>33.8</v>
+      </c>
+      <c r="FI13" t="n">
+        <v>33.1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -6099,10 +6132,11 @@
       <c r="FF14"/>
       <c r="FG14"/>
       <c r="FH14"/>
+      <c r="FI14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6591,12 +6625,15 @@
         <v>409.2</v>
       </c>
       <c r="FH15" t="n">
-        <v>400.7</v>
+        <v>401.5</v>
+      </c>
+      <c r="FI15" t="n">
+        <v>471.3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -7085,12 +7122,15 @@
         <v>342.2</v>
       </c>
       <c r="FH16" t="n">
-        <v>328.1</v>
+        <v>329</v>
+      </c>
+      <c r="FI16" t="n">
+        <v>352.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -7255,10 +7295,11 @@
       <c r="FF17"/>
       <c r="FG17"/>
       <c r="FH17"/>
+      <c r="FI17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7747,12 +7788,15 @@
         <v>59.2</v>
       </c>
       <c r="FH18" t="n">
-        <v>53.2</v>
+        <v>52.8</v>
+      </c>
+      <c r="FI18" t="n">
+        <v>54.2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -8241,12 +8285,15 @@
         <v>430</v>
       </c>
       <c r="FH19" t="n">
-        <v>396.8</v>
+        <v>397.3</v>
+      </c>
+      <c r="FI19" t="n">
+        <v>398.7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8735,12 +8782,15 @@
         <v>196.6</v>
       </c>
       <c r="FH20" t="n">
-        <v>181</v>
+        <v>180.2</v>
+      </c>
+      <c r="FI20" t="n">
+        <v>215.2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -9229,12 +9279,15 @@
         <v>137.1</v>
       </c>
       <c r="FH21" t="n">
-        <v>117</v>
+        <v>116.5</v>
+      </c>
+      <c r="FI21" t="n">
+        <v>122</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9724,11 +9777,14 @@
       </c>
       <c r="FH22" t="n">
         <v>98.2</v>
+      </c>
+      <c r="FI22" t="n">
+        <v>100.4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -10218,11 +10274,14 @@
       </c>
       <c r="FH23" t="n">
         <v>131.2</v>
+      </c>
+      <c r="FI23" t="n">
+        <v>155</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10712,11 +10771,14 @@
       </c>
       <c r="FH24" t="n">
         <v>133.3</v>
+      </c>
+      <c r="FI24" t="n">
+        <v>140</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -11205,12 +11267,15 @@
         <v>47.2</v>
       </c>
       <c r="FH25" t="n">
-        <v>39.7</v>
+        <v>39.8</v>
+      </c>
+      <c r="FI25" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11700,11 +11765,14 @@
       </c>
       <c r="FH26" t="n">
         <v>213.2</v>
+      </c>
+      <c r="FI26" t="n">
+        <v>214.3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -12194,11 +12262,14 @@
       </c>
       <c r="FH27" t="n">
         <v>213.9</v>
+      </c>
+      <c r="FI27" t="n">
+        <v>211.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -12688,11 +12759,14 @@
       </c>
       <c r="FH28" t="n">
         <v>265.8</v>
+      </c>
+      <c r="FI28" t="n">
+        <v>271.6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -13181,12 +13255,15 @@
         <v>202.3</v>
       </c>
       <c r="FH29" t="n">
-        <v>168.9</v>
+        <v>169.8</v>
+      </c>
+      <c r="FI29" t="n">
+        <v>164.2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -13675,12 +13752,15 @@
         <v>99.2</v>
       </c>
       <c r="FH30" t="n">
-        <v>93.7</v>
+        <v>95.1</v>
+      </c>
+      <c r="FI30" t="n">
+        <v>100.4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -13845,10 +13925,11 @@
       <c r="FF31"/>
       <c r="FG31"/>
       <c r="FH31"/>
+      <c r="FI31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -14338,11 +14419,14 @@
       </c>
       <c r="FH32" t="n">
         <v>35</v>
+      </c>
+      <c r="FI32" t="n">
+        <v>36.4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -14831,12 +14915,15 @@
         <v>90.8</v>
       </c>
       <c r="FH33" t="n">
-        <v>80.5</v>
+        <v>80.4</v>
+      </c>
+      <c r="FI33" t="n">
+        <v>82.3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -15325,12 +15412,15 @@
         <v>75.9</v>
       </c>
       <c r="FH34" t="n">
-        <v>73.1</v>
+        <v>72.7</v>
+      </c>
+      <c r="FI34" t="n">
+        <v>77.8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -15819,12 +15909,15 @@
         <v>40.3</v>
       </c>
       <c r="FH35" t="n">
-        <v>33.1</v>
+        <v>32</v>
+      </c>
+      <c r="FI35" t="n">
+        <v>32.6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B36" t="n">
         <v>314.2</v>
@@ -16313,12 +16406,15 @@
         <v>325.8</v>
       </c>
       <c r="FH36" t="n">
-        <v>263.6</v>
+        <v>265.8</v>
+      </c>
+      <c r="FI36" t="n">
+        <v>260.7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -16807,12 +16903,15 @@
         <v>73.9</v>
       </c>
       <c r="FH37" t="n">
-        <v>65.6</v>
+        <v>65.8</v>
+      </c>
+      <c r="FI37" t="n">
+        <v>75.8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -17302,11 +17401,14 @@
       </c>
       <c r="FH38" t="n">
         <v>555.1</v>
+      </c>
+      <c r="FI38" t="n">
+        <v>547.5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -17796,11 +17898,14 @@
       </c>
       <c r="FH39" t="n">
         <v>267.1</v>
+      </c>
+      <c r="FI39" t="n">
+        <v>312.8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -18290,11 +18395,14 @@
       </c>
       <c r="FH40" t="n">
         <v>29</v>
+      </c>
+      <c r="FI40" t="n">
+        <v>29.5</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -18783,12 +18891,15 @@
         <v>358</v>
       </c>
       <c r="FH41" t="n">
-        <v>349.5</v>
+        <v>349.6</v>
+      </c>
+      <c r="FI41" t="n">
+        <v>355.4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -19277,12 +19388,15 @@
         <v>142.4</v>
       </c>
       <c r="FH42" t="n">
-        <v>129.2</v>
+        <v>129.5</v>
+      </c>
+      <c r="FI42" t="n">
+        <v>135.7</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -19771,12 +19885,15 @@
         <v>143.6</v>
       </c>
       <c r="FH43" t="n">
-        <v>112.2</v>
+        <v>113.6</v>
+      </c>
+      <c r="FI43" t="n">
+        <v>116</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -20266,11 +20383,14 @@
       </c>
       <c r="FH44" t="n">
         <v>279.8</v>
+      </c>
+      <c r="FI44" t="n">
+        <v>291.4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B45" t="n">
         <v>31.3</v>
@@ -20760,11 +20880,14 @@
       </c>
       <c r="FH45" t="n">
         <v>23.1</v>
+      </c>
+      <c r="FI45" t="n">
+        <v>22.9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B46" t="n">
         <v>159.1</v>
@@ -21253,12 +21376,15 @@
         <v>161.4</v>
       </c>
       <c r="FH46" t="n">
-        <v>151.7</v>
+        <v>151.5</v>
+      </c>
+      <c r="FI46" t="n">
+        <v>157</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -21747,12 +21873,15 @@
         <v>34.7</v>
       </c>
       <c r="FH47" t="n">
-        <v>28.5</v>
+        <v>28.6</v>
+      </c>
+      <c r="FI47" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -22242,11 +22371,14 @@
       </c>
       <c r="FH48" t="n">
         <v>176.2</v>
+      </c>
+      <c r="FI48" t="n">
+        <v>190.3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -22735,12 +22867,15 @@
         <v>1175.5</v>
       </c>
       <c r="FH49" t="n">
-        <v>1094.2</v>
+        <v>1097.1</v>
+      </c>
+      <c r="FI49" t="n">
+        <v>1122.2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -23230,11 +23365,14 @@
       </c>
       <c r="FH50" t="n">
         <v>114.8</v>
+      </c>
+      <c r="FI50" t="n">
+        <v>122.2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -23724,11 +23862,14 @@
       </c>
       <c r="FH51" t="n">
         <v>25.7</v>
+      </c>
+      <c r="FI51" t="n">
+        <v>25.6</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -24218,11 +24359,14 @@
       </c>
       <c r="FH52" t="n">
         <v>294</v>
+      </c>
+      <c r="FI52" t="n">
+        <v>303.4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -24711,12 +24855,15 @@
         <v>261.2</v>
       </c>
       <c r="FH53" t="n">
-        <v>239.5</v>
+        <v>240.6</v>
+      </c>
+      <c r="FI53" t="n">
+        <v>227.8</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -25206,11 +25353,14 @@
       </c>
       <c r="FH54" t="n">
         <v>52.1</v>
+      </c>
+      <c r="FI54" t="n">
+        <v>54.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -25699,12 +25849,15 @@
         <v>187.8</v>
       </c>
       <c r="FH55" t="n">
-        <v>173.1</v>
+        <v>171.2</v>
+      </c>
+      <c r="FI55" t="n">
+        <v>171</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -26193,7 +26346,10 @@
         <v>29</v>
       </c>
       <c r="FH56" t="n">
-        <v>25</v>
+        <v>25.5</v>
+      </c>
+      <c r="FI56" t="n">
+        <v>25.9</v>
       </c>
     </row>
   </sheetData>
@@ -26667,10 +26823,13 @@
       <c r="EV4" t="s">
         <v>163</v>
       </c>
+      <c r="EW4" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -27120,15 +27279,18 @@
         <v>1.00241270997406</v>
       </c>
       <c r="EU5" t="n">
-        <v>1.59453082695134</v>
+        <v>1.51137154792294</v>
       </c>
       <c r="EV5" t="n">
-        <v>0.733438315680499</v>
+        <v>1.02573505619432</v>
+      </c>
+      <c r="EW5" t="n">
+        <v>0.650525147472913</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -27581,12 +27743,15 @@
         <v>0.853242320819113</v>
       </c>
       <c r="EV6" t="n">
-        <v>1.08630054315028</v>
+        <v>1.2070006035003</v>
+      </c>
+      <c r="EW6" t="n">
+        <v>1.52761457109285</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -28039,12 +28204,15 @@
         <v>2.70270270270271</v>
       </c>
       <c r="EV7" t="n">
-        <v>-3.09278350515463</v>
+        <v>-2.06185567010309</v>
+      </c>
+      <c r="EW7" t="n">
+        <v>-0.913242009132417</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -28497,12 +28665,15 @@
         <v>-3.33333333333333</v>
       </c>
       <c r="EV8" t="n">
-        <v>-2.77227722772276</v>
+        <v>-1.98019801980198</v>
+      </c>
+      <c r="EW8" t="n">
+        <v>-3.3870072182121</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -28956,11 +29127,14 @@
       </c>
       <c r="EV9" t="n">
         <v>0.60313630880579</v>
+      </c>
+      <c r="EW9" t="n">
+        <v>0.684931506849325</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -29413,12 +29587,15 @@
         <v>2.82163514147256</v>
       </c>
       <c r="EV10" t="n">
-        <v>3.44858554108667</v>
+        <v>2.52357431522226</v>
+      </c>
+      <c r="EW10" t="n">
+        <v>3.2115650969529</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -29871,12 +30048,15 @@
         <v>4.53089244851259</v>
       </c>
       <c r="EV11" t="n">
-        <v>4.78515624999999</v>
+        <v>5.078125</v>
+      </c>
+      <c r="EW11" t="n">
+        <v>3.8407494145199</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -30330,11 +30510,14 @@
       </c>
       <c r="EV12" t="n">
         <v>0.402819738167147</v>
+      </c>
+      <c r="EW12" t="n">
+        <v>0.501002004008016</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B13" t="n">
         <v>-1.98675496688743</v>
@@ -30787,12 +30970,15 @@
         <v>-1.65289256198346</v>
       </c>
       <c r="EV13" t="n">
-        <v>-0.294117647058828</v>
+        <v>-0.588235294117655</v>
+      </c>
+      <c r="EW13" t="n">
+        <v>-0.898203592814363</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -30945,10 +31131,11 @@
       <c r="ET14"/>
       <c r="EU14"/>
       <c r="EV14"/>
+      <c r="EW14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -31401,12 +31588,15 @@
         <v>0.0488997555012336</v>
       </c>
       <c r="EV15" t="n">
-        <v>0.124937531234369</v>
+        <v>0.324837581209384</v>
+      </c>
+      <c r="EW15" t="n">
+        <v>0.383386581469639</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -31859,12 +32049,15 @@
         <v>2.39377618192697</v>
       </c>
       <c r="EV16" t="n">
-        <v>2.65957446808511</v>
+        <v>2.94117647058823</v>
+      </c>
+      <c r="EW16" t="n">
+        <v>1.2072434607646</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -32017,10 +32210,11 @@
       <c r="ET17"/>
       <c r="EU17"/>
       <c r="EV17"/>
+      <c r="EW17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -32473,12 +32667,15 @@
         <v>-0.504201680672264</v>
       </c>
       <c r="EV18" t="n">
-        <v>0.188323917137466</v>
+        <v>-0.564971751412437</v>
+      </c>
+      <c r="EW18" t="n">
+        <v>-3.38680926916222</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -32931,12 +33128,15 @@
         <v>2.8462090408993</v>
       </c>
       <c r="EV19" t="n">
-        <v>-0.800000000000011</v>
+        <v>-0.675000000000011</v>
+      </c>
+      <c r="EW19" t="n">
+        <v>-2.77980980248721</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -33389,12 +33589,15 @@
         <v>-1.15635997988938</v>
       </c>
       <c r="EV20" t="n">
-        <v>5.72429906542057</v>
+        <v>5.25700934579439</v>
+      </c>
+      <c r="EW20" t="n">
+        <v>-4.1852181656278</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -33847,12 +34050,15 @@
         <v>3.54984894259822</v>
       </c>
       <c r="EV21" t="n">
-        <v>1.38648180242634</v>
+        <v>0.953206239168106</v>
+      </c>
+      <c r="EW21" t="n">
+        <v>0.993377483443711</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -34306,11 +34512,14 @@
       </c>
       <c r="EV22" t="n">
         <v>0.61475409836065</v>
+      </c>
+      <c r="EW22" t="n">
+        <v>-7.97433547204399</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -34764,11 +34973,14 @@
       </c>
       <c r="EV23" t="n">
         <v>1.46945088940447</v>
+      </c>
+      <c r="EW23" t="n">
+        <v>1.30718954248366</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -35222,11 +35434,14 @@
       </c>
       <c r="EV24" t="n">
         <v>0.755857898715041</v>
+      </c>
+      <c r="EW24" t="n">
+        <v>0.143061516452066</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -35679,12 +35894,15 @@
         <v>1.50537634408603</v>
       </c>
       <c r="EV25" t="n">
-        <v>0.761421319796965</v>
+        <v>1.01522842639595</v>
+      </c>
+      <c r="EW25" t="n">
+        <v>-0.25575447570331</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -36138,11 +36356,14 @@
       </c>
       <c r="EV26" t="n">
         <v>3.79746835443039</v>
+      </c>
+      <c r="EW26" t="n">
+        <v>3.87784779447408</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -36596,11 +36817,14 @@
       </c>
       <c r="EV27" t="n">
         <v>-0.418994413407824</v>
+      </c>
+      <c r="EW27" t="n">
+        <v>-0.517403574788332</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -37054,11 +37278,14 @@
       </c>
       <c r="EV28" t="n">
         <v>1.5666794038976</v>
+      </c>
+      <c r="EW28" t="n">
+        <v>1.99023657529105</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -37511,12 +37738,15 @@
         <v>1.14999999999999</v>
       </c>
       <c r="EV29" t="n">
-        <v>-1.57342657342657</v>
+        <v>-1.04895104895104</v>
+      </c>
+      <c r="EW29" t="n">
+        <v>-2.72511848341234</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -37969,12 +38199,15 @@
         <v>1.43149284253576</v>
       </c>
       <c r="EV30" t="n">
-        <v>-1.57563025210086</v>
+        <v>-0.105042016806732</v>
+      </c>
+      <c r="EW30" t="n">
+        <v>2.34454638124364</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -38127,10 +38360,11 @@
       <c r="ET31"/>
       <c r="EU31"/>
       <c r="EV31"/>
+      <c r="EW31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -38584,11 +38818,14 @@
       </c>
       <c r="EV32" t="n">
         <v>-1.9607843137255</v>
+      </c>
+      <c r="EW32" t="n">
+        <v>-1.8867924528302</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -39041,12 +39278,15 @@
         <v>2.83125707814269</v>
       </c>
       <c r="EV33" t="n">
-        <v>1.64141414141416</v>
+        <v>1.51515151515154</v>
+      </c>
+      <c r="EW33" t="n">
+        <v>1.73053152039554</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -39499,12 +39739,15 @@
         <v>3.54706684856752</v>
       </c>
       <c r="EV34" t="n">
-        <v>3.68794326241134</v>
+        <v>3.12056737588653</v>
+      </c>
+      <c r="EW34" t="n">
+        <v>2.63852242744065</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -39957,12 +40200,15 @@
         <v>2.8061224489796</v>
       </c>
       <c r="EV35" t="n">
-        <v>3.11526479750779</v>
+        <v>-0.311526479750783</v>
+      </c>
+      <c r="EW35" t="n">
+        <v>-4.39882697947214</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B36" t="n">
         <v>2.80076384468492</v>
@@ -40415,12 +40661,15 @@
         <v>1.84432635198501</v>
       </c>
       <c r="EV36" t="n">
-        <v>-0.715630885122402</v>
+        <v>0.11299435028249</v>
+      </c>
+      <c r="EW36" t="n">
+        <v>-1.39939485627836</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -40873,12 +41122,15 @@
         <v>3.35664335664336</v>
       </c>
       <c r="EV37" t="n">
-        <v>3.63349131121643</v>
+        <v>3.94944707740916</v>
+      </c>
+      <c r="EW37" t="n">
+        <v>5.71827057182705</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -41332,11 +41584,14 @@
       </c>
       <c r="EV38" t="n">
         <v>1.01910828025478</v>
+      </c>
+      <c r="EW38" t="n">
+        <v>1.08936484490398</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -41790,11 +42045,14 @@
       </c>
       <c r="EV39" t="n">
         <v>1.71363290175171</v>
+      </c>
+      <c r="EW39" t="n">
+        <v>1.42671854734111</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -42248,11 +42506,14 @@
       </c>
       <c r="EV40" t="n">
         <v>0.34602076124568</v>
+      </c>
+      <c r="EW40" t="n">
+        <v>-3.27868852459016</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -42705,12 +42966,15 @@
         <v>-1.18686171680928</v>
       </c>
       <c r="EV41" t="n">
-        <v>0.402183280666469</v>
+        <v>0.430910657856938</v>
+      </c>
+      <c r="EW41" t="n">
+        <v>1.83381088825216</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -43163,12 +43427,15 @@
         <v>2.89017341040465</v>
       </c>
       <c r="EV42" t="n">
-        <v>2.05371248025276</v>
+        <v>2.29067930489732</v>
+      </c>
+      <c r="EW42" t="n">
+        <v>2.49244712990935</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -43621,12 +43888,15 @@
         <v>1.41242937853109</v>
       </c>
       <c r="EV43" t="n">
-        <v>-1.49253731343284</v>
+        <v>-0.263388937664628</v>
+      </c>
+      <c r="EW43" t="n">
+        <v>0.259291270527223</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -44080,11 +44350,14 @@
       </c>
       <c r="EV44" t="n">
         <v>1.56079854809438</v>
+      </c>
+      <c r="EW44" t="n">
+        <v>1.95941217634708</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B45" t="n">
         <v>0.638977635782745</v>
@@ -44538,11 +44811,14 @@
       </c>
       <c r="EV45" t="n">
         <v>-2.53164556962026</v>
+      </c>
+      <c r="EW45" t="n">
+        <v>-1.71673819742489</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B46" t="n">
         <v>0.817096165933364</v>
@@ -44995,12 +45271,15 @@
         <v>0.560747663551405</v>
       </c>
       <c r="EV46" t="n">
-        <v>1.47157190635451</v>
+        <v>1.33779264214047</v>
+      </c>
+      <c r="EW46" t="n">
+        <v>1.42118863049095</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -45453,12 +45732,15 @@
         <v>1.16618075801749</v>
       </c>
       <c r="EV47" t="n">
-        <v>-0.696864111498255</v>
+        <v>-0.348432055749122</v>
+      </c>
+      <c r="EW47" t="n">
+        <v>1.010101010101</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -45912,11 +46194,14 @@
       </c>
       <c r="EV48" t="n">
         <v>3.52526439482961</v>
+      </c>
+      <c r="EW48" t="n">
+        <v>3.19956616052063</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -46369,12 +46654,15 @@
         <v>1.24020325553355</v>
       </c>
       <c r="EV49" t="n">
-        <v>0.82004975582789</v>
+        <v>1.08725697963696</v>
+      </c>
+      <c r="EW49" t="n">
+        <v>0.853779095892873</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -46828,11 +47116,14 @@
       </c>
       <c r="EV50" t="n">
         <v>4.26884650317894</v>
+      </c>
+      <c r="EW50" t="n">
+        <v>3.91156462585035</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -47286,11 +47577,14 @@
       </c>
       <c r="EV51" t="n">
         <v>-0.387596899224798</v>
+      </c>
+      <c r="EW51" t="n">
+        <v>-3.39622641509433</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -47744,11 +48038,14 @@
       </c>
       <c r="EV52" t="n">
         <v>4.62633451957295</v>
+      </c>
+      <c r="EW52" t="n">
+        <v>3.79746835443037</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -48201,12 +48498,15 @@
         <v>-0.985595147839259</v>
       </c>
       <c r="EV53" t="n">
-        <v>-2.20498162515313</v>
+        <v>-1.75581870151081</v>
+      </c>
+      <c r="EW53" t="n">
+        <v>-1.89491817398794</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -48660,11 +48960,14 @@
       </c>
       <c r="EV54" t="n">
         <v>1.16504854368931</v>
+      </c>
+      <c r="EW54" t="n">
+        <v>1.11317254174396</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -49117,12 +49420,15 @@
         <v>0.374131480491725</v>
       </c>
       <c r="EV55" t="n">
-        <v>1.10981308411215</v>
+        <v>0</v>
+      </c>
+      <c r="EW55" t="n">
+        <v>0.706713780918721</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -49575,7 +49881,10 @@
         <v>1.39860139860139</v>
       </c>
       <c r="EV56" t="n">
-        <v>3.73443983402491</v>
+        <v>5.8091286307054</v>
+      </c>
+      <c r="EW56" t="n">
+        <v>1.17187499999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM Update on December 18, 2025
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -510,6 +510,9 @@
     <t xml:space="preserve">08/01/2025</t>
   </si>
   <si>
+    <t xml:space="preserve">09/01/2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">United States</t>
   </si>
   <si>
@@ -1491,10 +1494,13 @@
       <c r="FI4" t="s">
         <v>164</v>
       </c>
+      <c r="FJ4" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1983,15 +1989,18 @@
         <v>10497.9</v>
       </c>
       <c r="FH5" t="n">
-        <v>9366.5</v>
+        <v>9374.4</v>
       </c>
       <c r="FI5" t="n">
-        <v>9793.9</v>
+        <v>9801.8</v>
+      </c>
+      <c r="FJ5" t="n">
+        <v>10884.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2483,12 +2492,15 @@
         <v>167.7</v>
       </c>
       <c r="FI6" t="n">
-        <v>172.8</v>
+        <v>172.5</v>
+      </c>
+      <c r="FJ6" t="n">
+        <v>179.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2980,12 +2992,15 @@
         <v>19</v>
       </c>
       <c r="FI7" t="n">
-        <v>21.7</v>
+        <v>22.7</v>
+      </c>
+      <c r="FJ7" t="n">
+        <v>26.9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3477,12 +3492,15 @@
         <v>148.5</v>
       </c>
       <c r="FI8" t="n">
-        <v>174</v>
+        <v>174.4</v>
+      </c>
+      <c r="FJ8" t="n">
+        <v>197.8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3975,11 +3993,14 @@
       </c>
       <c r="FI9" t="n">
         <v>88.2</v>
+      </c>
+      <c r="FJ9" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4471,12 +4492,15 @@
         <v>1141.6</v>
       </c>
       <c r="FI10" t="n">
-        <v>1192.3</v>
+        <v>1195.9</v>
+      </c>
+      <c r="FJ10" t="n">
+        <v>1271.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4968,12 +4992,15 @@
         <v>215.2</v>
       </c>
       <c r="FI11" t="n">
-        <v>221.7</v>
+        <v>222</v>
+      </c>
+      <c r="FJ11" t="n">
+        <v>240.7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5466,11 +5493,14 @@
       </c>
       <c r="FI12" t="n">
         <v>100.3</v>
+      </c>
+      <c r="FJ12" t="n">
+        <v>123.8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B13" t="n">
         <v>30.2</v>
@@ -5962,12 +5992,15 @@
         <v>33.8</v>
       </c>
       <c r="FI13" t="n">
-        <v>33.1</v>
+        <v>33.2</v>
+      </c>
+      <c r="FJ13" t="n">
+        <v>37.8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -6133,10 +6166,11 @@
       <c r="FG14"/>
       <c r="FH14"/>
       <c r="FI14"/>
+      <c r="FJ14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6628,12 +6662,15 @@
         <v>401.5</v>
       </c>
       <c r="FI15" t="n">
-        <v>471.3</v>
+        <v>471.2</v>
+      </c>
+      <c r="FJ15" t="n">
+        <v>498.8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -7125,12 +7162,15 @@
         <v>329</v>
       </c>
       <c r="FI16" t="n">
-        <v>352.1</v>
+        <v>348.9</v>
+      </c>
+      <c r="FJ16" t="n">
+        <v>351.7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -7296,10 +7336,11 @@
       <c r="FG17"/>
       <c r="FH17"/>
       <c r="FI17"/>
+      <c r="FJ17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7791,12 +7832,15 @@
         <v>52.8</v>
       </c>
       <c r="FI18" t="n">
-        <v>54.2</v>
+        <v>54.4</v>
+      </c>
+      <c r="FJ18" t="n">
+        <v>60.9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -8288,12 +8332,15 @@
         <v>397.3</v>
       </c>
       <c r="FI19" t="n">
-        <v>398.7</v>
+        <v>409.5</v>
+      </c>
+      <c r="FJ19" t="n">
+        <v>463</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8785,12 +8832,15 @@
         <v>180.2</v>
       </c>
       <c r="FI20" t="n">
-        <v>215.2</v>
+        <v>214.3</v>
+      </c>
+      <c r="FJ20" t="n">
+        <v>235</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -9282,12 +9332,15 @@
         <v>116.5</v>
       </c>
       <c r="FI21" t="n">
-        <v>122</v>
+        <v>122.3</v>
+      </c>
+      <c r="FJ21" t="n">
+        <v>146.7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9779,12 +9832,15 @@
         <v>98.2</v>
       </c>
       <c r="FI22" t="n">
-        <v>100.4</v>
+        <v>104.5</v>
+      </c>
+      <c r="FJ22" t="n">
+        <v>131.6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -10277,11 +10333,14 @@
       </c>
       <c r="FI23" t="n">
         <v>155</v>
+      </c>
+      <c r="FJ23" t="n">
+        <v>165.4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10773,12 +10832,15 @@
         <v>133.3</v>
       </c>
       <c r="FI24" t="n">
-        <v>140</v>
+        <v>140.8</v>
+      </c>
+      <c r="FJ24" t="n">
+        <v>151.2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -11270,12 +11332,15 @@
         <v>39.8</v>
       </c>
       <c r="FI25" t="n">
-        <v>39</v>
+        <v>38.9</v>
+      </c>
+      <c r="FJ25" t="n">
+        <v>47.8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11768,11 +11833,14 @@
       </c>
       <c r="FI26" t="n">
         <v>214.3</v>
+      </c>
+      <c r="FJ26" t="n">
+        <v>234.7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -12265,11 +12333,14 @@
       </c>
       <c r="FI27" t="n">
         <v>211.5</v>
+      </c>
+      <c r="FJ27" t="n">
+        <v>239.2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -12762,11 +12833,14 @@
       </c>
       <c r="FI28" t="n">
         <v>271.6</v>
+      </c>
+      <c r="FJ28" t="n">
+        <v>319.3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -13258,12 +13332,15 @@
         <v>169.8</v>
       </c>
       <c r="FI29" t="n">
-        <v>164.2</v>
+        <v>165.6</v>
+      </c>
+      <c r="FJ29" t="n">
+        <v>199.3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -13755,12 +13832,15 @@
         <v>95.1</v>
       </c>
       <c r="FI30" t="n">
-        <v>100.4</v>
+        <v>99.7</v>
+      </c>
+      <c r="FJ30" t="n">
+        <v>105.2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -13926,10 +14006,11 @@
       <c r="FG31"/>
       <c r="FH31"/>
       <c r="FI31"/>
+      <c r="FJ31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -14422,11 +14503,14 @@
       </c>
       <c r="FI32" t="n">
         <v>36.4</v>
+      </c>
+      <c r="FJ32" t="n">
+        <v>41.2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -14919,11 +15003,14 @@
       </c>
       <c r="FI33" t="n">
         <v>82.3</v>
+      </c>
+      <c r="FJ33" t="n">
+        <v>95.1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -15415,12 +15502,15 @@
         <v>72.7</v>
       </c>
       <c r="FI34" t="n">
-        <v>77.8</v>
+        <v>76.7</v>
+      </c>
+      <c r="FJ34" t="n">
+        <v>88.3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -15913,11 +16003,14 @@
       </c>
       <c r="FI35" t="n">
         <v>32.6</v>
+      </c>
+      <c r="FJ35" t="n">
+        <v>44.3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B36" t="n">
         <v>314.2</v>
@@ -16409,12 +16502,15 @@
         <v>265.8</v>
       </c>
       <c r="FI36" t="n">
-        <v>260.7</v>
+        <v>261.4</v>
+      </c>
+      <c r="FJ36" t="n">
+        <v>315.9</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -16906,12 +17002,15 @@
         <v>65.8</v>
       </c>
       <c r="FI37" t="n">
-        <v>75.8</v>
+        <v>76</v>
+      </c>
+      <c r="FJ37" t="n">
+        <v>83.2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -17404,11 +17503,14 @@
       </c>
       <c r="FI38" t="n">
         <v>547.5</v>
+      </c>
+      <c r="FJ38" t="n">
+        <v>645.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -17901,11 +18003,14 @@
       </c>
       <c r="FI39" t="n">
         <v>312.8</v>
+      </c>
+      <c r="FJ39" t="n">
+        <v>342.6</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -18398,11 +18503,14 @@
       </c>
       <c r="FI40" t="n">
         <v>29.5</v>
+      </c>
+      <c r="FJ40" t="n">
+        <v>38.5</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -18894,12 +19002,15 @@
         <v>349.6</v>
       </c>
       <c r="FI41" t="n">
-        <v>355.4</v>
+        <v>354.3</v>
+      </c>
+      <c r="FJ41" t="n">
+        <v>384.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -19391,12 +19502,15 @@
         <v>129.5</v>
       </c>
       <c r="FI42" t="n">
-        <v>135.7</v>
+        <v>135.3</v>
+      </c>
+      <c r="FJ42" t="n">
+        <v>154.4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -19888,12 +20002,15 @@
         <v>113.6</v>
       </c>
       <c r="FI43" t="n">
-        <v>116</v>
+        <v>115.7</v>
+      </c>
+      <c r="FJ43" t="n">
+        <v>130.4</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -20386,11 +20503,14 @@
       </c>
       <c r="FI44" t="n">
         <v>291.4</v>
+      </c>
+      <c r="FJ44" t="n">
+        <v>335.7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B45" t="n">
         <v>31.3</v>
@@ -20883,11 +21003,14 @@
       </c>
       <c r="FI45" t="n">
         <v>22.9</v>
+      </c>
+      <c r="FJ45" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B46" t="n">
         <v>159.1</v>
@@ -21379,12 +21502,15 @@
         <v>151.5</v>
       </c>
       <c r="FI46" t="n">
-        <v>157</v>
+        <v>157.9</v>
+      </c>
+      <c r="FJ46" t="n">
+        <v>167.1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -21876,12 +22002,15 @@
         <v>28.6</v>
       </c>
       <c r="FI47" t="n">
-        <v>30</v>
+        <v>29.8</v>
+      </c>
+      <c r="FJ47" t="n">
+        <v>37.9</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -22374,11 +22503,14 @@
       </c>
       <c r="FI48" t="n">
         <v>190.3</v>
+      </c>
+      <c r="FJ48" t="n">
+        <v>216.5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -22870,12 +23002,15 @@
         <v>1097.1</v>
       </c>
       <c r="FI49" t="n">
-        <v>1122.2</v>
+        <v>1124.2</v>
+      </c>
+      <c r="FJ49" t="n">
+        <v>1195</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -23368,11 +23503,14 @@
       </c>
       <c r="FI50" t="n">
         <v>122.2</v>
+      </c>
+      <c r="FJ50" t="n">
+        <v>137.3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -23864,12 +24002,15 @@
         <v>25.7</v>
       </c>
       <c r="FI51" t="n">
-        <v>25.6</v>
+        <v>25.9</v>
+      </c>
+      <c r="FJ51" t="n">
+        <v>32.7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -24362,11 +24503,14 @@
       </c>
       <c r="FI52" t="n">
         <v>303.4</v>
+      </c>
+      <c r="FJ52" t="n">
+        <v>337.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -24858,12 +25002,15 @@
         <v>240.6</v>
       </c>
       <c r="FI53" t="n">
-        <v>227.8</v>
+        <v>228</v>
+      </c>
+      <c r="FJ53" t="n">
+        <v>243</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -25356,11 +25503,14 @@
       </c>
       <c r="FI54" t="n">
         <v>54.5</v>
+      </c>
+      <c r="FJ54" t="n">
+        <v>60.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -25852,12 +26002,15 @@
         <v>171.2</v>
       </c>
       <c r="FI55" t="n">
-        <v>171</v>
+        <v>171.5</v>
+      </c>
+      <c r="FJ55" t="n">
+        <v>202</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -26349,7 +26502,10 @@
         <v>25.5</v>
       </c>
       <c r="FI56" t="n">
-        <v>25.9</v>
+        <v>25.7</v>
+      </c>
+      <c r="FJ56" t="n">
+        <v>29.8</v>
       </c>
     </row>
   </sheetData>
@@ -26826,10 +26982,13 @@
       <c r="EW4" t="s">
         <v>164</v>
       </c>
+      <c r="EX4" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -27282,15 +27441,18 @@
         <v>1.51137154792294</v>
       </c>
       <c r="EV5" t="n">
-        <v>1.02573505619432</v>
+        <v>1.11094333110426</v>
       </c>
       <c r="EW5" t="n">
-        <v>0.650525147472913</v>
+        <v>0.731712330174901</v>
+      </c>
+      <c r="EX5" t="n">
+        <v>0.685438366048158</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -27746,12 +27908,15 @@
         <v>1.2070006035003</v>
       </c>
       <c r="EW6" t="n">
-        <v>1.52761457109285</v>
+        <v>1.35135135135136</v>
+      </c>
+      <c r="EX6" t="n">
+        <v>1.52714932126696</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -28207,12 +28372,15 @@
         <v>-2.06185567010309</v>
       </c>
       <c r="EW7" t="n">
-        <v>-0.913242009132417</v>
+        <v>3.65296803652968</v>
+      </c>
+      <c r="EX7" t="n">
+        <v>-1.1029411764706</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -28668,12 +28836,15 @@
         <v>-1.98019801980198</v>
       </c>
       <c r="EW8" t="n">
-        <v>-3.3870072182121</v>
+        <v>-3.16490838423099</v>
+      </c>
+      <c r="EX8" t="n">
+        <v>-1.543056246889</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -29130,11 +29301,14 @@
       </c>
       <c r="EW9" t="n">
         <v>0.684931506849325</v>
+      </c>
+      <c r="EX9" t="n">
+        <v>0.591715976331355</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -29590,12 +29764,15 @@
         <v>2.52357431522226</v>
       </c>
       <c r="EW10" t="n">
-        <v>3.2115650969529</v>
+        <v>3.52319944598338</v>
+      </c>
+      <c r="EX10" t="n">
+        <v>3.06494770128922</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -30051,12 +30228,15 @@
         <v>5.078125</v>
       </c>
       <c r="EW11" t="n">
-        <v>3.8407494145199</v>
+        <v>3.98126463700234</v>
+      </c>
+      <c r="EX11" t="n">
+        <v>3.57142857142856</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -30513,11 +30693,14 @@
       </c>
       <c r="EW12" t="n">
         <v>0.501002004008016</v>
+      </c>
+      <c r="EX12" t="n">
+        <v>0.65040650406505</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B13" t="n">
         <v>-1.98675496688743</v>
@@ -30973,12 +31156,15 @@
         <v>-0.588235294117655</v>
       </c>
       <c r="EW13" t="n">
-        <v>-0.898203592814363</v>
+        <v>-0.598802395209568</v>
+      </c>
+      <c r="EX13" t="n">
+        <v>-1.04712041884818</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -31132,10 +31318,11 @@
       <c r="EU14"/>
       <c r="EV14"/>
       <c r="EW14"/>
+      <c r="EX14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -31591,12 +31778,15 @@
         <v>0.324837581209384</v>
       </c>
       <c r="EW15" t="n">
-        <v>0.383386581469639</v>
+        <v>0.362087326943555</v>
+      </c>
+      <c r="EX15" t="n">
+        <v>0.382370698329651</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -32052,12 +32242,15 @@
         <v>2.94117647058823</v>
       </c>
       <c r="EW16" t="n">
-        <v>1.2072434607646</v>
+        <v>0.287438919229664</v>
+      </c>
+      <c r="EX16" t="n">
+        <v>-0.649717514124281</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -32211,10 +32404,11 @@
       <c r="EU17"/>
       <c r="EV17"/>
       <c r="EW17"/>
+      <c r="EX17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -32670,12 +32864,15 @@
         <v>-0.564971751412437</v>
       </c>
       <c r="EW18" t="n">
-        <v>-3.38680926916222</v>
+        <v>-3.03030303030304</v>
+      </c>
+      <c r="EX18" t="n">
+        <v>-0.490196078431379</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -33131,12 +33328,15 @@
         <v>-0.675000000000011</v>
       </c>
       <c r="EW19" t="n">
-        <v>-2.77980980248721</v>
+        <v>-0.146305779078279</v>
+      </c>
+      <c r="EX19" t="n">
+        <v>2.88888888888889</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -33592,12 +33792,15 @@
         <v>5.25700934579439</v>
       </c>
       <c r="EW20" t="n">
-        <v>-4.1852181656278</v>
+        <v>-4.58593054318789</v>
+      </c>
+      <c r="EX20" t="n">
+        <v>0.988397077782558</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -34053,12 +34256,15 @@
         <v>0.953206239168106</v>
       </c>
       <c r="EW21" t="n">
-        <v>0.993377483443711</v>
+        <v>1.24172185430464</v>
+      </c>
+      <c r="EX21" t="n">
+        <v>1.52249134948096</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -34514,12 +34720,15 @@
         <v>0.61475409836065</v>
       </c>
       <c r="EW22" t="n">
-        <v>-7.97433547204399</v>
+        <v>-4.21631530705774</v>
+      </c>
+      <c r="EX22" t="n">
+        <v>-0.903614457831338</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -34976,11 +35185,14 @@
       </c>
       <c r="EW23" t="n">
         <v>1.30718954248366</v>
+      </c>
+      <c r="EX23" t="n">
+        <v>1.28597672994488</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -35436,12 +35648,15 @@
         <v>0.755857898715041</v>
       </c>
       <c r="EW24" t="n">
-        <v>0.143061516452066</v>
+        <v>0.715307582260372</v>
+      </c>
+      <c r="EX24" t="n">
+        <v>0.598802395209566</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -35897,12 +36112,15 @@
         <v>1.01522842639595</v>
       </c>
       <c r="EW25" t="n">
-        <v>-0.25575447570331</v>
+        <v>-0.511508951406639</v>
+      </c>
+      <c r="EX25" t="n">
+        <v>-0.416666666666673</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -36359,11 +36577,14 @@
       </c>
       <c r="EW26" t="n">
         <v>3.87784779447408</v>
+      </c>
+      <c r="EX26" t="n">
+        <v>3.75773651635722</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -36820,11 +37041,14 @@
       </c>
       <c r="EW27" t="n">
         <v>-0.517403574788332</v>
+      </c>
+      <c r="EX27" t="n">
+        <v>-0.457761131918445</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -37281,11 +37505,14 @@
       </c>
       <c r="EW28" t="n">
         <v>1.99023657529105</v>
+      </c>
+      <c r="EX28" t="n">
+        <v>2.20870678617159</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -37741,12 +37968,15 @@
         <v>-1.04895104895104</v>
       </c>
       <c r="EW29" t="n">
-        <v>-2.72511848341234</v>
+        <v>-1.89573459715641</v>
+      </c>
+      <c r="EX29" t="n">
+        <v>-0.845771144278601</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -38202,12 +38432,15 @@
         <v>-0.105042016806732</v>
       </c>
       <c r="EW30" t="n">
-        <v>2.34454638124364</v>
+        <v>1.6309887869521</v>
+      </c>
+      <c r="EX30" t="n">
+        <v>1.0566762728146</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -38361,10 +38594,11 @@
       <c r="EU31"/>
       <c r="EV31"/>
       <c r="EW31"/>
+      <c r="EX31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -38821,11 +39055,14 @@
       </c>
       <c r="EW32" t="n">
         <v>-1.8867924528302</v>
+      </c>
+      <c r="EX32" t="n">
+        <v>-1.43540669856458</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -39282,11 +39519,14 @@
       </c>
       <c r="EW33" t="n">
         <v>1.73053152039554</v>
+      </c>
+      <c r="EX33" t="n">
+        <v>1.38592750533047</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -39742,12 +39982,15 @@
         <v>3.12056737588653</v>
       </c>
       <c r="EW34" t="n">
-        <v>2.63852242744065</v>
+        <v>1.18733509234829</v>
+      </c>
+      <c r="EX34" t="n">
+        <v>1.1454753722795</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -40204,11 +40447,14 @@
       </c>
       <c r="EW35" t="n">
         <v>-4.39882697947214</v>
+      </c>
+      <c r="EX35" t="n">
+        <v>0.681818181818175</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B36" t="n">
         <v>2.80076384468492</v>
@@ -40664,12 +40910,15 @@
         <v>0.11299435028249</v>
       </c>
       <c r="EW36" t="n">
-        <v>-1.39939485627836</v>
+        <v>-1.13464447806354</v>
+      </c>
+      <c r="EX36" t="n">
+        <v>0.381315538608213</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -41125,12 +41374,15 @@
         <v>3.94944707740916</v>
       </c>
       <c r="EW37" t="n">
-        <v>5.71827057182705</v>
+        <v>5.99721059972106</v>
+      </c>
+      <c r="EX37" t="n">
+        <v>5.98726114649682</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -41587,11 +41839,14 @@
       </c>
       <c r="EW38" t="n">
         <v>1.08936484490398</v>
+      </c>
+      <c r="EX38" t="n">
+        <v>0.124107973937318</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -42048,11 +42303,14 @@
       </c>
       <c r="EW39" t="n">
         <v>1.42671854734111</v>
+      </c>
+      <c r="EX39" t="n">
+        <v>1.39094406629182</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -42509,11 +42767,14 @@
       </c>
       <c r="EW40" t="n">
         <v>-3.27868852459016</v>
+      </c>
+      <c r="EX40" t="n">
+        <v>-0.259067357512957</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -42969,12 +43230,15 @@
         <v>0.430910657856938</v>
       </c>
       <c r="EW41" t="n">
-        <v>1.83381088825216</v>
+        <v>1.51862464183381</v>
+      </c>
+      <c r="EX41" t="n">
+        <v>0.365821792526777</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -43430,12 +43694,15 @@
         <v>2.29067930489732</v>
       </c>
       <c r="EW42" t="n">
-        <v>2.49244712990935</v>
+        <v>2.19033232628399</v>
+      </c>
+      <c r="EX42" t="n">
+        <v>1.84696569920841</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -43891,12 +44158,15 @@
         <v>-0.263388937664628</v>
       </c>
       <c r="EW43" t="n">
-        <v>0.259291270527223</v>
+        <v>0</v>
+      </c>
+      <c r="EX43" t="n">
+        <v>0.694980694980699</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -44353,11 +44623,14 @@
       </c>
       <c r="EW44" t="n">
         <v>1.95941217634708</v>
+      </c>
+      <c r="EX44" t="n">
+        <v>1.75810851773263</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B45" t="n">
         <v>0.638977635782745</v>
@@ -44814,11 +45087,14 @@
       </c>
       <c r="EW45" t="n">
         <v>-1.71673819742489</v>
+      </c>
+      <c r="EX45" t="n">
+        <v>-1.36054421768707</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B46" t="n">
         <v>0.817096165933364</v>
@@ -45274,12 +45550,15 @@
         <v>1.33779264214047</v>
       </c>
       <c r="EW46" t="n">
-        <v>1.42118863049095</v>
+        <v>2.00258397932814</v>
+      </c>
+      <c r="EX46" t="n">
+        <v>1.08892921960072</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -45735,12 +46014,15 @@
         <v>-0.348432055749122</v>
       </c>
       <c r="EW47" t="n">
-        <v>1.010101010101</v>
+        <v>0.33670033670033</v>
+      </c>
+      <c r="EX47" t="n">
+        <v>0.797872340425562</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -46197,11 +46479,14 @@
       </c>
       <c r="EW48" t="n">
         <v>3.19956616052063</v>
+      </c>
+      <c r="EX48" t="n">
+        <v>3.34128878281623</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -46657,12 +46942,15 @@
         <v>1.08725697963696</v>
       </c>
       <c r="EW49" t="n">
-        <v>0.853779095892873</v>
+        <v>1.03352206344927</v>
+      </c>
+      <c r="EX49" t="n">
+        <v>1.84080449974432</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -47119,11 +47407,14 @@
       </c>
       <c r="EW50" t="n">
         <v>3.91156462585035</v>
+      </c>
+      <c r="EX50" t="n">
+        <v>3.70090634441088</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -47579,12 +47870,15 @@
         <v>-0.387596899224798</v>
       </c>
       <c r="EW51" t="n">
-        <v>-3.39622641509433</v>
+        <v>-2.26415094339622</v>
+      </c>
+      <c r="EX51" t="n">
+        <v>3.80952380952382</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -48041,11 +48335,14 @@
       </c>
       <c r="EW52" t="n">
         <v>3.79746835443037</v>
+      </c>
+      <c r="EX52" t="n">
+        <v>2.67965895249698</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -48501,12 +48798,15 @@
         <v>-1.75581870151081</v>
       </c>
       <c r="EW53" t="n">
-        <v>-1.89491817398794</v>
+        <v>-1.80878552971577</v>
+      </c>
+      <c r="EX53" t="n">
+        <v>-1.93704600484261</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -48963,11 +49263,14 @@
       </c>
       <c r="EW54" t="n">
         <v>1.11317254174396</v>
+      </c>
+      <c r="EX54" t="n">
+        <v>0.665557404326121</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -49423,12 +49726,15 @@
         <v>0</v>
       </c>
       <c r="EW55" t="n">
-        <v>0.706713780918721</v>
+        <v>1.00117785630152</v>
+      </c>
+      <c r="EX55" t="n">
+        <v>-1.75097276264591</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -49884,7 +50190,10 @@
         <v>5.8091286307054</v>
       </c>
       <c r="EW56" t="n">
-        <v>1.17187499999999</v>
+        <v>0.390625000000006</v>
+      </c>
+      <c r="EX56" t="n">
+        <v>-0.334448160535122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SEM update on Jan. 9 2026
</commit_message>
<xml_diff>
--- a/static/data/source/state_and_local_public_education_employment.xlsx
+++ b/static/data/source/state_and_local_public_education_employment.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
   <si>
     <t xml:space="preserve">Geography</t>
   </si>
@@ -513,6 +513,12 @@
     <t xml:space="preserve">09/01/2025</t>
   </si>
   <si>
+    <t xml:space="preserve">10/01/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/01/2025</t>
+  </si>
+  <si>
     <t xml:space="preserve">United States</t>
   </si>
   <si>
@@ -1497,10 +1503,16 @@
       <c r="FJ4" t="s">
         <v>165</v>
       </c>
+      <c r="FK4" t="s">
+        <v>166</v>
+      </c>
+      <c r="FL4" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" t="n">
         <v>10186.6</v>
@@ -1996,11 +2008,17 @@
       </c>
       <c r="FJ5" t="n">
         <v>10884.7</v>
+      </c>
+      <c r="FK5" t="n">
+        <v>11201.1</v>
+      </c>
+      <c r="FL5" t="n">
+        <v>11312.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B6" t="n">
         <v>162</v>
@@ -2496,11 +2514,17 @@
       </c>
       <c r="FJ6" t="n">
         <v>179.5</v>
+      </c>
+      <c r="FK6" t="n">
+        <v>182.5</v>
+      </c>
+      <c r="FL6" t="n">
+        <v>183.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" t="n">
         <v>30.4</v>
@@ -2996,11 +3020,17 @@
       </c>
       <c r="FJ7" t="n">
         <v>26.9</v>
+      </c>
+      <c r="FK7" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="FL7" t="n">
+        <v>28.4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" t="n">
         <v>190.5</v>
@@ -3496,11 +3526,17 @@
       </c>
       <c r="FJ8" t="n">
         <v>197.8</v>
+      </c>
+      <c r="FK8" t="n">
+        <v>201.3</v>
+      </c>
+      <c r="FL8" t="n">
+        <v>204.1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" t="n">
         <v>104.8</v>
@@ -3996,11 +4032,17 @@
       </c>
       <c r="FJ9" t="n">
         <v>102</v>
+      </c>
+      <c r="FK9" t="n">
+        <v>103.7</v>
+      </c>
+      <c r="FL9" t="n">
+        <v>103.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" t="n">
         <v>1132.3</v>
@@ -4496,11 +4538,17 @@
       </c>
       <c r="FJ10" t="n">
         <v>1271.1</v>
+      </c>
+      <c r="FK10" t="n">
+        <v>1312.7</v>
+      </c>
+      <c r="FL10" t="n">
+        <v>1334.7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" t="n">
         <v>184.5</v>
@@ -4996,11 +5044,17 @@
       </c>
       <c r="FJ11" t="n">
         <v>240.7</v>
+      </c>
+      <c r="FK11" t="n">
+        <v>246.1</v>
+      </c>
+      <c r="FL11" t="n">
+        <v>248.7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" t="n">
         <v>122.1</v>
@@ -5496,11 +5550,17 @@
       </c>
       <c r="FJ12" t="n">
         <v>123.8</v>
+      </c>
+      <c r="FK12" t="n">
+        <v>127.3</v>
+      </c>
+      <c r="FL12" t="n">
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" t="n">
         <v>30.2</v>
@@ -5996,11 +6056,17 @@
       </c>
       <c r="FJ13" t="n">
         <v>37.8</v>
+      </c>
+      <c r="FK13" t="n">
+        <v>39</v>
+      </c>
+      <c r="FL13" t="n">
+        <v>39.4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -6167,10 +6233,12 @@
       <c r="FH14"/>
       <c r="FI14"/>
       <c r="FJ14"/>
+      <c r="FK14"/>
+      <c r="FL14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B15" t="n">
         <v>490.3</v>
@@ -6666,11 +6734,17 @@
       </c>
       <c r="FJ15" t="n">
         <v>498.8</v>
+      </c>
+      <c r="FK15" t="n">
+        <v>506.3</v>
+      </c>
+      <c r="FL15" t="n">
+        <v>505.8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B16" t="n">
         <v>345.9</v>
@@ -7166,11 +7240,17 @@
       </c>
       <c r="FJ16" t="n">
         <v>351.7</v>
+      </c>
+      <c r="FK16" t="n">
+        <v>354.6</v>
+      </c>
+      <c r="FL16" t="n">
+        <v>355.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -7337,10 +7417,12 @@
       <c r="FH17"/>
       <c r="FI17"/>
       <c r="FJ17"/>
+      <c r="FK17"/>
+      <c r="FL17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B18" t="n">
         <v>52.4</v>
@@ -7836,11 +7918,17 @@
       </c>
       <c r="FJ18" t="n">
         <v>60.9</v>
+      </c>
+      <c r="FK18" t="n">
+        <v>62.9</v>
+      </c>
+      <c r="FL18" t="n">
+        <v>63.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B19" t="n">
         <v>435.1</v>
@@ -8336,11 +8424,17 @@
       </c>
       <c r="FJ19" t="n">
         <v>463</v>
+      </c>
+      <c r="FK19" t="n">
+        <v>471.8</v>
+      </c>
+      <c r="FL19" t="n">
+        <v>473.6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B20" t="n">
         <v>236</v>
@@ -8836,11 +8930,17 @@
       </c>
       <c r="FJ20" t="n">
         <v>235</v>
+      </c>
+      <c r="FK20" t="n">
+        <v>235.6</v>
+      </c>
+      <c r="FL20" t="n">
+        <v>237.8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B21" t="n">
         <v>139</v>
@@ -9336,11 +9436,17 @@
       </c>
       <c r="FJ21" t="n">
         <v>146.7</v>
+      </c>
+      <c r="FK21" t="n">
+        <v>152.4</v>
+      </c>
+      <c r="FL21" t="n">
+        <v>153.6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B22" t="n">
         <v>135.1</v>
@@ -9836,11 +9942,17 @@
       </c>
       <c r="FJ22" t="n">
         <v>131.6</v>
+      </c>
+      <c r="FK22" t="n">
+        <v>137.6</v>
+      </c>
+      <c r="FL22" t="n">
+        <v>138.7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B23" t="n">
         <v>171.5</v>
@@ -10336,11 +10448,17 @@
       </c>
       <c r="FJ23" t="n">
         <v>165.4</v>
+      </c>
+      <c r="FK23" t="n">
+        <v>167.1</v>
+      </c>
+      <c r="FL23" t="n">
+        <v>168.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B24" t="n">
         <v>160.9</v>
@@ -10836,11 +10954,17 @@
       </c>
       <c r="FJ24" t="n">
         <v>151.2</v>
+      </c>
+      <c r="FK24" t="n">
+        <v>154.1</v>
+      </c>
+      <c r="FL24" t="n">
+        <v>155.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B25" t="n">
         <v>50.7</v>
@@ -11336,11 +11460,17 @@
       </c>
       <c r="FJ25" t="n">
         <v>47.8</v>
+      </c>
+      <c r="FK25" t="n">
+        <v>49.1</v>
+      </c>
+      <c r="FL25" t="n">
+        <v>49.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B26" t="n">
         <v>194.8</v>
@@ -11836,11 +11966,17 @@
       </c>
       <c r="FJ26" t="n">
         <v>234.7</v>
+      </c>
+      <c r="FK26" t="n">
+        <v>237.4</v>
+      </c>
+      <c r="FL26" t="n">
+        <v>240.7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B27" t="n">
         <v>216.5</v>
@@ -12336,11 +12472,17 @@
       </c>
       <c r="FJ27" t="n">
         <v>239.2</v>
+      </c>
+      <c r="FK27" t="n">
+        <v>245.5</v>
+      </c>
+      <c r="FL27" t="n">
+        <v>248.1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B28" t="n">
         <v>326.8</v>
@@ -12836,11 +12978,17 @@
       </c>
       <c r="FJ28" t="n">
         <v>319.3</v>
+      </c>
+      <c r="FK28" t="n">
+        <v>330.2</v>
+      </c>
+      <c r="FL28" t="n">
+        <v>334.2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B29" t="n">
         <v>201</v>
@@ -13336,11 +13484,17 @@
       </c>
       <c r="FJ29" t="n">
         <v>199.3</v>
+      </c>
+      <c r="FK29" t="n">
+        <v>211.3</v>
+      </c>
+      <c r="FL29" t="n">
+        <v>213.7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B30" t="n">
         <v>106.5</v>
@@ -13836,11 +13990,17 @@
       </c>
       <c r="FJ30" t="n">
         <v>105.2</v>
+      </c>
+      <c r="FK30" t="n">
+        <v>105.4</v>
+      </c>
+      <c r="FL30" t="n">
+        <v>105.9</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -14007,10 +14167,12 @@
       <c r="FH31"/>
       <c r="FI31"/>
       <c r="FJ31"/>
+      <c r="FK31"/>
+      <c r="FL31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B32" t="n">
         <v>42.2</v>
@@ -14506,11 +14668,17 @@
       </c>
       <c r="FJ32" t="n">
         <v>41.2</v>
+      </c>
+      <c r="FK32" t="n">
+        <v>41.4</v>
+      </c>
+      <c r="FL32" t="n">
+        <v>41.9</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B33" t="n">
         <v>86.4</v>
@@ -15006,11 +15174,17 @@
       </c>
       <c r="FJ33" t="n">
         <v>95.1</v>
+      </c>
+      <c r="FK33" t="n">
+        <v>98.7</v>
+      </c>
+      <c r="FL33" t="n">
+        <v>99.2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B34" t="n">
         <v>66.2</v>
@@ -15506,11 +15680,17 @@
       </c>
       <c r="FJ34" t="n">
         <v>88.3</v>
+      </c>
+      <c r="FK34" t="n">
+        <v>89.5</v>
+      </c>
+      <c r="FL34" t="n">
+        <v>90.9</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B35" t="n">
         <v>47.3</v>
@@ -16006,11 +16186,17 @@
       </c>
       <c r="FJ35" t="n">
         <v>44.3</v>
+      </c>
+      <c r="FK35" t="n">
+        <v>45.7</v>
+      </c>
+      <c r="FL35" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B36" t="n">
         <v>314.2</v>
@@ -16506,11 +16692,17 @@
       </c>
       <c r="FJ36" t="n">
         <v>315.9</v>
+      </c>
+      <c r="FK36" t="n">
+        <v>336.8</v>
+      </c>
+      <c r="FL36" t="n">
+        <v>339.8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B37" t="n">
         <v>77.3</v>
@@ -17006,11 +17198,17 @@
       </c>
       <c r="FJ37" t="n">
         <v>83.2</v>
+      </c>
+      <c r="FK37" t="n">
+        <v>84.5</v>
+      </c>
+      <c r="FL37" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B38" t="n">
         <v>634.6</v>
@@ -17506,11 +17704,17 @@
       </c>
       <c r="FJ38" t="n">
         <v>645.4</v>
+      </c>
+      <c r="FK38" t="n">
+        <v>671.3</v>
+      </c>
+      <c r="FL38" t="n">
+        <v>676.4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B39" t="n">
         <v>340.2</v>
@@ -18006,11 +18210,17 @@
       </c>
       <c r="FJ39" t="n">
         <v>342.6</v>
+      </c>
+      <c r="FK39" t="n">
+        <v>350.1</v>
+      </c>
+      <c r="FL39" t="n">
+        <v>352.1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B40" t="n">
         <v>37.1</v>
@@ -18506,11 +18716,17 @@
       </c>
       <c r="FJ40" t="n">
         <v>38.5</v>
+      </c>
+      <c r="FK40" t="n">
+        <v>40.4</v>
+      </c>
+      <c r="FL40" t="n">
+        <v>40.9</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B41" t="n">
         <v>374.9</v>
@@ -19006,11 +19222,17 @@
       </c>
       <c r="FJ41" t="n">
         <v>384.1</v>
+      </c>
+      <c r="FK41" t="n">
+        <v>392.5</v>
+      </c>
+      <c r="FL41" t="n">
+        <v>395.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B42" t="n">
         <v>146.7</v>
@@ -19506,11 +19728,17 @@
       </c>
       <c r="FJ42" t="n">
         <v>154.4</v>
+      </c>
+      <c r="FK42" t="n">
+        <v>158.3</v>
+      </c>
+      <c r="FL42" t="n">
+        <v>159.4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B43" t="n">
         <v>130.3</v>
@@ -20006,11 +20234,17 @@
       </c>
       <c r="FJ43" t="n">
         <v>130.4</v>
+      </c>
+      <c r="FK43" t="n">
+        <v>141.4</v>
+      </c>
+      <c r="FL43" t="n">
+        <v>142.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B44" t="n">
         <v>343.9</v>
@@ -20506,11 +20740,17 @@
       </c>
       <c r="FJ44" t="n">
         <v>335.7</v>
+      </c>
+      <c r="FK44" t="n">
+        <v>343.1</v>
+      </c>
+      <c r="FL44" t="n">
+        <v>348.4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B45" t="n">
         <v>31.3</v>
@@ -21006,11 +21246,17 @@
       </c>
       <c r="FJ45" t="n">
         <v>29</v>
+      </c>
+      <c r="FK45" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="FL45" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B46" t="n">
         <v>159.1</v>
@@ -21506,11 +21752,17 @@
       </c>
       <c r="FJ46" t="n">
         <v>167.1</v>
+      </c>
+      <c r="FK46" t="n">
+        <v>168.2</v>
+      </c>
+      <c r="FL46" t="n">
+        <v>169.3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B47" t="n">
         <v>35</v>
@@ -22006,11 +22258,17 @@
       </c>
       <c r="FJ47" t="n">
         <v>37.9</v>
+      </c>
+      <c r="FK47" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="FL47" t="n">
+        <v>39.4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B48" t="n">
         <v>194.7</v>
@@ -22506,11 +22764,17 @@
       </c>
       <c r="FJ48" t="n">
         <v>216.5</v>
+      </c>
+      <c r="FK48" t="n">
+        <v>222.5</v>
+      </c>
+      <c r="FL48" t="n">
+        <v>224.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B49" t="n">
         <v>1029.4</v>
@@ -23006,11 +23270,17 @@
       </c>
       <c r="FJ49" t="n">
         <v>1195</v>
+      </c>
+      <c r="FK49" t="n">
+        <v>1226.4</v>
+      </c>
+      <c r="FL49" t="n">
+        <v>1233.3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B50" t="n">
         <v>109.5</v>
@@ -23506,11 +23776,17 @@
       </c>
       <c r="FJ50" t="n">
         <v>137.3</v>
+      </c>
+      <c r="FK50" t="n">
+        <v>140.8</v>
+      </c>
+      <c r="FL50" t="n">
+        <v>142</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B51" t="n">
         <v>33</v>
@@ -24006,11 +24282,17 @@
       </c>
       <c r="FJ51" t="n">
         <v>32.7</v>
+      </c>
+      <c r="FK51" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="FL51" t="n">
+        <v>34.4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B52" t="n">
         <v>311.5</v>
@@ -24506,11 +24788,17 @@
       </c>
       <c r="FJ52" t="n">
         <v>337.2</v>
+      </c>
+      <c r="FK52" t="n">
+        <v>348.1</v>
+      </c>
+      <c r="FL52" t="n">
+        <v>354.1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B53" t="n">
         <v>240.6</v>
@@ -25006,11 +25294,17 @@
       </c>
       <c r="FJ53" t="n">
         <v>243</v>
+      </c>
+      <c r="FK53" t="n">
+        <v>258.6</v>
+      </c>
+      <c r="FL53" t="n">
+        <v>263.4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B54" t="n">
         <v>68.9</v>
@@ -25506,11 +25800,17 @@
       </c>
       <c r="FJ54" t="n">
         <v>60.5</v>
+      </c>
+      <c r="FK54" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="FL54" t="n">
+        <v>63.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B55" t="n">
         <v>199.2</v>
@@ -26006,11 +26306,17 @@
       </c>
       <c r="FJ55" t="n">
         <v>202</v>
+      </c>
+      <c r="FK55" t="n">
+        <v>208.3</v>
+      </c>
+      <c r="FL55" t="n">
+        <v>210.7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B56" t="n">
         <v>31.4</v>
@@ -26506,6 +26812,12 @@
       </c>
       <c r="FJ56" t="n">
         <v>29.8</v>
+      </c>
+      <c r="FK56" t="n">
+        <v>31</v>
+      </c>
+      <c r="FL56" t="n">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -26985,10 +27297,16 @@
       <c r="EX4" t="s">
         <v>165</v>
       </c>
+      <c r="EY4" t="s">
+        <v>166</v>
+      </c>
+      <c r="EZ4" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" t="n">
         <v>-0.321009954253634</v>
@@ -27448,11 +27766,17 @@
       </c>
       <c r="EX5" t="n">
         <v>0.685438366048158</v>
+      </c>
+      <c r="EY5" t="n">
+        <v>0.298178692311802</v>
+      </c>
+      <c r="EZ5" t="n">
+        <v>0.274795897563197</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B6" t="n">
         <v>-0.370370370370367</v>
@@ -27912,11 +28236,17 @@
       </c>
       <c r="EX6" t="n">
         <v>1.52714932126696</v>
+      </c>
+      <c r="EY6" t="n">
+        <v>1.10803324099723</v>
+      </c>
+      <c r="EZ6" t="n">
+        <v>1.10071546505228</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" t="n">
         <v>-0.328947368421057</v>
@@ -28376,11 +28706,17 @@
       </c>
       <c r="EX7" t="n">
         <v>-1.1029411764706</v>
+      </c>
+      <c r="EY7" t="n">
+        <v>-1.40350877192982</v>
+      </c>
+      <c r="EZ7" t="n">
+        <v>-1.04529616724739</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" t="n">
         <v>1.67979002624671</v>
@@ -28840,11 +29176,17 @@
       </c>
       <c r="EX8" t="n">
         <v>-1.543056246889</v>
+      </c>
+      <c r="EY8" t="n">
+        <v>-1.12966601178781</v>
+      </c>
+      <c r="EZ8" t="n">
+        <v>-0.826044703595732</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B9" t="n">
         <v>0.0954198473282388</v>
@@ -29304,11 +29646,17 @@
       </c>
       <c r="EX9" t="n">
         <v>0.591715976331355</v>
+      </c>
+      <c r="EY9" t="n">
+        <v>0.67961165048544</v>
+      </c>
+      <c r="EZ9" t="n">
+        <v>0.678294573643414</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B10" t="n">
         <v>-0.556389649386201</v>
@@ -29768,11 +30116,17 @@
       </c>
       <c r="EX10" t="n">
         <v>3.06494770128922</v>
+      </c>
+      <c r="EY10" t="n">
+        <v>1.65724463718732</v>
+      </c>
+      <c r="EZ10" t="n">
+        <v>1.83108262760355</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B11" t="n">
         <v>0.433604336043367</v>
@@ -30232,11 +30586,17 @@
       </c>
       <c r="EX11" t="n">
         <v>3.57142857142856</v>
+      </c>
+      <c r="EY11" t="n">
+        <v>3.35993280134396</v>
+      </c>
+      <c r="EZ11" t="n">
+        <v>3.15221899626711</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B12" t="n">
         <v>1.06470106470107</v>
@@ -30696,11 +31056,17 @@
       </c>
       <c r="EX12" t="n">
         <v>0.65040650406505</v>
+      </c>
+      <c r="EY12" t="n">
+        <v>1.59616919393457</v>
+      </c>
+      <c r="EZ12" t="n">
+        <v>1.50674068199842</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" t="n">
         <v>-1.98675496688743</v>
@@ -31160,11 +31526,17 @@
       </c>
       <c r="EX13" t="n">
         <v>-1.04712041884818</v>
+      </c>
+      <c r="EY13" t="n">
+        <v>-0.51020408163266</v>
+      </c>
+      <c r="EZ13" t="n">
+        <v>-0.755667506297222</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -31319,10 +31691,12 @@
       <c r="EV14"/>
       <c r="EW14"/>
       <c r="EX14"/>
+      <c r="EY14"/>
+      <c r="EZ14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B15" t="n">
         <v>0.877014073016534</v>
@@ -31782,11 +32156,17 @@
       </c>
       <c r="EX15" t="n">
         <v>0.382370698329651</v>
+      </c>
+      <c r="EY15" t="n">
+        <v>1.13863363963244</v>
+      </c>
+      <c r="EZ15" t="n">
+        <v>0.377058940265921</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B16" t="n">
         <v>-1.35877421220004</v>
@@ -32246,11 +32626,17 @@
       </c>
       <c r="EX16" t="n">
         <v>-0.649717514124281</v>
+      </c>
+      <c r="EY16" t="n">
+        <v>-0.365271143579644</v>
+      </c>
+      <c r="EZ16" t="n">
+        <v>-0.420285794340151</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -32405,10 +32791,12 @@
       <c r="EV17"/>
       <c r="EW17"/>
       <c r="EX17"/>
+      <c r="EY17"/>
+      <c r="EZ17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B18" t="n">
         <v>3.43511450381679</v>
@@ -32868,11 +33256,17 @@
       </c>
       <c r="EX18" t="n">
         <v>-0.490196078431379</v>
+      </c>
+      <c r="EY18" t="n">
+        <v>-2.48062015503875</v>
+      </c>
+      <c r="EZ18" t="n">
+        <v>-2.00617283950617</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B19" t="n">
         <v>1.33302689037002</v>
@@ -33332,11 +33726,17 @@
       </c>
       <c r="EX19" t="n">
         <v>2.88888888888889</v>
+      </c>
+      <c r="EY19" t="n">
+        <v>1.96671709531012</v>
+      </c>
+      <c r="EZ19" t="n">
+        <v>1.8494623655914</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B20" t="n">
         <v>-1.48305084745763</v>
@@ -33796,11 +34196,17 @@
       </c>
       <c r="EX20" t="n">
         <v>0.988397077782558</v>
+      </c>
+      <c r="EY20" t="n">
+        <v>-0.211774671749247</v>
+      </c>
+      <c r="EZ20" t="n">
+        <v>-1.4504765851637</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B21" t="n">
         <v>0.143884892086323</v>
@@ -34260,11 +34666,17 @@
       </c>
       <c r="EX21" t="n">
         <v>1.52249134948096</v>
+      </c>
+      <c r="EY21" t="n">
+        <v>1.8716577540107</v>
+      </c>
+      <c r="EZ21" t="n">
+        <v>1.72185430463576</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B22" t="n">
         <v>-0.888230940044403</v>
@@ -34724,11 +35136,17 @@
       </c>
       <c r="EX22" t="n">
         <v>-0.903614457831338</v>
+      </c>
+      <c r="EY22" t="n">
+        <v>-0.649819494584842</v>
+      </c>
+      <c r="EZ22" t="n">
+        <v>-0.64469914040115</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B23" t="n">
         <v>-0.349854227405261</v>
@@ -35188,11 +35606,17 @@
       </c>
       <c r="EX23" t="n">
         <v>1.28597672994488</v>
+      </c>
+      <c r="EY23" t="n">
+        <v>1.45719489981785</v>
+      </c>
+      <c r="EZ23" t="n">
+        <v>0.958657878969439</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B24" t="n">
         <v>-3.60472343070231</v>
@@ -35652,11 +36076,17 @@
       </c>
       <c r="EX24" t="n">
         <v>0.598802395209566</v>
+      </c>
+      <c r="EY24" t="n">
+        <v>0.195058517555255</v>
+      </c>
+      <c r="EZ24" t="n">
+        <v>0.258231116849584</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B25" t="n">
         <v>0.986193293885616</v>
@@ -36116,11 +36546,17 @@
       </c>
       <c r="EX25" t="n">
         <v>-0.416666666666673</v>
+      </c>
+      <c r="EY25" t="n">
+        <v>-0.607287449392735</v>
+      </c>
+      <c r="EZ25" t="n">
+        <v>-0.402414486921535</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B26" t="n">
         <v>1.43737166324436</v>
@@ -36580,11 +37016,17 @@
       </c>
       <c r="EX26" t="n">
         <v>3.75773651635722</v>
+      </c>
+      <c r="EY26" t="n">
+        <v>3.12771503040834</v>
+      </c>
+      <c r="EZ26" t="n">
+        <v>2.90722530996153</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B27" t="n">
         <v>1.10854503464202</v>
@@ -37044,11 +37486,17 @@
       </c>
       <c r="EX27" t="n">
         <v>-0.457761131918445</v>
+      </c>
+      <c r="EY27" t="n">
+        <v>-0.324807145757211</v>
+      </c>
+      <c r="EZ27" t="n">
+        <v>0.0806776926179865</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B28" t="n">
         <v>-2.47858017135862</v>
@@ -37508,11 +37956,17 @@
       </c>
       <c r="EX28" t="n">
         <v>2.20870678617159</v>
+      </c>
+      <c r="EY28" t="n">
+        <v>2.76999688764394</v>
+      </c>
+      <c r="EZ28" t="n">
+        <v>3.11632212280159</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B29" t="n">
         <v>1.19402985074626</v>
@@ -37972,11 +38426,17 @@
       </c>
       <c r="EX29" t="n">
         <v>-0.845771144278601</v>
+      </c>
+      <c r="EY29" t="n">
+        <v>-0.471031559114461</v>
+      </c>
+      <c r="EZ29" t="n">
+        <v>0.0468164794007464</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B30" t="n">
         <v>0.281690140845068</v>
@@ -38436,11 +38896,17 @@
       </c>
       <c r="EX30" t="n">
         <v>1.0566762728146</v>
+      </c>
+      <c r="EY30" t="n">
+        <v>0.380952380952386</v>
+      </c>
+      <c r="EZ30" t="n">
+        <v>0.665399239543742</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -38595,10 +39061,12 @@
       <c r="EV31"/>
       <c r="EW31"/>
       <c r="EX31"/>
+      <c r="EY31"/>
+      <c r="EZ31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B32" t="n">
         <v>3.31753554502368</v>
@@ -39058,11 +39526,17 @@
       </c>
       <c r="EX32" t="n">
         <v>-1.43540669856458</v>
+      </c>
+      <c r="EY32" t="n">
+        <v>-1.42857142857143</v>
+      </c>
+      <c r="EZ32" t="n">
+        <v>-1.87353629976582</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B33" t="n">
         <v>0.694444444444438</v>
@@ -39522,11 +39996,17 @@
       </c>
       <c r="EX33" t="n">
         <v>1.38592750533047</v>
+      </c>
+      <c r="EY33" t="n">
+        <v>0.817160367722163</v>
+      </c>
+      <c r="EZ33" t="n">
+        <v>1.01832993890019</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B34" t="n">
         <v>2.71903323262839</v>
@@ -39986,11 +40466,17 @@
       </c>
       <c r="EX34" t="n">
         <v>1.1454753722795</v>
+      </c>
+      <c r="EY34" t="n">
+        <v>1.01580135440181</v>
+      </c>
+      <c r="EZ34" t="n">
+        <v>0.887902330743631</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B35" t="n">
         <v>0.211416490486261</v>
@@ -40450,11 +40936,17 @@
       </c>
       <c r="EX35" t="n">
         <v>0.681818181818175</v>
+      </c>
+      <c r="EY35" t="n">
+        <v>0.883002207505531</v>
+      </c>
+      <c r="EZ35" t="n">
+        <v>1.54525386313466</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B36" t="n">
         <v>2.80076384468492</v>
@@ -40914,11 +41406,17 @@
       </c>
       <c r="EX36" t="n">
         <v>0.381315538608213</v>
+      </c>
+      <c r="EY36" t="n">
+        <v>0.687593423019418</v>
+      </c>
+      <c r="EZ36" t="n">
+        <v>0.324771183938579</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B37" t="n">
         <v>2.84605433376456</v>
@@ -41378,11 +41876,17 @@
       </c>
       <c r="EX37" t="n">
         <v>5.98726114649682</v>
+      </c>
+      <c r="EY37" t="n">
+        <v>6.02258469259724</v>
+      </c>
+      <c r="EZ37" t="n">
+        <v>6.56753407682775</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B38" t="n">
         <v>-1.41821619918059</v>
@@ -41842,11 +42346,17 @@
       </c>
       <c r="EX38" t="n">
         <v>0.124107973937318</v>
+      </c>
+      <c r="EY38" t="n">
+        <v>0.208986415882964</v>
+      </c>
+      <c r="EZ38" t="n">
+        <v>0.266824785057822</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B39" t="n">
         <v>0.205761316872425</v>
@@ -42306,11 +42816,17 @@
       </c>
       <c r="EX39" t="n">
         <v>1.39094406629182</v>
+      </c>
+      <c r="EY39" t="n">
+        <v>0.806219406852868</v>
+      </c>
+      <c r="EZ39" t="n">
+        <v>0.427837992013691</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B40" t="n">
         <v>1.61725067385445</v>
@@ -42770,11 +43286,17 @@
       </c>
       <c r="EX40" t="n">
         <v>-0.259067357512957</v>
+      </c>
+      <c r="EY40" t="n">
+        <v>0.999999999999996</v>
+      </c>
+      <c r="EZ40" t="n">
+        <v>1.48883374689828</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B41" t="n">
         <v>1.94718591624434</v>
@@ -43234,11 +43756,17 @@
       </c>
       <c r="EX41" t="n">
         <v>0.365821792526777</v>
+      </c>
+      <c r="EY41" t="n">
+        <v>0.744353182751549</v>
+      </c>
+      <c r="EZ41" t="n">
+        <v>0.0506457330969981</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B42" t="n">
         <v>0.749829584185428</v>
@@ -43698,11 +44226,17 @@
       </c>
       <c r="EX42" t="n">
         <v>1.84696569920841</v>
+      </c>
+      <c r="EY42" t="n">
+        <v>2.2609819121447</v>
+      </c>
+      <c r="EZ42" t="n">
+        <v>2.44215938303343</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B43" t="n">
         <v>-0.383729854182655</v>
@@ -44162,11 +44696,17 @@
       </c>
       <c r="EX43" t="n">
         <v>0.694980694980699</v>
+      </c>
+      <c r="EY43" t="n">
+        <v>-0.632466619817291</v>
+      </c>
+      <c r="EZ43" t="n">
+        <v>-1.58839779005526</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B44" t="n">
         <v>-0.726955510322752</v>
@@ -44626,11 +45166,17 @@
       </c>
       <c r="EX44" t="n">
         <v>1.75810851773263</v>
+      </c>
+      <c r="EY44" t="n">
+        <v>1.50887573964496</v>
+      </c>
+      <c r="EZ44" t="n">
+        <v>1.2496367335077</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B45" t="n">
         <v>0.638977635782745</v>
@@ -45090,11 +45636,17 @@
       </c>
       <c r="EX45" t="n">
         <v>-1.36054421768707</v>
+      </c>
+      <c r="EY45" t="n">
+        <v>-1.66666666666667</v>
+      </c>
+      <c r="EZ45" t="n">
+        <v>-0.662251655629137</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B46" t="n">
         <v>0.817096165933364</v>
@@ -45554,11 +46106,17 @@
       </c>
       <c r="EX46" t="n">
         <v>1.08892921960072</v>
+      </c>
+      <c r="EY46" t="n">
+        <v>0.83932853717025</v>
+      </c>
+      <c r="EZ46" t="n">
+        <v>0.355660936573813</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -46018,11 +46576,17 @@
       </c>
       <c r="EX47" t="n">
         <v>0.797872340425562</v>
+      </c>
+      <c r="EY47" t="n">
+        <v>-0.25510204081633</v>
+      </c>
+      <c r="EZ47" t="n">
+        <v>-0.505050505050494</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B48" t="n">
         <v>-0.924499229583967</v>
@@ -46482,11 +47046,17 @@
       </c>
       <c r="EX48" t="n">
         <v>3.34128878281623</v>
+      </c>
+      <c r="EY48" t="n">
+        <v>2.77136258660508</v>
+      </c>
+      <c r="EZ48" t="n">
+        <v>3.07480495640203</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B49" t="n">
         <v>0.553720613949856</v>
@@ -46946,11 +47516,17 @@
       </c>
       <c r="EX49" t="n">
         <v>1.84080449974432</v>
+      </c>
+      <c r="EY49" t="n">
+        <v>1.34699611602348</v>
+      </c>
+      <c r="EZ49" t="n">
+        <v>1.09845069267972</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B50" t="n">
         <v>1.91780821917808</v>
@@ -47410,11 +47986,17 @@
       </c>
       <c r="EX50" t="n">
         <v>3.70090634441088</v>
+      </c>
+      <c r="EY50" t="n">
+        <v>3.45334313005145</v>
+      </c>
+      <c r="EZ50" t="n">
+        <v>3.19767441860466</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B51" t="n">
         <v>1.81818181818182</v>
@@ -47874,11 +48456,17 @@
       </c>
       <c r="EX51" t="n">
         <v>3.80952380952382</v>
+      </c>
+      <c r="EY51" t="n">
+        <v>1.80180180180181</v>
+      </c>
+      <c r="EZ51" t="n">
+        <v>2.6865671641791</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B52" t="n">
         <v>-0.802568218298555</v>
@@ -48338,11 +48926,17 @@
       </c>
       <c r="EX52" t="n">
         <v>2.67965895249698</v>
+      </c>
+      <c r="EY52" t="n">
+        <v>3.35510688836105</v>
+      </c>
+      <c r="EZ52" t="n">
+        <v>4.05524537173083</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B53" t="n">
         <v>1.91188694929342</v>
@@ -48802,11 +49396,17 @@
       </c>
       <c r="EX53" t="n">
         <v>-1.93704600484261</v>
+      </c>
+      <c r="EY53" t="n">
+        <v>-2.11960635881906</v>
+      </c>
+      <c r="EZ53" t="n">
+        <v>-2.08178438661711</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B54" t="n">
         <v>-0.290275761973879</v>
@@ -49266,11 +49866,17 @@
       </c>
       <c r="EX54" t="n">
         <v>0.665557404326121</v>
+      </c>
+      <c r="EY54" t="n">
+        <v>0.644122383252827</v>
+      </c>
+      <c r="EZ54" t="n">
+        <v>1.11464968152866</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B55" t="n">
         <v>-0.753012048192771</v>
@@ -49730,11 +50336,17 @@
       </c>
       <c r="EX55" t="n">
         <v>-1.75097276264591</v>
+      </c>
+      <c r="EY55" t="n">
+        <v>-2.52690687880205</v>
+      </c>
+      <c r="EZ55" t="n">
+        <v>-1.77156177156178</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B56" t="n">
         <v>0.955414012738856</v>
@@ -50194,6 +50806,12 @@
       </c>
       <c r="EX56" t="n">
         <v>-0.334448160535122</v>
+      </c>
+      <c r="EY56" t="n">
+        <v>-0.64102564102565</v>
+      </c>
+      <c r="EZ56" t="n">
+        <v>-1.27388535031847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>